<commit_message>
run faster and right
</commit_message>
<xml_diff>
--- a/output_result/news_data_with_topics_0225.xlsx
+++ b/output_result/news_data_with_topics_0225.xlsx
@@ -532,12 +532,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "COMEX白银期货跌幅扩大至1.5%，现报28.71美元/盎司", "news_prompt2": "沪银跌近3%，现报7230元/千克", "news_prompt3": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "沪银跌近3%，现报7230元/千克"}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"沪银跌近3%，现报7230元/千克": {"topic": "“金融”", "similarity": 0.45425719022750854, "prompt": "新闻文本是“沪银跌近3%，现报7230元/千克”，包含的情绪词典是：下跌/下降(fall):-0.6,贬值/减值(devaluation):-0.5"}}</t>
+          <t>{"沪银跌近3%，现报7230元/千克": {"topic": "“金融”", "similarity": 0.4542572796344757, "prompt": "新闻文本是“沪银跌近3%，现报7230元/千克”，包含的情绪词典是：下跌/下降(fall):-0.6,贬值/减值(devaluation):-0.5"}}</t>
         </is>
       </c>
     </row>
@@ -583,12 +583,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "21世纪资管研究院吴霜，实习生朱一乔综合整理 　　一、监管和政策 　　1、央行：继续坚持支持性的货币政策立场，研究储备增量政策举措 　　8月26日，中国人民银行召开专家学者及金融企业负责人座谈会", "news_prompt2": "潘功胜表示，大家提出了很好的意见建议", "news_prompt3": "今年以来，中国人民银行坚决贯彻落实党中央、国务院决策部署，稳健的货币政策灵活适度、精准有效，在2月、5月、7月先后三次实施了比较大的货币政策调整，有力支持经济回升向好", "news_prompt4": "下一阶段，中国人民银行将深入贯彻党的二十届三中全会精神，落实好中央政治局会议关于“宏观政策要持续用力、更加给力”的要求，继续坚持支持性的货币政策立场，加强逆周期调节，综合运用多种货币政策工具，加大金融对实体经济的支持力度", "news_prompt5": "2、住建部权威解读房屋养老金：不需要居民额外缴费，不会增加个人负担 　　近日，房屋养老金的话题引发社会广泛关注", "news_prompt6": "8月26日，住房城乡建设部相关司局负责人就社会关注的房屋养老金相关问题进行权威解读", "news_prompt7": "问：房屋养老金的资金来源是什么", "news_prompt8": "答：房屋养老金由个人账户和公共账户两部分组成", "news_prompt9": "个人账户就是业主交存的住宅专项维修资金，交存按现行规定执行", "news_prompt10": "公共账户按照“取之于房、用之于房”“不增加个人负担、不减损个人权益”的原则，由政府负责建立，从试点城市看，地方政府可以通过财政补一点、土地出让金归集一些等方式筹集，目的是建立稳定的房屋安全管理资金渠道，不需要居民额外缴费，不会增加个人负担", "news_prompt11": "3、中央财办副主任韩文秀：合理扩大地方政府专项债券支持范围，适当扩大用作资本金的领域、规模、比例 　　中央财办分管日常工作的副主任韩文秀在8月27日出版的《人民日报》上发表《深化财税体制改革》文章指出，健全政府债务管理体系", "news_prompt12": "按照统筹发展和安全要求，完善政府债务管理制度，更好发挥债券资金促进经济社会发展的积极作用", "news_prompt13": "一是加快建立同高质量发展相适应的政府债务管理机制", "news_prompt14": "二是建立全口径地方债务监测监管体系和防范化解隐性债务风险长效机制", "news_prompt15": "三是加强地方政府专项债券管理", "news_prompt16": "四是加快地方融资平台改革转型", "news_prompt17": "加强对融资平台公司的综合治理，持续规范融资管理，禁止各种变相举债行为，推动形成政府和企业界限清晰、责任明确、风险可控的科学管理机制", "news_prompt18": "4、六部门：严禁为没有收益或收益不足的市政基础设施资产违法违规举债 　　8月26日，财政部等六部门制定印发《市政基础设施资产管理办法（试行）》", "news_prompt19": "办法强调，政府投资建设的市政基础设施资产应当依法严格履行基本建设审批程序，落实资金来源，加强预算约束，防范政府债务风险", "news_prompt20": "严禁为没有收益或收益不足的市政基础设施资产违法违规举债，不得增加隐性债务", "news_prompt21": "通过发行地方政府专项债券建设的市政基础设施管护期间产生的有偿使用收入，按规定优先用于偿还对应项目的地方政府专项债券本息，不得挪作他用", "news_prompt22": "本办法自2024年9月1日起施行", "news_prompt23": "5、金融监管总局：正会同财政部等研究制定地方资产管理公司监管办法 　　8月26日，金融时报发文称，近日，金融监管总局发布了《国家金融监督管理总局对十四届全国人大二次会议第8632号建议的答复》，对王立生代表提出的关于鼓励支持壮大省级资产管理公司有效处置中小金融机构不良资产的建议，作出答复", "news_prompt24": "答复中指出：“金融监管总局正在会同财政部等部门研究制定地方资产管理公司监管办法，全面贯彻落实中央金融工作会议精神，立足于强监管防风险，坚持问题导向，针对行业发展与监管中存在的突出问题，进一步细化业务经营、公司治理与风险管理、监督管理等方面监管规则，促进地方资产管理公司专注主业、健康规范发展", "news_prompt25": "”此外，在该答复中，金融监管总局还透露，将会同财政部综合考虑不良贷款转让试点情况、相关企业展业情况、高风险机构及不良贷款转让处置需求等因素，研究出台有关制度，扩大试点范围或推进试点政策常态化实施，助力银行业金融机构不断拓展不良资产处置渠道和处置方式", "news_prompt26": "6、央行等八部门：支持公募基金管理人积极布局绿色低碳主题公募基金 　　8月27日，央行等八部门发布《关于进一步做好金融支持长江经济带绿色低碳高质量发展的指导意见》", "news_prompt27": "其中，在发挥多层次资本市场作用方面，提出支持符合条件的长江经济带绿色低碳企业利用多层次资本市场，通过发行上市、再融资、并购重组、新三板挂牌等方式融资发展", "news_prompt28": "此外，支持长江经济带相关企业符合条件的基础设施项目发行资产证券化产品和基础设施领域不动产投资信托基金（REITs）", "news_prompt29": "支持公募基金管理人积极布局相关主题公募基金", "news_prompt30": "研究编制绿色低碳发展指数，推出更多绿色低碳发展相关指数化投资产品", "news_prompt31": "7、央行官网增加“公开市场国债买卖业务公告”栏目 　　8月28日，中国人民银行网站显示，公开市场业务栏目增加“公开市场国债买卖业务公告”", "news_prompt32": "央行日前发布的2024年第二季度中国货币政策执行报告称，中央金融工作会议提出，要充实货币政策工具箱，在央行公开市场操作中逐"}</t>
+          <t>{"news_prompt1": "21世纪资管研究院吴霜，实习生朱一乔综合整理 　　一、监管和政策 　　1、央行：继续坚持支持性的货币政策立场，研究储备增量政策举措 　　8月26日，中国人民银行召开专家学者及金融企业负责人座谈会", "news_prompt2": "今年以来，中国人民银行坚决贯彻落实党中央、国务院决策部署，稳健的货币政策灵活适度、精准有效，在2月、5月、7月先后三次实施了比较大的货币政策调整，有力支持经济回升向好", "news_prompt3": "下一阶段，中国人民银行将深入贯彻党的二十届三中全会精神，落实好中央政治局会议关于“宏观政策要持续用力、更加给力”的要求，继续坚持支持性的货币政策立场，加强逆周期调节，综合运用多种货币政策工具，加大金融对实体经济的支持力度", "news_prompt4": "2、住建部权威解读房屋养老金：不需要居民额外缴费，不会增加个人负担 　　近日，房屋养老金的话题引发社会广泛关注", "news_prompt5": "8月26日，住房城乡建设部相关司局负责人就社会关注的房屋养老金相关问题进行权威解读", "news_prompt6": "问：房屋养老金的资金来源是什么", "news_prompt7": "答：房屋养老金由个人账户和公共账户两部分组成", "news_prompt8": "个人账户就是业主交存的住宅专项维修资金，交存按现行规定执行", "news_prompt9": "公共账户按照“取之于房、用之于房”“不增加个人负担、不减损个人权益”的原则，由政府负责建立，从试点城市看，地方政府可以通过财政补一点、土地出让金归集一些等方式筹集，目的是建立稳定的房屋安全管理资金渠道，不需要居民额外缴费，不会增加个人负担", "news_prompt10": "3、中央财办副主任韩文秀：合理扩大地方政府专项债券支持范围，适当扩大用作资本金的领域、规模、比例 　　中央财办分管日常工作的副主任韩文秀在8月27日出版的《人民日报》上发表《深化财税体制改革》文章指出，健全政府债务管理体系", "news_prompt11": "按照统筹发展和安全要求，完善政府债务管理制度，更好发挥债券资金促进经济社会发展的积极作用", "news_prompt12": "一是加快建立同高质量发展相适应的政府债务管理机制", "news_prompt13": "二是建立全口径地方债务监测监管体系和防范化解隐性债务风险长效机制", "news_prompt14": "三是加强地方政府专项债券管理", "news_prompt15": "四是加快地方融资平台改革转型", "news_prompt16": "加强对融资平台公司的综合治理，持续规范融资管理，禁止各种变相举债行为，推动形成政府和企业界限清晰、责任明确、风险可控的科学管理机制", "news_prompt17": "4、六部门：严禁为没有收益或收益不足的市政基础设施资产违法违规举债 　　8月26日，财政部等六部门制定印发《市政基础设施资产管理办法（试行）》", "news_prompt18": "办法强调，政府投资建设的市政基础设施资产应当依法严格履行基本建设审批程序，落实资金来源，加强预算约束，防范政府债务风险", "news_prompt19": "严禁为没有收益或收益不足的市政基础设施资产违法违规举债，不得增加隐性债务", "news_prompt20": "通过发行地方政府专项债券建设的市政基础设施管护期间产生的有偿使用收入，按规定优先用于偿还对应项目的地方政府专项债券本息，不得挪作他用", "news_prompt21": "本办法自2024年9月1日起施行", "news_prompt22": "5、金融监管总局：正会同财政部等研究制定地方资产管理公司监管办法 　　8月26日，金融时报发文称，近日，金融监管总局发布了《国家金融监督管理总局对十四届全国人大二次会议第8632号建议的答复》，对王立生代表提出的关于鼓励支持壮大省级资产管理公司有效处置中小金融机构不良资产的建议，作出答复", "news_prompt23": "6、央行等八部门：支持公募基金管理人积极布局绿色低碳主题公募基金 　　8月27日，央行等八部门发布《关于进一步做好金融支持长江经济带绿色低碳高质量发展的指导意见》", "news_prompt24": "其中，在发挥多层次资本市场作用方面，提出支持符合条件的长江经济带绿色低碳企业利用多层次资本市场，通过发行上市、再融资、并购重组、新三板挂牌等方式融资发展", "news_prompt25": "此外，支持长江经济带相关企业符合条件的基础设施项目发行资产证券化产品和基础设施领域不动产投资信托基金（REITs）", "news_prompt26": "支持公募基金管理人积极布局相关主题公募基金", "news_prompt27": "研究编制绿色低碳发展指数，推出更多绿色低碳发展相关指数化投资产品", "news_prompt28": "7、央行官网增加“公开市场国债买卖业务公告”栏目 　　8月28日，中国人民银行网站显示，公开市场业务栏目增加“公开市场国债买卖业务公告”", "news_prompt29": "央行日前发布的2024年第二季度中国货币政策执行报告称，中央金融工作会议提出，要充实货币政策工具箱，在央行公开市场操作中逐"}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"21世纪资管研究院吴霜，实习生朱一乔综合整理 　　一、监管和政策 　　1、央行：继续坚持支持性的货币政策立场，研究储备增量政策举措 　　8月26日，中国人民银行召开专家学者及金融企业负责人座谈会": {"topic": "“金融”", "similarity": 0.7434403896331787, "prompt": "新闻文本是“21世纪资管研究院吴霜，实习生朱一乔综合整理 　　一、监管和政策 　　1、央行：继续坚持支持性的货币政策立场，研究储备增量政策举措 　　8月26日，中国人民银行召开专家学者及金融企业负责人座谈会”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,受监管的/受调控的(regulated):0.0"}, "今年以来，中国人民银行坚决贯彻落实党中央、国务院决策部署，稳健的货币政策灵活适度、精准有效，在2月、5月、7月先后三次实施了比较大的货币政策调整，有力支持经济回升向好": {"topic": "“宏观经济”", "similarity": 0.6990376710891724, "prompt": "新闻文本是“今年以来，中国人民银行坚决贯彻落实党中央、国务院决策部署，稳健的货币政策灵活适度、精准有效，在2月、5月、7月先后三次实施了比较大的货币政策调整，有力支持经济回升向好”，包含的情绪词典是：金融的/财政的(financial):0.0,监管/调控(regulation):0.0"}, "下一阶段，中国人民银行将深入贯彻党的二十届三中全会精神，落实好中央政治局会议关于“宏观政策要持续用力、更加给力”的要求，继续坚持支持性的货币政策立场，加强逆周期调节，综合运用多种货币政策工具，加大金融对实体经济的支持力度": {"topic": "“宏观经济”", "similarity": 0.7075463533401489, "prompt": "新闻文本是“下一阶段，中国人民银行将深入贯彻党的二十届三中全会精神，落实好中央政治局会议关于“宏观政策要持续用力、更加给力”的要求，继续坚持支持性的货币政策立场，加强逆周期调节，综合运用多种货币政策工具，加大金融对实体经济的支持力度”，包含的情绪词典是：货币/通货(currency):0.0,金融的/财政的(financial):0.0"}, "2、住建部权威解读房屋养老金：不需要居民额外缴费，不会增加个人负担 　　近日，房屋养老金的话题引发社会广泛关注": {"topic": "“房地产”", "similarity": 0.6563060283660889, "prompt": "新闻文本是“2、住建部权威解读房屋养老金：不需要居民额外缴费，不会增加个人负担 　　近日，房屋养老金的话题引发社会广泛关注”，包含的情绪词典是：房子/住宅(house):0.0,居民/住户(resident):0.0"}, "8月26日，住房城乡建设部相关司局负责人就社会关注的房屋养老金相关问题进行权威解读": {"topic": "“房地产”", "similarity": 0.6021968126296997, "prompt": "新闻文本是“8月26日，住房城乡建设部相关司局负责人就社会关注的房屋养老金相关问题进行权威解读”，包含的情绪词典是：房子/住宅(house):0.0,房地产/财产(estate):0.0"}, "问：房屋养老金的资金来源是什么": {"topic": "“房地产”", "similarity": 0.46724992990493774, "prompt": "新闻文本是“问：房屋养老金的资金来源是什么”，包含的情绪词典是：基金/资金(fund):0.1,房子/住宅(house):0.0"}, "答：房屋养老金由个人账户和公共账户两部分组成": {"topic": "“房地产”", "similarity": 0.5297958850860596, "prompt": "新闻文本是“答：房屋养老金由个人账户和公共账户两部分组成”，包含的情绪词典是：账户/账目(account):0.0,房子/住宅(house):0.0"}, "个人账户就是业主交存的住宅专项维修资金，交存按现行规定执行": {"topic": "“房地产”", "similarity": 0.5604603290557861, "prompt": "新闻文本是“个人账户就是业主交存的住宅专项维修资金，交存按现行规定执行”，包含的情绪词典是：账户/账目(account):0.0,居民/住户(resident):0.0"}, "公共账户按照“取之于房、用之于房”“不增加个人负担、不减损个人权益”的原则，由政府负责建立，从试点城市看，地方政府可以通过财政补一点、土地出让金归集一些等方式筹集，目的是建立稳定的房屋安全管理资金渠道，不需要居民额外缴费，不会增加个人负担": {"topic": "“房地产”", "similarity": 0.6416574716567993, "prompt": "新闻文本是“公共账户按照“取之于房、用之于房”“不增加个人负担、不减损个人权益”的原则，由政府负责建立，从试点城市看，地方政府可以通过财政补一点、土地出让金归集一些等方式筹集，目的是建立稳定的房屋安全管理资金渠道，不需要居民额外缴费，不会增加个人负担”，包含的情绪词典是：房子/住宅(house):0.0,居民/住户(resident):0.0"}, "3、中央财办副主任韩文秀：合理扩大地方政府专项债券支持范围，适当扩大用作资本金的领域、规模、比例 　　中央财办分管日常工作的副主任韩文秀在8月27日出版的《人民日报》上发表《深化财税体制改革》文章指出，健全政府债务管理体系": {"topic": "“金融”", "similarity": 0.6664038896560669, "prompt": "新闻文本是“3、中央财办副主任韩文秀：合理扩大地方政府专项债券支持范围，适当扩大用作资本金的领域、规模、比例 　　中央财办分管日常工作的副主任韩文秀在8月27日出版的《人民日报》上发表《深化财税体制改革》文章指出，健全政府债务管理体系”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "按照统筹发展和安全要求，完善政府债务管理制度，更好发挥债券资金促进经济社会发展的积极作用": {"topic": "“金融”", "similarity": 0.48477911949157715, "prompt": "新闻文本是“按照统筹发展和安全要求，完善政府债务管理制度，更好发挥债券资金促进经济社会发展的积极作用”，包含的情绪词典是：债券/结合(bond):0.0,负债的/欠债的(indebted):-0.5"}, "一是加快建立同高质量发展相适应的政府债务管理机制": {"topic": "“宏观经济”", "similarity": 0.5222164988517761, "prompt": "新闻文本是“一是加快建立同高质量发展相适应的政府债务管理机制”，包含的情绪词典是：债券/结合(bond):0.0,负债的/欠债的(indebted):-0.5"}, "二是建立全口径地方债务监测监管体系和防范化解隐性债务风险长效机制": {"topic": "“宏观经济”", "similarity": 0.5031692385673523, "prompt": "新闻文本是“二是建立全口径地方债务监测监管体系和防范化解隐性债务风险长效机制”，包含的情绪词典是：负债的/欠债的(indebted):-0.5,偿债能力/偿付能力(solvency):0.3"}, "三是加强地方政府专项债券管理": {"topic": "“金融”", "similarity": 0.48812541365623474, "prompt": "新闻文本是“三是加强地方政府专项债券管理”，包含的情绪词典是：债券/结合(bond):0.0,加强/增强(strengthen):0.7"}, "四是加快地方融资平台改革转型": {"topic": "“金融”", "similarity": 0.5280762910842896, "prompt": "新闻文本是“四是加快地方融资平台改革转型”，包含的情绪词典是：金融/财政(finance):0.0,资本/资金(capital):0.1"}, "加强对融资平台公司的综合治理，持续规范融资管理，禁止各种变相举债行为，推动形成政府和企业界限清晰、责任明确、风险可控的科学管理机制": {"topic": "“金融”", "similarity": 0.5951088666915894, "prompt": "新闻文本是“加强对融资平台公司的综合治理，持续规范融资管理，禁止各种变相举债行为，推动形成政府和企业界限清晰、责任明确、风险可控的科学管理机制”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,监管的/调控的(regulatory):0.0"}, "4、六部门：严禁为没有收益或收益不足的市政基础设施资产违法违规举债 　　8月26日，财政部等六部门制定印发《市政基础设施资产管理办法（试行）》": {"topic": "“房地产”", "similarity": 0.6391754150390625, "prompt": "新闻文本是“4、六部门：严禁为没有收益或收益不足的市政基础设施资产违法违规举债 　　8月26日，财政部等六部门制定印发《市政基础设施资产管理办法（试行）》”，包含的情绪词典是：资金不足的(underfunded):-0.3,资产/财产(asset):0.3"}, "办法强调，政府投资建设的市政基础设施资产应当依法严格履行基本建设审批程序，落实资金来源，加强预算约束，防范政府债务风险": {"topic": "“房地产”", "similarity": 0.575090229511261, "prompt": "新闻文本是“办法强调，政府投资建设的市政基础设施资产应当依法严格履行基本建设审批程序，落实资金来源，加强预算约束，防范政府债务风险”，包含的情绪词典是：负债的/欠债的(indebted):-0.5,资产/财产(asset):0.3"}, "严禁为没有收益或收益不足的市政基础设施资产违法违规举债，不得增加隐性债务": {"topic": "“房地产”", "similarity": 0.5156071186065674, "prompt": "新闻文本是“严禁为没有收益或收益不足的市政基础设施资产违法违规举债，不得增加隐性债务”，包含的情绪词典是：资金不足的(underfunded):-0.3,未充分利用的(underutilized):-0.4"}, "通过发行地方政府专项债券建设的市政基础设施管护期间产生的有偿使用收入，按规定优先用于偿还对应项目的地方政府专项债券本息，不得挪作他用": {"topic": "“房地产”", "similarity": 0.5596761703491211, "prompt": "新闻文本是“通过发行地方政府专项债券建设的市政基础设施管护期间产生的有偿使用收入，按规定优先用于偿还对应项目的地方政府专项债券本息，不得挪作他用”，包含的情绪词典是：债券/结合(bond):0.0,指定用途/专款专用(earmarking):0.0"}, "本办法自2024年9月1日起施行": {"topic": "“生产投资”", "similarity": 0.4501095414161682, "prompt": "新闻文本是“本办法自2024年9月1日起施行”，包含的情绪词典是：颁布法令/发布政令(decreeing):0.0,法令/法规(statute):0.0"}, "5、金融监管总局：正会同财政部等研究制定地方资产管理公司监管办法 　　8月26日，金融时报发文称，近日，金融监管总局发布了《国家金融监督管理总局对十四届全国人大二次会议第8632号建议的答复》，对王立生代表提出的关于鼓励支持壮大省级资产管理公司有效处置中小金融机构不良资产的建议，作出答复": {"topic": "“金融”", "similarity": 0.6950241923332214, "prompt": "新闻文本是“5、金融监管总局：正会同财政部等研究制定地方资产管理公司监管办法 　　8月26日，金融时报发文称，近日，金融监管总局发布了《国家金融监督管理总局对十四届全国人大二次会议第8632号建议的答复》，对王立生代表提出的关于鼓励支持壮大省级资产管理公司有效处置中小金融机构不良资产的建议，作出答复”，包含的情绪词典是：金融的/财政的(financial):0.0,资产/财产(asset):0.3"}, "答复中指出：“金融监管总局正在会同财政部等部门研究制定地方资产管理公司监管办法，全面贯彻落实中央金融工作会议精神，立足于强监管防风险，坚持问题导向，针对行业发展与监管中存在的突出问题，进一步细化业务经营、公司治理与风险管理、监督管理等方面监管规则，促进地方资产管理公司专注主业、健康规范发展": {"topic": "“房地产”", "similarity": 0.663959801197052}, "”此外，在该答复中，金融监管总局还透露，将会同财政部综合考虑不良贷款转让试点情况、相关企业展业情况、高风险机构及不良贷款转让处置需求等因素，研究出台有关制度，扩大试点范围或推进试点政策常态化实施，助力银行业金融机构不断拓展不良资产处置渠道和处置方式": {"topic": "“金融”", "similarity": 0.6194922924041748}, "6、央行等八部门：支持公募基金管理人积极布局绿色低碳主题公募基金 　　8月27日，央行等八部门发布《关于进一步做好金融支持长江经济带绿色低碳高质量发展的指导意见》": {"topic": "“金融”", "similarity": 0.6756401062011719, "prompt": "新闻文本是“6、央行等八部门：支持公募基金管理人积极布局绿色低碳主题公募基金 　　8月27日，央行等八部门发布《关于进一步做好金融支持长江经济带绿色低碳高质量发展的指导意见》”，包含的情绪词典是：基金/资金(fund):0.1,基本的/根本的(fundamental):0.3"}, "其中，在发挥多层次资本市场作用方面，提出支持符合条件的长江经济带绿色低碳企业利用多层次资本市场，通过发行上市、再融资、并购重组、新三板挂牌等方式融资发展": {"topic": "“生产投资”", "similarity": 0.6829119920730591, "prompt": "新闻文本是“其中，在发挥多层次资本市场作用方面，提出支持符合条件的长江经济带绿色低碳企业利用多层次资本市场，通过发行上市、再融资、并购重组、新三板挂牌等方式融资发展”，包含的情绪词典是：发展/开发(development):0.4,资本/资金(capital):0.1"}, "此外，支持长江经济带相关企业符合条件的基础设施项目发行资产证券化产品和基础设施领域不动产投资信托基金（REITs）": {"topic": "“金融”", "similarity": 0.5559415817260742, "prompt": "新闻文本是“此外，支持长江经济带相关企业符合条件的基础设施项目发行资产证券化产品和基础设施领域不动产投资信托基金（REITs）”，包含的情绪词典是：基金/资金(fund):0.1,房地产/财产(estate):0.0"}, "支持公募基金管理人积极布局相关主题公募基金": {"topic": "“金融”", "similarity": 0.546876072883606, "prompt": "新闻文本是“支持公募基金管理人积极布局相关主题公募基金”，包含的情绪词典是：基金/资金(fund):0.1,支撑/支持(bolster):0.5"}, "研究编制绿色低碳发展指数，推出更多绿色低碳发展相关指数化投资产品": {"topic": "“金融”", "similarity": 0.4951046109199524, "prompt": "新闻文本是“研究编制绿色低碳发展指数，推出更多绿色低碳发展相关指数化投资产品”，包含的情绪词典是：指数/指标(index):0.0,发展/开发(development):0.4"}, "7、央行官网增加“公开市场国债买卖业务公告”栏目 　　8月28日，中国人民银行网站显示，公开市场业务栏目增加“公开市场国债买卖业务公告”": {"topic": "“金融”", "similarity": 0.6391689777374268, "prompt": "新闻文本是“7、央行官网增加“公开市场国债买卖业务公告”栏目 　　8月28日，中国人民银行网站显示，公开市场业务栏目增加“公开市场国债买卖业务公告””，包含的情绪词典是：债券/结合(bond):0.0,金融的/财政的(financial):0.0"}, "央行日前发布的2024年第二季度中国货币政策执行报告称，中央金融工作会议提出，要充实货币政策工具箱，在央行公开市场操作中逐": {"topic": "“宏观经济”", "similarity": 0.6001434922218323, "prompt": "新闻文本是“央行日前发布的2024年第二季度中国货币政策执行报告称，中央金融工作会议提出，要充实货币政策工具箱，在央行公开市场操作中逐”，包含的情绪词典是：执行的/实施的(executory):0.0,金融的/财政的(financial):0.0"}}</t>
+          <t>{"21世纪资管研究院吴霜，实习生朱一乔综合整理 　　一、监管和政策 　　1、央行：继续坚持支持性的货币政策立场，研究储备增量政策举措 　　8月26日，中国人民银行召开专家学者及金融企业负责人座谈会": {"topic": "“金融”", "similarity": 0.7434406280517578, "prompt": "新闻文本是“21世纪资管研究院吴霜，实习生朱一乔综合整理 　　一、监管和政策 　　1、央行：继续坚持支持性的货币政策立场，研究储备增量政策举措 　　8月26日，中国人民银行召开专家学者及金融企业负责人座谈会”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,受监管的/受调控的(regulated):0.0"}, "今年以来，中国人民银行坚决贯彻落实党中央、国务院决策部署，稳健的货币政策灵活适度、精准有效，在2月、5月、7月先后三次实施了比较大的货币政策调整，有力支持经济回升向好": {"topic": "“宏观经济”", "similarity": 0.6990377902984619, "prompt": "新闻文本是“今年以来，中国人民银行坚决贯彻落实党中央、国务院决策部署，稳健的货币政策灵活适度、精准有效，在2月、5月、7月先后三次实施了比较大的货币政策调整，有力支持经济回升向好”，包含的情绪词典是：金融的/财政的(financial):0.0,监管/调控(regulation):0.0"}, "下一阶段，中国人民银行将深入贯彻党的二十届三中全会精神，落实好中央政治局会议关于“宏观政策要持续用力、更加给力”的要求，继续坚持支持性的货币政策立场，加强逆周期调节，综合运用多种货币政策工具，加大金融对实体经济的支持力度": {"topic": "“宏观经济”", "similarity": 0.7075464725494385, "prompt": "新闻文本是“下一阶段，中国人民银行将深入贯彻党的二十届三中全会精神，落实好中央政治局会议关于“宏观政策要持续用力、更加给力”的要求，继续坚持支持性的货币政策立场，加强逆周期调节，综合运用多种货币政策工具，加大金融对实体经济的支持力度”，包含的情绪词典是：货币/通货(currency):0.0,金融的/财政的(financial):0.0"}, "2、住建部权威解读房屋养老金：不需要居民额外缴费，不会增加个人负担 　　近日，房屋养老金的话题引发社会广泛关注": {"topic": "“房地产”", "similarity": 0.6563060283660889, "prompt": "新闻文本是“2、住建部权威解读房屋养老金：不需要居民额外缴费，不会增加个人负担 　　近日，房屋养老金的话题引发社会广泛关注”，包含的情绪词典是：房子/住宅(house):0.0,居民/住户(resident):0.0"}, "8月26日，住房城乡建设部相关司局负责人就社会关注的房屋养老金相关问题进行权威解读": {"topic": "“房地产”", "similarity": 0.6021970510482788, "prompt": "新闻文本是“8月26日，住房城乡建设部相关司局负责人就社会关注的房屋养老金相关问题进行权威解读”，包含的情绪词典是：房子/住宅(house):0.0,房地产/财产(estate):0.0"}, "问：房屋养老金的资金来源是什么": {"topic": "“房地产”", "similarity": 0.46724992990493774, "prompt": "新闻文本是“问：房屋养老金的资金来源是什么”，包含的情绪词典是：基金/资金(fund):0.1,房子/住宅(house):0.0"}, "答：房屋养老金由个人账户和公共账户两部分组成": {"topic": "“房地产”", "similarity": 0.5297958850860596, "prompt": "新闻文本是“答：房屋养老金由个人账户和公共账户两部分组成”，包含的情绪词典是：账户/账目(account):0.0,房子/住宅(house):0.0"}, "个人账户就是业主交存的住宅专项维修资金，交存按现行规定执行": {"topic": "“房地产”", "similarity": 0.5604602098464966, "prompt": "新闻文本是“个人账户就是业主交存的住宅专项维修资金，交存按现行规定执行”，包含的情绪词典是：账户/账目(account):0.0,居民/住户(resident):0.0"}, "公共账户按照“取之于房、用之于房”“不增加个人负担、不减损个人权益”的原则，由政府负责建立，从试点城市看，地方政府可以通过财政补一点、土地出让金归集一些等方式筹集，目的是建立稳定的房屋安全管理资金渠道，不需要居民额外缴费，不会增加个人负担": {"topic": "“房地产”", "similarity": 0.6416575908660889, "prompt": "新闻文本是“公共账户按照“取之于房、用之于房”“不增加个人负担、不减损个人权益”的原则，由政府负责建立，从试点城市看，地方政府可以通过财政补一点、土地出让金归集一些等方式筹集，目的是建立稳定的房屋安全管理资金渠道，不需要居民额外缴费，不会增加个人负担”，包含的情绪词典是：房子/住宅(house):0.0,居民/住户(resident):0.0"}, "3、中央财办副主任韩文秀：合理扩大地方政府专项债券支持范围，适当扩大用作资本金的领域、规模、比例 　　中央财办分管日常工作的副主任韩文秀在8月27日出版的《人民日报》上发表《深化财税体制改革》文章指出，健全政府债务管理体系": {"topic": "“金融”", "similarity": 0.6664038896560669, "prompt": "新闻文本是“3、中央财办副主任韩文秀：合理扩大地方政府专项债券支持范围，适当扩大用作资本金的领域、规模、比例 　　中央财办分管日常工作的副主任韩文秀在8月27日出版的《人民日报》上发表《深化财税体制改革》文章指出，健全政府债务管理体系”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "按照统筹发展和安全要求，完善政府债务管理制度，更好发挥债券资金促进经济社会发展的积极作用": {"topic": "“金融”", "similarity": 0.4847792983055115, "prompt": "新闻文本是“按照统筹发展和安全要求，完善政府债务管理制度，更好发挥债券资金促进经济社会发展的积极作用”，包含的情绪词典是：债券/结合(bond):0.0,负债的/欠债的(indebted):-0.5"}, "一是加快建立同高质量发展相适应的政府债务管理机制": {"topic": "“宏观经济”", "similarity": 0.5222166180610657, "prompt": "新闻文本是“一是加快建立同高质量发展相适应的政府债务管理机制”，包含的情绪词典是：债券/结合(bond):0.0,负债的/欠债的(indebted):-0.5"}, "二是建立全口径地方债务监测监管体系和防范化解隐性债务风险长效机制": {"topic": "“宏观经济”", "similarity": 0.5031694173812866, "prompt": "新闻文本是“二是建立全口径地方债务监测监管体系和防范化解隐性债务风险长效机制”，包含的情绪词典是：负债的/欠债的(indebted):-0.5,偿债能力/偿付能力(solvency):0.3"}, "三是加强地方政府专项债券管理": {"topic": "“金融”", "similarity": 0.48812544345855713, "prompt": "新闻文本是“三是加强地方政府专项债券管理”，包含的情绪词典是：债券/结合(bond):0.0,加强/增强(strengthen):0.7"}, "四是加快地方融资平台改革转型": {"topic": "“金融”", "similarity": 0.5280763506889343, "prompt": "新闻文本是“四是加快地方融资平台改革转型”，包含的情绪词典是：金融/财政(finance):0.0,资本/资金(capital):0.1"}, "加强对融资平台公司的综合治理，持续规范融资管理，禁止各种变相举债行为，推动形成政府和企业界限清晰、责任明确、风险可控的科学管理机制": {"topic": "“金融”", "similarity": 0.5951089859008789, "prompt": "新闻文本是“加强对融资平台公司的综合治理，持续规范融资管理，禁止各种变相举债行为，推动形成政府和企业界限清晰、责任明确、风险可控的科学管理机制”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,监管的/调控的(regulatory):0.0"}, "4、六部门：严禁为没有收益或收益不足的市政基础设施资产违法违规举债 　　8月26日，财政部等六部门制定印发《市政基础设施资产管理办法（试行）》": {"topic": "“房地产”", "similarity": 0.6391754150390625, "prompt": "新闻文本是“4、六部门：严禁为没有收益或收益不足的市政基础设施资产违法违规举债 　　8月26日，财政部等六部门制定印发《市政基础设施资产管理办法（试行）》”，包含的情绪词典是：资金不足的(underfunded):-0.3,资产/财产(asset):0.3"}, "办法强调，政府投资建设的市政基础设施资产应当依法严格履行基本建设审批程序，落实资金来源，加强预算约束，防范政府债务风险": {"topic": "“房地产”", "similarity": 0.575090229511261, "prompt": "新闻文本是“办法强调，政府投资建设的市政基础设施资产应当依法严格履行基本建设审批程序，落实资金来源，加强预算约束，防范政府债务风险”，包含的情绪词典是：负债的/欠债的(indebted):-0.5,资产/财产(asset):0.3"}, "严禁为没有收益或收益不足的市政基础设施资产违法违规举债，不得增加隐性债务": {"topic": "“房地产”", "similarity": 0.5156071782112122, "prompt": "新闻文本是“严禁为没有收益或收益不足的市政基础设施资产违法违规举债，不得增加隐性债务”，包含的情绪词典是：资金不足的(underfunded):-0.3,未充分利用的(underutilized):-0.4"}, "通过发行地方政府专项债券建设的市政基础设施管护期间产生的有偿使用收入，按规定优先用于偿还对应项目的地方政府专项债券本息，不得挪作他用": {"topic": "“房地产”", "similarity": 0.5596761703491211, "prompt": "新闻文本是“通过发行地方政府专项债券建设的市政基础设施管护期间产生的有偿使用收入，按规定优先用于偿还对应项目的地方政府专项债券本息，不得挪作他用”，包含的情绪词典是：债券/结合(bond):0.0,指定用途/专款专用(earmarking):0.0"}, "本办法自2024年9月1日起施行": {"topic": "“生产投资”", "similarity": 0.450109601020813, "prompt": "新闻文本是“本办法自2024年9月1日起施行”，包含的情绪词典是：颁布法令/发布政令(decreeing):0.0,法令/法规(statute):0.0"}, "5、金融监管总局：正会同财政部等研究制定地方资产管理公司监管办法 　　8月26日，金融时报发文称，近日，金融监管总局发布了《国家金融监督管理总局对十四届全国人大二次会议第8632号建议的答复》，对王立生代表提出的关于鼓励支持壮大省级资产管理公司有效处置中小金融机构不良资产的建议，作出答复": {"topic": "“金融”", "similarity": 0.6950242519378662, "prompt": "新闻文本是“5、金融监管总局：正会同财政部等研究制定地方资产管理公司监管办法 　　8月26日，金融时报发文称，近日，金融监管总局发布了《国家金融监督管理总局对十四届全国人大二次会议第8632号建议的答复》，对王立生代表提出的关于鼓励支持壮大省级资产管理公司有效处置中小金融机构不良资产的建议，作出答复”，包含的情绪词典是：金融的/财政的(financial):0.0,资产/财产(asset):0.3"}, "6、央行等八部门：支持公募基金管理人积极布局绿色低碳主题公募基金 　　8月27日，央行等八部门发布《关于进一步做好金融支持长江经济带绿色低碳高质量发展的指导意见》": {"topic": "“金融”", "similarity": 0.6756401062011719, "prompt": "新闻文本是“6、央行等八部门：支持公募基金管理人积极布局绿色低碳主题公募基金 　　8月27日，央行等八部门发布《关于进一步做好金融支持长江经济带绿色低碳高质量发展的指导意见》”，包含的情绪词典是：基金/资金(fund):0.1,基本的/根本的(fundamental):0.3"}, "其中，在发挥多层次资本市场作用方面，提出支持符合条件的长江经济带绿色低碳企业利用多层次资本市场，通过发行上市、再融资、并购重组、新三板挂牌等方式融资发展": {"topic": "“生产投资”", "similarity": 0.6829118728637695, "prompt": "新闻文本是“其中，在发挥多层次资本市场作用方面，提出支持符合条件的长江经济带绿色低碳企业利用多层次资本市场，通过发行上市、再融资、并购重组、新三板挂牌等方式融资发展”，包含的情绪词典是：发展/开发(development):0.4,资本/资金(capital):0.1"}, "此外，支持长江经济带相关企业符合条件的基础设施项目发行资产证券化产品和基础设施领域不动产投资信托基金（REITs）": {"topic": "“金融”", "similarity": 0.5559417605400085, "prompt": "新闻文本是“此外，支持长江经济带相关企业符合条件的基础设施项目发行资产证券化产品和基础设施领域不动产投资信托基金（REITs）”，包含的情绪词典是：基金/资金(fund):0.1,房地产/财产(estate):0.0"}, "支持公募基金管理人积极布局相关主题公募基金": {"topic": "“金融”", "similarity": 0.546876072883606, "prompt": "新闻文本是“支持公募基金管理人积极布局相关主题公募基金”，包含的情绪词典是：基金/资金(fund):0.1,支撑/支持(bolster):0.5"}, "研究编制绿色低碳发展指数，推出更多绿色低碳发展相关指数化投资产品": {"topic": "“金融”", "similarity": 0.4951048195362091, "prompt": "新闻文本是“研究编制绿色低碳发展指数，推出更多绿色低碳发展相关指数化投资产品”，包含的情绪词典是：指数/指标(index):0.0,发展/开发(development):0.4"}, "7、央行官网增加“公开市场国债买卖业务公告”栏目 　　8月28日，中国人民银行网站显示，公开市场业务栏目增加“公开市场国债买卖业务公告”": {"topic": "“金融”", "similarity": 0.6391689777374268, "prompt": "新闻文本是“7、央行官网增加“公开市场国债买卖业务公告”栏目 　　8月28日，中国人民银行网站显示，公开市场业务栏目增加“公开市场国债买卖业务公告””，包含的情绪词典是：债券/结合(bond):0.0,金融的/财政的(financial):0.0"}, "央行日前发布的2024年第二季度中国货币政策执行报告称，中央金融工作会议提出，要充实货币政策工具箱，在央行公开市场操作中逐": {"topic": "“宏观经济”", "similarity": 0.6001436710357666, "prompt": "新闻文本是“央行日前发布的2024年第二季度中国货币政策执行报告称，中央金融工作会议提出，要充实货币政策工具箱，在央行公开市场操作中逐”，包含的情绪词典是：执行的/实施的(executory):0.0,金融的/财政的(financial):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -632,16 +632,8 @@
           <t>每日经济新闻</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>{"news_prompt1": "每经AI快讯，9月2日，PTA期货主力合约下跌4%，报5196元/吨", "news_prompt2": "（文章来源：每日经济新闻）"}</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>{"（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -685,12 +677,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "每天清晨，水寨镇黄狮新村的网格员陈妙芬都会打理自家庭院，养养花、种种草，日子过得惬意自在", "news_prompt2": "这份舒心来自于五华全面推进人居环境整治攻坚，各乡镇村容村貌焕然一新", "news_prompt3": "告别“脏乱差”，迎来“绿富美”", "news_prompt4": "五华各镇村迅速行动，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面，干群齐心共建美丽家园，持续提升宜居品质", "news_prompt5": "据了解，人居环境整治工作在五华县已经持续了一段时间", "news_prompt6": "按照有关部署要求，五华县将人居环境整治工作视为一场硬仗，集中人力物力推动整治工作重点攻坚，推动“百千万工程”迈上新台阶", "news_prompt7": "●南方日报记者汪思婷 　　干群动起来 　　网格化织密整治网络 　　“我们将环境整治分组包干，定点到户，全体镇村干部职工分为九大攻坚组，组织党员群众、志愿者、保洁员和群众等多方力量参与", "news_prompt8": "”龙村镇相关负责人表示，该镇通过网格化形式织密农村人居环境整治网络，全面推进人居环境整治攻坚", "news_prompt9": "自8月13日五华县“百县千镇万村高质量发展工程”指挥部印发《五华县开展农村人居环境整治和农房风貌提升攻坚行动工作方案》（下称《方案》）以来，五华各镇村迅速行动，全面组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面", "news_prompt10": "在人居环境整治方面，五华县主要围绕居住环境“干净、整洁、有序、宜居”目标，提出坚持典型引路，以点带面，将示范路段、典型镇村、沿路“六边”（高铁边、高速边、国道边、省道边、县道边、村主干道边）作为重点，按照“县级统筹、镇级主抓、村级落实、群众参与”的原则，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，干群齐心共建美丽家园，持续提升宜居品质", "news_prompt11": "在长布镇长生村，伴随着挖掘机“轰隆隆”的响声，涉及26户占地1700平方米的危旧祖屋被顺利拆除，村容村貌瞬间焕然一新", "news_prompt12": "当前，长布镇“三清三拆三整治”攻坚行动正在进行，在全镇村干部带动下，党群合力深入推进百千万群众干“百千万工程”，出资出力，做好农村人居环境整治工作", "news_prompt13": "据介绍，五华县各镇紧紧聚焦典型镇圩镇、典型村为中心，连接到镇政府、高速路口、圩镇、主干道等路线，并摸清县城建成区主干道、示范路线沿线，以典型镇、典型村为中心连接到镇政府、高速路口、圩镇、主干道等的路线可视范围以及典型镇圩镇、典型村区域内、面上镇、面上村“六边”的人居环境整治“三拆除”问题，全力推进农村人居环境整治", "news_prompt14": "环境美起来 　　注重长期推进显实效 　　“很漂亮，整个村都像穿上了新衣裳一样，赏心悦目", "news_prompt15": "”河东镇太和村村民周平安指着刚画好的墙绘说", "news_prompt16": "近日，河东镇邀请广东工程职业技术学院广东青年大学生“百千万工程”突击队到太和村开展特色墙绘活动，进一步掀起百千万群众干“百千万工程”热潮", "news_prompt17": "“为更好展示当地特色，我们先对当地进行实地调研，在确定社会主义核心价值观、乡村振兴、‘百千万工程’等主题后，把丝苗米元素融入到墙绘中", "news_prompt18": "”突击队队长李海涛说", "news_prompt19": "绘画现场，突击队员们夜以继日，手持画笔、以墙为纸、观景入画，满怀激情地投入到创作中，从刷漆打底到定位起稿，再从填色勾边到最后刷罩面漆，圆满完成了2米高、21米长和1.5米高、20米长的两处大面积墙绘，“绘”出了百千万群众干“百千万工程”的热闹图景，“画”出了景美人和的美丽乡村新画卷", "news_prompt20": "陈妙芬在水寨镇黄狮新村开展人居环境整治清理工作的同时，还不忘通过拉家常的方式向群众宣扬“美丽庭院”建设的好处", "news_prompt21": "怀着给周边邻居做个示范的想法，陈妙芬在2023年6月成功打造了自家的“美丽庭院”", "news_prompt22": "水寨镇坚持“党建引领美丽庭院”建设，加强宣传、打造典型、强化指导、干群合力", "news_prompt23": "同时，定期到各村指导做好“美丽庭院”的摸底、宣传、示范户的建设工作，并将庭院建设与村风家风相融合，赋予庭院更多的文化内涵，助推庭院建设“内外兼修”", "news_prompt24": "今年该镇拟建设“美丽庭院”87户，目前已完成73户", "news_prompt25": "人居环境整治是一场攻坚战、持久战，既要短期攻坚看变化，更要长期推进出实效长效", "news_prompt26": "五华明确提出，至2025年，全县80%以上村庄要达到“美丽宜居”村标准", "news_prompt27": "在此过程中，突出以“百千万工程”为统领，以“美丽五华·和美乡村”为主题，坚持全方位实施，打造宜居宜业和美乡村的五华样板", "news_prompt28": "城乡绿起来 　　爱绿植绿成了新风尚 　　走进转水镇五星村，村口新种的苗木和杜鹃花让人眼前一亮", "news_prompt29": "往村里走去，只见铺上沥青路面的村道两旁以及村民的房前屋后，新种了不少观赏苗木和鲜花", "news_prompt30": "今年，在村“两委”干部号召下，当地村民曾祥军在山坡上种下了数十棵果树，还在自家房前屋后种下桂花树，为绿美生态建设贡献力量", "news_prompt31": "“绿化搞好了，大家都受益，多好的事情", "news_prompt32": "”曾祥军说", "news_prompt33": "转水镇党委副书记陈锋告诉记者，该镇将绿美工作纳入村规民约，引导群众以主人翁的姿态积极投入绿"}</t>
+          <t>{"news_prompt1": "五华各镇村迅速行动，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面，干群齐心共建美丽家园，持续提升宜居品质", "news_prompt2": "按照有关部署要求，五华县将人居环境整治工作视为一场硬仗，集中人力物力推动整治工作重点攻坚，推动“百千万工程”迈上新台阶", "news_prompt3": "●南方日报记者汪思婷 　　干群动起来 　　网格化织密整治网络 　　“我们将环境整治分组包干，定点到户，全体镇村干部职工分为九大攻坚组，组织党员群众、志愿者、保洁员和群众等多方力量参与", "news_prompt4": "在长布镇长生村，伴随着挖掘机“轰隆隆”的响声，涉及26户占地1700平方米的危旧祖屋被顺利拆除，村容村貌瞬间焕然一新", "news_prompt5": "当前，长布镇“三清三拆三整治”攻坚行动正在进行，在全镇村干部带动下，党群合力深入推进百千万群众干“百千万工程”，出资出力，做好农村人居环境整治工作", "news_prompt6": "环境美起来 　　注重长期推进显实效 　　“很漂亮，整个村都像穿上了新衣裳一样，赏心悦目", "news_prompt7": "近日，河东镇邀请广东工程职业技术学院广东青年大学生“百千万工程”突击队到太和村开展特色墙绘活动，进一步掀起百千万群众干“百千万工程”热潮", "news_prompt8": "“为更好展示当地特色，我们先对当地进行实地调研，在确定社会主义核心价值观、乡村振兴、‘百千万工程’等主题后，把丝苗米元素融入到墙绘中", "news_prompt9": "绘画现场，突击队员们夜以继日，手持画笔、以墙为纸、观景入画，满怀激情地投入到创作中，从刷漆打底到定位起稿，再从填色勾边到最后刷罩面漆，圆满完成了2米高、21米长和1.5米高、20米长的两处大面积墙绘，“绘”出了百千万群众干“百千万工程”的热闹图景，“画”出了景美人和的美丽乡村新画卷", "news_prompt10": "同时，定期到各村指导做好“美丽庭院”的摸底、宣传、示范户的建设工作，并将庭院建设与村风家风相融合，赋予庭院更多的文化内涵，助推庭院建设“内外兼修”", "news_prompt11": "人居环境整治是一场攻坚战、持久战，既要短期攻坚看变化，更要长期推进出实效长效", "news_prompt12": "五华明确提出，至2025年，全县80%以上村庄要达到“美丽宜居”村标准", "news_prompt13": "在此过程中，突出以“百千万工程”为统领，以“美丽五华·和美乡村”为主题，坚持全方位实施，打造宜居宜业和美乡村的五华样板"}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"五华各镇村迅速行动，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面，干群齐心共建美丽家园，持续提升宜居品质": {"topic": "“房地产”", "similarity": 0.5316509008407593, "prompt": "新闻文本是“五华各镇村迅速行动，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面，干群齐心共建美丽家园，持续提升宜居品质”，包含的情绪词典是：建设性的/有益的(constructive):0.4,居民/住户(resident):0.0"}, "按照有关部署要求，五华县将人居环境整治工作视为一场硬仗，集中人力物力推动整治工作重点攻坚，推动“百千万工程”迈上新台阶": {"topic": "“生产投资”", "similarity": 0.5064556002616882, "prompt": "新闻文本是“按照有关部署要求，五华县将人居环境整治工作视为一场硬仗，集中人力物力推动整治工作重点攻坚，推动“百千万工程”迈上新台阶”，包含的情绪词典是：居民/住户(resident):0.0,人工地/人造地(artificially):-0.1"}, "●南方日报记者汪思婷 　　干群动起来 　　网格化织密整治网络 　　“我们将环境整治分组包干，定点到户，全体镇村干部职工分为九大攻坚组，组织党员群众、志愿者、保洁员和群众等多方力量参与": {"topic": "“消费”", "similarity": 0.4850171208381653, "prompt": "新闻文本是“●南方日报记者汪思婷 　　干群动起来 　　网格化织密整治网络 　　“我们将环境整治分组包干，定点到户，全体镇村干部职工分为九大攻坚组，组织党员群众、志愿者、保洁员和群众等多方力量参与”，包含的情绪词典是：团体/群体(group):0.0,净的/纯的(net):0.0"}, "自8月13日五华县“百县千镇万村高质量发展工程”指挥部印发《五华县开展农村人居环境整治和农房风貌提升攻坚行动工作方案》（下称《方案》）以来，五华各镇村迅速行动，全面组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面": {"topic": "“房地产”", "similarity": 0.5059940218925476}, "在人居环境整治方面，五华县主要围绕居住环境“干净、整洁、有序、宜居”目标，提出坚持典型引路，以点带面，将示范路段、典型镇村、沿路“六边”（高铁边、高速边、国道边、省道边、县道边、村主干道边）作为重点，按照“县级统筹、镇级主抓、村级落实、群众参与”的原则，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，干群齐心共建美丽家园，持续提升宜居品质": {"topic": "“消费”", "similarity": 0.5276011824607849}, "在长布镇长生村，伴随着挖掘机“轰隆隆”的响声，涉及26户占地1700平方米的危旧祖屋被顺利拆除，村容村貌瞬间焕然一新": {"topic": "“生产投资”", "similarity": 0.45063987374305725, "prompt": "新闻文本是“在长布镇长生村，伴随着挖掘机“轰隆隆”的响声，涉及26户占地1700平方米的危旧祖屋被顺利拆除，村容村貌瞬间焕然一新”，包含的情绪词典是：拆除/毁坏(demolition):-0.5,拆除/毁坏(demolishes):-0.7"}, "当前，长布镇“三清三拆三整治”攻坚行动正在进行，在全镇村干部带动下，党群合力深入推进百千万群众干“百千万工程”，出资出力，做好农村人居环境整治工作": {"topic": "“生产投资”", "similarity": 0.5317630767822266, "prompt": "新闻文本是“当前，长布镇“三清三拆三整治”攻坚行动正在进行，在全镇村干部带动下，党群合力深入推进百千万群众干“百千万工程”，出资出力，做好农村人居环境整治工作”，包含的情绪词典是：拆除/毁坏(demolish):-0.7,拆除/毁坏(demolishes):-0.7"}, "据介绍，五华县各镇紧紧聚焦典型镇圩镇、典型村为中心，连接到镇政府、高速路口、圩镇、主干道等路线，并摸清县城建成区主干道、示范路线沿线，以典型镇、典型村为中心连接到镇政府、高速路口、圩镇、主干道等的路线可视范围以及典型镇圩镇、典型村区域内、面上镇、面上村“六边”的人居环境整治“三拆除”问题，全力推进农村人居环境整治": {"topic": "“消费”", "similarity": 0.5049054622650146}, "环境美起来 　　注重长期推进显实效 　　“很漂亮，整个村都像穿上了新衣裳一样，赏心悦目": {"topic": "“生产投资”", "similarity": 0.4716074466705322, "prompt": "新闻文本是“环境美起来 　　注重长期推进显实效 　　“很漂亮，整个村都像穿上了新衣裳一样，赏心悦目”，包含的情绪词典是：美丽的/漂亮的(beautiful):0.7,美丽地/漂亮地(beautifully):0.7"}, "近日，河东镇邀请广东工程职业技术学院广东青年大学生“百千万工程”突击队到太和村开展特色墙绘活动，进一步掀起百千万群众干“百千万工程”热潮": {"topic": "“生产投资”", "similarity": 0.45976677536964417, "prompt": "新闻文本是“近日，河东镇邀请广东工程职业技术学院广东青年大学生“百千万工程”突击队到太和村开展特色墙绘活动，进一步掀起百千万群众干“百千万工程”热潮”，包含的情绪词典是：项目/工程(project):0.0,绘制/吸引(draw):0.0"}, "“为更好展示当地特色，我们先对当地进行实地调研，在确定社会主义核心价值观、乡村振兴、‘百千万工程’等主题后，把丝苗米元素融入到墙绘中": {"topic": "“生产投资”", "similarity": 0.4725487530231476, "prompt": "新闻文本是““为更好展示当地特色，我们先对当地进行实地调研，在确定社会主义核心价值观、乡村振兴、‘百千万工程’等主题后，把丝苗米元素融入到墙绘中”，包含的情绪词典是：独特的/有特色的(distinctive):0.0,独特地/有特色地(distinctively):0.0"}, "绘画现场，突击队员们夜以继日，手持画笔、以墙为纸、观景入画，满怀激情地投入到创作中，从刷漆打底到定位起稿，再从填色勾边到最后刷罩面漆，圆满完成了2米高、21米长和1.5米高、20米长的两处大面积墙绘，“绘”出了百千万群众干“百千万工程”的热闹图景，“画”出了景美人和的美丽乡村新画卷": {"topic": "“生产投资”", "similarity": 0.5024532675743103, "prompt": "新闻文本是“绘画现场，突击队员们夜以继日，手持画笔、以墙为纸、观景入画，满怀激情地投入到创作中，从刷漆打底到定位起稿，再从填色勾边到最后刷罩面漆，圆满完成了2米高、21米长和1.5米高、20米长的两处大面积墙绘，“绘”出了百千万群众干“百千万工程”的热闹图景，“画”出了景美人和的美丽乡村新画卷”，包含的情绪词典是：绘制/吸引(draw):0.0,图片/描绘(picture):0.0"}, "同时，定期到各村指导做好“美丽庭院”的摸底、宣传、示范户的建设工作，并将庭院建设与村风家风相融合，赋予庭院更多的文化内涵，助推庭院建设“内外兼修”": {"topic": "“生产投资”", "similarity": 0.4332965612411499, "prompt": "新闻文本是“同时，定期到各村指导做好“美丽庭院”的摸底、宣传、示范户的建设工作，并将庭院建设与村风家风相融合，赋予庭院更多的文化内涵，助推庭院建设“内外兼修””，包含的情绪词典是：建设性的/有益的(constructive):0.4,建设性地/有益地(constructively):0.3"}, "人居环境整治是一场攻坚战、持久战，既要短期攻坚看变化，更要长期推进出实效长效": {"topic": "“房地产”", "similarity": 0.4964410662651062, "prompt": "新闻文本是“人居环境整治是一场攻坚战、持久战，既要短期攻坚看变化，更要长期推进出实效长效”，包含的情绪词典是：居民/住户(resident):0.0,持久的/永久的(abiding):0.1"}, "五华明确提出，至2025年，全县80%以上村庄要达到“美丽宜居”村标准": {"topic": "“生产投资”", "similarity": 0.4422730803489685, "prompt": "新闻文本是“五华明确提出，至2025年，全县80%以上村庄要达到“美丽宜居”村标准”，包含的情绪词典是：美丽的/漂亮的(beautiful):0.7,居民/住户(resident):0.0"}, "在此过程中，突出以“百千万工程”为统领，以“美丽五华·和美乡村”为主题，坚持全方位实施，打造宜居宜业和美乡村的五华样板": {"topic": "“生产投资”", "similarity": 0.5416193008422852, "prompt": "新闻文本是“在此过程中，突出以“百千万工程”为统领，以“美丽五华·和美乡村”为主题，坚持全方位实施，打造宜居宜业和美乡村的五华样板”，包含的情绪词典是：项目/工程(project):0.0,计划/方案(programme):0.0"}}</t>
+          <t>{"五华各镇村迅速行动，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面，干群齐心共建美丽家园，持续提升宜居品质": {"topic": "“房地产”", "similarity": 0.531650960445404, "prompt": "新闻文本是“五华各镇村迅速行动，全面推进“三清三拆”“六乱整治”“三线整治”等人居环境整治工作，组织发动社会各方力量积极参与，大力营造共谋共建、共管共享的良好局面，干群齐心共建美丽家园，持续提升宜居品质”，包含的情绪词典是：建设性的/有益的(constructive):0.4,居民/住户(resident):0.0"}, "按照有关部署要求，五华县将人居环境整治工作视为一场硬仗，集中人力物力推动整治工作重点攻坚，推动“百千万工程”迈上新台阶": {"topic": "“生产投资”", "similarity": 0.5064556002616882, "prompt": "新闻文本是“按照有关部署要求，五华县将人居环境整治工作视为一场硬仗，集中人力物力推动整治工作重点攻坚，推动“百千万工程”迈上新台阶”，包含的情绪词典是：居民/住户(resident):0.0,人工地/人造地(artificially):-0.1"}, "●南方日报记者汪思婷 　　干群动起来 　　网格化织密整治网络 　　“我们将环境整治分组包干，定点到户，全体镇村干部职工分为九大攻坚组，组织党员群众、志愿者、保洁员和群众等多方力量参与": {"topic": "“消费”", "similarity": 0.48501724004745483, "prompt": "新闻文本是“●南方日报记者汪思婷 　　干群动起来 　　网格化织密整治网络 　　“我们将环境整治分组包干，定点到户，全体镇村干部职工分为九大攻坚组，组织党员群众、志愿者、保洁员和群众等多方力量参与”，包含的情绪词典是：团体/群体(group):0.0,净的/纯的(net):0.0"}, "在长布镇长生村，伴随着挖掘机“轰隆隆”的响声，涉及26户占地1700平方米的危旧祖屋被顺利拆除，村容村貌瞬间焕然一新": {"topic": "“生产投资”", "similarity": 0.45063984394073486, "prompt": "新闻文本是“在长布镇长生村，伴随着挖掘机“轰隆隆”的响声，涉及26户占地1700平方米的危旧祖屋被顺利拆除，村容村貌瞬间焕然一新”，包含的情绪词典是：拆除/毁坏(demolition):-0.5,拆除/毁坏(demolishes):-0.7"}, "当前，长布镇“三清三拆三整治”攻坚行动正在进行，在全镇村干部带动下，党群合力深入推进百千万群众干“百千万工程”，出资出力，做好农村人居环境整治工作": {"topic": "“生产投资”", "similarity": 0.5317631959915161, "prompt": "新闻文本是“当前，长布镇“三清三拆三整治”攻坚行动正在进行，在全镇村干部带动下，党群合力深入推进百千万群众干“百千万工程”，出资出力，做好农村人居环境整治工作”，包含的情绪词典是：拆除/毁坏(demolish):-0.7,拆除/毁坏(demolishes):-0.7"}, "环境美起来 　　注重长期推进显实效 　　“很漂亮，整个村都像穿上了新衣裳一样，赏心悦目": {"topic": "“生产投资”", "similarity": 0.471607506275177, "prompt": "新闻文本是“环境美起来 　　注重长期推进显实效 　　“很漂亮，整个村都像穿上了新衣裳一样，赏心悦目”，包含的情绪词典是：美丽的/漂亮的(beautiful):0.7,美丽地/漂亮地(beautifully):0.7"}, "近日，河东镇邀请广东工程职业技术学院广东青年大学生“百千万工程”突击队到太和村开展特色墙绘活动，进一步掀起百千万群众干“百千万工程”热潮": {"topic": "“生产投资”", "similarity": 0.45976680517196655, "prompt": "新闻文本是“近日，河东镇邀请广东工程职业技术学院广东青年大学生“百千万工程”突击队到太和村开展特色墙绘活动，进一步掀起百千万群众干“百千万工程”热潮”，包含的情绪词典是：项目/工程(project):0.0,绘制/吸引(draw):0.0"}, "“为更好展示当地特色，我们先对当地进行实地调研，在确定社会主义核心价值观、乡村振兴、‘百千万工程’等主题后，把丝苗米元素融入到墙绘中": {"topic": "“生产投资”", "similarity": 0.4725487232208252, "prompt": "新闻文本是““为更好展示当地特色，我们先对当地进行实地调研，在确定社会主义核心价值观、乡村振兴、‘百千万工程’等主题后，把丝苗米元素融入到墙绘中”，包含的情绪词典是：独特的/有特色的(distinctive):0.0,独特地/有特色地(distinctively):0.0"}, "绘画现场，突击队员们夜以继日，手持画笔、以墙为纸、观景入画，满怀激情地投入到创作中，从刷漆打底到定位起稿，再从填色勾边到最后刷罩面漆，圆满完成了2米高、21米长和1.5米高、20米长的两处大面积墙绘，“绘”出了百千万群众干“百千万工程”的热闹图景，“画”出了景美人和的美丽乡村新画卷": {"topic": "“生产投资”", "similarity": 0.5024532675743103, "prompt": "新闻文本是“绘画现场，突击队员们夜以继日，手持画笔、以墙为纸、观景入画，满怀激情地投入到创作中，从刷漆打底到定位起稿，再从填色勾边到最后刷罩面漆，圆满完成了2米高、21米长和1.5米高、20米长的两处大面积墙绘，“绘”出了百千万群众干“百千万工程”的热闹图景，“画”出了景美人和的美丽乡村新画卷”，包含的情绪词典是：绘制/吸引(draw):0.0,图片/描绘(picture):0.0"}, "同时，定期到各村指导做好“美丽庭院”的摸底、宣传、示范户的建设工作，并将庭院建设与村风家风相融合，赋予庭院更多的文化内涵，助推庭院建设“内外兼修”": {"topic": "“生产投资”", "similarity": 0.4332965910434723, "prompt": "新闻文本是“同时，定期到各村指导做好“美丽庭院”的摸底、宣传、示范户的建设工作，并将庭院建设与村风家风相融合，赋予庭院更多的文化内涵，助推庭院建设“内外兼修””，包含的情绪词典是：建设性的/有益的(constructive):0.4,建设性地/有益地(constructively):0.3"}, "人居环境整治是一场攻坚战、持久战，既要短期攻坚看变化，更要长期推进出实效长效": {"topic": "“房地产”", "similarity": 0.49644118547439575, "prompt": "新闻文本是“人居环境整治是一场攻坚战、持久战，既要短期攻坚看变化，更要长期推进出实效长效”，包含的情绪词典是：居民/住户(resident):0.0,持久的/永久的(abiding):0.1"}, "五华明确提出，至2025年，全县80%以上村庄要达到“美丽宜居”村标准": {"topic": "“生产投资”", "similarity": 0.4422731101512909, "prompt": "新闻文本是“五华明确提出，至2025年，全县80%以上村庄要达到“美丽宜居”村标准”，包含的情绪词典是：美丽的/漂亮的(beautiful):0.7,居民/住户(resident):0.0"}, "在此过程中，突出以“百千万工程”为统领，以“美丽五华·和美乡村”为主题，坚持全方位实施，打造宜居宜业和美乡村的五华样板": {"topic": "“生产投资”", "similarity": 0.5416193008422852, "prompt": "新闻文本是“在此过程中，突出以“百千万工程”为统领，以“美丽五华·和美乡村”为主题，坚持全方位实施，打造宜居宜业和美乡村的五华样板”，包含的情绪词典是：项目/工程(project):0.0,计划/方案(programme):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -736,12 +728,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081）在2024年8月29日召开的第七届董事会第八次会议和第七届监事会第八次会议上，审议并通过了关于2024年半年度计提资产减值准备的议案", "news_prompt2": "根据公告，公司及下属子公司对截至2024年6月30日的资产进行了全面清查和评估，计提了总额为13,228.88万元的资产减值准备，占2023年度归属于上市公司股东净利润的12.92%", "news_prompt3": "此次计提主要涉及应收账款、应收票据、其他应收款、存货等资产，其中应收账款减值损失为13,413.53万元，占减值准备总额的大部分", "news_prompt4": "计提资产减值准备后，预计将减少公司2024年半年度归属于上市公司所有者的净利润11,244.55万元，并对公司所有者权益产生相应影响", "news_prompt5": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "根据公告，公司及下属子公司对截至2024年6月30日的资产进行了全面清查和评估，计提了总额为13,228.88万元的资产减值准备，占2023年度归属于上市公司股东净利润的12.92%", "news_prompt2": "此次计提主要涉及应收账款、应收票据、其他应收款、存货等资产，其中应收账款减值损失为13,413.53万元，占减值准备总额的大部分", "news_prompt3": "计提资产减值准备后，预计将减少公司2024年半年度归属于上市公司所有者的净利润11,244.55万元，并对公司所有者权益产生相应影响"}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081）在2024年8月29日召开的第七届董事会第八次会议和第七届监事会第八次会议上，审议并通过了关于2024年半年度计提资产减值准备的议案": {"topic": "“金融”", "similarity": 0.49797970056533813}, "根据公告，公司及下属子公司对截至2024年6月30日的资产进行了全面清查和评估，计提了总额为13,228.88万元的资产减值准备，占2023年度归属于上市公司股东净利润的12.92%": {"topic": "“金融”", "similarity": 0.4782968759536743, "prompt": "新闻文本是“根据公告，公司及下属子公司对截至2024年6月30日的资产进行了全面清查和评估，计提了总额为13,228.88万元的资产减值准备，占2023年度归属于上市公司股东净利润的12.92%”，包含的情绪词典是：减记/减值(writedown):-0.1,贬值/减值(devaluation):-0.5"}, "此次计提主要涉及应收账款、应收票据、其他应收款、存货等资产，其中应收账款减值损失为13,413.53万元，占减值准备总额的大部分": {"topic": "“金融”", "similarity": 0.4680666923522949, "prompt": "新闻文本是“此次计提主要涉及应收账款、应收票据、其他应收款、存货等资产，其中应收账款减值损失为13,413.53万元，占减值准备总额的大部分”，包含的情绪词典是：减记/减值(writedown):-0.1,损失/亏损(loss):-0.7"}, "计提资产减值准备后，预计将减少公司2024年半年度归属于上市公司所有者的净利润11,244.55万元，并对公司所有者权益产生相应影响": {"topic": "“金融”", "similarity": 0.4414622485637665, "prompt": "新闻文本是“计提资产减值准备后，预计将减少公司2024年半年度归属于上市公司所有者的净利润11,244.55万元，并对公司所有者权益产生相应影响”，包含的情绪词典是：减记/减值(writedown):-0.1,使贬值/使减值(devalue):-0.4"}}</t>
+          <t>{"根据公告，公司及下属子公司对截至2024年6月30日的资产进行了全面清查和评估，计提了总额为13,228.88万元的资产减值准备，占2023年度归属于上市公司股东净利润的12.92%": {"topic": "“金融”", "similarity": 0.4782969355583191, "prompt": "新闻文本是“根据公告，公司及下属子公司对截至2024年6月30日的资产进行了全面清查和评估，计提了总额为13,228.88万元的资产减值准备，占2023年度归属于上市公司股东净利润的12.92%”，包含的情绪词典是：减记/减值(writedown):-0.1,贬值/减值(devaluation):-0.5"}, "此次计提主要涉及应收账款、应收票据、其他应收款、存货等资产，其中应收账款减值损失为13,413.53万元，占减值准备总额的大部分": {"topic": "“金融”", "similarity": 0.46806684136390686, "prompt": "新闻文本是“此次计提主要涉及应收账款、应收票据、其他应收款、存货等资产，其中应收账款减值损失为13,413.53万元，占减值准备总额的大部分”，包含的情绪词典是：减记/减值(writedown):-0.1,损失/亏损(loss):-0.7"}, "计提资产减值准备后，预计将减少公司2024年半年度归属于上市公司所有者的净利润11,244.55万元，并对公司所有者权益产生相应影响": {"topic": "“金融”", "similarity": 0.44146230816841125, "prompt": "新闻文本是“计提资产减值准备后，预计将减少公司2024年半年度归属于上市公司所有者的净利润11,244.55万元，并对公司所有者权益产生相应影响”，包含的情绪词典是：减记/减值(writedown):-0.1,使贬值/使减值(devalue):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -787,12 +779,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "日前，兴业银行(A股代码：601166.SH)发布半年报并披露兴业信托上半年经营数据显示，截至报告期末，兴业信托总资产678.21亿元，所有者权益212.13亿元", "news_prompt2": "报告期内兴业信托实现营业收入8.30亿元，净利润-5.97亿元", "news_prompt3": "截至报告期末，兴业信托管理资产规模2796.54亿元，较上年末增长51%", "news_prompt4": "存续信托业务规模2727.10亿元，其中，主动管理信托业务存续规模1695.15亿元，占比62.16%", "news_prompt5": "公开资料显示，兴业信托成立于2003年3月，注册资本100亿元，为兴业银行控股子公司，兴业银行持股比例为73%", "news_prompt6": "兴业信托经营范围包括资金信托、动产信托、不动产信托、有价证券信托、其他财产或财产权信托，以及法律法规规定或监管部门批准的其他业务", "news_prompt7": "（文章来源：中国网财经）"}</t>
+          <t>{"news_prompt1": "报告期内兴业信托实现营业收入8.30亿元，净利润-5.97亿元", "news_prompt2": "截至报告期末，兴业信托管理资产规模2796.54亿元，较上年末增长51%", "news_prompt3": "存续信托业务规模2727.10亿元，其中，主动管理信托业务存续规模1695.15亿元，占比62.16%", "news_prompt4": "公开资料显示，兴业信托成立于2003年3月，注册资本100亿元，为兴业银行控股子公司，兴业银行持股比例为73%", "news_prompt5": "兴业信托经营范围包括资金信托、动产信托、不动产信托、有价证券信托、其他财产或财产权信托，以及法律法规规定或监管部门批准的其他业务"}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"日前，兴业银行(A股代码：601166.SH)发布半年报并披露兴业信托上半年经营数据显示，截至报告期末，兴业信托总资产678.21亿元，所有者权益212.13亿元": {"topic": "“金融”", "similarity": 0.5997973680496216}, "报告期内兴业信托实现营业收入8.30亿元，净利润-5.97亿元": {"topic": "“金融”", "similarity": 0.5114030241966248, "prompt": "新闻文本是“报告期内兴业信托实现营业收入8.30亿元，净利润-5.97亿元”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "截至报告期末，兴业信托管理资产规模2796.54亿元，较上年末增长51%": {"topic": "“金融”", "similarity": 0.45802247524261475, "prompt": "新闻文本是“截至报告期末，兴业信托管理资产规模2796.54亿元，较上年末增长51%”，包含的情绪词典是：资产/财产(asset):0.3,投资/投资额(investment):0.4"}, "存续信托业务规模2727.10亿元，其中，主动管理信托业务存续规模1695.15亿元，占比62.16%": {"topic": "“金融”", "similarity": 0.5351318120956421, "prompt": "新闻文本是“存续信托业务规模2727.10亿元，其中，主动管理信托业务存续规模1695.15亿元，占比62.16%”，包含的情绪词典是：被托管的/被提存的(escrowed):0.0,托管/提存(escrow):0.0"}, "公开资料显示，兴业信托成立于2003年3月，注册资本100亿元，为兴业银行控股子公司，兴业银行持股比例为73%": {"topic": "“金融”", "similarity": 0.6286134719848633, "prompt": "新闻文本是“公开资料显示，兴业信托成立于2003年3月，注册资本100亿元，为兴业银行控股子公司，兴业银行持股比例为73%”，包含的情绪词典是：受托人/保管人(bailee):0.0"}, "兴业信托经营范围包括资金信托、动产信托、不动产信托、有价证券信托、其他财产或财产权信托，以及法律法规规定或监管部门批准的其他业务": {"topic": "“金融”", "similarity": 0.6068205833435059, "prompt": "新闻文本是“兴业信托经营范围包括资金信托、动产信托、不动产信托、有价证券信托、其他财产或财产权信托，以及法律法规规定或监管部门批准的其他业务”，包含的情绪词典是：资产/财产(asset):0.3,动产/财物(chattel):0.0"}, "（文章来源：中国网财经）": {"topic": "“生产投资”", "similarity": 0.44495803117752075, "prompt": "新闻文本是“（文章来源：中国网财经）”，包含的情绪词典是：金融/财政(finance):0.0,金融的/财政的(financial):0.0"}}</t>
+          <t>{"报告期内兴业信托实现营业收入8.30亿元，净利润-5.97亿元": {"topic": "“金融”", "similarity": 0.5114032030105591, "prompt": "新闻文本是“报告期内兴业信托实现营业收入8.30亿元，净利润-5.97亿元”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "截至报告期末，兴业信托管理资产规模2796.54亿元，较上年末增长51%": {"topic": "“金融”", "similarity": 0.4580225944519043, "prompt": "新闻文本是“截至报告期末，兴业信托管理资产规模2796.54亿元，较上年末增长51%”，包含的情绪词典是：资产/财产(asset):0.3,投资/投资额(investment):0.4"}, "存续信托业务规模2727.10亿元，其中，主动管理信托业务存续规模1695.15亿元，占比62.16%": {"topic": "“金融”", "similarity": 0.5351319313049316, "prompt": "新闻文本是“存续信托业务规模2727.10亿元，其中，主动管理信托业务存续规模1695.15亿元，占比62.16%”，包含的情绪词典是：被托管的/被提存的(escrowed):0.0,托管/提存(escrow):0.0"}, "公开资料显示，兴业信托成立于2003年3月，注册资本100亿元，为兴业银行控股子公司，兴业银行持股比例为73%": {"topic": "“金融”", "similarity": 0.6286135911941528, "prompt": "新闻文本是“公开资料显示，兴业信托成立于2003年3月，注册资本100亿元，为兴业银行控股子公司，兴业银行持股比例为73%”，包含的情绪词典是：受托人/保管人(bailee):0.0"}, "兴业信托经营范围包括资金信托、动产信托、不动产信托、有价证券信托、其他财产或财产权信托，以及法律法规规定或监管部门批准的其他业务": {"topic": "“金融”", "similarity": 0.606820821762085, "prompt": "新闻文本是“兴业信托经营范围包括资金信托、动产信托、不动产信托、有价证券信托、其他财产或财产权信托，以及法律法规规定或监管部门批准的其他业务”，包含的情绪词典是：资产/财产(asset):0.3,动产/财物(chattel):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -838,12 +830,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "主要产品连续六个季度增长", "news_prompt2": "裕太微跨过行业低谷以太网芯片未来市场潜力显现　　随着半导体行业周期性收尾，市场需求持续复苏，高速有线通信芯片领域龙头企业裕太微上半年销售收入实现爆发", "news_prompt3": "裕太微发布的2024年上半年度财报显示，公司报告期内实现营业收入15,467.65 万元，较上年同期增长42.61%", "news_prompt4": "裕太微表示，今年公司下游客户需求有所增长，同时公司近年推出的2.5G网通以太网物理层芯片等新产品经下游用户陆续验证导入，销售放量增长，使得本期营业收入较上年同期增长", "news_prompt5": "就行业应用而言，5G网络、数据中心、工业互联网等新型基础设施建设进度加快，数据资源将与人工智能技术耦合发展，不断催生新产业、新模式、新业态，生成新的经济增长点", "news_prompt6": "以太网作为信息网络底层的支持性技术，也将随着半导体产业周期步入上行区间、产业应用持续创新，而迎来新的发展机遇期", "news_prompt7": "跨过行业低谷实现连续六个季度营收增长　　在裕太微强研发战略的引导下，公司已经顺利迈过行业下行周期，整体营收向好发展", "news_prompt8": "财报显示，除2024年上半年整体营收同比增长42.61%外，公司营收端还有诸多亮点，意味着公司已成功跨过高研发和产业周期的低谷，将顺利进入下一轮成长期", "news_prompt9": "在2023年至今年上半年的连续6个季度中，裕太微实现主要产品收入的逐季上涨", "news_prompt10": "其中在2024年一季度，裕太微主要产品收入实现7105.36万元，同比增长80.08%，环比增长6.18%", "news_prompt11": "2024年第二季度，裕太微主要产品收入实现8204.02万元，同比增长64.32%，环比增长15.46%", "news_prompt12": "2.5G网通以太网物理层芯片为裕太微战略产品项目之一，2024年上半年的销售收入超过去年全年", "news_prompt13": "2023年单口2.5G网通以太网物理层芯片实现营收2085.92万元，2024年上半年该产品实现营收3870.94万元，较之去年全年营收增长85.57%", "news_prompt14": "2024年第一季度，中国移动和中国电信均已发布家庭网关产品集采的通知，集采中将用到2.5G网通以太网物理层芯片，这也将为裕太微今年整体的单口2.5G网通以太网物理层芯片的销售带来较大增量", "news_prompt15": "不仅如此，在2024年上半年，裕太微此前发布的7大新品营收合计为5883.62万元，较去年全年增幅达到32.45%", "news_prompt16": "值得关注的是，裕太微千兆车载以太网物理层芯片于2023年年底提前问世，较之百兆车载以太网物理层芯片的整体测试验证和定点周期大大缩减", "news_prompt17": "今年作为千兆车载以太网物理层芯片的量产元年，上半年裕太微该产品已成功实现销售，在整体汽车智能化和网联化加深的推动下，更多的车企正在导入国产车载以太网产品系列，后续公司该类产品的营收将进一步走强", "news_prompt18": "芯片设计企业高研发投入期和收获期普遍存在一定的时间错配", "news_prompt19": "裕太微研发投入产品线已拓展到7条，按照其发展战略规划，其第二轮研发投入期已于2023年收尾，并在2023年下半年开始逐步进入收获期", "news_prompt20": "目前，裕太微已进入第三轮研发投入期，并预计在2024年底或2025年开始看到本轮投入的回报", "news_prompt21": "裕太微表示，第三轮次的研发投入金额较大，研发投入周期较长，研发产品难度系数大幅提升", "news_prompt22": "该轮次核心研发投入为补充2.5G系列网通产品、24口及以下网通交换机芯片、5G/10G 网通以太网物理层芯片、车载以太网交换机芯片、车载高速视频传输芯片、车载网关芯片", "news_prompt23": "这一系列产品将陆续于2024年到2026年量产出货，为后续的营收份额的提升做出贡献", "news_prompt24": "财报显示，裕太微当前整体的研发进展迅速、研发与市场导入衔接节奏紧密", "news_prompt25": "目前裕太微自主研发的3款新品，包括4口2.5G网通以太网物理层芯片、16口网通以太网交换机芯片和24口网通以太网交换机芯片已经完成初步研发，预计将于2024年年底推出量产样片", "news_prompt26": "另外，还有1款新品车载以太网交换机芯片也在加紧研发中，预计将于2025年年初问世，问世时间较之预期提前了大半年，实现较大突破", "news_prompt27": "今年上半年，裕太微研发费用为13,456.50 万元，同比增长37.00%", "news_prompt28": "研发费用占当期营业收入比例达到87.00%", "news_prompt29": "随着裕太微新品持续推出并走向中高端领域、市场渗透不断加深、应用场景接续扩大，公司的核心竞争力也将在更大的蓝海中日渐凸显", "news_prompt30": "以太网技术迎来新机遇多场景需求将突破成长　　以太网技术作为先进数字产业的创新底座支持，当前正迎来新的发展机遇", "news_prompt31": "随着5G网络、数据中心、工业互联网等新型基础设施建设进度加速，新基建以信息网络为基础，面向高质量发展需要，提供数字转型、智能升级、融合创新等服务的基础设施体系，为以太网芯片的发展提供了强大动能", "news_prompt32": "《中国互联网发展报告（2024）》 提出，数字技术创新将逐步推动互联网向智能化迈进，算法、算力与数据的核心作用将更加凸显，而算力发展需求推动高端芯片自主研发和制造能力不断提升", "news_prompt33": "在通信行业，上半年电信业务量持续稳步增长", "news_prompt34": "通信行业的新"}</t>
+          <t>{"news_prompt1": "主要产品连续六个季度增长", "news_prompt2": "裕太微跨过行业低谷以太网芯片未来市场潜力显现　　随着半导体行业周期性收尾，市场需求持续复苏，高速有线通信芯片领域龙头企业裕太微上半年销售收入实现爆发", "news_prompt3": "裕太微表示，今年公司下游客户需求有所增长，同时公司近年推出的2.5G网通以太网物理层芯片等新产品经下游用户陆续验证导入，销售放量增长，使得本期营业收入较上年同期增长", "news_prompt4": "就行业应用而言，5G网络、数据中心、工业互联网等新型基础设施建设进度加快，数据资源将与人工智能技术耦合发展，不断催生新产业、新模式、新业态，生成新的经济增长点", "news_prompt5": "以太网作为信息网络底层的支持性技术，也将随着半导体产业周期步入上行区间、产业应用持续创新，而迎来新的发展机遇期", "news_prompt6": "跨过行业低谷实现连续六个季度营收增长　　在裕太微强研发战略的引导下，公司已经顺利迈过行业下行周期，整体营收向好发展", "news_prompt7": "财报显示，除2024年上半年整体营收同比增长42.61%外，公司营收端还有诸多亮点，意味着公司已成功跨过高研发和产业周期的低谷，将顺利进入下一轮成长期", "news_prompt8": "其中在2024年一季度，裕太微主要产品收入实现7105.36万元，同比增长80.08%，环比增长6.18%", "news_prompt9": "值得关注的是，裕太微千兆车载以太网物理层芯片于2023年年底提前问世，较之百兆车载以太网物理层芯片的整体测试验证和定点周期大大缩减", "news_prompt10": "芯片设计企业高研发投入期和收获期普遍存在一定的时间错配", "news_prompt11": "目前，裕太微已进入第三轮研发投入期，并预计在2024年底或2025年开始看到本轮投入的回报", "news_prompt12": "裕太微表示，第三轮次的研发投入金额较大，研发投入周期较长，研发产品难度系数大幅提升", "news_prompt13": "该轮次核心研发投入为补充2.5G系列网通产品、24口及以下网通交换机芯片、5G/10G 网通以太网物理层芯片、车载以太网交换机芯片、车载高速视频传输芯片、车载网关芯片", "news_prompt14": "这一系列产品将陆续于2024年到2026年量产出货，为后续的营收份额的提升做出贡献", "news_prompt15": "另外，还有1款新品车载以太网交换机芯片也在加紧研发中，预计将于2025年年初问世，问世时间较之预期提前了大半年，实现较大突破", "news_prompt16": "今年上半年，裕太微研发费用为13,456.50 万元，同比增长37.00%", "news_prompt17": "研发费用占当期营业收入比例达到87.00%", "news_prompt18": "随着裕太微新品持续推出并走向中高端领域、市场渗透不断加深、应用场景接续扩大，公司的核心竞争力也将在更大的蓝海中日渐凸显", "news_prompt19": "以太网技术迎来新机遇多场景需求将突破成长　　以太网技术作为先进数字产业的创新底座支持，当前正迎来新的发展机遇", "news_prompt20": "随着5G网络、数据中心、工业互联网等新型基础设施建设进度加速，新基建以信息网络为基础，面向高质量发展需要，提供数字转型、智能升级、融合创新等服务的基础设施体系，为以太网芯片的发展提供了强大动能", "news_prompt21": "《中国互联网发展报告（2024）》 提出，数字技术创新将逐步推动互联网向智能化迈进，算法、算力与数据的核心作用将更加凸显，而算力发展需求推动高端芯片自主研发和制造能力不断提升", "news_prompt22": "在通信行业，上半年电信业务量持续稳步增长", "news_prompt23": "通信行业的新"}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"主要产品连续六个季度增长": {"topic": "“生产投资”", "similarity": 0.4323791265487671, "prompt": "新闻文本是“主要产品连续六个季度增长”，包含的情绪词典是：增长/发展(growth):0.7,产品/产物(product):0.15"}, "裕太微跨过行业低谷以太网芯片未来市场潜力显现　　随着半导体行业周期性收尾，市场需求持续复苏，高速有线通信芯片领域龙头企业裕太微上半年销售收入实现爆发": {"topic": "“生产投资”", "similarity": 0.5408048033714294, "prompt": "新闻文本是“裕太微跨过行业低谷以太网芯片未来市场潜力显现　　随着半导体行业周期性收尾，市场需求持续复苏，高速有线通信芯片领域龙头企业裕太微上半年销售收入实现爆发”，包含的情绪词典是：潜在的/潜力(potential):0.3,有利可图的/盈利的(profitable):0.8"}, "裕太微发布的2024年上半年度财报显示，公司报告期内实现营业收入15,467.65 万元，较上年同期增长42.61%": {"topic": "“宏观经济”", "similarity": 0.4999121129512787}, "裕太微表示，今年公司下游客户需求有所增长，同时公司近年推出的2.5G网通以太网物理层芯片等新产品经下游用户陆续验证导入，销售放量增长，使得本期营业收入较上年同期增长": {"topic": "“生产投资”", "similarity": 0.5455929636955261, "prompt": "新闻文本是“裕太微表示，今年公司下游客户需求有所增长，同时公司近年推出的2.5G网通以太网物理层芯片等新产品经下游用户陆续验证导入，销售放量增长，使得本期营业收入较上年同期增长”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "就行业应用而言，5G网络、数据中心、工业互联网等新型基础设施建设进度加快，数据资源将与人工智能技术耦合发展，不断催生新产业、新模式、新业态，生成新的经济增长点": {"topic": "“生产投资”", "similarity": 0.7250816822052002, "prompt": "新闻文本是“就行业应用而言，5G网络、数据中心、工业互联网等新型基础设施建设进度加快，数据资源将与人工智能技术耦合发展，不断催生新产业、新模式、新业态，生成新的经济增长点”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,增长/发展(growth):0.7"}, "以太网作为信息网络底层的支持性技术，也将随着半导体产业周期步入上行区间、产业应用持续创新，而迎来新的发展机遇期": {"topic": "“生产投资”", "similarity": 0.6224624514579773, "prompt": "新闻文本是“以太网作为信息网络底层的支持性技术，也将随着半导体产业周期步入上行区间、产业应用持续创新，而迎来新的发展机遇期”，包含的情绪词典是：机会/时机(opportunity):0.5,创新的/革新的(innovative):0.7"}, "跨过行业低谷实现连续六个季度营收增长　　在裕太微强研发战略的引导下，公司已经顺利迈过行业下行周期，整体营收向好发展": {"topic": "“宏观经济”", "similarity": 0.5376030206680298, "prompt": "新闻文本是“跨过行业低谷实现连续六个季度营收增长　　在裕太微强研发战略的引导下，公司已经顺利迈过行业下行周期，整体营收向好发展”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,增长/发展(growth):0.7"}, "财报显示，除2024年上半年整体营收同比增长42.61%外，公司营收端还有诸多亮点，意味着公司已成功跨过高研发和产业周期的低谷，将顺利进入下一轮成长期": {"topic": "“生产投资”", "similarity": 0.5458856821060181, "prompt": "新闻文本是“财报显示，除2024年上半年整体营收同比增长42.61%外，公司营收端还有诸多亮点，意味着公司已成功跨过高研发和产业周期的低谷，将顺利进入下一轮成长期”，包含的情绪词典是：增长/发展(growth):0.7,营业额/周转(turnover):0.0"}, "其中在2024年一季度，裕太微主要产品收入实现7105.36万元，同比增长80.08%，环比增长6.18%": {"topic": "“宏观经济”", "similarity": 0.5011640787124634, "prompt": "新闻文本是“其中在2024年一季度，裕太微主要产品收入实现7105.36万元，同比增长80.08%，环比增长6.18%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "2024年第二季度，裕太微主要产品收入实现8204.02万元，同比增长64.32%，环比增长15.46%": {"topic": "“宏观经济”", "similarity": 0.5052940249443054}, "2.5G网通以太网物理层芯片为裕太微战略产品项目之一，2024年上半年的销售收入超过去年全年": {"topic": "“生产投资”", "similarity": 0.5236594676971436}, "2023年单口2.5G网通以太网物理层芯片实现营收2085.92万元，2024年上半年该产品实现营收3870.94万元，较之去年全年营收增长85.57%": {"topic": "“生产投资”", "similarity": 0.544086217880249}, "2024年第一季度，中国移动和中国电信均已发布家庭网关产品集采的通知，集采中将用到2.5G网通以太网物理层芯片，这也将为裕太微今年整体的单口2.5G网通以太网物理层芯片的销售带来较大增量": {"topic": "“生产投资”", "similarity": 0.5276907086372375}, "不仅如此，在2024年上半年，裕太微此前发布的7大新品营收合计为5883.62万元，较去年全年增幅达到32.45%": {"topic": "“消费”", "similarity": 0.507499098777771}, "值得关注的是，裕太微千兆车载以太网物理层芯片于2023年年底提前问世，较之百兆车载以太网物理层芯片的整体测试验证和定点周期大大缩减": {"topic": "“生产投资”", "similarity": 0.5208159685134888, "prompt": "新闻文本是“值得关注的是，裕太微千兆车载以太网物理层芯片于2023年年底提前问世，较之百兆车载以太网物理层芯片的整体测试验证和定点周期大大缩减”，包含的情绪词典是：迟的/晚的(late):-0.3"}, "今年作为千兆车载以太网物理层芯片的量产元年，上半年裕太微该产品已成功实现销售，在整体汽车智能化和网联化加深的推动下，更多的车企正在导入国产车载以太网产品系列，后续公司该类产品的营收将进一步走强": {"topic": "“生产投资”", "similarity": 0.5907258987426758}, "芯片设计企业高研发投入期和收获期普遍存在一定的时间错配": {"topic": "“生产投资”", "similarity": 0.5694518089294434, "prompt": "新闻文本是“芯片设计企业高研发投入期和收获期普遍存在一定的时间错配”，包含的情绪词典是：不匹配/错配(mismatching):-0.3,不匹配的/错配的(mismatched):-0.3"}, "裕太微研发投入产品线已拓展到7条，按照其发展战略规划，其第二轮研发投入期已于2023年收尾，并在2023年下半年开始逐步进入收获期": {"topic": "“生产投资”", "similarity": 0.5363641977310181}, "目前，裕太微已进入第三轮研发投入期，并预计在2024年底或2025年开始看到本轮投入的回报": {"topic": "“生产投资”", "similarity": 0.45102745294570923, "prompt": "新闻文本是“目前，裕太微已进入第三轮研发投入期，并预计在2024年底或2025年开始看到本轮投入的回报”，包含的情绪词典是：正在改善的/正在改进的(improving):0.5,延期偿付/缓期执行(moratorium):0.0"}, "裕太微表示，第三轮次的研发投入金额较大，研发投入周期较长，研发产品难度系数大幅提升": {"topic": "“生产投资”", "similarity": 0.45282918214797974, "prompt": "新闻文本是“裕太微表示，第三轮次的研发投入金额较大，研发投入周期较长，研发产品难度系数大幅提升”，包含的情绪词典是：投资/投资额(investment):0.4,产能过剩(overcapacity):-0.5"}, "该轮次核心研发投入为补充2.5G系列网通产品、24口及以下网通交换机芯片、5G/10G 网通以太网物理层芯片、车载以太网交换机芯片、车载高速视频传输芯片、车载网关芯片": {"topic": "“生产投资”", "similarity": 0.6005163788795471, "prompt": "新闻文本是“该轮次核心研发投入为补充2.5G系列网通产品、24口及以下网通交换机芯片、5G/10G 网通以太网物理层芯片、车载以太网交换机芯片、车载高速视频传输芯片、车载网关芯片”，包含的情绪词典是：汽车/机动车(automobile):0.0,车辆/交通工具(vehicle):0.0"}, "这一系列产品将陆续于2024年到2026年量产出货，为后续的营收份额的提升做出贡献": {"topic": "“生产投资”", "similarity": 0.4734188914299011, "prompt": "新闻文本是“这一系列产品将陆续于2024年到2026年量产出货，为后续的营收份额的提升做出贡献”，包含的情绪词典是：产品/产物(product):0.15,产量/输出(output):0.0"}, "目前裕太微自主研发的3款新品，包括4口2.5G网通以太网物理层芯片、16口网通以太网交换机芯片和24口网通以太网交换机芯片已经完成初步研发，预计将于2024年年底推出量产样片": {"topic": "“生产投资”", "similarity": 0.502643346786499}, "另外，还有1款新品车载以太网交换机芯片也在加紧研发中，预计将于2025年年初问世，问世时间较之预期提前了大半年，实现较大突破": {"topic": "“生产投资”", "similarity": 0.5783023238182068, "prompt": "新闻文本是“另外，还有1款新品车载以太网交换机芯片也在加紧研发中，预计将于2025年年初问世，问世时间较之预期提前了大半年，实现较大突破”，包含的情绪词典是：汽车的/机动车的(automotive):0.0,汽车/机动车(automobile):0.0"}, "今年上半年，裕太微研发费用为13,456.50 万元，同比增长37.00%": {"topic": "“生产投资”", "similarity": 0.4441618025302887, "prompt": "新闻文本是“今年上半年，裕太微研发费用为13,456.50 万元，同比增长37.00%”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "研发费用占当期营业收入比例达到87.00%": {"topic": "“生产投资”", "similarity": 0.42869433760643005, "prompt": "新闻文本是“研发费用占当期营业收入比例达到87.00%”，包含的情绪词典是：百分比(percentage):0.0,发展/开发(development):0.4"}, "随着裕太微新品持续推出并走向中高端领域、市场渗透不断加深、应用场景接续扩大，公司的核心竞争力也将在更大的蓝海中日渐凸显": {"topic": "“消费”", "similarity": 0.5540193319320679, "prompt": "新闻文本是“随着裕太微新品持续推出并走向中高端领域、市场渗透不断加深、应用场景接续扩大，公司的核心竞争力也将在更大的蓝海中日渐凸显”，包含的情绪词典是：增长/发展(growth):0.7,前进/进步(advance):0.6"}, "以太网技术迎来新机遇多场景需求将突破成长　　以太网技术作为先进数字产业的创新底座支持，当前正迎来新的发展机遇": {"topic": "“生产投资”", "similarity": 0.581430196762085, "prompt": "新闻文本是“以太网技术迎来新机遇多场景需求将突破成长　　以太网技术作为先进数字产业的创新底座支持，当前正迎来新的发展机遇”，包含的情绪词典是：突破/重大进展(breakthrough):0.5,机会/时机(opportunity):0.5"}, "随着5G网络、数据中心、工业互联网等新型基础设施建设进度加速，新基建以信息网络为基础，面向高质量发展需要，提供数字转型、智能升级、融合创新等服务的基础设施体系，为以太网芯片的发展提供了强大动能": {"topic": "“生产投资”", "similarity": 0.6464564204216003, "prompt": "新闻文本是“随着5G网络、数据中心、工业互联网等新型基础设施建设进度加速，新基建以信息网络为基础，面向高质量发展需要，提供数字转型、智能升级、融合创新等服务的基础设施体系，为以太网芯片的发展提供了强大动能”，包含的情绪词典是：进步/进展(progresses):0.6,进步/进展(progress):0.6"}, "《中国互联网发展报告（2024）》 提出，数字技术创新将逐步推动互联网向智能化迈进，算法、算力与数据的核心作用将更加凸显，而算力发展需求推动高端芯片自主研发和制造能力不断提升": {"topic": "“生产投资”", "similarity": 0.6837671995162964, "prompt": "新闻文本是“《中国互联网发展报告（2024）》 提出，数字技术创新将逐步推动互联网向智能化迈进，算法、算力与数据的核心作用将更加凸显，而算力发展需求推动高端芯片自主研发和制造能力不断提升”，包含的情绪词典是：数字的/数码的(digital):0.0,正在改善的/正在改进的(improving):0.5"}, "在通信行业，上半年电信业务量持续稳步增长": {"topic": "“消费”", "similarity": 0.45660877227783203, "prompt": "新闻文本是“在通信行业，上半年电信业务量持续稳步增长”，包含的情绪词典是：稳定/稳定性(stability):0.6,增长/发展(growth):0.7"}, "通信行业的新": {"topic": "“生产投资”", "similarity": 0.5078346133232117, "prompt": "新闻文本是“通信行业的新”，包含的情绪词典是：电子的(electronic):0.0,新的/新鲜的(new):0.0"}}</t>
+          <t>{"主要产品连续六个季度增长": {"topic": "“生产投资”", "similarity": 0.4323791563510895, "prompt": "新闻文本是“主要产品连续六个季度增长”，包含的情绪词典是：增长/发展(growth):0.7,产品/产物(product):0.15"}, "裕太微跨过行业低谷以太网芯片未来市场潜力显现　　随着半导体行业周期性收尾，市场需求持续复苏，高速有线通信芯片领域龙头企业裕太微上半年销售收入实现爆发": {"topic": "“生产投资”", "similarity": 0.5408048629760742, "prompt": "新闻文本是“裕太微跨过行业低谷以太网芯片未来市场潜力显现　　随着半导体行业周期性收尾，市场需求持续复苏，高速有线通信芯片领域龙头企业裕太微上半年销售收入实现爆发”，包含的情绪词典是：潜在的/潜力(potential):0.3,有利可图的/盈利的(profitable):0.8"}, "裕太微表示，今年公司下游客户需求有所增长，同时公司近年推出的2.5G网通以太网物理层芯片等新产品经下游用户陆续验证导入，销售放量增长，使得本期营业收入较上年同期增长": {"topic": "“生产投资”", "similarity": 0.5455930233001709, "prompt": "新闻文本是“裕太微表示，今年公司下游客户需求有所增长，同时公司近年推出的2.5G网通以太网物理层芯片等新产品经下游用户陆续验证导入，销售放量增长，使得本期营业收入较上年同期增长”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "就行业应用而言，5G网络、数据中心、工业互联网等新型基础设施建设进度加快，数据资源将与人工智能技术耦合发展，不断催生新产业、新模式、新业态，生成新的经济增长点": {"topic": "“生产投资”", "similarity": 0.7250815629959106, "prompt": "新闻文本是“就行业应用而言，5G网络、数据中心、工业互联网等新型基础设施建设进度加快，数据资源将与人工智能技术耦合发展，不断催生新产业、新模式、新业态，生成新的经济增长点”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,增长/发展(growth):0.7"}, "以太网作为信息网络底层的支持性技术，也将随着半导体产业周期步入上行区间、产业应用持续创新，而迎来新的发展机遇期": {"topic": "“生产投资”", "similarity": 0.6224623918533325, "prompt": "新闻文本是“以太网作为信息网络底层的支持性技术，也将随着半导体产业周期步入上行区间、产业应用持续创新，而迎来新的发展机遇期”，包含的情绪词典是：机会/时机(opportunity):0.5,创新的/革新的(innovative):0.7"}, "跨过行业低谷实现连续六个季度营收增长　　在裕太微强研发战略的引导下，公司已经顺利迈过行业下行周期，整体营收向好发展": {"topic": "“宏观经济”", "similarity": 0.5376031398773193, "prompt": "新闻文本是“跨过行业低谷实现连续六个季度营收增长　　在裕太微强研发战略的引导下，公司已经顺利迈过行业下行周期，整体营收向好发展”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,增长/发展(growth):0.7"}, "财报显示，除2024年上半年整体营收同比增长42.61%外，公司营收端还有诸多亮点，意味着公司已成功跨过高研发和产业周期的低谷，将顺利进入下一轮成长期": {"topic": "“生产投资”", "similarity": 0.5458858013153076, "prompt": "新闻文本是“财报显示，除2024年上半年整体营收同比增长42.61%外，公司营收端还有诸多亮点，意味着公司已成功跨过高研发和产业周期的低谷，将顺利进入下一轮成长期”，包含的情绪词典是：增长/发展(growth):0.7,营业额/周转(turnover):0.0"}, "其中在2024年一季度，裕太微主要产品收入实现7105.36万元，同比增长80.08%，环比增长6.18%": {"topic": "“宏观经济”", "similarity": 0.5011642575263977, "prompt": "新闻文本是“其中在2024年一季度，裕太微主要产品收入实现7105.36万元，同比增长80.08%，环比增长6.18%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "值得关注的是，裕太微千兆车载以太网物理层芯片于2023年年底提前问世，较之百兆车载以太网物理层芯片的整体测试验证和定点周期大大缩减": {"topic": "“生产投资”", "similarity": 0.5208160877227783, "prompt": "新闻文本是“值得关注的是，裕太微千兆车载以太网物理层芯片于2023年年底提前问世，较之百兆车载以太网物理层芯片的整体测试验证和定点周期大大缩减”，包含的情绪词典是：迟的/晚的(late):-0.3"}, "芯片设计企业高研发投入期和收获期普遍存在一定的时间错配": {"topic": "“生产投资”", "similarity": 0.5694519281387329, "prompt": "新闻文本是“芯片设计企业高研发投入期和收获期普遍存在一定的时间错配”，包含的情绪词典是：不匹配/错配(mismatching):-0.3,不匹配的/错配的(mismatched):-0.3"}, "目前，裕太微已进入第三轮研发投入期，并预计在2024年底或2025年开始看到本轮投入的回报": {"topic": "“生产投资”", "similarity": 0.45102766156196594, "prompt": "新闻文本是“目前，裕太微已进入第三轮研发投入期，并预计在2024年底或2025年开始看到本轮投入的回报”，包含的情绪词典是：正在改善的/正在改进的(improving):0.5,延期偿付/缓期执行(moratorium):0.0"}, "裕太微表示，第三轮次的研发投入金额较大，研发投入周期较长，研发产品难度系数大幅提升": {"topic": "“生产投资”", "similarity": 0.45282939076423645, "prompt": "新闻文本是“裕太微表示，第三轮次的研发投入金额较大，研发投入周期较长，研发产品难度系数大幅提升”，包含的情绪词典是：投资/投资额(investment):0.4,产能过剩(overcapacity):-0.5"}, "该轮次核心研发投入为补充2.5G系列网通产品、24口及以下网通交换机芯片、5G/10G 网通以太网物理层芯片、车载以太网交换机芯片、车载高速视频传输芯片、车载网关芯片": {"topic": "“生产投资”", "similarity": 0.6005165576934814, "prompt": "新闻文本是“该轮次核心研发投入为补充2.5G系列网通产品、24口及以下网通交换机芯片、5G/10G 网通以太网物理层芯片、车载以太网交换机芯片、车载高速视频传输芯片、车载网关芯片”，包含的情绪词典是：汽车/机动车(automobile):0.0,车辆/交通工具(vehicle):0.0"}, "这一系列产品将陆续于2024年到2026年量产出货，为后续的营收份额的提升做出贡献": {"topic": "“生产投资”", "similarity": 0.4734188914299011, "prompt": "新闻文本是“这一系列产品将陆续于2024年到2026年量产出货，为后续的营收份额的提升做出贡献”，包含的情绪词典是：产品/产物(product):0.15,产量/输出(output):0.0"}, "另外，还有1款新品车载以太网交换机芯片也在加紧研发中，预计将于2025年年初问世，问世时间较之预期提前了大半年，实现较大突破": {"topic": "“生产投资”", "similarity": 0.5783025622367859, "prompt": "新闻文本是“另外，还有1款新品车载以太网交换机芯片也在加紧研发中，预计将于2025年年初问世，问世时间较之预期提前了大半年，实现较大突破”，包含的情绪词典是：汽车的/机动车的(automotive):0.0,汽车/机动车(automobile):0.0"}, "今年上半年，裕太微研发费用为13,456.50 万元，同比增长37.00%": {"topic": "“生产投资”", "similarity": 0.44416192173957825, "prompt": "新闻文本是“今年上半年，裕太微研发费用为13,456.50 万元，同比增长37.00%”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "研发费用占当期营业收入比例达到87.00%": {"topic": "“生产投资”", "similarity": 0.42869430780410767, "prompt": "新闻文本是“研发费用占当期营业收入比例达到87.00%”，包含的情绪词典是：百分比(percentage):0.0,发展/开发(development):0.4"}, "随着裕太微新品持续推出并走向中高端领域、市场渗透不断加深、应用场景接续扩大，公司的核心竞争力也将在更大的蓝海中日渐凸显": {"topic": "“消费”", "similarity": 0.5540194511413574, "prompt": "新闻文本是“随着裕太微新品持续推出并走向中高端领域、市场渗透不断加深、应用场景接续扩大，公司的核心竞争力也将在更大的蓝海中日渐凸显”，包含的情绪词典是：增长/发展(growth):0.7,前进/进步(advance):0.6"}, "以太网技术迎来新机遇多场景需求将突破成长　　以太网技术作为先进数字产业的创新底座支持，当前正迎来新的发展机遇": {"topic": "“生产投资”", "similarity": 0.5814303159713745, "prompt": "新闻文本是“以太网技术迎来新机遇多场景需求将突破成长　　以太网技术作为先进数字产业的创新底座支持，当前正迎来新的发展机遇”，包含的情绪词典是：突破/重大进展(breakthrough):0.5,机会/时机(opportunity):0.5"}, "随着5G网络、数据中心、工业互联网等新型基础设施建设进度加速，新基建以信息网络为基础，面向高质量发展需要，提供数字转型、智能升级、融合创新等服务的基础设施体系，为以太网芯片的发展提供了强大动能": {"topic": "“生产投资”", "similarity": 0.6464565992355347, "prompt": "新闻文本是“随着5G网络、数据中心、工业互联网等新型基础设施建设进度加速，新基建以信息网络为基础，面向高质量发展需要，提供数字转型、智能升级、融合创新等服务的基础设施体系，为以太网芯片的发展提供了强大动能”，包含的情绪词典是：进步/进展(progresses):0.6,进步/进展(progress):0.6"}, "《中国互联网发展报告（2024）》 提出，数字技术创新将逐步推动互联网向智能化迈进，算法、算力与数据的核心作用将更加凸显，而算力发展需求推动高端芯片自主研发和制造能力不断提升": {"topic": "“生产投资”", "similarity": 0.6837673187255859, "prompt": "新闻文本是“《中国互联网发展报告（2024）》 提出，数字技术创新将逐步推动互联网向智能化迈进，算法、算力与数据的核心作用将更加凸显，而算力发展需求推动高端芯片自主研发和制造能力不断提升”，包含的情绪词典是：数字的/数码的(digital):0.0,正在改善的/正在改进的(improving):0.5"}, "在通信行业，上半年电信业务量持续稳步增长": {"topic": "“消费”", "similarity": 0.45660877227783203, "prompt": "新闻文本是“在通信行业，上半年电信业务量持续稳步增长”，包含的情绪词典是：稳定/稳定性(stability):0.6,增长/发展(growth):0.7"}, "通信行业的新": {"topic": "“生产投资”", "similarity": 0.5078346133232117, "prompt": "新闻文本是“通信行业的新”，包含的情绪词典是：电子的(electronic):0.0,新的/新鲜的(new):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -889,12 +881,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日上午，中船系概念震荡走低，中国船舶跌超6%，中船防务跌超5%，中国动力、中国重工、中船科技、久之洋等跟跌", "news_prompt2": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "9月2日上午，中船系概念震荡走低，中国船舶跌超6%，中船防务跌超5%，中国动力、中国重工、中船科技、久之洋等跟跌"}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"9月2日上午，中船系概念震荡走低，中国船舶跌超6%，中船防务跌超5%，中国动力、中国重工、中船科技、久之洋等跟跌": {"topic": "“金融”", "similarity": 0.558018684387207, "prompt": "新闻文本是“9月2日上午，中船系概念震荡走低，中国船舶跌超6%，中船防务跌超5%，中国动力、中国重工、中船科技、久之洋等跟跌”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退的/不景气的(recessionary):-0.8"}}</t>
+          <t>{"9月2日上午，中船系概念震荡走低，中国船舶跌超6%，中船防务跌超5%，中国动力、中国重工、中船科技、久之洋等跟跌": {"topic": "“金融”", "similarity": 0.5580189228057861, "prompt": "新闻文本是“9月2日上午，中船系概念震荡走低，中国船舶跌超6%，中船防务跌超5%，中国动力、中国重工、中船科技、久之洋等跟跌”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退的/不景气的(recessionary):-0.8"}}</t>
         </is>
       </c>
     </row>
@@ -940,12 +932,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，天微电子(688511.SH)发布2024年中报", "news_prompt2": "公司营业总收入为4483.52万元，在已披露的同业公司中排名第61，较去年同报告期营业总收入减少2033.50万元，同比较去年同期下降31.20%", "news_prompt3": "归母净利润为138.87万元，在已披露的同业公司中排名第37，较去年同报告期归母净利润减少2614.28万元，同比较去年同期下降94.96%", "news_prompt4": "经营活动现金净流入为948.43万元，在已披露的同业公司中排名第15，较去年同报告期经营活动现金净流入增加710.09万元，同比较去年同期上涨297.92%", "news_prompt5": "公司最新资产负债率为10.14%，在已披露的同业公司中排名第7，较上季度资产负债率减少0.46个百分点，较去年同季度资产负债率增加0.69个百分点", "news_prompt6": "公司最新毛利率为63.69%，在已披露的同业公司中排名第5，较上季度毛利率增加0.16个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.50个百分点", "news_prompt7": "最新ROE为0.16%，在已披露的同业公司中排名第36，较去年同季度ROE减少3.19个百分点", "news_prompt8": "公司摊薄每股收益为0.02元，在已披露的同业公司中排名第33，较去年同报告期摊薄每股收益减少0.33元，同比较去年同期下降94.94%", "news_prompt9": "公司最新总资产周转率为0.05次，在已披露的同业公司中排名第51，较去年同季度总资产周转率减少0.03次，同比较去年同期下降36.25%", "news_prompt10": "最新存货周转率为0.18次，在已披露的同业公司中排名第53，较去年同季度存货周转率减少0.11次，同比较去年同期下降37.52%", "news_prompt11": "公司股东户数为6236户，前十大股东持股数量为4922.18万股，占总股本比例为61.53%", "news_prompt12": "前十大股东分别为巨万里、张超、巨万珍、石敬、成都爱航私募基金管理有限公司-成都盈创德弘航空创业投资合伙企业(有限合伙)、中金公司-招商银行-中金公司天微电子1号员工参与科创板战略配售集合资产管理计划、南京皓海越信息技术咨询中心(有限合伙)、丁丑生、中国建设银行股份有限公司-长信国防军工量化灵活配置混合型证券投资基金、陈建，持股比例分别为43.08%、6.24%、5.47%、1.87%、1.00%、0.94%、0.82%、0.78%、0.72%、0.61%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为4483.52万元，在已披露的同业公司中排名第61，较去年同报告期营业总收入减少2033.50万元，同比较去年同期下降31.20%", "news_prompt2": "归母净利润为138.87万元，在已披露的同业公司中排名第37，较去年同报告期归母净利润减少2614.28万元，同比较去年同期下降94.96%", "news_prompt3": "经营活动现金净流入为948.43万元，在已披露的同业公司中排名第15，较去年同报告期经营活动现金净流入增加710.09万元，同比较去年同期上涨297.92%", "news_prompt4": "公司最新资产负债率为10.14%，在已披露的同业公司中排名第7，较上季度资产负债率减少0.46个百分点，较去年同季度资产负债率增加0.69个百分点", "news_prompt5": "公司最新毛利率为63.69%，在已披露的同业公司中排名第5，较上季度毛利率增加0.16个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.50个百分点", "news_prompt6": "公司摊薄每股收益为0.02元，在已披露的同业公司中排名第33，较去年同报告期摊薄每股收益减少0.33元，同比较去年同期下降94.94%", "news_prompt7": "公司最新总资产周转率为0.05次，在已披露的同业公司中排名第51，较去年同季度总资产周转率减少0.03次，同比较去年同期下降36.25%", "news_prompt8": "最新存货周转率为0.18次，在已披露的同业公司中排名第53，较去年同季度存货周转率减少0.11次，同比较去年同期下降37.52%", "news_prompt9": "公司股东户数为6236户，前十大股东持股数量为4922.18万股，占总股本比例为61.53%"}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，天微电子(688511.SH)发布2024年中报": {"topic": "“生产投资”", "similarity": 0.517818033695221, "prompt": "新闻文本是“2024年8月31日，天微电子(688511.SH)发布2024年中报”，包含的情绪词典是：电子的(electronic):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司营业总收入为4483.52万元，在已披露的同业公司中排名第61，较去年同报告期营业总收入减少2033.50万元，同比较去年同期下降31.20%": {"topic": "“消费”", "similarity": 0.5161714553833008, "prompt": "新闻文本是“公司营业总收入为4483.52万元，在已披露的同业公司中排名第61，较去年同报告期营业总收入减少2033.50万元，同比较去年同期下降31.20%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "归母净利润为138.87万元，在已披露的同业公司中排名第37，较去年同报告期归母净利润减少2614.28万元，同比较去年同期下降94.96%": {"topic": "“消费”", "similarity": 0.49962174892425537, "prompt": "新闻文本是“归母净利润为138.87万元，在已披露的同业公司中排名第37，较去年同报告期归母净利润减少2614.28万元，同比较去年同期下降94.96%”，包含的情绪词典是：减少/降低(reduction):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为948.43万元，在已披露的同业公司中排名第15，较去年同报告期经营活动现金净流入增加710.09万元，同比较去年同期上涨297.92%": {"topic": "“金融”", "similarity": 0.5483537316322327, "prompt": "新闻文本是“经营活动现金净流入为948.43万元，在已披露的同业公司中排名第15，较去年同报告期经营活动现金净流入增加710.09万元，同比较去年同期上涨297.92%”，包含的情绪词典是：营业额/周转(turnover):0.0,利润/利益(profit):0.8"}, "公司最新资产负债率为10.14%，在已披露的同业公司中排名第7，较上季度资产负债率减少0.46个百分点，较去年同季度资产负债率增加0.69个百分点": {"topic": "“消费”", "similarity": 0.46907609701156616, "prompt": "新闻文本是“公司最新资产负债率为10.14%，在已披露的同业公司中排名第7，较上季度资产负债率减少0.46个百分点，较去年同季度资产负债率增加0.69个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,表现不佳/业绩低于预期(underperform):-0.4"}, "公司最新毛利率为63.69%，在已披露的同业公司中排名第5，较上季度毛利率增加0.16个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.50个百分点": {"topic": "“消费”", "similarity": 0.45496705174446106, "prompt": "新闻文本是“公司最新毛利率为63.69%，在已披露的同业公司中排名第5，较上季度毛利率增加0.16个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.50个百分点”，包含的情绪词典是：百分比(percentage):0.0,盈利能力/获利能力(profitability):0.6"}, "公司摊薄每股收益为0.02元，在已披露的同业公司中排名第33，较去年同报告期摊薄每股收益减少0.33元，同比较去年同期下降94.94%": {"topic": "“金融”", "similarity": 0.4690268039703369, "prompt": "新闻文本是“公司摊薄每股收益为0.02元，在已披露的同业公司中排名第33，较去年同报告期摊薄每股收益减少0.33元，同比较去年同期下降94.94%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "公司最新总资产周转率为0.05次，在已披露的同业公司中排名第51，较去年同季度总资产周转率减少0.03次，同比较去年同期下降36.25%": {"topic": "“消费”", "similarity": 0.4941653907299042, "prompt": "新闻文本是“公司最新总资产周转率为0.05次，在已披露的同业公司中排名第51，较去年同季度总资产周转率减少0.03次，同比较去年同期下降36.25%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "最新存货周转率为0.18次，在已披露的同业公司中排名第53，较去年同季度存货周转率减少0.11次，同比较去年同期下降37.52%": {"topic": "“消费”", "similarity": 0.442441463470459, "prompt": "新闻文本是“最新存货周转率为0.18次，在已披露的同业公司中排名第53，较去年同季度存货周转率减少0.11次，同比较去年同期下降37.52%”，包含的情绪词典是：营业额/周转(turnover):0.0,周期/循环(cycle):0.0"}, "公司股东户数为6236户，前十大股东持股数量为4922.18万股，占总股本比例为61.53%": {"topic": "“金融”", "similarity": 0.48282313346862793, "prompt": "新闻文本是“公司股东户数为6236户，前十大股东持股数量为4922.18万股，占总股本比例为61.53%”，包含的情绪词典是：百分比(percentage):0.0,公司的/企业的(corporate):0.0"}, "前十大股东分别为巨万里、张超、巨万珍、石敬、成都爱航私募基金管理有限公司-成都盈创德弘航空创业投资合伙企业(有限合伙)、中金公司-招商银行-中金公司天微电子1号员工参与科创板战略配售集合资产管理计划、南京皓海越信息技术咨询中心(有限合伙)、丁丑生、中国建设银行股份有限公司-长信国防军工量化灵活配置混合型证券投资基金、陈建，持股比例分别为43.08%、6.24%、5.47%、1.87%、1.00%、0.94%、0.82%、0.78%、0.72%、0.61%": {"topic": "“生产投资”", "similarity": 0.6453565359115601}}</t>
+          <t>{"公司营业总收入为4483.52万元，在已披露的同业公司中排名第61，较去年同报告期营业总收入减少2033.50万元，同比较去年同期下降31.20%": {"topic": "“消费”", "similarity": 0.5161714553833008, "prompt": "新闻文本是“公司营业总收入为4483.52万元，在已披露的同业公司中排名第61，较去年同报告期营业总收入减少2033.50万元，同比较去年同期下降31.20%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "归母净利润为138.87万元，在已披露的同业公司中排名第37，较去年同报告期归母净利润减少2614.28万元，同比较去年同期下降94.96%": {"topic": "“消费”", "similarity": 0.49962174892425537, "prompt": "新闻文本是“归母净利润为138.87万元，在已披露的同业公司中排名第37，较去年同报告期归母净利润减少2614.28万元，同比较去年同期下降94.96%”，包含的情绪词典是：减少/降低(reduction):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为948.43万元，在已披露的同业公司中排名第15，较去年同报告期经营活动现金净流入增加710.09万元，同比较去年同期上涨297.92%": {"topic": "“金融”", "similarity": 0.5483537912368774, "prompt": "新闻文本是“经营活动现金净流入为948.43万元，在已披露的同业公司中排名第15，较去年同报告期经营活动现金净流入增加710.09万元，同比较去年同期上涨297.92%”，包含的情绪词典是：营业额/周转(turnover):0.0,利润/利益(profit):0.8"}, "公司最新资产负债率为10.14%，在已披露的同业公司中排名第7，较上季度资产负债率减少0.46个百分点，较去年同季度资产负债率增加0.69个百分点": {"topic": "“消费”", "similarity": 0.46907612681388855, "prompt": "新闻文本是“公司最新资产负债率为10.14%，在已披露的同业公司中排名第7，较上季度资产负债率减少0.46个百分点，较去年同季度资产负债率增加0.69个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,表现不佳/业绩低于预期(underperform):-0.4"}, "公司最新毛利率为63.69%，在已披露的同业公司中排名第5，较上季度毛利率增加0.16个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.50个百分点": {"topic": "“消费”", "similarity": 0.4549671709537506, "prompt": "新闻文本是“公司最新毛利率为63.69%，在已披露的同业公司中排名第5，较上季度毛利率增加0.16个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.50个百分点”，包含的情绪词典是：百分比(percentage):0.0,盈利能力/获利能力(profitability):0.6"}, "公司摊薄每股收益为0.02元，在已披露的同业公司中排名第33，较去年同报告期摊薄每股收益减少0.33元，同比较去年同期下降94.94%": {"topic": "“金融”", "similarity": 0.46902701258659363, "prompt": "新闻文本是“公司摊薄每股收益为0.02元，在已披露的同业公司中排名第33，较去年同报告期摊薄每股收益减少0.33元，同比较去年同期下降94.94%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "公司最新总资产周转率为0.05次，在已披露的同业公司中排名第51，较去年同季度总资产周转率减少0.03次，同比较去年同期下降36.25%": {"topic": "“消费”", "similarity": 0.4941655397415161, "prompt": "新闻文本是“公司最新总资产周转率为0.05次，在已披露的同业公司中排名第51，较去年同季度总资产周转率减少0.03次，同比较去年同期下降36.25%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "最新存货周转率为0.18次，在已披露的同业公司中排名第53，较去年同季度存货周转率减少0.11次，同比较去年同期下降37.52%": {"topic": "“消费”", "similarity": 0.44244155287742615, "prompt": "新闻文本是“最新存货周转率为0.18次，在已披露的同业公司中排名第53，较去年同季度存货周转率减少0.11次，同比较去年同期下降37.52%”，包含的情绪词典是：营业额/周转(turnover):0.0,周期/循环(cycle):0.0"}, "公司股东户数为6236户，前十大股东持股数量为4922.18万股，占总股本比例为61.53%": {"topic": "“金融”", "similarity": 0.48282334208488464, "prompt": "新闻文本是“公司股东户数为6236户，前十大股东持股数量为4922.18万股，占总股本比例为61.53%”，包含的情绪词典是：百分比(percentage):0.0,公司的/企业的(corporate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -991,12 +983,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上周公布的美国经济数据令投资者更加乐观看待美国经济“软着陆”的前景，市场同时预计美联储9月会小幅降息，美股板块轮动持续，三大股指上周涨跌不一，但是整体波动幅度都不太大", "news_prompt2": "而回顾刚刚过去的8月，美国三大股指全月集体累计上涨，主要得益于美联储释放的明确降息信号", "news_prompt3": "其中道指上涨1.76%，标普500指数上涨2.28%，纳指涨0.66%", "news_prompt4": "8月美油期价累计跌超5% 国际金价上涨超2% 　　大宗商品方面，上周美油期价下跌1.71%，布油期价跌0.28%", "news_prompt5": "回顾整个8月，国际能源署和多家华尔街投行的报告均预计，原油市场未来短期可能出现供应过剩的局面，引发油价震荡下行", "news_prompt6": "美油期价下跌5.60%，布油期价下跌2.38%", "news_prompt7": "而国际金价则在美联储降息预期的助推下，全月累计上涨2.21%", "news_prompt8": "本周美国8月非农就业数据受关注将影响美联储本月利率决议 　　本周一美股因传统节假日休市一天，在其余的时间里，市场将首先聚焦美国就业数据", "news_prompt9": "本周五，美国劳工统计局将发布8月非农就业数据，这也是9月美联储决议前最后一份重磅就业数据，可能将成为美联储决定降息25还是50个基点的关键，因为在通胀压力已经明显缓解的背景下，眼下美联储更关注的是就业市场的健康状况", "news_prompt10": "目前市场普遍预计，美国8月新增非农就业人数为16.5万人，较此前一个月的11.4万明显增加，失业率可能小幅下降，显示出美国就业市场仍具韧性", "news_prompt11": "本周美联储经济状况褐皮书将出炉  　　此外，本周四美联储将公布最新一期的经济状况褐皮书，从中投资者可以更全面了解到美国各个地区的经济现状", "news_prompt12": "以上这些数据都将给本月中旬到来的美联储利率决议提供更多参考", "news_prompt13": "美联储观察的数据显示，目前市场认为美联储届时降息25个基点的概率约为70%", "news_prompt14": "本周德国柏林国际消费电子展将开幕展会迎来第100周年 　　欧洲市场方面，2024年德国柏林国际消费电子展，也就是IFA将于本周五开幕，作为全球最大的消费电子展之一，IFA因其更聚焦家用以及发布的新品能更快抵达消费者而备注关注", "news_prompt15": "特别要提到的是今年是IFA成立的第一百周年，展会期间也将有众多科技企业带着最新产品亮相", "news_prompt16": "本周法国、德国的8月PMI终值数据将陆续出炉", "news_prompt17": "加拿大央行还将公布最新的利率决议", "news_prompt18": "（文章来源：央视财经）"}</t>
+          <t>{"news_prompt1": "上周公布的美国经济数据令投资者更加乐观看待美国经济“软着陆”的前景，市场同时预计美联储9月会小幅降息，美股板块轮动持续，三大股指上周涨跌不一，但是整体波动幅度都不太大", "news_prompt2": "而回顾刚刚过去的8月，美国三大股指全月集体累计上涨，主要得益于美联储释放的明确降息信号", "news_prompt3": "8月美油期价累计跌超5% 国际金价上涨超2% 　　大宗商品方面，上周美油期价下跌1.71%，布油期价跌0.28%", "news_prompt4": "回顾整个8月，国际能源署和多家华尔街投行的报告均预计，原油市场未来短期可能出现供应过剩的局面，引发油价震荡下行", "news_prompt5": "本周美国8月非农就业数据受关注将影响美联储本月利率决议 　　本周一美股因传统节假日休市一天，在其余的时间里，市场将首先聚焦美国就业数据", "news_prompt6": "本周五，美国劳工统计局将发布8月非农就业数据，这也是9月美联储决议前最后一份重磅就业数据，可能将成为美联储决定降息25还是50个基点的关键，因为在通胀压力已经明显缓解的背景下，眼下美联储更关注的是就业市场的健康状况", "news_prompt7": "目前市场普遍预计，美国8月新增非农就业人数为16.5万人，较此前一个月的11.4万明显增加，失业率可能小幅下降，显示出美国就业市场仍具韧性", "news_prompt8": "本周美联储经济状况褐皮书将出炉  　　此外，本周四美联储将公布最新一期的经济状况褐皮书，从中投资者可以更全面了解到美国各个地区的经济现状", "news_prompt9": "以上这些数据都将给本月中旬到来的美联储利率决议提供更多参考", "news_prompt10": "特别要提到的是今年是IFA成立的第一百周年，展会期间也将有众多科技企业带着最新产品亮相", "news_prompt11": "本周法国、德国的8月PMI终值数据将陆续出炉", "news_prompt12": "加拿大央行还将公布最新的利率决议"}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"上周公布的美国经济数据令投资者更加乐观看待美国经济“软着陆”的前景，市场同时预计美联储9月会小幅降息，美股板块轮动持续，三大股指上周涨跌不一，但是整体波动幅度都不太大": {"topic": "“金融”", "similarity": 0.6803925633430481, "prompt": "新闻文本是“上周公布的美国经济数据令投资者更加乐观看待美国经济“软着陆”的前景，市场同时预计美联储9月会小幅降息，美股板块轮动持续，三大股指上周涨跌不一，但是整体波动幅度都不太大”，包含的情绪词典是：乐观的/看好的(optimistic):0.7,好转/向上趋势(upturn):0.4"}, "而回顾刚刚过去的8月，美国三大股指全月集体累计上涨，主要得益于美联储释放的明确降息信号": {"topic": "“金融”", "similarity": 0.45306187868118286, "prompt": "新闻文本是“而回顾刚刚过去的8月，美国三大股指全月集体累计上涨，主要得益于美联储释放的明确降息信号”，包含的情绪词典是：上升/上涨(rise):0.5,反弹/回升(rebound):0.1"}, "8月美油期价累计跌超5% 国际金价上涨超2% 　　大宗商品方面，上周美油期价下跌1.71%，布油期价跌0.28%": {"topic": "“通货膨胀”", "similarity": 0.5039295554161072, "prompt": "新闻文本是“8月美油期价累计跌超5% 国际金价上涨超2% 　　大宗商品方面，上周美油期价下跌1.71%，布油期价跌0.28%”，包含的情绪词典是：石油/油类(oil):0.0,下跌/下降(fall):-0.6"}, "回顾整个8月，国际能源署和多家华尔街投行的报告均预计，原油市场未来短期可能出现供应过剩的局面，引发油价震荡下行": {"topic": "“通货膨胀”", "similarity": 0.49689000844955444, "prompt": "新闻文本是“回顾整个8月，国际能源署和多家华尔街投行的报告均预计，原油市场未来短期可能出现供应过剩的局面，引发油价震荡下行”，包含的情绪词典是：供应过剩(oversupply):-0.2,供应过剩的(oversupplied):-0.3"}, "本周美国8月非农就业数据受关注将影响美联储本月利率决议 　　本周一美股因传统节假日休市一天，在其余的时间里，市场将首先聚焦美国就业数据": {"topic": "“金融”", "similarity": 0.5655388236045837, "prompt": "新闻文本是“本周美国8月非农就业数据受关注将影响美联储本月利率决议 　　本周一美股因传统节假日休市一天，在其余的时间里，市场将首先聚焦美国就业数据”，包含的情绪词典是：失业/失业率(unemployment):-0.7,失业的/无工作的(unemployed):-0.8"}, "本周五，美国劳工统计局将发布8月非农就业数据，这也是9月美联储决议前最后一份重磅就业数据，可能将成为美联储决定降息25还是50个基点的关键，因为在通胀压力已经明显缓解的背景下，眼下美联储更关注的是就业市场的健康状况": {"topic": "“宏观经济”", "similarity": 0.6157585382461548, "prompt": "新闻文本是“本周五，美国劳工统计局将发布8月非农就业数据，这也是9月美联储决议前最后一份重磅就业数据，可能将成为美联储决定降息25还是50个基点的关键，因为在通胀压力已经明显缓解的背景下，眼下美联储更关注的是就业市场的健康状况”，包含的情绪词典是：失业/失业率(unemployment):-0.7,裁员/下岗(layoff):-0.7"}, "目前市场普遍预计，美国8月新增非农就业人数为16.5万人，较此前一个月的11.4万明显增加，失业率可能小幅下降，显示出美国就业市场仍具韧性": {"topic": "“宏观经济”", "similarity": 0.5472025871276855, "prompt": "新闻文本是“目前市场普遍预计，美国8月新增非农就业人数为16.5万人，较此前一个月的11.4万明显增加，失业率可能小幅下降，显示出美国就业市场仍具韧性”，包含的情绪词典是：劳动力/职工总数(workforce):0.01,失业/失业率(unemployment):-0.7"}, "本周美联储经济状况褐皮书将出炉  　　此外，本周四美联储将公布最新一期的经济状况褐皮书，从中投资者可以更全面了解到美国各个地区的经济现状": {"topic": "“宏观经济”", "similarity": 0.5466283559799194, "prompt": "新闻文本是“本周美联储经济状况褐皮书将出炉  　　此外，本周四美联储将公布最新一期的经济状况褐皮书，从中投资者可以更全面了解到美国各个地区的经济现状”，包含的情绪词典是：经济/经济体(economy):0.0,经济的/经济学的(economic):0.0"}, "以上这些数据都将给本月中旬到来的美联储利率决议提供更多参考": {"topic": "“宏观经济”", "similarity": 0.46543294191360474, "prompt": "新闻文本是“以上这些数据都将给本月中旬到来的美联储利率决议提供更多参考”，包含的情绪词典是：假定/推测(presuming):0.0,预测性的/预兆的(predictive):0.2"}, "本周德国柏林国际消费电子展将开幕展会迎来第100周年 　　欧洲市场方面，2024年德国柏林国际消费电子展，也就是IFA将于本周五开幕，作为全球最大的消费电子展之一，IFA因其更聚焦家用以及发布的新品能更快抵达消费者而备注关注": {"topic": "“消费”", "similarity": 0.5595207810401917}, "特别要提到的是今年是IFA成立的第一百周年，展会期间也将有众多科技企业带着最新产品亮相": {"topic": "“生产投资”", "similarity": 0.44587385654449463, "prompt": "新闻文本是“特别要提到的是今年是IFA成立的第一百周年，展会期间也将有众多科技企业带着最新产品亮相”，包含的情绪词典是：技术(tech):0.0,展示/表明(show):0.0"}, "本周法国、德国的8月PMI终值数据将陆续出炉": {"topic": "“宏观经济”", "similarity": 0.4952538013458252, "prompt": "新闻文本是“本周法国、德国的8月PMI终值数据将陆续出炉”，包含的情绪词典是：通货紧缩(deflation):-0.6,法国的/法语的(french):0.0"}, "加拿大央行还将公布最新的利率决议": {"topic": "“宏观经济”", "similarity": 0.44129928946495056, "prompt": "新闻文本是“加拿大央行还将公布最新的利率决议”，包含的情绪词典是：比率/率(rate):0.0,通货膨胀(inflation):-0.5"}, "（文章来源：央视财经）": {"topic": "“宏观经济”", "similarity": 0.4717864692211151, "prompt": "新闻文本是“（文章来源：央视财经）”，包含的情绪词典是：金融的/财政的(financial):0.0,金钱/货币(money):0.2"}}</t>
+          <t>{"上周公布的美国经济数据令投资者更加乐观看待美国经济“软着陆”的前景，市场同时预计美联储9月会小幅降息，美股板块轮动持续，三大股指上周涨跌不一，但是整体波动幅度都不太大": {"topic": "“金融”", "similarity": 0.6803927421569824, "prompt": "新闻文本是“上周公布的美国经济数据令投资者更加乐观看待美国经济“软着陆”的前景，市场同时预计美联储9月会小幅降息，美股板块轮动持续，三大股指上周涨跌不一，但是整体波动幅度都不太大”，包含的情绪词典是：乐观的/看好的(optimistic):0.7,好转/向上趋势(upturn):0.4"}, "而回顾刚刚过去的8月，美国三大股指全月集体累计上涨，主要得益于美联储释放的明确降息信号": {"topic": "“金融”", "similarity": 0.4530622363090515, "prompt": "新闻文本是“而回顾刚刚过去的8月，美国三大股指全月集体累计上涨，主要得益于美联储释放的明确降息信号”，包含的情绪词典是：上升/上涨(rise):0.5,反弹/回升(rebound):0.1"}, "8月美油期价累计跌超5% 国际金价上涨超2% 　　大宗商品方面，上周美油期价下跌1.71%，布油期价跌0.28%": {"topic": "“通货膨胀”", "similarity": 0.5039297342300415, "prompt": "新闻文本是“8月美油期价累计跌超5% 国际金价上涨超2% 　　大宗商品方面，上周美油期价下跌1.71%，布油期价跌0.28%”，包含的情绪词典是：石油/油类(oil):0.0,下跌/下降(fall):-0.6"}, "回顾整个8月，国际能源署和多家华尔街投行的报告均预计，原油市场未来短期可能出现供应过剩的局面，引发油价震荡下行": {"topic": "“通货膨胀”", "similarity": 0.49689021706581116, "prompt": "新闻文本是“回顾整个8月，国际能源署和多家华尔街投行的报告均预计，原油市场未来短期可能出现供应过剩的局面，引发油价震荡下行”，包含的情绪词典是：供应过剩(oversupply):-0.2,供应过剩的(oversupplied):-0.3"}, "本周美国8月非农就业数据受关注将影响美联储本月利率决议 　　本周一美股因传统节假日休市一天，在其余的时间里，市场将首先聚焦美国就业数据": {"topic": "“金融”", "similarity": 0.5655389428138733, "prompt": "新闻文本是“本周美国8月非农就业数据受关注将影响美联储本月利率决议 　　本周一美股因传统节假日休市一天，在其余的时间里，市场将首先聚焦美国就业数据”，包含的情绪词典是：失业/失业率(unemployment):-0.7,失业的/无工作的(unemployed):-0.8"}, "本周五，美国劳工统计局将发布8月非农就业数据，这也是9月美联储决议前最后一份重磅就业数据，可能将成为美联储决定降息25还是50个基点的关键，因为在通胀压力已经明显缓解的背景下，眼下美联储更关注的是就业市场的健康状况": {"topic": "“宏观经济”", "similarity": 0.6157586574554443, "prompt": "新闻文本是“本周五，美国劳工统计局将发布8月非农就业数据，这也是9月美联储决议前最后一份重磅就业数据，可能将成为美联储决定降息25还是50个基点的关键，因为在通胀压力已经明显缓解的背景下，眼下美联储更关注的是就业市场的健康状况”，包含的情绪词典是：失业/失业率(unemployment):-0.7,裁员/下岗(layoff):-0.7"}, "目前市场普遍预计，美国8月新增非农就业人数为16.5万人，较此前一个月的11.4万明显增加，失业率可能小幅下降，显示出美国就业市场仍具韧性": {"topic": "“宏观经济”", "similarity": 0.5472027063369751, "prompt": "新闻文本是“目前市场普遍预计，美国8月新增非农就业人数为16.5万人，较此前一个月的11.4万明显增加，失业率可能小幅下降，显示出美国就业市场仍具韧性”，包含的情绪词典是：劳动力/职工总数(workforce):0.01,失业/失业率(unemployment):-0.7"}, "本周美联储经济状况褐皮书将出炉  　　此外，本周四美联储将公布最新一期的经济状况褐皮书，从中投资者可以更全面了解到美国各个地区的经济现状": {"topic": "“宏观经济”", "similarity": 0.546628475189209, "prompt": "新闻文本是“本周美联储经济状况褐皮书将出炉  　　此外，本周四美联储将公布最新一期的经济状况褐皮书，从中投资者可以更全面了解到美国各个地区的经济现状”，包含的情绪词典是：经济/经济体(economy):0.0,经济的/经济学的(economic):0.0"}, "以上这些数据都将给本月中旬到来的美联储利率决议提供更多参考": {"topic": "“宏观经济”", "similarity": 0.46543312072753906, "prompt": "新闻文本是“以上这些数据都将给本月中旬到来的美联储利率决议提供更多参考”，包含的情绪词典是：假定/推测(presuming):0.0,预测性的/预兆的(predictive):0.2"}, "特别要提到的是今年是IFA成立的第一百周年，展会期间也将有众多科技企业带着最新产品亮相": {"topic": "“生产投资”", "similarity": 0.4458741545677185, "prompt": "新闻文本是“特别要提到的是今年是IFA成立的第一百周年，展会期间也将有众多科技企业带着最新产品亮相”，包含的情绪词典是：技术(tech):0.0,展示/表明(show):0.0"}, "本周法国、德国的8月PMI终值数据将陆续出炉": {"topic": "“宏观经济”", "similarity": 0.49525386095046997, "prompt": "新闻文本是“本周法国、德国的8月PMI终值数据将陆续出炉”，包含的情绪词典是：通货紧缩(deflation):-0.6,法国的/法语的(french):0.0"}, "加拿大央行还将公布最新的利率决议": {"topic": "“宏观经济”", "similarity": 0.4412993788719177, "prompt": "新闻文本是“加拿大央行还将公布最新的利率决议”，包含的情绪词典是：比率/率(rate):0.0,通货膨胀(inflation):-0.5"}}</t>
         </is>
       </c>
     </row>
@@ -1042,12 +1034,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日，招商银行行长王良在该行2024年中期业绩交流会上表示：“针对转按揭的政策，我们也是在媒体上看到了这样的信息，但是我们还没有接到宏观管理部门人民银行或者金融总局有这方面的意见，也没有征求过商业银行的意见，所以目前这个政策还没有得到确认，只是一些媒体上的传言", "news_prompt2": "” 　　王良表示，如果这一政策要推出，会对银行业的存量按揭利率带来一定的负面影响，宏观管理部门会做好充分的论证和研究再推出这样的政策", "news_prompt3": "（文章来源：澎湃新闻）"}</t>
+          <t>{"news_prompt1": "” 　　王良表示，如果这一政策要推出，会对银行业的存量按揭利率带来一定的负面影响，宏观管理部门会做好充分的论证和研究再推出这样的政策"}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"9月2日，招商银行行长王良在该行2024年中期业绩交流会上表示：“针对转按揭的政策，我们也是在媒体上看到了这样的信息，但是我们还没有接到宏观管理部门人民银行或者金融总局有这方面的意见，也没有征求过商业银行的意见，所以目前这个政策还没有得到确认，只是一些媒体上的传言": {"topic": "“房地产”", "similarity": 0.6600347757339478}, "” 　　王良表示，如果这一政策要推出，会对银行业的存量按揭利率带来一定的负面影响，宏观管理部门会做好充分的论证和研究再推出这样的政策": {"topic": "“房地产”", "similarity": 0.6310836672782898, "prompt": "新闻文本是“” 　　王良表示，如果这一政策要推出，会对银行业的存量按揭利率带来一定的负面影响，宏观管理部门会做好充分的论证和研究再推出这样的政策”，包含的情绪词典是：高利贷的/高利剥削的(usurious):-0.8,高利贷/高利剥削(usury):-0.7"}}</t>
+          <t>{"” 　　王良表示，如果这一政策要推出，会对银行业的存量按揭利率带来一定的负面影响，宏观管理部门会做好充分的论证和研究再推出这样的政策": {"topic": "“房地产”", "similarity": 0.6310838460922241, "prompt": "新闻文本是“” 　　王良表示，如果这一政策要推出，会对银行业的存量按揭利率带来一定的负面影响，宏观管理部门会做好充分的论证和研究再推出这样的政策”，包含的情绪词典是：高利贷的/高利剥削的(usurious):-0.8,高利贷/高利剥削(usury):-0.7"}}</t>
         </is>
       </c>
     </row>
@@ -1097,12 +1089,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "证券时报网讯，国海证券研报指出，短期来看，铝价仍然偏强，旺季对需求的提升逐步体现，阶段性铝价高位和意外事件不影响去库大趋势", "news_prompt2": "美联储9月降息预期进一步强化，随着旺季到来，下游需求和铝价有望进一步上涨", "news_prompt3": "而短期铝土矿供应仍然紧张，后续几内亚雨季影响或逐步显现，氧化铝价格探涨，仍然是铝价的支撑，一体化经营的公司将明显受益，关注板块投资机会", "news_prompt4": "长期来看，铝行业长期供给增量有限，而需求仍有增长点，行业或将维持高景气", "news_prompt5": "建议关注：天山铝业、中国铝业、云铝股份等", "news_prompt6": "（文章来源：证券时报网）"}</t>
+          <t>{"news_prompt1": "而短期铝土矿供应仍然紧张，后续几内亚雨季影响或逐步显现，氧化铝价格探涨，仍然是铝价的支撑，一体化经营的公司将明显受益，关注板块投资机会", "news_prompt2": "长期来看，铝行业长期供给增量有限，而需求仍有增长点，行业或将维持高景气"}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，国海证券研报指出，短期来看，铝价仍然偏强，旺季对需求的提升逐步体现，阶段性铝价高位和意外事件不影响去库大趋势": {"topic": "“金融”", "similarity": 0.5101388096809387}, "而短期铝土矿供应仍然紧张，后续几内亚雨季影响或逐步显现，氧化铝价格探涨，仍然是铝价的支撑，一体化经营的公司将明显受益，关注板块投资机会": {"topic": "“金融”", "similarity": 0.5783871412277222, "prompt": "新闻文本是“而短期铝土矿供应仍然紧张，后续几内亚雨季影响或逐步显现，氧化铝价格探涨，仍然是铝价的支撑，一体化经营的公司将明显受益，关注板块投资机会”，包含的情绪词典是：选矿/精选(beneficiation):0.4,有利可图的/盈利的(profitable):0.8"}, "长期来看，铝行业长期供给增量有限，而需求仍有增长点，行业或将维持高景气": {"topic": "“宏观经济”", "similarity": 0.5018649101257324, "prompt": "新闻文本是“长期来看，铝行业长期供给增量有限，而需求仍有增长点，行业或将维持高景气”，包含的情绪词典是：供应过剩(oversupply):-0.2,有限的/被限制的(limited):-0.1"}, "建议关注：天山铝业、中国铝业、云铝股份等": {"topic": "“金融”", "similarity": 0.5821696519851685, "prompt": "新闻文本是“建议关注：天山铝业、中国铝业、云铝股份等”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "（文章来源：证券时报网）": {"topic": "“金融”", "similarity": 0.4481872320175171, "prompt": "新闻文本是“（文章来源：证券时报网）”，包含的情绪词典是：股票/库存(stock):0.0,资本/资金(capital):0.1"}}</t>
+          <t>{"而短期铝土矿供应仍然紧张，后续几内亚雨季影响或逐步显现，氧化铝价格探涨，仍然是铝价的支撑，一体化经营的公司将明显受益，关注板块投资机会": {"topic": "“金融”", "similarity": 0.5783872604370117, "prompt": "新闻文本是“而短期铝土矿供应仍然紧张，后续几内亚雨季影响或逐步显现，氧化铝价格探涨，仍然是铝价的支撑，一体化经营的公司将明显受益，关注板块投资机会”，包含的情绪词典是：选矿/精选(beneficiation):0.4,有利可图的/盈利的(profitable):0.8"}, "长期来看，铝行业长期供给增量有限，而需求仍有增长点，行业或将维持高景气": {"topic": "“宏观经济”", "similarity": 0.501865029335022, "prompt": "新闻文本是“长期来看，铝行业长期供给增量有限，而需求仍有增长点，行业或将维持高景气”，包含的情绪词典是：供应过剩(oversupply):-0.2,有限的/被限制的(limited):-0.1"}}</t>
         </is>
       </c>
     </row>
@@ -1148,12 +1140,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月30日，豆粕ETF(159985.SZ)收涨0.95%，成交2.29亿元", "news_prompt2": "净流入1380.53万元（净申购份额*单位净值），居全市场第一梯队", "news_prompt3": "拉长时间看，该基金连续5天资金净流入，合计吸金7762.39万元，居全市场第一梯队", "news_prompt4": "资金流入也助力了份额的提升，该基金最新份额较前一日增加720.00万份，突破7.80亿份，创历史新高", "news_prompt5": "与此同时，该基金最新规模突破15.00亿元，创近1个月新高", "news_prompt6": "豆粕ETF(159985.SZ)，场外联接(A：007937", "news_prompt7": "C：007938)", "news_prompt8": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "净流入1380.53万元（净申购份额*单位净值），居全市场第一梯队", "news_prompt2": "拉长时间看，该基金连续5天资金净流入，合计吸金7762.39万元，居全市场第一梯队", "news_prompt3": "资金流入也助力了份额的提升，该基金最新份额较前一日增加720.00万份，突破7.80亿份，创历史新高", "news_prompt4": "与此同时，该基金最新规模突破15.00亿元，创近1个月新高", "news_prompt5": "C：007938)"}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"净流入1380.53万元（净申购份额*单位净值），居全市场第一梯队": {"topic": "“金融”", "similarity": 0.539293646812439, "prompt": "新闻文本是“净流入1380.53万元（净申购份额*单位净值），居全市场第一梯队”，包含的情绪词典是：第一/首先(first):0.0,投资/投入(invest):0.3"}, "拉长时间看，该基金连续5天资金净流入，合计吸金7762.39万元，居全市场第一梯队": {"topic": "“金融”", "similarity": 0.5131226778030396, "prompt": "新闻文本是“拉长时间看，该基金连续5天资金净流入，合计吸金7762.39万元，居全市场第一梯队”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "资金流入也助力了份额的提升，该基金最新份额较前一日增加720.00万份，突破7.80亿份，创历史新高": {"topic": "“金融”", "similarity": 0.44012847542762756, "prompt": "新闻文本是“资金流入也助力了份额的提升，该基金最新份额较前一日增加720.00万份，突破7.80亿份，创历史新高”，包含的情绪词典是：部分/份额(portion):0.0,基金/资金(fund):0.1"}, "与此同时，该基金最新规模突破15.00亿元，创近1个月新高": {"topic": "“金融”", "similarity": 0.45768749713897705, "prompt": "新闻文本是“与此同时，该基金最新规模突破15.00亿元，创近1个月新高”，包含的情绪词典是：飙升/猛增(soar):0.7,投资/投资额(investment):0.4"}, "C：007938)": {"topic": "“金融”", "similarity": 0.4374920725822449, "prompt": "新闻文本是“C：007938)”，包含的情绪词典是：股票/库存(stock):0.0,事故/意外(accident):-0.3"}}</t>
+          <t>{"净流入1380.53万元（净申购份额*单位净值），居全市场第一梯队": {"topic": "“金融”", "similarity": 0.5392937660217285, "prompt": "新闻文本是“净流入1380.53万元（净申购份额*单位净值），居全市场第一梯队”，包含的情绪词典是：第一/首先(first):0.0,投资/投入(invest):0.3"}, "拉长时间看，该基金连续5天资金净流入，合计吸金7762.39万元，居全市场第一梯队": {"topic": "“金融”", "similarity": 0.5131229162216187, "prompt": "新闻文本是“拉长时间看，该基金连续5天资金净流入，合计吸金7762.39万元，居全市场第一梯队”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "资金流入也助力了份额的提升，该基金最新份额较前一日增加720.00万份，突破7.80亿份，创历史新高": {"topic": "“金融”", "similarity": 0.44012874364852905, "prompt": "新闻文本是“资金流入也助力了份额的提升，该基金最新份额较前一日增加720.00万份，突破7.80亿份，创历史新高”，包含的情绪词典是：部分/份额(portion):0.0,基金/资金(fund):0.1"}, "与此同时，该基金最新规模突破15.00亿元，创近1个月新高": {"topic": "“金融”", "similarity": 0.4576876759529114, "prompt": "新闻文本是“与此同时，该基金最新规模突破15.00亿元，创近1个月新高”，包含的情绪词典是：飙升/猛增(soar):0.7,投资/投资额(investment):0.4"}, "C：007938)": {"topic": "“金融”", "similarity": 0.4374919533729553, "prompt": "新闻文本是“C：007938)”，包含的情绪词典是：股票/库存(stock):0.0,事故/意外(accident):-0.3"}}</t>
         </is>
       </c>
     </row>
@@ -1199,12 +1191,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月1日16时，载有200余名旅客、50余辆车的“棒棰岛”轮在旅顺港鸣笛起航，驶向目的地天津，标志着停航近十年的连津客滚航线正式复航", "news_prompt2": "“旅顺—天津”航线具有悠久的历史，在连接辽南与京津地区间物流通道、人流通道方面发挥着重要作用", "news_prompt3": "近年来，随着大连与天津两地间货运、旅游人流逐日增加，两地港口集疏运网络日趋完善，车客源日趋充足，旅顺至天津客滚航线的复航水到渠成", "news_prompt4": "据旅顺港生产业务部部长宋永翔介绍说，“棒棰岛”轮载客量1200人，载车线835米，初始航班计划为每4天一班", "news_prompt5": "乘坐该航线船舶的旅客可以带车上船(非新能源车)，也可以携带宠物(需包舱或寄存)，目前邮轮上有六人间、四人间和单人间", "news_prompt6": "在航次安排方面，大连旅顺至天津客滚航线航次安排为每4天一个往返，9月1日16时从旅顺新港始发，9月2日22时天津国际邮轮母港始发", "news_prompt7": "“十一”期间计划每两天一班", "news_prompt8": "“暑假带孩子来大连玩，听说今天连津航线复航，就赶紧提前预订了船票", "news_prompt9": "”来大连旅游的张女士说，从大连到天津13个小时旅途中，可以领略阳光洒在浪花上的闪烁，目睹日出的壮丽，这种航海体验简直太棒了", "news_prompt10": "此次大连旅顺至天津客滚航线复航，将进一步加强连、津两市及腹地城市间经济文化交流，进而促进两地经济发展", "news_prompt11": "(完)（文章来源：中国新闻网）"}</t>
+          <t>{"news_prompt1": "近年来，随着大连与天津两地间货运、旅游人流逐日增加，两地港口集疏运网络日趋完善，车客源日趋充足，旅顺至天津客滚航线的复航水到渠成", "news_prompt2": "“暑假带孩子来大连玩，听说今天连津航线复航，就赶紧提前预订了船票", "news_prompt3": "”来大连旅游的张女士说，从大连到天津13个小时旅途中，可以领略阳光洒在浪花上的闪烁，目睹日出的壮丽，这种航海体验简直太棒了", "news_prompt4": "此次大连旅顺至天津客滚航线复航，将进一步加强连、津两市及腹地城市间经济文化交流，进而促进两地经济发展"}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>{"近年来，随着大连与天津两地间货运、旅游人流逐日增加，两地港口集疏运网络日趋完善，车客源日趋充足，旅顺至天津客滚航线的复航水到渠成": {"topic": "“消费”", "similarity": 0.49359917640686035, "prompt": "新闻文本是“近年来，随着大连与天津两地间货运、旅游人流逐日增加，两地港口集疏运网络日趋完善，车客源日趋充足，旅顺至天津客滚航线的复航水到渠成”，包含的情绪词典是：善于接受的/能接纳的(receptive):0.3,有益的/有回报的(rewarding):0.5"}, "在航次安排方面，大连旅顺至天津客滚航线航次安排为每4天一个往返，9月1日16时从旅顺新港始发，9月2日22时天津国际邮轮母港始发": {"topic": "“消费”", "similarity": 0.4295056462287903}, "“暑假带孩子来大连玩，听说今天连津航线复航，就赶紧提前预订了船票": {"topic": "“消费”", "similarity": 0.4215705394744873, "prompt": "新闻文本是““暑假带孩子来大连玩，听说今天连津航线复航，就赶紧提前预订了船票”，包含的情绪词典是：预期的/预料的(anticipated):0.2,复苏的/复兴的(resurgent):0.3"}, "”来大连旅游的张女士说，从大连到天津13个小时旅途中，可以领略阳光洒在浪花上的闪烁，目睹日出的壮丽，这种航海体验简直太棒了": {"topic": "“消费”", "similarity": 0.4761435091495514, "prompt": "新闻文本是“”来大连旅游的张女士说，从大连到天津13个小时旅途中，可以领略阳光洒在浪花上的闪烁，目睹日出的壮丽，这种航海体验简直太棒了”，包含的情绪词典是：壮观的/惊人的(spectacular):0.8,壮观地/惊人地(spectacularly):0.8"}, "此次大连旅顺至天津客滚航线复航，将进一步加强连、津两市及腹地城市间经济文化交流，进而促进两地经济发展": {"topic": "“消费”", "similarity": 0.5036327242851257, "prompt": "新闻文本是“此次大连旅顺至天津客滚航线复航，将进一步加强连、津两市及腹地城市间经济文化交流，进而促进两地经济发展”，包含的情绪词典是：复苏/复兴(resurgence):0.3,复苏的/复兴的(resurgent):0.3"}}</t>
+          <t>{"近年来，随着大连与天津两地间货运、旅游人流逐日增加，两地港口集疏运网络日趋完善，车客源日趋充足，旅顺至天津客滚航线的复航水到渠成": {"topic": "“消费”", "similarity": 0.4935992360115051, "prompt": "新闻文本是“近年来，随着大连与天津两地间货运、旅游人流逐日增加，两地港口集疏运网络日趋完善，车客源日趋充足，旅顺至天津客滚航线的复航水到渠成”，包含的情绪词典是：善于接受的/能接纳的(receptive):0.3,有益的/有回报的(rewarding):0.5"}, "“暑假带孩子来大连玩，听说今天连津航线复航，就赶紧提前预订了船票": {"topic": "“消费”", "similarity": 0.42157068848609924, "prompt": "新闻文本是““暑假带孩子来大连玩，听说今天连津航线复航，就赶紧提前预订了船票”，包含的情绪词典是：预期的/预料的(anticipated):0.2,复苏的/复兴的(resurgent):0.3"}, "”来大连旅游的张女士说，从大连到天津13个小时旅途中，可以领略阳光洒在浪花上的闪烁，目睹日出的壮丽，这种航海体验简直太棒了": {"topic": "“消费”", "similarity": 0.47614359855651855, "prompt": "新闻文本是“”来大连旅游的张女士说，从大连到天津13个小时旅途中，可以领略阳光洒在浪花上的闪烁，目睹日出的壮丽，这种航海体验简直太棒了”，包含的情绪词典是：壮观的/惊人的(spectacular):0.8,壮观地/惊人地(spectacularly):0.8"}, "此次大连旅顺至天津客滚航线复航，将进一步加强连、津两市及腹地城市间经济文化交流，进而促进两地经济发展": {"topic": "“消费”", "similarity": 0.5036327838897705, "prompt": "新闻文本是“此次大连旅顺至天津客滚航线复航，将进一步加强连、津两市及腹地城市间经济文化交流，进而促进两地经济发展”，包含的情绪词典是：复苏/复兴(resurgence):0.3,复苏的/复兴的(resurgent):0.3"}}</t>
         </is>
       </c>
     </row>
@@ -1250,12 +1242,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上证报中国证券网讯 9月2日，3家公司临停：ST锦港、ST锦港B、宝鹰股份、广汇物流，1家公司复牌：ST新潮", "news_prompt2": "来源：Choice （文章来源：上海证券报·中国证券网）"}</t>
+          <t>{"news_prompt1": "上证报中国证券网讯 9月2日，3家公司临停：ST锦港、ST锦港B、宝鹰股份、广汇物流，1家公司复牌：ST新潮"}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"上证报中国证券网讯 9月2日，3家公司临停：ST锦港、ST锦港B、宝鹰股份、广汇物流，1家公司复牌：ST新潮": {"topic": "“金融”", "similarity": 0.5157498121261597, "prompt": "新闻文本是“上证报中国证券网讯 9月2日，3家公司临停：ST锦港、ST锦港B、宝鹰股份、广汇物流，1家公司复牌：ST新潮”，包含的情绪词典是：已停业的/已倒闭的(defunct):-0.6,停滞的/不景气的(stagnant):-0.5"}, "来源：Choice （文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.5434427857398987, "prompt": "新闻文本是“来源：Choice （文章来源：上海证券报·中国证券网）”，包含的情绪词典是：选矿/精选(beneficiation):0.4,精选的/受益的(beneficiated):0.5"}}</t>
+          <t>{"上证报中国证券网讯 9月2日，3家公司临停：ST锦港、ST锦港B、宝鹰股份、广汇物流，1家公司复牌：ST新潮": {"topic": "“金融”", "similarity": 0.5157498121261597, "prompt": "新闻文本是“上证报中国证券网讯 9月2日，3家公司临停：ST锦港、ST锦港B、宝鹰股份、广汇物流，1家公司复牌：ST新潮”，包含的情绪词典是：已停业的/已倒闭的(defunct):-0.6,停滞的/不景气的(stagnant):-0.5"}}</t>
         </is>
       </c>
     </row>
@@ -1301,12 +1293,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "中国网财经9月2日讯日前，华厦眼科发布了2024年半年报，报告期内公司实现营业收入20.51亿元，同比增加2.85%，实现归属于上市公司股东的净利润2.65亿元，同比减少25.15%", "news_prompt2": "此次净利润下跌，是华厦眼科自2022年11月上市以来的首次“告负”", "news_prompt3": "质疑纷至沓来，说其内外交困者有之", "news_prompt4": "对其未来担心者更甚", "news_prompt5": "中国网财经记者在仔细研究华厦眼科半年报后发现，顶着此前的超额增长带来的压力，华厦眼科或在积极适应环境变化，以谋未来更大的布局", "news_prompt6": "而已经将爱迪眼科收入囊中的华厦眼科，已悄然成为了国内首家，也是唯一一个拥有“双三甲”眼科医院的集团", "news_prompt7": "危中有机，谋局在即", "news_prompt8": "近三年复合增长率稳健，符合行业预期 　　拉长时间来看，近年来华厦眼科业绩始终稳健增长", "news_prompt9": "数据显示，2021-2023年，华厦眼科营收同比增幅分别为21.86%、5.51%和24.12%，近三年营收复合增长率为16.86%", "news_prompt10": "同期归母净利润同比增幅分别为36.01%、12.95%和29.60%，近三年净利润复合增长率为25.80%", "news_prompt11": "需要指出的是，眼科医疗服务行业受消费环境变化的影响，2023年下半年至今市场竞争加剧，屈光板块出现价格战现象，对行业内公司造成持续影响", "news_prompt12": "根据Gangtise投研数据，Gangtise选取的5家眼科医疗服务上市公司2024Q1平均营收增速仅有3%，归母净利润增速-5.3%", "news_prompt13": "彼时，Gangtise投研做出预测：2024年眼科医疗服务行业增速相对疲软，行业性的降速趋势客观存在", "news_prompt14": "对此，一位长期跟踪华厦眼科的分析师向中国网财经记者表示，“此前，华厦眼科连续三年保持了亮眼的业绩增长，尤其是2023年上半年公司净利润增速达50.08%，在去年高基数的挑战面前，今年上半年华厦眼科的业绩变动态势与行业变动基本一致，而近三年半年报的复合增长率其实与此前很多行业研究报告的增速预测也基本吻合", "news_prompt15": "” 　　该分析师对中国网财经强调称：“从这个维度来看，一定程度上也体现了华厦眼科这家公司对抗风险和贡献利润的能力", "news_prompt16": "” 　　从半年报数据来看，2024年上半年华厦眼科营业成本同比增长12.08%，究其原因，或与华厦眼科的内在增长韧性相关", "news_prompt17": "近两年，华厦旗下临沂眼科医院、台州五官科医院、兰州华厦眼科医院、镇江康复眼科医院等多家医院搬迁新址，以全新面貌亮相", "news_prompt18": "上述医院的搬迁或许是对公司利润增速造成影响的原因之一", "news_prompt19": "前述分析师对中国网财经记者表示，华厦眼科敢于加大投入、牺牲短期利润来苦练内功，提升自身服务能力是基于当前市场竞争做出的最优战略选择", "news_prompt20": "从长远发展来看，乔迁升级或使临沂、台州、镇江等地医院更好服务当地眼疾病患，实现全新跨越，后续为公司带来持续收益", "news_prompt21": "目前唯一“双三甲”眼科医院集团 　　事实上，按照既定战略有序推进全国医疗服务网络布局是华厦眼科近年来一直在做的事情", "news_prompt22": "2024年上半年，华厦眼科完成四川源聚爱迪眼科医院管理有限公司(以下简称“爱迪眼科”)51%股权的收购", "news_prompt23": "据悉，爱迪眼科控股多家眼科医院，包括成都爱迪眼科医院(以下简称“成都爱迪”)、恩施慧宜眼科医院、微山医大眼科医院及睢宁复兴眼科医院", "news_prompt24": "公告显示，成都爱迪是华厦眼科旗下第二家三甲眼科专科医院，也是成都市唯一一家三甲眼科专科医院", "news_prompt25": "业绩方面，2023年度，成都爱迪实现营收3.61亿元，同期净利润4717.05万元", "news_prompt26": "2024年1-2月，成都爱迪实现营收7000.25万元，同期净利润1348.99万元", "news_prompt27": "上述分析师对中国网财经记者表示，“成都爱迪眼科医院2021年晋级三甲医院，凭借多年品牌积累稳坐成都眼科市场第一梯队，此时华厦眼科的收购之举无疑是对成都市场的优质资源整合", "news_prompt28": "收购成都爱迪后，华厦眼科成为国内唯一拥有‘双三甲’眼科医院的集团，其在眼病诊疗领域的技术、人才含金量不言而喻", "news_prompt29": "” 　　华厦眼科半年度报告显示，成都爱迪汇聚了胡玉章教授、张军军教授、刘谊教授等多位国内眼科顶尖专家，具备高水平的诊疗服务能力，同时进一步壮大了华厦眼科领军人才队伍，提升其诊疗技术、科研和教学水平", "news_prompt30": "此外，围绕医院本地化需求，天津华厦、深圳南山以及视光中心建设的持续推进，使华厦眼科形成“1+N”医疗服务网络布局，不仅深耕了重点市场，同时完善全国布局", "news_prompt31": "截至2024H1，华厦眼科已在全国18个省和直辖市、49个城市开设61家眼科专科医院和65家视光中心，辐射国内华东、华中、华南、西南、华北等广大地区，高水平的诊疗服务能力和连锁运营的优势得到进一步体现", "news_prompt32": "聚势添能行业新质生产力发展 　　除了医疗服务网络布局，华厦眼科的科研创新能力也持续稳步提升", "news_prompt33": "2024年上半年，华厦眼科新增专利授权21项，软件著作权6项", "news_prompt34": "在各类期刊新增发表科研文章32篇，SCI收录9篇", "news_prompt35": "新增参与专家指南和共识编写6篇", "news_prompt36": "新增获批医学科研项目23项，新增"}</t>
+          <t>{"news_prompt1": "此次净利润下跌，是华厦眼科自2022年11月上市以来的首次“告负”", "news_prompt2": "质疑纷至沓来，说其内外交困者有之", "news_prompt3": "对其未来担心者更甚", "news_prompt4": "中国网财经记者在仔细研究华厦眼科半年报后发现，顶着此前的超额增长带来的压力，华厦眼科或在积极适应环境变化，以谋未来更大的布局", "news_prompt5": "而已经将爱迪眼科收入囊中的华厦眼科，已悄然成为了国内首家，也是唯一一个拥有“双三甲”眼科医院的集团", "news_prompt6": "危中有机，谋局在即", "news_prompt7": "近三年复合增长率稳健，符合行业预期 　　拉长时间来看，近年来华厦眼科业绩始终稳健增长", "news_prompt8": "同期归母净利润同比增幅分别为36.01%、12.95%和29.60%，近三年净利润复合增长率为25.80%", "news_prompt9": "需要指出的是，眼科医疗服务行业受消费环境变化的影响，2023年下半年至今市场竞争加剧，屈光板块出现价格战现象，对行业内公司造成持续影响", "news_prompt10": "彼时，Gangtise投研做出预测：2024年眼科医疗服务行业增速相对疲软，行业性的降速趋势客观存在", "news_prompt11": "” 　　该分析师对中国网财经强调称：“从这个维度来看，一定程度上也体现了华厦眼科这家公司对抗风险和贡献利润的能力", "news_prompt12": "前述分析师对中国网财经记者表示，华厦眼科敢于加大投入、牺牲短期利润来苦练内功，提升自身服务能力是基于当前市场竞争做出的最优战略选择", "news_prompt13": "从长远发展来看，乔迁升级或使临沂、台州、镇江等地医院更好服务当地眼疾病患，实现全新跨越，后续为公司带来持续收益", "news_prompt14": "2024年1-2月，成都爱迪实现营收7000.25万元，同期净利润1348.99万元", "news_prompt15": "此外，围绕医院本地化需求，天津华厦、深圳南山以及视光中心建设的持续推进，使华厦眼科形成“1+N”医疗服务网络布局，不仅深耕了重点市场，同时完善全国布局", "news_prompt16": "聚势添能行业新质生产力发展 　　除了医疗服务网络布局，华厦眼科的科研创新能力也持续稳步提升", "news_prompt17": "2024年上半年，华厦眼科新增专利授权21项，软件著作权6项", "news_prompt18": "在各类期刊新增发表科研文章32篇，SCI收录9篇"}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"此次净利润下跌，是华厦眼科自2022年11月上市以来的首次“告负”": {"topic": "“金融”", "similarity": 0.4488491415977478, "prompt": "新闻文本是“此次净利润下跌，是华厦眼科自2022年11月上市以来的首次“告负””，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "质疑纷至沓来，说其内外交困者有之": {"topic": "“宏观经济”", "similarity": 0.4465073347091675, "prompt": "新闻文本是“质疑纷至沓来，说其内外交困者有之”，包含的情绪词典是：怀疑/疑虑(doubts):-0.2,怀疑/猜疑(suspicion):-0.3"}, "对其未来担心者更甚": {"topic": "“宏观经济”", "similarity": 0.4487535357475281, "prompt": "新闻文本是“对其未来担心者更甚”，包含的情绪词典是：令人担忧的/担心的(worrying):-0.4,有关的/担忧的(concerned):-0.2"}, "中国网财经记者在仔细研究华厦眼科半年报后发现，顶着此前的超额增长带来的压力，华厦眼科或在积极适应环境变化，以谋未来更大的布局": {"topic": "“生产投资”", "similarity": 0.5182923078536987, "prompt": "新闻文本是“中国网财经记者在仔细研究华厦眼科半年报后发现，顶着此前的超额增长带来的压力，华厦眼科或在积极适应环境变化，以谋未来更大的布局”，包含的情绪词典是：超支/超出预算(overrun):-0.2,正在改善的/正在改进的(improving):0.5"}, "而已经将爱迪眼科收入囊中的华厦眼科，已悄然成为了国内首家，也是唯一一个拥有“双三甲”眼科医院的集团": {"topic": "“生产投资”", "similarity": 0.4433427155017853, "prompt": "新闻文本是“而已经将爱迪眼科收入囊中的华厦眼科，已悄然成为了国内首家，也是唯一一个拥有“双三甲”眼科医院的集团”，包含的情绪词典是：公司的/企业的(corporate):0.0,国内的/本国的(domestic):0.0"}, "危中有机，谋局在即": {"topic": "“金融”", "similarity": 0.4937320947647095, "prompt": "新闻文本是“危中有机，谋局在即”，包含的情绪词典是：正在密谋/正在共谋(conspiring):-0.5,濒危的/受到危害的(endangered):-0.8"}, "近三年复合增长率稳健，符合行业预期 　　拉长时间来看，近年来华厦眼科业绩始终稳健增长": {"topic": "“金融”", "similarity": 0.44426262378692627, "prompt": "新闻文本是“近三年复合增长率稳健，符合行业预期 　　拉长时间来看，近年来华厦眼科业绩始终稳健增长”，包含的情绪词典是：已稳定的/稳定的(stabilized):0.5,稳定的/稳固的(stable):0.5"}, "数据显示，2021-2023年，华厦眼科营收同比增幅分别为21.86%、5.51%和24.12%，近三年营收复合增长率为16.86%": {"topic": "“消费”", "similarity": 0.47550949454307556}, "同期归母净利润同比增幅分别为36.01%、12.95%和29.60%，近三年净利润复合增长率为25.80%": {"topic": "“金融”", "similarity": 0.4290580153465271, "prompt": "新闻文本是“同期归母净利润同比增幅分别为36.01%、12.95%和29.60%，近三年净利润复合增长率为25.80%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "需要指出的是，眼科医疗服务行业受消费环境变化的影响，2023年下半年至今市场竞争加剧，屈光板块出现价格战现象，对行业内公司造成持续影响": {"topic": "“消费”", "similarity": 0.5701330900192261, "prompt": "新闻文本是“需要指出的是，眼科医疗服务行业受消费环境变化的影响，2023年下半年至今市场竞争加剧，屈光板块出现价格战现象，对行业内公司造成持续影响”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,竞争者/竞争对手(competitor):0.0"}, "根据Gangtise投研数据，Gangtise选取的5家眼科医疗服务上市公司2024Q1平均营收增速仅有3%，归母净利润增速-5.3%": {"topic": "“生产投资”", "similarity": 0.5048032999038696}, "彼时，Gangtise投研做出预测：2024年眼科医疗服务行业增速相对疲软，行业性的降速趋势客观存在": {"topic": "“生产投资”", "similarity": 0.4885988235473633, "prompt": "新闻文本是“彼时，Gangtise投研做出预测：2024年眼科医疗服务行业增速相对疲软，行业性的降速趋势客观存在”，包含的情绪词典是：下降/衰退(decline):-0.6,衰退的/不景气的(recessionary):-0.8"}, "对此，一位长期跟踪华厦眼科的分析师向中国网财经记者表示，“此前，华厦眼科连续三年保持了亮眼的业绩增长，尤其是2023年上半年公司净利润增速达50.08%，在去年高基数的挑战面前，今年上半年华厦眼科的业绩变动态势与行业变动基本一致，而近三年半年报的复合增长率其实与此前很多行业研究报告的增速预测也基本吻合": {"topic": "“生产投资”", "similarity": 0.4964612126350403}, "” 　　该分析师对中国网财经强调称：“从这个维度来看，一定程度上也体现了华厦眼科这家公司对抗风险和贡献利润的能力": {"topic": "“金融”", "similarity": 0.42773449420928955, "prompt": "新闻文本是“” 　　该分析师对中国网财经强调称：“从这个维度来看，一定程度上也体现了华厦眼科这家公司对抗风险和贡献利润的能力”，包含的情绪词典是：有深刻见解的/富有洞察力的(insightful):0.4,盈利能力/获利能力(profitability):0.6"}, "” 　　从半年报数据来看，2024年上半年华厦眼科营业成本同比增长12.08%，究其原因，或与华厦眼科的内在增长韧性相关": {"topic": "“消费”", "similarity": 0.4943990707397461}, "近两年，华厦旗下临沂眼科医院、台州五官科医院、兰州华厦眼科医院、镇江康复眼科医院等多家医院搬迁新址，以全新面貌亮相": {"topic": "“生产投资”", "similarity": 0.46162378787994385}, "前述分析师对中国网财经记者表示，华厦眼科敢于加大投入、牺牲短期利润来苦练内功，提升自身服务能力是基于当前市场竞争做出的最优战略选择": {"topic": "“生产投资”", "similarity": 0.45927172899246216, "prompt": "新闻文本是“前述分析师对中国网财经记者表示，华厦眼科敢于加大投入、牺牲短期利润来苦练内功，提升自身服务能力是基于当前市场竞争做出的最优战略选择”，包含的情绪词典是：牺牲性的/奉献性的(sacrificial):-0.4,竞争力/竞争能力(competitiveness):0.3"}, "从长远发展来看，乔迁升级或使临沂、台州、镇江等地医院更好服务当地眼疾病患，实现全新跨越，后续为公司带来持续收益": {"topic": "“生产投资”", "similarity": 0.461302787065506, "prompt": "新闻文本是“从长远发展来看，乔迁升级或使临沂、台州、镇江等地医院更好服务当地眼疾病患，实现全新跨越，后续为公司带来持续收益”，包含的情绪词典是：进步/提升(advancement):0.5,正在改善的/正在改进的(improving):0.5"}, "目前唯一“双三甲”眼科医院集团 　　事实上，按照既定战略有序推进全国医疗服务网络布局是华厦眼科近年来一直在做的事情": {"topic": "“生产投资”", "similarity": 0.4689333736896515}, "2024年上半年，华厦眼科完成四川源聚爱迪眼科医院管理有限公司(以下简称“爱迪眼科”)51%股权的收购": {"topic": "“生产投资”", "similarity": 0.5111373662948608}, "据悉，爱迪眼科控股多家眼科医院，包括成都爱迪眼科医院(以下简称“成都爱迪”)、恩施慧宜眼科医院、微山医大眼科医院及睢宁复兴眼科医院": {"topic": "“生产投资”", "similarity": 0.4899744391441345}, "公告显示，成都爱迪是华厦眼科旗下第二家三甲眼科专科医院，也是成都市唯一一家三甲眼科专科医院": {"topic": "“房地产”", "similarity": 0.42279207706451416}, "业绩方面，2023年度，成都爱迪实现营收3.61亿元，同期净利润4717.05万元": {"topic": "“生产投资”", "similarity": 0.4580799341201782}, "2024年1-2月，成都爱迪实现营收7000.25万元，同期净利润1348.99万元": {"topic": "“生产投资”", "similarity": 0.48561277985572815, "prompt": "新闻文本是“2024年1-2月，成都爱迪实现营收7000.25万元，同期净利润1348.99万元”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6"}, "上述分析师对中国网财经记者表示，“成都爱迪眼科医院2021年晋级三甲医院，凭借多年品牌积累稳坐成都眼科市场第一梯队，此时华厦眼科的收购之举无疑是对成都市场的优质资源整合": {"topic": "“生产投资”", "similarity": 0.4529957175254822}, "收购成都爱迪后，华厦眼科成为国内唯一拥有‘双三甲’眼科医院的集团，其在眼病诊疗领域的技术、人才含金量不言而喻": {"topic": "“生产投资”", "similarity": 0.5004294514656067}, "” 　　华厦眼科半年度报告显示，成都爱迪汇聚了胡玉章教授、张军军教授、刘谊教授等多位国内眼科顶尖专家，具备高水平的诊疗服务能力，同时进一步壮大了华厦眼科领军人才队伍，提升其诊疗技术、科研和教学水平": {"topic": "“生产投资”", "similarity": 0.4631642699241638}, "此外，围绕医院本地化需求，天津华厦、深圳南山以及视光中心建设的持续推进，使华厦眼科形成“1+N”医疗服务网络布局，不仅深耕了重点市场，同时完善全国布局": {"topic": "“生产投资”", "similarity": 0.47397059202194214, "prompt": "新闻文本是“此外，围绕医院本地化需求，天津华厦、深圳南山以及视光中心建设的持续推进，使华厦眼科形成“1+N”医疗服务网络布局，不仅深耕了重点市场，同时完善全国布局”，包含的情绪词典是：有深刻见解的/富有洞察力的(insightful):0.4,国内的/本国的(domestic):0.0"}, "截至2024H1，华厦眼科已在全国18个省和直辖市、49个城市开设61家眼科专科医院和65家视光中心，辐射国内华东、华中、华南、西南、华北等广大地区，高水平的诊疗服务能力和连锁运营的优势得到进一步体现": {"topic": "“消费”", "similarity": 0.4847090542316437}, "聚势添能行业新质生产力发展 　　除了医疗服务网络布局，华厦眼科的科研创新能力也持续稳步提升": {"topic": "“生产投资”", "similarity": 0.5337584018707275, "prompt": "新闻文本是“聚势添能行业新质生产力发展 　　除了医疗服务网络布局，华厦眼科的科研创新能力也持续稳步提升”，包含的情绪词典是：多产的/富有成效的(productive):0.7,能力/容量(capacity):0.0"}, "2024年上半年，华厦眼科新增专利授权21项，软件著作权6项": {"topic": "“生产投资”", "similarity": 0.47624853253364563, "prompt": "新闻文本是“2024年上半年，华厦眼科新增专利授权21项，软件著作权6项”，包含的情绪词典是：专利权人(patentee):0.0,可获许可的/可被授权的(licensable):0.0"}, "在各类期刊新增发表科研文章32篇，SCI收录9篇": {"topic": "“生产投资”", "similarity": 0.432091623544693, "prompt": "新闻文本是“在各类期刊新增发表科研文章32篇，SCI收录9篇”，包含的情绪词典是：增长/发展(growth):0.7,提供信息的/增长见闻的(informative):0.5"}}</t>
+          <t>{"此次净利润下跌，是华厦眼科自2022年11月上市以来的首次“告负”": {"topic": "“金融”", "similarity": 0.44884932041168213, "prompt": "新闻文本是“此次净利润下跌，是华厦眼科自2022年11月上市以来的首次“告负””，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "质疑纷至沓来，说其内外交困者有之": {"topic": "“宏观经济”", "similarity": 0.44650739431381226, "prompt": "新闻文本是“质疑纷至沓来，说其内外交困者有之”，包含的情绪词典是：怀疑/疑虑(doubts):-0.2,怀疑/猜疑(suspicion):-0.3"}, "对其未来担心者更甚": {"topic": "“宏观经济”", "similarity": 0.4487537145614624, "prompt": "新闻文本是“对其未来担心者更甚”，包含的情绪词典是：令人担忧的/担心的(worrying):-0.4,有关的/担忧的(concerned):-0.2"}, "中国网财经记者在仔细研究华厦眼科半年报后发现，顶着此前的超额增长带来的压力，华厦眼科或在积极适应环境变化，以谋未来更大的布局": {"topic": "“生产投资”", "similarity": 0.5182923674583435, "prompt": "新闻文本是“中国网财经记者在仔细研究华厦眼科半年报后发现，顶着此前的超额增长带来的压力，华厦眼科或在积极适应环境变化，以谋未来更大的布局”，包含的情绪词典是：超支/超出预算(overrun):-0.2,正在改善的/正在改进的(improving):0.5"}, "而已经将爱迪眼科收入囊中的华厦眼科，已悄然成为了国内首家，也是唯一一个拥有“双三甲”眼科医院的集团": {"topic": "“生产投资”", "similarity": 0.44334280490875244, "prompt": "新闻文本是“而已经将爱迪眼科收入囊中的华厦眼科，已悄然成为了国内首家，也是唯一一个拥有“双三甲”眼科医院的集团”，包含的情绪词典是：公司的/企业的(corporate):0.0,国内的/本国的(domestic):0.0"}, "危中有机，谋局在即": {"topic": "“金融”", "similarity": 0.493732213973999, "prompt": "新闻文本是“危中有机，谋局在即”，包含的情绪词典是：正在密谋/正在共谋(conspiring):-0.5,濒危的/受到危害的(endangered):-0.8"}, "近三年复合增长率稳健，符合行业预期 　　拉长时间来看，近年来华厦眼科业绩始终稳健增长": {"topic": "“金融”", "similarity": 0.44426286220550537, "prompt": "新闻文本是“近三年复合增长率稳健，符合行业预期 　　拉长时间来看，近年来华厦眼科业绩始终稳健增长”，包含的情绪词典是：已稳定的/稳定的(stabilized):0.5,稳定的/稳固的(stable):0.5"}, "同期归母净利润同比增幅分别为36.01%、12.95%和29.60%，近三年净利润复合增长率为25.80%": {"topic": "“金融”", "similarity": 0.4290582537651062, "prompt": "新闻文本是“同期归母净利润同比增幅分别为36.01%、12.95%和29.60%，近三年净利润复合增长率为25.80%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "需要指出的是，眼科医疗服务行业受消费环境变化的影响，2023年下半年至今市场竞争加剧，屈光板块出现价格战现象，对行业内公司造成持续影响": {"topic": "“消费”", "similarity": 0.5701331496238708, "prompt": "新闻文本是“需要指出的是，眼科医疗服务行业受消费环境变化的影响，2023年下半年至今市场竞争加剧，屈光板块出现价格战现象，对行业内公司造成持续影响”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,竞争者/竞争对手(competitor):0.0"}, "彼时，Gangtise投研做出预测：2024年眼科医疗服务行业增速相对疲软，行业性的降速趋势客观存在": {"topic": "“生产投资”", "similarity": 0.4885990023612976, "prompt": "新闻文本是“彼时，Gangtise投研做出预测：2024年眼科医疗服务行业增速相对疲软，行业性的降速趋势客观存在”，包含的情绪词典是：下降/衰退(decline):-0.6,衰退的/不景气的(recessionary):-0.8"}, "” 　　该分析师对中国网财经强调称：“从这个维度来看，一定程度上也体现了华厦眼科这家公司对抗风险和贡献利润的能力": {"topic": "“金融”", "similarity": 0.4277345538139343, "prompt": "新闻文本是“” 　　该分析师对中国网财经强调称：“从这个维度来看，一定程度上也体现了华厦眼科这家公司对抗风险和贡献利润的能力”，包含的情绪词典是：有深刻见解的/富有洞察力的(insightful):0.4,盈利能力/获利能力(profitability):0.6"}, "前述分析师对中国网财经记者表示，华厦眼科敢于加大投入、牺牲短期利润来苦练内功，提升自身服务能力是基于当前市场竞争做出的最优战略选择": {"topic": "“生产投资”", "similarity": 0.45927178859710693, "prompt": "新闻文本是“前述分析师对中国网财经记者表示，华厦眼科敢于加大投入、牺牲短期利润来苦练内功，提升自身服务能力是基于当前市场竞争做出的最优战略选择”，包含的情绪词典是：牺牲性的/奉献性的(sacrificial):-0.4,竞争力/竞争能力(competitiveness):0.3"}, "从长远发展来看，乔迁升级或使临沂、台州、镇江等地医院更好服务当地眼疾病患，实现全新跨越，后续为公司带来持续收益": {"topic": "“生产投资”", "similarity": 0.46130287647247314, "prompt": "新闻文本是“从长远发展来看，乔迁升级或使临沂、台州、镇江等地医院更好服务当地眼疾病患，实现全新跨越，后续为公司带来持续收益”，包含的情绪词典是：进步/提升(advancement):0.5,正在改善的/正在改进的(improving):0.5"}, "2024年1-2月，成都爱迪实现营收7000.25万元，同期净利润1348.99万元": {"topic": "“生产投资”", "similarity": 0.485612690448761, "prompt": "新闻文本是“2024年1-2月，成都爱迪实现营收7000.25万元，同期净利润1348.99万元”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6"}, "此外，围绕医院本地化需求，天津华厦、深圳南山以及视光中心建设的持续推进，使华厦眼科形成“1+N”医疗服务网络布局，不仅深耕了重点市场，同时完善全国布局": {"topic": "“生产投资”", "similarity": 0.4739706516265869, "prompt": "新闻文本是“此外，围绕医院本地化需求，天津华厦、深圳南山以及视光中心建设的持续推进，使华厦眼科形成“1+N”医疗服务网络布局，不仅深耕了重点市场，同时完善全国布局”，包含的情绪词典是：有深刻见解的/富有洞察力的(insightful):0.4,国内的/本国的(domestic):0.0"}, "聚势添能行业新质生产力发展 　　除了医疗服务网络布局，华厦眼科的科研创新能力也持续稳步提升": {"topic": "“生产投资”", "similarity": 0.5337584018707275, "prompt": "新闻文本是“聚势添能行业新质生产力发展 　　除了医疗服务网络布局，华厦眼科的科研创新能力也持续稳步提升”，包含的情绪词典是：多产的/富有成效的(productive):0.7,能力/容量(capacity):0.0"}, "2024年上半年，华厦眼科新增专利授权21项，软件著作权6项": {"topic": "“生产投资”", "similarity": 0.4762486219406128, "prompt": "新闻文本是“2024年上半年，华厦眼科新增专利授权21项，软件著作权6项”，包含的情绪词典是：专利权人(patentee):0.0,可获许可的/可被授权的(licensable):0.0"}, "在各类期刊新增发表科研文章32篇，SCI收录9篇": {"topic": "“生产投资”", "similarity": 0.4320916533470154, "prompt": "新闻文本是“在各类期刊新增发表科研文章32篇，SCI收录9篇”，包含的情绪词典是：增长/发展(growth):0.7,提供信息的/增长见闻的(informative):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -1352,12 +1344,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "澳大利亚央行副行长Andrew Hauser表示，澳大利亚利率可能在不久的将来保持不变，因为当地通胀与美国相比“有点更具粘性”，突显出美联储准备放松政策之际的全球政策分化", "news_prompt2": "“我们还没有像美联储主席杰罗姆·鲍威尔那么有信心，没有那么确信澳大利亚通胀率回到可持续的回归目标轨道上，”Hauser在一则播客中称", "news_prompt3": "“因此，我们必须暂时维持利率不变", "news_prompt4": "”但他补充说，“我们将对改变利率和放松利率的可能性保持警惕", "news_prompt5": "” （文章来源：财联社）"}</t>
+          <t>{"news_prompt1": "“因此，我们必须暂时维持利率不变"}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"澳大利亚央行副行长Andrew Hauser表示，澳大利亚利率可能在不久的将来保持不变，因为当地通胀与美国相比“有点更具粘性”，突显出美联储准备放松政策之际的全球政策分化": {"topic": "“通货膨胀”", "similarity": 0.4802776575088501}, "“我们还没有像美联储主席杰罗姆·鲍威尔那么有信心，没有那么确信澳大利亚通胀率回到可持续的回归目标轨道上，”Hauser在一则播客中称": {"topic": "“通货膨胀”", "similarity": 0.4883161187171936}, "“因此，我们必须暂时维持利率不变": {"topic": "“宏观经济”", "similarity": 0.4372999370098114, "prompt": "新闻文本是““因此，我们必须暂时维持利率不变”，包含的情绪词典是：保持/保留(keep):0.0,比率/率(rate):0.0"}, "” （文章来源：财联社）": {"topic": "“金融”", "similarity": 0.4526078701019287, "prompt": "新闻文本是“” （文章来源：财联社）”，包含的情绪词典是：金融的/财政的(financial):0.0,金钱/货币(money):0.2"}}</t>
+          <t>{"“因此，我们必须暂时维持利率不变": {"topic": "“宏观经济”", "similarity": 0.43730002641677856, "prompt": "新闻文本是““因此，我们必须暂时维持利率不变”，包含的情绪词典是：保持/保留(keep):0.0,比率/率(rate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -1403,12 +1395,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "■编者按　　“承韵秦汉匠心五华”，高铁五华站即将开门迎客", "news_prompt2": "龙龙高铁梅龙段（梅龙高铁）预计9月具备开通运营条件，目前已进入试运行阶段", "news_prompt3": "届时广州、深圳等粤港澳大湾区城市到五华的最短通行时间将缩至1.5小时左右", "news_prompt4": "作为梅州人口最多的一个县，五华将因梅龙高铁的开通迎来新机遇", "news_prompt5": "即日起，《南方日报·五华视窗》推出“坐高铁，来五华，常来长乐”栏目，借光影之手，感五华之美，带您玩转五华这个宝藏小城", "news_prompt6": "敬请垂注", "news_prompt7": "当350公里时速的梅龙高铁疾驰而过，穿越历史底蕴深厚的五华县，历史与现代在这座岭南小城发出最诚挚的邀请：相约五华，常来长乐", "news_prompt8": "相约五华，常来长乐，乐在文化", "news_prompt9": "深埋千年的秦汉遗址，根植本土的南粤文化，中国内地现代足球从这里发源", "news_prompt10": "世界球王李惠堂、清代客家才子温训、梅州唯一武状元李威光……他们，讲述着五华这块土地上的历史与人文", "news_prompt11": "工匠之乡、足球之乡、文化之乡、诗词之乡、戏剧之乡，走进五华，如同翻阅一本厚厚的客家历史，粗看回味，细看惊叹", "news_prompt12": "相约五华，常来长乐，乐在山水", "news_prompt13": "用“高铁速度”寻味岭南风光，五华这座宝藏小城总会给你惊喜，或是城市的喧嚣，或是乡野的宁静，自然和谐共生的乐趣从不缺失，以绿色为主基调的山水五华，养眼更舒心", "news_prompt14": "广东“小千岛湖”益塘水库旅游区、热矿泥温泉度假村、汉光超顺农旅园（黄龙基地）、足球小镇、球王故里文化旅游区奥体中心片区……每一处，都能找到属于自己的打卡方式", "news_prompt15": "相约五华，常来长乐，乐在美食", "news_prompt16": "味蕾的享受，不再因距离而变得遥不可及", "news_prompt17": "从原产地到餐桌，每一道食材都历经了大自然的馈赠与五华人的精心呵护", "news_prompt18": "五华鱼生，薄如蝉翼，晶莹剔透，搭配特制的酱料，鲜美爽口，让人一试难忘", "news_prompt19": "盐焗鸡，皮脆肉嫩，咸香四溢，是五华人家宴上的必备佳肴", "news_prompt20": "白切鸡，原汁原味，肉质鲜美，简单却又不失风味", "news_prompt21": "酿豆腐、梅菜扣肉、咸菜焖猪肉、菩米等美食，更是各有千秋", "news_prompt22": "相约五华，常来长乐，乐在未来", "news_prompt23": "随着时代的发展，五华正以崭新的姿态迎接未来", "news_prompt24": "不断完善的基础设施，日益优化的营商环境，吸引着越来越多的人前来投资兴业、安居乐业", "news_prompt25": "教育、医疗等各项事业蓬勃发展，为五华的未来奠定了坚实的基础", "news_prompt26": "相约五华，常来长乐，乐不停，乐不止，总有说不完的理由，道不尽的情愫", "news_prompt27": "坐着高铁赴五华之约，五华等着你，共赴美好", "news_prompt28": "文：南方日报记者黄培强（文章来源：南方日报）"}</t>
+          <t>{"news_prompt1": "龙龙高铁梅龙段（梅龙高铁）预计9月具备开通运营条件，目前已进入试运行阶段", "news_prompt2": "届时广州、深圳等粤港澳大湾区城市到五华的最短通行时间将缩至1.5小时左右", "news_prompt3": "作为梅州人口最多的一个县，五华将因梅龙高铁的开通迎来新机遇", "news_prompt4": "即日起，《南方日报·五华视窗》推出“坐高铁，来五华，常来长乐”栏目，借光影之手，感五华之美，带您玩转五华这个宝藏小城", "news_prompt5": "当350公里时速的梅龙高铁疾驰而过，穿越历史底蕴深厚的五华县，历史与现代在这座岭南小城发出最诚挚的邀请：相约五华，常来长乐", "news_prompt6": "工匠之乡、足球之乡、文化之乡、诗词之乡、戏剧之乡，走进五华，如同翻阅一本厚厚的客家历史，粗看回味，细看惊叹", "news_prompt7": "用“高铁速度”寻味岭南风光，五华这座宝藏小城总会给你惊喜，或是城市的喧嚣，或是乡野的宁静，自然和谐共生的乐趣从不缺失，以绿色为主基调的山水五华，养眼更舒心", "news_prompt8": "广东“小千岛湖”益塘水库旅游区、热矿泥温泉度假村、汉光超顺农旅园（黄龙基地）、足球小镇、球王故里文化旅游区奥体中心片区……每一处，都能找到属于自己的打卡方式", "news_prompt9": "随着时代的发展，五华正以崭新的姿态迎接未来", "news_prompt10": "不断完善的基础设施，日益优化的营商环境，吸引着越来越多的人前来投资兴业、安居乐业", "news_prompt11": "教育、医疗等各项事业蓬勃发展，为五华的未来奠定了坚实的基础", "news_prompt12": "相约五华，常来长乐，乐不停，乐不止，总有说不完的理由，道不尽的情愫"}</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"龙龙高铁梅龙段（梅龙高铁）预计9月具备开通运营条件，目前已进入试运行阶段": {"topic": "“生产投资”", "similarity": 0.44007110595703125, "prompt": "新闻文本是“龙龙高铁梅龙段（梅龙高铁）预计9月具备开通运营条件，目前已进入试运行阶段”，包含的情绪词典是：试验性的/暂定的(tentative):0.0,初步的/预备性的(preliminary):0.0"}, "届时广州、深圳等粤港澳大湾区城市到五华的最短通行时间将缩至1.5小时左右": {"topic": "“生产投资”", "similarity": 0.4434991478919983, "prompt": "新闻文本是“届时广州、深圳等粤港澳大湾区城市到五华的最短通行时间将缩至1.5小时左右”，包含的情绪词典是：收缩/缩小(contracting):0.0,减少/缩小(diminution):-0.4"}, "作为梅州人口最多的一个县，五华将因梅龙高铁的开通迎来新机遇": {"topic": "“生产投资”", "similarity": 0.4737577438354492, "prompt": "新闻文本是“作为梅州人口最多的一个县，五华将因梅龙高铁的开通迎来新机遇”，包含的情绪词典是：机会/时机(opportunity):0.5,繁荣/兴旺(prospering):0.7"}, "即日起，《南方日报·五华视窗》推出“坐高铁，来五华，常来长乐”栏目，借光影之手，感五华之美，带您玩转五华这个宝藏小城": {"topic": "“消费”", "similarity": 0.43514418601989746, "prompt": "新闻文本是“即日起，《南方日报·五华视窗》推出“坐高铁，来五华，常来长乐”栏目，借光影之手，感五华之美，带您玩转五华这个宝藏小城”，包含的情绪词典是：令人愉快的/可享受的(enjoyable):0.6,享受/喜爱(enjoyment):0.5"}, "敬请垂注": {"topic": "“金融”", "similarity": 0.4526215195655823, "prompt": "新闻文本是“敬请垂注”，包含的情绪词典是：尊重/敬重(respect):0.4,使高兴/请(please):0.3"}, "当350公里时速的梅龙高铁疾驰而过，穿越历史底蕴深厚的五华县，历史与现代在这座岭南小城发出最诚挚的邀请：相约五华，常来长乐": {"topic": "“消费”", "similarity": 0.4651842713356018, "prompt": "新闻文本是“当350公里时速的梅龙高铁疾驰而过，穿越历史底蕴深厚的五华县，历史与现代在这座岭南小城发出最诚挚的邀请：相约五华，常来长乐”，包含的情绪词典是：在某处(somewhere):0.0,令人愉快的/可享受的(enjoyable):0.6"}, "工匠之乡、足球之乡、文化之乡、诗词之乡、戏剧之乡，走进五华，如同翻阅一本厚厚的客家历史，粗看回味，细看惊叹": {"topic": "“生产投资”", "similarity": 0.45238977670669556, "prompt": "新闻文本是“工匠之乡、足球之乡、文化之乡、诗词之乡、戏剧之乡，走进五华，如同翻阅一本厚厚的客家历史，粗看回味，细看惊叹”，包含的情绪词典是：中国的/中国人的(chinese):0.0,地方的/当地的(local):0.0"}, "用“高铁速度”寻味岭南风光，五华这座宝藏小城总会给你惊喜，或是城市的喧嚣，或是乡野的宁静，自然和谐共生的乐趣从不缺失，以绿色为主基调的山水五华，养眼更舒心": {"topic": "“消费”", "similarity": 0.4836914539337158, "prompt": "新闻文本是“用“高铁速度”寻味岭南风光，五华这座宝藏小城总会给你惊喜，或是城市的喧嚣，或是乡野的宁静，自然和谐共生的乐趣从不缺失，以绿色为主基调的山水五华，养眼更舒心”，包含的情绪词典是：独特的/有特色的(distinctive):0.0,享受/喜爱(enjoyment):0.5"}, "广东“小千岛湖”益塘水库旅游区、热矿泥温泉度假村、汉光超顺农旅园（黄龙基地）、足球小镇、球王故里文化旅游区奥体中心片区……每一处，都能找到属于自己的打卡方式": {"topic": "“消费”", "similarity": 0.5219109058380127, "prompt": "新闻文本是“广东“小千岛湖”益塘水库旅游区、热矿泥温泉度假村、汉光超顺农旅园（黄龙基地）、足球小镇、球王故里文化旅游区奥体中心片区……每一处，都能找到属于自己的打卡方式”，包含的情绪词典是：在某处(somewhere):0.0"}, "随着时代的发展，五华正以崭新的姿态迎接未来": {"topic": "“生产投资”", "similarity": 0.44795191287994385, "prompt": "新闻文本是“随着时代的发展，五华正以崭新的姿态迎接未来”，包含的情绪词典是：正在改善的/正在改进的(improving):0.5,未来/将来(future):0.0"}, "不断完善的基础设施，日益优化的营商环境，吸引着越来越多的人前来投资兴业、安居乐业": {"topic": "“生产投资”", "similarity": 0.5416292548179626, "prompt": "新闻文本是“不断完善的基础设施，日益优化的营商环境，吸引着越来越多的人前来投资兴业、安居乐业”，包含的情绪词典是：投资/投资额(investment):0.4,正在改善的/正在改进的(improving):0.5"}, "教育、医疗等各项事业蓬勃发展，为五华的未来奠定了坚实的基础": {"topic": "“生产投资”", "similarity": 0.4347658157348633, "prompt": "新闻文本是“教育、医疗等各项事业蓬勃发展，为五华的未来奠定了坚实的基础”，包含的情绪词典是：繁荣/兴旺(prospering):0.7,增长/发展(growth):0.7"}, "相约五华，常来长乐，乐不停，乐不止，总有说不完的理由，道不尽的情愫": {"topic": "“消费”", "similarity": 0.44261258840560913, "prompt": "新闻文本是“相约五华，常来长乐，乐不停，乐不止，总有说不完的理由，道不尽的情愫”，包含的情绪词典是：快乐/乐趣(pleasure):0.6,令人愉快的/可享受的(enjoyable):0.6"}, "文：南方日报记者黄培强（文章来源：南方日报）": {"topic": "“消费”", "similarity": 0.43006467819213867, "prompt": "新闻文本是“文：南方日报记者黄培强（文章来源：南方日报）”，包含的情绪词典是：强加/征收(imposition):-0.3,强迫/强制(compulsion):-0.1"}}</t>
+          <t>{"龙龙高铁梅龙段（梅龙高铁）预计9月具备开通运营条件，目前已进入试运行阶段": {"topic": "“生产投资”", "similarity": 0.44007110595703125, "prompt": "新闻文本是“龙龙高铁梅龙段（梅龙高铁）预计9月具备开通运营条件，目前已进入试运行阶段”，包含的情绪词典是：试验性的/暂定的(tentative):0.0,初步的/预备性的(preliminary):0.0"}, "届时广州、深圳等粤港澳大湾区城市到五华的最短通行时间将缩至1.5小时左右": {"topic": "“生产投资”", "similarity": 0.44349926710128784, "prompt": "新闻文本是“届时广州、深圳等粤港澳大湾区城市到五华的最短通行时间将缩至1.5小时左右”，包含的情绪词典是：收缩/缩小(contracting):0.0,减少/缩小(diminution):-0.4"}, "作为梅州人口最多的一个县，五华将因梅龙高铁的开通迎来新机遇": {"topic": "“生产投资”", "similarity": 0.47375768423080444, "prompt": "新闻文本是“作为梅州人口最多的一个县，五华将因梅龙高铁的开通迎来新机遇”，包含的情绪词典是：机会/时机(opportunity):0.5,繁荣/兴旺(prospering):0.7"}, "即日起，《南方日报·五华视窗》推出“坐高铁，来五华，常来长乐”栏目，借光影之手，感五华之美，带您玩转五华这个宝藏小城": {"topic": "“消费”", "similarity": 0.43514424562454224, "prompt": "新闻文本是“即日起，《南方日报·五华视窗》推出“坐高铁，来五华，常来长乐”栏目，借光影之手，感五华之美，带您玩转五华这个宝藏小城”，包含的情绪词典是：令人愉快的/可享受的(enjoyable):0.6,享受/喜爱(enjoyment):0.5"}, "当350公里时速的梅龙高铁疾驰而过，穿越历史底蕴深厚的五华县，历史与现代在这座岭南小城发出最诚挚的邀请：相约五华，常来长乐": {"topic": "“消费”", "similarity": 0.4651843309402466, "prompt": "新闻文本是“当350公里时速的梅龙高铁疾驰而过，穿越历史底蕴深厚的五华县，历史与现代在这座岭南小城发出最诚挚的邀请：相约五华，常来长乐”，包含的情绪词典是：在某处(somewhere):0.0,令人愉快的/可享受的(enjoyable):0.6"}, "工匠之乡、足球之乡、文化之乡、诗词之乡、戏剧之乡，走进五华，如同翻阅一本厚厚的客家历史，粗看回味，细看惊叹": {"topic": "“生产投资”", "similarity": 0.45238977670669556, "prompt": "新闻文本是“工匠之乡、足球之乡、文化之乡、诗词之乡、戏剧之乡，走进五华，如同翻阅一本厚厚的客家历史，粗看回味，细看惊叹”，包含的情绪词典是：中国的/中国人的(chinese):0.0,地方的/当地的(local):0.0"}, "用“高铁速度”寻味岭南风光，五华这座宝藏小城总会给你惊喜，或是城市的喧嚣，或是乡野的宁静，自然和谐共生的乐趣从不缺失，以绿色为主基调的山水五华，养眼更舒心": {"topic": "“消费”", "similarity": 0.48369142413139343, "prompt": "新闻文本是“用“高铁速度”寻味岭南风光，五华这座宝藏小城总会给你惊喜，或是城市的喧嚣，或是乡野的宁静，自然和谐共生的乐趣从不缺失，以绿色为主基调的山水五华，养眼更舒心”，包含的情绪词典是：独特的/有特色的(distinctive):0.0,享受/喜爱(enjoyment):0.5"}, "广东“小千岛湖”益塘水库旅游区、热矿泥温泉度假村、汉光超顺农旅园（黄龙基地）、足球小镇、球王故里文化旅游区奥体中心片区……每一处，都能找到属于自己的打卡方式": {"topic": "“消费”", "similarity": 0.5219109058380127, "prompt": "新闻文本是“广东“小千岛湖”益塘水库旅游区、热矿泥温泉度假村、汉光超顺农旅园（黄龙基地）、足球小镇、球王故里文化旅游区奥体中心片区……每一处，都能找到属于自己的打卡方式”，包含的情绪词典是：在某处(somewhere):0.0"}, "随着时代的发展，五华正以崭新的姿态迎接未来": {"topic": "“生产投资”", "similarity": 0.4479520320892334, "prompt": "新闻文本是“随着时代的发展，五华正以崭新的姿态迎接未来”，包含的情绪词典是：正在改善的/正在改进的(improving):0.5,未来/将来(future):0.0"}, "不断完善的基础设施，日益优化的营商环境，吸引着越来越多的人前来投资兴业、安居乐业": {"topic": "“生产投资”", "similarity": 0.5416293740272522, "prompt": "新闻文本是“不断完善的基础设施，日益优化的营商环境，吸引着越来越多的人前来投资兴业、安居乐业”，包含的情绪词典是：投资/投资额(investment):0.4,正在改善的/正在改进的(improving):0.5"}, "教育、医疗等各项事业蓬勃发展，为五华的未来奠定了坚实的基础": {"topic": "“生产投资”", "similarity": 0.43476590514183044, "prompt": "新闻文本是“教育、医疗等各项事业蓬勃发展，为五华的未来奠定了坚实的基础”，包含的情绪词典是：繁荣/兴旺(prospering):0.7,增长/发展(growth):0.7"}, "相约五华，常来长乐，乐不停，乐不止，总有说不完的理由，道不尽的情愫": {"topic": "“消费”", "similarity": 0.44261276721954346, "prompt": "新闻文本是“相约五华，常来长乐，乐不停，乐不止，总有说不完的理由，道不尽的情愫”，包含的情绪词典是：快乐/乐趣(pleasure):0.6,令人愉快的/可享受的(enjoyable):0.6"}}</t>
         </is>
       </c>
     </row>
@@ -1454,12 +1446,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月30日，光伏ETF指数基金(159618.SZ)收涨0.95%，成交580.33万元", "news_prompt2": "净流出796.35万元（净赎回份额*单位净值），居可比基金前二", "news_prompt3": "拉长时间看，该基金连续3天资金净流出，累计流出1682.62万元，居全市场第一梯队", "news_prompt4": "资金流出也带来了份额的减少，该基金最新份额较前一日减少1500.00万份，跌破2.50亿份，居可比基金倒数前二", "news_prompt5": "与此同时，该基金最新规模达1.30亿元，居可比基金倒数前二", "news_prompt6": "光伏ETF指数基金(159618.SZ)，场外联接(A：013105", "news_prompt7": "C：013106)", "news_prompt8": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "2024年8月30日，光伏ETF指数基金(159618.SZ)收涨0.95%，成交580.33万元", "news_prompt2": "净流出796.35万元（净赎回份额*单位净值），居可比基金前二", "news_prompt3": "拉长时间看，该基金连续3天资金净流出，累计流出1682.62万元，居全市场第一梯队", "news_prompt4": "资金流出也带来了份额的减少，该基金最新份额较前一日减少1500.00万份，跌破2.50亿份，居可比基金倒数前二", "news_prompt5": "与此同时，该基金最新规模达1.30亿元，居可比基金倒数前二", "news_prompt6": "光伏ETF指数基金(159618.SZ)，场外联接(A：013105", "news_prompt7": "C：013106)"}</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>{"2024年8月30日，光伏ETF指数基金(159618.SZ)收涨0.95%，成交580.33万元": {"topic": "“生产投资”", "similarity": 0.467471718788147, "prompt": "新闻文本是“2024年8月30日，光伏ETF指数基金(159618.SZ)收涨0.95%，成交580.33万元”，包含的情绪词典是：基金/资金(fund):0.1,股票/库存(stock):0.0"}, "净流出796.35万元（净赎回份额*单位净值），居可比基金前二": {"topic": "“金融”", "similarity": 0.5074794888496399, "prompt": "新闻文本是“净流出796.35万元（净赎回份额*单位净值），居可比基金前二”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeout):-0.2"}, "拉长时间看，该基金连续3天资金净流出，累计流出1682.62万元，居全市场第一梯队": {"topic": "“金融”", "similarity": 0.5325808525085449, "prompt": "新闻文本是“拉长时间看，该基金连续3天资金净流出，累计流出1682.62万元，居全市场第一梯队”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeouts):-0.2"}, "资金流出也带来了份额的减少，该基金最新份额较前一日减少1500.00万份，跌破2.50亿份，居可比基金倒数前二": {"topic": "“金融”", "similarity": 0.5628052949905396, "prompt": "新闻文本是“资金流出也带来了份额的减少，该基金最新份额较前一日减少1500.00万份，跌破2.50亿份，居可比基金倒数前二”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退/低迷(downturn):-0.6"}, "与此同时，该基金最新规模达1.30亿元，居可比基金倒数前二": {"topic": "“金融”", "similarity": 0.46741318702697754, "prompt": "新闻文本是“与此同时，该基金最新规模达1.30亿元，居可比基金倒数前二”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "光伏ETF指数基金(159618.SZ)，场外联接(A：013105": {"topic": "“金融”", "similarity": 0.49143311381340027, "prompt": "新闻文本是“光伏ETF指数基金(159618.SZ)，场外联接(A：013105”，包含的情绪词典是：基金/资金(fund):0.1,指数/指标(index):0.0"}, "C：013106)": {"topic": "“金融”", "similarity": 0.43629276752471924, "prompt": "新闻文本是“C：013106)”，包含的情绪词典是：数字/数位(digit):0.0,事故/意外(accident):-0.3"}}</t>
+          <t>{"2024年8月30日，光伏ETF指数基金(159618.SZ)收涨0.95%，成交580.33万元": {"topic": "“生产投资”", "similarity": 0.4674718379974365, "prompt": "新闻文本是“2024年8月30日，光伏ETF指数基金(159618.SZ)收涨0.95%，成交580.33万元”，包含的情绪词典是：基金/资金(fund):0.1,股票/库存(stock):0.0"}, "净流出796.35万元（净赎回份额*单位净值），居可比基金前二": {"topic": "“金融”", "similarity": 0.5074796080589294, "prompt": "新闻文本是“净流出796.35万元（净赎回份额*单位净值），居可比基金前二”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeout):-0.2"}, "拉长时间看，该基金连续3天资金净流出，累计流出1682.62万元，居全市场第一梯队": {"topic": "“金融”", "similarity": 0.532581090927124, "prompt": "新闻文本是“拉长时间看，该基金连续3天资金净流出，累计流出1682.62万元，居全市场第一梯队”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeouts):-0.2"}, "资金流出也带来了份额的减少，该基金最新份额较前一日减少1500.00万份，跌破2.50亿份，居可比基金倒数前二": {"topic": "“金融”", "similarity": 0.5628054141998291, "prompt": "新闻文本是“资金流出也带来了份额的减少，该基金最新份额较前一日减少1500.00万份，跌破2.50亿份，居可比基金倒数前二”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退/低迷(downturn):-0.6"}, "与此同时，该基金最新规模达1.30亿元，居可比基金倒数前二": {"topic": "“金融”", "similarity": 0.46741342544555664, "prompt": "新闻文本是“与此同时，该基金最新规模达1.30亿元，居可比基金倒数前二”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "光伏ETF指数基金(159618.SZ)，场外联接(A：013105": {"topic": "“金融”", "similarity": 0.4914332628250122, "prompt": "新闻文本是“光伏ETF指数基金(159618.SZ)，场外联接(A：013105”，包含的情绪词典是：基金/资金(fund):0.1,指数/指标(index):0.0"}, "C：013106)": {"topic": "“金融”", "similarity": 0.43629276752471924, "prompt": "新闻文本是“C：013106)”，包含的情绪词典是：数字/数位(digit):0.0,事故/意外(accident):-0.3"}}</t>
         </is>
       </c>
     </row>
@@ -1505,12 +1497,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上证报中国证券网讯 9月2日早盘，社会服务板块震荡上行", "news_prompt2": "截至9时55分，中国高科涨超6%，祥源文旅涨逾4%，中公教育、长白山、三特索道等跟涨", "news_prompt3": "（文章来源：上海证券报·中国证券网）"}</t>
+          <t>{"news_prompt1": "上证报中国证券网讯 9月2日早盘，社会服务板块震荡上行", "news_prompt2": "截至9时55分，中国高科涨超6%，祥源文旅涨逾4%，中公教育、长白山、三特索道等跟涨"}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"上证报中国证券网讯 9月2日早盘，社会服务板块震荡上行": {"topic": "“金融”", "similarity": 0.44361913204193115, "prompt": "新闻文本是“上证报中国证券网讯 9月2日早盘，社会服务板块震荡上行”，包含的情绪词典是：冲击/波动(buffet):0.0,服务/业务(service):0.0"}, "截至9时55分，中国高科涨超6%，祥源文旅涨逾4%，中公教育、长白山、三特索道等跟涨": {"topic": "“金融”", "similarity": 0.5373921394348145, "prompt": "新闻文本是“截至9时55分，中国高科涨超6%，祥源文旅涨逾4%，中公教育、长白山、三特索道等跟涨”，包含的情绪词典是：高的/高等的(high):0.7,上升/上涨(rise):0.5"}, "（文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.4783601760864258, "prompt": "新闻文本是“（文章来源：上海证券报·中国证券网）”，包含的情绪词典是：投资者/投资人(investor):0.4,股票/库存(stock):0.0"}}</t>
+          <t>{"上证报中国证券网讯 9月2日早盘，社会服务板块震荡上行": {"topic": "“金融”", "similarity": 0.4436192512512207, "prompt": "新闻文本是“上证报中国证券网讯 9月2日早盘，社会服务板块震荡上行”，包含的情绪词典是：冲击/波动(buffet):0.0,服务/业务(service):0.0"}, "截至9时55分，中国高科涨超6%，祥源文旅涨逾4%，中公教育、长白山、三特索道等跟涨": {"topic": "“金融”", "similarity": 0.5373921990394592, "prompt": "新闻文本是“截至9时55分，中国高科涨超6%，祥源文旅涨逾4%，中公教育、长白山、三特索道等跟涨”，包含的情绪词典是：高的/高等的(high):0.7,上升/上涨(rise):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -1560,12 +1552,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日，#小天鹅被羊毛党一夜薅走7000万#登上微博热搜", "news_prompt2": "该事件源于8月28日凌晨，一家安徽县城只有6人的淘宝小店遭遇“灭顶之灾”，由于电商运营人员价格设置错误，该店铺20分钟内以进货价4~5折的价格“卖出”货值超7000万元的货品", "news_prompt3": "据“小天鹅东山专卖店”公告，由于运营人员价格设置错误，导致全店洗衣机产品以远低于市场价的价格售出，在短短的20分钟内有近4万个订单，其中大部分订单为一人多单多台，据核算，本次事件下单金额近4000万元，货值超7000万元，这意味着如果按规定发货该店将直接损失超3000万元", "news_prompt4": "最终，该店铺为这近4万个订单做退款处理", "news_prompt5": "与此同时，不少网友在社交媒体爆料称，8月28日晚因“小天鹅东山专卖店”出现价格设置错误，以超低价格买到了洗衣机，甚至还有不少人以该价格下了4~5单并寻求转手", "news_prompt6": "而那些大肆扫货的“羊毛党”之所以消息灵通，是因为出现低价bug后，有人在群里号召，互相通知，“羊毛党”再纷纷出动下单", "news_prompt7": "除了小天鹅东山专卖店，8月28日凌晨，天猫的林氏旗舰店、华帝官方旗舰店也出现了超低价销售的情况", "news_prompt8": "一些产品的优惠折扣甚至低至1~2折，短时间内被多位消费者抢购", "news_prompt9": "华帝是1992年成立于广东中山的一家厨房燃具品牌", "news_prompt10": "林氏则是2007年成立于广东的一家家居品牌", "news_prompt11": "目前，对于28日凌晨0点“活动”为什么会出现这个bug，而且几家品牌同时出现问题，天猫并没有给出解释", "news_prompt12": "在买到低价货后，“羊毛党”们有自己的“发财”之路——进行二次售卖", "news_prompt13": "比如一位拍下华帝产品的消费者称，他低价拍下的华帝抽油烟机产品可一台加价200元出", "news_prompt14": "一位连拍5单林氏产品并在社交平台上公开售卖的消费者也称，低价销售的消息是在她加入的微信群里看见的，她看见了就拍了，若有人想买，她就以实拍的价格加价出，床、梳妆台类大件加价100元或者80元，懒人椅、凳子等加30元即可，可走咸鱼平台付款", "news_prompt15": "“如若店家发货，在淘宝上直接修改地址", "news_prompt16": "店家若不发货，也可直接咸鱼平台退款", "news_prompt17": "” 　　上述消费者还表示：“这种群里有许多黄牛，他们花时间去蹲低价的东西，再加价卖给你，但不会加很多，还是会低于商家的售卖价", "news_prompt18": "等于他们多花时间，你多花钱", "news_prompt19": "专业搞这种的一般都五六个手机，专门赚差价", "news_prompt20": "” 　　这次事件暴露了电商运营中潜在的风险，尤其是价格设置错误可能带来的巨大损失", "news_prompt21": "值得注意的是，“薅羊毛”行为虽然在表面上看似是利用商家失误获取优惠，但实际上，当这种行为达到一定规模，就可能触及法律界限", "news_prompt22": "《上海市长宁区2018-2020年诈骗犯罪刑事检察白皮书》中记录了一起案例，有人因从电商平台“薅羊毛”高达510余万元而被追究刑事责任", "news_prompt23": "对于消费者而言，追求“优惠”无可厚非的，但以不法手段或侥幸心理“薅羊毛”则很有可能触及法律禁区", "news_prompt24": "（时代财经记者张汀雯，综合自蓝鲸新闻、正在新闻、中华网", "news_prompt25": "）（文章来源：时代财经）"}</t>
+          <t>{"news_prompt1": "9月2日，#小天鹅被羊毛党一夜薅走7000万#登上微博热搜", "news_prompt2": "该事件源于8月28日凌晨，一家安徽县城只有6人的淘宝小店遭遇“灭顶之灾”，由于电商运营人员价格设置错误，该店铺20分钟内以进货价4~5折的价格“卖出”货值超7000万元的货品", "news_prompt3": "据“小天鹅东山专卖店”公告，由于运营人员价格设置错误，导致全店洗衣机产品以远低于市场价的价格售出，在短短的20分钟内有近4万个订单，其中大部分订单为一人多单多台，据核算，本次事件下单金额近4000万元，货值超7000万元，这意味着如果按规定发货该店将直接损失超3000万元", "news_prompt4": "与此同时，不少网友在社交媒体爆料称，8月28日晚因“小天鹅东山专卖店”出现价格设置错误，以超低价格买到了洗衣机，甚至还有不少人以该价格下了4~5单并寻求转手", "news_prompt5": "而那些大肆扫货的“羊毛党”之所以消息灵通，是因为出现低价bug后，有人在群里号召，互相通知，“羊毛党”再纷纷出动下单", "news_prompt6": "一些产品的优惠折扣甚至低至1~2折，短时间内被多位消费者抢购", "news_prompt7": "华帝是1992年成立于广东中山的一家厨房燃具品牌", "news_prompt8": "林氏则是2007年成立于广东的一家家居品牌", "news_prompt9": "在买到低价货后，“羊毛党”们有自己的“发财”之路——进行二次售卖", "news_prompt10": "比如一位拍下华帝产品的消费者称，他低价拍下的华帝抽油烟机产品可一台加价200元出", "news_prompt11": "” 　　上述消费者还表示：“这种群里有许多黄牛，他们花时间去蹲低价的东西，再加价卖给你，但不会加很多，还是会低于商家的售卖价", "news_prompt12": "等于他们多花时间，你多花钱", "news_prompt13": "专业搞这种的一般都五六个手机，专门赚差价", "news_prompt14": "” 　　这次事件暴露了电商运营中潜在的风险，尤其是价格设置错误可能带来的巨大损失", "news_prompt15": "值得注意的是，“薅羊毛”行为虽然在表面上看似是利用商家失误获取优惠，但实际上，当这种行为达到一定规模，就可能触及法律界限", "news_prompt16": "《上海市长宁区2018-2020年诈骗犯罪刑事检察白皮书》中记录了一起案例，有人因从电商平台“薅羊毛”高达510余万元而被追究刑事责任", "news_prompt17": "对于消费者而言，追求“优惠”无可厚非的，但以不法手段或侥幸心理“薅羊毛”则很有可能触及法律禁区", "news_prompt18": "（时代财经记者张汀雯，综合自蓝鲸新闻、正在新闻、中华网"}</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>{"9月2日，#小天鹅被羊毛党一夜薅走7000万#登上微博热搜": {"topic": "“消费”", "similarity": 0.4662685990333557, "prompt": "新闻文本是“9月2日，#小天鹅被羊毛党一夜薅走7000万#登上微博热搜”，包含的情绪词典是：征收/没收(expropriation):-0.6,追回款/回收款(clawbacks):0.0"}, "该事件源于8月28日凌晨，一家安徽县城只有6人的淘宝小店遭遇“灭顶之灾”，由于电商运营人员价格设置错误，该店铺20分钟内以进货价4~5折的价格“卖出”货值超7000万元的货品": {"topic": "“消费”", "similarity": 0.5397298336029053, "prompt": "新闻文本是“该事件源于8月28日凌晨，一家安徽县城只有6人的淘宝小店遭遇“灭顶之灾”，由于电商运营人员价格设置错误，该店铺20分钟内以进货价4~5折的价格“卖出”货值超7000万元的货品”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,错价/定价错误(misprice):-0.35"}, "据“小天鹅东山专卖店”公告，由于运营人员价格设置错误，导致全店洗衣机产品以远低于市场价的价格售出，在短短的20分钟内有近4万个订单，其中大部分订单为一人多单多台，据核算，本次事件下单金额近4000万元，货值超7000万元，这意味着如果按规定发货该店将直接损失超3000万元": {"topic": "“消费”", "similarity": 0.5494963526725769, "prompt": "新闻文本是“据“小天鹅东山专卖店”公告，由于运营人员价格设置错误，导致全店洗衣机产品以远低于市场价的价格售出，在短短的20分钟内有近4万个订单，其中大部分订单为一人多单多台，据核算，本次事件下单金额近4000万元，货值超7000万元，这意味着如果按规定发货该店将直接损失超3000万元”，包含的情绪词典是：削价/低价出售(undercut):-0.3,错价/定价错误(mispricing):-0.4"}, "与此同时，不少网友在社交媒体爆料称，8月28日晚因“小天鹅东山专卖店”出现价格设置错误，以超低价格买到了洗衣机，甚至还有不少人以该价格下了4~5单并寻求转手": {"topic": "“消费”", "similarity": 0.5172284841537476, "prompt": "新闻文本是“与此同时，不少网友在社交媒体爆料称，8月28日晚因“小天鹅东山专卖店”出现价格设置错误，以超低价格买到了洗衣机，甚至还有不少人以该价格下了4~5单并寻求转手”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,错价/定价错误(misprice):-0.35"}, "而那些大肆扫货的“羊毛党”之所以消息灵通，是因为出现低价bug后，有人在群里号召，互相通知，“羊毛党”再纷纷出动下单": {"topic": "“消费”", "similarity": 0.5024923086166382, "prompt": "新闻文本是“而那些大肆扫货的“羊毛党”之所以消息灵通，是因为出现低价bug后，有人在群里号召，互相通知，“羊毛党”再纷纷出动下单”，包含的情绪词典是：削价/低价出售(undercuts):-0.3,削价/低价出售(undercut):-0.3"}, "一些产品的优惠折扣甚至低至1~2折，短时间内被多位消费者抢购": {"topic": "“消费”", "similarity": 0.49651479721069336, "prompt": "新闻文本是“一些产品的优惠折扣甚至低至1~2折，短时间内被多位消费者抢购”，包含的情绪词典是：削价/低价出售(undercut):-0.3,削价/低价出售(undercuts):-0.3"}, "华帝是1992年成立于广东中山的一家厨房燃具品牌": {"topic": "“消费”", "similarity": 0.4304659366607666, "prompt": "新闻文本是“华帝是1992年成立于广东中山的一家厨房燃具品牌”，包含的情绪词典是：消费者/用户(consumer):0.0,生产/制造(produce):0.3"}, "林氏则是2007年成立于广东的一家家居品牌": {"topic": "“消费”", "similarity": 0.45983749628067017, "prompt": "新闻文本是“林氏则是2007年成立于广东的一家家居品牌”，包含的情绪词典是：企业/事业(enterprise):0.0,品牌/商标(brand):0.0"}, "目前，对于28日凌晨0点“活动”为什么会出现这个bug，而且几家品牌同时出现问题，天猫并没有给出解释": {"topic": "“消费”", "similarity": 0.49783486127853394}, "在买到低价货后，“羊毛党”们有自己的“发财”之路——进行二次售卖": {"topic": "“消费”", "similarity": 0.43990957736968994, "prompt": "新闻文本是“在买到低价货后，“羊毛党”们有自己的“发财”之路——进行二次售卖”，包含的情绪词典是：削价/低价出售(undercuts):-0.3,削价/低价出售(undercut):-0.3"}, "比如一位拍下华帝产品的消费者称，他低价拍下的华帝抽油烟机产品可一台加价200元出": {"topic": "“消费”", "similarity": 0.4770805835723877, "prompt": "新闻文本是“比如一位拍下华帝产品的消费者称，他低价拍下的华帝抽油烟机产品可一台加价200元出”，包含的情绪词典是：消费者/用户(consumer):0.0,削价/低价出售(undercut):-0.3"}, "一位连拍5单林氏产品并在社交平台上公开售卖的消费者也称，低价销售的消息是在她加入的微信群里看见的，她看见了就拍了，若有人想买，她就以实拍的价格加价出，床、梳妆台类大件加价100元或者80元，懒人椅、凳子等加30元即可，可走咸鱼平台付款": {"topic": "“消费”", "similarity": 0.49131688475608826}, "” 　　上述消费者还表示：“这种群里有许多黄牛，他们花时间去蹲低价的东西，再加价卖给你，但不会加很多，还是会低于商家的售卖价": {"topic": "“消费”", "similarity": 0.5004439353942871, "prompt": "新闻文本是“” 　　上述消费者还表示：“这种群里有许多黄牛，他们花时间去蹲低价的东西，再加价卖给你，但不会加很多，还是会低于商家的售卖价”，包含的情绪词典是：消费者/用户(consumer):0.0,削价/低价出售(undercuts):-0.3"}, "等于他们多花时间，你多花钱": {"topic": "“消费”", "similarity": 0.424648642539978, "prompt": "新闻文本是“等于他们多花时间，你多花钱”，包含的情绪词典是：多付的/支付过多的(overpaid):-0.3,多付/支付过多(overpayment):-0.3"}, "专业搞这种的一般都五六个手机，专门赚差价": {"topic": "“消费”", "similarity": 0.4588134288787842, "prompt": "新闻文本是“专业搞这种的一般都五六个手机，专门赚差价”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,多才多艺的/多功能的(versatile):0.3"}, "” 　　这次事件暴露了电商运营中潜在的风险，尤其是价格设置错误可能带来的巨大损失": {"topic": "“通货膨胀”", "similarity": 0.4374816417694092, "prompt": "新闻文本是“” 　　这次事件暴露了电商运营中潜在的风险，尤其是价格设置错误可能带来的巨大损失”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,错价/定价错误(misprice):-0.35"}, "值得注意的是，“薅羊毛”行为虽然在表面上看似是利用商家失误获取优惠，但实际上，当这种行为达到一定规模，就可能触及法律界限": {"topic": "“消费”", "similarity": 0.5694487690925598, "prompt": "新闻文本是“值得注意的是，“薅羊毛”行为虽然在表面上看似是利用商家失误获取优惠，但实际上，当这种行为达到一定规模，就可能触及法律界限”，包含的情绪词典是：不法行为/坏事(wrongdoing):-0.5,不正当的/不合法的(wrongful):-0.6"}, "《上海市长宁区2018-2020年诈骗犯罪刑事检察白皮书》中记录了一起案例，有人因从电商平台“薅羊毛”高达510余万元而被追究刑事责任": {"topic": "“消费”", "similarity": 0.5665444731712341, "prompt": "新闻文本是“《上海市长宁区2018-2020年诈骗犯罪刑事检察白皮书》中记录了一起案例，有人因从电商平台“薅羊毛”高达510余万元而被追究刑事责任”，包含的情绪词典是：被诈骗的/受骗的(defrauded):-0.5,欺骗性的/欺诈性的(deceptive):-0.5"}, "对于消费者而言，追求“优惠”无可厚非的，但以不法手段或侥幸心理“薅羊毛”则很有可能触及法律禁区": {"topic": "“消费”", "similarity": 0.5283695459365845, "prompt": "新闻文本是“对于消费者而言，追求“优惠”无可厚非的，但以不法手段或侥幸心理“薅羊毛”则很有可能触及法律禁区”，包含的情绪词典是：非法的/不合法的(unlawful):-0.6,不正当的/不合法的(wrongful):-0.6"}, "（时代财经记者张汀雯，综合自蓝鲸新闻、正在新闻、中华网": {"topic": "“生产投资”", "similarity": 0.6035628914833069, "prompt": "新闻文本是“（时代财经记者张汀雯，综合自蓝鲸新闻、正在新闻、中华网”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "）（文章来源：时代财经）": {"topic": "“金融”", "similarity": 0.4212809205055237, "prompt": "新闻文本是“）（文章来源：时代财经）”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}}</t>
+          <t>{"9月2日，#小天鹅被羊毛党一夜薅走7000万#登上微博热搜": {"topic": "“消费”", "similarity": 0.4662685990333557, "prompt": "新闻文本是“9月2日，#小天鹅被羊毛党一夜薅走7000万#登上微博热搜”，包含的情绪词典是：征收/没收(expropriation):-0.6,追回款/回收款(clawbacks):0.0"}, "该事件源于8月28日凌晨，一家安徽县城只有6人的淘宝小店遭遇“灭顶之灾”，由于电商运营人员价格设置错误，该店铺20分钟内以进货价4~5折的价格“卖出”货值超7000万元的货品": {"topic": "“消费”", "similarity": 0.5397297739982605, "prompt": "新闻文本是“该事件源于8月28日凌晨，一家安徽县城只有6人的淘宝小店遭遇“灭顶之灾”，由于电商运营人员价格设置错误，该店铺20分钟内以进货价4~5折的价格“卖出”货值超7000万元的货品”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,错价/定价错误(misprice):-0.35"}, "据“小天鹅东山专卖店”公告，由于运营人员价格设置错误，导致全店洗衣机产品以远低于市场价的价格售出，在短短的20分钟内有近4万个订单，其中大部分订单为一人多单多台，据核算，本次事件下单金额近4000万元，货值超7000万元，这意味着如果按规定发货该店将直接损失超3000万元": {"topic": "“消费”", "similarity": 0.5494963526725769, "prompt": "新闻文本是“据“小天鹅东山专卖店”公告，由于运营人员价格设置错误，导致全店洗衣机产品以远低于市场价的价格售出，在短短的20分钟内有近4万个订单，其中大部分订单为一人多单多台，据核算，本次事件下单金额近4000万元，货值超7000万元，这意味着如果按规定发货该店将直接损失超3000万元”，包含的情绪词典是：削价/低价出售(undercut):-0.3,错价/定价错误(mispricing):-0.4"}, "与此同时，不少网友在社交媒体爆料称，8月28日晚因“小天鹅东山专卖店”出现价格设置错误，以超低价格买到了洗衣机，甚至还有不少人以该价格下了4~5单并寻求转手": {"topic": "“消费”", "similarity": 0.5172284841537476, "prompt": "新闻文本是“与此同时，不少网友在社交媒体爆料称，8月28日晚因“小天鹅东山专卖店”出现价格设置错误，以超低价格买到了洗衣机，甚至还有不少人以该价格下了4~5单并寻求转手”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,错价/定价错误(misprice):-0.35"}, "而那些大肆扫货的“羊毛党”之所以消息灵通，是因为出现低价bug后，有人在群里号召，互相通知，“羊毛党”再纷纷出动下单": {"topic": "“消费”", "similarity": 0.5024924278259277, "prompt": "新闻文本是“而那些大肆扫货的“羊毛党”之所以消息灵通，是因为出现低价bug后，有人在群里号召，互相通知，“羊毛党”再纷纷出动下单”，包含的情绪词典是：削价/低价出售(undercuts):-0.3,削价/低价出售(undercut):-0.3"}, "一些产品的优惠折扣甚至低至1~2折，短时间内被多位消费者抢购": {"topic": "“消费”", "similarity": 0.49651506543159485, "prompt": "新闻文本是“一些产品的优惠折扣甚至低至1~2折，短时间内被多位消费者抢购”，包含的情绪词典是：削价/低价出售(undercut):-0.3,削价/低价出售(undercuts):-0.3"}, "华帝是1992年成立于广东中山的一家厨房燃具品牌": {"topic": "“消费”", "similarity": 0.43046602606773376, "prompt": "新闻文本是“华帝是1992年成立于广东中山的一家厨房燃具品牌”，包含的情绪词典是：消费者/用户(consumer):0.0,生产/制造(produce):0.3"}, "林氏则是2007年成立于广东的一家家居品牌": {"topic": "“消费”", "similarity": 0.4598376154899597, "prompt": "新闻文本是“林氏则是2007年成立于广东的一家家居品牌”，包含的情绪词典是：企业/事业(enterprise):0.0,品牌/商标(brand):0.0"}, "在买到低价货后，“羊毛党”们有自己的“发财”之路——进行二次售卖": {"topic": "“消费”", "similarity": 0.43990981578826904, "prompt": "新闻文本是“在买到低价货后，“羊毛党”们有自己的“发财”之路——进行二次售卖”，包含的情绪词典是：削价/低价出售(undercuts):-0.3,削价/低价出售(undercut):-0.3"}, "比如一位拍下华帝产品的消费者称，他低价拍下的华帝抽油烟机产品可一台加价200元出": {"topic": "“消费”", "similarity": 0.47708070278167725, "prompt": "新闻文本是“比如一位拍下华帝产品的消费者称，他低价拍下的华帝抽油烟机产品可一台加价200元出”，包含的情绪词典是：消费者/用户(consumer):0.0,削价/低价出售(undercut):-0.3"}, "” 　　上述消费者还表示：“这种群里有许多黄牛，他们花时间去蹲低价的东西，再加价卖给你，但不会加很多，还是会低于商家的售卖价": {"topic": "“消费”", "similarity": 0.5004442930221558, "prompt": "新闻文本是“” 　　上述消费者还表示：“这种群里有许多黄牛，他们花时间去蹲低价的东西，再加价卖给你，但不会加很多，还是会低于商家的售卖价”，包含的情绪词典是：消费者/用户(consumer):0.0,削价/低价出售(undercuts):-0.3"}, "等于他们多花时间，你多花钱": {"topic": "“消费”", "similarity": 0.4246487021446228, "prompt": "新闻文本是“等于他们多花时间，你多花钱”，包含的情绪词典是：多付的/支付过多的(overpaid):-0.3,多付/支付过多(overpayment):-0.3"}, "专业搞这种的一般都五六个手机，专门赚差价": {"topic": "“消费”", "similarity": 0.45881354808807373, "prompt": "新闻文本是“专业搞这种的一般都五六个手机，专门赚差价”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,多才多艺的/多功能的(versatile):0.3"}, "” 　　这次事件暴露了电商运营中潜在的风险，尤其是价格设置错误可能带来的巨大损失": {"topic": "“通货膨胀”", "similarity": 0.4374820291996002, "prompt": "新闻文本是“” 　　这次事件暴露了电商运营中潜在的风险，尤其是价格设置错误可能带来的巨大损失”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,错价/定价错误(misprice):-0.35"}, "值得注意的是，“薅羊毛”行为虽然在表面上看似是利用商家失误获取优惠，但实际上，当这种行为达到一定规模，就可能触及法律界限": {"topic": "“消费”", "similarity": 0.5694488286972046, "prompt": "新闻文本是“值得注意的是，“薅羊毛”行为虽然在表面上看似是利用商家失误获取优惠，但实际上，当这种行为达到一定规模，就可能触及法律界限”，包含的情绪词典是：不法行为/坏事(wrongdoing):-0.5,不正当的/不合法的(wrongful):-0.6"}, "《上海市长宁区2018-2020年诈骗犯罪刑事检察白皮书》中记录了一起案例，有人因从电商平台“薅羊毛”高达510余万元而被追究刑事责任": {"topic": "“消费”", "similarity": 0.5665445923805237, "prompt": "新闻文本是“《上海市长宁区2018-2020年诈骗犯罪刑事检察白皮书》中记录了一起案例，有人因从电商平台“薅羊毛”高达510余万元而被追究刑事责任”，包含的情绪词典是：被诈骗的/受骗的(defrauded):-0.5,欺骗性的/欺诈性的(deceptive):-0.5"}, "对于消费者而言，追求“优惠”无可厚非的，但以不法手段或侥幸心理“薅羊毛”则很有可能触及法律禁区": {"topic": "“消费”", "similarity": 0.5283697843551636, "prompt": "新闻文本是“对于消费者而言，追求“优惠”无可厚非的，但以不法手段或侥幸心理“薅羊毛”则很有可能触及法律禁区”，包含的情绪词典是：非法的/不合法的(unlawful):-0.6,不正当的/不合法的(wrongful):-0.6"}, "（时代财经记者张汀雯，综合自蓝鲸新闻、正在新闻、中华网": {"topic": "“生产投资”", "similarity": 0.6035630702972412, "prompt": "新闻文本是“（时代财经记者张汀雯，综合自蓝鲸新闻、正在新闻、中华网”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -1611,12 +1603,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "为进一步推广合同节水管理，发挥典型案例示范引领作用，助力节水产业发展，水利部组织开展了合同节水管理典型案例征集遴选，择优推出39个合同节水管理典型案例，形成了一批可复制推广的经验做法", "news_prompt2": "推广合同节水管理是发展节水产业的重要举措，是水利行业贯彻落实习近平总书记“节水优先、空间均衡、系统治理、两手发力”治水思路和关于治水重要论述精神的生动实践", "news_prompt3": "水利部高度重视合同节水管理工作，通过加强顶层设计、建立标准体系、搭建信息平台、开展宣传指导等举措，推动实施了800多项合同节水管理项目，吸引社会资本近90亿元，为推动节水创新链、产业链、资金链、政策链融合发展创造了有利条件", "news_prompt4": "本次入选的合同节水管理典型案例，是从地方推荐的近百项案例中，经过初步审查、专家评审、实地调研、网上公示等环节遴选而出，涵盖了工业、农业、公共机构、供水管网漏损控制、水环境治理等领域", "news_prompt5": "公布的合同节水管理典型案例从不同角度展现了合同节水管理的应用场景、盈利模式和实施成效，着重总结合同节水管理项目实施的主要做法，突出亮点特色，展示先进适用的节水技术和综合管理措施，提炼出“效果保证+效益分享”“用水托管+效益分享”“特许经营+水权交易”“水权交易+综合农事托管服务”等合同节水管理创新模式，充分调动社会资本和用水单位参与节水的积极性", "news_prompt6": "下一步，水利部将指导各地加大合同节水管理典型案例宣传推广力度，开展形式多样、内容丰富的经验分享和技术交流等活动", "news_prompt7": "加强合同节水管理工作跟踪辅导，积极促进用水单位和节水服务企业沟通对接，发挥“节水贷”等绿色金融作用，及时总结提炼经验做法，以点带面推动合同节水管理在重点领域广泛实施", "news_prompt8": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "为进一步推广合同节水管理，发挥典型案例示范引领作用，助力节水产业发展，水利部组织开展了合同节水管理典型案例征集遴选，择优推出39个合同节水管理典型案例，形成了一批可复制推广的经验做法", "news_prompt2": "推广合同节水管理是发展节水产业的重要举措，是水利行业贯彻落实习近平总书记“节水优先、空间均衡、系统治理、两手发力”治水思路和关于治水重要论述精神的生动实践", "news_prompt3": "水利部高度重视合同节水管理工作，通过加强顶层设计、建立标准体系、搭建信息平台、开展宣传指导等举措，推动实施了800多项合同节水管理项目，吸引社会资本近90亿元，为推动节水创新链、产业链、资金链、政策链融合发展创造了有利条件", "news_prompt4": "本次入选的合同节水管理典型案例，是从地方推荐的近百项案例中，经过初步审查、专家评审、实地调研、网上公示等环节遴选而出，涵盖了工业、农业、公共机构、供水管网漏损控制、水环境治理等领域", "news_prompt5": "公布的合同节水管理典型案例从不同角度展现了合同节水管理的应用场景、盈利模式和实施成效，着重总结合同节水管理项目实施的主要做法，突出亮点特色，展示先进适用的节水技术和综合管理措施，提炼出“效果保证+效益分享”“用水托管+效益分享”“特许经营+水权交易”“水权交易+综合农事托管服务”等合同节水管理创新模式，充分调动社会资本和用水单位参与节水的积极性", "news_prompt6": "下一步，水利部将指导各地加大合同节水管理典型案例宣传推广力度，开展形式多样、内容丰富的经验分享和技术交流等活动", "news_prompt7": "加强合同节水管理工作跟踪辅导，积极促进用水单位和节水服务企业沟通对接，发挥“节水贷”等绿色金融作用，及时总结提炼经验做法，以点带面推动合同节水管理在重点领域广泛实施"}</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>{"为进一步推广合同节水管理，发挥典型案例示范引领作用，助力节水产业发展，水利部组织开展了合同节水管理典型案例征集遴选，择优推出39个合同节水管理典型案例，形成了一批可复制推广的经验做法": {"topic": "“生产投资”", "similarity": 0.5162226557731628, "prompt": "新闻文本是“为进一步推广合同节水管理，发挥典型案例示范引领作用，助力节水产业发展，水利部组织开展了合同节水管理典型案例征集遴选，择优推出39个合同节水管理典型案例，形成了一批可复制推广的经验做法”，包含的情绪词典是：合同的/契约的(contractual):0.0,依照合同地/依照契约地(contractually):0.0"}, "推广合同节水管理是发展节水产业的重要举措，是水利行业贯彻落实习近平总书记“节水优先、空间均衡、系统治理、两手发力”治水思路和关于治水重要论述精神的生动实践": {"topic": "“生产投资”", "similarity": 0.538425087928772, "prompt": "新闻文本是“推广合同节水管理是发展节水产业的重要举措，是水利行业贯彻落实习近平总书记“节水优先、空间均衡、系统治理、两手发力”治水思路和关于治水重要论述精神的生动实践”，包含的情绪词典是：合同的/契约的(contractual):0.0,水/水资源(water):0.0"}, "水利部高度重视合同节水管理工作，通过加强顶层设计、建立标准体系、搭建信息平台、开展宣传指导等举措，推动实施了800多项合同节水管理项目，吸引社会资本近90亿元，为推动节水创新链、产业链、资金链、政策链融合发展创造了有利条件": {"topic": "“生产投资”", "similarity": 0.5834358334541321, "prompt": "新闻文本是“水利部高度重视合同节水管理工作，通过加强顶层设计、建立标准体系、搭建信息平台、开展宣传指导等举措，推动实施了800多项合同节水管理项目，吸引社会资本近90亿元，为推动节水创新链、产业链、资金链、政策链融合发展创造了有利条件”，包含的情绪词典是：合同的/契约的(contractual):0.0,水/水资源(water):0.0"}, "本次入选的合同节水管理典型案例，是从地方推荐的近百项案例中，经过初步审查、专家评审、实地调研、网上公示等环节遴选而出，涵盖了工业、农业、公共机构、供水管网漏损控制、水环境治理等领域": {"topic": "“消费”", "similarity": 0.5367840528488159, "prompt": "新闻文本是“本次入选的合同节水管理典型案例，是从地方推荐的近百项案例中，经过初步审查、专家评审、实地调研、网上公示等环节遴选而出，涵盖了工业、农业、公共机构、供水管网漏损控制、水环境治理等领域”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}, "公布的合同节水管理典型案例从不同角度展现了合同节水管理的应用场景、盈利模式和实施成效，着重总结合同节水管理项目实施的主要做法，突出亮点特色，展示先进适用的节水技术和综合管理措施，提炼出“效果保证+效益分享”“用水托管+效益分享”“特许经营+水权交易”“水权交易+综合农事托管服务”等合同节水管理创新模式，充分调动社会资本和用水单位参与节水的积极性": {"topic": "“消费”", "similarity": 0.5689890384674072, "prompt": "新闻文本是“公布的合同节水管理典型案例从不同角度展现了合同节水管理的应用场景、盈利模式和实施成效，着重总结合同节水管理项目实施的主要做法，突出亮点特色，展示先进适用的节水技术和综合管理措施，提炼出“效果保证+效益分享”“用水托管+效益分享”“特许经营+水权交易”“水权交易+综合农事托管服务”等合同节水管理创新模式，充分调动社会资本和用水单位参与节水的积极性”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}, "下一步，水利部将指导各地加大合同节水管理典型案例宣传推广力度，开展形式多样、内容丰富的经验分享和技术交流等活动": {"topic": "“生产投资”", "similarity": 0.5082374811172485, "prompt": "新闻文本是“下一步，水利部将指导各地加大合同节水管理典型案例宣传推广力度，开展形式多样、内容丰富的经验分享和技术交流等活动”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}, "加强合同节水管理工作跟踪辅导，积极促进用水单位和节水服务企业沟通对接，发挥“节水贷”等绿色金融作用，及时总结提炼经验做法，以点带面推动合同节水管理在重点领域广泛实施": {"topic": "“消费”", "similarity": 0.5324375629425049, "prompt": "新闻文本是“加强合同节水管理工作跟踪辅导，积极促进用水单位和节水服务企业沟通对接，发挥“节水贷”等绿色金融作用，及时总结提炼经验做法，以点带面推动合同节水管理在重点领域广泛实施”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}}</t>
+          <t>{"为进一步推广合同节水管理，发挥典型案例示范引领作用，助力节水产业发展，水利部组织开展了合同节水管理典型案例征集遴选，择优推出39个合同节水管理典型案例，形成了一批可复制推广的经验做法": {"topic": "“生产投资”", "similarity": 0.5162226557731628, "prompt": "新闻文本是“为进一步推广合同节水管理，发挥典型案例示范引领作用，助力节水产业发展，水利部组织开展了合同节水管理典型案例征集遴选，择优推出39个合同节水管理典型案例，形成了一批可复制推广的经验做法”，包含的情绪词典是：合同的/契约的(contractual):0.0,依照合同地/依照契约地(contractually):0.0"}, "推广合同节水管理是发展节水产业的重要举措，是水利行业贯彻落实习近平总书记“节水优先、空间均衡、系统治理、两手发力”治水思路和关于治水重要论述精神的生动实践": {"topic": "“生产投资”", "similarity": 0.538425087928772, "prompt": "新闻文本是“推广合同节水管理是发展节水产业的重要举措，是水利行业贯彻落实习近平总书记“节水优先、空间均衡、系统治理、两手发力”治水思路和关于治水重要论述精神的生动实践”，包含的情绪词典是：合同的/契约的(contractual):0.0,水/水资源(water):0.0"}, "水利部高度重视合同节水管理工作，通过加强顶层设计、建立标准体系、搭建信息平台、开展宣传指导等举措，推动实施了800多项合同节水管理项目，吸引社会资本近90亿元，为推动节水创新链、产业链、资金链、政策链融合发展创造了有利条件": {"topic": "“生产投资”", "similarity": 0.5834359526634216, "prompt": "新闻文本是“水利部高度重视合同节水管理工作，通过加强顶层设计、建立标准体系、搭建信息平台、开展宣传指导等举措，推动实施了800多项合同节水管理项目，吸引社会资本近90亿元，为推动节水创新链、产业链、资金链、政策链融合发展创造了有利条件”，包含的情绪词典是：合同的/契约的(contractual):0.0,水/水资源(water):0.0"}, "本次入选的合同节水管理典型案例，是从地方推荐的近百项案例中，经过初步审查、专家评审、实地调研、网上公示等环节遴选而出，涵盖了工业、农业、公共机构、供水管网漏损控制、水环境治理等领域": {"topic": "“消费”", "similarity": 0.5367840528488159, "prompt": "新闻文本是“本次入选的合同节水管理典型案例，是从地方推荐的近百项案例中，经过初步审查、专家评审、实地调研、网上公示等环节遴选而出，涵盖了工业、农业、公共机构、供水管网漏损控制、水环境治理等领域”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}, "公布的合同节水管理典型案例从不同角度展现了合同节水管理的应用场景、盈利模式和实施成效，着重总结合同节水管理项目实施的主要做法，突出亮点特色，展示先进适用的节水技术和综合管理措施，提炼出“效果保证+效益分享”“用水托管+效益分享”“特许经营+水权交易”“水权交易+综合农事托管服务”等合同节水管理创新模式，充分调动社会资本和用水单位参与节水的积极性": {"topic": "“消费”", "similarity": 0.5689892172813416, "prompt": "新闻文本是“公布的合同节水管理典型案例从不同角度展现了合同节水管理的应用场景、盈利模式和实施成效，着重总结合同节水管理项目实施的主要做法，突出亮点特色，展示先进适用的节水技术和综合管理措施，提炼出“效果保证+效益分享”“用水托管+效益分享”“特许经营+水权交易”“水权交易+综合农事托管服务”等合同节水管理创新模式，充分调动社会资本和用水单位参与节水的积极性”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}, "下一步，水利部将指导各地加大合同节水管理典型案例宣传推广力度，开展形式多样、内容丰富的经验分享和技术交流等活动": {"topic": "“生产投资”", "similarity": 0.5082376003265381, "prompt": "新闻文本是“下一步，水利部将指导各地加大合同节水管理典型案例宣传推广力度，开展形式多样、内容丰富的经验分享和技术交流等活动”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}, "加强合同节水管理工作跟踪辅导，积极促进用水单位和节水服务企业沟通对接，发挥“节水贷”等绿色金融作用，及时总结提炼经验做法，以点带面推动合同节水管理在重点领域广泛实施": {"topic": "“消费”", "similarity": 0.5324376821517944, "prompt": "新闻文本是“加强合同节水管理工作跟踪辅导，积极促进用水单位和节水服务企业沟通对接，发挥“节水贷”等绿色金融作用，及时总结提炼经验做法，以点带面推动合同节水管理在重点领域广泛实施”，包含的情绪词典是：水/水资源(water):0.0,合同的/契约的(contractual):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -1662,12 +1654,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "比亚迪汽车官博9月2日消息，比亚迪王朝8月销售178040辆，1月-8月累销1132867辆", "news_prompt2": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "比亚迪汽车官博9月2日消息，比亚迪王朝8月销售178040辆，1月-8月累销1132867辆"}</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>{"比亚迪汽车官博9月2日消息，比亚迪王朝8月销售178040辆，1月-8月累销1132867辆": {"topic": "“生产投资”", "similarity": 0.4851452112197876, "prompt": "新闻文本是“比亚迪汽车官博9月2日消息，比亚迪王朝8月销售178040辆，1月-8月累销1132867辆”，包含的情绪词典是：产量/输出(output):0.0,产能过剩(overcapacity):-0.5"}}</t>
+          <t>{"比亚迪汽车官博9月2日消息，比亚迪王朝8月销售178040辆，1月-8月累销1132867辆": {"topic": "“生产投资”", "similarity": 0.48514524102211, "prompt": "新闻文本是“比亚迪汽车官博9月2日消息，比亚迪王朝8月销售178040辆，1月-8月累销1132867辆”，包含的情绪词典是：产量/输出(output):0.0,产能过剩(overcapacity):-0.5"}}</t>
         </is>
       </c>
     </row>
@@ -1713,12 +1705,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "界面新闻记者 | 朱咏玲 　　又是9月开学季，刚刚结束了暑假的学生们重返校园", "news_prompt2": "当不少中小学生穿着崭新校服满怀期待地开启新学期时，全国大大小小的校服企业也刚刚度过了一年中最忙碌的时期", "news_prompt3": "中国校服生产企业中，95%以上都是小微企业", "news_prompt4": "这是来自中国服装协会发布的《2019中国校服产业白皮书》（以下简称《白皮书》）的数据，统计范围是原中国纤检局（现中国纤维质量监测中心）2018年调研时登记在册的1500余家校服生产企业", "news_prompt5": "如果把范围放得更宽，天眼查APP显示，截至目前，全国经营范围包括“校服”、且存续/在业的企业超过了6326家，其中5527家为小微企业，占比约87%", "news_prompt6": "这些小微企业合计占据着不小的市场份额", "news_prompt7": "中国校服行业规模约在千亿级别，但头部企业寥寥", "news_prompt8": "据《2022年全国教育事业发展统计公报》，当年中小学在校学生人数约为1.85亿，再结合《白皮书》中引用的针对各地校服价格理想区间的调查结果，假设每位学生每年在校服上的花费为662元，由此可估算出，目前中国校服产业的需求量大约是1225亿元", "news_prompt9": "可对比参考的是，据欧睿国际数据，2021年中国童装行业的市场规模约为2564亿元", "news_prompt10": "然而，不同于童装市场中已经发展出如巴拉巴拉这样市占率超5%的头部品牌，中国服装协会发布的《中国校服采购现状调查》指出，中国校服行业中年营收规模超1亿元的企业屈指可数，也几乎没有全国性的品牌", "news_prompt11": "另据恒州博智《2021-2027中国校服市场现状及未来发展趋势》，2020年前十大校服厂商所占份额仅有6.97%", "news_prompt12": "造成行业格局分散的原因是多方面的", "news_prompt13": "由于校服属于定制化的批发生意，它与零售服装相比在各方面都大有不同", "news_prompt14": "首先在校服采购方面，通常情况是政府、学校或家委会组织通过招投标方式进行集体采购，只有在如深圳这种全市校服统一的极个别地区，家长和学生才能通过零售渠道自行购买", "news_prompt15": "此外，部分地区至今还保留着利好本地企业的招投标政策", "news_prompt16": "因此，校服并非一个直接面向消费者、完全开放和自由竞争的市场", "news_prompt17": "另一方面，由于校服强调的是平等和共同的身份而非个性，加上学校尤其是公立学校为确保普惠性通常会对校服限价，因此它不像零售服装那样，需要靠时尚创意或高端科技竞争，门槛相对较低，一些小微企业就能满足需求", "news_prompt18": "在此情况下，大大小小的本地校服企业就有了近水楼台的优势", "news_prompt19": "它们不仅能更及时地获知地方的校服采购需求，与所在地的学校合作起来也更方便", "news_prompt20": "报喜鸟旗下的校服企业衣俪特的设计经理姚滟若告诉界面新闻，在与学校的合作前期阶段，校服企业通常要走访学校实地调研，比如衣俪特的设计师会在了解当地的气候特点、学生的课程安排、学校的理念文化等基础上，综合多方面因素来设计校服", "news_prompt21": "“比如在华南地区，考虑到回南天，在条件允许的情况下，我们会推荐使用吸湿速干的面料", "news_prompt22": "”姚滟若说", "news_prompt23": "“北方的水质可能碱性程度比较高，偏硬，我们会推荐使用不那么鲜艳或者不那么深的颜色，因为长时间洗涤可能会改变衣服的颜色，比如更推荐使用色织面料", "news_prompt24": "” 　　此外，在完成交付后，公司也要回访学校提供售后服务", "news_prompt25": "部分情况下，校服企业还会在学校内设置一个校服售卖点，由专人负责定期开放服务", "news_prompt26": "也就是说，从走访调研到售后服务，距离学校更近的校服企业总是更方便的", "news_prompt27": "虽然校服市场相对封闭和分散、本土小企业居多、整体竞争还不够充分，且毛利率通常低于零售服装，但它胜在需求相对稳定，受市场环境波动的影响较小", "news_prompt28": "近年来，也有不少以零售业务为主的服装集团开始涉足这一领域", "news_prompt29": "前述衣俪特就是报喜鸟在2016年与韩国校服品牌elite basic成立的合资公司", "news_prompt30": "与之相似的还有波司登旗下的飒美特，该公司由波司登与韩国校服品牌SMART F&amp;D在2015年合资成立", "news_prompt31": "此外，主营职业装的乔治白在2015年进军校服领域，森马服饰在2020年开始运营自有校服品牌Hey junior，海澜之家旗下的圣凯诺职业装品牌从2020年起提到要开拓校服市场，谋求科技战略转型的童装企业安奈儿则在2023年尝试合作推出功能面料校服", "news_prompt32": "由于业务规模尚小，前述企业很少在财报中单独披露校服业务的业绩", "news_prompt33": "23/24财年（截至2024年3月底），飒美特的营收同比增长1.3%至1.89亿元，由其贡献超九成的多元化服装业务的毛利率为20.2%", "news_prompt34": "2023年，报喜鸟旗下包括衣俪特在内的“其他”品牌营收为1.43亿元，同比增长18.03%", "news_prompt35": "包括职业装和校服的团购业务毛利率为46.40%，低于报喜鸟主营业务毛利率的65.93%", "news_prompt36": "这些起步较晚的品牌还不足以排到行业头部位置", "news_prompt37": "可作为对比的是，隶属于中国机械工业集团的上市企业苏美达旗下也有校服品牌伊顿纪德，该品牌于2008年成立，2023年的营收同比增长16.94%至11.09亿元，毛利率为34.43%", "news_prompt38": "另外还有一些非上市企业如重庆立泰服饰集团、广"}</t>
+          <t>{"news_prompt1": "界面新闻记者 | 朱咏玲 　　又是9月开学季，刚刚结束了暑假的学生们重返校园", "news_prompt2": "当不少中小学生穿着崭新校服满怀期待地开启新学期时，全国大大小小的校服企业也刚刚度过了一年中最忙碌的时期", "news_prompt3": "中国校服生产企业中，95%以上都是小微企业", "news_prompt4": "这些小微企业合计占据着不小的市场份额", "news_prompt5": "中国校服行业规模约在千亿级别，但头部企业寥寥", "news_prompt6": "可对比参考的是，据欧睿国际数据，2021年中国童装行业的市场规模约为2564亿元", "news_prompt7": "造成行业格局分散的原因是多方面的", "news_prompt8": "“北方的水质可能碱性程度比较高，偏硬，我们会推荐使用不那么鲜艳或者不那么深的颜色，因为长时间洗涤可能会改变衣服的颜色，比如更推荐使用色织面料", "news_prompt9": "虽然校服市场相对封闭和分散、本土小企业居多、整体竞争还不够充分，且毛利率通常低于零售服装，但它胜在需求相对稳定，受市场环境波动的影响较小", "news_prompt10": "近年来，也有不少以零售业务为主的服装集团开始涉足这一领域", "news_prompt11": "包括职业装和校服的团购业务毛利率为46.40%，低于报喜鸟主营业务毛利率的65.93%", "news_prompt12": "这些起步较晚的品牌还不足以排到行业头部位置", "news_prompt13": "另外还有一些非上市企业如重庆立泰服饰集团、广"}</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>{"界面新闻记者 | 朱咏玲 　　又是9月开学季，刚刚结束了暑假的学生们重返校园": {"topic": "“生产投资”", "similarity": 0.437238484621048, "prompt": "新闻文本是“界面新闻记者 | 朱咏玲 　　又是9月开学季，刚刚结束了暑假的学生们重返校园”，包含的情绪词典是：学校/学派(school):0.0,重新获得/恢复(regain):0.5"}, "当不少中小学生穿着崭新校服满怀期待地开启新学期时，全国大大小小的校服企业也刚刚度过了一年中最忙碌的时期": {"topic": "“消费”", "similarity": 0.5192172527313232, "prompt": "新闻文本是“当不少中小学生穿着崭新校服满怀期待地开启新学期时，全国大大小小的校服企业也刚刚度过了一年中最忙碌的时期”，包含的情绪词典是：征服/制服(subdue):-0.3,学校/学派(school):0.0"}, "中国校服生产企业中，95%以上都是小微企业": {"topic": "“生产投资”", "similarity": 0.4865662455558777, "prompt": "新闻文本是“中国校服生产企业中，95%以上都是小微企业”，包含的情绪词典是：小的/小型的(small):0.0,企业/事业(enterprise):0.0"}, "这是来自中国服装协会发布的《2019中国校服产业白皮书》（以下简称《白皮书》）的数据，统计范围是原中国纤检局（现中国纤维质量监测中心）2018年调研时登记在册的1500余家校服生产企业": {"topic": "“消费”", "similarity": 0.5347472429275513}, "如果把范围放得更宽，天眼查APP显示，截至目前，全国经营范围包括“校服”、且存续/在业的企业超过了6326家，其中5527家为小微企业，占比约87%": {"topic": "“消费”", "similarity": 0.5924848318099976}, "这些小微企业合计占据着不小的市场份额": {"topic": "“消费”", "similarity": 0.5544635057449341, "prompt": "新闻文本是“这些小微企业合计占据着不小的市场份额”，包含的情绪词典是：轻微的/少量的(slight):0.0,小的/小型的(small):0.0"}, "中国校服行业规模约在千亿级别，但头部企业寥寥": {"topic": "“消费”", "similarity": 0.47099095582962036, "prompt": "新闻文本是“中国校服行业规模约在千亿级别，但头部企业寥寥”，包含的情绪词典是：征服/制服(subdue):-0.3,规模/尺度(scale):0.0"}, "据《2022年全国教育事业发展统计公报》，当年中小学在校学生人数约为1.85亿，再结合《白皮书》中引用的针对各地校服价格理想区间的调查结果，假设每位学生每年在校服上的花费为662元，由此可估算出，目前中国校服产业的需求量大约是1225亿元": {"topic": "“消费”", "similarity": 0.599766194820404}, "可对比参考的是，据欧睿国际数据，2021年中国童装行业的市场规模约为2564亿元": {"topic": "“消费”", "similarity": 0.57683926820755, "prompt": "新闻文本是“可对比参考的是，据欧睿国际数据，2021年中国童装行业的市场规模约为2564亿元”，包含的情绪词典是：相当大的/可观的(sizeable):0.0"}, "然而，不同于童装市场中已经发展出如巴拉巴拉这样市占率超5%的头部品牌，中国服装协会发布的《中国校服采购现状调查》指出，中国校服行业中年营收规模超1亿元的企业屈指可数，也几乎没有全国性的品牌": {"topic": "“消费”", "similarity": 0.5236330032348633}, "另据恒州博智《2021-2027中国校服市场现状及未来发展趋势》，2020年前十大校服厂商所占份额仅有6.97%": {"topic": "“消费”", "similarity": 0.5318480730056763}, "造成行业格局分散的原因是多方面的": {"topic": "“生产投资”", "similarity": 0.5059031844139099, "prompt": "新闻文本是“造成行业格局分散的原因是多方面的”，包含的情绪词典是：分裂/分开(split):-0.2,解散/解体(dissolution):-0.4"}, "首先在校服采购方面，通常情况是政府、学校或家委会组织通过招投标方式进行集体采购，只有在如深圳这种全市校服统一的极个别地区，家长和学生才能通过零售渠道自行购买": {"topic": "“消费”", "similarity": 0.5163873434066772}, "另一方面，由于校服强调的是平等和共同的身份而非个性，加上学校尤其是公立学校为确保普惠性通常会对校服限价，因此它不像零售服装那样，需要靠时尚创意或高端科技竞争，门槛相对较低，一些小微企业就能满足需求": {"topic": "“消费”", "similarity": 0.4418400228023529}, "“北方的水质可能碱性程度比较高，偏硬，我们会推荐使用不那么鲜艳或者不那么深的颜色，因为长时间洗涤可能会改变衣服的颜色，比如更推荐使用色织面料": {"topic": "“消费”", "similarity": 0.42993515729904175, "prompt": "新闻文本是““北方的水质可能碱性程度比较高，偏硬，我们会推荐使用不那么鲜艳或者不那么深的颜色，因为长时间洗涤可能会改变衣服的颜色，比如更推荐使用色织面料”，包含的情绪词典是：北方/北部(north):0.0"}, "虽然校服市场相对封闭和分散、本土小企业居多、整体竞争还不够充分，且毛利率通常低于零售服装，但它胜在需求相对稳定，受市场环境波动的影响较小": {"topic": "“消费”", "similarity": 0.5396018028259277, "prompt": "新闻文本是“虽然校服市场相对封闭和分散、本土小企业居多、整体竞争还不够充分，且毛利率通常低于零售服装，但它胜在需求相对稳定，受市场环境波动的影响较小”，包含的情绪词典是：稳定的/稳固的(stable):0.5,学校/学派(school):0.0"}, "近年来，也有不少以零售业务为主的服装集团开始涉足这一领域": {"topic": "“消费”", "similarity": 0.4834190011024475, "prompt": "新闻文本是“近年来，也有不少以零售业务为主的服装集团开始涉足这一领域”，包含的情绪词典是：商业的/贸易的(commercial):0.0,征服/制服(subdue):-0.3"}, "此外，主营职业装的乔治白在2015年进军校服领域，森马服饰在2020年开始运营自有校服品牌Hey junior，海澜之家旗下的圣凯诺职业装品牌从2020年起提到要开拓校服市场，谋求科技战略转型的童装企业安奈儿则在2023年尝试合作推出功能面料校服": {"topic": "“消费”", "similarity": 0.49094682931900024}, "2023年，报喜鸟旗下包括衣俪特在内的“其他”品牌营收为1.43亿元，同比增长18.03%": {"topic": "“消费”", "similarity": 0.47370606660842896}, "包括职业装和校服的团购业务毛利率为46.40%，低于报喜鸟主营业务毛利率的65.93%": {"topic": "“消费”", "similarity": 0.4916273057460785, "prompt": "新闻文本是“包括职业装和校服的团购业务毛利率为46.40%，低于报喜鸟主营业务毛利率的65.93%”，包含的情绪词典是：百分比(percentage):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "这些起步较晚的品牌还不足以排到行业头部位置": {"topic": "“消费”", "similarity": 0.51780104637146, "prompt": "新闻文本是“这些起步较晚的品牌还不足以排到行业头部位置”，包含的情绪词典是：初期的/未发展的(inchoate):0.0,资本不足的(undercapitalized):-0.4"}, "可作为对比的是，隶属于中国机械工业集团的上市企业苏美达旗下也有校服品牌伊顿纪德，该品牌于2008年成立，2023年的营收同比增长16.94%至11.09亿元，毛利率为34.43%": {"topic": "“消费”", "similarity": 0.4728648066520691}, "另外还有一些非上市企业如重庆立泰服饰集团、广": {"topic": "“金融”", "similarity": 0.5216596722602844, "prompt": "新闻文本是“另外还有一些非上市企业如重庆立泰服饰集团、广”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}}</t>
+          <t>{"界面新闻记者 | 朱咏玲 　　又是9月开学季，刚刚结束了暑假的学生们重返校园": {"topic": "“生产投资”", "similarity": 0.43723875284194946, "prompt": "新闻文本是“界面新闻记者 | 朱咏玲 　　又是9月开学季，刚刚结束了暑假的学生们重返校园”，包含的情绪词典是：学校/学派(school):0.0,重新获得/恢复(regain):0.5"}, "当不少中小学生穿着崭新校服满怀期待地开启新学期时，全国大大小小的校服企业也刚刚度过了一年中最忙碌的时期": {"topic": "“消费”", "similarity": 0.519217312335968, "prompt": "新闻文本是“当不少中小学生穿着崭新校服满怀期待地开启新学期时，全国大大小小的校服企业也刚刚度过了一年中最忙碌的时期”，包含的情绪词典是：征服/制服(subdue):-0.3,学校/学派(school):0.0"}, "中国校服生产企业中，95%以上都是小微企业": {"topic": "“生产投资”", "similarity": 0.4865662753582001, "prompt": "新闻文本是“中国校服生产企业中，95%以上都是小微企业”，包含的情绪词典是：小的/小型的(small):0.0,企业/事业(enterprise):0.0"}, "这些小微企业合计占据着不小的市场份额": {"topic": "“消费”", "similarity": 0.5544636249542236, "prompt": "新闻文本是“这些小微企业合计占据着不小的市场份额”，包含的情绪词典是：轻微的/少量的(slight):0.0,小的/小型的(small):0.0"}, "中国校服行业规模约在千亿级别，但头部企业寥寥": {"topic": "“消费”", "similarity": 0.4709910750389099, "prompt": "新闻文本是“中国校服行业规模约在千亿级别，但头部企业寥寥”，包含的情绪词典是：征服/制服(subdue):-0.3,规模/尺度(scale):0.0"}, "可对比参考的是，据欧睿国际数据，2021年中国童装行业的市场规模约为2564亿元": {"topic": "“消费”", "similarity": 0.5768395066261292, "prompt": "新闻文本是“可对比参考的是，据欧睿国际数据，2021年中国童装行业的市场规模约为2564亿元”，包含的情绪词典是：相当大的/可观的(sizeable):0.0"}, "造成行业格局分散的原因是多方面的": {"topic": "“生产投资”", "similarity": 0.5059032440185547, "prompt": "新闻文本是“造成行业格局分散的原因是多方面的”，包含的情绪词典是：分裂/分开(split):-0.2,解散/解体(dissolution):-0.4"}, "“北方的水质可能碱性程度比较高，偏硬，我们会推荐使用不那么鲜艳或者不那么深的颜色，因为长时间洗涤可能会改变衣服的颜色，比如更推荐使用色织面料": {"topic": "“消费”", "similarity": 0.4299353063106537, "prompt": "新闻文本是““北方的水质可能碱性程度比较高，偏硬，我们会推荐使用不那么鲜艳或者不那么深的颜色，因为长时间洗涤可能会改变衣服的颜色，比如更推荐使用色织面料”，包含的情绪词典是：北方/北部(north):0.0"}, "虽然校服市场相对封闭和分散、本土小企业居多、整体竞争还不够充分，且毛利率通常低于零售服装，但它胜在需求相对稳定，受市场环境波动的影响较小": {"topic": "“消费”", "similarity": 0.5396018624305725, "prompt": "新闻文本是“虽然校服市场相对封闭和分散、本土小企业居多、整体竞争还不够充分，且毛利率通常低于零售服装，但它胜在需求相对稳定，受市场环境波动的影响较小”，包含的情绪词典是：稳定的/稳固的(stable):0.5,学校/学派(school):0.0"}, "近年来，也有不少以零售业务为主的服装集团开始涉足这一领域": {"topic": "“消费”", "similarity": 0.4834192991256714, "prompt": "新闻文本是“近年来，也有不少以零售业务为主的服装集团开始涉足这一领域”，包含的情绪词典是：商业的/贸易的(commercial):0.0,征服/制服(subdue):-0.3"}, "包括职业装和校服的团购业务毛利率为46.40%，低于报喜鸟主营业务毛利率的65.93%": {"topic": "“消费”", "similarity": 0.49162739515304565, "prompt": "新闻文本是“包括职业装和校服的团购业务毛利率为46.40%，低于报喜鸟主营业务毛利率的65.93%”，包含的情绪词典是：百分比(percentage):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "这些起步较晚的品牌还不足以排到行业头部位置": {"topic": "“消费”", "similarity": 0.5178011655807495, "prompt": "新闻文本是“这些起步较晚的品牌还不足以排到行业头部位置”，包含的情绪词典是：初期的/未发展的(inchoate):0.0,资本不足的(undercapitalized):-0.4"}, "另外还有一些非上市企业如重庆立泰服饰集团、广": {"topic": "“金融”", "similarity": 0.5216597318649292, "prompt": "新闻文本是“另外还有一些非上市企业如重庆立泰服饰集团、广”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -1764,12 +1756,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "天风证券09月02日发布研报称，给予居然之家（000785.SZ，最新价：2.58元）买入评级", "news_prompt2": "评级理由主要包括：1）巩固资源优势，家居主业保持稳步发展", "news_prompt3": "2）三大数智化转型工具更加成熟，数智化转型成效明显", "news_prompt4": "风险提示：行业政策变动风险", "news_prompt5": "市场竞争加剧风险", "news_prompt6": "折旧摊销拖累业绩表现风险等", "news_prompt7": "AI点评：居然之家近一个月获得1份券商研报关注", "news_prompt8": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "评级理由主要包括：1）巩固资源优势，家居主业保持稳步发展", "news_prompt2": "2）三大数智化转型工具更加成熟，数智化转型成效明显", "news_prompt3": "市场竞争加剧风险", "news_prompt4": "折旧摊销拖累业绩表现风险等", "news_prompt5": "AI点评：居然之家近一个月获得1份券商研报关注"}</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>{"天风证券09月02日发布研报称，给予居然之家（000785.SZ，最新价：2.58元）买入评级": {"topic": "“金融”", "similarity": 0.44269096851348877}, "评级理由主要包括：1）巩固资源优势，家居主业保持稳步发展": {"topic": "“消费”", "similarity": 0.47160136699676514, "prompt": "新闻文本是“评级理由主要包括：1）巩固资源优势，家居主业保持稳步发展”，包含的情绪词典是：稳定/稳定性(stability):0.6,稳定的/稳固的(stable):0.5"}, "2）三大数智化转型工具更加成熟，数智化转型成效明显": {"topic": "“生产投资”", "similarity": 0.5141083002090454, "prompt": "新闻文本是“2）三大数智化转型工具更加成熟，数智化转型成效明显”，包含的情绪词典是：数字的/数码的(digital):0.0,数字/数位(digit):0.0"}, "风险提示：行业政策变动风险": {"topic": "“金融”", "similarity": 0.569650411605835, "prompt": "新闻文本是“风险提示：行业政策变动风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "市场竞争加剧风险": {"topic": "“金融”", "similarity": 0.5059287548065186, "prompt": "新闻文本是“市场竞争加剧风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "折旧摊销拖累业绩表现风险等": {"topic": "“金融”", "similarity": 0.5047401785850525, "prompt": "新闻文本是“折旧摊销拖累业绩表现风险等”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperformance):-0.4"}, "AI点评：居然之家近一个月获得1份券商研报关注": {"topic": "“消费”", "similarity": 0.435944139957428, "prompt": "新闻文本是“AI点评：居然之家近一个月获得1份券商研报关注”，包含的情绪词典是：消费者/用户(consumer):0.0,一点/少量(bit):0.0"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"评级理由主要包括：1）巩固资源优势，家居主业保持稳步发展": {"topic": "“消费”", "similarity": 0.4716017246246338, "prompt": "新闻文本是“评级理由主要包括：1）巩固资源优势，家居主业保持稳步发展”，包含的情绪词典是：稳定/稳定性(stability):0.6,稳定的/稳固的(stable):0.5"}, "2）三大数智化转型工具更加成熟，数智化转型成效明显": {"topic": "“生产投资”", "similarity": 0.5141083598136902, "prompt": "新闻文本是“2）三大数智化转型工具更加成熟，数智化转型成效明显”，包含的情绪词典是：数字的/数码的(digital):0.0,数字/数位(digit):0.0"}, "市场竞争加剧风险": {"topic": "“金融”", "similarity": 0.5059287548065186, "prompt": "新闻文本是“市场竞争加剧风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "折旧摊销拖累业绩表现风险等": {"topic": "“金融”", "similarity": 0.5047401785850525, "prompt": "新闻文本是“折旧摊销拖累业绩表现风险等”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperformance):-0.4"}, "AI点评：居然之家近一个月获得1份券商研报关注": {"topic": "“消费”", "similarity": 0.4359443783760071, "prompt": "新闻文本是“AI点评：居然之家近一个月获得1份券商研报关注”，包含的情绪词典是：消费者/用户(consumer):0.0,一点/少量(bit):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -1815,12 +1807,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月30日，科创芯片ETF(588200.SH)收涨3.12%，成交5.55亿元", "news_prompt2": "净流出1.19亿元（净赎回份额*单位净值），居可比基金第一", "news_prompt3": "拉长时间看，该基金连续4天资金净流出，累计流出3.23亿元，居可比基金首位", "news_prompt4": "资金流出也带来了份额的减少，该基金最新份额较前一日减少1.29亿份，跌破73.00亿份", "news_prompt5": "与此同时，该基金最新规模达67.32亿元", "news_prompt6": "科创芯片ETF(588200.SH)，场外联接(A：017469", "news_prompt7": "C：017470", "news_prompt8": "I：021870)", "news_prompt9": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "2024年8月30日，科创芯片ETF(588200.SH)收涨3.12%，成交5.55亿元", "news_prompt2": "净流出1.19亿元（净赎回份额*单位净值），居可比基金第一", "news_prompt3": "拉长时间看，该基金连续4天资金净流出，累计流出3.23亿元，居可比基金首位", "news_prompt4": "资金流出也带来了份额的减少，该基金最新份额较前一日减少1.29亿份，跌破73.00亿份", "news_prompt5": "与此同时，该基金最新规模达67.32亿元", "news_prompt6": "科创芯片ETF(588200.SH)，场外联接(A：017469"}</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>{"2024年8月30日，科创芯片ETF(588200.SH)收涨3.12%，成交5.55亿元": {"topic": "“金融”", "similarity": 0.5332895517349243, "prompt": "新闻文本是“2024年8月30日，科创芯片ETF(588200.SH)收涨3.12%，成交5.55亿元”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "净流出1.19亿元（净赎回份额*单位净值），居可比基金第一": {"topic": "“金融”", "similarity": 0.5288675427436829, "prompt": "新闻文本是“净流出1.19亿元（净赎回份额*单位净值），居可比基金第一”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "拉长时间看，该基金连续4天资金净流出，累计流出3.23亿元，居可比基金首位": {"topic": "“金融”", "similarity": 0.5405932068824768, "prompt": "新闻文本是“拉长时间看，该基金连续4天资金净流出，累计流出3.23亿元，居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeout):-0.2"}, "资金流出也带来了份额的减少，该基金最新份额较前一日减少1.29亿份，跌破73.00亿份": {"topic": "“金融”", "similarity": 0.46890735626220703, "prompt": "新闻文本是“资金流出也带来了份额的减少，该基金最新份额较前一日减少1.29亿份，跌破73.00亿份”，包含的情绪词典是：下跌/下降(fall):-0.6,资金不足的(underfunded):-0.3"}, "与此同时，该基金最新规模达67.32亿元": {"topic": "“金融”", "similarity": 0.49192512035369873, "prompt": "新闻文本是“与此同时，该基金最新规模达67.32亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "科创芯片ETF(588200.SH)，场外联接(A：017469": {"topic": "“金融”", "similarity": 0.541593611240387, "prompt": "新闻文本是“科创芯片ETF(588200.SH)，场外联接(A：017469”，包含的情绪词典是：基金/资金(fund):0.1,投资者/投资人(investor):0.4"}}</t>
+          <t>{"2024年8月30日，科创芯片ETF(588200.SH)收涨3.12%，成交5.55亿元": {"topic": "“金融”", "similarity": 0.5332896113395691, "prompt": "新闻文本是“2024年8月30日，科创芯片ETF(588200.SH)收涨3.12%，成交5.55亿元”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "净流出1.19亿元（净赎回份额*单位净值），居可比基金第一": {"topic": "“金融”", "similarity": 0.5288676619529724, "prompt": "新闻文本是“净流出1.19亿元（净赎回份额*单位净值），居可比基金第一”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "拉长时间看，该基金连续4天资金净流出，累计流出3.23亿元，居可比基金首位": {"topic": "“金融”", "similarity": 0.5405933260917664, "prompt": "新闻文本是“拉长时间看，该基金连续4天资金净流出，累计流出3.23亿元，居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeout):-0.2"}, "资金流出也带来了份额的减少，该基金最新份额较前一日减少1.29亿份，跌破73.00亿份": {"topic": "“金融”", "similarity": 0.46890753507614136, "prompt": "新闻文本是“资金流出也带来了份额的减少，该基金最新份额较前一日减少1.29亿份，跌破73.00亿份”，包含的情绪词典是：下跌/下降(fall):-0.6,资金不足的(underfunded):-0.3"}, "与此同时，该基金最新规模达67.32亿元": {"topic": "“金融”", "similarity": 0.49192512035369873, "prompt": "新闻文本是“与此同时，该基金最新规模达67.32亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "科创芯片ETF(588200.SH)，场外联接(A：017469": {"topic": "“金融”", "similarity": 0.5415935516357422, "prompt": "新闻文本是“科创芯片ETF(588200.SH)，场外联接(A：017469”，包含的情绪词典是：基金/资金(fund):0.1,投资者/投资人(investor):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -1870,12 +1862,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上证报中国证券网讯日前，沪市半导体公司均已完成2024年半年报披露", "news_prompt2": "上半年，沪市130余家半导体公司合计实现营业收入2112亿元，同比增长18.7%，超7成公司营业收入同比正增长，超5成公司净利润较去年同期有所改善", "news_prompt3": "分季度来看，2024年第二季度，营收环比增长14.6%，净利润环比增长74.9%，其中近9成公司营收环比正增长，7成公司净利润环比改善", "news_prompt4": "亮眼的二季度业绩展现出半导体行业良好的复苏态势", "news_prompt5": "与此同时，沪市半导体公司积极践行“提质增效重回报”专项行动方案，积极通过中期分红回馈投资者，共有13家公司披露中期分红预案，合计分红金额约7亿元", "news_prompt6": "需求复苏推动龙头公司业绩回暖 　　今年第二季度，以成熟制程为主的晶圆代工需求复苏，国内龙头代工厂的收入、毛利率、产能利用率等关键指标环比均显著提升，且高于前期指引", "news_prompt7": "中芯国际2024年第二季度实现营收19.01亿美元，同比增长21.8%，环比增长8.6%，出货量环比增长近17.7%，毛利率为13.9%", "news_prompt8": "对于今年第三季度，公司给出的收入指引为环比增长13%-15%，毛利率介于18%-20%范围内", "news_prompt9": "华虹公司第二季度实现销售收入4.79亿美元，毛利率为10.5%，均实现环比增长", "news_prompt10": "公司已接近全方位满产，总体产能利用率为97.9%，较上季度提升6.2个百分点", "news_prompt11": "第三季度，公司预计销售收入为5亿美元至5.2亿美元之间，毛利率约在10%至12%之间", "news_prompt12": "半导体设备、材料行业的多家公司经营业绩延续良好态势，营收、净利润环比均呈现较快增长趋势", "news_prompt13": "天岳先进作为国内碳化硅衬底龙头企业，在导电型碳化硅衬底领域实现后来居上，2023年市场规模跃居全球前二", "news_prompt14": "公司是继Wolfspeed后全球第二家宣布批量供应8英寸衬底厂商，并已经进入博世、英飞凌等海外一线器件企业的供应体系", "news_prompt15": "上半年，天岳先进实现营业收入9.12亿元，同比增长108.27%", "news_prompt16": "归母净利润1.02亿元，同比扭亏为盈", "news_prompt17": "华海清科从推出国内首台拥有自主知识产权的12英寸CMP设备，到如今第500台顺利交付，助力国内CMP设备产业自主发展", "news_prompt18": "上半年，公司实现营业收入14.97亿元，同比增长21.23%", "news_prompt19": "归母净利润4.33亿元，同比增长15.65%", "news_prompt20": "封测需求底部复苏明确，先进封装技术引领新增长，龙头公司业绩加速回暖", "news_prompt21": "今年上半年，封测行业的景气度延续复苏态势，主要公司的稼动率整体呈现稳定回升趋势，行业整体毛利率稳步回升，企业盈利能力得到显著改善", "news_prompt22": "长电科技是国内封测龙头公司，上半年实现营业收入154.87亿元，同比增长27.22%", "news_prompt23": "归母净利润6.19亿元，同比增长24.96%", "news_prompt24": "公司上半年业绩显著增长，得益于下游需求逐步复苏，部分客户业务量持续上升", "news_prompt25": "同时，公司大力拓展先进封装业务，聚焦新兴应用领域，积极进行产能利用率调控", "news_prompt26": "甬矽电子专注于集成电路的先进封装与测试，上半年实现营业收入16.29亿元，同比增长65.81%", "news_prompt27": "归母净利润1210.59万元，扭亏为盈", "news_prompt28": "公司坚持自身中高端先进封装业务定位，晶圆级封装、汽车电子等产品线持续丰富，“Bumping+CP+FC+FT”的一站式交付能力形成，公司竞争力持续增强", "news_prompt29": "消费市场回暖助力公司亮眼业绩 　　受益于消费电子复苏延续，汽车电子维持强劲，多家芯片设计公司业绩亮眼", "news_prompt30": "韦尔股份专注于图像传感器、显示及模拟解决方案", "news_prompt31": "得益于消费市场持续回暖、公司在高端智能手机市场成功推出新品以及自动驾驶技术在汽车市场的不断深入应用，上半年，公司实现营收120.91亿元，同比增长36.50%", "news_prompt32": "归母净利润13.67亿元，同比增长792.79%", "news_prompt33": "纳芯微聚焦传感器、信号链和电源管理三大产品方向", "news_prompt34": "公司第二季度实现营业收入4.86亿元，环比增长34.18%", "news_prompt35": "半年报显示，其营收增长动力主要来自公司汽车电子领域相关产品持续放量，以及消费电子领域景气度的持续改善", "news_prompt36": "存储芯片整体延续回暖趋势，相关公司业绩出色", "news_prompt37": "存储芯片价格经历快速上涨，市场的供需结构逐步改善，沪市存储芯片设计公司业绩表现抢眼", "news_prompt38": "兆易创新专注于存储器、微控制器及传感器的研发", "news_prompt39": "公司上半年实现营业收入36.09亿元，同比增长21.69%", "news_prompt40": "归母净利润5.17亿元，同比增长53.88%", "news_prompt41": "随着今年上半年消费和网通市场的显著回暖，公司存储芯片产品迎来销售高峰，直接推动产品销量和经营业绩大幅增加", "news_prompt42": "澜起科技上半年实现营业收入16.65亿元，较上年同期增长79.49%", "news_prompt43": "归母净利润5.93亿元，较上年同期增长624.63%", "news_prompt44": "随着存储行业的复苏、AI服务器需求量快速增长，公司DDR5渗透率持续提升，高性能运力芯片新产品实现规模出货", "news_prompt45": "沪市半导体公司立足新发展阶段、贯彻新发展理念，不断加大研发投入和产品创新力度", "news_prompt46": "截至目前，相关公司上半年合计投入研发费"}</t>
+          <t>{"news_prompt1": "上证报中国证券网讯日前，沪市半导体公司均已完成2024年半年报披露", "news_prompt2": "上半年，沪市130余家半导体公司合计实现营业收入2112亿元，同比增长18.7%，超7成公司营业收入同比正增长，超5成公司净利润较去年同期有所改善", "news_prompt3": "分季度来看，2024年第二季度，营收环比增长14.6%，净利润环比增长74.9%，其中近9成公司营收环比正增长，7成公司净利润环比改善", "news_prompt4": "亮眼的二季度业绩展现出半导体行业良好的复苏态势", "news_prompt5": "与此同时，沪市半导体公司积极践行“提质增效重回报”专项行动方案，积极通过中期分红回馈投资者，共有13家公司披露中期分红预案，合计分红金额约7亿元", "news_prompt6": "需求复苏推动龙头公司业绩回暖 　　今年第二季度，以成熟制程为主的晶圆代工需求复苏，国内龙头代工厂的收入、毛利率、产能利用率等关键指标环比均显著提升，且高于前期指引", "news_prompt7": "对于今年第三季度，公司给出的收入指引为环比增长13%-15%，毛利率介于18%-20%范围内", "news_prompt8": "公司已接近全方位满产，总体产能利用率为97.9%，较上季度提升6.2个百分点", "news_prompt9": "半导体设备、材料行业的多家公司经营业绩延续良好态势，营收、净利润环比均呈现较快增长趋势", "news_prompt10": "天岳先进作为国内碳化硅衬底龙头企业，在导电型碳化硅衬底领域实现后来居上，2023年市场规模跃居全球前二", "news_prompt11": "上半年，天岳先进实现营业收入9.12亿元，同比增长108.27%", "news_prompt12": "上半年，公司实现营业收入14.97亿元，同比增长21.23%", "news_prompt13": "归母净利润4.33亿元，同比增长15.65%", "news_prompt14": "封测需求底部复苏明确，先进封装技术引领新增长，龙头公司业绩加速回暖", "news_prompt15": "今年上半年，封测行业的景气度延续复苏态势，主要公司的稼动率整体呈现稳定回升趋势，行业整体毛利率稳步回升，企业盈利能力得到显著改善", "news_prompt16": "长电科技是国内封测龙头公司，上半年实现营业收入154.87亿元，同比增长27.22%", "news_prompt17": "公司上半年业绩显著增长，得益于下游需求逐步复苏，部分客户业务量持续上升", "news_prompt18": "同时，公司大力拓展先进封装业务，聚焦新兴应用领域，积极进行产能利用率调控", "news_prompt19": "甬矽电子专注于集成电路的先进封装与测试，上半年实现营业收入16.29亿元，同比增长65.81%", "news_prompt20": "公司坚持自身中高端先进封装业务定位，晶圆级封装、汽车电子等产品线持续丰富，“Bumping+CP+FC+FT”的一站式交付能力形成，公司竞争力持续增强", "news_prompt21": "消费市场回暖助力公司亮眼业绩 　　受益于消费电子复苏延续，汽车电子维持强劲，多家芯片设计公司业绩亮眼", "news_prompt22": "纳芯微聚焦传感器、信号链和电源管理三大产品方向", "news_prompt23": "半年报显示，其营收增长动力主要来自公司汽车电子领域相关产品持续放量，以及消费电子领域景气度的持续改善", "news_prompt24": "存储芯片整体延续回暖趋势，相关公司业绩出色", "news_prompt25": "存储芯片价格经历快速上涨，市场的供需结构逐步改善，沪市存储芯片设计公司业绩表现抢眼", "news_prompt26": "兆易创新专注于存储器、微控制器及传感器的研发", "news_prompt27": "随着今年上半年消费和网通市场的显著回暖，公司存储芯片产品迎来销售高峰，直接推动产品销量和经营业绩大幅增加", "news_prompt28": "澜起科技上半年实现营业收入16.65亿元，较上年同期增长79.49%", "news_prompt29": "随着存储行业的复苏、AI服务器需求量快速增长，公司DDR5渗透率持续提升，高性能运力芯片新产品实现规模出货", "news_prompt30": "沪市半导体公司立足新发展阶段、贯彻新发展理念，不断加大研发投入和产品创新力度", "news_prompt31": "截至目前，相关公司上半年合计投入研发费"}</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>{"上证报中国证券网讯日前，沪市半导体公司均已完成2024年半年报披露": {"topic": "“生产投资”", "similarity": 0.4512546956539154, "prompt": "新闻文本是“上证报中国证券网讯日前，沪市半导体公司均已完成2024年半年报披露”，包含的情绪词典是：完成/实现(accomplishes):0.6,完成/实现(accomplish):0.6"}, "上半年，沪市130余家半导体公司合计实现营业收入2112亿元，同比增长18.7%，超7成公司营业收入同比正增长，超5成公司净利润较去年同期有所改善": {"topic": "“生产投资”", "similarity": 0.554355800151825, "prompt": "新闻文本是“上半年，沪市130余家半导体公司合计实现营业收入2112亿元，同比增长18.7%，超7成公司营业收入同比正增长，超5成公司净利润较去年同期有所改善”，包含的情绪词典是：利润/利益(profit):0.8,有利可图的/盈利的(profitable):0.8"}, "分季度来看，2024年第二季度，营收环比增长14.6%，净利润环比增长74.9%，其中近9成公司营收环比正增长，7成公司净利润环比改善": {"topic": "“生产投资”", "similarity": 0.5821152925491333, "prompt": "新闻文本是“分季度来看，2024年第二季度，营收环比增长14.6%，净利润环比增长74.9%，其中近9成公司营收环比正增长，7成公司净利润环比改善”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,有利可图的/盈利的(profitable):0.8"}, "亮眼的二季度业绩展现出半导体行业良好的复苏态势": {"topic": "“生产投资”", "similarity": 0.47958919405937195, "prompt": "新闻文本是“亮眼的二季度业绩展现出半导体行业良好的复苏态势”，包含的情绪词典是：复苏的/复兴的(resurgent):0.3,复苏/复兴(resurgence):0.3"}, "与此同时，沪市半导体公司积极践行“提质增效重回报”专项行动方案，积极通过中期分红回馈投资者，共有13家公司披露中期分红预案，合计分红金额约7亿元": {"topic": "“金融”", "similarity": 0.5649686455726624, "prompt": "新闻文本是“与此同时，沪市半导体公司积极践行“提质增效重回报”专项行动方案，积极通过中期分红回馈投资者，共有13家公司披露中期分红预案，合计分红金额约7亿元”，包含的情绪词典是：有益的/有回报的(rewarding):0.5,有利可图的/盈利的(profitable):0.8"}, "需求复苏推动龙头公司业绩回暖 　　今年第二季度，以成熟制程为主的晶圆代工需求复苏，国内龙头代工厂的收入、毛利率、产能利用率等关键指标环比均显著提升，且高于前期指引": {"topic": "“生产投资”", "similarity": 0.5923700928688049, "prompt": "新闻文本是“需求复苏推动龙头公司业绩回暖 　　今年第二季度，以成熟制程为主的晶圆代工需求复苏，国内龙头代工厂的收入、毛利率、产能利用率等关键指标环比均显著提升，且高于前期指引”，包含的情绪词典是：复苏的/复兴的(resurgent):0.3,反弹/回升(rebounding):0.3"}, "中芯国际2024年第二季度实现营收19.01亿美元，同比增长21.8%，环比增长8.6%，出货量环比增长近17.7%，毛利率为13.9%": {"topic": "“生产投资”", "similarity": 0.5626674294471741}, "对于今年第三季度，公司给出的收入指引为环比增长13%-15%，毛利率介于18%-20%范围内": {"topic": "“宏观经济”", "similarity": 0.4552828073501587, "prompt": "新闻文本是“对于今年第三季度，公司给出的收入指引为环比增长13%-15%，毛利率介于18%-20%范围内”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司已接近全方位满产，总体产能利用率为97.9%，较上季度提升6.2个百分点": {"topic": "“生产投资”", "similarity": 0.47419995069503784, "prompt": "新闻文本是“公司已接近全方位满产，总体产能利用率为97.9%，较上季度提升6.2个百分点”，包含的情绪词典是：生产/产量(production):0.4,多产的/富有成效的(productive):0.7"}, "半导体设备、材料行业的多家公司经营业绩延续良好态势，营收、净利润环比均呈现较快增长趋势": {"topic": "“生产投资”", "similarity": 0.4845622479915619, "prompt": "新闻文本是“半导体设备、材料行业的多家公司经营业绩延续良好态势，营收、净利润环比均呈现较快增长趋势”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,多产的/富有成效的(productive):0.7"}, "天岳先进作为国内碳化硅衬底龙头企业，在导电型碳化硅衬底领域实现后来居上，2023年市场规模跃居全球前二": {"topic": "“生产投资”", "similarity": 0.5732889175415039, "prompt": "新闻文本是“天岳先进作为国内碳化硅衬底龙头企业，在导电型碳化硅衬底领域实现后来居上，2023年市场规模跃居全球前二”，包含的情绪词典是：前进/进步(advance):0.6,上升的/占优势的(ascendant):0.3"}, "上半年，天岳先进实现营业收入9.12亿元，同比增长108.27%": {"topic": "“生产投资”", "similarity": 0.45743417739868164, "prompt": "新闻文本是“上半年，天岳先进实现营业收入9.12亿元，同比增长108.27%”，包含的情绪词典是：增长/发展(growth):0.7,营业额/周转(turnover):0.0"}, "华海清科从推出国内首台拥有自主知识产权的12英寸CMP设备，到如今第500台顺利交付，助力国内CMP设备产业自主发展": {"topic": "“生产投资”", "similarity": 0.5482317805290222}, "上半年，公司实现营业收入14.97亿元，同比增长21.23%": {"topic": "“宏观经济”", "similarity": 0.4416991174221039, "prompt": "新闻文本是“上半年，公司实现营业收入14.97亿元，同比增长21.23%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "归母净利润4.33亿元，同比增长15.65%": {"topic": "“生产投资”", "similarity": 0.42030060291290283, "prompt": "新闻文本是“归母净利润4.33亿元，同比增长15.65%”，包含的情绪词典是：增长/发展(growth):0.7,利润/利益(profit):0.8"}, "封测需求底部复苏明确，先进封装技术引领新增长，龙头公司业绩加速回暖": {"topic": "“生产投资”", "similarity": 0.49129706621170044, "prompt": "新闻文本是“封测需求底部复苏明确，先进封装技术引领新增长，龙头公司业绩加速回暖”，包含的情绪词典是：复苏的/复兴的(resurgent):0.3,复苏/复兴(resurgence):0.3"}, "今年上半年，封测行业的景气度延续复苏态势，主要公司的稼动率整体呈现稳定回升趋势，行业整体毛利率稳步回升，企业盈利能力得到显著改善": {"topic": "“生产投资”", "similarity": 0.5645349621772766, "prompt": "新闻文本是“今年上半年，封测行业的景气度延续复苏态势，主要公司的稼动率整体呈现稳定回升趋势，行业整体毛利率稳步回升，企业盈利能力得到显著改善”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "长电科技是国内封测龙头公司，上半年实现营业收入154.87亿元，同比增长27.22%": {"topic": "“生产投资”", "similarity": 0.5641677379608154, "prompt": "新闻文本是“长电科技是国内封测龙头公司，上半年实现营业收入154.87亿元，同比增长27.22%”，包含的情绪词典是：电子的(electronic):0.0,垄断者(monopolist):-0.3"}, "公司上半年业绩显著增长，得益于下游需求逐步复苏，部分客户业务量持续上升": {"topic": "“生产投资”", "similarity": 0.44050872325897217, "prompt": "新闻文本是“公司上半年业绩显著增长，得益于下游需求逐步复苏，部分客户业务量持续上升”，包含的情绪词典是：上升/上涨(rise):0.5,复苏的/复兴的(resurgent):0.3"}, "同时，公司大力拓展先进封装业务，聚焦新兴应用领域，积极进行产能利用率调控": {"topic": "“生产投资”", "similarity": 0.5012398958206177, "prompt": "新闻文本是“同时，公司大力拓展先进封装业务，聚焦新兴应用领域，积极进行产能利用率调控”，包含的情绪词典是：产能过剩(overcapacity):-0.5,开发/利用(exploit):-0.5"}, "甬矽电子专注于集成电路的先进封装与测试，上半年实现营业收入16.29亿元，同比增长65.81%": {"topic": "“生产投资”", "similarity": 0.5693292021751404, "prompt": "新闻文本是“甬矽电子专注于集成电路的先进封装与测试，上半年实现营业收入16.29亿元，同比增长65.81%”，包含的情绪词典是：电子的(electronic):0.0,公司/企业(firm):0.0"}, "公司坚持自身中高端先进封装业务定位，晶圆级封装、汽车电子等产品线持续丰富，“Bumping+CP+FC+FT”的一站式交付能力形成，公司竞争力持续增强": {"topic": "“生产投资”", "similarity": 0.5856317281723022, "prompt": "新闻文本是“公司坚持自身中高端先进封装业务定位，晶圆级封装、汽车电子等产品线持续丰富，“Bumping+CP+FC+FT”的一站式交付能力形成，公司竞争力持续增强”，包含的情绪词典是：公司的/企业的(corporate):0.0,增强的/提高的(enhanced):0.6"}, "消费市场回暖助力公司亮眼业绩 　　受益于消费电子复苏延续，汽车电子维持强劲，多家芯片设计公司业绩亮眼": {"topic": "“消费”", "similarity": 0.5464971661567688, "prompt": "新闻文本是“消费市场回暖助力公司亮眼业绩 　　受益于消费电子复苏延续，汽车电子维持强劲，多家芯片设计公司业绩亮眼”，包含的情绪词典是：消费者/用户(consumer):0.0,复苏的/复兴的(resurgent):0.3"}, "得益于消费市场持续回暖、公司在高端智能手机市场成功推出新品以及自动驾驶技术在汽车市场的不断深入应用，上半年，公司实现营收120.91亿元，同比增长36.50%": {"topic": "“消费”", "similarity": 0.5884538292884827}, "纳芯微聚焦传感器、信号链和电源管理三大产品方向": {"topic": "“生产投资”", "similarity": 0.46824002265930176, "prompt": "新闻文本是“纳芯微聚焦传感器、信号链和电源管理三大产品方向”，包含的情绪词典是：产品/产物(product):0.15,电子的(electronic):0.0"}, "半年报显示，其营收增长动力主要来自公司汽车电子领域相关产品持续放量，以及消费电子领域景气度的持续改善": {"topic": "“生产投资”", "similarity": 0.49196648597717285, "prompt": "新闻文本是“半年报显示，其营收增长动力主要来自公司汽车电子领域相关产品持续放量，以及消费电子领域景气度的持续改善”，包含的情绪词典是：电子的(electronic):0.0,汽车的/机动车的(automotive):0.0"}, "存储芯片整体延续回暖趋势，相关公司业绩出色": {"topic": "“金融”", "similarity": 0.4549444615840912, "prompt": "新闻文本是“存储芯片整体延续回暖趋势，相关公司业绩出色”，包含的情绪词典是：好转/向上趋势(upturn):0.4,反弹/回升(rebounding):0.3"}, "存储芯片价格经历快速上涨，市场的供需结构逐步改善，沪市存储芯片设计公司业绩表现抢眼": {"topic": "“金融”", "similarity": 0.5011666417121887, "prompt": "新闻文本是“存储芯片价格经历快速上涨，市场的供需结构逐步改善，沪市存储芯片设计公司业绩表现抢眼”，包含的情绪词典是：上升/上涨(rise):0.5,跑赢/表现优于(outperform):0.65"}, "兆易创新专注于存储器、微控制器及传感器的研发": {"topic": "“生产投资”", "similarity": 0.49244385957717896, "prompt": "新闻文本是“兆易创新专注于存储器、微控制器及传感器的研发”，包含的情绪词典是：创新/革新(innovation):0.7,创新/革新(innovate):0.6"}, "随着今年上半年消费和网通市场的显著回暖，公司存储芯片产品迎来销售高峰，直接推动产品销量和经营业绩大幅增加": {"topic": "“生产投资”", "similarity": 0.5518536567687988, "prompt": "新闻文本是“随着今年上半年消费和网通市场的显著回暖，公司存储芯片产品迎来销售高峰，直接推动产品销量和经营业绩大幅增加”，包含的情绪词典是：增加/增长(increase):0.6,营业额/周转(turnover):0.0"}, "澜起科技上半年实现营业收入16.65亿元，较上年同期增长79.49%": {"topic": "“生产投资”", "similarity": 0.45421522855758667, "prompt": "新闻文本是“澜起科技上半年实现营业收入16.65亿元，较上年同期增长79.49%”，包含的情绪词典是：增长/发展(growth):0.7,营业额/周转(turnover):0.0"}, "随着存储行业的复苏、AI服务器需求量快速增长，公司DDR5渗透率持续提升，高性能运力芯片新产品实现规模出货": {"topic": "“生产投资”", "similarity": 0.5429130792617798, "prompt": "新闻文本是“随着存储行业的复苏、AI服务器需求量快速增长，公司DDR5渗透率持续提升，高性能运力芯片新产品实现规模出货”，包含的情绪词典是：增加/增长(increase):0.6,繁荣的/兴旺的(prosperous):0.9"}, "沪市半导体公司立足新发展阶段、贯彻新发展理念，不断加大研发投入和产品创新力度": {"topic": "“生产投资”", "similarity": 0.5297757983207703, "prompt": "新闻文本是“沪市半导体公司立足新发展阶段、贯彻新发展理念，不断加大研发投入和产品创新力度”，包含的情绪词典是：发展/开发(development):0.4,创新的/革新的(innovative):0.7"}, "截至目前，相关公司上半年合计投入研发费": {"topic": "“生产投资”", "similarity": 0.4811916947364807, "prompt": "新闻文本是“截至目前，相关公司上半年合计投入研发费”，包含的情绪词典是：投资/投入(invest):0.3,投资/投资额(investment):0.4"}}</t>
+          <t>{"上证报中国证券网讯日前，沪市半导体公司均已完成2024年半年报披露": {"topic": "“生产投资”", "similarity": 0.451254665851593, "prompt": "新闻文本是“上证报中国证券网讯日前，沪市半导体公司均已完成2024年半年报披露”，包含的情绪词典是：完成/实现(accomplishes):0.6,完成/实现(accomplish):0.6"}, "上半年，沪市130余家半导体公司合计实现营业收入2112亿元，同比增长18.7%，超7成公司营业收入同比正增长，超5成公司净利润较去年同期有所改善": {"topic": "“生产投资”", "similarity": 0.554355800151825, "prompt": "新闻文本是“上半年，沪市130余家半导体公司合计实现营业收入2112亿元，同比增长18.7%，超7成公司营业收入同比正增长，超5成公司净利润较去年同期有所改善”，包含的情绪词典是：利润/利益(profit):0.8,有利可图的/盈利的(profitable):0.8"}, "分季度来看，2024年第二季度，营收环比增长14.6%，净利润环比增长74.9%，其中近9成公司营收环比正增长，7成公司净利润环比改善": {"topic": "“生产投资”", "similarity": 0.5821153521537781, "prompt": "新闻文本是“分季度来看，2024年第二季度，营收环比增长14.6%，净利润环比增长74.9%，其中近9成公司营收环比正增长，7成公司净利润环比改善”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,有利可图的/盈利的(profitable):0.8"}, "亮眼的二季度业绩展现出半导体行业良好的复苏态势": {"topic": "“生产投资”", "similarity": 0.4795893430709839, "prompt": "新闻文本是“亮眼的二季度业绩展现出半导体行业良好的复苏态势”，包含的情绪词典是：复苏的/复兴的(resurgent):0.3,复苏/复兴(resurgence):0.3"}, "与此同时，沪市半导体公司积极践行“提质增效重回报”专项行动方案，积极通过中期分红回馈投资者，共有13家公司披露中期分红预案，合计分红金额约7亿元": {"topic": "“金融”", "similarity": 0.5649688839912415, "prompt": "新闻文本是“与此同时，沪市半导体公司积极践行“提质增效重回报”专项行动方案，积极通过中期分红回馈投资者，共有13家公司披露中期分红预案，合计分红金额约7亿元”，包含的情绪词典是：有益的/有回报的(rewarding):0.5,有利可图的/盈利的(profitable):0.8"}, "需求复苏推动龙头公司业绩回暖 　　今年第二季度，以成熟制程为主的晶圆代工需求复苏，国内龙头代工厂的收入、毛利率、产能利用率等关键指标环比均显著提升，且高于前期指引": {"topic": "“生产投资”", "similarity": 0.5923702120780945, "prompt": "新闻文本是“需求复苏推动龙头公司业绩回暖 　　今年第二季度，以成熟制程为主的晶圆代工需求复苏，国内龙头代工厂的收入、毛利率、产能利用率等关键指标环比均显著提升，且高于前期指引”，包含的情绪词典是：复苏的/复兴的(resurgent):0.3,反弹/回升(rebounding):0.3"}, "对于今年第三季度，公司给出的收入指引为环比增长13%-15%，毛利率介于18%-20%范围内": {"topic": "“宏观经济”", "similarity": 0.45528316497802734, "prompt": "新闻文本是“对于今年第三季度，公司给出的收入指引为环比增长13%-15%，毛利率介于18%-20%范围内”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司已接近全方位满产，总体产能利用率为97.9%，较上季度提升6.2个百分点": {"topic": "“生产投资”", "similarity": 0.4742000997066498, "prompt": "新闻文本是“公司已接近全方位满产，总体产能利用率为97.9%，较上季度提升6.2个百分点”，包含的情绪词典是：生产/产量(production):0.4,多产的/富有成效的(productive):0.7"}, "半导体设备、材料行业的多家公司经营业绩延续良好态势，营收、净利润环比均呈现较快增长趋势": {"topic": "“生产投资”", "similarity": 0.4845622181892395, "prompt": "新闻文本是“半导体设备、材料行业的多家公司经营业绩延续良好态势，营收、净利润环比均呈现较快增长趋势”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,多产的/富有成效的(productive):0.7"}, "天岳先进作为国内碳化硅衬底龙头企业，在导电型碳化硅衬底领域实现后来居上，2023年市场规模跃居全球前二": {"topic": "“生产投资”", "similarity": 0.5732889175415039, "prompt": "新闻文本是“天岳先进作为国内碳化硅衬底龙头企业，在导电型碳化硅衬底领域实现后来居上，2023年市场规模跃居全球前二”，包含的情绪词典是：前进/进步(advance):0.6,上升的/占优势的(ascendant):0.3"}, "上半年，天岳先进实现营业收入9.12亿元，同比增长108.27%": {"topic": "“生产投资”", "similarity": 0.4574343264102936, "prompt": "新闻文本是“上半年，天岳先进实现营业收入9.12亿元，同比增长108.27%”，包含的情绪词典是：增长/发展(growth):0.7,营业额/周转(turnover):0.0"}, "上半年，公司实现营业收入14.97亿元，同比增长21.23%": {"topic": "“宏观经济”", "similarity": 0.4416993260383606, "prompt": "新闻文本是“上半年，公司实现营业收入14.97亿元，同比增长21.23%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "归母净利润4.33亿元，同比增长15.65%": {"topic": "“生产投资”", "similarity": 0.42030054330825806, "prompt": "新闻文本是“归母净利润4.33亿元，同比增长15.65%”，包含的情绪词典是：增长/发展(growth):0.7,利润/利益(profit):0.8"}, "封测需求底部复苏明确，先进封装技术引领新增长，龙头公司业绩加速回暖": {"topic": "“生产投资”", "similarity": 0.4912971556186676, "prompt": "新闻文本是“封测需求底部复苏明确，先进封装技术引领新增长，龙头公司业绩加速回暖”，包含的情绪词典是：复苏的/复兴的(resurgent):0.3,复苏/复兴(resurgence):0.3"}, "今年上半年，封测行业的景气度延续复苏态势，主要公司的稼动率整体呈现稳定回升趋势，行业整体毛利率稳步回升，企业盈利能力得到显著改善": {"topic": "“生产投资”", "similarity": 0.5645349621772766, "prompt": "新闻文本是“今年上半年，封测行业的景气度延续复苏态势，主要公司的稼动率整体呈现稳定回升趋势，行业整体毛利率稳步回升，企业盈利能力得到显著改善”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "长电科技是国内封测龙头公司，上半年实现营业收入154.87亿元，同比增长27.22%": {"topic": "“生产投资”", "similarity": 0.5641677379608154, "prompt": "新闻文本是“长电科技是国内封测龙头公司，上半年实现营业收入154.87亿元，同比增长27.22%”，包含的情绪词典是：电子的(electronic):0.0,垄断者(monopolist):-0.3"}, "公司上半年业绩显著增长，得益于下游需求逐步复苏，部分客户业务量持续上升": {"topic": "“生产投资”", "similarity": 0.44050881266593933, "prompt": "新闻文本是“公司上半年业绩显著增长，得益于下游需求逐步复苏，部分客户业务量持续上升”，包含的情绪词典是：上升/上涨(rise):0.5,复苏的/复兴的(resurgent):0.3"}, "同时，公司大力拓展先进封装业务，聚焦新兴应用领域，积极进行产能利用率调控": {"topic": "“生产投资”", "similarity": 0.5012398958206177, "prompt": "新闻文本是“同时，公司大力拓展先进封装业务，聚焦新兴应用领域，积极进行产能利用率调控”，包含的情绪词典是：产能过剩(overcapacity):-0.5,开发/利用(exploit):-0.5"}, "甬矽电子专注于集成电路的先进封装与测试，上半年实现营业收入16.29亿元，同比增长65.81%": {"topic": "“生产投资”", "similarity": 0.5693290829658508, "prompt": "新闻文本是“甬矽电子专注于集成电路的先进封装与测试，上半年实现营业收入16.29亿元，同比增长65.81%”，包含的情绪词典是：电子的(electronic):0.0,公司/企业(firm):0.0"}, "公司坚持自身中高端先进封装业务定位，晶圆级封装、汽车电子等产品线持续丰富，“Bumping+CP+FC+FT”的一站式交付能力形成，公司竞争力持续增强": {"topic": "“生产投资”", "similarity": 0.5856316685676575, "prompt": "新闻文本是“公司坚持自身中高端先进封装业务定位，晶圆级封装、汽车电子等产品线持续丰富，“Bumping+CP+FC+FT”的一站式交付能力形成，公司竞争力持续增强”，包含的情绪词典是：公司的/企业的(corporate):0.0,增强的/提高的(enhanced):0.6"}, "消费市场回暖助力公司亮眼业绩 　　受益于消费电子复苏延续，汽车电子维持强劲，多家芯片设计公司业绩亮眼": {"topic": "“消费”", "similarity": 0.5464972257614136, "prompt": "新闻文本是“消费市场回暖助力公司亮眼业绩 　　受益于消费电子复苏延续，汽车电子维持强劲，多家芯片设计公司业绩亮眼”，包含的情绪词典是：消费者/用户(consumer):0.0,复苏的/复兴的(resurgent):0.3"}, "纳芯微聚焦传感器、信号链和电源管理三大产品方向": {"topic": "“生产投资”", "similarity": 0.46824008226394653, "prompt": "新闻文本是“纳芯微聚焦传感器、信号链和电源管理三大产品方向”，包含的情绪词典是：产品/产物(product):0.15,电子的(electronic):0.0"}, "半年报显示，其营收增长动力主要来自公司汽车电子领域相关产品持续放量，以及消费电子领域景气度的持续改善": {"topic": "“生产投资”", "similarity": 0.49196651577949524, "prompt": "新闻文本是“半年报显示，其营收增长动力主要来自公司汽车电子领域相关产品持续放量，以及消费电子领域景气度的持续改善”，包含的情绪词典是：电子的(electronic):0.0,汽车的/机动车的(automotive):0.0"}, "存储芯片整体延续回暖趋势，相关公司业绩出色": {"topic": "“金融”", "similarity": 0.4549446105957031, "prompt": "新闻文本是“存储芯片整体延续回暖趋势，相关公司业绩出色”，包含的情绪词典是：好转/向上趋势(upturn):0.4,反弹/回升(rebounding):0.3"}, "存储芯片价格经历快速上涨，市场的供需结构逐步改善，沪市存储芯片设计公司业绩表现抢眼": {"topic": "“金融”", "similarity": 0.5011667609214783, "prompt": "新闻文本是“存储芯片价格经历快速上涨，市场的供需结构逐步改善，沪市存储芯片设计公司业绩表现抢眼”，包含的情绪词典是：上升/上涨(rise):0.5,跑赢/表现优于(outperform):0.65"}, "兆易创新专注于存储器、微控制器及传感器的研发": {"topic": "“生产投资”", "similarity": 0.4924437999725342, "prompt": "新闻文本是“兆易创新专注于存储器、微控制器及传感器的研发”，包含的情绪词典是：创新/革新(innovation):0.7,创新/革新(innovate):0.6"}, "随着今年上半年消费和网通市场的显著回暖，公司存储芯片产品迎来销售高峰，直接推动产品销量和经营业绩大幅增加": {"topic": "“生产投资”", "similarity": 0.5518537759780884, "prompt": "新闻文本是“随着今年上半年消费和网通市场的显著回暖，公司存储芯片产品迎来销售高峰，直接推动产品销量和经营业绩大幅增加”，包含的情绪词典是：增加/增长(increase):0.6,营业额/周转(turnover):0.0"}, "澜起科技上半年实现营业收入16.65亿元，较上年同期增长79.49%": {"topic": "“生产投资”", "similarity": 0.454215407371521, "prompt": "新闻文本是“澜起科技上半年实现营业收入16.65亿元，较上年同期增长79.49%”，包含的情绪词典是：增长/发展(growth):0.7,营业额/周转(turnover):0.0"}, "随着存储行业的复苏、AI服务器需求量快速增长，公司DDR5渗透率持续提升，高性能运力芯片新产品实现规模出货": {"topic": "“生产投资”", "similarity": 0.5429131984710693, "prompt": "新闻文本是“随着存储行业的复苏、AI服务器需求量快速增长，公司DDR5渗透率持续提升，高性能运力芯片新产品实现规模出货”，包含的情绪词典是：增加/增长(increase):0.6,繁荣的/兴旺的(prosperous):0.9"}, "沪市半导体公司立足新发展阶段、贯彻新发展理念，不断加大研发投入和产品创新力度": {"topic": "“生产投资”", "similarity": 0.5297759175300598, "prompt": "新闻文本是“沪市半导体公司立足新发展阶段、贯彻新发展理念，不断加大研发投入和产品创新力度”，包含的情绪词典是：发展/开发(development):0.4,创新的/革新的(innovative):0.7"}, "截至目前，相关公司上半年合计投入研发费": {"topic": "“生产投资”", "similarity": 0.4811916947364807, "prompt": "新闻文本是“截至目前，相关公司上半年合计投入研发费”，包含的情绪词典是：投资/投入(invest):0.3,投资/投资额(investment):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -1921,12 +1913,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "ST恒久再度涨停，4个交易日内录得3个涨停，累计涨幅为20.48%，累计换手率为23.76%", "news_prompt2": "截至10:31，该股今日成交量998.57万股，成交金额1936.63万元，换手率5.36%", "news_prompt3": "最新A股总市值达5.38亿元，A股流通市值3.73亿元", "news_prompt4": "8月29日公司发布的半年报数据显示，上半年公司共实现营业总收入0.74亿元，同比增长9.15%，实现净利润-0.13亿元，同比下降223.52%", "news_prompt5": "（数据宝）　　近日该股表现日期当日涨跌幅（%）换手率（%）主力资金净流入（万元）2024.08.304.975.8599.592024.08.294.026.57-117.432024.08.284.825.9841.332024.08.271.843.6581.962024.08.260.002.74-133.712024.08.23-5.234.24-101.902024.08.221.183.59-126.632024.08.211.192.0819.622024.08.201.202.6294.222024.08.19-2.922.06-3.36（文章来源：证券时报网）"}</t>
+          <t>{"news_prompt1": "ST恒久再度涨停，4个交易日内录得3个涨停，累计涨幅为20.48%，累计换手率为23.76%", "news_prompt2": "截至10:31，该股今日成交量998.57万股，成交金额1936.63万元，换手率5.36%", "news_prompt3": "最新A股总市值达5.38亿元，A股流通市值3.73亿元", "news_prompt4": "8月29日公司发布的半年报数据显示，上半年公司共实现营业总收入0.74亿元，同比增长9.15%，实现净利润-0.13亿元，同比下降223.52%"}</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>{"ST恒久再度涨停，4个交易日内录得3个涨停，累计涨幅为20.48%，累计换手率为23.76%": {"topic": "“金融”", "similarity": 0.5223444104194641, "prompt": "新闻文本是“ST恒久再度涨停，4个交易日内录得3个涨停，累计涨幅为20.48%，累计换手率为23.76%”，包含的情绪词典是：持久的/永久的(abiding):0.1,恒定的/不变的(constant):0.05"}, "截至10:31，该股今日成交量998.57万股，成交金额1936.63万元，换手率5.36%": {"topic": "“金融”", "similarity": 0.5640245079994202, "prompt": "新闻文本是“截至10:31，该股今日成交量998.57万股，成交金额1936.63万元，换手率5.36%”，包含的情绪词典是：股票/库存(stock):0.0,清仓/抛售(closeout):-0.2"}, "最新A股总市值达5.38亿元，A股流通市值3.73亿元": {"topic": "“金融”", "similarity": 0.597398042678833, "prompt": "新闻文本是“最新A股总市值达5.38亿元，A股流通市值3.73亿元”，包含的情绪词典是：资本/资金(capital):0.1,投资/投资额(investment):0.4"}, "8月29日公司发布的半年报数据显示，上半年公司共实现营业总收入0.74亿元，同比增长9.15%，实现净利润-0.13亿元，同比下降223.52%": {"topic": "“消费”", "similarity": 0.5765836238861084, "prompt": "新闻文本是“8月29日公司发布的半年报数据显示，上半年公司共实现营业总收入0.74亿元，同比增长9.15%，实现净利润-0.13亿元，同比下降223.52%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "（数据宝）　　近日该股表现日期当日涨跌幅（%）换手率（%）主力资金净流入（万元）2024.08.304.975.8599.592024.08.294.026.57-117.432024.08.284.825.9841.332024.08.271.843.6581.962024.08.260.002.74-133.712024.08.23-5.234.24-101.902024.08.221.183.59-126.632024.08.211.192.0819.622024.08.201.202.6294.222024.08.19-2.922.06-3.36（文章来源：证券时报网）": {"topic": "“消费”", "similarity": 0.5665487051010132}}</t>
+          <t>{"ST恒久再度涨停，4个交易日内录得3个涨停，累计涨幅为20.48%，累计换手率为23.76%": {"topic": "“金融”", "similarity": 0.5223443508148193, "prompt": "新闻文本是“ST恒久再度涨停，4个交易日内录得3个涨停，累计涨幅为20.48%，累计换手率为23.76%”，包含的情绪词典是：持久的/永久的(abiding):0.1,恒定的/不变的(constant):0.05"}, "截至10:31，该股今日成交量998.57万股，成交金额1936.63万元，换手率5.36%": {"topic": "“金融”", "similarity": 0.5640247464179993, "prompt": "新闻文本是“截至10:31，该股今日成交量998.57万股，成交金额1936.63万元，换手率5.36%”，包含的情绪词典是：股票/库存(stock):0.0,清仓/抛售(closeout):-0.2"}, "最新A股总市值达5.38亿元，A股流通市值3.73亿元": {"topic": "“金融”", "similarity": 0.5973982810974121, "prompt": "新闻文本是“最新A股总市值达5.38亿元，A股流通市值3.73亿元”，包含的情绪词典是：资本/资金(capital):0.1,投资/投资额(investment):0.4"}, "8月29日公司发布的半年报数据显示，上半年公司共实现营业总收入0.74亿元，同比增长9.15%，实现净利润-0.13亿元，同比下降223.52%": {"topic": "“消费”", "similarity": 0.5765836238861084, "prompt": "新闻文本是“8月29日公司发布的半年报数据显示，上半年公司共实现营业总收入0.74亿元，同比增长9.15%，实现净利润-0.13亿元，同比下降223.52%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -1976,12 +1968,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "证券时报网讯，国金证券研报指出，苹果iPhone16系列新机即将发布，新机备货8800万—9000万部，Apple Intelligence有望给iPhone16新机赋能，加快换机周期，苹果产业链竞争格局较好，有望迎来量价齐升", "news_prompt2": "下半年智能手机、AI PC将迎来众多新机发布，云厂商二季度资本开支乐观，英伟达GB200延后不改向好趋势，继续看好消费电子创新/需求复苏、AI驱动及自主可控受益产业链", "news_prompt3": "建议关注：立讯精密、水晶光电、沪电股份等", "news_prompt4": "（文章来源：证券时报网）"}</t>
+          <t>{"news_prompt1": "证券时报网讯，国金证券研报指出，苹果iPhone16系列新机即将发布，新机备货8800万—9000万部，Apple Intelligence有望给iPhone16新机赋能，加快换机周期，苹果产业链竞争格局较好，有望迎来量价齐升", "news_prompt2": "下半年智能手机、AI PC将迎来众多新机发布，云厂商二季度资本开支乐观，英伟达GB200延后不改向好趋势，继续看好消费电子创新/需求复苏、AI驱动及自主可控受益产业链"}</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，国金证券研报指出，苹果iPhone16系列新机即将发布，新机备货8800万—9000万部，Apple Intelligence有望给iPhone16新机赋能，加快换机周期，苹果产业链竞争格局较好，有望迎来量价齐升": {"topic": "“生产投资”", "similarity": 0.5295904874801636, "prompt": "新闻文本是“证券时报网讯，国金证券研报指出，苹果iPhone16系列新机即将发布，新机备货8800万—9000万部，Apple Intelligence有望给iPhone16新机赋能，加快换机周期，苹果产业链竞争格局较好，有望迎来量价齐升”，包含的情绪词典是：储备/囤积(stockpile):0.1"}, "下半年智能手机、AI PC将迎来众多新机发布，云厂商二季度资本开支乐观，英伟达GB200延后不改向好趋势，继续看好消费电子创新/需求复苏、AI驱动及自主可控受益产业链": {"topic": "“生产投资”", "similarity": 0.6198190450668335, "prompt": "新闻文本是“下半年智能手机、AI PC将迎来众多新机发布，云厂商二季度资本开支乐观，英伟达GB200延后不改向好趋势，继续看好消费电子创新/需求复苏、AI驱动及自主可控受益产业链”，包含的情绪词典是：数字的/数码的(digital):0.0,下一个/接下来的(next):0.0"}, "建议关注：立讯精密、水晶光电、沪电股份等": {"topic": "“生产投资”", "similarity": 0.5754582285881042, "prompt": "新闻文本是“建议关注：立讯精密、水晶光电、沪电股份等”，包含的情绪词典是：电子的(electronic):0.0,电的/电气的(electrical):0.0"}, "（文章来源：证券时报网）": {"topic": "“金融”", "similarity": 0.4481872320175171, "prompt": "新闻文本是“（文章来源：证券时报网）”，包含的情绪词典是：股票/库存(stock):0.0,资本/资金(capital):0.1"}}</t>
+          <t>{"证券时报网讯，国金证券研报指出，苹果iPhone16系列新机即将发布，新机备货8800万—9000万部，Apple Intelligence有望给iPhone16新机赋能，加快换机周期，苹果产业链竞争格局较好，有望迎来量价齐升": {"topic": "“生产投资”", "similarity": 0.5295906662940979, "prompt": "新闻文本是“证券时报网讯，国金证券研报指出，苹果iPhone16系列新机即将发布，新机备货8800万—9000万部，Apple Intelligence有望给iPhone16新机赋能，加快换机周期，苹果产业链竞争格局较好，有望迎来量价齐升”，包含的情绪词典是：储备/囤积(stockpile):0.1"}, "下半年智能手机、AI PC将迎来众多新机发布，云厂商二季度资本开支乐观，英伟达GB200延后不改向好趋势，继续看好消费电子创新/需求复苏、AI驱动及自主可控受益产业链": {"topic": "“生产投资”", "similarity": 0.6198190450668335, "prompt": "新闻文本是“下半年智能手机、AI PC将迎来众多新机发布，云厂商二季度资本开支乐观，英伟达GB200延后不改向好趋势，继续看好消费电子创新/需求复苏、AI驱动及自主可控受益产业链”，包含的情绪词典是：数字的/数码的(digital):0.0,下一个/接下来的(next):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -2025,16 +2017,8 @@
           <t>南方财经网</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>{"news_prompt1": "南方财经9月2日电，AI眼镜概念局部回暖，星星科技涨超10%，卓翼科技涨停，宜安科技、博士眼镜、联合光电等跟涨", "news_prompt2": "（文章来源：南方财经网）"}</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>{"南方财经9月2日电，AI眼镜概念局部回暖，星星科技涨超10%，卓翼科技涨停，宜安科技、博士眼镜、联合光电等跟涨": {"topic": "“金融”", "similarity": 0.45845916867256165}, "（文章来源：南方财经网）": {"topic": "“金融”", "similarity": 0.4414668679237366, "prompt": "新闻文本是“（文章来源：南方财经网）”，包含的情绪词典是：金融/财政(finance):0.0,金融的/财政的(financial):0.0"}}</t>
-        </is>
-      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2082,12 +2066,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "8月31日，锴威特披露上半年业绩，公司实现营业总收入5763.07万元", "news_prompt2": "上半年，受数字经济、AI及新质生产力发展的推动，与数字芯片相关的晶圆代工及封测呈恢复态势，但功率及模拟类仍不达预期，功率半导体行业竞争加剧，成本不断上升", "news_prompt3": "为积极应对市场挑战，进一步提升市场份额，锴威特持续加大产品研发投入，针对高可靠、新能源、储能、智能电网等重点应用领域进行产品布局", "news_prompt4": "报告期内，公司研发费用为2498.00万元，同比增长43.58%，研发费用占营业收入的比例为43.35%", "news_prompt5": "同时，丰富公司产品布局", "news_prompt6": "PWM控制IC方面：完成了反激、正激、半桥、推挽、全桥、移相全桥等隔离拓扑产品系列化，推出了输入电压高达100V以上同步Buck控制器、同步Boost控制器等新品", "news_prompt7": "为提高电源系统效率，推出了可支持反激、QR、LLC等拓扑的同步整流驱动IC，工作频率可高达1MHz，工作电压可达300V", "news_prompt8": "功率驱动IC方面：推出80V 3A集成MOSFET的单芯片H桥驱动芯片，同时可支持100%占空比工作，进一步提升系统的安全及可靠性", "news_prompt9": "推出180V GaN专用半桥驱动芯片，工作频率高达1MHz以上", "news_prompt10": "在功率MOSFET方面，开发完善了沟槽MOSFET及高压超结的工艺平台优化和产品布局，开发了100V SGT工艺平台及12寸20V-40V的沟槽工艺平台，完成了650V 100A大电流的超结产品开发", "news_prompt11": "SiC MOSFET方面：公司与国内晶圆代工厂合作开发了1200V、1700V、2600V、3300VSiC MOSFET的生产工艺平台，其中1200V SiC MOSFET工艺平台已成功进入中试阶段，新推出2600V和3300V SiC MOSFET产品，目前，产品正在客户验证中", "news_prompt12": "值得一提的是，为回报广大投资者对公司的信任，稳定投资者信心，提振市场情绪，切实保护投资者利益，公司拟实施2024年度中期分红，拟向全体股东每10股派发现金红利1元（含税）", "news_prompt13": "（宁晖）（文章来源：上海证券报·中国证券网）"}</t>
+          <t>{"news_prompt1": "8月31日，锴威特披露上半年业绩，公司实现营业总收入5763.07万元", "news_prompt2": "上半年，受数字经济、AI及新质生产力发展的推动，与数字芯片相关的晶圆代工及封测呈恢复态势，但功率及模拟类仍不达预期，功率半导体行业竞争加剧，成本不断上升", "news_prompt3": "为积极应对市场挑战，进一步提升市场份额，锴威特持续加大产品研发投入，针对高可靠、新能源、储能、智能电网等重点应用领域进行产品布局", "news_prompt4": "报告期内，公司研发费用为2498.00万元，同比增长43.58%，研发费用占营业收入的比例为43.35%", "news_prompt5": "同时，丰富公司产品布局", "news_prompt6": "PWM控制IC方面：完成了反激、正激、半桥、推挽、全桥、移相全桥等隔离拓扑产品系列化，推出了输入电压高达100V以上同步Buck控制器、同步Boost控制器等新品", "news_prompt7": "为提高电源系统效率，推出了可支持反激、QR、LLC等拓扑的同步整流驱动IC，工作频率可高达1MHz，工作电压可达300V", "news_prompt8": "功率驱动IC方面：推出80V 3A集成MOSFET的单芯片H桥驱动芯片，同时可支持100%占空比工作，进一步提升系统的安全及可靠性", "news_prompt9": "在功率MOSFET方面，开发完善了沟槽MOSFET及高压超结的工艺平台优化和产品布局，开发了100V SGT工艺平台及12寸20V-40V的沟槽工艺平台，完成了650V 100A大电流的超结产品开发", "news_prompt10": "SiC MOSFET方面：公司与国内晶圆代工厂合作开发了1200V、1700V、2600V、3300VSiC MOSFET的生产工艺平台，其中1200V SiC MOSFET工艺平台已成功进入中试阶段，新推出2600V和3300V SiC MOSFET产品，目前，产品正在客户验证中", "news_prompt11": "值得一提的是，为回报广大投资者对公司的信任，稳定投资者信心，提振市场情绪，切实保护投资者利益，公司拟实施2024年度中期分红，拟向全体股东每10股派发现金红利1元（含税）"}</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>{"8月31日，锴威特披露上半年业绩，公司实现营业总收入5763.07万元": {"topic": "“生产投资”", "similarity": 0.42213261127471924, "prompt": "新闻文本是“8月31日，锴威特披露上半年业绩，公司实现营业总收入5763.07万元”，包含的情绪词典是：营业额/周转(turnover):0.0,公司/企业(company):0.0"}, "上半年，受数字经济、AI及新质生产力发展的推动，与数字芯片相关的晶圆代工及封测呈恢复态势，但功率及模拟类仍不达预期，功率半导体行业竞争加剧，成本不断上升": {"topic": "“生产投资”", "similarity": 0.6571200489997864, "prompt": "新闻文本是“上半年，受数字经济、AI及新质生产力发展的推动，与数字芯片相关的晶圆代工及封测呈恢复态势，但功率及模拟类仍不达预期，功率半导体行业竞争加剧，成本不断上升”，包含的情绪词典是：生产不足的/产量低于预期的(underproduced):-0.5,数字的/数码的(digital):0.0"}, "为积极应对市场挑战，进一步提升市场份额，锴威特持续加大产品研发投入，针对高可靠、新能源、储能、智能电网等重点应用领域进行产品布局": {"topic": "“生产投资”", "similarity": 0.6166322231292725, "prompt": "新闻文本是“为积极应对市场挑战，进一步提升市场份额，锴威特持续加大产品研发投入，针对高可靠、新能源、储能、智能电网等重点应用领域进行产品布局”，包含的情绪词典是：发展/开发(development):0.4,进步/提升(advancement):0.5"}, "报告期内，公司研发费用为2498.00万元，同比增长43.58%，研发费用占营业收入的比例为43.35%": {"topic": "“生产投资”", "similarity": 0.4934045374393463, "prompt": "新闻文本是“报告期内，公司研发费用为2498.00万元，同比增长43.58%，研发费用占营业收入的比例为43.35%”，包含的情绪词典是：发展/开发(development):0.4,增加/增长(increase):0.6"}, "同时，丰富公司产品布局": {"topic": "“生产投资”", "similarity": 0.42212629318237305, "prompt": "新闻文本是“同时，丰富公司产品布局”，包含的情绪词典是：丰富/充裕(abundance):0.7,丰富的/充裕的(abundant):0.7"}, "PWM控制IC方面：完成了反激、正激、半桥、推挽、全桥、移相全桥等隔离拓扑产品系列化，推出了输入电压高达100V以上同步Buck控制器、同步Boost控制器等新品": {"topic": "“生产投资”", "similarity": 0.5240331888198853, "prompt": "新闻文本是“PWM控制IC方面：完成了反激、正激、半桥、推挽、全桥、移相全桥等隔离拓扑产品系列化，推出了输入电压高达100V以上同步Buck控制器、同步Boost控制器等新品”，包含的情绪词典是：电的/电气的(electrical):0.0,电子的(electronic):0.0"}, "为提高电源系统效率，推出了可支持反激、QR、LLC等拓扑的同步整流驱动IC，工作频率可高达1MHz，工作电压可达300V": {"topic": "“生产投资”", "similarity": 0.4423852562904358, "prompt": "新闻文本是“为提高电源系统效率，推出了可支持反激、QR、LLC等拓扑的同步整流驱动IC，工作频率可高达1MHz，工作电压可达300V”，包含的情绪词典是：电的/电气的(electrical):0.0,电子的(electronic):0.0"}, "功率驱动IC方面：推出80V 3A集成MOSFET的单芯片H桥驱动芯片，同时可支持100%占空比工作，进一步提升系统的安全及可靠性": {"topic": "“生产投资”", "similarity": 0.5231931805610657, "prompt": "新闻文本是“功率驱动IC方面：推出80V 3A集成MOSFET的单芯片H桥驱动芯片，同时可支持100%占空比工作，进一步提升系统的安全及可靠性”，包含的情绪词典是：电子的(electronic):0.0,技术的/工艺的(technical):0.0"}, "在功率MOSFET方面，开发完善了沟槽MOSFET及高压超结的工艺平台优化和产品布局，开发了100V SGT工艺平台及12寸20V-40V的沟槽工艺平台，完成了650V 100A大电流的超结产品开发": {"topic": "“生产投资”", "similarity": 0.5858602523803711, "prompt": "新闻文本是“在功率MOSFET方面，开发完善了沟槽MOSFET及高压超结的工艺平台优化和产品布局，开发了100V SGT工艺平台及12寸20V-40V的沟槽工艺平台，完成了650V 100A大电流的超结产品开发”，包含的情绪词典是：已改善的/已改进的(improved):0.5,正在改善的/正在改进的(improving):0.5"}, "SiC MOSFET方面：公司与国内晶圆代工厂合作开发了1200V、1700V、2600V、3300VSiC MOSFET的生产工艺平台，其中1200V SiC MOSFET工艺平台已成功进入中试阶段，新推出2600V和3300V SiC MOSFET产品，目前，产品正在客户验证中": {"topic": "“生产投资”", "similarity": 0.568509578704834, "prompt": "新闻文本是“SiC MOSFET方面：公司与国内晶圆代工厂合作开发了1200V、1700V、2600V、3300VSiC MOSFET的生产工艺平台，其中1200V SiC MOSFET工艺平台已成功进入中试阶段，新推出2600V和3300V SiC MOSFET产品，目前，产品正在客户验证中”，包含的情绪词典是：电的/电气的(electrical):0.0"}, "值得一提的是，为回报广大投资者对公司的信任，稳定投资者信心，提振市场情绪，切实保护投资者利益，公司拟实施2024年度中期分红，拟向全体股东每10股派发现金红利1元（含税）": {"topic": "“金融”", "similarity": 0.5492623448371887, "prompt": "新闻文本是“值得一提的是，为回报广大投资者对公司的信任，稳定投资者信心，提振市场情绪，切实保护投资者利益，公司拟实施2024年度中期分红，拟向全体股东每10股派发现金红利1元（含税）”，包含的情绪词典是：有益的/有回报的(rewarding):0.5"}, "（宁晖）（文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.47504258155822754, "prompt": "新闻文本是“（宁晖）（文章来源：上海证券报·中国证券网）”，包含的情绪词典是：投资者/投资人(investor):0.4,投资/投资额(investment):0.4"}}</t>
+          <t>{"8月31日，锴威特披露上半年业绩，公司实现营业总收入5763.07万元": {"topic": "“生产投资”", "similarity": 0.422132670879364, "prompt": "新闻文本是“8月31日，锴威特披露上半年业绩，公司实现营业总收入5763.07万元”，包含的情绪词典是：营业额/周转(turnover):0.0,公司/企业(company):0.0"}, "上半年，受数字经济、AI及新质生产力发展的推动，与数字芯片相关的晶圆代工及封测呈恢复态势，但功率及模拟类仍不达预期，功率半导体行业竞争加剧，成本不断上升": {"topic": "“生产投资”", "similarity": 0.6571201682090759, "prompt": "新闻文本是“上半年，受数字经济、AI及新质生产力发展的推动，与数字芯片相关的晶圆代工及封测呈恢复态势，但功率及模拟类仍不达预期，功率半导体行业竞争加剧，成本不断上升”，包含的情绪词典是：生产不足的/产量低于预期的(underproduced):-0.5,数字的/数码的(digital):0.0"}, "为积极应对市场挑战，进一步提升市场份额，锴威特持续加大产品研发投入，针对高可靠、新能源、储能、智能电网等重点应用领域进行产品布局": {"topic": "“生产投资”", "similarity": 0.6166322231292725, "prompt": "新闻文本是“为积极应对市场挑战，进一步提升市场份额，锴威特持续加大产品研发投入，针对高可靠、新能源、储能、智能电网等重点应用领域进行产品布局”，包含的情绪词典是：发展/开发(development):0.4,进步/提升(advancement):0.5"}, "报告期内，公司研发费用为2498.00万元，同比增长43.58%，研发费用占营业收入的比例为43.35%": {"topic": "“生产投资”", "similarity": 0.4934046268463135, "prompt": "新闻文本是“报告期内，公司研发费用为2498.00万元，同比增长43.58%，研发费用占营业收入的比例为43.35%”，包含的情绪词典是：发展/开发(development):0.4,增加/增长(increase):0.6"}, "同时，丰富公司产品布局": {"topic": "“生产投资”", "similarity": 0.4221263527870178, "prompt": "新闻文本是“同时，丰富公司产品布局”，包含的情绪词典是：丰富/充裕(abundance):0.7,丰富的/充裕的(abundant):0.7"}, "PWM控制IC方面：完成了反激、正激、半桥、推挽、全桥、移相全桥等隔离拓扑产品系列化，推出了输入电压高达100V以上同步Buck控制器、同步Boost控制器等新品": {"topic": "“生产投资”", "similarity": 0.5240331292152405, "prompt": "新闻文本是“PWM控制IC方面：完成了反激、正激、半桥、推挽、全桥、移相全桥等隔离拓扑产品系列化，推出了输入电压高达100V以上同步Buck控制器、同步Boost控制器等新品”，包含的情绪词典是：电的/电气的(electrical):0.0,电子的(electronic):0.0"}, "为提高电源系统效率，推出了可支持反激、QR、LLC等拓扑的同步整流驱动IC，工作频率可高达1MHz，工作电压可达300V": {"topic": "“生产投资”", "similarity": 0.44238531589508057, "prompt": "新闻文本是“为提高电源系统效率，推出了可支持反激、QR、LLC等拓扑的同步整流驱动IC，工作频率可高达1MHz，工作电压可达300V”，包含的情绪词典是：电的/电气的(electrical):0.0,电子的(electronic):0.0"}, "功率驱动IC方面：推出80V 3A集成MOSFET的单芯片H桥驱动芯片，同时可支持100%占空比工作，进一步提升系统的安全及可靠性": {"topic": "“生产投资”", "similarity": 0.5231932997703552, "prompt": "新闻文本是“功率驱动IC方面：推出80V 3A集成MOSFET的单芯片H桥驱动芯片，同时可支持100%占空比工作，进一步提升系统的安全及可靠性”，包含的情绪词典是：电子的(electronic):0.0,技术的/工艺的(technical):0.0"}, "在功率MOSFET方面，开发完善了沟槽MOSFET及高压超结的工艺平台优化和产品布局，开发了100V SGT工艺平台及12寸20V-40V的沟槽工艺平台，完成了650V 100A大电流的超结产品开发": {"topic": "“生产投资”", "similarity": 0.5858603119850159, "prompt": "新闻文本是“在功率MOSFET方面，开发完善了沟槽MOSFET及高压超结的工艺平台优化和产品布局，开发了100V SGT工艺平台及12寸20V-40V的沟槽工艺平台，完成了650V 100A大电流的超结产品开发”，包含的情绪词典是：已改善的/已改进的(improved):0.5,正在改善的/正在改进的(improving):0.5"}, "SiC MOSFET方面：公司与国内晶圆代工厂合作开发了1200V、1700V、2600V、3300VSiC MOSFET的生产工艺平台，其中1200V SiC MOSFET工艺平台已成功进入中试阶段，新推出2600V和3300V SiC MOSFET产品，目前，产品正在客户验证中": {"topic": "“生产投资”", "similarity": 0.5685096979141235, "prompt": "新闻文本是“SiC MOSFET方面：公司与国内晶圆代工厂合作开发了1200V、1700V、2600V、3300VSiC MOSFET的生产工艺平台，其中1200V SiC MOSFET工艺平台已成功进入中试阶段，新推出2600V和3300V SiC MOSFET产品，目前，产品正在客户验证中”，包含的情绪词典是：电的/电气的(electrical):0.0"}, "值得一提的是，为回报广大投资者对公司的信任，稳定投资者信心，提振市场情绪，切实保护投资者利益，公司拟实施2024年度中期分红，拟向全体股东每10股派发现金红利1元（含税）": {"topic": "“金融”", "similarity": 0.549262523651123, "prompt": "新闻文本是“值得一提的是，为回报广大投资者对公司的信任，稳定投资者信心，提振市场情绪，切实保护投资者利益，公司拟实施2024年度中期分红，拟向全体股东每10股派发现金红利1元（含税）”，包含的情绪词典是：有益的/有回报的(rewarding):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -2137,12 +2121,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月第一天，国内多家新势力公布8月交付数据", "news_prompt2": "8月，理想汽车蝉联第一，交付新车48,122辆，同比增长37.8%", "news_prompt3": "广汽埃安8月全球销量35355辆", "news_prompt4": "鸿蒙智行8月全系交付新车33699辆", "news_prompt5": "此外，零跑汽车月度交付量首次突破3万辆，交付30305辆，连创历史新高，同比增长超113%", "news_prompt6": "蔚来交付新车20,176辆，连续4个月超2万辆", "news_prompt7": "8月极氪交付18,015辆，同比增长46%", "news_prompt8": "小鹏汽车8月共交付新车14,036辆，同比微增3%", "news_prompt9": "哪吒汽车8月全系整车交付11,005辆", "news_prompt10": "继7月新能源汽车渗透率突破50%之后，乘联会预计8月新能源零售可达98.0万辆，渗透率预计将进一步提升至53.2%", "news_prompt11": "零跑汽车首次突破3万辆 　　根据乘联会的调研，8月，插电混动市场稳定发力的同时，低价纯电产品销量也有较为明显的提升，8月新能源市场持续走高，表现十分强劲", "news_prompt12": "具体来看，理想汽车8月交付新车48,122辆，同比增长37.8%", "news_prompt13": "其中，理想L6成为销量担当，连续3个月交付量突破2万辆", "news_prompt14": "“在20万元以上新能源汽车市场，理想汽车7月的市占率达到18%，超越特斯拉成为新能源汽车品牌销量冠军", "news_prompt15": "” 理想汽车董事长兼CEO李想表示", "news_prompt16": "广汽埃安8月全球销量35355辆", "news_prompt17": "广汽埃安透露，埃安霸王龙上市交付首月突破6000辆", "news_prompt18": "8月，鸿蒙智行全系交付新车33699辆，同比下滑23.6%", "news_prompt19": "问界仍是其销量主力，8月交付新车31216辆", "news_prompt20": "另一家交付量超过3万辆的是零跑汽车", "news_prompt21": "8月交付量达到30305辆，同比增长超113%，环比增长超37%", "news_prompt22": "其中，零跑汽车SUV家族当月交付占比超72%，零跑C16交付超8000台", "news_prompt23": "蔚来8月交付新车20,176辆，这是蔚来连续第4个月交付超2万辆", "news_prompt24": "极氪8月交付18,015辆，同比增长46%，环比增长15%", "news_prompt25": "小鹏汽车共交付新车14,036辆，同比增长3%，环比增长26%", "news_prompt26": "哪吒汽车8月全系整车交付11,005辆", "news_prompt27": "小米汽车宣布8月交付量超1万辆，目前已连续3个月达成破万辆交付目标，预计11月提前完成全年10万辆交付目标", "news_prompt28": "卖车走量仍是关键任务 　　8月淡季不淡，多家新势力录得交付量同比增长", "news_prompt29": "展望9月及第四季度，新势力们推新品、卷技术的节奏继续加快", "news_prompt30": "8月底、9月初，今年的第二个A级车展成都车展正在进行", "news_prompt31": "小鹏汽车在成都车展上开启了MONA M03的交付", "news_prompt32": "根据小鹏汽车披露的数据，MONA M03起售48小时，大定超过3万辆", "news_prompt33": "作为小鹏汽车成立十周年节点上推出的全新产品序列，MONA M03瞄准更低价的市场，其起售价仅11.98万元", "news_prompt34": "从当前的订单数据来看，MONA“以价换量”的策略或初见成效", "news_prompt35": "今年来，小鹏汽车月交付量始终在1万辆左右徘徊，艾媒咨询首席分析师张毅向时代财经表示：“尽管MONA M03具备价格优势，但今年完成年销目标的挑战仍然比较大", "news_prompt36": "” 　　对于MONA M03，小鹏汽车的目标是月销至少1万辆", "news_prompt37": "小鹏汽车董事长何小鹏在二季度财报电话会上表示：“小鹏汽车有信心在今年三季度和四季度交付量环比大幅增长，并在四季度创交付量新高", "news_prompt38": "” 　　成立十周年，蔚来同样选择推出第二品牌乐道面向下沉市场", "news_prompt39": "今年5月，乐道汽车首款中型SUV乐道L60启动预售，预售价为21.99万元", "news_prompt40": "当前，乐道汽车正在加速布局销售渠道，9月1日，其宣布百家门店同天开业，已经覆盖全国55座城市", "news_prompt41": "和MONA一样，作为蔚来的第二品牌，乐道汽车肩负着走量任务", "news_prompt42": "蔚来董事长李斌此前在一季度财报电话会上强调，第二品牌新产品线将主要承担销量增长任务，在早期阶段，产品销量的优先级高于毛利率", "news_prompt43": "华为智能汽车解决方案BU董事长余承东则在成都车展上为鸿蒙智行站台", "news_prompt44": "享界S9、智界R7与问界新M7 Pro三款新车型均亮相车展", "news_prompt45": "车展前夕，问界新M7 Pro正式上市，售价24.98万元起", "news_prompt46": "今年7月、8月，鸿蒙智行与理想汽车交付量差距拉大", "news_prompt47": "从二者的主销产品来看，理想L6目前连续3个月实现月销2万辆以上，问界新M7的1-8月的交付量则分别约为3.1万、1.8万、2.5万、1.1万、0.7万、1.8万辆、1.7万辆、1.0万辆", "news_prompt48": "业内有观点认为，问界新M7需要一款新配置车型来提振销量", "news_prompt49": "此次问界M7 Pro的上市以及后续家用SUV车型对理想汽车下半年整体以及后续销量的影响受到行业关注", "news_prompt50": "李想在二季度财报电话会回应称：“鸿蒙智行是我们在市场上最强的竞争对手，我认为我们会长期健康地共存下去", "news_prompt51": "另外一个角度来说，我们自己的核心态度是要长期、持续向华为的技术研发体系和经营管理体系学习", "news_prompt52": "我们作为一个初创企业，有这样的学习榜样对我们而言太重要了", "news_prompt53": "” 　　销量突破新高的零跑汽车则希望再造爆款", "news_prompt54": "据悉，四季度，零跑将在巴黎车展亮相全新平台的首款产品B10，该款车面向全球年轻消费群体", "news_prompt55": "“有望成"}</t>
+          <t>{"news_prompt1": "9月第一天，国内多家新势力公布8月交付数据", "news_prompt2": "8月，理想汽车蝉联第一，交付新车48,122辆，同比增长37.8%", "news_prompt3": "鸿蒙智行8月全系交付新车33699辆", "news_prompt4": "此外，零跑汽车月度交付量首次突破3万辆，交付30305辆，连创历史新高，同比增长超113%", "news_prompt5": "蔚来交付新车20,176辆，连续4个月超2万辆", "news_prompt6": "小鹏汽车8月共交付新车14,036辆，同比微增3%", "news_prompt7": "继7月新能源汽车渗透率突破50%之后，乘联会预计8月新能源零售可达98.0万辆，渗透率预计将进一步提升至53.2%", "news_prompt8": "其中，理想L6成为销量担当，连续3个月交付量突破2万辆", "news_prompt9": "“在20万元以上新能源汽车市场，理想汽车7月的市占率达到18%，超越特斯拉成为新能源汽车品牌销量冠军", "news_prompt10": "” 理想汽车董事长兼CEO李想表示", "news_prompt11": "广汽埃安透露，埃安霸王龙上市交付首月突破6000辆", "news_prompt12": "8月，鸿蒙智行全系交付新车33699辆，同比下滑23.6%", "news_prompt13": "问界仍是其销量主力，8月交付新车31216辆", "news_prompt14": "另一家交付量超过3万辆的是零跑汽车", "news_prompt15": "8月交付量达到30305辆，同比增长超113%，环比增长超37%", "news_prompt16": "其中，零跑汽车SUV家族当月交付占比超72%，零跑C16交付超8000台", "news_prompt17": "蔚来8月交付新车20,176辆，这是蔚来连续第4个月交付超2万辆", "news_prompt18": "小鹏汽车共交付新车14,036辆，同比增长3%，环比增长26%", "news_prompt19": "小米汽车宣布8月交付量超1万辆，目前已连续3个月达成破万辆交付目标，预计11月提前完成全年10万辆交付目标", "news_prompt20": "卖车走量仍是关键任务 　　8月淡季不淡，多家新势力录得交付量同比增长", "news_prompt21": "展望9月及第四季度，新势力们推新品、卷技术的节奏继续加快", "news_prompt22": "根据小鹏汽车披露的数据，MONA M03起售48小时，大定超过3万辆", "news_prompt23": "小鹏汽车董事长何小鹏在二季度财报电话会上表示：“小鹏汽车有信心在今年三季度和四季度交付量环比大幅增长，并在四季度创交付量新高", "news_prompt24": "” 　　成立十周年，蔚来同样选择推出第二品牌乐道面向下沉市场", "news_prompt25": "今年5月，乐道汽车首款中型SUV乐道L60启动预售，预售价为21.99万元", "news_prompt26": "当前，乐道汽车正在加速布局销售渠道，9月1日，其宣布百家门店同天开业，已经覆盖全国55座城市", "news_prompt27": "蔚来董事长李斌此前在一季度财报电话会上强调，第二品牌新产品线将主要承担销量增长任务，在早期阶段，产品销量的优先级高于毛利率", "news_prompt28": "华为智能汽车解决方案BU董事长余承东则在成都车展上为鸿蒙智行站台", "news_prompt29": "车展前夕，问界新M7 Pro正式上市，售价24.98万元起", "news_prompt30": "今年7月、8月，鸿蒙智行与理想汽车交付量差距拉大", "news_prompt31": "业内有观点认为，问界新M7需要一款新配置车型来提振销量", "news_prompt32": "此次问界M7 Pro的上市以及后续家用SUV车型对理想汽车下半年整体以及后续销量的影响受到行业关注", "news_prompt33": "另外一个角度来说，我们自己的核心态度是要长期、持续向华为的技术研发体系和经营管理体系学习", "news_prompt34": "” 　　销量突破新高的零跑汽车则希望再造爆款", "news_prompt35": "据悉，四季度，零跑将在巴黎车展亮相全新平台的首款产品B10，该款车面向全球年轻消费群体"}</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>{"9月第一天，国内多家新势力公布8月交付数据": {"topic": "“生产投资”", "similarity": 0.446771502494812, "prompt": "新闻文本是“9月第一天，国内多家新势力公布8月交付数据”，包含的情绪词典是：产量/输出(output):0.0,劳动力/职工总数(workforce):0.01"}, "8月，理想汽车蝉联第一，交付新车48,122辆，同比增长37.8%": {"topic": "“消费”", "similarity": 0.42139631509780884, "prompt": "新闻文本是“8月，理想汽车蝉联第一，交付新车48,122辆，同比增长37.8%”，包含的情绪词典是：理想的/完美的(ideal):0.5,汽车/轿车(car):0.0"}, "鸿蒙智行8月全系交付新车33699辆": {"topic": "“生产投资”", "similarity": 0.4440087378025055, "prompt": "新闻文本是“鸿蒙智行8月全系交付新车33699辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车/轿车(car):0.0"}, "此外，零跑汽车月度交付量首次突破3万辆，交付30305辆，连创历史新高，同比增长超113%": {"topic": "“消费”", "similarity": 0.45589491724967957, "prompt": "新闻文本是“此外，零跑汽车月度交付量首次突破3万辆，交付30305辆，连创历史新高，同比增长超113%”，包含的情绪词典是：汽车的/机动车的(automotive):0.0,汽车/机动车(automobile):0.0"}, "蔚来交付新车20,176辆，连续4个月超2万辆": {"topic": "“生产投资”", "similarity": 0.42156580090522766, "prompt": "新闻文本是“蔚来交付新车20,176辆，连续4个月超2万辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车/轿车(car):0.0"}, "小鹏汽车8月共交付新车14,036辆，同比微增3%": {"topic": "“生产投资”", "similarity": 0.4550912082195282, "prompt": "新闻文本是“小鹏汽车8月共交付新车14,036辆，同比微增3%”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "继7月新能源汽车渗透率突破50%之后，乘联会预计8月新能源零售可达98.0万辆，渗透率预计将进一步提升至53.2%": {"topic": "“消费”", "similarity": 0.5690963864326477, "prompt": "新闻文本是“继7月新能源汽车渗透率突破50%之后，乘联会预计8月新能源零售可达98.0万辆，渗透率预计将进一步提升至53.2%”，包含的情绪词典是：汽车/机动车(automobile):0.0,车辆/交通工具(vehicle):0.0"}, "零跑汽车首次突破3万辆 　　根据乘联会的调研，8月，插电混动市场稳定发力的同时，低价纯电产品销量也有较为明显的提升，8月新能源市场持续走高，表现十分强劲": {"topic": "“消费”", "similarity": 0.5818485617637634}, "其中，理想L6成为销量担当，连续3个月交付量突破2万辆": {"topic": "“消费”", "similarity": 0.4743955135345459, "prompt": "新闻文本是“其中，理想L6成为销量担当，连续3个月交付量突破2万辆”，包含的情绪词典是：理想的/完美的(ideal):0.5,汽车/轿车(car):0.0"}, "“在20万元以上新能源汽车市场，理想汽车7月的市占率达到18%，超越特斯拉成为新能源汽车品牌销量冠军": {"topic": "“消费”", "similarity": 0.522523045539856, "prompt": "新闻文本是““在20万元以上新能源汽车市场，理想汽车7月的市占率达到18%，超越特斯拉成为新能源汽车品牌销量冠军”，包含的情绪词典是：理想的/完美的(ideal):0.5"}, "” 理想汽车董事长兼CEO李想表示": {"topic": "“生产投资”", "similarity": 0.4732262194156647, "prompt": "新闻文本是“” 理想汽车董事长兼CEO李想表示”，包含的情绪词典是：理想的/完美的(ideal):0.5,合意的/理想的(desirable):0.5"}, "广汽埃安透露，埃安霸王龙上市交付首月突破6000辆": {"topic": "“生产投资”", "similarity": 0.437889039516449, "prompt": "新闻文本是“广汽埃安透露，埃安霸王龙上市交付首月突破6000辆”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "8月，鸿蒙智行全系交付新车33699辆，同比下滑23.6%": {"topic": "“生产投资”", "similarity": 0.4748629927635193, "prompt": "新闻文本是“8月，鸿蒙智行全系交付新车33699辆，同比下滑23.6%”，包含的情绪词典是：下跌/下降(fall):-0.6,生产不足/产量低于预期(underproduction):-0.5"}, "问界仍是其销量主力，8月交付新车31216辆": {"topic": "“消费”", "similarity": 0.43154019117355347, "prompt": "新闻文本是“问界仍是其销量主力，8月交付新车31216辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车的/机动车的(automotive):0.0"}, "另一家交付量超过3万辆的是零跑汽车": {"topic": "“消费”", "similarity": 0.4360872209072113, "prompt": "新闻文本是“另一家交付量超过3万辆的是零跑汽车”，包含的情绪词典是：超过量/超越量(exceedances):0.2,超过量/超越量(exceedance):0.2"}, "8月交付量达到30305辆，同比增长超113%，环比增长超37%": {"topic": "“生产投资”", "similarity": 0.45969653129577637, "prompt": "新闻文本是“8月交付量达到30305辆，同比增长超113%，环比增长超37%”，包含的情绪词典是：交付/递送(deliver):0.3,产量/输出(output):0.0"}, "其中，零跑汽车SUV家族当月交付占比超72%，零跑C16交付超8000台": {"topic": "“消费”", "similarity": 0.4673023223876953, "prompt": "新闻文本是“其中，零跑汽车SUV家族当月交付占比超72%，零跑C16交付超8000台”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "蔚来8月交付新车20,176辆，这是蔚来连续第4个月交付超2万辆": {"topic": "“生产投资”", "similarity": 0.43203771114349365, "prompt": "新闻文本是“蔚来8月交付新车20,176辆，这是蔚来连续第4个月交付超2万辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,产量/输出(output):0.0"}, "小鹏汽车共交付新车14,036辆，同比增长3%，环比增长26%": {"topic": "“生产投资”", "similarity": 0.4367242455482483, "prompt": "新闻文本是“小鹏汽车共交付新车14,036辆，同比增长3%，环比增长26%”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "小米汽车宣布8月交付量超1万辆，目前已连续3个月达成破万辆交付目标，预计11月提前完成全年10万辆交付目标": {"topic": "“生产投资”", "similarity": 0.5377331972122192, "prompt": "新闻文本是“小米汽车宣布8月交付量超1万辆，目前已连续3个月达成破万辆交付目标，预计11月提前完成全年10万辆交付目标”，包含的情绪词典是：达到/实现(achieve):0.6,达到/实现(achieving):0.6"}, "卖车走量仍是关键任务 　　8月淡季不淡，多家新势力录得交付量同比增长": {"topic": "“消费”", "similarity": 0.44630753993988037, "prompt": "新闻文本是“卖车走量仍是关键任务 　　8月淡季不淡，多家新势力录得交付量同比增长”，包含的情绪词典是：汽车/机动车(automobile):0.0,车辆/交通工具(vehicle):0.0"}, "展望9月及第四季度，新势力们推新品、卷技术的节奏继续加快": {"topic": "“生产投资”", "similarity": 0.4846259653568268, "prompt": "新闻文本是“展望9月及第四季度，新势力们推新品、卷技术的节奏继续加快”，包含的情绪词典是：季度/四分之一(quarter):0.0,加速(accelerate):0.6"}, "根据小鹏汽车披露的数据，MONA M03起售48小时，大定超过3万辆": {"topic": "“生产投资”", "similarity": 0.47475045919418335, "prompt": "新闻文本是“根据小鹏汽车披露的数据，MONA M03起售48小时，大定超过3万辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,垄断/专卖(monopoly):-0.4"}, "作为小鹏汽车成立十周年节点上推出的全新产品序列，MONA M03瞄准更低价的市场，其起售价仅11.98万元": {"topic": "“消费”", "similarity": 0.4302174746990204}, "今年来，小鹏汽车月交付量始终在1万辆左右徘徊，艾媒咨询首席分析师张毅向时代财经表示：“尽管MONA M03具备价格优势，但今年完成年销目标的挑战仍然比较大": {"topic": "“消费”", "similarity": 0.47258931398391724}, "小鹏汽车董事长何小鹏在二季度财报电话会上表示：“小鹏汽车有信心在今年三季度和四季度交付量环比大幅增长，并在四季度创交付量新高": {"topic": "“生产投资”", "similarity": 0.5218040943145752, "prompt": "新闻文本是“小鹏汽车董事长何小鹏在二季度财报电话会上表示：“小鹏汽车有信心在今年三季度和四季度交付量环比大幅增长，并在四季度创交付量新高”，包含的情绪词典是：季度/四分之一(quarter):0.0"}, "” 　　成立十周年，蔚来同样选择推出第二品牌乐道面向下沉市场": {"topic": "“消费”", "similarity": 0.4559575319290161, "prompt": "新闻文本是“” 　　成立十周年，蔚来同样选择推出第二品牌乐道面向下沉市场”，包含的情绪词典是：下沉/沉没(sink):-0.5,向下的/下行的(downward):-0.5"}, "今年5月，乐道汽车首款中型SUV乐道L60启动预售，预售价为21.99万元": {"topic": "“消费”", "similarity": 0.4768628776073456, "prompt": "新闻文本是“今年5月，乐道汽车首款中型SUV乐道L60启动预售，预售价为21.99万元”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,削价/低价出售(undercut):-0.3"}, "当前，乐道汽车正在加速布局销售渠道，9月1日，其宣布百家门店同天开业，已经覆盖全国55座城市": {"topic": "“消费”", "similarity": 0.48980391025543213, "prompt": "新闻文本是“当前，乐道汽车正在加速布局销售渠道，9月1日，其宣布百家门店同天开业，已经覆盖全国55座城市”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车的/机动车的(automotive):0.0"}, "蔚来董事长李斌此前在一季度财报电话会上强调，第二品牌新产品线将主要承担销量增长任务，在早期阶段，产品销量的优先级高于毛利率": {"topic": "“生产投资”", "similarity": 0.5122241973876953, "prompt": "新闻文本是“蔚来董事长李斌此前在一季度财报电话会上强调，第二品牌新产品线将主要承担销量增长任务，在早期阶段，产品销量的优先级高于毛利率”，包含的情绪词典是：领导的/主要的(leading):0.4,盈利能力/获利能力(profitability):0.6"}, "华为智能汽车解决方案BU董事长余承东则在成都车展上为鸿蒙智行站台": {"topic": "“生产投资”", "similarity": 0.4451301097869873, "prompt": "新闻文本是“华为智能汽车解决方案BU董事长余承东则在成都车展上为鸿蒙智行站台”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "车展前夕，问界新M7 Pro正式上市，售价24.98万元起": {"topic": "“消费”", "similarity": 0.5085185766220093, "prompt": "新闻文本是“车展前夕，问界新M7 Pro正式上市，售价24.98万元起”，包含的情绪词典是：汽车/机动车(automobile):0.0,减价/降价(markdown):0.0"}, "今年7月、8月，鸿蒙智行与理想汽车交付量差距拉大": {"topic": "“生产投资”", "similarity": 0.45918697118759155, "prompt": "新闻文本是“今年7月、8月，鸿蒙智行与理想汽车交付量差距拉大”，包含的情绪词典是：差距/差异(disparity):-0.5,产量/输出(output):0.0"}, "从二者的主销产品来看，理想L6目前连续3个月实现月销2万辆以上，问界新M7的1-8月的交付量则分别约为3.1万、1.8万、2.5万、1.1万、0.7万、1.8万辆、1.7万辆、1.0万辆": {"topic": "“消费”", "similarity": 0.5093158483505249}, "业内有观点认为，问界新M7需要一款新配置车型来提振销量": {"topic": "“消费”", "similarity": 0.4570859670639038, "prompt": "新闻文本是“业内有观点认为，问界新M7需要一款新配置车型来提振销量”，包含的情绪词典是：需要/需求(need):0.0,改善/改进(improve):0.5"}, "此次问界M7 Pro的上市以及后续家用SUV车型对理想汽车下半年整体以及后续销量的影响受到行业关注": {"topic": "“消费”", "similarity": 0.5055691599845886, "prompt": "新闻文本是“此次问界M7 Pro的上市以及后续家用SUV车型对理想汽车下半年整体以及后续销量的影响受到行业关注”，包含的情绪词典是：理想的/完美的(ideal):0.5,车辆/交通工具(vehicle):0.0"}, "另外一个角度来说，我们自己的核心态度是要长期、持续向华为的技术研发体系和经营管理体系学习": {"topic": "“生产投资”", "similarity": 0.4459173083305359, "prompt": "新闻文本是“另外一个角度来说，我们自己的核心态度是要长期、持续向华为的技术研发体系和经营管理体系学习”，包含的情绪词典是：持续的/坚持不懈的(persistent):0.2,技术(tech):0.0"}, "” 　　销量突破新高的零跑汽车则希望再造爆款": {"topic": "“消费”", "similarity": 0.4430774450302124, "prompt": "新闻文本是“” 　　销量突破新高的零跑汽车则希望再造爆款”，包含的情绪词典是：跑赢/表现优于(outperform):0.65,运行/奔跑(run):0.0"}, "据悉，四季度，零跑将在巴黎车展亮相全新平台的首款产品B10，该款车面向全球年轻消费群体": {"topic": "“消费”", "similarity": 0.4393783211708069, "prompt": "新闻文本是“据悉，四季度，零跑将在巴黎车展亮相全新平台的首款产品B10，该款车面向全球年轻消费群体”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车的/机动车的(automotive):0.0"}, "“有望成": {"topic": "“生产投资”", "similarity": 0.4708526134490967, "prompt": "新闻文本是““有望成”，包含的情绪词典是：达到/实现(achieving):0.6,达到/实现(achieve):0.6"}}</t>
+          <t>{"9月第一天，国内多家新势力公布8月交付数据": {"topic": "“生产投资”", "similarity": 0.446771502494812, "prompt": "新闻文本是“9月第一天，国内多家新势力公布8月交付数据”，包含的情绪词典是：产量/输出(output):0.0,劳动力/职工总数(workforce):0.01"}, "8月，理想汽车蝉联第一，交付新车48,122辆，同比增长37.8%": {"topic": "“消费”", "similarity": 0.4213963747024536, "prompt": "新闻文本是“8月，理想汽车蝉联第一，交付新车48,122辆，同比增长37.8%”，包含的情绪词典是：理想的/完美的(ideal):0.5,汽车/轿车(car):0.0"}, "鸿蒙智行8月全系交付新车33699辆": {"topic": "“生产投资”", "similarity": 0.4440087676048279, "prompt": "新闻文本是“鸿蒙智行8月全系交付新车33699辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车/轿车(car):0.0"}, "此外，零跑汽车月度交付量首次突破3万辆，交付30305辆，连创历史新高，同比增长超113%": {"topic": "“消费”", "similarity": 0.4558951258659363, "prompt": "新闻文本是“此外，零跑汽车月度交付量首次突破3万辆，交付30305辆，连创历史新高，同比增长超113%”，包含的情绪词典是：汽车的/机动车的(automotive):0.0,汽车/机动车(automobile):0.0"}, "蔚来交付新车20,176辆，连续4个月超2万辆": {"topic": "“生产投资”", "similarity": 0.4215658903121948, "prompt": "新闻文本是“蔚来交付新车20,176辆，连续4个月超2万辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车/轿车(car):0.0"}, "小鹏汽车8月共交付新车14,036辆，同比微增3%": {"topic": "“生产投资”", "similarity": 0.45509135723114014, "prompt": "新闻文本是“小鹏汽车8月共交付新车14,036辆，同比微增3%”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "继7月新能源汽车渗透率突破50%之后，乘联会预计8月新能源零售可达98.0万辆，渗透率预计将进一步提升至53.2%": {"topic": "“消费”", "similarity": 0.5690964460372925, "prompt": "新闻文本是“继7月新能源汽车渗透率突破50%之后，乘联会预计8月新能源零售可达98.0万辆，渗透率预计将进一步提升至53.2%”，包含的情绪词典是：汽车/机动车(automobile):0.0,车辆/交通工具(vehicle):0.0"}, "其中，理想L6成为销量担当，连续3个月交付量突破2万辆": {"topic": "“消费”", "similarity": 0.474395751953125, "prompt": "新闻文本是“其中，理想L6成为销量担当，连续3个月交付量突破2万辆”，包含的情绪词典是：理想的/完美的(ideal):0.5,汽车/轿车(car):0.0"}, "“在20万元以上新能源汽车市场，理想汽车7月的市占率达到18%，超越特斯拉成为新能源汽车品牌销量冠军": {"topic": "“消费”", "similarity": 0.5225231051445007, "prompt": "新闻文本是““在20万元以上新能源汽车市场，理想汽车7月的市占率达到18%，超越特斯拉成为新能源汽车品牌销量冠军”，包含的情绪词典是：理想的/完美的(ideal):0.5"}, "” 理想汽车董事长兼CEO李想表示": {"topic": "“生产投资”", "similarity": 0.4732263684272766, "prompt": "新闻文本是“” 理想汽车董事长兼CEO李想表示”，包含的情绪词典是：理想的/完美的(ideal):0.5,合意的/理想的(desirable):0.5"}, "广汽埃安透露，埃安霸王龙上市交付首月突破6000辆": {"topic": "“生产投资”", "similarity": 0.43788909912109375, "prompt": "新闻文本是“广汽埃安透露，埃安霸王龙上市交付首月突破6000辆”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "8月，鸿蒙智行全系交付新车33699辆，同比下滑23.6%": {"topic": "“生产投资”", "similarity": 0.4748631715774536, "prompt": "新闻文本是“8月，鸿蒙智行全系交付新车33699辆，同比下滑23.6%”，包含的情绪词典是：下跌/下降(fall):-0.6,生产不足/产量低于预期(underproduction):-0.5"}, "问界仍是其销量主力，8月交付新车31216辆": {"topic": "“消费”", "similarity": 0.43154042959213257, "prompt": "新闻文本是“问界仍是其销量主力，8月交付新车31216辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车的/机动车的(automotive):0.0"}, "另一家交付量超过3万辆的是零跑汽车": {"topic": "“消费”", "similarity": 0.43608734011650085, "prompt": "新闻文本是“另一家交付量超过3万辆的是零跑汽车”，包含的情绪词典是：超过量/超越量(exceedances):0.2,超过量/超越量(exceedance):0.2"}, "8月交付量达到30305辆，同比增长超113%，环比增长超37%": {"topic": "“生产投资”", "similarity": 0.45969659090042114, "prompt": "新闻文本是“8月交付量达到30305辆，同比增长超113%，环比增长超37%”，包含的情绪词典是：交付/递送(deliver):0.3,产量/输出(output):0.0"}, "其中，零跑汽车SUV家族当月交付占比超72%，零跑C16交付超8000台": {"topic": "“消费”", "similarity": 0.46730250120162964, "prompt": "新闻文本是“其中，零跑汽车SUV家族当月交付占比超72%，零跑C16交付超8000台”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "蔚来8月交付新车20,176辆，这是蔚来连续第4个月交付超2万辆": {"topic": "“生产投资”", "similarity": 0.432037889957428, "prompt": "新闻文本是“蔚来8月交付新车20,176辆，这是蔚来连续第4个月交付超2万辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,产量/输出(output):0.0"}, "小鹏汽车共交付新车14,036辆，同比增长3%，环比增长26%": {"topic": "“生产投资”", "similarity": 0.4367244243621826, "prompt": "新闻文本是“小鹏汽车共交付新车14,036辆，同比增长3%，环比增长26%”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "小米汽车宣布8月交付量超1万辆，目前已连续3个月达成破万辆交付目标，预计11月提前完成全年10万辆交付目标": {"topic": "“生产投资”", "similarity": 0.5377333164215088, "prompt": "新闻文本是“小米汽车宣布8月交付量超1万辆，目前已连续3个月达成破万辆交付目标，预计11月提前完成全年10万辆交付目标”，包含的情绪词典是：达到/实现(achieve):0.6,达到/实现(achieving):0.6"}, "卖车走量仍是关键任务 　　8月淡季不淡，多家新势力录得交付量同比增长": {"topic": "“消费”", "similarity": 0.44630780816078186, "prompt": "新闻文本是“卖车走量仍是关键任务 　　8月淡季不淡，多家新势力录得交付量同比增长”，包含的情绪词典是：汽车/机动车(automobile):0.0,车辆/交通工具(vehicle):0.0"}, "展望9月及第四季度，新势力们推新品、卷技术的节奏继续加快": {"topic": "“生产投资”", "similarity": 0.4846261143684387, "prompt": "新闻文本是“展望9月及第四季度，新势力们推新品、卷技术的节奏继续加快”，包含的情绪词典是：季度/四分之一(quarter):0.0,加速(accelerate):0.6"}, "根据小鹏汽车披露的数据，MONA M03起售48小时，大定超过3万辆": {"topic": "“生产投资”", "similarity": 0.47475048899650574, "prompt": "新闻文本是“根据小鹏汽车披露的数据，MONA M03起售48小时，大定超过3万辆”，包含的情绪词典是：汽车/机动车(automobile):0.0,垄断/专卖(monopoly):-0.4"}, "小鹏汽车董事长何小鹏在二季度财报电话会上表示：“小鹏汽车有信心在今年三季度和四季度交付量环比大幅增长，并在四季度创交付量新高": {"topic": "“生产投资”", "similarity": 0.5218043327331543, "prompt": "新闻文本是“小鹏汽车董事长何小鹏在二季度财报电话会上表示：“小鹏汽车有信心在今年三季度和四季度交付量环比大幅增长，并在四季度创交付量新高”，包含的情绪词典是：季度/四分之一(quarter):0.0"}, "” 　　成立十周年，蔚来同样选择推出第二品牌乐道面向下沉市场": {"topic": "“消费”", "similarity": 0.4559577703475952, "prompt": "新闻文本是“” 　　成立十周年，蔚来同样选择推出第二品牌乐道面向下沉市场”，包含的情绪词典是：下沉/沉没(sink):-0.5,向下的/下行的(downward):-0.5"}, "今年5月，乐道汽车首款中型SUV乐道L60启动预售，预售价为21.99万元": {"topic": "“消费”", "similarity": 0.47686299681663513, "prompt": "新闻文本是“今年5月，乐道汽车首款中型SUV乐道L60启动预售，预售价为21.99万元”，包含的情绪词典是：错价/定价错误(mispricing):-0.4,削价/低价出售(undercut):-0.3"}, "当前，乐道汽车正在加速布局销售渠道，9月1日，其宣布百家门店同天开业，已经覆盖全国55座城市": {"topic": "“消费”", "similarity": 0.4898042678833008, "prompt": "新闻文本是“当前，乐道汽车正在加速布局销售渠道，9月1日，其宣布百家门店同天开业，已经覆盖全国55座城市”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车的/机动车的(automotive):0.0"}, "蔚来董事长李斌此前在一季度财报电话会上强调，第二品牌新产品线将主要承担销量增长任务，在早期阶段，产品销量的优先级高于毛利率": {"topic": "“生产投资”", "similarity": 0.5122244358062744, "prompt": "新闻文本是“蔚来董事长李斌此前在一季度财报电话会上强调，第二品牌新产品线将主要承担销量增长任务，在早期阶段，产品销量的优先级高于毛利率”，包含的情绪词典是：领导的/主要的(leading):0.4,盈利能力/获利能力(profitability):0.6"}, "华为智能汽车解决方案BU董事长余承东则在成都车展上为鸿蒙智行站台": {"topic": "“生产投资”", "similarity": 0.44513022899627686, "prompt": "新闻文本是“华为智能汽车解决方案BU董事长余承东则在成都车展上为鸿蒙智行站台”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "车展前夕，问界新M7 Pro正式上市，售价24.98万元起": {"topic": "“消费”", "similarity": 0.508518636226654, "prompt": "新闻文本是“车展前夕，问界新M7 Pro正式上市，售价24.98万元起”，包含的情绪词典是：汽车/机动车(automobile):0.0,减价/降价(markdown):0.0"}, "今年7月、8月，鸿蒙智行与理想汽车交付量差距拉大": {"topic": "“生产投资”", "similarity": 0.4591870605945587, "prompt": "新闻文本是“今年7月、8月，鸿蒙智行与理想汽车交付量差距拉大”，包含的情绪词典是：差距/差异(disparity):-0.5,产量/输出(output):0.0"}, "业内有观点认为，问界新M7需要一款新配置车型来提振销量": {"topic": "“消费”", "similarity": 0.45708614587783813, "prompt": "新闻文本是“业内有观点认为，问界新M7需要一款新配置车型来提振销量”，包含的情绪词典是：需要/需求(need):0.0,改善/改进(improve):0.5"}, "此次问界M7 Pro的上市以及后续家用SUV车型对理想汽车下半年整体以及后续销量的影响受到行业关注": {"topic": "“消费”", "similarity": 0.505569338798523, "prompt": "新闻文本是“此次问界M7 Pro的上市以及后续家用SUV车型对理想汽车下半年整体以及后续销量的影响受到行业关注”，包含的情绪词典是：理想的/完美的(ideal):0.5,车辆/交通工具(vehicle):0.0"}, "另外一个角度来说，我们自己的核心态度是要长期、持续向华为的技术研发体系和经营管理体系学习": {"topic": "“生产投资”", "similarity": 0.4459174871444702, "prompt": "新闻文本是“另外一个角度来说，我们自己的核心态度是要长期、持续向华为的技术研发体系和经营管理体系学习”，包含的情绪词典是：持续的/坚持不懈的(persistent):0.2,技术(tech):0.0"}, "” 　　销量突破新高的零跑汽车则希望再造爆款": {"topic": "“消费”", "similarity": 0.44307762384414673, "prompt": "新闻文本是“” 　　销量突破新高的零跑汽车则希望再造爆款”，包含的情绪词典是：跑赢/表现优于(outperform):0.65,运行/奔跑(run):0.0"}, "据悉，四季度，零跑将在巴黎车展亮相全新平台的首款产品B10，该款车面向全球年轻消费群体": {"topic": "“消费”", "similarity": 0.4393784999847412, "prompt": "新闻文本是“据悉，四季度，零跑将在巴黎车展亮相全新平台的首款产品B10，该款车面向全球年轻消费群体”，包含的情绪词典是：汽车/机动车(automobile):0.0,汽车的/机动车的(automotive):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -2188,12 +2172,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "东莞证券09月02日发布研报称，给予伯特利（603596.SH，最新价：36.74元）增持评级", "news_prompt2": "评级理由主要包括：1）产品销量稳定增长，持续开拓定点项目", "news_prompt3": "2）持续加强研发，推动新产品研发及量产交付", "news_prompt4": "3）推进产能建设及全球化布局", "news_prompt5": "风险提示：下游汽车销量不及预期", "news_prompt6": "行业竞争加剧风险", "news_prompt7": "产能建设不及预期风险", "news_prompt8": "毛利率下滑风险", "news_prompt9": "汇率波动风险等", "news_prompt10": "AI点评：伯特利近一个月获得8份券商研报关注，买入7家，平均目标价为58.95元，与最新价36.74元相比，高22.21元，目标均价涨幅60.45%", "news_prompt11": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "评级理由主要包括：1）产品销量稳定增长，持续开拓定点项目", "news_prompt2": "2）持续加强研发，推动新产品研发及量产交付", "news_prompt3": "3）推进产能建设及全球化布局", "news_prompt4": "行业竞争加剧风险", "news_prompt5": "产能建设不及预期风险", "news_prompt6": "毛利率下滑风险", "news_prompt7": "汇率波动风险等", "news_prompt8": "AI点评：伯特利近一个月获得8份券商研报关注，买入7家，平均目标价为58.95元，与最新价36.74元相比，高22.21元，目标均价涨幅60.45%"}</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>{"东莞证券09月02日发布研报称，给予伯特利（603596.SH，最新价：36.74元）增持评级": {"topic": "“金融”", "similarity": 0.46974876523017883}, "评级理由主要包括：1）产品销量稳定增长，持续开拓定点项目": {"topic": "“生产投资”", "similarity": 0.4534393548965454, "prompt": "新闻文本是“评级理由主要包括：1）产品销量稳定增长，持续开拓定点项目”，包含的情绪词典是：增长/发展(growth):0.7,稳定的/稳固的(stable):0.5"}, "2）持续加强研发，推动新产品研发及量产交付": {"topic": "“生产投资”", "similarity": 0.48716169595718384, "prompt": "新闻文本是“2）持续加强研发，推动新产品研发及量产交付”，包含的情绪词典是：发展/开发(development):0.4,开发/利用(exploiting):-0.5"}, "3）推进产能建设及全球化布局": {"topic": "“生产投资”", "similarity": 0.5709830522537231, "prompt": "新闻文本是“3）推进产能建设及全球化布局”，包含的情绪词典是：产能过剩(overcapacity):-0.5,工业/产业(industry):0.0"}, "风险提示：下游汽车销量不及预期": {"topic": "“宏观经济”", "similarity": 0.519684374332428, "prompt": "新闻文本是“风险提示：下游汽车销量不及预期”，包含的情绪词典是：风险(risk):-0.4,生产不足/产量低于预期(underproduction):-0.5"}, "行业竞争加剧风险": {"topic": "“金融”", "similarity": 0.5141422748565674, "prompt": "新闻文本是“行业竞争加剧风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "产能建设不及预期风险": {"topic": "“生产投资”", "similarity": 0.5630052089691162, "prompt": "新闻文本是“产能建设不及预期风险”，包含的情绪词典是：生产不足/产量低于预期(underproduction):-0.5,生产不足的/产量低于预期的(underproduced):-0.5"}, "毛利率下滑风险": {"topic": "“宏观经济”", "similarity": 0.47622352838516235, "prompt": "新闻文本是“毛利率下滑风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "汇率波动风险等": {"topic": "“金融”", "similarity": 0.574752688407898, "prompt": "新闻文本是“汇率波动风险等”，包含的情绪词典是：风险(risk):-0.4,波动/起伏(fluctuates):-0.2"}, "AI点评：伯特利近一个月获得8份券商研报关注，买入7家，平均目标价为58.95元，与最新价36.74元相比，高22.21元，目标均价涨幅60.45%": {"topic": "“金融”", "similarity": 0.5228064060211182, "prompt": "新闻文本是“AI点评：伯特利近一个月获得8份券商研报关注，买入7家，平均目标价为58.95元，与最新价36.74元相比，高22.21元，目标均价涨幅60.45%”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,盈利能力/获利能力(profitability):0.6"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"评级理由主要包括：1）产品销量稳定增长，持续开拓定点项目": {"topic": "“生产投资”", "similarity": 0.45343947410583496, "prompt": "新闻文本是“评级理由主要包括：1）产品销量稳定增长，持续开拓定点项目”，包含的情绪词典是：增长/发展(growth):0.7,稳定的/稳固的(stable):0.5"}, "2）持续加强研发，推动新产品研发及量产交付": {"topic": "“生产投资”", "similarity": 0.4871618151664734, "prompt": "新闻文本是“2）持续加强研发，推动新产品研发及量产交付”，包含的情绪词典是：发展/开发(development):0.4,开发/利用(exploiting):-0.5"}, "3）推进产能建设及全球化布局": {"topic": "“生产投资”", "similarity": 0.5709829926490784, "prompt": "新闻文本是“3）推进产能建设及全球化布局”，包含的情绪词典是：产能过剩(overcapacity):-0.5,工业/产业(industry):0.0"}, "行业竞争加剧风险": {"topic": "“金融”", "similarity": 0.5141422748565674, "prompt": "新闻文本是“行业竞争加剧风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "产能建设不及预期风险": {"topic": "“生产投资”", "similarity": 0.5630052089691162, "prompt": "新闻文本是“产能建设不及预期风险”，包含的情绪词典是：生产不足/产量低于预期(underproduction):-0.5,生产不足的/产量低于预期的(underproduced):-0.5"}, "毛利率下滑风险": {"topic": "“宏观经济”", "similarity": 0.47622376680374146, "prompt": "新闻文本是“毛利率下滑风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "汇率波动风险等": {"topic": "“金融”", "similarity": 0.574752688407898, "prompt": "新闻文本是“汇率波动风险等”，包含的情绪词典是：风险(risk):-0.4,波动/起伏(fluctuates):-0.2"}, "AI点评：伯特利近一个月获得8份券商研报关注，买入7家，平均目标价为58.95元，与最新价36.74元相比，高22.21元，目标均价涨幅60.45%": {"topic": "“金融”", "similarity": 0.5228064656257629, "prompt": "新闻文本是“AI点评：伯特利近一个月获得8份券商研报关注，买入7家，平均目标价为58.95元，与最新价36.74元相比，高22.21元，目标均价涨幅60.45%”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,盈利能力/获利能力(profitability):0.6"}}</t>
         </is>
       </c>
     </row>
@@ -2239,12 +2223,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，华孚时尚(002042.SZ)发布2024年中报", "news_prompt2": "公司营业总收入为65.23亿元，在已披露的同业公司中排名第2，较去年同报告期营业总收入减少12.30亿元，同比较去年同期下降15.87%", "news_prompt3": "归母净利润为4480.46万元，在已披露的同业公司中排名第17，较去年同报告期归母净利润减少3659.82万元，同比较去年同期下降44.96%", "news_prompt4": "经营活动现金净流入为10.93亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入减少4.32亿元，同比较去年同期下降28.30%", "news_prompt5": "公司最新资产负债率为63.98%，在已披露的同业公司中排名第30，较上季度资产负债率减少0.17个百分点，较去年同季度资产负债率增加1.14个百分点", "news_prompt6": "公司最新毛利率为6.21%，在已披露的同业公司中排名第30，较上季度毛利率增加0.93个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.83个百分点", "news_prompt7": "最新ROE为0.74%，在已披露的同业公司中排名第24，较去年同季度ROE减少0.57个百分点", "news_prompt8": "公司摊薄每股收益为0.03元，在已披露的同业公司中排名第23，较去年同报告期摊薄每股收益减少0.02元，同比较去年同期下降45.09%", "news_prompt9": "公司最新总资产周转率为0.38次，在已披露的同业公司中排名第9，较去年同季度总资产周转率减少0.05次，同比较去年同期下降12.25%", "news_prompt10": "最新存货周转率为1.40次，在已披露的同业公司中排名第20，较去年同季度存货周转率减少0.31次，同比较去年同期下降18.12%", "news_prompt11": "公司股东户数为2.99万户，前十大股东持股数量为8.72亿股，占总股本比例为51.27%", "news_prompt12": "前十大股东分别为华孚控股有限公司、安徽飞亚纺织有限公司、深圳市华人投资有限公司、广西沣盛供应链管理有限公司、金元顺安基金-兴业银行-上海爱建信托-爱建信托欣欣7号定向增发事务管理类单一资金信托、金鹰基金-工商银行-万向信托-万向信托-星辰39号事务管理类单一资金信托、陆超祖、杨三宝、陆敏、中航鑫港担保有限公司，持股比例分别为29.50%、7.59%、4.82%、2.66%、1.65%、1.42%、1.03%、0.99%、0.98%、0.62%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为65.23亿元，在已披露的同业公司中排名第2，较去年同报告期营业总收入减少12.30亿元，同比较去年同期下降15.87%", "news_prompt2": "归母净利润为4480.46万元，在已披露的同业公司中排名第17，较去年同报告期归母净利润减少3659.82万元，同比较去年同期下降44.96%", "news_prompt3": "经营活动现金净流入为10.93亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入减少4.32亿元，同比较去年同期下降28.30%", "news_prompt4": "公司最新资产负债率为63.98%，在已披露的同业公司中排名第30，较上季度资产负债率减少0.17个百分点，较去年同季度资产负债率增加1.14个百分点", "news_prompt5": "公司最新毛利率为6.21%，在已披露的同业公司中排名第30，较上季度毛利率增加0.93个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.83个百分点", "news_prompt6": "公司摊薄每股收益为0.03元，在已披露的同业公司中排名第23，较去年同报告期摊薄每股收益减少0.02元，同比较去年同期下降45.09%", "news_prompt7": "公司最新总资产周转率为0.38次，在已披露的同业公司中排名第9，较去年同季度总资产周转率减少0.05次，同比较去年同期下降12.25%", "news_prompt8": "最新存货周转率为1.40次，在已披露的同业公司中排名第20，较去年同季度存货周转率减少0.31次，同比较去年同期下降18.12%", "news_prompt9": "公司股东户数为2.99万户，前十大股东持股数量为8.72亿股，占总股本比例为51.27%"}</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，华孚时尚(002042.SZ)发布2024年中报": {"topic": "“消费”", "similarity": 0.47680842876434326, "prompt": "新闻文本是“2024年8月31日，华孚时尚(002042.SZ)发布2024年中报”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司营业总收入为65.23亿元，在已披露的同业公司中排名第2，较去年同报告期营业总收入减少12.30亿元，同比较去年同期下降15.87%": {"topic": "“消费”", "similarity": 0.544075608253479, "prompt": "新闻文本是“公司营业总收入为65.23亿元，在已披露的同业公司中排名第2，较去年同报告期营业总收入减少12.30亿元，同比较去年同期下降15.87%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "归母净利润为4480.46万元，在已披露的同业公司中排名第17，较去年同报告期归母净利润减少3659.82万元，同比较去年同期下降44.96%": {"topic": "“消费”", "similarity": 0.5097399950027466, "prompt": "新闻文本是“归母净利润为4480.46万元，在已披露的同业公司中排名第17，较去年同报告期归母净利润减少3659.82万元，同比较去年同期下降44.96%”，包含的情绪词典是：减损/贬低(derogation):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为10.93亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入减少4.32亿元，同比较去年同期下降28.30%": {"topic": "“金融”", "similarity": 0.5478696823120117, "prompt": "新闻文本是“经营活动现金净流入为10.93亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入减少4.32亿元，同比较去年同期下降28.30%”，包含的情绪词典是：营业额/周转(turnover):0.0,盈利能力/获利能力(profitability):0.6"}, "公司最新资产负债率为63.98%，在已披露的同业公司中排名第30，较上季度资产负债率减少0.17个百分点，较去年同季度资产负债率增加1.14个百分点": {"topic": "“消费”", "similarity": 0.4825443923473358, "prompt": "新闻文本是“公司最新资产负债率为63.98%，在已披露的同业公司中排名第30，较上季度资产负债率减少0.17个百分点，较去年同季度资产负债率增加1.14个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,赤字/亏损(deficit):-0.6"}, "公司最新毛利率为6.21%，在已披露的同业公司中排名第30，较上季度毛利率增加0.93个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.83个百分点": {"topic": "“消费”", "similarity": 0.46568793058395386, "prompt": "新闻文本是“公司最新毛利率为6.21%，在已披露的同业公司中排名第30，较上季度毛利率增加0.93个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.83个百分点”，包含的情绪词典是：百分比(percentage):0.0,利润/利益(profit):0.8"}, "公司摊薄每股收益为0.03元，在已披露的同业公司中排名第23，较去年同报告期摊薄每股收益减少0.02元，同比较去年同期下降45.09%": {"topic": "“金融”", "similarity": 0.4721742272377014, "prompt": "新闻文本是“公司摊薄每股收益为0.03元，在已披露的同业公司中排名第23，较去年同报告期摊薄每股收益减少0.02元，同比较去年同期下降45.09%”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新总资产周转率为0.38次，在已披露的同业公司中排名第9，较去年同季度总资产周转率减少0.05次，同比较去年同期下降12.25%": {"topic": "“消费”", "similarity": 0.4822200536727905, "prompt": "新闻文本是“公司最新总资产周转率为0.38次，在已披露的同业公司中排名第9，较去年同季度总资产周转率减少0.05次，同比较去年同期下降12.25%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "最新存货周转率为1.40次，在已披露的同业公司中排名第20，较去年同季度存货周转率减少0.31次，同比较去年同期下降18.12%": {"topic": "“消费”", "similarity": 0.4450295567512512, "prompt": "新闻文本是“最新存货周转率为1.40次，在已披露的同业公司中排名第20，较去年同季度存货周转率减少0.31次，同比较去年同期下降18.12%”，包含的情绪词典是：营业额/周转(turnover):0.0,减少/降低(reduction):-0.4"}, "公司股东户数为2.99万户，前十大股东持股数量为8.72亿股，占总股本比例为51.27%": {"topic": "“金融”", "similarity": 0.4728095531463623, "prompt": "新闻文本是“公司股东户数为2.99万户，前十大股东持股数量为8.72亿股，占总股本比例为51.27%”，包含的情绪词典是：公司/企业(company):0.0,公司/企业(firm):0.0"}, "前十大股东分别为华孚控股有限公司、安徽飞亚纺织有限公司、深圳市华人投资有限公司、广西沣盛供应链管理有限公司、金元顺安基金-兴业银行-上海爱建信托-爱建信托欣欣7号定向增发事务管理类单一资金信托、金鹰基金-工商银行-万向信托-万向信托-星辰39号事务管理类单一资金信托、陆超祖、杨三宝、陆敏、中航鑫港担保有限公司，持股比例分别为29.50%、7.59%、4.82%、2.66%、1.65%、1.42%、1.03%、0.99%、0.98%、0.62%": {"topic": "“生产投资”", "similarity": 0.6072463989257812}}</t>
+          <t>{"公司营业总收入为65.23亿元，在已披露的同业公司中排名第2，较去年同报告期营业总收入减少12.30亿元，同比较去年同期下降15.87%": {"topic": "“消费”", "similarity": 0.5440757274627686, "prompt": "新闻文本是“公司营业总收入为65.23亿元，在已披露的同业公司中排名第2，较去年同报告期营业总收入减少12.30亿元，同比较去年同期下降15.87%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "归母净利润为4480.46万元，在已披露的同业公司中排名第17，较去年同报告期归母净利润减少3659.82万元，同比较去年同期下降44.96%": {"topic": "“消费”", "similarity": 0.5097399950027466, "prompt": "新闻文本是“归母净利润为4480.46万元，在已披露的同业公司中排名第17，较去年同报告期归母净利润减少3659.82万元，同比较去年同期下降44.96%”，包含的情绪词典是：减损/贬低(derogation):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为10.93亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入减少4.32亿元，同比较去年同期下降28.30%": {"topic": "“金融”", "similarity": 0.5478698015213013, "prompt": "新闻文本是“经营活动现金净流入为10.93亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入减少4.32亿元，同比较去年同期下降28.30%”，包含的情绪词典是：营业额/周转(turnover):0.0,盈利能力/获利能力(profitability):0.6"}, "公司最新资产负债率为63.98%，在已披露的同业公司中排名第30，较上季度资产负债率减少0.17个百分点，较去年同季度资产负债率增加1.14个百分点": {"topic": "“消费”", "similarity": 0.4825444519519806, "prompt": "新闻文本是“公司最新资产负债率为63.98%，在已披露的同业公司中排名第30，较上季度资产负债率减少0.17个百分点，较去年同季度资产负债率增加1.14个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,赤字/亏损(deficit):-0.6"}, "公司最新毛利率为6.21%，在已披露的同业公司中排名第30，较上季度毛利率增加0.93个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.83个百分点": {"topic": "“消费”", "similarity": 0.4656880497932434, "prompt": "新闻文本是“公司最新毛利率为6.21%，在已披露的同业公司中排名第30，较上季度毛利率增加0.93个百分点，实现2个季度连续上涨，较去年同季度毛利率增加0.83个百分点”，包含的情绪词典是：百分比(percentage):0.0,利润/利益(profit):0.8"}, "公司摊薄每股收益为0.03元，在已披露的同业公司中排名第23，较去年同报告期摊薄每股收益减少0.02元，同比较去年同期下降45.09%": {"topic": "“金融”", "similarity": 0.47217440605163574, "prompt": "新闻文本是“公司摊薄每股收益为0.03元，在已披露的同业公司中排名第23，较去年同报告期摊薄每股收益减少0.02元，同比较去年同期下降45.09%”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新总资产周转率为0.38次，在已披露的同业公司中排名第9，较去年同季度总资产周转率减少0.05次，同比较去年同期下降12.25%": {"topic": "“消费”", "similarity": 0.4822201728820801, "prompt": "新闻文本是“公司最新总资产周转率为0.38次，在已披露的同业公司中排名第9，较去年同季度总资产周转率减少0.05次，同比较去年同期下降12.25%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "最新存货周转率为1.40次，在已披露的同业公司中排名第20，较去年同季度存货周转率减少0.31次，同比较去年同期下降18.12%": {"topic": "“消费”", "similarity": 0.44502967596054077, "prompt": "新闻文本是“最新存货周转率为1.40次，在已披露的同业公司中排名第20，较去年同季度存货周转率减少0.31次，同比较去年同期下降18.12%”，包含的情绪词典是：营业额/周转(turnover):0.0,减少/降低(reduction):-0.4"}, "公司股东户数为2.99万户，前十大股东持股数量为8.72亿股，占总股本比例为51.27%": {"topic": "“金融”", "similarity": 0.4728097915649414, "prompt": "新闻文本是“公司股东户数为2.99万户，前十大股东持股数量为8.72亿股，占总股本比例为51.27%”，包含的情绪词典是：公司/企业(company):0.0,公司/企业(firm):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -2292,16 +2276,8 @@
           <t>上海证券报·中国证券网</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>{"news_prompt1": "上证报中国证券网讯白云山9月1日晚公告，公司董事张春波因个人原因辞职", "news_prompt2": "9月2日，据知情人士透露，张春波“上次董事会就没参加了", "news_prompt3": "”  　　8月30日，白云山发布《第九届董事会第十四次会议决议公告》显示，“执行董事张春波因个人原因缺席会议”", "news_prompt4": "wind资料显示，张春波自2015年1月至2021年8月任白云山副总经理，任职时长达6年8个月，自2019年6月28日起任白云山董事，陆续任广药集团党委委员，副总经理，白云山党委委员，中一药业与奇星药业党委书记，董事长，天心药业董事，广州白云山医药销售有限公司董事，广州医药海马品牌整合传播有限公司(“海马公司”)董事和医药公司董事", "news_prompt5": "此前，白云山于7月22日晚公告，公司董事长李楚源因个人原因辞去董事长、执行董事及战略发展与投资委员会主任职务，辞职后不再担任任何职务", "news_prompt6": "8月30日，据南粤清风网消息，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查", "news_prompt7": "（何治民 ）（文章来源：上海证券报·中国证券网）"}</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>{"”  　　8月30日，白云山发布《第九届董事会第十四次会议决议公告》显示，“执行董事张春波因个人原因缺席会议”": {"topic": "“金融”", "similarity": 0.4510177969932556}, "wind资料显示，张春波自2015年1月至2021年8月任白云山副总经理，任职时长达6年8个月，自2019年6月28日起任白云山董事，陆续任广药集团党委委员，副总经理，白云山党委委员，中一药业与奇星药业党委书记，董事长，天心药业董事，广州白云山医药销售有限公司董事，广州医药海马品牌整合传播有限公司(“海马公司”)董事和医药公司董事": {"topic": "“生产投资”", "similarity": 0.4915749728679657}, "此前，白云山于7月22日晚公告，公司董事长李楚源因个人原因辞去董事长、执行董事及战略发展与投资委员会主任职务，辞职后不再担任任何职务": {"topic": "“生产投资”", "similarity": 0.4550020098686218}, "8月30日，据南粤清风网消息，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查": {"topic": "“生产投资”", "similarity": 0.4514555335044861}, "（何治民 ）（文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.5131739377975464, "prompt": "新闻文本是“（何治民 ）（文章来源：上海证券报·中国证券网）”，包含的情绪词典是：中国的/中国人的(chinese):0.0,投资者/投资人(investor):0.4"}}</t>
-        </is>
-      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2345,12 +2321,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "日前，梅江区政协召开“发挥政协优势，助力招商引资”专题协商座谈会，梅江区政协党组书记、主席房科辉，副主席杜延生、刘伟球、孙伟华、徐莉、陈启泰、卢小敬，部分政协参加单位负责同志、政协委员及有关单位负责人参加了会议", "news_prompt2": "会上，梅江区招商服务中心、区委统战部、深圳招商队、数字经济招商队汇报了发挥政协优势参与服务招商引资具体实践，参会人员围绕如何更好发挥政协优势、助力招商引资工作进行深入交流和探讨，并提出意见建议", "news_prompt3": "会议充分肯定了政协各参加单位、政协委员在助力招商引资工作上的履职成效", "news_prompt4": "房科辉指出，招商引资是推动梅江“百千万工程”走深走实的重要抓手，人民政协在参与项目引进、广泛开展招商引资工作上有着独特的优势", "news_prompt5": "他强调，一要发挥政协组织优势聚众力，积极为政协参加单位和政协委员搭建参与招商引资的工作平台，把招商引资工作作为履职的重要内容，优化履职服务，强化激励机制，健全沟通机制，共促招商引资工作提质增效", "news_prompt6": "二要发挥政协专委会优势汇众智，聚焦招商引资、项目建设、营商环境的热点难点问题履职尽责，对外交流联谊时要宣传推介梅江资源禀赋优势，了解当地政协委员中的明星企业信息，做好牵线搭桥、服务协调等工作，为招商引资工作献计出力", "news_prompt7": "三要发挥政协委员优势激众力，自觉担负起宣传家乡、推介家乡的责任，准确把握梅江农业、工业、服务业等发展方向及招商重点，围绕产业链强链补链延链，坚持以情招商、以诚引商、以商引商，吸引更多的大项目、好项目在梅江落地生根、开花结果，展现委员在招商引资工作中的风采", "news_prompt8": "南方日报记者魏丽文通讯员黄健（文章来源：南方日报）"}</t>
+          <t>{"news_prompt1": "日前，梅江区政协召开“发挥政协优势，助力招商引资”专题协商座谈会，梅江区政协党组书记、主席房科辉，副主席杜延生、刘伟球、孙伟华、徐莉、陈启泰、卢小敬，部分政协参加单位负责同志、政协委员及有关单位负责人参加了会议", "news_prompt2": "会上，梅江区招商服务中心、区委统战部、深圳招商队、数字经济招商队汇报了发挥政协优势参与服务招商引资具体实践，参会人员围绕如何更好发挥政协优势、助力招商引资工作进行深入交流和探讨，并提出意见建议", "news_prompt3": "会议充分肯定了政协各参加单位、政协委员在助力招商引资工作上的履职成效", "news_prompt4": "房科辉指出，招商引资是推动梅江“百千万工程”走深走实的重要抓手，人民政协在参与项目引进、广泛开展招商引资工作上有着独特的优势", "news_prompt5": "他强调，一要发挥政协组织优势聚众力，积极为政协参加单位和政协委员搭建参与招商引资的工作平台，把招商引资工作作为履职的重要内容，优化履职服务，强化激励机制，健全沟通机制，共促招商引资工作提质增效", "news_prompt6": "二要发挥政协专委会优势汇众智，聚焦招商引资、项目建设、营商环境的热点难点问题履职尽责，对外交流联谊时要宣传推介梅江资源禀赋优势，了解当地政协委员中的明星企业信息，做好牵线搭桥、服务协调等工作，为招商引资工作献计出力", "news_prompt7": "三要发挥政协委员优势激众力，自觉担负起宣传家乡、推介家乡的责任，准确把握梅江农业、工业、服务业等发展方向及招商重点，围绕产业链强链补链延链，坚持以情招商、以诚引商、以商引商，吸引更多的大项目、好项目在梅江落地生根、开花结果，展现委员在招商引资工作中的风采"}</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>{"日前，梅江区政协召开“发挥政协优势，助力招商引资”专题协商座谈会，梅江区政协党组书记、主席房科辉，副主席杜延生、刘伟球、孙伟华、徐莉、陈启泰、卢小敬，部分政协参加单位负责同志、政协委员及有关单位负责人参加了会议": {"topic": "“生产投资”", "similarity": 0.5937801003456116, "prompt": "新闻文本是“日前，梅江区政协召开“发挥政协优势，助力招商引资”专题协商座谈会，梅江区政协党组书记、主席房科辉，副主席杜延生、刘伟球、孙伟华、徐莉、陈启泰、卢小敬，部分政协参加单位负责同志、政协委员及有关单位负责人参加了会议”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}, "会上，梅江区招商服务中心、区委统战部、深圳招商队、数字经济招商队汇报了发挥政协优势参与服务招商引资具体实践，参会人员围绕如何更好发挥政协优势、助力招商引资工作进行深入交流和探讨，并提出意见建议": {"topic": "“生产投资”", "similarity": 0.5720745325088501, "prompt": "新闻文本是“会上，梅江区招商服务中心、区委统战部、深圳招商队、数字经济招商队汇报了发挥政协优势参与服务招商引资具体实践，参会人员围绕如何更好发挥政协优势、助力招商引资工作进行深入交流和探讨，并提出意见建议”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}, "会议充分肯定了政协各参加单位、政协委员在助力招商引资工作上的履职成效": {"topic": "“生产投资”", "similarity": 0.5197257995605469, "prompt": "新闻文本是“会议充分肯定了政协各参加单位、政协委员在助力招商引资工作上的履职成效”，包含的情绪词典是：多产的/富有成效的(productive):0.7,议会(parliament):0.0"}, "房科辉指出，招商引资是推动梅江“百千万工程”走深走实的重要抓手，人民政协在参与项目引进、广泛开展招商引资工作上有着独特的优势": {"topic": "“生产投资”", "similarity": 0.5860968232154846, "prompt": "新闻文本是“房科辉指出，招商引资是推动梅江“百千万工程”走深走实的重要抓手，人民政协在参与项目引进、广泛开展招商引资工作上有着独特的优势”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}, "他强调，一要发挥政协组织优势聚众力，积极为政协参加单位和政协委员搭建参与招商引资的工作平台，把招商引资工作作为履职的重要内容，优化履职服务，强化激励机制，健全沟通机制，共促招商引资工作提质增效": {"topic": "“生产投资”", "similarity": 0.6032367944717407, "prompt": "新闻文本是“他强调，一要发挥政协组织优势聚众力，积极为政协参加单位和政协委员搭建参与招商引资的工作平台，把招商引资工作作为履职的重要内容，优化履职服务，强化激励机制，健全沟通机制，共促招商引资工作提质增效”，包含的情绪词典是：建设性的/有益的(constructive):0.4,组织/机构(organization):0.0"}, "二要发挥政协专委会优势汇众智，聚焦招商引资、项目建设、营商环境的热点难点问题履职尽责，对外交流联谊时要宣传推介梅江资源禀赋优势，了解当地政协委员中的明星企业信息，做好牵线搭桥、服务协调等工作，为招商引资工作献计出力": {"topic": "“生产投资”", "similarity": 0.6078019142150879, "prompt": "新闻文本是“二要发挥政协专委会优势汇众智，聚焦招商引资、项目建设、营商环境的热点难点问题履职尽责，对外交流联谊时要宣传推介梅江资源禀赋优势，了解当地政协委员中的明星企业信息，做好牵线搭桥、服务协调等工作，为招商引资工作献计出力”，包含的情绪词典是：建设性的/有益的(constructive):0.4,处于优势的/有利的(advantaged):0.7"}, "三要发挥政协委员优势激众力，自觉担负起宣传家乡、推介家乡的责任，准确把握梅江农业、工业、服务业等发展方向及招商重点，围绕产业链强链补链延链，坚持以情招商、以诚引商、以商引商，吸引更多的大项目、好项目在梅江落地生根、开花结果，展现委员在招商引资工作中的风采": {"topic": "“生产投资”", "similarity": 0.6217477917671204, "prompt": "新闻文本是“三要发挥政协委员优势激众力，自觉担负起宣传家乡、推介家乡的责任，准确把握梅江农业、工业、服务业等发展方向及招商重点，围绕产业链强链补链延链，坚持以情招商、以诚引商、以商引商，吸引更多的大项目、好项目在梅江落地生根、开花结果，展现委员在招商引资工作中的风采”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}}</t>
+          <t>{"日前，梅江区政协召开“发挥政协优势，助力招商引资”专题协商座谈会，梅江区政协党组书记、主席房科辉，副主席杜延生、刘伟球、孙伟华、徐莉、陈启泰、卢小敬，部分政协参加单位负责同志、政协委员及有关单位负责人参加了会议": {"topic": "“生产投资”", "similarity": 0.5937801599502563, "prompt": "新闻文本是“日前，梅江区政协召开“发挥政协优势，助力招商引资”专题协商座谈会，梅江区政协党组书记、主席房科辉，副主席杜延生、刘伟球、孙伟华、徐莉、陈启泰、卢小敬，部分政协参加单位负责同志、政协委员及有关单位负责人参加了会议”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}, "会上，梅江区招商服务中心、区委统战部、深圳招商队、数字经济招商队汇报了发挥政协优势参与服务招商引资具体实践，参会人员围绕如何更好发挥政协优势、助力招商引资工作进行深入交流和探讨，并提出意见建议": {"topic": "“生产投资”", "similarity": 0.5720745325088501, "prompt": "新闻文本是“会上，梅江区招商服务中心、区委统战部、深圳招商队、数字经济招商队汇报了发挥政协优势参与服务招商引资具体实践，参会人员围绕如何更好发挥政协优势、助力招商引资工作进行深入交流和探讨，并提出意见建议”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}, "会议充分肯定了政协各参加单位、政协委员在助力招商引资工作上的履职成效": {"topic": "“生产投资”", "similarity": 0.5197258591651917, "prompt": "新闻文本是“会议充分肯定了政协各参加单位、政协委员在助力招商引资工作上的履职成效”，包含的情绪词典是：多产的/富有成效的(productive):0.7,议会(parliament):0.0"}, "房科辉指出，招商引资是推动梅江“百千万工程”走深走实的重要抓手，人民政协在参与项目引进、广泛开展招商引资工作上有着独特的优势": {"topic": "“生产投资”", "similarity": 0.5860968828201294, "prompt": "新闻文本是“房科辉指出，招商引资是推动梅江“百千万工程”走深走实的重要抓手，人民政协在参与项目引进、广泛开展招商引资工作上有着独特的优势”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}, "他强调，一要发挥政协组织优势聚众力，积极为政协参加单位和政协委员搭建参与招商引资的工作平台，把招商引资工作作为履职的重要内容，优化履职服务，强化激励机制，健全沟通机制，共促招商引资工作提质增效": {"topic": "“生产投资”", "similarity": 0.603236734867096, "prompt": "新闻文本是“他强调，一要发挥政协组织优势聚众力，积极为政协参加单位和政协委员搭建参与招商引资的工作平台，把招商引资工作作为履职的重要内容，优化履职服务，强化激励机制，健全沟通机制，共促招商引资工作提质增效”，包含的情绪词典是：建设性的/有益的(constructive):0.4,组织/机构(organization):0.0"}, "二要发挥政协专委会优势汇众智，聚焦招商引资、项目建设、营商环境的热点难点问题履职尽责，对外交流联谊时要宣传推介梅江资源禀赋优势，了解当地政协委员中的明星企业信息，做好牵线搭桥、服务协调等工作，为招商引资工作献计出力": {"topic": "“生产投资”", "similarity": 0.6078019738197327, "prompt": "新闻文本是“二要发挥政协专委会优势汇众智，聚焦招商引资、项目建设、营商环境的热点难点问题履职尽责，对外交流联谊时要宣传推介梅江资源禀赋优势，了解当地政协委员中的明星企业信息，做好牵线搭桥、服务协调等工作，为招商引资工作献计出力”，包含的情绪词典是：建设性的/有益的(constructive):0.4,处于优势的/有利的(advantaged):0.7"}, "三要发挥政协委员优势激众力，自觉担负起宣传家乡、推介家乡的责任，准确把握梅江农业、工业、服务业等发展方向及招商重点，围绕产业链强链补链延链，坚持以情招商、以诚引商、以商引商，吸引更多的大项目、好项目在梅江落地生根、开花结果，展现委员在招商引资工作中的风采": {"topic": "“生产投资”", "similarity": 0.6217477917671204, "prompt": "新闻文本是“三要发挥政协委员优势激众力，自觉担负起宣传家乡、推介家乡的责任，准确把握梅江农业、工业、服务业等发展方向及招商重点，围绕产业链强链补链延链，坚持以情招商、以诚引商、以商引商，吸引更多的大项目、好项目在梅江落地生根、开花结果，展现委员在招商引资工作中的风采”，包含的情绪词典是：处于优势的/有利的(advantaged):0.7,优势/有利条件(advantage):0.7"}}</t>
         </is>
       </c>
     </row>
@@ -2396,12 +2372,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日，无问芯穹（Infinigence AI）宣布完成近5亿元A轮融资", "news_prompt2": "在成立1年4个月内，无问芯穹累计已完成近10亿元融资", "news_prompt3": "无问芯穹本轮融资联合领投方为社保基金中关村自主创新专项基金（君联资本担任管理人）、启明创投和洪泰基金，跟投方包括联想创投、小米、软通高科等战略投资方，国开科创、上海人工智能产业投资基金（临港科创投担任管理人）、徐汇科创投等国资基金，以及顺为资本、达晨财智、德同资本、尚势资本、森若玉坤、申万宏源、正景资本等财务机构", "news_prompt4": "无问芯穹本次融资募集的资金将用于加强技术人才吸纳与技术研发，推动产品商业化发展，强化生态合作等方面", "news_prompt5": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "9月2日，无问芯穹（Infinigence AI）宣布完成近5亿元A轮融资", "news_prompt2": "在成立1年4个月内，无问芯穹累计已完成近10亿元融资", "news_prompt3": "无问芯穹本次融资募集的资金将用于加强技术人才吸纳与技术研发，推动产品商业化发展，强化生态合作等方面"}</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>{"9月2日，无问芯穹（Infinigence AI）宣布完成近5亿元A轮融资": {"topic": "“生产投资”", "similarity": 0.48648688197135925, "prompt": "新闻文本是“9月2日，无问芯穹（Infinigence AI）宣布完成近5亿元A轮融资”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "在成立1年4个月内，无问芯穹累计已完成近10亿元融资": {"topic": "“生产投资”", "similarity": 0.4842492341995239, "prompt": "新闻文本是“在成立1年4个月内，无问芯穹累计已完成近10亿元融资”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "无问芯穹本轮融资联合领投方为社保基金中关村自主创新专项基金（君联资本担任管理人）、启明创投和洪泰基金，跟投方包括联想创投、小米、软通高科等战略投资方，国开科创、上海人工智能产业投资基金（临港科创投担任管理人）、徐汇科创投等国资基金，以及顺为资本、达晨财智、德同资本、尚势资本、森若玉坤、申万宏源、正景资本等财务机构": {"topic": "“生产投资”", "similarity": 0.5917584896087646}, "无问芯穹本次融资募集的资金将用于加强技术人才吸纳与技术研发，推动产品商业化发展，强化生态合作等方面": {"topic": "“生产投资”", "similarity": 0.5502171516418457, "prompt": "新闻文本是“无问芯穹本次融资募集的资金将用于加强技术人才吸纳与技术研发，推动产品商业化发展，强化生态合作等方面”，包含的情绪词典是：基金/资金(fund):0.1,资本/资金(capital):0.1"}}</t>
+          <t>{"9月2日，无问芯穹（Infinigence AI）宣布完成近5亿元A轮融资": {"topic": "“生产投资”", "similarity": 0.48648685216903687, "prompt": "新闻文本是“9月2日，无问芯穹（Infinigence AI）宣布完成近5亿元A轮融资”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "在成立1年4个月内，无问芯穹累计已完成近10亿元融资": {"topic": "“生产投资”", "similarity": 0.484249472618103, "prompt": "新闻文本是“在成立1年4个月内，无问芯穹累计已完成近10亿元融资”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "无问芯穹本次融资募集的资金将用于加强技术人才吸纳与技术研发，推动产品商业化发展，强化生态合作等方面": {"topic": "“生产投资”", "similarity": 0.5502171516418457, "prompt": "新闻文本是“无问芯穹本次融资募集的资金将用于加强技术人才吸纳与技术研发，推动产品商业化发展，强化生态合作等方面”，包含的情绪词典是：基金/资金(fund):0.1,资本/资金(capital):0.1"}}</t>
         </is>
       </c>
     </row>
@@ -2447,12 +2423,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "8月30日,由中国食品科学技术学会主办的“第二十四届中国方便食品大会暨方便食品展”于昆山国际会展中心正式落幕", "news_prompt2": "白象中国面作为方便面领域的国货创新代表受邀参加,并在行业专家见证下,白象汤好喝山菌老母鸡汤面和白象超香香香香香香菜面获颁“方便食品行业创新产品”奖项", "news_prompt3": "中国方便食品大会被认为是方便食品行业最具影响力的行业大会,此次大会有近百位行业嘉宾出席,大会还发布了《2023-2024年度方便食品行业创新趋势》,为行业高质量发展传达价值风向标", "news_prompt4": "与大会同期的方便食品展,是行业创新成果展示的舞台,涵盖方便面(粉丝)类、挂面类、冷冻食品类等6大品类方便食品,本次展览总面积首超1万平方米,包括白象在内的150余家展商,吸引了全国数万名专业观众到访", "news_prompt5": "据行业趋势报告,创新成为中国方便食品产业高质量发展的重要支撑,方便食品企业在创新开发中则越来越注重健康及产品给消费者提供的情绪价值", "news_prompt6": "以此次获奖的白象为例,近年来不断推出符合新消费趋势、年轻人喜欢的创新产品,通过健康升级和细分品类的口味研发筑起市场护城河,始终在年轻人群中保持着高热度", "news_prompt7": "如作为白象流量最高产品之一的香菜面,过去一年在社媒平台的声量远高于其他方便面细分品类,特别是收获了年轻网友的关注", "news_prompt8": "此次方便食品展上,白象展区亦备受关注,汤好喝桶面装置亮眼醒目,现场的互动游戏也为展会增添了几分趣味,不少业内人士和经销商在展区内进行深度交流", "news_prompt9": "与此同时,白象展区的试吃台人头攒动,爆款香菜面吸引了不少“香菜党”,老母鸡汤面浓香四溢,大分量蟹黄酱包让人口齿留香,大辣娇火锅面鲜爽麻辣让人直呼过瘾……众多产品得到了现场行业权威人士的高度认可", "news_prompt10": "根据权威市场调研机构欧睿国际发布的认证声明,白象老母鸡汤面“全球销量第一”,成为更多消费者健康美味且安全的食品选择", "news_prompt11": "公开资料显示,白象2003年推出“1元大骨面”成为高汤面品类开创者,2018年推出汤好喝老母鸡汤面,6小时熬制高汤包取代粉包酱包,一年销量破10亿元大关", "news_prompt12": "在刚刚过去的白象航天食品联合实验室成立仪式上,白象官宣汤好喝高汤面系列在维持价格不变的基础上,实现产品“0添加防腐剂和0反式脂肪酸”的“双0”升级,配菜升级", "news_prompt13": "除了探索方便速食行业品类升级迭代的新方向,白象的产品创新还体现在对小众猎奇口味的开发,牢牢占据着话题C位", "news_prompt14": "此次获奖的白象超香香香香香香菜面,从前期精准的市场洞察,到激发全网热议的话题营销,让更多年轻群体关注到白象产品的更新进阶", "news_prompt15": "在亮眼成绩背后,是基于白象中国面27年来只为做好一碗中国面的坚持,也是白象持续深化产品创新,以地道中国味和创新风味俘获年轻人“中国胃”的体现", "news_prompt16": "据了解,白象多款产品频频出圈,备受好评,除了此次获奖的老母鸡汤面和香菜面,还有主打地域口味和地道风味的蟹黄拌面,以及被网友戏称“掌管哈喇子的神”的大辣娇牛油麻辣火锅面", "news_prompt17": "不断推动产品和技术创新,可以预见的是,白象将为方便食品行业增长提供更大的想象空间", "news_prompt18": "（文章来源：羊城晚报）"}</t>
+          <t>{"news_prompt1": "8月30日,由中国食品科学技术学会主办的“第二十四届中国方便食品大会暨方便食品展”于昆山国际会展中心正式落幕", "news_prompt2": "中国方便食品大会被认为是方便食品行业最具影响力的行业大会,此次大会有近百位行业嘉宾出席,大会还发布了《2023-2024年度方便食品行业创新趋势》,为行业高质量发展传达价值风向标", "news_prompt3": "与大会同期的方便食品展,是行业创新成果展示的舞台,涵盖方便面(粉丝)类、挂面类、冷冻食品类等6大品类方便食品,本次展览总面积首超1万平方米,包括白象在内的150余家展商,吸引了全国数万名专业观众到访", "news_prompt4": "据行业趋势报告,创新成为中国方便食品产业高质量发展的重要支撑,方便食品企业在创新开发中则越来越注重健康及产品给消费者提供的情绪价值", "news_prompt5": "以此次获奖的白象为例,近年来不断推出符合新消费趋势、年轻人喜欢的创新产品,通过健康升级和细分品类的口味研发筑起市场护城河,始终在年轻人群中保持着高热度", "news_prompt6": "如作为白象流量最高产品之一的香菜面,过去一年在社媒平台的声量远高于其他方便面细分品类,特别是收获了年轻网友的关注", "news_prompt7": "此次方便食品展上,白象展区亦备受关注,汤好喝桶面装置亮眼醒目,现场的互动游戏也为展会增添了几分趣味,不少业内人士和经销商在展区内进行深度交流", "news_prompt8": "与此同时,白象展区的试吃台人头攒动,爆款香菜面吸引了不少“香菜党”,老母鸡汤面浓香四溢,大分量蟹黄酱包让人口齿留香,大辣娇火锅面鲜爽麻辣让人直呼过瘾……众多产品得到了现场行业权威人士的高度认可", "news_prompt9": "根据权威市场调研机构欧睿国际发布的认证声明,白象老母鸡汤面“全球销量第一”,成为更多消费者健康美味且安全的食品选择", "news_prompt10": "除了探索方便速食行业品类升级迭代的新方向,白象的产品创新还体现在对小众猎奇口味的开发,牢牢占据着话题C位", "news_prompt11": "此次获奖的白象超香香香香香香菜面,从前期精准的市场洞察,到激发全网热议的话题营销,让更多年轻群体关注到白象产品的更新进阶", "news_prompt12": "在亮眼成绩背后,是基于白象中国面27年来只为做好一碗中国面的坚持,也是白象持续深化产品创新,以地道中国味和创新风味俘获年轻人“中国胃”的体现", "news_prompt13": "不断推动产品和技术创新,可以预见的是,白象将为方便食品行业增长提供更大的想象空间"}</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>{"8月30日,由中国食品科学技术学会主办的“第二十四届中国方便食品大会暨方便食品展”于昆山国际会展中心正式落幕": {"topic": "“消费”", "similarity": 0.5448175072669983, "prompt": "新闻文本是“8月30日,由中国食品科学技术学会主办的“第二十四届中国方便食品大会暨方便食品展”于昆山国际会展中心正式落幕”，包含的情绪词典是：食物/食品(food):0.0,产品/产物(product):0.15"}, "白象中国面作为方便面领域的国货创新代表受邀参加,并在行业专家见证下,白象汤好喝山菌老母鸡汤面和白象超香香香香香香菜面获颁“方便食品行业创新产品”奖项": {"topic": "“消费”", "similarity": 0.5226649045944214}, "中国方便食品大会被认为是方便食品行业最具影响力的行业大会,此次大会有近百位行业嘉宾出席,大会还发布了《2023-2024年度方便食品行业创新趋势》,为行业高质量发展传达价值风向标": {"topic": "“消费”", "similarity": 0.5820236206054688, "prompt": "新闻文本是“中国方便食品大会被认为是方便食品行业最具影响力的行业大会,此次大会有近百位行业嘉宾出席,大会还发布了《2023-2024年度方便食品行业创新趋势》,为行业高质量发展传达价值风向标”，包含的情绪词典是：有影响力的/有势力的(influential):0.4,食物/食品(food):0.0"}, "与大会同期的方便食品展,是行业创新成果展示的舞台,涵盖方便面(粉丝)类、挂面类、冷冻食品类等6大品类方便食品,本次展览总面积首超1万平方米,包括白象在内的150余家展商,吸引了全国数万名专业观众到访": {"topic": "“消费”", "similarity": 0.5796998739242554, "prompt": "新闻文本是“与大会同期的方便食品展,是行业创新成果展示的舞台,涵盖方便面(粉丝)类、挂面类、冷冻食品类等6大品类方便食品,本次展览总面积首超1万平方米,包括白象在内的150余家展商,吸引了全国数万名专业观众到访”，包含的情绪词典是：食物/食品(food):0.0,物体/对象(object):0.0"}, "据行业趋势报告,创新成为中国方便食品产业高质量发展的重要支撑,方便食品企业在创新开发中则越来越注重健康及产品给消费者提供的情绪价值": {"topic": "“消费”", "similarity": 0.6255625486373901, "prompt": "新闻文本是“据行业趋势报告,创新成为中国方便食品产业高质量发展的重要支撑,方便食品企业在创新开发中则越来越注重健康及产品给消费者提供的情绪价值”，包含的情绪词典是：创新的/革新的(innovative):0.7,创新/革新(innovate):0.6"}, "以此次获奖的白象为例,近年来不断推出符合新消费趋势、年轻人喜欢的创新产品,通过健康升级和细分品类的口味研发筑起市场护城河,始终在年轻人群中保持着高热度": {"topic": "“消费”", "similarity": 0.6113975048065186, "prompt": "新闻文本是“以此次获奖的白象为例,近年来不断推出符合新消费趋势、年轻人喜欢的创新产品,通过健康升级和细分品类的口味研发筑起市场护城河,始终在年轻人群中保持着高热度”，包含的情绪词典是：创新的/革新的(innovative):0.7,有影响力的/有势力的(influential):0.4"}, "如作为白象流量最高产品之一的香菜面,过去一年在社媒平台的声量远高于其他方便面细分品类,特别是收获了年轻网友的关注": {"topic": "“消费”", "similarity": 0.5286710262298584, "prompt": "新闻文本是“如作为白象流量最高产品之一的香菜面,过去一年在社媒平台的声量远高于其他方便面细分品类,特别是收获了年轻网友的关注”，包含的情绪词典是：产品/产物(product):0.15,食物/食品(food):0.0"}, "此次方便食品展上,白象展区亦备受关注,汤好喝桶面装置亮眼醒目,现场的互动游戏也为展会增添了几分趣味,不少业内人士和经销商在展区内进行深度交流": {"topic": "“消费”", "similarity": 0.5365208387374878, "prompt": "新闻文本是“此次方便食品展上,白象展区亦备受关注,汤好喝桶面装置亮眼醒目,现场的互动游戏也为展会增添了几分趣味,不少业内人士和经销商在展区内进行深度交流”，包含的情绪词典是：食物/食品(food):0.0,物体/对象(object):0.0"}, "与此同时,白象展区的试吃台人头攒动,爆款香菜面吸引了不少“香菜党”,老母鸡汤面浓香四溢,大分量蟹黄酱包让人口齿留香,大辣娇火锅面鲜爽麻辣让人直呼过瘾……众多产品得到了现场行业权威人士的高度认可": {"topic": "“消费”", "similarity": 0.5906807780265808, "prompt": "新闻文本是“与此同时,白象展区的试吃台人头攒动,爆款香菜面吸引了不少“香菜党”,老母鸡汤面浓香四溢,大分量蟹黄酱包让人口齿留香,大辣娇火锅面鲜爽麻辣让人直呼过瘾……众多产品得到了现场行业权威人士的高度认可”，包含的情绪词典是：有吸引力的/吸引人的(attractive):0.5,吸引人的/有吸引力的(appealing):0.2"}, "根据权威市场调研机构欧睿国际发布的认证声明,白象老母鸡汤面“全球销量第一”,成为更多消费者健康美味且安全的食品选择": {"topic": "“消费”", "similarity": 0.5419738292694092, "prompt": "新闻文本是“根据权威市场调研机构欧睿国际发布的认证声明,白象老母鸡汤面“全球销量第一”,成为更多消费者健康美味且安全的食品选择”，包含的情绪词典是：已公证的/已证实的(notarized):0.0,消费者/用户(consumer):0.0"}, "公开资料显示,白象2003年推出“1元大骨面”成为高汤面品类开创者,2018年推出汤好喝老母鸡汤面,6小时熬制高汤包取代粉包酱包,一年销量破10亿元大关": {"topic": "“消费”", "similarity": 0.5316485166549683}, "在刚刚过去的白象航天食品联合实验室成立仪式上,白象官宣汤好喝高汤面系列在维持价格不变的基础上,实现产品“0添加防腐剂和0反式脂肪酸”的“双0”升级,配菜升级": {"topic": "“消费”", "similarity": 0.5204581022262573}, "除了探索方便速食行业品类升级迭代的新方向,白象的产品创新还体现在对小众猎奇口味的开发,牢牢占据着话题C位": {"topic": "“消费”", "similarity": 0.5500870943069458, "prompt": "新闻文本是“除了探索方便速食行业品类升级迭代的新方向,白象的产品创新还体现在对小众猎奇口味的开发,牢牢占据着话题C位”，包含的情绪词典是：创新的/革新的(innovative):0.7,创新/革新(innovate):0.6"}, "此次获奖的白象超香香香香香香菜面,从前期精准的市场洞察,到激发全网热议的话题营销,让更多年轻群体关注到白象产品的更新进阶": {"topic": "“消费”", "similarity": 0.560193657875061, "prompt": "新闻文本是“此次获奖的白象超香香香香香香菜面,从前期精准的市场洞察,到激发全网热议的话题营销,让更多年轻群体关注到白象产品的更新进阶”，包含的情绪词典是：食物/食品(food):0.0,吸引人的/有吸引力的(appealing):0.2"}, "在亮眼成绩背后,是基于白象中国面27年来只为做好一碗中国面的坚持,也是白象持续深化产品创新,以地道中国味和创新风味俘获年轻人“中国胃”的体现": {"topic": "“消费”", "similarity": 0.5931860208511353, "prompt": "新闻文本是“在亮眼成绩背后,是基于白象中国面27年来只为做好一碗中国面的坚持,也是白象持续深化产品创新,以地道中国味和创新风味俘获年轻人“中国胃”的体现”，包含的情绪词典是：中国的/中国人的(chinese):0.0,成功的/圆满的(successful):0.9"}, "据了解,白象多款产品频频出圈,备受好评,除了此次获奖的老母鸡汤面和香菜面,还有主打地域口味和地道风味的蟹黄拌面,以及被网友戏称“掌管哈喇子的神”的大辣娇牛油麻辣火锅面": {"topic": "“消费”", "similarity": 0.5372625589370728}, "不断推动产品和技术创新,可以预见的是,白象将为方便食品行业增长提供更大的想象空间": {"topic": "“消费”", "similarity": 0.43551307916641235, "prompt": "新闻文本是“不断推动产品和技术创新,可以预见的是,白象将为方便食品行业增长提供更大的想象空间”，包含的情绪词典是：可想象的/可设想的(conceivable):0.0,创新/革新(innovation):0.7"}}</t>
+          <t>{"8月30日,由中国食品科学技术学会主办的“第二十四届中国方便食品大会暨方便食品展”于昆山国际会展中心正式落幕": {"topic": "“消费”", "similarity": 0.5448175072669983, "prompt": "新闻文本是“8月30日,由中国食品科学技术学会主办的“第二十四届中国方便食品大会暨方便食品展”于昆山国际会展中心正式落幕”，包含的情绪词典是：食物/食品(food):0.0,产品/产物(product):0.15"}, "中国方便食品大会被认为是方便食品行业最具影响力的行业大会,此次大会有近百位行业嘉宾出席,大会还发布了《2023-2024年度方便食品行业创新趋势》,为行业高质量发展传达价值风向标": {"topic": "“消费”", "similarity": 0.5820237398147583, "prompt": "新闻文本是“中国方便食品大会被认为是方便食品行业最具影响力的行业大会,此次大会有近百位行业嘉宾出席,大会还发布了《2023-2024年度方便食品行业创新趋势》,为行业高质量发展传达价值风向标”，包含的情绪词典是：有影响力的/有势力的(influential):0.4,食物/食品(food):0.0"}, "与大会同期的方便食品展,是行业创新成果展示的舞台,涵盖方便面(粉丝)类、挂面类、冷冻食品类等6大品类方便食品,本次展览总面积首超1万平方米,包括白象在内的150余家展商,吸引了全国数万名专业观众到访": {"topic": "“消费”", "similarity": 0.5796999931335449, "prompt": "新闻文本是“与大会同期的方便食品展,是行业创新成果展示的舞台,涵盖方便面(粉丝)类、挂面类、冷冻食品类等6大品类方便食品,本次展览总面积首超1万平方米,包括白象在内的150余家展商,吸引了全国数万名专业观众到访”，包含的情绪词典是：食物/食品(food):0.0,物体/对象(object):0.0"}, "据行业趋势报告,创新成为中国方便食品产业高质量发展的重要支撑,方便食品企业在创新开发中则越来越注重健康及产品给消费者提供的情绪价值": {"topic": "“消费”", "similarity": 0.6255626678466797, "prompt": "新闻文本是“据行业趋势报告,创新成为中国方便食品产业高质量发展的重要支撑,方便食品企业在创新开发中则越来越注重健康及产品给消费者提供的情绪价值”，包含的情绪词典是：创新的/革新的(innovative):0.7,创新/革新(innovate):0.6"}, "以此次获奖的白象为例,近年来不断推出符合新消费趋势、年轻人喜欢的创新产品,通过健康升级和细分品类的口味研发筑起市场护城河,始终在年轻人群中保持着高热度": {"topic": "“消费”", "similarity": 0.6113976240158081, "prompt": "新闻文本是“以此次获奖的白象为例,近年来不断推出符合新消费趋势、年轻人喜欢的创新产品,通过健康升级和细分品类的口味研发筑起市场护城河,始终在年轻人群中保持着高热度”，包含的情绪词典是：创新的/革新的(innovative):0.7,有影响力的/有势力的(influential):0.4"}, "如作为白象流量最高产品之一的香菜面,过去一年在社媒平台的声量远高于其他方便面细分品类,特别是收获了年轻网友的关注": {"topic": "“消费”", "similarity": 0.528671145439148, "prompt": "新闻文本是“如作为白象流量最高产品之一的香菜面,过去一年在社媒平台的声量远高于其他方便面细分品类,特别是收获了年轻网友的关注”，包含的情绪词典是：产品/产物(product):0.15,食物/食品(food):0.0"}, "此次方便食品展上,白象展区亦备受关注,汤好喝桶面装置亮眼醒目,现场的互动游戏也为展会增添了几分趣味,不少业内人士和经销商在展区内进行深度交流": {"topic": "“消费”", "similarity": 0.5365210175514221, "prompt": "新闻文本是“此次方便食品展上,白象展区亦备受关注,汤好喝桶面装置亮眼醒目,现场的互动游戏也为展会增添了几分趣味,不少业内人士和经销商在展区内进行深度交流”，包含的情绪词典是：食物/食品(food):0.0,物体/对象(object):0.0"}, "与此同时,白象展区的试吃台人头攒动,爆款香菜面吸引了不少“香菜党”,老母鸡汤面浓香四溢,大分量蟹黄酱包让人口齿留香,大辣娇火锅面鲜爽麻辣让人直呼过瘾……众多产品得到了现场行业权威人士的高度认可": {"topic": "“消费”", "similarity": 0.5906808972358704, "prompt": "新闻文本是“与此同时,白象展区的试吃台人头攒动,爆款香菜面吸引了不少“香菜党”,老母鸡汤面浓香四溢,大分量蟹黄酱包让人口齿留香,大辣娇火锅面鲜爽麻辣让人直呼过瘾……众多产品得到了现场行业权威人士的高度认可”，包含的情绪词典是：有吸引力的/吸引人的(attractive):0.5,吸引人的/有吸引力的(appealing):0.2"}, "根据权威市场调研机构欧睿国际发布的认证声明,白象老母鸡汤面“全球销量第一”,成为更多消费者健康美味且安全的食品选择": {"topic": "“消费”", "similarity": 0.541973888874054, "prompt": "新闻文本是“根据权威市场调研机构欧睿国际发布的认证声明,白象老母鸡汤面“全球销量第一”,成为更多消费者健康美味且安全的食品选择”，包含的情绪词典是：已公证的/已证实的(notarized):0.0,消费者/用户(consumer):0.0"}, "除了探索方便速食行业品类升级迭代的新方向,白象的产品创新还体现在对小众猎奇口味的开发,牢牢占据着话题C位": {"topic": "“消费”", "similarity": 0.5500872135162354, "prompt": "新闻文本是“除了探索方便速食行业品类升级迭代的新方向,白象的产品创新还体现在对小众猎奇口味的开发,牢牢占据着话题C位”，包含的情绪词典是：创新的/革新的(innovative):0.7,创新/革新(innovate):0.6"}, "此次获奖的白象超香香香香香香菜面,从前期精准的市场洞察,到激发全网热议的话题营销,让更多年轻群体关注到白象产品的更新进阶": {"topic": "“消费”", "similarity": 0.5601937174797058, "prompt": "新闻文本是“此次获奖的白象超香香香香香香菜面,从前期精准的市场洞察,到激发全网热议的话题营销,让更多年轻群体关注到白象产品的更新进阶”，包含的情绪词典是：食物/食品(food):0.0,吸引人的/有吸引力的(appealing):0.2"}, "在亮眼成绩背后,是基于白象中国面27年来只为做好一碗中国面的坚持,也是白象持续深化产品创新,以地道中国味和创新风味俘获年轻人“中国胃”的体现": {"topic": "“消费”", "similarity": 0.5931860208511353, "prompt": "新闻文本是“在亮眼成绩背后,是基于白象中国面27年来只为做好一碗中国面的坚持,也是白象持续深化产品创新,以地道中国味和创新风味俘获年轻人“中国胃”的体现”，包含的情绪词典是：中国的/中国人的(chinese):0.0,成功的/圆满的(successful):0.9"}, "不断推动产品和技术创新,可以预见的是,白象将为方便食品行业增长提供更大的想象空间": {"topic": "“消费”", "similarity": 0.43551337718963623, "prompt": "新闻文本是“不断推动产品和技术创新,可以预见的是,白象将为方便食品行业增长提供更大的想象空间”，包含的情绪词典是：可想象的/可设想的(conceivable):0.0,创新/革新(innovation):0.7"}}</t>
         </is>
       </c>
     </row>
@@ -2498,12 +2474,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "医疗器械板块半年度业绩利好频传，医疗器械ETF（562600）上周连续2日大涨", "news_prompt2": "2024年9月2日早盘，医疗器械指数小幅调整，而冠昊生物（细胞免疫治疗概念）、奥美医疗涨停，中源协和、奥泰生物等大涨", "news_prompt3": "相关机构指出，医疗设备更新政策当前已完成各省规划阶段，预计于Q3开始落地，Q4大规模落地", "news_prompt4": "延迟1年左右的医疗设备采购需求将于2025年陆续释放，医疗器械龙头有望实现亮眼的收入端及利润端增长", "news_prompt5": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "医疗器械板块半年度业绩利好频传，医疗器械ETF（562600）上周连续2日大涨", "news_prompt2": "2024年9月2日早盘，医疗器械指数小幅调整，而冠昊生物（细胞免疫治疗概念）、奥美医疗涨停，中源协和、奥泰生物等大涨", "news_prompt3": "相关机构指出，医疗设备更新政策当前已完成各省规划阶段，预计于Q3开始落地，Q4大规模落地", "news_prompt4": "延迟1年左右的医疗设备采购需求将于2025年陆续释放，医疗器械龙头有望实现亮眼的收入端及利润端增长"}</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>{"医疗器械板块半年度业绩利好频传，医疗器械ETF（562600）上周连续2日大涨": {"topic": "“金融”", "similarity": 0.46720293164253235, "prompt": "新闻文本是“医疗器械板块半年度业绩利好频传，医疗器械ETF（562600）上周连续2日大涨”，包含的情绪词典是：上升/上涨(rise):0.5,有利的/有益的(advantageous):0.8"}, "2024年9月2日早盘，医疗器械指数小幅调整，而冠昊生物（细胞免疫治疗概念）、奥美医疗涨停，中源协和、奥泰生物等大涨": {"topic": "“金融”", "similarity": 0.5609329342842102, "prompt": "新闻文本是“2024年9月2日早盘，医疗器械指数小幅调整，而冠昊生物（细胞免疫治疗概念）、奥美医疗涨停，中源协和、奥泰生物等大涨”，包含的情绪词典是：股票/库存(stock):0.0"}, "相关机构指出，医疗设备更新政策当前已完成各省规划阶段，预计于Q3开始落地，Q4大规模落地": {"topic": "“生产投资”", "similarity": 0.5379135608673096, "prompt": "新闻文本是“相关机构指出，医疗设备更新政策当前已完成各省规划阶段，预计于Q3开始落地，Q4大规模落地”，包含的情绪词典是：完成的/实现的(accomplished):0.6,准备好的/现成的(ready):0.2"}, "延迟1年左右的医疗设备采购需求将于2025年陆续释放，医疗器械龙头有望实现亮眼的收入端及利润端增长": {"topic": "“生产投资”", "similarity": 0.47938692569732666, "prompt": "新闻文本是“延迟1年左右的医疗设备采购需求将于2025年陆续释放，医疗器械龙头有望实现亮眼的收入端及利润端增长”，包含的情绪词典是：拖延的/延长的(protracted):0.0,被延迟的/被耽搁的(delayed):-0.3"}}</t>
+          <t>{"医疗器械板块半年度业绩利好频传，医疗器械ETF（562600）上周连续2日大涨": {"topic": "“金融”", "similarity": 0.46720314025878906, "prompt": "新闻文本是“医疗器械板块半年度业绩利好频传，医疗器械ETF（562600）上周连续2日大涨”，包含的情绪词典是：上升/上涨(rise):0.5,有利的/有益的(advantageous):0.8"}, "2024年9月2日早盘，医疗器械指数小幅调整，而冠昊生物（细胞免疫治疗概念）、奥美医疗涨停，中源协和、奥泰生物等大涨": {"topic": "“金融”", "similarity": 0.560932993888855, "prompt": "新闻文本是“2024年9月2日早盘，医疗器械指数小幅调整，而冠昊生物（细胞免疫治疗概念）、奥美医疗涨停，中源协和、奥泰生物等大涨”，包含的情绪词典是：股票/库存(stock):0.0"}, "相关机构指出，医疗设备更新政策当前已完成各省规划阶段，预计于Q3开始落地，Q4大规模落地": {"topic": "“生产投资”", "similarity": 0.5379136204719543, "prompt": "新闻文本是“相关机构指出，医疗设备更新政策当前已完成各省规划阶段，预计于Q3开始落地，Q4大规模落地”，包含的情绪词典是：完成的/实现的(accomplished):0.6,准备好的/现成的(ready):0.2"}, "延迟1年左右的医疗设备采购需求将于2025年陆续释放，医疗器械龙头有望实现亮眼的收入端及利润端增长": {"topic": "“生产投资”", "similarity": 0.479387104511261, "prompt": "新闻文本是“延迟1年左右的医疗设备采购需求将于2025年陆续释放，医疗器械龙头有望实现亮眼的收入端及利润端增长”，包含的情绪词典是：拖延的/延长的(protracted):0.0,被延迟的/被耽搁的(delayed):-0.3"}}</t>
         </is>
       </c>
     </row>
@@ -2549,12 +2525,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "每经AI快讯，中信证券研报认为，2024年以来，家电内需渐入“地产竣工周期负反馈”", "news_prompt2": "“以旧换新”政策适逢其时，用以对冲需求下行", "news_prompt3": "较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期", "news_prompt4": "缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力", "news_prompt5": "“以旧换新”的政策成效仍需观察", "news_prompt6": "但上述逻辑预期，或阶段性构建家电板块A/H股的交易性机会", "news_prompt7": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "每经AI快讯，中信证券研报认为，2024年以来，家电内需渐入“地产竣工周期负反馈”", "news_prompt2": "“以旧换新”政策适逢其时，用以对冲需求下行", "news_prompt3": "较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期", "news_prompt4": "缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力", "news_prompt5": "“以旧换新”的政策成效仍需观察", "news_prompt6": "但上述逻辑预期，或阶段性构建家电板块A/H股的交易性机会"}</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>{"每经AI快讯，中信证券研报认为，2024年以来，家电内需渐入“地产竣工周期负反馈”": {"topic": "“生产投资”", "similarity": 0.5229156017303467, "prompt": "新闻文本是“每经AI快讯，中信证券研报认为，2024年以来，家电内需渐入“地产竣工周期负反馈””，包含的情绪词典是：衰退的/不景气的(recessionary):-0.8,衰退/不景气(recession):-0.95"}, "“以旧换新”政策适逢其时，用以对冲需求下行": {"topic": "“消费”", "similarity": 0.487125039100647, "prompt": "新闻文本是““以旧换新”政策适逢其时，用以对冲需求下行”，包含的情绪词典是：贬值/减值(devaluation):-0.5,衰退/不景气(recession):-0.95"}, "较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期": {"topic": "“消费”", "similarity": 0.5888746380805969, "prompt": "新闻文本是“较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期”，包含的情绪词典是：监管/调控(regulation):0.0,调控性的/监管性的(regulative):0.0"}, "缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力": {"topic": "“金融”", "similarity": 0.4990229308605194, "prompt": "新闻文本是“缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力”，包含的情绪词典是：缓和/放松(easing):0.3,盈利能力/获利能力(profitability):0.6"}, "“以旧换新”的政策成效仍需观察": {"topic": "“生产投资”", "similarity": 0.5199661254882812, "prompt": "新闻文本是““以旧换新”的政策成效仍需观察”，包含的情绪词典是：政策(policy):0.0,重新分配/再分配(reassign):0.0"}, "但上述逻辑预期，或阶段性构建家电板块A/H股的交易性机会": {"topic": "“金融”", "similarity": 0.5020240545272827, "prompt": "新闻文本是“但上述逻辑预期，或阶段性构建家电板块A/H股的交易性机会”，包含的情绪词典是：预期/预料(anticipation):0.0,预期/预料(anticipate):0.2"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"每经AI快讯，中信证券研报认为，2024年以来，家电内需渐入“地产竣工周期负反馈”": {"topic": "“生产投资”", "similarity": 0.522915780544281, "prompt": "新闻文本是“每经AI快讯，中信证券研报认为，2024年以来，家电内需渐入“地产竣工周期负反馈””，包含的情绪词典是：衰退的/不景气的(recessionary):-0.8,衰退/不景气(recession):-0.95"}, "“以旧换新”政策适逢其时，用以对冲需求下行": {"topic": "“消费”", "similarity": 0.4871252179145813, "prompt": "新闻文本是““以旧换新”政策适逢其时，用以对冲需求下行”，包含的情绪词典是：贬值/减值(devaluation):-0.5,衰退/不景气(recession):-0.95"}, "较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期": {"topic": "“消费”", "similarity": 0.5888748168945312, "prompt": "新闻文本是“较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期”，包含的情绪词典是：监管/调控(regulation):0.0,调控性的/监管性的(regulative):0.0"}, "缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力": {"topic": "“金融”", "similarity": 0.4990233778953552, "prompt": "新闻文本是“缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力”，包含的情绪词典是：缓和/放松(easing):0.3,盈利能力/获利能力(profitability):0.6"}, "“以旧换新”的政策成效仍需观察": {"topic": "“生产投资”", "similarity": 0.5199661254882812, "prompt": "新闻文本是““以旧换新”的政策成效仍需观察”，包含的情绪词典是：政策(policy):0.0,重新分配/再分配(reassign):0.0"}, "但上述逻辑预期，或阶段性构建家电板块A/H股的交易性机会": {"topic": "“金融”", "similarity": 0.5020241737365723, "prompt": "新闻文本是“但上述逻辑预期，或阶段性构建家电板块A/H股的交易性机会”，包含的情绪词典是：预期/预料(anticipation):0.0,预期/预料(anticipate):0.2"}}</t>
         </is>
       </c>
     </row>
@@ -2600,12 +2576,12 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "中指研究院报告显示，8月楼市整体成交量环比同比皆下降，其中环比降幅较小", "news_prompt2": "一线城市同比上涨，涨幅5.05%，其中北京实现了环比同比均上涨，涨幅分别为19.6%和19.2%", "news_prompt3": "二三四线城市均下降", "news_prompt4": "库存面积总量环比小幅下降0.76%，上海降幅最大，两城市上涨", "news_prompt5": "土地方面，8月监测城市总体供求同比下降，宅地推出量同比降逾四成，整体成交方面量价双降，一线城市成交量降逾五成", "news_prompt6": "房企非银融资类型以中期票据、公司债为主，部分企业通过超短期融资券等方式获取资金", "news_prompt7": "房企拿地城市集中在南京、杭州、镇江、福州等城市", "news_prompt8": "其中，绿城18.87亿元竞得杭州拱墅区一宗宅地，溢价率25.21%", "news_prompt9": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "中指研究院报告显示，8月楼市整体成交量环比同比皆下降，其中环比降幅较小", "news_prompt2": "一线城市同比上涨，涨幅5.05%，其中北京实现了环比同比均上涨，涨幅分别为19.6%和19.2%", "news_prompt3": "二三四线城市均下降", "news_prompt4": "库存面积总量环比小幅下降0.76%，上海降幅最大，两城市上涨", "news_prompt5": "土地方面，8月监测城市总体供求同比下降，宅地推出量同比降逾四成，整体成交方面量价双降，一线城市成交量降逾五成", "news_prompt6": "房企非银融资类型以中期票据、公司债为主，部分企业通过超短期融资券等方式获取资金", "news_prompt7": "房企拿地城市集中在南京、杭州、镇江、福州等城市", "news_prompt8": "其中，绿城18.87亿元竞得杭州拱墅区一宗宅地，溢价率25.21%"}</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>{"中指研究院报告显示，8月楼市整体成交量环比同比皆下降，其中环比降幅较小": {"topic": "“房地产”", "similarity": 0.5498696565628052, "prompt": "新闻文本是“中指研究院报告显示，8月楼市整体成交量环比同比皆下降，其中环比降幅较小”，包含的情绪词典是：下降的/衰退的(declining):-0.6,减价/降价(markdown):0.0"}, "一线城市同比上涨，涨幅5.05%，其中北京实现了环比同比均上涨，涨幅分别为19.6%和19.2%": {"topic": "“房地产”", "similarity": 0.5206336975097656, "prompt": "新闻文本是“一线城市同比上涨，涨幅5.05%，其中北京实现了环比同比均上涨，涨幅分别为19.6%和19.2%”，包含的情绪词典是：上升/上涨(rise):0.5,增长/发展(growth):0.7"}, "二三四线城市均下降": {"topic": "“房地产”", "similarity": 0.5490805506706238, "prompt": "新闻文本是“二三四线城市均下降”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "库存面积总量环比小幅下降0.76%，上海降幅最大，两城市上涨": {"topic": "“房地产”", "similarity": 0.5027612447738647, "prompt": "新闻文本是“库存面积总量环比小幅下降0.76%，上海降幅最大，两城市上涨”，包含的情绪词典是：减价/降价(markdown):0.0,减少/降低(reduction):-0.4"}, "土地方面，8月监测城市总体供求同比下降，宅地推出量同比降逾四成，整体成交方面量价双降，一线城市成交量降逾五成": {"topic": "“房地产”", "similarity": 0.6549956202507019, "prompt": "新闻文本是“土地方面，8月监测城市总体供求同比下降，宅地推出量同比降逾四成，整体成交方面量价双降，一线城市成交量降逾五成”，包含的情绪词典是：房地产/财产(estate):0.0,减价/降价(markdown):0.0"}, "房企非银融资类型以中期票据、公司债为主，部分企业通过超短期融资券等方式获取资金": {"topic": "“房地产”", "similarity": 0.6232518553733826, "prompt": "新闻文本是“房企非银融资类型以中期票据、公司债为主，部分企业通过超短期融资券等方式获取资金”，包含的情绪词典是：房地产/财产(estate):0.0,债券/结合(bond):0.0"}, "房企拿地城市集中在南京、杭州、镇江、福州等城市": {"topic": "“房地产”", "similarity": 0.5958953499794006, "prompt": "新闻文本是“房企拿地城市集中在南京、杭州、镇江、福州等城市”，包含的情绪词典是：房地产/财产(estate):0.0,人工地/人造地(artificially):-0.1"}, "其中，绿城18.87亿元竞得杭州拱墅区一宗宅地，溢价率25.21%": {"topic": "“房地产”", "similarity": 0.4846600890159607, "prompt": "新闻文本是“其中，绿城18.87亿元竞得杭州拱墅区一宗宅地，溢价率25.21%”，包含的情绪词典是：按比例地/可估价地(ratably):0.0,房地产/财产(estate):0.0"}}</t>
+          <t>{"中指研究院报告显示，8月楼市整体成交量环比同比皆下降，其中环比降幅较小": {"topic": "“房地产”", "similarity": 0.5498698353767395, "prompt": "新闻文本是“中指研究院报告显示，8月楼市整体成交量环比同比皆下降，其中环比降幅较小”，包含的情绪词典是：下降的/衰退的(declining):-0.6,减价/降价(markdown):0.0"}, "一线城市同比上涨，涨幅5.05%，其中北京实现了环比同比均上涨，涨幅分别为19.6%和19.2%": {"topic": "“房地产”", "similarity": 0.5206339359283447, "prompt": "新闻文本是“一线城市同比上涨，涨幅5.05%，其中北京实现了环比同比均上涨，涨幅分别为19.6%和19.2%”，包含的情绪词典是：上升/上涨(rise):0.5,增长/发展(growth):0.7"}, "二三四线城市均下降": {"topic": "“房地产”", "similarity": 0.549080491065979, "prompt": "新闻文本是“二三四线城市均下降”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "库存面积总量环比小幅下降0.76%，上海降幅最大，两城市上涨": {"topic": "“房地产”", "similarity": 0.5027612447738647, "prompt": "新闻文本是“库存面积总量环比小幅下降0.76%，上海降幅最大，两城市上涨”，包含的情绪词典是：减价/降价(markdown):0.0,减少/降低(reduction):-0.4"}, "土地方面，8月监测城市总体供求同比下降，宅地推出量同比降逾四成，整体成交方面量价双降，一线城市成交量降逾五成": {"topic": "“房地产”", "similarity": 0.6549956202507019, "prompt": "新闻文本是“土地方面，8月监测城市总体供求同比下降，宅地推出量同比降逾四成，整体成交方面量价双降，一线城市成交量降逾五成”，包含的情绪词典是：房地产/财产(estate):0.0,减价/降价(markdown):0.0"}, "房企非银融资类型以中期票据、公司债为主，部分企业通过超短期融资券等方式获取资金": {"topic": "“房地产”", "similarity": 0.6232520341873169, "prompt": "新闻文本是“房企非银融资类型以中期票据、公司债为主，部分企业通过超短期融资券等方式获取资金”，包含的情绪词典是：房地产/财产(estate):0.0,债券/结合(bond):0.0"}, "房企拿地城市集中在南京、杭州、镇江、福州等城市": {"topic": "“房地产”", "similarity": 0.5958954095840454, "prompt": "新闻文本是“房企拿地城市集中在南京、杭州、镇江、福州等城市”，包含的情绪词典是：房地产/财产(estate):0.0,人工地/人造地(artificially):-0.1"}, "其中，绿城18.87亿元竞得杭州拱墅区一宗宅地，溢价率25.21%": {"topic": "“房地产”", "similarity": 0.48466014862060547, "prompt": "新闻文本是“其中，绿城18.87亿元竞得杭州拱墅区一宗宅地，溢价率25.21%”，包含的情绪词典是：按比例地/可估价地(ratably):0.0,房地产/财产(estate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -2651,12 +2627,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "日前，广州市荔湾区政务服务和数据管理局局长罗健华带队到梅江区政务服务和数据管理局交流座谈，双方签订政务服务“跨域通办”合作协议，梅江区副区长张瑜祥参加活动", "news_prompt2": "双方签订了政务服务“跨域通办”合作协议", "news_prompt3": "据了解，双方在去年签署结对帮扶协议的基础上，紧密联系互动，进一步打破地域限制，提升两地企业群众尤其是“反向飞地”企业办事便利度", "news_prompt4": "首先在涉企政务服务领域拓展“跨域通办”合作，通过线上线下融合办，实行“全程网办+大厅窗口+帮办代办”的方式，全方位立体式为市场主体和群众提供跨域服务，着力解决企业和群众异地办事“多地跑”“折返跑”等堵点难点问题", "news_prompt5": "梅江第一批涉及税务、人社、交通、市场监管、医保、卫健等企业服务领域的187个事项，可通过线下开设“跨域通办”专窗、线上全流程网办等形式实现“跨域通办”", "news_prompt6": "荔湾第一批涉及住建、水务、市场监管、农业农村等408个事项可在线上全流程网办，涉及文化广电、自然资源、消防等126个事项可在线下“跨域通办”专窗办理", "news_prompt7": "座谈会上，双方就推动政务服务事项便利化、提升政务服务中心服务质量、优化经营性涉企服务、产业园区政务服务、数字政府建设、开展数据要素流通等多方面进行充分交流", "news_prompt8": "南方日报记者魏丽文　　通讯员黄慕兴李泽龙（文章来源：南方日报）"}</t>
+          <t>{"news_prompt1": "日前，广州市荔湾区政务服务和数据管理局局长罗健华带队到梅江区政务服务和数据管理局交流座谈，双方签订政务服务“跨域通办”合作协议，梅江区副区长张瑜祥参加活动", "news_prompt2": "双方签订了政务服务“跨域通办”合作协议", "news_prompt3": "据了解，双方在去年签署结对帮扶协议的基础上，紧密联系互动，进一步打破地域限制，提升两地企业群众尤其是“反向飞地”企业办事便利度", "news_prompt4": "首先在涉企政务服务领域拓展“跨域通办”合作，通过线上线下融合办，实行“全程网办+大厅窗口+帮办代办”的方式，全方位立体式为市场主体和群众提供跨域服务，着力解决企业和群众异地办事“多地跑”“折返跑”等堵点难点问题", "news_prompt5": "荔湾第一批涉及住建、水务、市场监管、农业农村等408个事项可在线上全流程网办，涉及文化广电、自然资源、消防等126个事项可在线下“跨域通办”专窗办理", "news_prompt6": "座谈会上，双方就推动政务服务事项便利化、提升政务服务中心服务质量、优化经营性涉企服务、产业园区政务服务、数字政府建设、开展数据要素流通等多方面进行充分交流"}</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>{"日前，广州市荔湾区政务服务和数据管理局局长罗健华带队到梅江区政务服务和数据管理局交流座谈，双方签订政务服务“跨域通办”合作协议，梅江区副区长张瑜祥参加活动": {"topic": "“消费”", "similarity": 0.4983559250831604, "prompt": "新闻文本是“日前，广州市荔湾区政务服务和数据管理局局长罗健华带队到梅江区政务服务和数据管理局交流座谈，双方签订政务服务“跨域通办”合作协议，梅江区副区长张瑜祥参加活动”，包含的情绪词典是：服务/业务(service):0.0,地区的/区域的(regional):0.0"}, "双方签订了政务服务“跨域通办”合作协议": {"topic": "“生产投资”", "similarity": 0.4665135145187378, "prompt": "新闻文本是“双方签订了政务服务“跨域通办”合作协议”，包含的情绪词典是：协议/协定(agreement):0.4,服务/业务(service):0.0"}, "据了解，双方在去年签署结对帮扶协议的基础上，紧密联系互动，进一步打破地域限制，提升两地企业群众尤其是“反向飞地”企业办事便利度": {"topic": "“生产投资”", "similarity": 0.5690820217132568, "prompt": "新闻文本是“据了解，双方在去年签署结对帮扶协议的基础上，紧密联系互动，进一步打破地域限制，提升两地企业群众尤其是“反向飞地”企业办事便利度”，包含的情绪词典是：企业/事业(enterprise):0.0,合作性的/协作性的(collaborative):0.3"}, "首先在涉企政务服务领域拓展“跨域通办”合作，通过线上线下融合办，实行“全程网办+大厅窗口+帮办代办”的方式，全方位立体式为市场主体和群众提供跨域服务，着力解决企业和群众异地办事“多地跑”“折返跑”等堵点难点问题": {"topic": "“消费”", "similarity": 0.6269766092300415, "prompt": "新闻文本是“首先在涉企政务服务领域拓展“跨域通办”合作，通过线上线下融合办，实行“全程网办+大厅窗口+帮办代办”的方式，全方位立体式为市场主体和群众提供跨域服务，着力解决企业和群众异地办事“多地跑”“折返跑”等堵点难点问题”，包含的情绪词典是：企业/事业(enterprise):0.0,广泛的/大规模的(extensive):0.2"}, "梅江第一批涉及税务、人社、交通、市场监管、医保、卫健等企业服务领域的187个事项，可通过线下开设“跨域通办”专窗、线上全流程网办等形式实现“跨域通办”": {"topic": "“消费”", "similarity": 0.5178698301315308}, "荔湾第一批涉及住建、水务、市场监管、农业农村等408个事项可在线上全流程网办，涉及文化广电、自然资源、消防等126个事项可在线下“跨域通办”专窗办理": {"topic": "“消费”", "similarity": 0.5284450054168701, "prompt": "新闻文本是“荔湾第一批涉及住建、水务、市场监管、农业农村等408个事项可在线上全流程网办，涉及文化广电、自然资源、消防等126个事项可在线下“跨域通办”专窗办理”，包含的情绪词典是：可得到的/可用的(available):0.1,可获许可的/可被授权的(licensable):0.0"}, "座谈会上，双方就推动政务服务事项便利化、提升政务服务中心服务质量、优化经营性涉企服务、产业园区政务服务、数字政府建设、开展数据要素流通等多方面进行充分交流": {"topic": "“生产投资”", "similarity": 0.6089338660240173, "prompt": "新闻文本是“座谈会上，双方就推动政务服务事项便利化、提升政务服务中心服务质量、优化经营性涉企服务、产业园区政务服务、数字政府建设、开展数据要素流通等多方面进行充分交流”，包含的情绪词典是：会议/会面(meeting):0.0,提供信息的/增长见闻的(informative):0.5"}, "南方日报记者魏丽文　　通讯员黄慕兴李泽龙（文章来源：南方日报）": {"topic": "“消费”", "similarity": 0.43919333815574646, "prompt": "新闻文本是“南方日报记者魏丽文　　通讯员黄慕兴李泽龙（文章来源：南方日报）”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,令状/文书(writ):0.0"}}</t>
+          <t>{"日前，广州市荔湾区政务服务和数据管理局局长罗健华带队到梅江区政务服务和数据管理局交流座谈，双方签订政务服务“跨域通办”合作协议，梅江区副区长张瑜祥参加活动": {"topic": "“消费”", "similarity": 0.4983561038970947, "prompt": "新闻文本是“日前，广州市荔湾区政务服务和数据管理局局长罗健华带队到梅江区政务服务和数据管理局交流座谈，双方签订政务服务“跨域通办”合作协议，梅江区副区长张瑜祥参加活动”，包含的情绪词典是：服务/业务(service):0.0,地区的/区域的(regional):0.0"}, "双方签订了政务服务“跨域通办”合作协议": {"topic": "“生产投资”", "similarity": 0.4665134847164154, "prompt": "新闻文本是“双方签订了政务服务“跨域通办”合作协议”，包含的情绪词典是：协议/协定(agreement):0.4,服务/业务(service):0.0"}, "据了解，双方在去年签署结对帮扶协议的基础上，紧密联系互动，进一步打破地域限制，提升两地企业群众尤其是“反向飞地”企业办事便利度": {"topic": "“生产投资”", "similarity": 0.5690821409225464, "prompt": "新闻文本是“据了解，双方在去年签署结对帮扶协议的基础上，紧密联系互动，进一步打破地域限制，提升两地企业群众尤其是“反向飞地”企业办事便利度”，包含的情绪词典是：企业/事业(enterprise):0.0,合作性的/协作性的(collaborative):0.3"}, "首先在涉企政务服务领域拓展“跨域通办”合作，通过线上线下融合办，实行“全程网办+大厅窗口+帮办代办”的方式，全方位立体式为市场主体和群众提供跨域服务，着力解决企业和群众异地办事“多地跑”“折返跑”等堵点难点问题": {"topic": "“消费”", "similarity": 0.6269766092300415, "prompt": "新闻文本是“首先在涉企政务服务领域拓展“跨域通办”合作，通过线上线下融合办，实行“全程网办+大厅窗口+帮办代办”的方式，全方位立体式为市场主体和群众提供跨域服务，着力解决企业和群众异地办事“多地跑”“折返跑”等堵点难点问题”，包含的情绪词典是：企业/事业(enterprise):0.0,广泛的/大规模的(extensive):0.2"}, "荔湾第一批涉及住建、水务、市场监管、农业农村等408个事项可在线上全流程网办，涉及文化广电、自然资源、消防等126个事项可在线下“跨域通办”专窗办理": {"topic": "“消费”", "similarity": 0.5284450054168701, "prompt": "新闻文本是“荔湾第一批涉及住建、水务、市场监管、农业农村等408个事项可在线上全流程网办，涉及文化广电、自然资源、消防等126个事项可在线下“跨域通办”专窗办理”，包含的情绪词典是：可得到的/可用的(available):0.1,可获许可的/可被授权的(licensable):0.0"}, "座谈会上，双方就推动政务服务事项便利化、提升政务服务中心服务质量、优化经营性涉企服务、产业园区政务服务、数字政府建设、开展数据要素流通等多方面进行充分交流": {"topic": "“生产投资”", "similarity": 0.6089339256286621, "prompt": "新闻文本是“座谈会上，双方就推动政务服务事项便利化、提升政务服务中心服务质量、优化经营性涉企服务、产业园区政务服务、数字政府建设、开展数据要素流通等多方面进行充分交流”，包含的情绪词典是：会议/会面(meeting):0.0,提供信息的/增长见闻的(informative):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -2702,12 +2678,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "截至2024年9月2日 10:21，公司债ETF(511030)上涨0.01%，冲击4连涨", "news_prompt2": "最新价报10.52元，盘中成交额已达444.01万元", "news_prompt3": "国开债券ETF(159651)上涨0.05%，最新价报104.59元，盘中成交额已达5895.35万元", "news_prompt4": "活跃国债ETF(511020)上涨0.18%，最新价报112.8元，盘中成交额已达1259.70万元", "news_prompt5": "规模方面，公司债ETF最新规模达106.31亿元", "news_prompt6": "国开债券ETF最新规模达13.33亿元", "news_prompt7": "活跃国债ETF最新规模达13.87亿元", "news_prompt8": "资金流入方面，活跃国债ETF近5个交易日内，合计“吸金”1183.11万元", "news_prompt9": "9月2日早盘，国债期货开盘集体上涨，30年期主力合约涨0.31%，10年期主力合约涨0.16%，5年期主力合约涨0.08%，2年期主力合约涨0.01%", "news_prompt10": "8月30日，央行正式开启公开市场国债买卖操作，8月净买入1000亿元", "news_prompt11": "其操作模式非公开市场招标，避免了对市场利率的干扰，“买短卖长”的模式显示央行对于利率曲线“向上倾斜”的诉求较强", "news_prompt12": "净买入规模不算大，专家认为侧重于调节流动性", "news_prompt13": "华泰证券指出，货币政策方面，基本面趋势决定了四季度支持性的货币政策、稳中偏松的取向不变", "news_prompt14": "四季度降息落地概率不小，三季度末是降准的敏感时点", "news_prompt15": "不过，金融防风险是硬约束，央行对长期利率的管控态度预计还需要契机松动", "news_prompt16": "关注央行管控长期利率的可能措施，包括买卖债、临时隔夜正回购等", "news_prompt17": "平安基金债券ETF三剑客成员包括公司债ETF（511030）、国开债券ETF（159651）和活跃国债ETF（511020），产品类型包括国债、政金债和信用债，久期横跨长、中、短，能够助力投资者穿越债市周期", "news_prompt18": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "最新价报10.52元，盘中成交额已达444.01万元", "news_prompt2": "国开债券ETF(159651)上涨0.05%，最新价报104.59元，盘中成交额已达5895.35万元", "news_prompt3": "活跃国债ETF(511020)上涨0.18%，最新价报112.8元，盘中成交额已达1259.70万元", "news_prompt4": "规模方面，公司债ETF最新规模达106.31亿元", "news_prompt5": "国开债券ETF最新规模达13.33亿元", "news_prompt6": "活跃国债ETF最新规模达13.87亿元", "news_prompt7": "资金流入方面，活跃国债ETF近5个交易日内，合计“吸金”1183.11万元", "news_prompt8": "9月2日早盘，国债期货开盘集体上涨，30年期主力合约涨0.31%，10年期主力合约涨0.16%，5年期主力合约涨0.08%，2年期主力合约涨0.01%", "news_prompt9": "8月30日，央行正式开启公开市场国债买卖操作，8月净买入1000亿元", "news_prompt10": "其操作模式非公开市场招标，避免了对市场利率的干扰，“买短卖长”的模式显示央行对于利率曲线“向上倾斜”的诉求较强", "news_prompt11": "净买入规模不算大，专家认为侧重于调节流动性", "news_prompt12": "华泰证券指出，货币政策方面，基本面趋势决定了四季度支持性的货币政策、稳中偏松的取向不变", "news_prompt13": "四季度降息落地概率不小，三季度末是降准的敏感时点", "news_prompt14": "不过，金融防风险是硬约束，央行对长期利率的管控态度预计还需要契机松动", "news_prompt15": "关注央行管控长期利率的可能措施，包括买卖债、临时隔夜正回购等"}</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>{"最新价报10.52元，盘中成交额已达444.01万元": {"topic": "“房地产”", "similarity": 0.4457170367240906, "prompt": "新闻文本是“最新价报10.52元，盘中成交额已达444.01万元”，包含的情绪词典是：削价/低价出售(undercut):-0.3,价格/代价(price):0.0"}, "国开债券ETF(159651)上涨0.05%，最新价报104.59元，盘中成交额已达5895.35万元": {"topic": "“金融”", "similarity": 0.457504540681839, "prompt": "新闻文本是“国开债券ETF(159651)上涨0.05%，最新价报104.59元，盘中成交额已达5895.35万元”，包含的情绪词典是：债券/结合(bond):0.0,股票/库存(stock):0.0"}, "活跃国债ETF(511020)上涨0.18%，最新价报112.8元，盘中成交额已达1259.70万元": {"topic": "“金融”", "similarity": 0.4737144112586975, "prompt": "新闻文本是“活跃国债ETF(511020)上涨0.18%，最新价报112.8元，盘中成交额已达1259.70万元”，包含的情绪词典是：债券/结合(bond):0.0,按比例的/可估价的(rata):0.0"}, "规模方面，公司债ETF最新规模达106.31亿元": {"topic": "“金融”", "similarity": 0.5204037427902222, "prompt": "新闻文本是“规模方面，公司债ETF最新规模达106.31亿元”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(firm):0.0"}, "国开债券ETF最新规模达13.33亿元": {"topic": "“金融”", "similarity": 0.4827101528644562, "prompt": "新闻文本是“国开债券ETF最新规模达13.33亿元”，包含的情绪词典是：基金/资金(fund):0.1,债券/结合(bond):0.0"}, "活跃国债ETF最新规模达13.87亿元": {"topic": "“金融”", "similarity": 0.49697017669677734, "prompt": "新闻文本是“活跃国债ETF最新规模达13.87亿元”，包含的情绪词典是：基金/资金(fund):0.1,债券/结合(bond):0.0"}, "资金流入方面，活跃国债ETF近5个交易日内，合计“吸金”1183.11万元": {"topic": "“金融”", "similarity": 0.5256604552268982, "prompt": "新闻文本是“资金流入方面，活跃国债ETF近5个交易日内，合计“吸金”1183.11万元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "9月2日早盘，国债期货开盘集体上涨，30年期主力合约涨0.31%，10年期主力合约涨0.16%，5年期主力合约涨0.08%，2年期主力合约涨0.01%": {"topic": "“金融”", "similarity": 0.5222570300102234, "prompt": "新闻文本是“9月2日早盘，国债期货开盘集体上涨，30年期主力合约涨0.31%，10年期主力合约涨0.16%，5年期主力合约涨0.08%，2年期主力合约涨0.01%”，包含的情绪词典是：债券/结合(bond):0.0,通货膨胀(inflation):-0.5"}, "8月30日，央行正式开启公开市场国债买卖操作，8月净买入1000亿元": {"topic": "“金融”", "similarity": 0.5118561387062073, "prompt": "新闻文本是“8月30日，央行正式开启公开市场国债买卖操作，8月净买入1000亿元”，包含的情绪词典是：债券/结合(bond):0.0,金融的/财政的(financial):0.0"}, "其操作模式非公开市场招标，避免了对市场利率的干扰，“买短卖长”的模式显示央行对于利率曲线“向上倾斜”的诉求较强": {"topic": "“金融”", "similarity": 0.6016903519630432, "prompt": "新闻文本是“其操作模式非公开市场招标，避免了对市场利率的干扰，“买短卖长”的模式显示央行对于利率曲线“向上倾斜”的诉求较强”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,有利可图的/盈利的(profitable):0.8"}, "净买入规模不算大，专家认为侧重于调节流动性": {"topic": "“金融”", "similarity": 0.5072750449180603, "prompt": "新闻文本是“净买入规模不算大，专家认为侧重于调节流动性”，包含的情绪词典是：监管/调控(regulation):0.0,监管/调控(regulate):0.0"}, "华泰证券指出，货币政策方面，基本面趋势决定了四季度支持性的货币政策、稳中偏松的取向不变": {"topic": "“宏观经济”", "similarity": 0.5410767793655396, "prompt": "新闻文本是“华泰证券指出，货币政策方面，基本面趋势决定了四季度支持性的货币政策、稳中偏松的取向不变”，包含的情绪词典是：恒定的/不变的(constant):0.05,稳定的/稳固的(stable):0.5"}, "四季度降息落地概率不小，三季度末是降准的敏感时点": {"topic": "“宏观经济”", "similarity": 0.5784879922866821, "prompt": "新闻文本是“四季度降息落地概率不小，三季度末是降准的敏感时点”，包含的情绪词典是：季度/四分之一(quarter):0.0,降级/降低评级(downgrade):-0.6"}, "不过，金融防风险是硬约束，央行对长期利率的管控态度预计还需要契机松动": {"topic": "“金融”", "similarity": 0.5468115210533142, "prompt": "新闻文本是“不过，金融防风险是硬约束，央行对长期利率的管控态度预计还需要契机松动”，包含的情绪词典是：风险(risk):-0.4,调控性的/监管性的(regulative):0.0"}, "关注央行管控长期利率的可能措施，包括买卖债、临时隔夜正回购等": {"topic": "“金融”", "similarity": 0.5152861475944519, "prompt": "新闻文本是“关注央行管控长期利率的可能措施，包括买卖债、临时隔夜正回购等”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,监管的/调控的(regulatory):0.0"}, "平安基金债券ETF三剑客成员包括公司债ETF（511030）、国开债券ETF（159651）和活跃国债ETF（511020），产品类型包括国债、政金债和信用债，久期横跨长、中、短，能够助力投资者穿越债市周期": {"topic": "“金融”", "similarity": 0.5960706472396851}}</t>
+          <t>{"最新价报10.52元，盘中成交额已达444.01万元": {"topic": "“房地产”", "similarity": 0.4457172751426697, "prompt": "新闻文本是“最新价报10.52元，盘中成交额已达444.01万元”，包含的情绪词典是：削价/低价出售(undercut):-0.3,价格/代价(price):0.0"}, "国开债券ETF(159651)上涨0.05%，最新价报104.59元，盘中成交额已达5895.35万元": {"topic": "“金融”", "similarity": 0.4575047194957733, "prompt": "新闻文本是“国开债券ETF(159651)上涨0.05%，最新价报104.59元，盘中成交额已达5895.35万元”，包含的情绪词典是：债券/结合(bond):0.0,股票/库存(stock):0.0"}, "活跃国债ETF(511020)上涨0.18%，最新价报112.8元，盘中成交额已达1259.70万元": {"topic": "“金融”", "similarity": 0.4737144708633423, "prompt": "新闻文本是“活跃国债ETF(511020)上涨0.18%，最新价报112.8元，盘中成交额已达1259.70万元”，包含的情绪词典是：债券/结合(bond):0.0,按比例的/可估价的(rata):0.0"}, "规模方面，公司债ETF最新规模达106.31亿元": {"topic": "“金融”", "similarity": 0.5204038619995117, "prompt": "新闻文本是“规模方面，公司债ETF最新规模达106.31亿元”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(firm):0.0"}, "国开债券ETF最新规模达13.33亿元": {"topic": "“金融”", "similarity": 0.4827103316783905, "prompt": "新闻文本是“国开债券ETF最新规模达13.33亿元”，包含的情绪词典是：基金/资金(fund):0.1,债券/结合(bond):0.0"}, "活跃国债ETF最新规模达13.87亿元": {"topic": "“金融”", "similarity": 0.4969702959060669, "prompt": "新闻文本是“活跃国债ETF最新规模达13.87亿元”，包含的情绪词典是：基金/资金(fund):0.1,债券/结合(bond):0.0"}, "资金流入方面，活跃国债ETF近5个交易日内，合计“吸金”1183.11万元": {"topic": "“金融”", "similarity": 0.5256606340408325, "prompt": "新闻文本是“资金流入方面，活跃国债ETF近5个交易日内，合计“吸金”1183.11万元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "9月2日早盘，国债期货开盘集体上涨，30年期主力合约涨0.31%，10年期主力合约涨0.16%，5年期主力合约涨0.08%，2年期主力合约涨0.01%": {"topic": "“金融”", "similarity": 0.5222570300102234, "prompt": "新闻文本是“9月2日早盘，国债期货开盘集体上涨，30年期主力合约涨0.31%，10年期主力合约涨0.16%，5年期主力合约涨0.08%，2年期主力合约涨0.01%”，包含的情绪词典是：债券/结合(bond):0.0,通货膨胀(inflation):-0.5"}, "8月30日，央行正式开启公开市场国债买卖操作，8月净买入1000亿元": {"topic": "“金融”", "similarity": 0.5118563771247864, "prompt": "新闻文本是“8月30日，央行正式开启公开市场国债买卖操作，8月净买入1000亿元”，包含的情绪词典是：债券/结合(bond):0.0,金融的/财政的(financial):0.0"}, "其操作模式非公开市场招标，避免了对市场利率的干扰，“买短卖长”的模式显示央行对于利率曲线“向上倾斜”的诉求较强": {"topic": "“金融”", "similarity": 0.601690411567688, "prompt": "新闻文本是“其操作模式非公开市场招标，避免了对市场利率的干扰，“买短卖长”的模式显示央行对于利率曲线“向上倾斜”的诉求较强”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,有利可图的/盈利的(profitable):0.8"}, "净买入规模不算大，专家认为侧重于调节流动性": {"topic": "“金融”", "similarity": 0.5072751045227051, "prompt": "新闻文本是“净买入规模不算大，专家认为侧重于调节流动性”，包含的情绪词典是：监管/调控(regulation):0.0,监管/调控(regulate):0.0"}, "华泰证券指出，货币政策方面，基本面趋势决定了四季度支持性的货币政策、稳中偏松的取向不变": {"topic": "“宏观经济”", "similarity": 0.5410770773887634, "prompt": "新闻文本是“华泰证券指出，货币政策方面，基本面趋势决定了四季度支持性的货币政策、稳中偏松的取向不变”，包含的情绪词典是：恒定的/不变的(constant):0.05,稳定的/稳固的(stable):0.5"}, "四季度降息落地概率不小，三季度末是降准的敏感时点": {"topic": "“宏观经济”", "similarity": 0.5784881114959717, "prompt": "新闻文本是“四季度降息落地概率不小，三季度末是降准的敏感时点”，包含的情绪词典是：季度/四分之一(quarter):0.0,降级/降低评级(downgrade):-0.6"}, "不过，金融防风险是硬约束，央行对长期利率的管控态度预计还需要契机松动": {"topic": "“金融”", "similarity": 0.5468117594718933, "prompt": "新闻文本是“不过，金融防风险是硬约束，央行对长期利率的管控态度预计还需要契机松动”，包含的情绪词典是：风险(risk):-0.4,调控性的/监管性的(regulative):0.0"}, "关注央行管控长期利率的可能措施，包括买卖债、临时隔夜正回购等": {"topic": "“金融”", "similarity": 0.5152862071990967, "prompt": "新闻文本是“关注央行管控长期利率的可能措施，包括买卖债、临时隔夜正回购等”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,监管的/调控的(regulatory):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -2753,12 +2729,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月30日，科创100指数ETF(588030.SH)收涨1.49%，成交3.21亿元", "news_prompt2": "净流入4698.90万元（净申购份额*单位净值），居可比基金首位", "news_prompt3": "拉长时间看，该基金近30个交易日有20天资金净流入，合计吸金3.70亿元，居可比基金第一", "news_prompt4": "资金流入也助力了份额的提升，该基金最新份额较前一日增加6900.00万份，突破72.00亿份，居可比基金第一", "news_prompt5": "与此同时，该基金最新规模突破49.00亿元，居可比基金首位", "news_prompt6": "科创100指数ETF(588030.SH)，场外联接(A：019857", "news_prompt7": "C：019858)", "news_prompt8": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "2024年8月30日，科创100指数ETF(588030.SH)收涨1.49%，成交3.21亿元", "news_prompt2": "净流入4698.90万元（净申购份额*单位净值），居可比基金首位", "news_prompt3": "拉长时间看，该基金近30个交易日有20天资金净流入，合计吸金3.70亿元，居可比基金第一", "news_prompt4": "资金流入也助力了份额的提升，该基金最新份额较前一日增加6900.00万份，突破72.00亿份，居可比基金第一", "news_prompt5": "与此同时，该基金最新规模突破49.00亿元，居可比基金首位", "news_prompt6": "科创100指数ETF(588030.SH)，场外联接(A：019857", "news_prompt7": "C：019858)"}</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>{"2024年8月30日，科创100指数ETF(588030.SH)收涨1.49%，成交3.21亿元": {"topic": "“金融”", "similarity": 0.5303364396095276, "prompt": "新闻文本是“2024年8月30日，科创100指数ETF(588030.SH)收涨1.49%，成交3.21亿元”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "净流入4698.90万元（净申购份额*单位净值），居可比基金首位": {"topic": "“金融”", "similarity": 0.538465678691864, "prompt": "新闻文本是“净流入4698.90万元（净申购份额*单位净值），居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,投资/投入(invest):0.3"}, "拉长时间看，该基金近30个交易日有20天资金净流入，合计吸金3.70亿元，居可比基金第一": {"topic": "“金融”", "similarity": 0.5481926202774048, "prompt": "新闻文本是“拉长时间看，该基金近30个交易日有20天资金净流入，合计吸金3.70亿元，居可比基金第一”，包含的情绪词典是：相当大的/可观的(considerable):0.3,基金/资金(fund):0.1"}, "资金流入也助力了份额的提升，该基金最新份额较前一日增加6900.00万份，突破72.00亿份，居可比基金第一": {"topic": "“金融”", "similarity": 0.5675606727600098, "prompt": "新闻文本是“资金流入也助力了份额的提升，该基金最新份额较前一日增加6900.00万份，突破72.00亿份，居可比基金第一”，包含的情绪词典是：部分/份额(portion):0.0,基金/资金(fund):0.1"}, "与此同时，该基金最新规模突破49.00亿元，居可比基金首位": {"topic": "“金融”", "similarity": 0.47515714168548584, "prompt": "新闻文本是“与此同时，该基金最新规模突破49.00亿元，居可比基金首位”，包含的情绪词典是：相当大的/可观的(sizeable):0.0,基金/资金(fund):0.1"}, "科创100指数ETF(588030.SH)，场外联接(A：019857": {"topic": "“金融”", "similarity": 0.5231569409370422, "prompt": "新闻文本是“科创100指数ETF(588030.SH)，场外联接(A：019857”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeouts):-0.2"}, "C：019858)": {"topic": "“金融”", "similarity": 0.4339252710342407, "prompt": "新闻文本是“C：019858)”，包含的情绪词典是：事故/意外(accident):-0.3,网络犯罪(cybercrimes):-0.8"}}</t>
+          <t>{"2024年8月30日，科创100指数ETF(588030.SH)收涨1.49%，成交3.21亿元": {"topic": "“金融”", "similarity": 0.5303367376327515, "prompt": "新闻文本是“2024年8月30日，科创100指数ETF(588030.SH)收涨1.49%，成交3.21亿元”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "净流入4698.90万元（净申购份额*单位净值），居可比基金首位": {"topic": "“金融”", "similarity": 0.5384656190872192, "prompt": "新闻文本是“净流入4698.90万元（净申购份额*单位净值），居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,投资/投入(invest):0.3"}, "拉长时间看，该基金近30个交易日有20天资金净流入，合计吸金3.70亿元，居可比基金第一": {"topic": "“金融”", "similarity": 0.5481927394866943, "prompt": "新闻文本是“拉长时间看，该基金近30个交易日有20天资金净流入，合计吸金3.70亿元，居可比基金第一”，包含的情绪词典是：相当大的/可观的(considerable):0.3,基金/资金(fund):0.1"}, "资金流入也助力了份额的提升，该基金最新份额较前一日增加6900.00万份，突破72.00亿份，居可比基金第一": {"topic": "“金融”", "similarity": 0.5675607919692993, "prompt": "新闻文本是“资金流入也助力了份额的提升，该基金最新份额较前一日增加6900.00万份，突破72.00亿份，居可比基金第一”，包含的情绪词典是：部分/份额(portion):0.0,基金/资金(fund):0.1"}, "与此同时，该基金最新规模突破49.00亿元，居可比基金首位": {"topic": "“金融”", "similarity": 0.47515738010406494, "prompt": "新闻文本是“与此同时，该基金最新规模突破49.00亿元，居可比基金首位”，包含的情绪词典是：相当大的/可观的(sizeable):0.0,基金/资金(fund):0.1"}, "科创100指数ETF(588030.SH)，场外联接(A：019857": {"topic": "“金融”", "similarity": 0.523157000541687, "prompt": "新闻文本是“科创100指数ETF(588030.SH)，场外联接(A：019857”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeouts):-0.2"}, "C：019858)": {"topic": "“金融”", "similarity": 0.4339253306388855, "prompt": "新闻文本是“C：019858)”，包含的情绪词典是：事故/意外(accident):-0.3,网络犯罪(cybercrimes):-0.8"}}</t>
         </is>
       </c>
     </row>
@@ -2804,12 +2780,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "随着中秋节的临近，白酒迎来下半年的第一个旺季，消费市场逐渐活跃，名酒产品的终端价格也格外受关注", "news_prompt2": "根据南都湾财社-酒水新消费指数课题组记者整理发布的第三十三期《湾区酒价》，近期以来，广州、深圳、东莞等地不少线下商超都开启了酒水促销活动，线上平台的折扣力度也比较大，部门名酒产品的到手价格比平时更加优惠", "news_prompt3": "因此，本期飞天茅台、第八代五粮液等高端名酒的市场零售均价较上期有所下降，其中飞天茅台总体均价下降约200元", "news_prompt4": "降价促销也增加了一部分消费者的购买欲，从实地走访情况来看，广州、东莞有渠道“严重缺货”，也有商超在近期对多款名酒产品进行补货，节前白酒消费氛围向好", "news_prompt5": "广州：飞天茅台均价下降近百元，多家商超对名酒产品进行补货　　本期广州的白酒价格监控中，市场零售均价波动较为明显的是飞天茅台，均价由上期的2956元下降至本期的2871元，下降幅度超80元", "news_prompt6": "从具体渠道来看，本期飞天茅台在广州ole超市的售价为3099元，上期售价为3699元，直降600元", "news_prompt7": "在京东酒世界的售价为2890元，相比上期下降了100元", "news_prompt8": "但在经销商渠道，该产品的售价则出现一定上涨", "news_prompt9": "有酒商表示，近期临近中秋，飞天茅台的需求量有所提升，价格也会有相应的上调", "news_prompt10": "在广州多家商超及线上零售平台，南都湾财社-酒水新消费指数课题组发现，名酒零售价格以下调的趋势为主", "news_prompt11": "比如第八代五粮液在广州京东酒世界的价格由上期的979元下降至本期的949元，在ole的售价也由上期的1299元降至1189元", "news_prompt12": "青花郎在盒马的售价由上期的1190元降至本期的1090元", "news_prompt13": "国窖1573 在永旺的售价由上期的1099元降至本期的1049元", "news_prompt14": "君品习酒在永旺的售价近期更是大跳水，由1099元降至899元", "news_prompt15": "永旺超市工作人员表示，临近中秋节，白酒产品大多开展促销活动，优惠力度较大，比平时便宜大几百的都有", "news_prompt16": "此外，为迎合节前消费需求，近期广州多家商超也对此前出现断货的多款名酒产品进行了补货，总体来说近期出售的白酒产品品类选择更加多样", "news_prompt17": "深圳：临近中秋促销，部分名酒价格回落　　相比上期统计数据，在本期《湾区酒价》中，部分酒水的价格出现了不同程度的回落，其中降幅较为明显的为飞天茅台和第八代五粮液，而君品习酒、青花郎、国窖1573等则是有少量价格波动", "news_prompt18": "按照均价计算，本期飞天茅台在深圳的零售均价为2996元/瓶，相比上一期均价有所下跌，究其原因，主要是上期提价的华润ole报价出现回落，其价格降低至3099元/瓶，而在其他渠道方面，华润万家和山姆这一渠道显示缺货或无标价，同时京东酒世界深圳，对飞天茅台的价格标为2890元/瓶，与广州、东莞渠道同价", "news_prompt19": "第八代五粮液方面，本期均价为1091.3元/瓶，分渠道来看，京东酒世界、朴朴和华润万家，对该产品报价低于1000元/瓶，而其他渠道对产品报价坚持在1000元/瓶以上，其中华致酒行方面仍坚持1499元/瓶", "news_prompt20": "当然在部分产品均价下跌同期，有部分产品价格则是回调，例如洋河梦之蓝M6+，其均价为792.2元/瓶，比上期提升约20元，相比其他城市渠道，梦之蓝M6+在深圳渠道的报价均在750元/瓶以上，这拉高了产品的均价表现", "news_prompt21": "对于部分处于300元至500元价格带的产品，在本期酒价统计中均有一定程度的回落，例如国台国标酒、剑南春水晶剑、汾酒青花20等，均价下跌幅度在20元至40元左右", "news_prompt22": "部分次高端产品方面，古井贡古20均价与上一期持平，为633元/瓶，原因在于该酒款在深圳仅在1919及京东酒世界供货，其他渠道均未见踪迹", "news_prompt23": "另外，金沙摘要本期录得均价为629元/瓶，呈个位数下跌", "news_prompt24": "整体来看，随着中秋假期临近，降价促销、部分渠道断货等，均是本期深圳终端产品零售均价降价的主要原因，行业分析预判，随着中秋清库存需求增大，部分产品的零售价或进一步下调", "news_prompt25": "东莞：零售均价有回落，有渠道“严重缺货”　　与广州、深圳等市场相比，本期东莞市场的酒价同样出现价格回落的情况，整体来看，一线名酒的零售均价都有不同程度的下降，不过与广州、深圳情况不同的是，东莞有渠道出现较为明显的“售罄”“缺货”现象", "news_prompt26": "例如东莞的叮咚买菜渠道，在本期酒价中仅剩下飞天茅台与第八代五粮液有零售报价，其他产品均是显示为“缺货”", "news_prompt27": "类似的情况也出现在东莞华润超市和大润发，东莞华润超市有16款产品被售罄，而大润发东莞则是有11款产品显示缺货", "news_prompt28": "作为粤港澳大湾区酒水消费主阵地之一，中秋假期前夕东莞酒水市场的火热略超出市场预期，部分产品存在降价促销的情况，例如洋河梦之蓝M6+，在东莞的京东酒世界渠道报价为699元/瓶，这是除广州外，该产品首次在外市零售价低于700元/瓶的情况", "news_prompt29": "但与此同时，部分产品则是表现为挺价，例如剑南春水晶剑，其在东莞每个销售终端的零售价，普遍在470元/瓶以上，最低的价格仅为439元/瓶", "news_prompt30": "第八代五粮液价格表现同样坚"}</t>
+          <t>{"news_prompt1": "随着中秋节的临近，白酒迎来下半年的第一个旺季，消费市场逐渐活跃，名酒产品的终端价格也格外受关注", "news_prompt2": "因此，本期飞天茅台、第八代五粮液等高端名酒的市场零售均价较上期有所下降，其中飞天茅台总体均价下降约200元", "news_prompt3": "降价促销也增加了一部分消费者的购买欲，从实地走访情况来看，广州、东莞有渠道“严重缺货”，也有商超在近期对多款名酒产品进行补货，节前白酒消费氛围向好", "news_prompt4": "从具体渠道来看，本期飞天茅台在广州ole超市的售价为3099元，上期售价为3699元，直降600元", "news_prompt5": "在京东酒世界的售价为2890元，相比上期下降了100元", "news_prompt6": "但在经销商渠道，该产品的售价则出现一定上涨", "news_prompt7": "有酒商表示，近期临近中秋，飞天茅台的需求量有所提升，价格也会有相应的上调", "news_prompt8": "在广州多家商超及线上零售平台，南都湾财社-酒水新消费指数课题组发现，名酒零售价格以下调的趋势为主", "news_prompt9": "比如第八代五粮液在广州京东酒世界的价格由上期的979元下降至本期的949元，在ole的售价也由上期的1299元降至1189元", "news_prompt10": "青花郎在盒马的售价由上期的1190元降至本期的1090元", "news_prompt11": "国窖1573 在永旺的售价由上期的1099元降至本期的1049元", "news_prompt12": "君品习酒在永旺的售价近期更是大跳水，由1099元降至899元", "news_prompt13": "此外，为迎合节前消费需求，近期广州多家商超也对此前出现断货的多款名酒产品进行了补货，总体来说近期出售的白酒产品品类选择更加多样", "news_prompt14": "整体来看，随着中秋假期临近，降价促销、部分渠道断货等，均是本期深圳终端产品零售均价降价的主要原因，行业分析预判，随着中秋清库存需求增大，部分产品的零售价或进一步下调", "news_prompt15": "例如东莞的叮咚买菜渠道，在本期酒价中仅剩下飞天茅台与第八代五粮液有零售报价，其他产品均是显示为“缺货”", "news_prompt16": "类似的情况也出现在东莞华润超市和大润发，东莞华润超市有16款产品被售罄，而大润发东莞则是有11款产品显示缺货", "news_prompt17": "但与此同时，部分产品则是表现为挺价，例如剑南春水晶剑，其在东莞每个销售终端的零售价，普遍在470元/瓶以上，最低的价格仅为439元/瓶"}</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>{"随着中秋节的临近，白酒迎来下半年的第一个旺季，消费市场逐渐活跃，名酒产品的终端价格也格外受关注": {"topic": "“消费”", "similarity": 0.6065444350242615, "prompt": "新闻文本是“随着中秋节的临近，白酒迎来下半年的第一个旺季，消费市场逐渐活跃，名酒产品的终端价格也格外受关注”，包含的情绪词典是：酒精/乙醇(alcohol):0.0,消费者/用户(consumer):0.0"}, "根据南都湾财社-酒水新消费指数课题组记者整理发布的第三十三期《湾区酒价》，近期以来，广州、深圳、东莞等地不少线下商超都开启了酒水促销活动，线上平台的折扣力度也比较大，部门名酒产品的到手价格比平时更加优惠": {"topic": "“消费”", "similarity": 0.6276609897613525}, "因此，本期飞天茅台、第八代五粮液等高端名酒的市场零售均价较上期有所下降，其中飞天茅台总体均价下降约200元": {"topic": "“消费”", "similarity": 0.5716056823730469, "prompt": "新闻文本是“因此，本期飞天茅台、第八代五粮液等高端名酒的市场零售均价较上期有所下降，其中飞天茅台总体均价下降约200元”，包含的情绪词典是：减价/降价(markdown):0.0,下跌/下降(fall):-0.6"}, "降价促销也增加了一部分消费者的购买欲，从实地走访情况来看，广州、东莞有渠道“严重缺货”，也有商超在近期对多款名酒产品进行补货，节前白酒消费氛围向好": {"topic": "“消费”", "similarity": 0.6189886331558228, "prompt": "新闻文本是“降价促销也增加了一部分消费者的购买欲，从实地走访情况来看，广州、东莞有渠道“严重缺货”，也有商超在近期对多款名酒产品进行补货，节前白酒消费氛围向好”，包含的情绪词典是：减价/降价(markdown):0.0,缺口/亏空(shortfall):-0.5"}, "广州：飞天茅台均价下降近百元，多家商超对名酒产品进行补货　　本期广州的白酒价格监控中，市场零售均价波动较为明显的是飞天茅台，均价由上期的2956元下降至本期的2871元，下降幅度超80元": {"topic": "“消费”", "similarity": 0.5912945866584778}, "从具体渠道来看，本期飞天茅台在广州ole超市的售价为3099元，上期售价为3699元，直降600元": {"topic": "“消费”", "similarity": 0.5300228595733643, "prompt": "新闻文本是“从具体渠道来看，本期飞天茅台在广州ole超市的售价为3099元，上期售价为3699元，直降600元”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercuts):-0.3"}, "在京东酒世界的售价为2890元，相比上期下降了100元": {"topic": "“消费”", "similarity": 0.4663962125778198, "prompt": "新闻文本是“在京东酒世界的售价为2890元，相比上期下降了100元”，包含的情绪词典是：减价/降价(markdown):0.0,下跌/下降(fall):-0.6"}, "但在经销商渠道，该产品的售价则出现一定上涨": {"topic": "“通货膨胀”", "similarity": 0.4240633249282837, "prompt": "新闻文本是“但在经销商渠道，该产品的售价则出现一定上涨”，包含的情绪词典是：上升/上涨(rise):0.5,多收费/索价过高(overcharge):-0.4"}, "有酒商表示，近期临近中秋，飞天茅台的需求量有所提升，价格也会有相应的上调": {"topic": "“消费”", "similarity": 0.4808644652366638, "prompt": "新闻文本是“有酒商表示，近期临近中秋，飞天茅台的需求量有所提升，价格也会有相应的上调”，包含的情绪词典是：上升/上涨(rise):0.5,上升的/占优势的(ascendant):0.3"}, "在广州多家商超及线上零售平台，南都湾财社-酒水新消费指数课题组发现，名酒零售价格以下调的趋势为主": {"topic": "“消费”", "similarity": 0.6249932050704956, "prompt": "新闻文本是“在广州多家商超及线上零售平台，南都湾财社-酒水新消费指数课题组发现，名酒零售价格以下调的趋势为主”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercut):-0.3"}, "比如第八代五粮液在广州京东酒世界的价格由上期的979元下降至本期的949元，在ole的售价也由上期的1299元降至1189元": {"topic": "“消费”", "similarity": 0.5424414277076721, "prompt": "新闻文本是“比如第八代五粮液在广州京东酒世界的价格由上期的979元下降至本期的949元，在ole的售价也由上期的1299元降至1189元”，包含的情绪词典是：减价/降价(markdown):0.0,下跌/下降(fall):-0.6"}, "青花郎在盒马的售价由上期的1190元降至本期的1090元": {"topic": "“消费”", "similarity": 0.43189480900764465, "prompt": "新闻文本是“青花郎在盒马的售价由上期的1190元降至本期的1090元”，包含的情绪词典是：减价/降价(markdown):0.0,贬值/减值(devaluation):-0.5"}, "国窖1573 在永旺的售价由上期的1099元降至本期的1049元": {"topic": "“消费”", "similarity": 0.4745350480079651, "prompt": "新闻文本是“国窖1573 在永旺的售价由上期的1099元降至本期的1049元”，包含的情绪词典是：减价/降价(markdown):0.0,减少/降低(reduction):-0.4"}, "君品习酒在永旺的售价近期更是大跳水，由1099元降至899元": {"topic": "“消费”", "similarity": 0.4805128872394562, "prompt": "新闻文本是“君品习酒在永旺的售价近期更是大跳水，由1099元降至899元”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercut):-0.3"}, "永旺超市工作人员表示，临近中秋节，白酒产品大多开展促销活动，优惠力度较大，比平时便宜大几百的都有": {"topic": "“消费”", "similarity": 0.5370767116546631}, "此外，为迎合节前消费需求，近期广州多家商超也对此前出现断货的多款名酒产品进行了补货，总体来说近期出售的白酒产品品类选择更加多样": {"topic": "“消费”", "similarity": 0.5840238332748413, "prompt": "新闻文本是“此外，为迎合节前消费需求，近期广州多家商超也对此前出现断货的多款名酒产品进行了补货，总体来说近期出售的白酒产品品类选择更加多样”，包含的情绪词典是：商品/货物(commodity):0.0,供应过剩(oversupply):-0.2"}, "深圳：临近中秋促销，部分名酒价格回落　　相比上期统计数据，在本期《湾区酒价》中，部分酒水的价格出现了不同程度的回落，其中降幅较为明显的为飞天茅台和第八代五粮液，而君品习酒、青花郎、国窖1573等则是有少量价格波动": {"topic": "“消费”", "similarity": 0.5726386308670044}, "按照均价计算，本期飞天茅台在深圳的零售均价为2996元/瓶，相比上一期均价有所下跌，究其原因，主要是上期提价的华润ole报价出现回落，其价格降低至3099元/瓶，而在其他渠道方面，华润万家和山姆这一渠道显示缺货或无标价，同时京东酒世界深圳，对飞天茅台的价格标为2890元/瓶，与广州、东莞渠道同价": {"topic": "“消费”", "similarity": 0.544425368309021}, "第八代五粮液方面，本期均价为1091.3元/瓶，分渠道来看，京东酒世界、朴朴和华润万家，对该产品报价低于1000元/瓶，而其他渠道对产品报价坚持在1000元/瓶以上，其中华致酒行方面仍坚持1499元/瓶": {"topic": "“消费”", "similarity": 0.5081664323806763}, "当然在部分产品均价下跌同期，有部分产品价格则是回调，例如洋河梦之蓝M6+，其均价为792.2元/瓶，比上期提升约20元，相比其他城市渠道，梦之蓝M6+在深圳渠道的报价均在750元/瓶以上，这拉高了产品的均价表现": {"topic": "“消费”", "similarity": 0.5688854455947876}, "对于部分处于300元至500元价格带的产品，在本期酒价统计中均有一定程度的回落，例如国台国标酒、剑南春水晶剑、汾酒青花20等，均价下跌幅度在20元至40元左右": {"topic": "“消费”", "similarity": 0.5971986055374146}, "部分次高端产品方面，古井贡古20均价与上一期持平，为633元/瓶，原因在于该酒款在深圳仅在1919及京东酒世界供货，其他渠道均未见踪迹": {"topic": "“消费”", "similarity": 0.5320715308189392}, "整体来看，随着中秋假期临近，降价促销、部分渠道断货等，均是本期深圳终端产品零售均价降价的主要原因，行业分析预判，随着中秋清库存需求增大，部分产品的零售价或进一步下调": {"topic": "“消费”", "similarity": 0.6015979051589966, "prompt": "新闻文本是“整体来看，随着中秋假期临近，降价促销、部分渠道断货等，均是本期深圳终端产品零售均价降价的主要原因，行业分析预判，随着中秋清库存需求增大，部分产品的零售价或进一步下调”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercuts):-0.3"}, "东莞：零售均价有回落，有渠道“严重缺货”　　与广州、深圳等市场相比，本期东莞市场的酒价同样出现价格回落的情况，整体来看，一线名酒的零售均价都有不同程度的下降，不过与广州、深圳情况不同的是，东莞有渠道出现较为明显的“售罄”“缺货”现象": {"topic": "“消费”", "similarity": 0.5877647399902344}, "例如东莞的叮咚买菜渠道，在本期酒价中仅剩下飞天茅台与第八代五粮液有零售报价，其他产品均是显示为“缺货”": {"topic": "“消费”", "similarity": 0.5669139623641968, "prompt": "新闻文本是“例如东莞的叮咚买菜渠道，在本期酒价中仅剩下飞天茅台与第八代五粮液有零售报价，其他产品均是显示为“缺货””，包含的情绪词典是：滞销(unsellable):-0.4,无销路的/滞销的(unmarketable):-0.5"}, "类似的情况也出现在东莞华润超市和大润发，东莞华润超市有16款产品被售罄，而大润发东莞则是有11款产品显示缺货": {"topic": "“消费”", "similarity": 0.584662675857544, "prompt": "新闻文本是“类似的情况也出现在东莞华润超市和大润发，东莞华润超市有16款产品被售罄，而大润发东莞则是有11款产品显示缺货”，包含的情绪词典是：滞销(unsellable):-0.4,无销路的/卖不掉的(unsaleable):-0.3"}, "作为粤港澳大湾区酒水消费主阵地之一，中秋假期前夕东莞酒水市场的火热略超出市场预期，部分产品存在降价促销的情况，例如洋河梦之蓝M6+，在东莞的京东酒世界渠道报价为699元/瓶，这是除广州外，该产品首次在外市零售价低于700元/瓶的情况": {"topic": "“消费”", "similarity": 0.555825412273407}, "但与此同时，部分产品则是表现为挺价，例如剑南春水晶剑，其在东莞每个销售终端的零售价，普遍在470元/瓶以上，最低的价格仅为439元/瓶": {"topic": "“消费”", "similarity": 0.5321160554885864, "prompt": "新闻文本是“但与此同时，部分产品则是表现为挺价，例如剑南春水晶剑，其在东莞每个销售终端的零售价，普遍在470元/瓶以上，最低的价格仅为439元/瓶”，包含的情绪词典是：削价/低价出售(undercut):-0.3,滞销(unsellable):-0.4"}}</t>
+          <t>{"随着中秋节的临近，白酒迎来下半年的第一个旺季，消费市场逐渐活跃，名酒产品的终端价格也格外受关注": {"topic": "“消费”", "similarity": 0.6065444946289062, "prompt": "新闻文本是“随着中秋节的临近，白酒迎来下半年的第一个旺季，消费市场逐渐活跃，名酒产品的终端价格也格外受关注”，包含的情绪词典是：酒精/乙醇(alcohol):0.0,消费者/用户(consumer):0.0"}, "因此，本期飞天茅台、第八代五粮液等高端名酒的市场零售均价较上期有所下降，其中飞天茅台总体均价下降约200元": {"topic": "“消费”", "similarity": 0.5716058015823364, "prompt": "新闻文本是“因此，本期飞天茅台、第八代五粮液等高端名酒的市场零售均价较上期有所下降，其中飞天茅台总体均价下降约200元”，包含的情绪词典是：减价/降价(markdown):0.0,下跌/下降(fall):-0.6"}, "降价促销也增加了一部分消费者的购买欲，从实地走访情况来看，广州、东莞有渠道“严重缺货”，也有商超在近期对多款名酒产品进行补货，节前白酒消费氛围向好": {"topic": "“消费”", "similarity": 0.6189886927604675, "prompt": "新闻文本是“降价促销也增加了一部分消费者的购买欲，从实地走访情况来看，广州、东莞有渠道“严重缺货”，也有商超在近期对多款名酒产品进行补货，节前白酒消费氛围向好”，包含的情绪词典是：减价/降价(markdown):0.0,缺口/亏空(shortfall):-0.5"}, "从具体渠道来看，本期飞天茅台在广州ole超市的售价为3099元，上期售价为3699元，直降600元": {"topic": "“消费”", "similarity": 0.530022919178009, "prompt": "新闻文本是“从具体渠道来看，本期飞天茅台在广州ole超市的售价为3099元，上期售价为3699元，直降600元”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercuts):-0.3"}, "在京东酒世界的售价为2890元，相比上期下降了100元": {"topic": "“消费”", "similarity": 0.46639639139175415, "prompt": "新闻文本是“在京东酒世界的售价为2890元，相比上期下降了100元”，包含的情绪词典是：减价/降价(markdown):0.0,下跌/下降(fall):-0.6"}, "但在经销商渠道，该产品的售价则出现一定上涨": {"topic": "“通货膨胀”", "similarity": 0.42406362295150757, "prompt": "新闻文本是“但在经销商渠道，该产品的售价则出现一定上涨”，包含的情绪词典是：上升/上涨(rise):0.5,多收费/索价过高(overcharge):-0.4"}, "有酒商表示，近期临近中秋，飞天茅台的需求量有所提升，价格也会有相应的上调": {"topic": "“消费”", "similarity": 0.48086464405059814, "prompt": "新闻文本是“有酒商表示，近期临近中秋，飞天茅台的需求量有所提升，价格也会有相应的上调”，包含的情绪词典是：上升/上涨(rise):0.5,上升的/占优势的(ascendant):0.3"}, "在广州多家商超及线上零售平台，南都湾财社-酒水新消费指数课题组发现，名酒零售价格以下调的趋势为主": {"topic": "“消费”", "similarity": 0.6249933242797852, "prompt": "新闻文本是“在广州多家商超及线上零售平台，南都湾财社-酒水新消费指数课题组发现，名酒零售价格以下调的趋势为主”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercut):-0.3"}, "比如第八代五粮液在广州京东酒世界的价格由上期的979元下降至本期的949元，在ole的售价也由上期的1299元降至1189元": {"topic": "“消费”", "similarity": 0.5424415469169617, "prompt": "新闻文本是“比如第八代五粮液在广州京东酒世界的价格由上期的979元下降至本期的949元，在ole的售价也由上期的1299元降至1189元”，包含的情绪词典是：减价/降价(markdown):0.0,下跌/下降(fall):-0.6"}, "青花郎在盒马的售价由上期的1190元降至本期的1090元": {"topic": "“消费”", "similarity": 0.43189477920532227, "prompt": "新闻文本是“青花郎在盒马的售价由上期的1190元降至本期的1090元”，包含的情绪词典是：减价/降价(markdown):0.0,贬值/减值(devaluation):-0.5"}, "国窖1573 在永旺的售价由上期的1099元降至本期的1049元": {"topic": "“消费”", "similarity": 0.47453513741493225, "prompt": "新闻文本是“国窖1573 在永旺的售价由上期的1099元降至本期的1049元”，包含的情绪词典是：减价/降价(markdown):0.0,减少/降低(reduction):-0.4"}, "君品习酒在永旺的售价近期更是大跳水，由1099元降至899元": {"topic": "“消费”", "similarity": 0.4805130064487457, "prompt": "新闻文本是“君品习酒在永旺的售价近期更是大跳水，由1099元降至899元”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercut):-0.3"}, "此外，为迎合节前消费需求，近期广州多家商超也对此前出现断货的多款名酒产品进行了补货，总体来说近期出售的白酒产品品类选择更加多样": {"topic": "“消费”", "similarity": 0.5840239524841309, "prompt": "新闻文本是“此外，为迎合节前消费需求，近期广州多家商超也对此前出现断货的多款名酒产品进行了补货，总体来说近期出售的白酒产品品类选择更加多样”，包含的情绪词典是：商品/货物(commodity):0.0,供应过剩(oversupply):-0.2"}, "整体来看，随着中秋假期临近，降价促销、部分渠道断货等，均是本期深圳终端产品零售均价降价的主要原因，行业分析预判，随着中秋清库存需求增大，部分产品的零售价或进一步下调": {"topic": "“消费”", "similarity": 0.6015980243682861, "prompt": "新闻文本是“整体来看，随着中秋假期临近，降价促销、部分渠道断货等，均是本期深圳终端产品零售均价降价的主要原因，行业分析预判，随着中秋清库存需求增大，部分产品的零售价或进一步下调”，包含的情绪词典是：减价/降价(markdown):0.0,削价/低价出售(undercuts):-0.3"}, "例如东莞的叮咚买菜渠道，在本期酒价中仅剩下飞天茅台与第八代五粮液有零售报价，其他产品均是显示为“缺货”": {"topic": "“消费”", "similarity": 0.5669140815734863, "prompt": "新闻文本是“例如东莞的叮咚买菜渠道，在本期酒价中仅剩下飞天茅台与第八代五粮液有零售报价，其他产品均是显示为“缺货””，包含的情绪词典是：滞销(unsellable):-0.4,无销路的/滞销的(unmarketable):-0.5"}, "类似的情况也出现在东莞华润超市和大润发，东莞华润超市有16款产品被售罄，而大润发东莞则是有11款产品显示缺货": {"topic": "“消费”", "similarity": 0.5846627950668335, "prompt": "新闻文本是“类似的情况也出现在东莞华润超市和大润发，东莞华润超市有16款产品被售罄，而大润发东莞则是有11款产品显示缺货”，包含的情绪词典是：滞销(unsellable):-0.4,无销路的/卖不掉的(unsaleable):-0.3"}, "但与此同时，部分产品则是表现为挺价，例如剑南春水晶剑，其在东莞每个销售终端的零售价，普遍在470元/瓶以上，最低的价格仅为439元/瓶": {"topic": "“消费”", "similarity": 0.5321162343025208, "prompt": "新闻文本是“但与此同时，部分产品则是表现为挺价，例如剑南春水晶剑，其在东莞每个销售终端的零售价，普遍在470元/瓶以上，最低的价格仅为439元/瓶”，包含的情绪词典是：削价/低价出售(undercut):-0.3,滞销(unsellable):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2831,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "华安证券09月02日发布研报称，给予亚辉龙（688575.SH，最新价：20.31元）买入评级", "news_prompt2": "评级理由主要包括：1）非新冠自产持续高增长，海外增速高于国内", "news_prompt3": "2）自免带动常规逻辑兑现，三大常规试剂同比增长超50%", "news_prompt4": "3）创新为本+出海加速，形成公司高增长核心驱动力", "news_prompt5": "风险提示：新增装机不及预期风险、海外拓展不及预期风险、市场竞争加剧风险", "news_prompt6": "AI点评：亚辉龙近一个月获得3份券商研报关注，买入1家，平均目标价为25.45元，与最新价20.31元相比，高5.14元，目标均价涨幅25.31%", "news_prompt7": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "评级理由主要包括：1）非新冠自产持续高增长，海外增速高于国内", "news_prompt2": "2）自免带动常规逻辑兑现，三大常规试剂同比增长超50%", "news_prompt3": "3）创新为本+出海加速，形成公司高增长核心驱动力"}</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>{"华安证券09月02日发布研报称，给予亚辉龙（688575.SH，最新价：20.31元）买入评级": {"topic": "“金融”", "similarity": 0.47006893157958984}, "评级理由主要包括：1）非新冠自产持续高增长，海外增速高于国内": {"topic": "“生产投资”", "similarity": 0.5018904805183411, "prompt": "新闻文本是“评级理由主要包括：1）非新冠自产持续高增长，海外增速高于国内”，包含的情绪词典是：多产的/富有成效的(productive):0.7,上升的/占优势的(ascendant):0.3"}, "2）自免带动常规逻辑兑现，三大常规试剂同比增长超50%": {"topic": "“金融”", "similarity": 0.42435818910598755, "prompt": "新闻文本是“2）自免带动常规逻辑兑现，三大常规试剂同比增长超50%”，包含的情绪词典是：免除/豁免(exempt):0.0,赦免/免除(absolve):0.2"}, "3）创新为本+出海加速，形成公司高增长核心驱动力": {"topic": "“金融”", "similarity": 0.5480459332466125, "prompt": "新闻文本是“3）创新为本+出海加速，形成公司高增长核心驱动力”，包含的情绪词典是：创新/革新(innovation):0.7,创新/革新(innovate):0.6"}, "风险提示：新增装机不及预期风险、海外拓展不及预期风险、市场竞争加剧风险": {"topic": "“金融”", "similarity": 0.5434776544570923, "prompt": "新闻文本是“风险提示：新增装机不及预期风险、海外拓展不及预期风险、市场竞争加剧风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "AI点评：亚辉龙近一个月获得3份券商研报关注，买入1家，平均目标价为25.45元，与最新价20.31元相比，高5.14元，目标均价涨幅25.31%": {"topic": "“金融”", "similarity": 0.5549942851066589}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"评级理由主要包括：1）非新冠自产持续高增长，海外增速高于国内": {"topic": "“生产投资”", "similarity": 0.5018905401229858, "prompt": "新闻文本是“评级理由主要包括：1）非新冠自产持续高增长，海外增速高于国内”，包含的情绪词典是：多产的/富有成效的(productive):0.7,上升的/占优势的(ascendant):0.3"}, "2）自免带动常规逻辑兑现，三大常规试剂同比增长超50%": {"topic": "“金融”", "similarity": 0.4243583381175995, "prompt": "新闻文本是“2）自免带动常规逻辑兑现，三大常规试剂同比增长超50%”，包含的情绪词典是：免除/豁免(exempt):0.0,赦免/免除(absolve):0.2"}, "3）创新为本+出海加速，形成公司高增长核心驱动力": {"topic": "“金融”", "similarity": 0.5480460524559021, "prompt": "新闻文本是“3）创新为本+出海加速，形成公司高增长核心驱动力”，包含的情绪词典是：创新/革新(innovation):0.7,创新/革新(innovate):0.6"}}</t>
         </is>
       </c>
     </row>
@@ -2906,12 +2882,12 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，欧科亿(688308.SH)发布2024年中报", "news_prompt2": "公司营业总收入为5.79亿元，在已披露的同业公司中排名第97，较去年同报告期营业总收入增加4658.91万元，实现5年连续上涨，同比较去年同期上涨8.75%", "news_prompt3": "归母净利润为6009.42万元，在已披露的同业公司中排名第71，较去年同报告期归母净利润减少4833.79万元，同比较去年同期下降44.58%", "news_prompt4": "经营活动现金净流入为-1.07亿元，在已披露的同业公司中排名第213，较去年同报告期经营活动现金净流入减少6253.82万元", "news_prompt5": "公司最新资产负债率为31.95%，在已披露的同业公司中排名第121，较上季度资产负债率减少3.12个百分点，较去年同季度资产负债率增加3.86个百分点", "news_prompt6": "公司最新毛利率为26.14%，在已披露的同业公司中排名第132，较上季度毛利率增加1.06个百分点，较去年同季度毛利率减少6.51个百分点", "news_prompt7": "最新ROE为2.35%，在已披露的同业公司中排名第143，较去年同季度ROE减少1.94个百分点", "news_prompt8": "公司摊薄每股收益为0.38元，在已披露的同业公司中排名第51，较去年同报告期摊薄每股收益减少0.31元，同比较去年同期下降44.63%", "news_prompt9": "公司最新总资产周转率为0.15次，在已披露的同业公司中排名第183，较去年同季度总资产周转率减少0.01次，同比较去年同期下降4.77%", "news_prompt10": "最新存货周转率为0.80次，在已披露的同业公司中排名第163，较去年同季度存货周转率减少0.09次，同比较去年同期下降10.45%", "news_prompt11": "公司股东户数为5783户，前十大股东持股数量为8824.74万股，占总股本比例为55.58%", "news_prompt12": "前十大股东分别为袁美和、格林美股份有限公司、谭文清、乐清市德汇股权投资合伙企业(有限合伙)、南京精锐创业投资合伙企业(有限合伙)、通用技术创业投资有限公司-通用技术高端装备产业股权投资(桐乡)合伙企业(有限合伙)、广东粤科纵横融通创业投资合伙企业(有限合伙)、通用技术集团投资管理有限公司、马怀义、中国建设银行股份有限公司-中欧价值发现股票型证券投资基金，持股比例分别为15.92%、10.41%、9.04%、5.90%、5.13%、2.78%、1.93%、1.59%、1.55%、1.33%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为5.79亿元，在已披露的同业公司中排名第97，较去年同报告期营业总收入增加4658.91万元，实现5年连续上涨，同比较去年同期上涨8.75%", "news_prompt2": "归母净利润为6009.42万元，在已披露的同业公司中排名第71，较去年同报告期归母净利润减少4833.79万元，同比较去年同期下降44.58%", "news_prompt3": "经营活动现金净流入为-1.07亿元，在已披露的同业公司中排名第213，较去年同报告期经营活动现金净流入减少6253.82万元", "news_prompt4": "公司最新资产负债率为31.95%，在已披露的同业公司中排名第121，较上季度资产负债率减少3.12个百分点，较去年同季度资产负债率增加3.86个百分点", "news_prompt5": "公司最新毛利率为26.14%，在已披露的同业公司中排名第132，较上季度毛利率增加1.06个百分点，较去年同季度毛利率减少6.51个百分点", "news_prompt6": "公司摊薄每股收益为0.38元，在已披露的同业公司中排名第51，较去年同报告期摊薄每股收益减少0.31元，同比较去年同期下降44.63%", "news_prompt7": "公司最新总资产周转率为0.15次，在已披露的同业公司中排名第183，较去年同季度总资产周转率减少0.01次，同比较去年同期下降4.77%", "news_prompt8": "最新存货周转率为0.80次，在已披露的同业公司中排名第163，较去年同季度存货周转率减少0.09次，同比较去年同期下降10.45%", "news_prompt9": "公司股东户数为5783户，前十大股东持股数量为8824.74万股，占总股本比例为55.58%"}</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，欧科亿(688308.SH)发布2024年中报": {"topic": "“生产投资”", "similarity": 0.5168697237968445, "prompt": "新闻文本是“2024年8月31日，欧科亿(688308.SH)发布2024年中报”，包含的情绪词典是：欧元(euro):0.0,欧元区(eurozone):0.0"}, "公司营业总收入为5.79亿元，在已披露的同业公司中排名第97，较去年同报告期营业总收入增加4658.91万元，实现5年连续上涨，同比较去年同期上涨8.75%": {"topic": "“消费”", "similarity": 0.5431268215179443, "prompt": "新闻文本是“公司营业总收入为5.79亿元，在已披露的同业公司中排名第97，较去年同报告期营业总收入增加4658.91万元，实现5年连续上涨，同比较去年同期上涨8.75%”，包含的情绪词典是：上升/上涨(rise):0.5,公司的/企业的(corporate):0.0"}, "归母净利润为6009.42万元，在已披露的同业公司中排名第71，较去年同报告期归母净利润减少4833.79万元，同比较去年同期下降44.58%": {"topic": "“消费”", "similarity": 0.5170172452926636, "prompt": "新闻文本是“归母净利润为6009.42万元，在已披露的同业公司中排名第71，较去年同报告期归母净利润减少4833.79万元，同比较去年同期下降44.58%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为-1.07亿元，在已披露的同业公司中排名第213，较去年同报告期经营活动现金净流入减少6253.82万元": {"topic": "“金融”", "similarity": 0.527069628238678, "prompt": "新闻文本是“经营活动现金净流入为-1.07亿元，在已披露的同业公司中排名第213，较去年同报告期经营活动现金净流入减少6253.82万元”，包含的情绪词典是：营业额/周转(turnover):0.0,非流动性/缺乏流动性(illiquidity):-0.5"}, "公司最新资产负债率为31.95%，在已披露的同业公司中排名第121，较上季度资产负债率减少3.12个百分点，较去年同季度资产负债率增加3.86个百分点": {"topic": "“消费”", "similarity": 0.47670918703079224, "prompt": "新闻文本是“公司最新资产负债率为31.95%，在已披露的同业公司中排名第121，较上季度资产负债率减少3.12个百分点，较去年同季度资产负债率增加3.86个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,赤字/亏损(deficit):-0.6"}, "公司最新毛利率为26.14%，在已披露的同业公司中排名第132，较上季度毛利率增加1.06个百分点，较去年同季度毛利率减少6.51个百分点": {"topic": "“消费”", "similarity": 0.44969111680984497, "prompt": "新闻文本是“公司最新毛利率为26.14%，在已披露的同业公司中排名第132，较上季度毛利率增加1.06个百分点，较去年同季度毛利率减少6.51个百分点”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司摊薄每股收益为0.38元，在已披露的同业公司中排名第51，较去年同报告期摊薄每股收益减少0.31元，同比较去年同期下降44.63%": {"topic": "“金融”", "similarity": 0.46300020813941956, "prompt": "新闻文本是“公司摊薄每股收益为0.38元，在已披露的同业公司中排名第51，较去年同报告期摊薄每股收益减少0.31元，同比较去年同期下降44.63%”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新总资产周转率为0.15次，在已披露的同业公司中排名第183，较去年同季度总资产周转率减少0.01次，同比较去年同期下降4.77%": {"topic": "“消费”", "similarity": 0.4863094091415405, "prompt": "新闻文本是“公司最新总资产周转率为0.15次，在已披露的同业公司中排名第183，较去年同季度总资产周转率减少0.01次，同比较去年同期下降4.77%”，包含的情绪词典是：营业额/周转(turnover):0.0,季度地/按季度(quarterly):0.0"}, "最新存货周转率为0.80次，在已披露的同业公司中排名第163，较去年同季度存货周转率减少0.09次，同比较去年同期下降10.45%": {"topic": "“消费”", "similarity": 0.44661229848861694, "prompt": "新闻文本是“最新存货周转率为0.80次，在已披露的同业公司中排名第163，较去年同季度存货周转率减少0.09次，同比较去年同期下降10.45%”，包含的情绪词典是：营业额/周转(turnover):0.0,减少/降低(reduction):-0.4"}, "公司股东户数为5783户，前十大股东持股数量为8824.74万股，占总股本比例为55.58%": {"topic": "“金融”", "similarity": 0.48673808574676514, "prompt": "新闻文本是“公司股东户数为5783户，前十大股东持股数量为8824.74万股，占总股本比例为55.58%”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(firm):0.0"}, "前十大股东分别为袁美和、格林美股份有限公司、谭文清、乐清市德汇股权投资合伙企业(有限合伙)、南京精锐创业投资合伙企业(有限合伙)、通用技术创业投资有限公司-通用技术高端装备产业股权投资(桐乡)合伙企业(有限合伙)、广东粤科纵横融通创业投资合伙企业(有限合伙)、通用技术集团投资管理有限公司、马怀义、中国建设银行股份有限公司-中欧价值发现股票型证券投资基金，持股比例分别为15.92%、10.41%、9.04%、5.90%、5.13%、2.78%、1.93%、1.59%、1.55%、1.33%": {"topic": "“生产投资”", "similarity": 0.6524317860603333}}</t>
+          <t>{"公司营业总收入为5.79亿元，在已披露的同业公司中排名第97，较去年同报告期营业总收入增加4658.91万元，实现5年连续上涨，同比较去年同期上涨8.75%": {"topic": "“消费”", "similarity": 0.5431268811225891, "prompt": "新闻文本是“公司营业总收入为5.79亿元，在已披露的同业公司中排名第97，较去年同报告期营业总收入增加4658.91万元，实现5年连续上涨，同比较去年同期上涨8.75%”，包含的情绪词典是：上升/上涨(rise):0.5,公司的/企业的(corporate):0.0"}, "归母净利润为6009.42万元，在已披露的同业公司中排名第71，较去年同报告期归母净利润减少4833.79万元，同比较去年同期下降44.58%": {"topic": "“消费”", "similarity": 0.5170172452926636, "prompt": "新闻文本是“归母净利润为6009.42万元，在已披露的同业公司中排名第71，较去年同报告期归母净利润减少4833.79万元，同比较去年同期下降44.58%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为-1.07亿元，在已披露的同业公司中排名第213，较去年同报告期经营活动现金净流入减少6253.82万元": {"topic": "“金融”", "similarity": 0.5270697474479675, "prompt": "新闻文本是“经营活动现金净流入为-1.07亿元，在已披露的同业公司中排名第213，较去年同报告期经营活动现金净流入减少6253.82万元”，包含的情绪词典是：营业额/周转(turnover):0.0,非流动性/缺乏流动性(illiquidity):-0.5"}, "公司最新资产负债率为31.95%，在已披露的同业公司中排名第121，较上季度资产负债率减少3.12个百分点，较去年同季度资产负债率增加3.86个百分点": {"topic": "“消费”", "similarity": 0.476709246635437, "prompt": "新闻文本是“公司最新资产负债率为31.95%，在已披露的同业公司中排名第121，较上季度资产负债率减少3.12个百分点，较去年同季度资产负债率增加3.86个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,赤字/亏损(deficit):-0.6"}, "公司最新毛利率为26.14%，在已披露的同业公司中排名第132，较上季度毛利率增加1.06个百分点，较去年同季度毛利率减少6.51个百分点": {"topic": "“消费”", "similarity": 0.44969120621681213, "prompt": "新闻文本是“公司最新毛利率为26.14%，在已披露的同业公司中排名第132，较上季度毛利率增加1.06个百分点，较去年同季度毛利率减少6.51个百分点”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司摊薄每股收益为0.38元，在已披露的同业公司中排名第51，较去年同报告期摊薄每股收益减少0.31元，同比较去年同期下降44.63%": {"topic": "“金融”", "similarity": 0.4630002975463867, "prompt": "新闻文本是“公司摊薄每股收益为0.38元，在已披露的同业公司中排名第51，较去年同报告期摊薄每股收益减少0.31元，同比较去年同期下降44.63%”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新总资产周转率为0.15次，在已披露的同业公司中排名第183，较去年同季度总资产周转率减少0.01次，同比较去年同期下降4.77%": {"topic": "“消费”", "similarity": 0.4863094687461853, "prompt": "新闻文本是“公司最新总资产周转率为0.15次，在已披露的同业公司中排名第183，较去年同季度总资产周转率减少0.01次，同比较去年同期下降4.77%”，包含的情绪词典是：营业额/周转(turnover):0.0,季度地/按季度(quarterly):0.0"}, "最新存货周转率为0.80次，在已披露的同业公司中排名第163，较去年同季度存货周转率减少0.09次，同比较去年同期下降10.45%": {"topic": "“消费”", "similarity": 0.4466124176979065, "prompt": "新闻文本是“最新存货周转率为0.80次，在已披露的同业公司中排名第163，较去年同季度存货周转率减少0.09次，同比较去年同期下降10.45%”，包含的情绪词典是：营业额/周转(turnover):0.0,减少/降低(reduction):-0.4"}, "公司股东户数为5783户，前十大股东持股数量为8824.74万股，占总股本比例为55.58%": {"topic": "“金融”", "similarity": 0.4867381453514099, "prompt": "新闻文本是“公司股东户数为5783户，前十大股东持股数量为8824.74万股，占总股本比例为55.58%”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(firm):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -2957,12 +2933,12 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "国家发展改革委近日印发《教育强国基础设施建设工程(公共实训基地方向)中央预算内投资专项管理办法》", "news_prompt2": "其中提到，中央预算内投资对公共实训基地建设项目原则上按照东、中、西、东北地区（含根据国家相关政策享受中、西部政策的地区）分别不超过总投资（不含土地费用、市政费用，仅为工程建设投资，下同）40%、60%、80%、80%的比例进行支持", "news_prompt3": "西藏自治区、南疆四地州、四省涉藏州县项目最高可在中央预算内投资限额内全额支持", "news_prompt4": "享受特殊区域发展政策地区按照具体政策要求执行", "news_prompt5": "省级公共实训基地项目的支持上限为1亿元，市级公共实训基地项目的支持上限为7000万元，县级公共实训基地项目的支持上限为3000万元", "news_prompt6": "国家另有规定的，执行相关规定", "news_prompt7": "（文章来源：国家发改委）"}</t>
+          <t>{"news_prompt1": "国家发展改革委近日印发《教育强国基础设施建设工程(公共实训基地方向)中央预算内投资专项管理办法》", "news_prompt2": "其中提到，中央预算内投资对公共实训基地建设项目原则上按照东、中、西、东北地区（含根据国家相关政策享受中、西部政策的地区）分别不超过总投资（不含土地费用、市政费用，仅为工程建设投资，下同）40%、60%、80%、80%的比例进行支持", "news_prompt3": "西藏自治区、南疆四地州、四省涉藏州县项目最高可在中央预算内投资限额内全额支持", "news_prompt4": "享受特殊区域发展政策地区按照具体政策要求执行", "news_prompt5": "省级公共实训基地项目的支持上限为1亿元，市级公共实训基地项目的支持上限为7000万元，县级公共实训基地项目的支持上限为3000万元", "news_prompt6": "国家另有规定的，执行相关规定"}</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>{"国家发展改革委近日印发《教育强国基础设施建设工程(公共实训基地方向)中央预算内投资专项管理办法》": {"topic": "“生产投资”", "similarity": 0.5897393226623535, "prompt": "新闻文本是“国家发展改革委近日印发《教育强国基础设施建设工程(公共实训基地方向)中央预算内投资专项管理办法》”，包含的情绪词典是：项目/工程(project):0.0,计划/方案(programme):0.0"}, "其中提到，中央预算内投资对公共实训基地建设项目原则上按照东、中、西、东北地区（含根据国家相关政策享受中、西部政策的地区）分别不超过总投资（不含土地费用、市政费用，仅为工程建设投资，下同）40%、60%、80%、80%的比例进行支持": {"topic": "“生产投资”", "similarity": 0.6407554149627686, "prompt": "新闻文本是“其中提到，中央预算内投资对公共实训基地建设项目原则上按照东、中、西、东北地区（含根据国家相关政策享受中、西部政策的地区）分别不超过总投资（不含土地费用、市政费用，仅为工程建设投资，下同）40%、60%、80%、80%的比例进行支持”，包含的情绪词典是：项目/工程(project):0.0,基本的/根本的(fundamental):0.3"}, "西藏自治区、南疆四地州、四省涉藏州县项目最高可在中央预算内投资限额内全额支持": {"topic": "“生产投资”", "similarity": 0.5326117873191833, "prompt": "新闻文本是“西藏自治区、南疆四地州、四省涉藏州县项目最高可在中央预算内投资限额内全额支持”，包含的情绪词典是：投资/投资额(investment):0.4,项目/工程(project):0.0"}, "享受特殊区域发展政策地区按照具体政策要求执行": {"topic": "“房地产”", "similarity": 0.5455292463302612, "prompt": "新闻文本是“享受特殊区域发展政策地区按照具体政策要求执行”，包含的情绪词典是：执行的/实施的(executory):0.0,地区的/区域的(regional):0.0"}, "省级公共实训基地项目的支持上限为1亿元，市级公共实训基地项目的支持上限为7000万元，县级公共实训基地项目的支持上限为3000万元": {"topic": "“生产投资”", "similarity": 0.5800426602363586, "prompt": "新闻文本是“省级公共实训基地项目的支持上限为1亿元，市级公共实训基地项目的支持上限为7000万元，县级公共实训基地项目的支持上限为3000万元”，包含的情绪词典是：上限/限额(cap):0.0,限制/限定(limit):-0.1"}, "国家另有规定的，执行相关规定": {"topic": "“房地产”", "similarity": 0.4822700619697571, "prompt": "新闻文本是“国家另有规定的，执行相关规定”，包含的情绪词典是：法定的/法令的(statutory):0.0,强制的/法定的(mandatory):0.0"}, "（文章来源：国家发改委）": {"topic": "“生产投资”", "similarity": 0.4688243269920349, "prompt": "新闻文本是“（文章来源：国家发改委）”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"国家发展改革委近日印发《教育强国基础设施建设工程(公共实训基地方向)中央预算内投资专项管理办法》": {"topic": "“生产投资”", "similarity": 0.5897393822669983, "prompt": "新闻文本是“国家发展改革委近日印发《教育强国基础设施建设工程(公共实训基地方向)中央预算内投资专项管理办法》”，包含的情绪词典是：项目/工程(project):0.0,计划/方案(programme):0.0"}, "其中提到，中央预算内投资对公共实训基地建设项目原则上按照东、中、西、东北地区（含根据国家相关政策享受中、西部政策的地区）分别不超过总投资（不含土地费用、市政费用，仅为工程建设投资，下同）40%、60%、80%、80%的比例进行支持": {"topic": "“生产投资”", "similarity": 0.6407555937767029, "prompt": "新闻文本是“其中提到，中央预算内投资对公共实训基地建设项目原则上按照东、中、西、东北地区（含根据国家相关政策享受中、西部政策的地区）分别不超过总投资（不含土地费用、市政费用，仅为工程建设投资，下同）40%、60%、80%、80%的比例进行支持”，包含的情绪词典是：项目/工程(project):0.0,基本的/根本的(fundamental):0.3"}, "西藏自治区、南疆四地州、四省涉藏州县项目最高可在中央预算内投资限额内全额支持": {"topic": "“生产投资”", "similarity": 0.5326119065284729, "prompt": "新闻文本是“西藏自治区、南疆四地州、四省涉藏州县项目最高可在中央预算内投资限额内全额支持”，包含的情绪词典是：投资/投资额(investment):0.4,项目/工程(project):0.0"}, "享受特殊区域发展政策地区按照具体政策要求执行": {"topic": "“房地产”", "similarity": 0.545529305934906, "prompt": "新闻文本是“享受特殊区域发展政策地区按照具体政策要求执行”，包含的情绪词典是：执行的/实施的(executory):0.0,地区的/区域的(regional):0.0"}, "省级公共实训基地项目的支持上限为1亿元，市级公共实训基地项目的支持上限为7000万元，县级公共实训基地项目的支持上限为3000万元": {"topic": "“生产投资”", "similarity": 0.5800427794456482, "prompt": "新闻文本是“省级公共实训基地项目的支持上限为1亿元，市级公共实训基地项目的支持上限为7000万元，县级公共实训基地项目的支持上限为3000万元”，包含的情绪词典是：上限/限额(cap):0.0,限制/限定(limit):-0.1"}, "国家另有规定的，执行相关规定": {"topic": "“房地产”", "similarity": 0.48227018117904663, "prompt": "新闻文本是“国家另有规定的，执行相关规定”，包含的情绪词典是：法定的/法令的(statutory):0.0,强制的/法定的(mandatory):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3008,12 +2984,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "央广网北京9月2日消息（记者孙汝祥）截至8月31日，沪市上市公司完成2024年半年报披露", "news_prompt2": "数据显示，沪市公司经营业绩总体稳定", "news_prompt3": "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%", "news_prompt4": "二季度重拾上升轨道 　　2024年上半年，沪市公司总体业绩保持稳健态势，合计实现营业收入24.94万亿元，同比基本持平", "news_prompt5": "净利润2.36万亿元，同比略降1.4%", "news_prompt6": "扣非后净利润2.26万亿元，同比增长0.3%", "news_prompt7": "约八成公司实现盈利，其中850余家净利润同比增长，近240家净利润增幅超50%，120余家增幅超100%，110余家扭亏为盈", "news_prompt8": "分季度看，二季度重拾上升轨道，合计实现净利润1.18万亿元、扣非后净利润1.13万亿元，同比增长2.4%、2.6%", "news_prompt9": "二季度营业收入、净利润环比增速分别为4.9%、0.6%，净利润创近四个季度单季新高，较前四个季度平均净利润增长10.6%", "news_prompt10": "其中，实体企业二季度营业收入、净利润、扣非后净利润环比分别增长6.0%、7.7%、5.1%，边际改善更为明显", "news_prompt11": "分行业看，超九成行业保持盈利", "news_prompt12": "社会服务、汽车、有色金属、公用事业、轻工制造、食品饮料、电子等行业净利润增幅居前，同比增速达378%、45%、43%、22%、18%、17%、12%", "news_prompt13": "农林牧渔、钢铁、非银金融、基础化工等行业二季度恢复势头较好，增速较一季度加快278、200、58、24个百分点", "news_prompt14": "中期分红迎来井喷期 　　在保持经营业绩稳定增长的同时，沪市公司积极主动履行主体责任，夯实市场内生稳定性", "news_prompt15": "今年以来，沪市已有千余家公司披露“提质增效重回报”专项行动方案、400余家公司披露半年度评估报告", "news_prompt16": "发布方案的公司中，近200家公司业绩增幅超50%，见证了沪市公司积极主动提升自身投资价值的努力", "news_prompt17": "科创板公司积极借助“科创板八条”，依托产业并购做大做强，推出14单并购重组案例，金额超30亿元，是去年同期的2倍", "news_prompt18": "其中，普源精电收购标的耐数电子估值增值率超900%，交易方案自申报至证监会注册用时45日，成为“科创板八条”发布后首单注册的发股类交易", "news_prompt19": "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%，其中向境内投资者分红金额近3000亿元，同比增长193%", "news_prompt20": "中国移动、中国石油、中国平安等10余家公司分红超百亿元", "news_prompt21": "以真金白银回馈投资者的同时，沪市公司还通过回购增持提振市场信心", "news_prompt22": "2024年以来，新增回购计划560余家次，拟回购金额上限近800亿元", "news_prompt23": "新增大股东、董监高等主体增持计划350余家次，拟增持金额上限约330亿元", "news_prompt24": "（央广资本眼）（文章来源：央广网）"}</t>
+          <t>{"news_prompt1": "央广网北京9月2日消息（记者孙汝祥）截至8月31日，沪市上市公司完成2024年半年报披露", "news_prompt2": "数据显示，沪市公司经营业绩总体稳定", "news_prompt3": "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%", "news_prompt4": "二季度重拾上升轨道 　　2024年上半年，沪市公司总体业绩保持稳健态势，合计实现营业收入24.94万亿元，同比基本持平", "news_prompt5": "净利润2.36万亿元，同比略降1.4%", "news_prompt6": "扣非后净利润2.26万亿元，同比增长0.3%", "news_prompt7": "约八成公司实现盈利，其中850余家净利润同比增长，近240家净利润增幅超50%，120余家增幅超100%，110余家扭亏为盈", "news_prompt8": "分季度看，二季度重拾上升轨道，合计实现净利润1.18万亿元、扣非后净利润1.13万亿元，同比增长2.4%、2.6%", "news_prompt9": "二季度营业收入、净利润环比增速分别为4.9%、0.6%，净利润创近四个季度单季新高，较前四个季度平均净利润增长10.6%", "news_prompt10": "其中，实体企业二季度营业收入、净利润、扣非后净利润环比分别增长6.0%、7.7%、5.1%，边际改善更为明显", "news_prompt11": "分行业看，超九成行业保持盈利", "news_prompt12": "社会服务、汽车、有色金属、公用事业、轻工制造、食品饮料、电子等行业净利润增幅居前，同比增速达378%、45%、43%、22%、18%、17%、12%", "news_prompt13": "农林牧渔、钢铁、非银金融、基础化工等行业二季度恢复势头较好，增速较一季度加快278、200、58、24个百分点", "news_prompt14": "中期分红迎来井喷期 　　在保持经营业绩稳定增长的同时，沪市公司积极主动履行主体责任，夯实市场内生稳定性", "news_prompt15": "今年以来，沪市已有千余家公司披露“提质增效重回报”专项行动方案、400余家公司披露半年度评估报告", "news_prompt16": "发布方案的公司中，近200家公司业绩增幅超50%，见证了沪市公司积极主动提升自身投资价值的努力", "news_prompt17": "科创板公司积极借助“科创板八条”，依托产业并购做大做强，推出14单并购重组案例，金额超30亿元，是去年同期的2倍", "news_prompt18": "其中，普源精电收购标的耐数电子估值增值率超900%，交易方案自申报至证监会注册用时45日，成为“科创板八条”发布后首单注册的发股类交易", "news_prompt19": "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%，其中向境内投资者分红金额近3000亿元，同比增长193%", "news_prompt20": "中国移动、中国石油、中国平安等10余家公司分红超百亿元", "news_prompt21": "以真金白银回馈投资者的同时，沪市公司还通过回购增持提振市场信心", "news_prompt22": "2024年以来，新增回购计划560余家次，拟回购金额上限近800亿元", "news_prompt23": "新增大股东、董监高等主体增持计划350余家次，拟增持金额上限约330亿元"}</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>{"央广网北京9月2日消息（记者孙汝祥）截至8月31日，沪市上市公司完成2024年半年报披露": {"topic": "“金融”", "similarity": 0.444833904504776, "prompt": "新闻文本是“央广网北京9月2日消息（记者孙汝祥）截至8月31日，沪市上市公司完成2024年半年报披露”，包含的情绪词典是：完成/实现(accomplishes):0.6,完成/实现(accomplish):0.6"}, "数据显示，沪市公司经营业绩总体稳定": {"topic": "“金融”", "similarity": 0.5161686539649963, "prompt": "新闻文本是“数据显示，沪市公司经营业绩总体稳定”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%": {"topic": "“金融”", "similarity": 0.5716711282730103, "prompt": "新闻文本是“投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "二季度重拾上升轨道 　　2024年上半年，沪市公司总体业绩保持稳健态势，合计实现营业收入24.94万亿元，同比基本持平": {"topic": "“金融”", "similarity": 0.6389628052711487, "prompt": "新闻文本是“二季度重拾上升轨道 　　2024年上半年，沪市公司总体业绩保持稳健态势，合计实现营业收入24.94万亿元，同比基本持平”，包含的情绪词典是：上升的/占优势的(ascendant):0.3,上升/上涨(rise):0.5"}, "净利润2.36万亿元，同比略降1.4%": {"topic": "“宏观经济”", "similarity": 0.5002321600914001, "prompt": "新闻文本是“净利润2.36万亿元，同比略降1.4%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "扣非后净利润2.26万亿元，同比增长0.3%": {"topic": "“宏观经济”", "similarity": 0.4572671055793762, "prompt": "新闻文本是“扣非后净利润2.26万亿元，同比增长0.3%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "约八成公司实现盈利，其中850余家净利润同比增长，近240家净利润增幅超50%，120余家增幅超100%，110余家扭亏为盈": {"topic": "“金融”", "similarity": 0.5874866247177124, "prompt": "新闻文本是“约八成公司实现盈利，其中850余家净利润同比增长，近240家净利润增幅超50%，120余家增幅超100%，110余家扭亏为盈”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "分季度看，二季度重拾上升轨道，合计实现净利润1.18万亿元、扣非后净利润1.13万亿元，同比增长2.4%、2.6%": {"topic": "“生产投资”", "similarity": 0.610387921333313, "prompt": "新闻文本是“分季度看，二季度重拾上升轨道，合计实现净利润1.18万亿元、扣非后净利润1.13万亿元，同比增长2.4%、2.6%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "二季度营业收入、净利润环比增速分别为4.9%、0.6%，净利润创近四个季度单季新高，较前四个季度平均净利润增长10.6%": {"topic": "“宏观经济”", "similarity": 0.5358884930610657, "prompt": "新闻文本是“二季度营业收入、净利润环比增速分别为4.9%、0.6%，净利润创近四个季度单季新高，较前四个季度平均净利润增长10.6%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "其中，实体企业二季度营业收入、净利润、扣非后净利润环比分别增长6.0%、7.7%、5.1%，边际改善更为明显": {"topic": "“宏观经济”", "similarity": 0.536932110786438, "prompt": "新闻文本是“其中，实体企业二季度营业收入、净利润、扣非后净利润环比分别增长6.0%、7.7%、5.1%，边际改善更为明显”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "分行业看，超九成行业保持盈利": {"topic": "“消费”", "similarity": 0.5165116190910339, "prompt": "新闻文本是“分行业看，超九成行业保持盈利”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,利润/利益(profit):0.8"}, "社会服务、汽车、有色金属、公用事业、轻工制造、食品饮料、电子等行业净利润增幅居前，同比增速达378%、45%、43%、22%、18%、17%、12%": {"topic": "“消费”", "similarity": 0.6807118654251099, "prompt": "新闻文本是“社会服务、汽车、有色金属、公用事业、轻工制造、食品饮料、电子等行业净利润增幅居前，同比增速达378%、45%、43%、22%、18%、17%、12%”，包含的情绪词典是：服务/业务(service):0.0,部门/行业(sector):0.0"}, "农林牧渔、钢铁、非银金融、基础化工等行业二季度恢复势头较好，增速较一季度加快278、200、58、24个百分点": {"topic": "“宏观经济”", "similarity": 0.6317266225814819, "prompt": "新闻文本是“农林牧渔、钢铁、非银金融、基础化工等行业二季度恢复势头较好，增速较一季度加快278、200、58、24个百分点”，包含的情绪词典是：农业的/农学的(agricultural):0.0,好转/向上趋势(upturn):0.4"}, "中期分红迎来井喷期 　　在保持经营业绩稳定增长的同时，沪市公司积极主动履行主体责任，夯实市场内生稳定性": {"topic": "“金融”", "similarity": 0.5461905598640442, "prompt": "新闻文本是“中期分红迎来井喷期 　　在保持经营业绩稳定增长的同时，沪市公司积极主动履行主体责任，夯实市场内生稳定性”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,盈利能力/获利能力(profitability):0.6"}, "今年以来，沪市已有千余家公司披露“提质增效重回报”专项行动方案、400余家公司披露半年度评估报告": {"topic": "“金融”", "similarity": 0.44647154211997986, "prompt": "新闻文本是“今年以来，沪市已有千余家公司披露“提质增效重回报”专项行动方案、400余家公司披露半年度评估报告”，包含的情绪词典是：有益的/有回报的(rewarding):0.5,公司/企业(company):0.0"}, "发布方案的公司中，近200家公司业绩增幅超50%，见证了沪市公司积极主动提升自身投资价值的努力": {"topic": "“金融”", "similarity": 0.5299339890480042, "prompt": "新闻文本是“发布方案的公司中，近200家公司业绩增幅超50%，见证了沪市公司积极主动提升自身投资价值的努力”，包含的情绪词典是：进步/提升(advancement):0.5,增强/提高(enhancement):0.6"}, "科创板公司积极借助“科创板八条”，依托产业并购做大做强，推出14单并购重组案例，金额超30亿元，是去年同期的2倍": {"topic": "“生产投资”", "similarity": 0.6139217019081116, "prompt": "新闻文本是“科创板公司积极借助“科创板八条”，依托产业并购做大做强，推出14单并购重组案例，金额超30亿元，是去年同期的2倍”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(company):0.0"}, "其中，普源精电收购标的耐数电子估值增值率超900%，交易方案自申报至证监会注册用时45日，成为“科创板八条”发布后首单注册的发股类交易": {"topic": "“金融”", "similarity": 0.5897778272628784, "prompt": "新闻文本是“其中，普源精电收购标的耐数电子估值增值率超900%，交易方案自申报至证监会注册用时45日，成为“科创板八条”发布后首单注册的发股类交易”，包含的情绪词典是：按比例的/可估价的(ratable):0.0,按比例的/可估价的(rata):0.0"}, "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%，其中向境内投资者分红金额近3000亿元，同比增长193%": {"topic": "“金融”", "similarity": 0.6120954155921936, "prompt": "新闻文本是“投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%，其中向境内投资者分红金额近3000亿元，同比增长193%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,投资者/投资人(investor):0.4"}, "中国移动、中国石油、中国平安等10余家公司分红超百亿元": {"topic": "“金融”", "similarity": 0.4864964485168457, "prompt": "新闻文本是“中国移动、中国石油、中国平安等10余家公司分红超百亿元”，包含的情绪词典是：利润/利益(profit):0.8,公司/企业(company):0.0"}, "以真金白银回馈投资者的同时，沪市公司还通过回购增持提振市场信心": {"topic": "“金融”", "similarity": 0.45454472303390503, "prompt": "新闻文本是“以真金白银回馈投资者的同时，沪市公司还通过回购增持提振市场信心”，包含的情绪词典是：有益的/有回报的(rewarding):0.5,收回/重新占有(repossessed):-0.3"}, "2024年以来，新增回购计划560余家次，拟回购金额上限近800亿元": {"topic": "“金融”", "similarity": 0.5147383213043213, "prompt": "新闻文本是“2024年以来，新增回购计划560余家次，拟回购金额上限近800亿元”，包含的情绪词典是：收回/重新占有(repossession):-0.3,撤资/抛售(divestment):-0.2"}, "新增大股东、董监高等主体增持计划350余家次，拟增持金额上限约330亿元": {"topic": "“金融”", "similarity": 0.5587754249572754, "prompt": "新闻文本是“新增大股东、董监高等主体增持计划350余家次，拟增持金额上限约330亿元”，包含的情绪词典是：上限/限额(cap):0.0,投资/投资额(investment):0.4"}, "（央广资本眼）（文章来源：央广网）": {"topic": "“金融”", "similarity": 0.49211257696151733, "prompt": "新闻文本是“（央广资本眼）（文章来源：央广网）”，包含的情绪词典是：资本/资金(capital):0.1,资本不足的(undercapitalized):-0.4"}}</t>
+          <t>{"央广网北京9月2日消息（记者孙汝祥）截至8月31日，沪市上市公司完成2024年半年报披露": {"topic": "“金融”", "similarity": 0.4448342025279999, "prompt": "新闻文本是“央广网北京9月2日消息（记者孙汝祥）截至8月31日，沪市上市公司完成2024年半年报披露”，包含的情绪词典是：完成/实现(accomplishes):0.6,完成/实现(accomplish):0.6"}, "数据显示，沪市公司经营业绩总体稳定": {"topic": "“金融”", "similarity": 0.5161687135696411, "prompt": "新闻文本是“数据显示，沪市公司经营业绩总体稳定”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%": {"topic": "“金融”", "similarity": 0.5716713070869446, "prompt": "新闻文本是“投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "二季度重拾上升轨道 　　2024年上半年，沪市公司总体业绩保持稳健态势，合计实现营业收入24.94万亿元，同比基本持平": {"topic": "“金融”", "similarity": 0.6389629244804382, "prompt": "新闻文本是“二季度重拾上升轨道 　　2024年上半年，沪市公司总体业绩保持稳健态势，合计实现营业收入24.94万亿元，同比基本持平”，包含的情绪词典是：上升的/占优势的(ascendant):0.3,上升/上涨(rise):0.5"}, "净利润2.36万亿元，同比略降1.4%": {"topic": "“宏观经济”", "similarity": 0.5002322196960449, "prompt": "新闻文本是“净利润2.36万亿元，同比略降1.4%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "扣非后净利润2.26万亿元，同比增长0.3%": {"topic": "“宏观经济”", "similarity": 0.457267165184021, "prompt": "新闻文本是“扣非后净利润2.26万亿元，同比增长0.3%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "约八成公司实现盈利，其中850余家净利润同比增长，近240家净利润增幅超50%，120余家增幅超100%，110余家扭亏为盈": {"topic": "“金融”", "similarity": 0.5874866247177124, "prompt": "新闻文本是“约八成公司实现盈利，其中850余家净利润同比增长，近240家净利润增幅超50%，120余家增幅超100%，110余家扭亏为盈”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "分季度看，二季度重拾上升轨道，合计实现净利润1.18万亿元、扣非后净利润1.13万亿元，同比增长2.4%、2.6%": {"topic": "“生产投资”", "similarity": 0.6103879809379578, "prompt": "新闻文本是“分季度看，二季度重拾上升轨道，合计实现净利润1.18万亿元、扣非后净利润1.13万亿元，同比增长2.4%、2.6%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "二季度营业收入、净利润环比增速分别为4.9%、0.6%，净利润创近四个季度单季新高，较前四个季度平均净利润增长10.6%": {"topic": "“宏观经济”", "similarity": 0.5358885526657104, "prompt": "新闻文本是“二季度营业收入、净利润环比增速分别为4.9%、0.6%，净利润创近四个季度单季新高，较前四个季度平均净利润增长10.6%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "其中，实体企业二季度营业收入、净利润、扣非后净利润环比分别增长6.0%、7.7%、5.1%，边际改善更为明显": {"topic": "“宏观经济”", "similarity": 0.5369322896003723, "prompt": "新闻文本是“其中，实体企业二季度营业收入、净利润、扣非后净利润环比分别增长6.0%、7.7%、5.1%，边际改善更为明显”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "分行业看，超九成行业保持盈利": {"topic": "“消费”", "similarity": 0.5165117979049683, "prompt": "新闻文本是“分行业看，超九成行业保持盈利”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,利润/利益(profit):0.8"}, "社会服务、汽车、有色金属、公用事业、轻工制造、食品饮料、电子等行业净利润增幅居前，同比增速达378%、45%、43%、22%、18%、17%、12%": {"topic": "“消费”", "similarity": 0.6807119250297546, "prompt": "新闻文本是“社会服务、汽车、有色金属、公用事业、轻工制造、食品饮料、电子等行业净利润增幅居前，同比增速达378%、45%、43%、22%、18%、17%、12%”，包含的情绪词典是：服务/业务(service):0.0,部门/行业(sector):0.0"}, "农林牧渔、钢铁、非银金融、基础化工等行业二季度恢复势头较好，增速较一季度加快278、200、58、24个百分点": {"topic": "“宏观经济”", "similarity": 0.631726861000061, "prompt": "新闻文本是“农林牧渔、钢铁、非银金融、基础化工等行业二季度恢复势头较好，增速较一季度加快278、200、58、24个百分点”，包含的情绪词典是：农业的/农学的(agricultural):0.0,好转/向上趋势(upturn):0.4"}, "中期分红迎来井喷期 　　在保持经营业绩稳定增长的同时，沪市公司积极主动履行主体责任，夯实市场内生稳定性": {"topic": "“金融”", "similarity": 0.5461907386779785, "prompt": "新闻文本是“中期分红迎来井喷期 　　在保持经营业绩稳定增长的同时，沪市公司积极主动履行主体责任，夯实市场内生稳定性”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,盈利能力/获利能力(profitability):0.6"}, "今年以来，沪市已有千余家公司披露“提质增效重回报”专项行动方案、400余家公司披露半年度评估报告": {"topic": "“金融”", "similarity": 0.44647181034088135, "prompt": "新闻文本是“今年以来，沪市已有千余家公司披露“提质增效重回报”专项行动方案、400余家公司披露半年度评估报告”，包含的情绪词典是：有益的/有回报的(rewarding):0.5,公司/企业(company):0.0"}, "发布方案的公司中，近200家公司业绩增幅超50%，见证了沪市公司积极主动提升自身投资价值的努力": {"topic": "“金融”", "similarity": 0.529934287071228, "prompt": "新闻文本是“发布方案的公司中，近200家公司业绩增幅超50%，见证了沪市公司积极主动提升自身投资价值的努力”，包含的情绪词典是：进步/提升(advancement):0.5,增强/提高(enhancement):0.6"}, "科创板公司积极借助“科创板八条”，依托产业并购做大做强，推出14单并购重组案例，金额超30亿元，是去年同期的2倍": {"topic": "“生产投资”", "similarity": 0.6139216423034668, "prompt": "新闻文本是“科创板公司积极借助“科创板八条”，依托产业并购做大做强，推出14单并购重组案例，金额超30亿元，是去年同期的2倍”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(company):0.0"}, "其中，普源精电收购标的耐数电子估值增值率超900%，交易方案自申报至证监会注册用时45日，成为“科创板八条”发布后首单注册的发股类交易": {"topic": "“金融”", "similarity": 0.589777946472168, "prompt": "新闻文本是“其中，普源精电收购标的耐数电子估值增值率超900%，交易方案自申报至证监会注册用时45日，成为“科创板八条”发布后首单注册的发股类交易”，包含的情绪词典是：按比例的/可估价的(ratable):0.0,按比例的/可估价的(rata):0.0"}, "投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%，其中向境内投资者分红金额近3000亿元，同比增长193%": {"topic": "“金融”", "similarity": 0.6120954751968384, "prompt": "新闻文本是“投资者回报方面，中期分红迎来井喷期，分红家数合计337家，同比增长343%，合计分红金额近5000亿元，同比增长156%，其中向境内投资者分红金额近3000亿元，同比增长193%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,投资者/投资人(investor):0.4"}, "中国移动、中国石油、中国平安等10余家公司分红超百亿元": {"topic": "“金融”", "similarity": 0.48649656772613525, "prompt": "新闻文本是“中国移动、中国石油、中国平安等10余家公司分红超百亿元”，包含的情绪词典是：利润/利益(profit):0.8,公司/企业(company):0.0"}, "以真金白银回馈投资者的同时，沪市公司还通过回购增持提振市场信心": {"topic": "“金融”", "similarity": 0.45454490184783936, "prompt": "新闻文本是“以真金白银回馈投资者的同时，沪市公司还通过回购增持提振市场信心”，包含的情绪词典是：有益的/有回报的(rewarding):0.5,收回/重新占有(repossessed):-0.3"}, "2024年以来，新增回购计划560余家次，拟回购金额上限近800亿元": {"topic": "“金融”", "similarity": 0.5147384405136108, "prompt": "新闻文本是“2024年以来，新增回购计划560余家次，拟回购金额上限近800亿元”，包含的情绪词典是：收回/重新占有(repossession):-0.3,撤资/抛售(divestment):-0.2"}, "新增大股东、董监高等主体增持计划350余家次，拟增持金额上限约330亿元": {"topic": "“金融”", "similarity": 0.5587755441665649, "prompt": "新闻文本是“新增大股东、董监高等主体增持计划350余家次，拟增持金额上限约330亿元”，包含的情绪词典是：上限/限额(cap):0.0,投资/投资额(investment):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -3059,12 +3035,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "廉石、廉诗、廉画……走进梅州市梅江区金山街道周溪村，一步一廉景，处处是廉风，浓郁的清廉氛围与农家小院交相辉映，勾勒出和美“廉”村画卷", "news_prompt2": "周溪村，周溪河贯穿其中", "news_prompt3": "近年来，周溪村通过重建濂溪书院，打造廉政教育基地，不断涵养廉洁文化，引导村党员干部汲取廉洁养分、恪守清廉底线，以实干担当推动村民幸福指数持续提升", "news_prompt4": "2023年，周溪村入选省“百千万工程”首批典型村名单", "news_prompt5": "重建濂溪书院弘扬廉洁文化　　在周溪村，有一座古老的石拱桥叫“濂溪桥”", "news_prompt6": "“濂溪”是周敦颐的字号", "news_prompt7": "周溪河上为何会横跨一座濂溪桥呢", "news_prompt8": "据史料不完全记载，周敦颐可能曾经来过梅州，后人为纪念这位思想家，把梅城附近的一条小溪命名为周溪", "news_prompt9": "明孝宗弘治年间，江西永丰籍进士刘彬担任程乡知县，基于他对周敦颐道德学问、思想精深的仰慕，更基于周敦颐与梅州的历史渊源，他决定在周溪河畔建立濂溪书院，濂溪桥由此得名", "news_prompt10": "如今，濂溪书院在历史的风雨中淡去，濂溪桥却依然屹立在周溪之上", "news_prompt11": "为弘扬周敦颐“出淤泥而不染”的廉洁精神，2021年，梅江区纪委监委结合十里梅花长廊规划建设，在周溪河畔重建濂溪书院，打造梅江特色廉政文化主题基地，这也是目前我省第一所由官方重建的濂溪书院", "news_prompt12": "新建的濂溪书院占地面积约750平方米，布局为一中厅、两回廊、前后门、三面围栏", "news_prompt13": "布展内容包括周敦颐与濂溪书院的由来变迁、中国古代监察制度、历史上梅江区籍监察官员代表的事迹等内容", "news_prompt14": "“濂溪书院建成后，我们在饶公桥至梅江出口段以点带线设置廉石、廉刻景观，融廉入景、以景显廉，与周溪河流域人居环境、客家人文历史等相融相合，将廉政文化有机结合在一起，为十里梅花长廊增添一道亮丽的廉政风景线，使市民游客在休闲观光中潜移默化地接受廉政文化的熏陶", "news_prompt15": "”梅江区纪委监委相关负责人介绍，目前，濂溪书院已成了梅江区党员干部开展廉政教育的重要场所", "news_prompt16": "记者走访当天，恰好遇到前来参观学习的队伍", "news_prompt17": "周溪村“两委”干部侯飞翔耐心地讲解着廉洁文化相关内容", "news_prompt18": "“我们这次是来开展主题党日活动，参观完后对书院以及廉洁文化有了更深入的了解", "news_prompt19": "”中移铁通有限公司员工卓庆鑫表示", "news_prompt20": "“每年接待超过3000人次", "news_prompt21": "”侯飞翔介绍，自从濂溪书院重建后，村“两委”干部经过培训，全员上阵，成了廉政教育讲解员", "news_prompt22": "“每次讲解都有新的感悟，既要当好讲解员，更要当好践行者，清清白白做事，堂堂正正做人", "news_prompt23": "”侯飞翔表示", "news_prompt24": "汲取廉洁养分推动强村富民　　一座濂溪书院，连接古与今，周子精神代代传颂，教育着党员干部要廉洁奉公、严于律己", "news_prompt25": "在周溪村，党员干部将廉洁文化内化于心、外化于行", "news_prompt26": "该村不仅制度上墙，村里大小事，均严格落实“四议两公开”，自觉接受村民监督，让村务在阳光下运行", "news_prompt27": "有了制度约束，党员干部心无旁骛干事创业，干部队伍凝聚力、执行力、战斗力不断提升", "news_prompt28": "近年来，周溪村持续擦亮“廉”色、“古”色，将廉景打造与古色建筑修建结合，不断推动人居环境改善、村容村貌提升", "news_prompt29": "“环境越来越好，我每天都要到这里散步", "news_prompt30": "”市民黄佳介绍，周溪村靠近住宅区，随着环境的整体提升，已成为了不少人休闲的好去处", "news_prompt31": "党风带民风，清风促新风", "news_prompt32": "周溪村的变化让村民看在眼里，记在心里，更加齐心协力推动乡村振兴、“百千万工程”实施", "news_prompt33": "今年，周溪村广泛发动社会各界参与植绿护绿，得到了积极响应，筹集社会各界资金共92.29万元，种植树木2500多株，打造“党员先锋林”“乡贤林”等主题林", "news_prompt34": "“在群众的积极参与、支持下，我们村农房外立面焕然一新，环境越来越好，吸引了不少社会资金进驻，兴起了茶室、咖啡室等新业态", "news_prompt35": "”周溪村党总支书记侯国超介绍，如今不少村民可以通过出租房子得租金", "news_prompt36": "在推进环境绿化美化的同时，周溪村大力发展绿色产业，投入180万元，联动东街村、龙丰村、月梅村、芹洋村、福长村等五村抱团发展光伏产业，预计村集体经济可增收18万元", "news_prompt37": "当前，周溪村已形成“廉”色、“古”色、绿色为主的发展思路，正逐步推动人流变成现金流", "news_prompt38": "目前，金山街道与周溪村已共同成立强镇富村公司——梅州市金山文旅发展有限公司，计划整合利用百岁山郊野公园、周溪十里梅花长廊等资源，通过“山水生态”激活“山水经济”，打造休闲经济、体育经济和农旅经济，推动2024年周溪村集体收入突破50万元", "news_prompt39": "“依托百岁山郊野公园，接下来我们将充分发挥生态优势，计划在村里打造徒步、自行车、登山路道，推动文旅体融合发展", "news_prompt40": "”侯国超表示", "news_prompt41": "南方日报记者魏丽文　　通讯员肖惠媚（文章来源：南方日报）"}</t>
+          <t>{"news_prompt1": "近年来，周溪村通过重建濂溪书院，打造廉政教育基地，不断涵养廉洁文化，引导村党员干部汲取廉洁养分、恪守清廉底线，以实干担当推动村民幸福指数持续提升", "news_prompt2": "2023年，周溪村入选省“百千万工程”首批典型村名单", "news_prompt3": "布展内容包括周敦颐与濂溪书院的由来变迁、中国古代监察制度、历史上梅江区籍监察官员代表的事迹等内容", "news_prompt4": "”中移铁通有限公司员工卓庆鑫表示", "news_prompt5": "“每年接待超过3000人次", "news_prompt6": "汲取廉洁养分推动强村富民　　一座濂溪书院，连接古与今，周子精神代代传颂，教育着党员干部要廉洁奉公、严于律己", "news_prompt7": "今年，周溪村广泛发动社会各界参与植绿护绿，得到了积极响应，筹集社会各界资金共92.29万元，种植树木2500多株，打造“党员先锋林”“乡贤林”等主题林", "news_prompt8": "“在群众的积极参与、支持下，我们村农房外立面焕然一新，环境越来越好，吸引了不少社会资金进驻，兴起了茶室、咖啡室等新业态", "news_prompt9": "”周溪村党总支书记侯国超介绍，如今不少村民可以通过出租房子得租金", "news_prompt10": "“依托百岁山郊野公园，接下来我们将充分发挥生态优势，计划在村里打造徒步、自行车、登山路道，推动文旅体融合发展", "news_prompt11": "”侯国超表示"}</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>{"近年来，周溪村通过重建濂溪书院，打造廉政教育基地，不断涵养廉洁文化，引导村党员干部汲取廉洁养分、恪守清廉底线，以实干担当推动村民幸福指数持续提升": {"topic": "“消费”", "similarity": 0.43524423241615295, "prompt": "新闻文本是“近年来，周溪村通过重建濂溪书院，打造廉政教育基地，不断涵养廉洁文化，引导村党员干部汲取廉洁养分、恪守清廉底线，以实干担当推动村民幸福指数持续提升”，包含的情绪词典是：建设性的/有益的(constructive):0.4,可敬的/高尚的(honorable):0.6"}, "2023年，周溪村入选省“百千万工程”首批典型村名单": {"topic": "“生产投资”", "similarity": 0.4448189437389374, "prompt": "新闻文本是“2023年，周溪村入选省“百千万工程”首批典型村名单”，包含的情绪词典是：项目/工程(project):0.0,国家/乡村(country):0.0"}, "明孝宗弘治年间，江西永丰籍进士刘彬担任程乡知县，基于他对周敦颐道德学问、思想精深的仰慕，更基于周敦颐与梅州的历史渊源，他决定在周溪河畔建立濂溪书院，濂溪桥由此得名": {"topic": "“消费”", "similarity": 0.42246267199516296}, "为弘扬周敦颐“出淤泥而不染”的廉洁精神，2021年，梅江区纪委监委结合十里梅花长廊规划建设，在周溪河畔重建濂溪书院，打造梅江特色廉政文化主题基地，这也是目前我省第一所由官方重建的濂溪书院": {"topic": "“生产投资”", "similarity": 0.4214716851711273}, "布展内容包括周敦颐与濂溪书院的由来变迁、中国古代监察制度、历史上梅江区籍监察官员代表的事迹等内容": {"topic": "“生产投资”", "similarity": 0.4213404357433319, "prompt": "新闻文本是“布展内容包括周敦颐与濂溪书院的由来变迁、中国古代监察制度、历史上梅江区籍监察官员代表的事迹等内容”，包含的情绪词典是：展示/表明(show):0.0,贿赂/行贿(bribe):-0.55"}, "“濂溪书院建成后，我们在饶公桥至梅江出口段以点带线设置廉石、廉刻景观，融廉入景、以景显廉，与周溪河流域人居环境、客家人文历史等相融相合，将廉政文化有机结合在一起，为十里梅花长廊增添一道亮丽的廉政风景线，使市民游客在休闲观光中潜移默化地接受廉政文化的熏陶": {"topic": "“生产投资”", "similarity": 0.4707484245300293}, "”中移铁通有限公司员工卓庆鑫表示": {"topic": "“生产投资”", "similarity": 0.4770127534866333, "prompt": "新闻文本是“”中移铁通有限公司员工卓庆鑫表示”，包含的情绪词典是：报关员/申报者(declarant):0.0,工作/劳动(work):0.01"}, "“每年接待超过3000人次": {"topic": "“消费”", "similarity": 0.4495013952255249, "prompt": "新闻文本是““每年接待超过3000人次”，包含的情绪词典是：出席人数/产量(turnout):0.0,每年的/一年一度的(yearly):0.0"}, "汲取廉洁养分推动强村富民　　一座濂溪书院，连接古与今，周子精神代代传颂，教育着党员干部要廉洁奉公、严于律己": {"topic": "“消费”", "similarity": 0.432259738445282, "prompt": "新闻文本是“汲取廉洁养分推动强村富民　　一座濂溪书院，连接古与今，周子精神代代传颂，教育着党员干部要廉洁奉公、严于律己”，包含的情绪词典是：腐败的/贪污的(corrupt):-0.7,使腐败/使贪污(corrupting):-0.7"}, "今年，周溪村广泛发动社会各界参与植绿护绿，得到了积极响应，筹集社会各界资金共92.29万元，种植树木2500多株，打造“党员先锋林”“乡贤林”等主题林": {"topic": "“消费”", "similarity": 0.4415978193283081, "prompt": "新闻文本是“今年，周溪村广泛发动社会各界参与植绿护绿，得到了积极响应，筹集社会各界资金共92.29万元，种植树木2500多株，打造“党员先锋林”“乡贤林”等主题林”，包含的情绪词典是：植物/工厂(plant):0.0,国家/乡村(country):0.0"}, "“在群众的积极参与、支持下，我们村农房外立面焕然一新，环境越来越好，吸引了不少社会资金进驻，兴起了茶室、咖啡室等新业态": {"topic": "“消费”", "similarity": 0.5346287488937378, "prompt": "新闻文本是““在群众的积极参与、支持下，我们村农房外立面焕然一新，环境越来越好，吸引了不少社会资金进驻，兴起了茶室、咖啡室等新业态”，包含的情绪词典是：已改善的/已改进的(improved):0.5,正在改善的/正在改进的(improving):0.5"}, "”周溪村党总支书记侯国超介绍，如今不少村民可以通过出租房子得租金": {"topic": "“房地产”", "similarity": 0.43366920948028564, "prompt": "新闻文本是“”周溪村党总支书记侯国超介绍，如今不少村民可以通过出租房子得租金”，包含的情绪词典是：房子/住宅(house):0.0,居民/住户(resident):0.0"}, "在推进环境绿化美化的同时，周溪村大力发展绿色产业，投入180万元，联动东街村、龙丰村、月梅村、芹洋村、福长村等五村抱团发展光伏产业，预计村集体经济可增收18万元": {"topic": "“生产投资”", "similarity": 0.4362110495567322}, "目前，金山街道与周溪村已共同成立强镇富村公司——梅州市金山文旅发展有限公司，计划整合利用百岁山郊野公园、周溪十里梅花长廊等资源，通过“山水生态”激活“山水经济”，打造休闲经济、体育经济和农旅经济，推动2024年周溪村集体收入突破50万元": {"topic": "“消费”", "similarity": 0.48667579889297485}, "“依托百岁山郊野公园，接下来我们将充分发挥生态优势，计划在村里打造徒步、自行车、登山路道，推动文旅体融合发展": {"topic": "“消费”", "similarity": 0.426408588886261, "prompt": "新闻文本是““依托百岁山郊野公园，接下来我们将充分发挥生态优势，计划在村里打造徒步、自行车、登山路道，推动文旅体融合发展”，包含的情绪词典是：优势/有利条件(advantage):0.7,超龄的/过老的(overage):0.0"}, "”侯国超表示": {"topic": "“生产投资”", "similarity": 0.45833098888397217, "prompt": "新闻文本是“”侯国超表示”，包含的情绪词典是：上级的/较好的(superior):0.55,超过/超越(surpass):0.6"}}</t>
+          <t>{"近年来，周溪村通过重建濂溪书院，打造廉政教育基地，不断涵养廉洁文化，引导村党员干部汲取廉洁养分、恪守清廉底线，以实干担当推动村民幸福指数持续提升": {"topic": "“消费”", "similarity": 0.43524444103240967, "prompt": "新闻文本是“近年来，周溪村通过重建濂溪书院，打造廉政教育基地，不断涵养廉洁文化，引导村党员干部汲取廉洁养分、恪守清廉底线，以实干担当推动村民幸福指数持续提升”，包含的情绪词典是：建设性的/有益的(constructive):0.4,可敬的/高尚的(honorable):0.6"}, "2023年，周溪村入选省“百千万工程”首批典型村名单": {"topic": "“生产投资”", "similarity": 0.44481897354125977, "prompt": "新闻文本是“2023年，周溪村入选省“百千万工程”首批典型村名单”，包含的情绪词典是：项目/工程(project):0.0,国家/乡村(country):0.0"}, "布展内容包括周敦颐与濂溪书院的由来变迁、中国古代监察制度、历史上梅江区籍监察官员代表的事迹等内容": {"topic": "“生产投资”", "similarity": 0.4213404059410095, "prompt": "新闻文本是“布展内容包括周敦颐与濂溪书院的由来变迁、中国古代监察制度、历史上梅江区籍监察官员代表的事迹等内容”，包含的情绪词典是：展示/表明(show):0.0,贿赂/行贿(bribe):-0.55"}, "”中移铁通有限公司员工卓庆鑫表示": {"topic": "“生产投资”", "similarity": 0.47701287269592285, "prompt": "新闻文本是“”中移铁通有限公司员工卓庆鑫表示”，包含的情绪词典是：报关员/申报者(declarant):0.0,工作/劳动(work):0.01"}, "“每年接待超过3000人次": {"topic": "“消费”", "similarity": 0.44950154423713684, "prompt": "新闻文本是““每年接待超过3000人次”，包含的情绪词典是：出席人数/产量(turnout):0.0,每年的/一年一度的(yearly):0.0"}, "汲取廉洁养分推动强村富民　　一座濂溪书院，连接古与今，周子精神代代传颂，教育着党员干部要廉洁奉公、严于律己": {"topic": "“消费”", "similarity": 0.43225982785224915, "prompt": "新闻文本是“汲取廉洁养分推动强村富民　　一座濂溪书院，连接古与今，周子精神代代传颂，教育着党员干部要廉洁奉公、严于律己”，包含的情绪词典是：腐败的/贪污的(corrupt):-0.7,使腐败/使贪污(corrupting):-0.7"}, "今年，周溪村广泛发动社会各界参与植绿护绿，得到了积极响应，筹集社会各界资金共92.29万元，种植树木2500多株，打造“党员先锋林”“乡贤林”等主题林": {"topic": "“消费”", "similarity": 0.4415978491306305, "prompt": "新闻文本是“今年，周溪村广泛发动社会各界参与植绿护绿，得到了积极响应，筹集社会各界资金共92.29万元，种植树木2500多株，打造“党员先锋林”“乡贤林”等主题林”，包含的情绪词典是：植物/工厂(plant):0.0,国家/乡村(country):0.0"}, "“在群众的积极参与、支持下，我们村农房外立面焕然一新，环境越来越好，吸引了不少社会资金进驻，兴起了茶室、咖啡室等新业态": {"topic": "“消费”", "similarity": 0.5346288681030273, "prompt": "新闻文本是““在群众的积极参与、支持下，我们村农房外立面焕然一新，环境越来越好，吸引了不少社会资金进驻，兴起了茶室、咖啡室等新业态”，包含的情绪词典是：已改善的/已改进的(improved):0.5,正在改善的/正在改进的(improving):0.5"}, "”周溪村党总支书记侯国超介绍，如今不少村民可以通过出租房子得租金": {"topic": "“房地产”", "similarity": 0.43366938829421997, "prompt": "新闻文本是“”周溪村党总支书记侯国超介绍，如今不少村民可以通过出租房子得租金”，包含的情绪词典是：房子/住宅(house):0.0,居民/住户(resident):0.0"}, "“依托百岁山郊野公园，接下来我们将充分发挥生态优势，计划在村里打造徒步、自行车、登山路道，推动文旅体融合发展": {"topic": "“消费”", "similarity": 0.4264087378978729, "prompt": "新闻文本是““依托百岁山郊野公园，接下来我们将充分发挥生态优势，计划在村里打造徒步、自行车、登山路道，推动文旅体融合发展”，包含的情绪词典是：优势/有利条件(advantage):0.7,超龄的/过老的(overage):0.0"}, "”侯国超表示": {"topic": "“生产投资”", "similarity": 0.45833098888397217, "prompt": "新闻文本是“”侯国超表示”，包含的情绪词典是：上级的/较好的(superior):0.55,超过/超越(surpass):0.6"}}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3086,12 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上证报中国证券网讯 9月2日早盘，食品饮料板块震荡走低", "news_prompt2": "截至9时39分，千禾味业跌超7%，天味食品跌逾6%，泸州老窖、莫高股份等跟跌", "news_prompt3": "（文章来源：上海证券报·中国证券网）"}</t>
+          <t>{"news_prompt1": "上证报中国证券网讯 9月2日早盘，食品饮料板块震荡走低", "news_prompt2": "截至9时39分，千禾味业跌超7%，天味食品跌逾6%，泸州老窖、莫高股份等跟跌"}</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>{"上证报中国证券网讯 9月2日早盘，食品饮料板块震荡走低": {"topic": "“金融”", "similarity": 0.44668450951576233, "prompt": "新闻文本是“上证报中国证券网讯 9月2日早盘，食品饮料板块震荡走低”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退/低迷(downturn):-0.6"}, "截至9时39分，千禾味业跌超7%，天味食品跌逾6%，泸州老窖、莫高股份等跟跌": {"topic": "“金融”", "similarity": 0.5155947804450989, "prompt": "新闻文本是“截至9时39分，千禾味业跌超7%，天味食品跌逾6%，泸州老窖、莫高股份等跟跌”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "（文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.4783601760864258, "prompt": "新闻文本是“（文章来源：上海证券报·中国证券网）”，包含的情绪词典是：投资者/投资人(investor):0.4,股票/库存(stock):0.0"}}</t>
+          <t>{"上证报中国证券网讯 9月2日早盘，食品饮料板块震荡走低": {"topic": "“金融”", "similarity": 0.44668471813201904, "prompt": "新闻文本是“上证报中国证券网讯 9月2日早盘，食品饮料板块震荡走低”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退/低迷(downturn):-0.6"}, "截至9时39分，千禾味业跌超7%，天味食品跌逾6%，泸州老窖、莫高股份等跟跌": {"topic": "“金融”", "similarity": 0.5155948400497437, "prompt": "新闻文本是“截至9时39分，千禾味业跌超7%，天味食品跌逾6%，泸州老窖、莫高股份等跟跌”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -3161,12 +3137,12 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "东方财富Choice数据显示，上周（8月26日-8月30日），场内股票型ETF净申购145.57亿份", "news_prompt2": "其中，沪市股票型ETF净申购124.60亿份，深市股票型ETF净申购20.97亿份", "news_prompt3": "以最新净值计，上周净申购金额达413.94亿元", "news_prompt4": "游戏动漫ETF领涨 　　数据显示，上周场内股票型ETF中，游戏动漫ETF、游戏ETF（159869.SZ）、游戏ETF（516010.SH）涨幅靠前", "news_prompt5": "其中，游戏动漫ETF周涨7.17%，排名第1", "news_prompt6": "沪深300ETF申购最多 　　上周净申购金额最多的为沪深300 ETF，净申购金额131.92亿元", "news_prompt7": "此外，沪深300ETF易方达和中证1000ETF也获申购居前，净申购金额依次为90.47亿元和43.75亿元", "news_prompt8": "中证500ETF易方达遭赎回 　　数据还显示，上周净赎回金额最多的场内股票ETF为中证500ETF易方达，赎回金额18.28亿元", "news_prompt9": "沪深300ETF基金紧随其后，赎回金额3.44亿元", "news_prompt10": "机构看后市 　　华福证券认为，抵抗内外需双弱的同时，更应强调确定性的成长", "news_prompt11": "六月以来红利指数持续回调，高股息出现“缩圈”，银行是“缩圈”后的重要阵地", "news_prompt12": "四大行股价接连创下新高后，上周银行板块页自周三开始连续调整，或是“物极必反”的体现", "news_prompt13": "在此判断下，虽然中长期持续看好抵抗内外需双弱的港股高股息、黄金与船舶，但目前在内外流动性有望边际缓解、风格转换迹象初现的时点，更应强调确定性的成长，建议关注受益AI发展与全球科技上行周期下的互联网、光模块、果链，以及受益于亚非拉新兴市场爆发的逆变器、变压器", "news_prompt14": "东莞证券表示，上周五指数集体反弹，创业板相对更加强势，全市场超4600只股票收红，电子、房地产、传媒、非银金融等板块表现突出", "news_prompt15": "从技术面来看，创业板指日线形态已形成反弹格局，盘中强势站上10日均线，后续投资者需观察创业板指能否站稳20日均线", "news_prompt16": "从盘面上来看，前期强势的红利股的连续回调，或使资金进入其他相对低位的板块和个股，如创业板和中小盘个股，短期投资者宜规避高位调整的红利股，多关注前期处于低位，基本面较好的个股", "news_prompt17": "另外，央行的会议表示，下半年将研究出台增量政策举措，宏观政策将持续发力，且发力力度更大，同时考虑到即将进入金九银十传统旺季，市场或将走出一波反弹行情", "news_prompt18": "（文章来源：东方财富研究中心）"}</t>
+          <t>{"news_prompt1": "东方财富Choice数据显示，上周（8月26日-8月30日），场内股票型ETF净申购145.57亿份", "news_prompt2": "其中，沪市股票型ETF净申购124.60亿份，深市股票型ETF净申购20.97亿份", "news_prompt3": "以最新净值计，上周净申购金额达413.94亿元", "news_prompt4": "游戏动漫ETF领涨 　　数据显示，上周场内股票型ETF中，游戏动漫ETF、游戏ETF（159869.SZ）、游戏ETF（516010.SH）涨幅靠前", "news_prompt5": "沪深300ETF申购最多 　　上周净申购金额最多的为沪深300 ETF，净申购金额131.92亿元", "news_prompt6": "此外，沪深300ETF易方达和中证1000ETF也获申购居前，净申购金额依次为90.47亿元和43.75亿元", "news_prompt7": "中证500ETF易方达遭赎回 　　数据还显示，上周净赎回金额最多的场内股票ETF为中证500ETF易方达，赎回金额18.28亿元", "news_prompt8": "沪深300ETF基金紧随其后，赎回金额3.44亿元", "news_prompt9": "机构看后市 　　华福证券认为，抵抗内外需双弱的同时，更应强调确定性的成长", "news_prompt10": "六月以来红利指数持续回调，高股息出现“缩圈”，银行是“缩圈”后的重要阵地", "news_prompt11": "四大行股价接连创下新高后，上周银行板块页自周三开始连续调整，或是“物极必反”的体现", "news_prompt12": "东莞证券表示，上周五指数集体反弹，创业板相对更加强势，全市场超4600只股票收红，电子、房地产、传媒、非银金融等板块表现突出", "news_prompt13": "从技术面来看，创业板指日线形态已形成反弹格局，盘中强势站上10日均线，后续投资者需观察创业板指能否站稳20日均线", "news_prompt14": "从盘面上来看，前期强势的红利股的连续回调，或使资金进入其他相对低位的板块和个股，如创业板和中小盘个股，短期投资者宜规避高位调整的红利股，多关注前期处于低位，基本面较好的个股", "news_prompt15": "另外，央行的会议表示，下半年将研究出台增量政策举措，宏观政策将持续发力，且发力力度更大，同时考虑到即将进入金九银十传统旺季，市场或将走出一波反弹行情"}</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>{"东方财富Choice数据显示，上周（8月26日-8月30日），场内股票型ETF净申购145.57亿份": {"topic": "“金融”", "similarity": 0.5184255242347717, "prompt": "新闻文本是“东方财富Choice数据显示，上周（8月26日-8月30日），场内股票型ETF净申购145.57亿份”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "其中，沪市股票型ETF净申购124.60亿份，深市股票型ETF净申购20.97亿份": {"topic": "“金融”", "similarity": 0.5551952123641968, "prompt": "新闻文本是“其中，沪市股票型ETF净申购124.60亿份，深市股票型ETF净申购20.97亿份”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "以最新净值计，上周净申购金额达413.94亿元": {"topic": "“金融”", "similarity": 0.51517254114151, "prompt": "新闻文本是“以最新净值计，上周净申购金额达413.94亿元”，包含的情绪词典是：投资/投资额(investment):0.4,营业额/周转(turnover):0.0"}, "游戏动漫ETF领涨 　　数据显示，上周场内股票型ETF中，游戏动漫ETF、游戏ETF（159869.SZ）、游戏ETF（516010.SH）涨幅靠前": {"topic": "“金融”", "similarity": 0.5780243277549744, "prompt": "新闻文本是“游戏动漫ETF领涨 　　数据显示，上周场内股票型ETF中，游戏动漫ETF、游戏ETF（159869.SZ）、游戏ETF（516010.SH）涨幅靠前”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "沪深300ETF申购最多 　　上周净申购金额最多的为沪深300 ETF，净申购金额131.92亿元": {"topic": "“金融”", "similarity": 0.5780247449874878, "prompt": "新闻文本是“沪深300ETF申购最多 　　上周净申购金额最多的为沪深300 ETF，净申购金额131.92亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "此外，沪深300ETF易方达和中证1000ETF也获申购居前，净申购金额依次为90.47亿元和43.75亿元": {"topic": "“金融”", "similarity": 0.5738049149513245, "prompt": "新闻文本是“此外，沪深300ETF易方达和中证1000ETF也获申购居前，净申购金额依次为90.47亿元和43.75亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "中证500ETF易方达遭赎回 　　数据还显示，上周净赎回金额最多的场内股票ETF为中证500ETF易方达，赎回金额18.28亿元": {"topic": "“金融”", "similarity": 0.5630948543548584, "prompt": "新闻文本是“中证500ETF易方达遭赎回 　　数据还显示，上周净赎回金额最多的场内股票ETF为中证500ETF易方达，赎回金额18.28亿元”，包含的情绪词典是：清仓/抛售(closeouts):-0.2,清仓/抛售(closeout):-0.2"}, "沪深300ETF基金紧随其后，赎回金额3.44亿元": {"topic": "“金融”", "similarity": 0.5447779297828674, "prompt": "新闻文本是“沪深300ETF基金紧随其后，赎回金额3.44亿元”，包含的情绪词典是：基金/资金(fund):0.1,撤资/抛售(divestment):-0.2"}, "机构看后市 　　华福证券认为，抵抗内外需双弱的同时，更应强调确定性的成长": {"topic": "“金融”", "similarity": 0.5793373584747314, "prompt": "新闻文本是“机构看后市 　　华福证券认为，抵抗内外需双弱的同时，更应强调确定性的成长”，包含的情绪词典是：表现不佳/业绩低于预期(underperforms):-0.4,稳定的/稳固的(stable):0.5"}, "六月以来红利指数持续回调，高股息出现“缩圈”，银行是“缩圈”后的重要阵地": {"topic": "“金融”", "similarity": 0.601119875907898, "prompt": "新闻文本是“六月以来红利指数持续回调，高股息出现“缩圈”，银行是“缩圈”后的重要阵地”，包含的情绪词典是：高利贷/高利剥削(usury):-0.7,破产/倒闭(bankruptcy):-1.0"}, "四大行股价接连创下新高后，上周银行板块页自周三开始连续调整，或是“物极必反”的体现": {"topic": "“金融”", "similarity": 0.623806893825531, "prompt": "新闻文本是“四大行股价接连创下新高后，上周银行板块页自周三开始连续调整，或是“物极必反”的体现”，包含的情绪词典是：银行/河岸(bank):0.0,暴跌/衰退(slump):-0.7"}, "在此判断下，虽然中长期持续看好抵抗内外需双弱的港股高股息、黄金与船舶，但目前在内外流动性有望边际缓解、风格转换迹象初现的时点，更应强调确定性的成长，建议关注受益AI发展与全球科技上行周期下的互联网、光模块、果链，以及受益于亚非拉新兴市场爆发的逆变器、变压器": {"topic": "“金融”", "similarity": 0.662175178527832, "prompt": "新闻文本是“在此判断下，虽然中长期持续看好抵抗内外需双弱的港股高股息、黄金与船舶，但目前在内外流动性有望边际缓解、风格转换迹象初现的时点，更应强调确定性的成长，建议关注受益AI发展与全球科技上行周期下的互联网、光模块、果链，以及受益于亚非拉新兴市场爆发的逆变器、变压器”，包含的情绪词典是：好转/向上趋势(upturn):0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "东莞证券表示，上周五指数集体反弹，创业板相对更加强势，全市场超4600只股票收红，电子、房地产、传媒、非银金融等板块表现突出": {"topic": "“金融”", "similarity": 0.6633259654045105, "prompt": "新闻文本是“东莞证券表示，上周五指数集体反弹，创业板相对更加强势，全市场超4600只股票收红，电子、房地产、传媒、非银金融等板块表现突出”，包含的情绪词典是：反弹/回升(rebounding):0.3,反弹/回升(rebound):0.1"}, "从技术面来看，创业板指日线形态已形成反弹格局，盘中强势站上10日均线，后续投资者需观察创业板指能否站稳20日均线": {"topic": "“金融”", "similarity": 0.6467316150665283, "prompt": "新闻文本是“从技术面来看，创业板指日线形态已形成反弹格局，盘中强势站上10日均线，后续投资者需观察创业板指能否站稳20日均线”，包含的情绪词典是：反弹/回升(rebounding):0.3,反弹/回升(rebound):0.1"}, "从盘面上来看，前期强势的红利股的连续回调，或使资金进入其他相对低位的板块和个股，如创业板和中小盘个股，短期投资者宜规避高位调整的红利股，多关注前期处于低位，基本面较好的个股": {"topic": "“金融”", "similarity": 0.6782940626144409, "prompt": "新闻文本是“从盘面上来看，前期强势的红利股的连续回调，或使资金进入其他相对低位的板块和个股，如创业板和中小盘个股，短期投资者宜规避高位调整的红利股，多关注前期处于低位，基本面较好的个股”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,处于优势的/有利的(advantaged):0.7"}, "另外，央行的会议表示，下半年将研究出台增量政策举措，宏观政策将持续发力，且发力力度更大，同时考虑到即将进入金九银十传统旺季，市场或将走出一波反弹行情": {"topic": "“金融”", "similarity": 0.6864612102508545, "prompt": "新闻文本是“另外，央行的会议表示，下半年将研究出台增量政策举措，宏观政策将持续发力，且发力力度更大，同时考虑到即将进入金九银十传统旺季，市场或将走出一波反弹行情”，包含的情绪词典是：反弹/回升(rebounding):0.3,货币/通货(currency):0.0"}}</t>
+          <t>{"东方财富Choice数据显示，上周（8月26日-8月30日），场内股票型ETF净申购145.57亿份": {"topic": "“金融”", "similarity": 0.518425703048706, "prompt": "新闻文本是“东方财富Choice数据显示，上周（8月26日-8月30日），场内股票型ETF净申购145.57亿份”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "其中，沪市股票型ETF净申购124.60亿份，深市股票型ETF净申购20.97亿份": {"topic": "“金融”", "similarity": 0.5551955103874207, "prompt": "新闻文本是“其中，沪市股票型ETF净申购124.60亿份，深市股票型ETF净申购20.97亿份”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "以最新净值计，上周净申购金额达413.94亿元": {"topic": "“金融”", "similarity": 0.5151727795600891, "prompt": "新闻文本是“以最新净值计，上周净申购金额达413.94亿元”，包含的情绪词典是：投资/投资额(investment):0.4,营业额/周转(turnover):0.0"}, "游戏动漫ETF领涨 　　数据显示，上周场内股票型ETF中，游戏动漫ETF、游戏ETF（159869.SZ）、游戏ETF（516010.SH）涨幅靠前": {"topic": "“金融”", "similarity": 0.5780243873596191, "prompt": "新闻文本是“游戏动漫ETF领涨 　　数据显示，上周场内股票型ETF中，游戏动漫ETF、游戏ETF（159869.SZ）、游戏ETF（516010.SH）涨幅靠前”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "沪深300ETF申购最多 　　上周净申购金额最多的为沪深300 ETF，净申购金额131.92亿元": {"topic": "“金融”", "similarity": 0.5780248045921326, "prompt": "新闻文本是“沪深300ETF申购最多 　　上周净申购金额最多的为沪深300 ETF，净申购金额131.92亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "此外，沪深300ETF易方达和中证1000ETF也获申购居前，净申购金额依次为90.47亿元和43.75亿元": {"topic": "“金融”", "similarity": 0.5738051533699036, "prompt": "新闻文本是“此外，沪深300ETF易方达和中证1000ETF也获申购居前，净申购金额依次为90.47亿元和43.75亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "中证500ETF易方达遭赎回 　　数据还显示，上周净赎回金额最多的场内股票ETF为中证500ETF易方达，赎回金额18.28亿元": {"topic": "“金融”", "similarity": 0.563094973564148, "prompt": "新闻文本是“中证500ETF易方达遭赎回 　　数据还显示，上周净赎回金额最多的场内股票ETF为中证500ETF易方达，赎回金额18.28亿元”，包含的情绪词典是：清仓/抛售(closeouts):-0.2,清仓/抛售(closeout):-0.2"}, "沪深300ETF基金紧随其后，赎回金额3.44亿元": {"topic": "“金融”", "similarity": 0.5447781085968018, "prompt": "新闻文本是“沪深300ETF基金紧随其后，赎回金额3.44亿元”，包含的情绪词典是：基金/资金(fund):0.1,撤资/抛售(divestment):-0.2"}, "机构看后市 　　华福证券认为，抵抗内外需双弱的同时，更应强调确定性的成长": {"topic": "“金融”", "similarity": 0.5793376564979553, "prompt": "新闻文本是“机构看后市 　　华福证券认为，抵抗内外需双弱的同时，更应强调确定性的成长”，包含的情绪词典是：表现不佳/业绩低于预期(underperforms):-0.4,稳定的/稳固的(stable):0.5"}, "六月以来红利指数持续回调，高股息出现“缩圈”，银行是“缩圈”后的重要阵地": {"topic": "“金融”", "similarity": 0.6011202335357666, "prompt": "新闻文本是“六月以来红利指数持续回调，高股息出现“缩圈”，银行是“缩圈”后的重要阵地”，包含的情绪词典是：高利贷/高利剥削(usury):-0.7,破产/倒闭(bankruptcy):-1.0"}, "四大行股价接连创下新高后，上周银行板块页自周三开始连续调整，或是“物极必反”的体现": {"topic": "“金融”", "similarity": 0.6238069534301758, "prompt": "新闻文本是“四大行股价接连创下新高后，上周银行板块页自周三开始连续调整，或是“物极必反”的体现”，包含的情绪词典是：银行/河岸(bank):0.0,暴跌/衰退(slump):-0.7"}, "东莞证券表示，上周五指数集体反弹，创业板相对更加强势，全市场超4600只股票收红，电子、房地产、传媒、非银金融等板块表现突出": {"topic": "“金融”", "similarity": 0.6633260846138, "prompt": "新闻文本是“东莞证券表示，上周五指数集体反弹，创业板相对更加强势，全市场超4600只股票收红，电子、房地产、传媒、非银金融等板块表现突出”，包含的情绪词典是：反弹/回升(rebounding):0.3,反弹/回升(rebound):0.1"}, "从技术面来看，创业板指日线形态已形成反弹格局，盘中强势站上10日均线，后续投资者需观察创业板指能否站稳20日均线": {"topic": "“金融”", "similarity": 0.6467316150665283, "prompt": "新闻文本是“从技术面来看，创业板指日线形态已形成反弹格局，盘中强势站上10日均线，后续投资者需观察创业板指能否站稳20日均线”，包含的情绪词典是：反弹/回升(rebounding):0.3,反弹/回升(rebound):0.1"}, "从盘面上来看，前期强势的红利股的连续回调，或使资金进入其他相对低位的板块和个股，如创业板和中小盘个股，短期投资者宜规避高位调整的红利股，多关注前期处于低位，基本面较好的个股": {"topic": "“金融”", "similarity": 0.67829430103302, "prompt": "新闻文本是“从盘面上来看，前期强势的红利股的连续回调，或使资金进入其他相对低位的板块和个股，如创业板和中小盘个股，短期投资者宜规避高位调整的红利股，多关注前期处于低位，基本面较好的个股”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,处于优势的/有利的(advantaged):0.7"}, "另外，央行的会议表示，下半年将研究出台增量政策举措，宏观政策将持续发力，且发力力度更大，同时考虑到即将进入金九银十传统旺季，市场或将走出一波反弹行情": {"topic": "“金融”", "similarity": 0.686461329460144, "prompt": "新闻文本是“另外，央行的会议表示，下半年将研究出台增量政策举措，宏观政策将持续发力，且发力力度更大，同时考虑到即将进入金九银十传统旺季，市场或将走出一波反弹行情”，包含的情绪词典是：反弹/回升(rebounding):0.3,货币/通货(currency):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3212,12 +3188,12 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "手术机器人龙头微创机器人（02252.HK）发布最新财报", "news_prompt2": "得益于核心产品公司“图迈腔镜手术机器人”销售增长，2024年上半年收入达0.99亿元，同比增长108.5%", "news_prompt3": "通过大幅度的成本削减，公司上半年的净亏损已从2023年同期的人民币5.45亿元降至2.80亿元", "news_prompt4": "削减成本的成果包括行政开支同比下降61.2%、研发成本下降了47.3%", "news_prompt5": "此外，按权益法入账的被投资公司亏损也有所减少，今年上半年亏损980万元，下降41.6%", "news_prompt6": "不过微创机器人针对其投资公司Robocath的股权投资进行了减值测试，并因Robocath商业化进程的延迟及近期财务表现不佳，计提了约1570万元减值准备", "news_prompt7": "起主要推动作用的是图迈腔镜手术机器人，即微创机器人的核心产品", "news_prompt8": "根据披露，目前图迈在国内市场实现20家医院的商业化安装，居国产腔镜手术机器人市场份额第一", "news_prompt9": "图迈已通过NMPA批准，覆盖多科室应用，截至报告期，图迈已在国内完成超过1,300例的临床手术", "news_prompt10": "海外方面，2024年5月，图迈成功获得欧盟CE认证，成为第一且唯一获得此认证的国产腔镜手术机器人", "news_prompt11": "随后，图迈在海外市场也取得突破，成功完成了首两台商业化安装，海外市场订单累计超过十台", "news_prompt12": "公司已在全球范围内建立了近40家图迈临床应用及培训中心，并在报告期内完成了超过百人次的主刀医生认证培训", "news_prompt13": "此外，新推广的R-ONE血管介入机器人上半年在中国市场实现了首两台商业化安装，展示了公司在血管领域的技术布局", "news_prompt14": "目前微创机器人其他还核心品种包括：图迈单臂腔镜手术机器人（机器臂设计灵活，适应狭小空间操作，实现七个自由度，提供比多臂机器人更精细的操作能力，目前已处于NMPA审核阶段）、蜻蜓眼（作高分辨率的三维电子腹腔内窺镜，提供三维立体的手术视野，2021年获得NMPA上市注册证）、鸿鹄骨科手术机器人（集成了个性化手术规划和精确手术执行的骨科手术机器人系统，已经获得了包括FDA的510(k)认证、欧盟CE认证等多国认证）等", "news_prompt15": "尽管微创机器人已经上市并在研项目推进良好，但市场推广、研发活动及规模化生产等均依赖持续投入，目前财务仍面临较大压力", "news_prompt16": "如微创机器人现金及现金等价物从2023年底的5.08亿元减少至2024年中的2.21亿元", "news_prompt17": "短期内，公司融资需求迫切", "news_prompt18": "此外截至2024年6月30日，微创机器人的存货总额为2.43亿元，表明公司产品销售或不及预期", "news_prompt19": "手术机器人行业在中国仍处于早期发展阶段，且享受政策红利，具有巨大的成长空间", "news_prompt20": "根据“十四五”国民健康规划，中国政府鼓励医疗领域前沿技术和突破，支持高端医疗设备的自主创新和商业化", "news_prompt21": "2023年政府发布的大型医用设备配置许可管理目录以及“十四五”大型医用设备配置规划的通知，都明确提升了腹腔内窥镜手术系统的配置数量", "news_prompt22": "通过结合5G通讯和人工智能等新技术，中国国产手术机器人已在核心技术上取得重大突破，增强了其市场竞争力", "news_prompt23": "随着国际化战略的推动，鼓励企业“走出去”，参与全球市场竞争，预计将加速国产手术机器人在国际市场的拓展", "news_prompt24": "公司产品在海外市场表现值得关注", "news_prompt25": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "此外，按权益法入账的被投资公司亏损也有所减少，今年上半年亏损980万元，下降41.6%", "news_prompt2": "起主要推动作用的是图迈腔镜手术机器人，即微创机器人的核心产品", "news_prompt3": "根据披露，目前图迈在国内市场实现20家医院的商业化安装，居国产腔镜手术机器人市场份额第一", "news_prompt4": "尽管微创机器人已经上市并在研项目推进良好，但市场推广、研发活动及规模化生产等均依赖持续投入，目前财务仍面临较大压力", "news_prompt5": "如微创机器人现金及现金等价物从2023年底的5.08亿元减少至2024年中的2.21亿元", "news_prompt6": "短期内，公司融资需求迫切", "news_prompt7": "手术机器人行业在中国仍处于早期发展阶段，且享受政策红利，具有巨大的成长空间", "news_prompt8": "通过结合5G通讯和人工智能等新技术，中国国产手术机器人已在核心技术上取得重大突破，增强了其市场竞争力", "news_prompt9": "随着国际化战略的推动，鼓励企业“走出去”，参与全球市场竞争，预计将加速国产手术机器人在国际市场的拓展", "news_prompt10": "公司产品在海外市场表现值得关注"}</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>{"得益于核心产品公司“图迈腔镜手术机器人”销售增长，2024年上半年收入达0.99亿元，同比增长108.5%": {"topic": "“生产投资”", "similarity": 0.47469955682754517}, "此外，按权益法入账的被投资公司亏损也有所减少，今年上半年亏损980万元，下降41.6%": {"topic": "“金融”", "similarity": 0.43016910552978516, "prompt": "新闻文本是“此外，按权益法入账的被投资公司亏损也有所减少，今年上半年亏损980万元，下降41.6%”，包含的情绪词典是：减少/降低(reduction):-0.4,损失/亏损(loss):-0.7"}, "起主要推动作用的是图迈腔镜手术机器人，即微创机器人的核心产品": {"topic": "“生产投资”", "similarity": 0.5131797790527344, "prompt": "新闻文本是“起主要推动作用的是图迈腔镜手术机器人，即微创机器人的核心产品”，包含的情绪词典是：机械/机器(machinery):0.0,创新/革新(innovation):0.7"}, "根据披露，目前图迈在国内市场实现20家医院的商业化安装，居国产腔镜手术机器人市场份额第一": {"topic": "“生产投资”", "similarity": 0.49441415071487427, "prompt": "新闻文本是“根据披露，目前图迈在国内市场实现20家医院的商业化安装，居国产腔镜手术机器人市场份额第一”，包含的情绪词典是：机械/机器(machinery):0.0,技术的/工艺的(technical):0.0"}, "海外方面，2024年5月，图迈成功获得欧盟CE认证，成为第一且唯一获得此认证的国产腔镜手术机器人": {"topic": "“生产投资”", "similarity": 0.48013046383857727}, "目前微创机器人其他还核心品种包括：图迈单臂腔镜手术机器人（机器臂设计灵活，适应狭小空间操作，实现七个自由度，提供比多臂机器人更精细的操作能力，目前已处于NMPA审核阶段）、蜻蜓眼（作高分辨率的三维电子腹腔内窺镜，提供三维立体的手术视野，2021年获得NMPA上市注册证）、鸿鹄骨科手术机器人（集成了个性化手术规划和精确手术执行的骨科手术机器人系统，已经获得了包括FDA的510(k)认证、欧盟CE认证等多国认证）等": {"topic": "“生产投资”", "similarity": 0.49256575107574463}, "尽管微创机器人已经上市并在研项目推进良好，但市场推广、研发活动及规模化生产等均依赖持续投入，目前财务仍面临较大压力": {"topic": "“生产投资”", "similarity": 0.5132296681404114, "prompt": "新闻文本是“尽管微创机器人已经上市并在研项目推进良好，但市场推广、研发活动及规模化生产等均依赖持续投入，目前财务仍面临较大压力”，包含的情绪词典是：机械/机器(machinery):0.0,发明/创造(invention):0.4"}, "如微创机器人现金及现金等价物从2023年底的5.08亿元减少至2024年中的2.21亿元": {"topic": "“生产投资”", "similarity": 0.4605702757835388, "prompt": "新闻文本是“如微创机器人现金及现金等价物从2023年底的5.08亿元减少至2024年中的2.21亿元”，包含的情绪词典是：减少/降低(reduction):-0.4,贬值/减值(devaluation):-0.5"}, "短期内，公司融资需求迫切": {"topic": "“金融”", "similarity": 0.5708293914794922, "prompt": "新闻文本是“短期内，公司融资需求迫切”，包含的情绪词典是：需求/要求(demand):0.0,需要/需求(need):0.0"}, "手术机器人行业在中国仍处于早期发展阶段，且享受政策红利，具有巨大的成长空间": {"topic": "“生产投资”", "similarity": 0.515247106552124, "prompt": "新闻文本是“手术机器人行业在中国仍处于早期发展阶段，且享受政策红利，具有巨大的成长空间”，包含的情绪词典是：初期的/未发展的(inchoate):0.0,早期的/初期的(early):0.05"}, "根据“十四五”国民健康规划，中国政府鼓励医疗领域前沿技术和突破，支持高端医疗设备的自主创新和商业化": {"topic": "“生产投资”", "similarity": 0.5285881757736206}, "2023年政府发布的大型医用设备配置许可管理目录以及“十四五”大型医用设备配置规划的通知，都明确提升了腹腔内窥镜手术系统的配置数量": {"topic": "“生产投资”", "similarity": 0.5089854598045349}, "通过结合5G通讯和人工智能等新技术，中国国产手术机器人已在核心技术上取得重大突破，增强了其市场竞争力": {"topic": "“生产投资”", "similarity": 0.5696600079536438, "prompt": "新闻文本是“通过结合5G通讯和人工智能等新技术，中国国产手术机器人已在核心技术上取得重大突破，增强了其市场竞争力”，包含的情绪词典是：突破/重大进展(breakthrough):0.5,技术(tech):0.0"}, "随着国际化战略的推动，鼓励企业“走出去”，参与全球市场竞争，预计将加速国产手术机器人在国际市场的拓展": {"topic": "“生产投资”", "similarity": 0.5704113245010376, "prompt": "新闻文本是“随着国际化战略的推动，鼓励企业“走出去”，参与全球市场竞争，预计将加速国产手术机器人在国际市场的拓展”，包含的情绪词典是：海外的/国外的(overseas):0.0,国际的/国际关系的(international):0.0"}, "公司产品在海外市场表现值得关注": {"topic": "“生产投资”", "similarity": 0.49333876371383667, "prompt": "新闻文本是“公司产品在海外市场表现值得关注”，包含的情绪词典是：海外的/国外的(overseas):0.0,跑赢/表现优于(outperform):0.65"}}</t>
+          <t>{"此外，按权益法入账的被投资公司亏损也有所减少，今年上半年亏损980万元，下降41.6%": {"topic": "“金融”", "similarity": 0.4301692545413971, "prompt": "新闻文本是“此外，按权益法入账的被投资公司亏损也有所减少，今年上半年亏损980万元，下降41.6%”，包含的情绪词典是：减少/降低(reduction):-0.4,损失/亏损(loss):-0.7"}, "起主要推动作用的是图迈腔镜手术机器人，即微创机器人的核心产品": {"topic": "“生产投资”", "similarity": 0.5131798982620239, "prompt": "新闻文本是“起主要推动作用的是图迈腔镜手术机器人，即微创机器人的核心产品”，包含的情绪词典是：机械/机器(machinery):0.0,创新/革新(innovation):0.7"}, "根据披露，目前图迈在国内市场实现20家医院的商业化安装，居国产腔镜手术机器人市场份额第一": {"topic": "“生产投资”", "similarity": 0.49441415071487427, "prompt": "新闻文本是“根据披露，目前图迈在国内市场实现20家医院的商业化安装，居国产腔镜手术机器人市场份额第一”，包含的情绪词典是：机械/机器(machinery):0.0,技术的/工艺的(technical):0.0"}, "尽管微创机器人已经上市并在研项目推进良好，但市场推广、研发活动及规模化生产等均依赖持续投入，目前财务仍面临较大压力": {"topic": "“生产投资”", "similarity": 0.5132299065589905, "prompt": "新闻文本是“尽管微创机器人已经上市并在研项目推进良好，但市场推广、研发活动及规模化生产等均依赖持续投入，目前财务仍面临较大压力”，包含的情绪词典是：机械/机器(machinery):0.0,发明/创造(invention):0.4"}, "如微创机器人现金及现金等价物从2023年底的5.08亿元减少至2024年中的2.21亿元": {"topic": "“生产投资”", "similarity": 0.4605705142021179, "prompt": "新闻文本是“如微创机器人现金及现金等价物从2023年底的5.08亿元减少至2024年中的2.21亿元”，包含的情绪词典是：减少/降低(reduction):-0.4,贬值/减值(devaluation):-0.5"}, "短期内，公司融资需求迫切": {"topic": "“金融”", "similarity": 0.5708293914794922, "prompt": "新闻文本是“短期内，公司融资需求迫切”，包含的情绪词典是：需求/要求(demand):0.0,需要/需求(need):0.0"}, "手术机器人行业在中国仍处于早期发展阶段，且享受政策红利，具有巨大的成长空间": {"topic": "“生产投资”", "similarity": 0.5152471661567688, "prompt": "新闻文本是“手术机器人行业在中国仍处于早期发展阶段，且享受政策红利，具有巨大的成长空间”，包含的情绪词典是：初期的/未发展的(inchoate):0.0,早期的/初期的(early):0.05"}, "通过结合5G通讯和人工智能等新技术，中国国产手术机器人已在核心技术上取得重大突破，增强了其市场竞争力": {"topic": "“生产投资”", "similarity": 0.569659948348999, "prompt": "新闻文本是“通过结合5G通讯和人工智能等新技术，中国国产手术机器人已在核心技术上取得重大突破，增强了其市场竞争力”，包含的情绪词典是：突破/重大进展(breakthrough):0.5,技术(tech):0.0"}, "随着国际化战略的推动，鼓励企业“走出去”，参与全球市场竞争，预计将加速国产手术机器人在国际市场的拓展": {"topic": "“生产投资”", "similarity": 0.5704113245010376, "prompt": "新闻文本是“随着国际化战略的推动，鼓励企业“走出去”，参与全球市场竞争，预计将加速国产手术机器人在国际市场的拓展”，包含的情绪词典是：海外的/国外的(overseas):0.0,国际的/国际关系的(international):0.0"}, "公司产品在海外市场表现值得关注": {"topic": "“生产投资”", "similarity": 0.4933386445045471, "prompt": "新闻文本是“公司产品在海外市场表现值得关注”，包含的情绪词典是：海外的/国外的(overseas):0.0,跑赢/表现优于(outperform):0.65"}}</t>
         </is>
       </c>
     </row>
@@ -3263,12 +3239,12 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，双元科技(688623.SH)发布2024年中报", "news_prompt2": "公司营业总收入为1.78亿元，在已披露的同业公司中排名第68，较去年同报告期营业总收入减少5057.60万元，同比较去年同期下降22.10%", "news_prompt3": "归母净利润为5108.36万元，在已披露的同业公司中排名第30，较去年同报告期归母净利润减少990.41万元，同比较去年同期下降16.24%", "news_prompt4": "经营活动现金净流入为-744.15万元，在已披露的同业公司中排名第44，较去年同报告期经营活动现金净流入减少5355.85万元，同比较去年同期下降116.14%", "news_prompt5": "公司最新资产负债率为20.07%，在已披露的同业公司中排名第19，较上季度资产负债率减少1.10个百分点，较去年同季度资产负债率减少3.32个百分点", "news_prompt6": "公司最新毛利率为44.53%，在已披露的同业公司中排名第16，较上季度毛利率减少0.11个百分点，较去年同季度毛利率增加3.14个百分点", "news_prompt7": "最新ROE为2.40%，在已披露的同业公司中排名第42，较去年同季度ROE减少0.49个百分点", "news_prompt8": "公司摊薄每股收益为0.86元，在已披露的同业公司中排名第4，较去年同报告期摊薄每股收益减少0.17元，同比较去年同期下降16.24%", "news_prompt9": "公司最新总资产周转率为0.07次，在已披露的同业公司中排名第81，较去年同季度总资产周转率减少0.06次，同比较去年同期下降47.98%", "news_prompt10": "最新存货周转率为0.21次，在已披露的同业公司中排名第85，较去年同季度存货周转率减少0.15次，同比较去年同期下降41.24%", "news_prompt11": "公司股东户数为9196户，前十大股东持股数量为4507.88万股，占总股本比例为76.22%", "news_prompt12": "前十大股东分别为杭州凯毕特投资管理有限公司、郑建、杭州丰泉汇投资管理合伙企业(有限合伙)、胡美琴、宜宾晨道新能源产业股权投资合伙企业(有限合伙)、无锡蜂云能创企业管理合伙企业(有限合伙)、宁波银泰睿祺创业投资有限公司、民生证券投资有限公司、深圳市德弘联信私募股权基金管理有限公司-金华金开德弘联信毕方贰号投资中心(有限合伙)、惠州市利元亨投资有限公司，持股比例分别为39.21%、12.23%、8.82%、6.86%、3.57%、1.91%、1.33%、0.81%、0.74%、0.74%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为1.78亿元，在已披露的同业公司中排名第68，较去年同报告期营业总收入减少5057.60万元，同比较去年同期下降22.10%", "news_prompt2": "归母净利润为5108.36万元，在已披露的同业公司中排名第30，较去年同报告期归母净利润减少990.41万元，同比较去年同期下降16.24%", "news_prompt3": "经营活动现金净流入为-744.15万元，在已披露的同业公司中排名第44，较去年同报告期经营活动现金净流入减少5355.85万元，同比较去年同期下降116.14%", "news_prompt4": "公司最新资产负债率为20.07%，在已披露的同业公司中排名第19，较上季度资产负债率减少1.10个百分点，较去年同季度资产负债率减少3.32个百分点", "news_prompt5": "公司最新毛利率为44.53%，在已披露的同业公司中排名第16，较上季度毛利率减少0.11个百分点，较去年同季度毛利率增加3.14个百分点", "news_prompt6": "公司摊薄每股收益为0.86元，在已披露的同业公司中排名第4，较去年同报告期摊薄每股收益减少0.17元，同比较去年同期下降16.24%", "news_prompt7": "公司最新总资产周转率为0.07次，在已披露的同业公司中排名第81，较去年同季度总资产周转率减少0.06次，同比较去年同期下降47.98%", "news_prompt8": "最新存货周转率为0.21次，在已披露的同业公司中排名第85，较去年同季度存货周转率减少0.15次，同比较去年同期下降41.24%", "news_prompt9": "公司股东户数为9196户，前十大股东持股数量为4507.88万股，占总股本比例为76.22%"}</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，双元科技(688623.SH)发布2024年中报": {"topic": "“生产投资”", "similarity": 0.4912337362766266, "prompt": "新闻文本是“2024年8月31日，双元科技(688623.SH)发布2024年中报”，包含的情绪词典是：技术(tech):0.0,公司的/企业的(corporate):0.0"}, "公司营业总收入为1.78亿元，在已披露的同业公司中排名第68，较去年同报告期营业总收入减少5057.60万元，同比较去年同期下降22.10%": {"topic": "“消费”", "similarity": 0.5264370441436768, "prompt": "新闻文本是“公司营业总收入为1.78亿元，在已披露的同业公司中排名第68，较去年同报告期营业总收入减少5057.60万元，同比较去年同期下降22.10%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "归母净利润为5108.36万元，在已披露的同业公司中排名第30，较去年同报告期归母净利润减少990.41万元，同比较去年同期下降16.24%": {"topic": "“消费”", "similarity": 0.5130285024642944, "prompt": "新闻文本是“归母净利润为5108.36万元，在已披露的同业公司中排名第30，较去年同报告期归母净利润减少990.41万元，同比较去年同期下降16.24%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为-744.15万元，在已披露的同业公司中排名第44，较去年同报告期经营活动现金净流入减少5355.85万元，同比较去年同期下降116.14%": {"topic": "“金融”", "similarity": 0.5440278053283691, "prompt": "新闻文本是“经营活动现金净流入为-744.15万元，在已披露的同业公司中排名第44，较去年同报告期经营活动现金净流入减少5355.85万元，同比较去年同期下降116.14%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新资产负债率为20.07%，在已披露的同业公司中排名第19，较上季度资产负债率减少1.10个百分点，较去年同季度资产负债率减少3.32个百分点": {"topic": "“消费”", "similarity": 0.47198623418807983, "prompt": "新闻文本是“公司最新资产负债率为20.07%，在已披露的同业公司中排名第19，较上季度资产负债率减少1.10个百分点，较去年同季度资产负债率减少3.32个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新毛利率为44.53%，在已披露的同业公司中排名第16，较上季度毛利率减少0.11个百分点，较去年同季度毛利率增加3.14个百分点": {"topic": "“消费”", "similarity": 0.4373573362827301, "prompt": "新闻文本是“公司最新毛利率为44.53%，在已披露的同业公司中排名第16，较上季度毛利率减少0.11个百分点，较去年同季度毛利率增加3.14个百分点”，包含的情绪词典是：百分比(percentage):0.0,盈利能力/获利能力(profitability):0.6"}, "公司摊薄每股收益为0.86元，在已披露的同业公司中排名第4，较去年同报告期摊薄每股收益减少0.17元，同比较去年同期下降16.24%": {"topic": "“金融”", "similarity": 0.4603797495365143, "prompt": "新闻文本是“公司摊薄每股收益为0.86元，在已披露的同业公司中排名第4，较去年同报告期摊薄每股收益减少0.17元，同比较去年同期下降16.24%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新总资产周转率为0.07次，在已披露的同业公司中排名第81，较去年同季度总资产周转率减少0.06次，同比较去年同期下降47.98%": {"topic": "“消费”", "similarity": 0.5044676661491394, "prompt": "新闻文本是“公司最新总资产周转率为0.07次，在已披露的同业公司中排名第81，较去年同季度总资产周转率减少0.06次，同比较去年同期下降47.98%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "最新存货周转率为0.21次，在已披露的同业公司中排名第85，较去年同季度存货周转率减少0.15次，同比较去年同期下降41.24%": {"topic": "“消费”", "similarity": 0.4475003778934479, "prompt": "新闻文本是“最新存货周转率为0.21次，在已披露的同业公司中排名第85，较去年同季度存货周转率减少0.15次，同比较去年同期下降41.24%”，包含的情绪词典是：营业额/周转(turnover):0.0,周期/循环(cycle):0.0"}, "公司股东户数为9196户，前十大股东持股数量为4507.88万股，占总股本比例为76.22%": {"topic": "“金融”", "similarity": 0.4632147550582886, "prompt": "新闻文本是“公司股东户数为9196户，前十大股东持股数量为4507.88万股，占总股本比例为76.22%”，包含的情绪词典是：百分比(percentage):0.0,公司的/企业的(corporate):0.0"}, "前十大股东分别为杭州凯毕特投资管理有限公司、郑建、杭州丰泉汇投资管理合伙企业(有限合伙)、胡美琴、宜宾晨道新能源产业股权投资合伙企业(有限合伙)、无锡蜂云能创企业管理合伙企业(有限合伙)、宁波银泰睿祺创业投资有限公司、民生证券投资有限公司、深圳市德弘联信私募股权基金管理有限公司-金华金开德弘联信毕方贰号投资中心(有限合伙)、惠州市利元亨投资有限公司，持股比例分别为39.21%、12.23%、8.82%、6.86%、3.57%、1.91%、1.33%、0.81%、0.74%、0.74%": {"topic": "“生产投资”", "similarity": 0.648231029510498}}</t>
+          <t>{"公司营业总收入为1.78亿元，在已披露的同业公司中排名第68，较去年同报告期营业总收入减少5057.60万元，同比较去年同期下降22.10%": {"topic": "“消费”", "similarity": 0.5264371633529663, "prompt": "新闻文本是“公司营业总收入为1.78亿元，在已披露的同业公司中排名第68，较去年同报告期营业总收入减少5057.60万元，同比较去年同期下降22.10%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "归母净利润为5108.36万元，在已披露的同业公司中排名第30，较去年同报告期归母净利润减少990.41万元，同比较去年同期下降16.24%": {"topic": "“消费”", "similarity": 0.5130285024642944, "prompt": "新闻文本是“归母净利润为5108.36万元，在已披露的同业公司中排名第30，较去年同报告期归母净利润减少990.41万元，同比较去年同期下降16.24%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为-744.15万元，在已披露的同业公司中排名第44，较去年同报告期经营活动现金净流入减少5355.85万元，同比较去年同期下降116.14%": {"topic": "“金融”", "similarity": 0.5440279245376587, "prompt": "新闻文本是“经营活动现金净流入为-744.15万元，在已披露的同业公司中排名第44，较去年同报告期经营活动现金净流入减少5355.85万元，同比较去年同期下降116.14%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新资产负债率为20.07%，在已披露的同业公司中排名第19，较上季度资产负债率减少1.10个百分点，较去年同季度资产负债率减少3.32个百分点": {"topic": "“消费”", "similarity": 0.4719863533973694, "prompt": "新闻文本是“公司最新资产负债率为20.07%，在已披露的同业公司中排名第19，较上季度资产负债率减少1.10个百分点，较去年同季度资产负债率减少3.32个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新毛利率为44.53%，在已披露的同业公司中排名第16，较上季度毛利率减少0.11个百分点，较去年同季度毛利率增加3.14个百分点": {"topic": "“消费”", "similarity": 0.43735742568969727, "prompt": "新闻文本是“公司最新毛利率为44.53%，在已披露的同业公司中排名第16，较上季度毛利率减少0.11个百分点，较去年同季度毛利率增加3.14个百分点”，包含的情绪词典是：百分比(percentage):0.0,盈利能力/获利能力(profitability):0.6"}, "公司摊薄每股收益为0.86元，在已披露的同业公司中排名第4，较去年同报告期摊薄每股收益减少0.17元，同比较去年同期下降16.24%": {"topic": "“金融”", "similarity": 0.4603798985481262, "prompt": "新闻文本是“公司摊薄每股收益为0.86元，在已披露的同业公司中排名第4，较去年同报告期摊薄每股收益减少0.17元，同比较去年同期下降16.24%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新总资产周转率为0.07次，在已披露的同业公司中排名第81，较去年同季度总资产周转率减少0.06次，同比较去年同期下降47.98%": {"topic": "“消费”", "similarity": 0.5044678449630737, "prompt": "新闻文本是“公司最新总资产周转率为0.07次，在已披露的同业公司中排名第81，较去年同季度总资产周转率减少0.06次，同比较去年同期下降47.98%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "最新存货周转率为0.21次，在已披露的同业公司中排名第85，较去年同季度存货周转率减少0.15次，同比较去年同期下降41.24%": {"topic": "“消费”", "similarity": 0.4475005269050598, "prompt": "新闻文本是“最新存货周转率为0.21次，在已披露的同业公司中排名第85，较去年同季度存货周转率减少0.15次，同比较去年同期下降41.24%”，包含的情绪词典是：营业额/周转(turnover):0.0,周期/循环(cycle):0.0"}, "公司股东户数为9196户，前十大股东持股数量为4507.88万股，占总股本比例为76.22%": {"topic": "“金融”", "similarity": 0.4632149338722229, "prompt": "新闻文本是“公司股东户数为9196户，前十大股东持股数量为4507.88万股，占总股本比例为76.22%”，包含的情绪词典是：百分比(percentage):0.0,公司的/企业的(corporate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3318,12 +3294,12 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "证券时报网讯，8月30日，科创板两融余额合计856.63亿元，较上一交易日增加3.78亿元", "news_prompt2": "其中，融资余额合计850.09亿元，较上一交易日增加3.65亿元", "news_prompt3": "融券余额合计6.54亿元，较上一交易日增加0.13亿元", "news_prompt4": "（文章来源：证券时报网）"}</t>
+          <t>{"news_prompt1": "其中，融资余额合计850.09亿元，较上一交易日增加3.65亿元", "news_prompt2": "融券余额合计6.54亿元，较上一交易日增加0.13亿元"}</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，8月30日，科创板两融余额合计856.63亿元，较上一交易日增加3.78亿元": {"topic": "“金融”", "similarity": 0.5618448257446289}, "其中，融资余额合计850.09亿元，较上一交易日增加3.65亿元": {"topic": "“金融”", "similarity": 0.5347426533699036, "prompt": "新闻文本是“其中，融资余额合计850.09亿元，较上一交易日增加3.65亿元”，包含的情绪词典是：投资/投资额(investment):0.4,资本/资金(capital):0.1"}, "融券余额合计6.54亿元，较上一交易日增加0.13亿元": {"topic": "“金融”", "similarity": 0.5068063735961914, "prompt": "新闻文本是“融券余额合计6.54亿元，较上一交易日增加0.13亿元”，包含的情绪词典是：增加/增长(increase):0.6,投资/投资额(investment):0.4"}, "（文章来源：证券时报网）": {"topic": "“金融”", "similarity": 0.4481872320175171, "prompt": "新闻文本是“（文章来源：证券时报网）”，包含的情绪词典是：股票/库存(stock):0.0,资本/资金(capital):0.1"}}</t>
+          <t>{"其中，融资余额合计850.09亿元，较上一交易日增加3.65亿元": {"topic": "“金融”", "similarity": 0.5347427129745483, "prompt": "新闻文本是“其中，融资余额合计850.09亿元，较上一交易日增加3.65亿元”，包含的情绪词典是：投资/投资额(investment):0.4,资本/资金(capital):0.1"}, "融券余额合计6.54亿元，较上一交易日增加0.13亿元": {"topic": "“金融”", "similarity": 0.506806492805481, "prompt": "新闻文本是“融券余额合计6.54亿元，较上一交易日增加0.13亿元”，包含的情绪词典是：增加/增长(increase):0.6,投资/投资额(investment):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -3369,12 +3345,12 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日上午，白酒股震荡走低，泸州老窖跌超4%，山西汾酒、金徽酒、酒鬼酒、迎驾贡酒、舍得酒业、水井坊等跟跌", "news_prompt2": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "9月2日上午，白酒股震荡走低，泸州老窖跌超4%，山西汾酒、金徽酒、酒鬼酒、迎驾贡酒、舍得酒业、水井坊等跟跌"}</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>{"9月2日上午，白酒股震荡走低，泸州老窖跌超4%，山西汾酒、金徽酒、酒鬼酒、迎驾贡酒、舍得酒业、水井坊等跟跌": {"topic": "“金融”", "similarity": 0.5316798090934753, "prompt": "新闻文本是“9月2日上午，白酒股震荡走低，泸州老窖跌超4%，山西汾酒、金徽酒、酒鬼酒、迎驾贡酒、舍得酒业、水井坊等跟跌”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}}</t>
+          <t>{"9月2日上午，白酒股震荡走低，泸州老窖跌超4%，山西汾酒、金徽酒、酒鬼酒、迎驾贡酒、舍得酒业、水井坊等跟跌": {"topic": "“金融”", "similarity": 0.5316799879074097, "prompt": "新闻文本是“9月2日上午，白酒股震荡走低，泸州老窖跌超4%，山西汾酒、金徽酒、酒鬼酒、迎驾贡酒、舍得酒业、水井坊等跟跌”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -3420,12 +3396,12 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月30日，中证2000ETF基金(159533.SZ)收涨2.17%，成交120.05万元", "news_prompt2": "净流出536.70万元（净赎回份额*单位净值），居可比基金首位", "news_prompt3": "拉长时间看，该基金连续3天资金净流出，累计流出1585.14万元，居可比基金首位", "news_prompt4": "资金流出也带来了份额的减少，该基金最新份额较前一日减少600.00万份，跌破4400.00万份，居可比基金后排", "news_prompt5": "与此同时，该基金最新规模跌破3900.00万元", "news_prompt6": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "2024年8月30日，中证2000ETF基金(159533.SZ)收涨2.17%，成交120.05万元", "news_prompt2": "净流出536.70万元（净赎回份额*单位净值），居可比基金首位", "news_prompt3": "拉长时间看，该基金连续3天资金净流出，累计流出1585.14万元，居可比基金首位", "news_prompt4": "资金流出也带来了份额的减少，该基金最新份额较前一日减少600.00万份，跌破4400.00万份，居可比基金后排", "news_prompt5": "与此同时，该基金最新规模跌破3900.00万元"}</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>{"2024年8月30日，中证2000ETF基金(159533.SZ)收涨2.17%，成交120.05万元": {"topic": "“金融”", "similarity": 0.5230659246444702, "prompt": "新闻文本是“2024年8月30日，中证2000ETF基金(159533.SZ)收涨2.17%，成交120.05万元”，包含的情绪词典是：基金/资金(fund):0.1,股票/库存(stock):0.0"}, "净流出536.70万元（净赎回份额*单位净值），居可比基金首位": {"topic": "“金融”", "similarity": 0.506809651851654, "prompt": "新闻文本是“净流出536.70万元（净赎回份额*单位净值），居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeout):-0.2"}, "拉长时间看，该基金连续3天资金净流出，累计流出1585.14万元，居可比基金首位": {"topic": "“金融”", "similarity": 0.5396890640258789, "prompt": "新闻文本是“拉长时间看，该基金连续3天资金净流出，累计流出1585.14万元，居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeouts):-0.2"}, "资金流出也带来了份额的减少，该基金最新份额较前一日减少600.00万份，跌破4400.00万份，居可比基金后排": {"topic": "“金融”", "similarity": 0.5840692520141602, "prompt": "新闻文本是“资金流出也带来了份额的减少，该基金最新份额较前一日减少600.00万份，跌破4400.00万份，居可比基金后排”，包含的情绪词典是：下跌/下降(fall):-0.6,资金不足的(underfunded):-0.3"}, "与此同时，该基金最新规模跌破3900.00万元": {"topic": "“金融”", "similarity": 0.4516943097114563, "prompt": "新闻文本是“与此同时，该基金最新规模跌破3900.00万元”，包含的情绪词典是：下跌/下降(fall):-0.6,暴跌/衰退(slump):-0.7"}}</t>
+          <t>{"2024年8月30日，中证2000ETF基金(159533.SZ)收涨2.17%，成交120.05万元": {"topic": "“金融”", "similarity": 0.5230660438537598, "prompt": "新闻文本是“2024年8月30日，中证2000ETF基金(159533.SZ)收涨2.17%，成交120.05万元”，包含的情绪词典是：基金/资金(fund):0.1,股票/库存(stock):0.0"}, "净流出536.70万元（净赎回份额*单位净值），居可比基金首位": {"topic": "“金融”", "similarity": 0.5068097710609436, "prompt": "新闻文本是“净流出536.70万元（净赎回份额*单位净值），居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeout):-0.2"}, "拉长时间看，该基金连续3天资金净流出，累计流出1585.14万元，居可比基金首位": {"topic": "“金融”", "similarity": 0.539689302444458, "prompt": "新闻文本是“拉长时间看，该基金连续3天资金净流出，累计流出1585.14万元，居可比基金首位”，包含的情绪词典是：基金/资金(fund):0.1,清仓/抛售(closeouts):-0.2"}, "资金流出也带来了份额的减少，该基金最新份额较前一日减少600.00万份，跌破4400.00万份，居可比基金后排": {"topic": "“金融”", "similarity": 0.5840693116188049, "prompt": "新闻文本是“资金流出也带来了份额的减少，该基金最新份额较前一日减少600.00万份，跌破4400.00万份，居可比基金后排”，包含的情绪词典是：下跌/下降(fall):-0.6,资金不足的(underfunded):-0.3"}, "与此同时，该基金最新规模跌破3900.00万元": {"topic": "“金融”", "similarity": 0.4516943693161011, "prompt": "新闻文本是“与此同时，该基金最新规模跌破3900.00万元”，包含的情绪词典是：下跌/下降(fall):-0.6,暴跌/衰退(slump):-0.7"}}</t>
         </is>
       </c>
     </row>
@@ -3471,12 +3447,12 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "21世纪经济报道记者高江虹实习生张亿珍北京报道 　　8月结束，各企业财报陆续发出", "news_prompt2": "在备受瞩目的业务方面，Lululemon增长放缓，未来能否继续“长红”受到关注", "news_prompt3": "Brunello Cucinelli营业利润大涨", "news_prompt4": "Gap误发财报后停牌", "news_prompt5": "Birkenstock第三季度收入创历史新高，股价反跌14%", "news_prompt6": "市场风云变幻莫测", "news_prompt7": "同时，各项文化活动、贸易展会以及时装周都在悄悄预热", "news_prompt8": "第四届“钟表与奇迹”高级钟表展在上海开幕", "news_prompt9": "“迪奥倾世之金”展览亮相北京", "news_prompt10": "巴黎时装周预热展会准备就绪", "news_prompt11": "eBay也宣布将举办二手时装周", "news_prompt12": "另外，上周凯悦酒店集团宣布了一起新收购，宝诗龙官宣TWICE组合成员Mina为品牌代言人，维密秀也将于10月回归", "news_prompt13": "1. 增长放缓", "news_prompt14": "Lululemon下调年度预测 　　8月29日，Lululemon公布了2024财年第二季度财报，全球净营收同比增长7%，相较上年同季度的18%，增长明显放缓", "news_prompt15": "从地区上看，2024财年第二季度国际市场净营收同比增长29%", "news_prompt16": "lululemon最大的北美市场净营收增长1%，可比销售额下降3%", "news_prompt17": "在第二季度财报发布后的电话会议上，有分析师询问lululemon女装领域的核心客户是否发生了变化", "news_prompt18": "其品牌首席执行官Calvin McDonald表示，“如果你想按年龄人口结构来划分，我想我过去已经提到过了", "news_prompt19": "对于不同年龄段的人群，我们继续在所有这些人群中招募新客人……我们将继续招募和获取客人，这意味着真正跨越年龄和规模", "news_prompt20": "” 　　点评：除中国市场增长34%外，Lululemon在其他市场的表现似乎都不理想", "news_prompt21": "同时，Breezethrough产品的突然下架以及环保质疑风波都让其面临压力", "news_prompt22": "洞察市场，不断调整，扩展产品矩阵……想重造增长神话，企业要做的还很多", "news_prompt23": "2. Brunello Cucinelli上半年营业利润大涨19% 　　8月28日，意大利奢侈品集团Brunello Cucinelli发布上半年财务报告，期内，其营业利润增长19.3%，达到 1.046 亿欧元", "news_prompt24": "执行主席 Brunello Cucinelli表示，品牌非常成功地完成了 2024 年夏季销售，冬季销售也取得了非常好的开局", "news_prompt25": "在上个月，该集团就已报告称，由于亚洲和美洲的两位数增长，其上半年收入按固定汇率计算增长了14.7％", "news_prompt26": "点评：奢侈品市场竞争日趋白热化，Cucinelli是否有足够的创新和品牌忠诚度来继续抵御未来的不确定性", "news_prompt27": "3. 第四届“钟表与奇迹”高级钟表展在上海开幕 　　8月28日，2024第四届“钟表与奇迹”高级钟表展正式于上海西岸艺术中心开幕，展出品牌包括朗格（A. LANGE &amp; SHNE）、名士表（BAUME &amp; MERCIER） 、 卡地亚（CARTIER）、IWC万国表（IWC SCHAFFHAUSEN）、 NOMOS GLASHTTE 、沛纳海（PANERAI）、伯爵（PIAGET）、罗杰杜彼（ROGER DUBUIS）、江诗丹顿（VACHERON CONSTANTIN）9家高级制表品牌在内", "news_prompt28": "本次展会的开放时间为8月28日至9月1日，前两日仅面向专业人士开放，随后首次对公众开放三天", "news_prompt29": "据官方统计数据，25%的公众日门票由25岁以下的人年轻人购买，整体购票人群的平均年龄为35岁", "news_prompt30": "点评：刚刚过去的7月已经是瑞士钟表在华业绩持续下跌的第七个月，在钟表遇冷的当下，此类展会或可保持人们对制表业的热情，并提高大众对于制表师作品的认知", "news_prompt31": "4. “迪奥倾世之金”展览亮相北京 　　9月2日至29日，迪奥将于北京嘉德艺术中心举办“迪奥倾世之金” (L'OR DE DIOR)展览", "news_prompt32": "在使用“金色”这一贯穿迪奥品牌历史的经典传承元素的同时，以崭新的场景叙事，传递其象征力量与魅力", "news_prompt33": "据悉，展览将带来品牌创始人克里斯汀·迪奥 (CHRISTIAN DIOR)及其继任创意总监在“金色”的灵感启迪之下所创作的作品", "news_prompt34": "点评：作为全球奢侈品市场的重要一部分，中国早已成为各大品牌竞相争夺的战场", "news_prompt35": "本次“金色大秀”也意在通过品牌文化和艺术的高规格展示，进一步巩固迪奥在中国市场的影响力，同时表达对中国消费者的高度重视", "news_prompt36": "5. 巴黎时装周预热准备就绪 　　Who's Next 贸易展将于9月8日举办名为“Bouncy Thirties”的庆祝活动，庆祝其成立30周年，并在巴黎拉开行业贸易展季的序幕，比巴黎女装周开幕提前两周， 　　除此之外，同期将有Bijorhca、Impact、Curve Paris 和Interfilière Paris五场展会在在凡尔赛门展览中心 7 号展厅举办，展览包括珠宝、皮革制品、鞋类、织物、配饰和一系列精品专业供应商，以及专门面向创意产业的新展区Loud，该展区将举办由法国女性成衣联合会FFPAP"}</t>
+          <t>{"news_prompt1": "21世纪经济报道记者高江虹实习生张亿珍北京报道 　　8月结束，各企业财报陆续发出", "news_prompt2": "市场风云变幻莫测", "news_prompt3": "另外，上周凯悦酒店集团宣布了一起新收购，宝诗龙官宣TWICE组合成员Mina为品牌代言人，维密秀也将于10月回归", "news_prompt4": "1. 增长放缓", "news_prompt5": "对于不同年龄段的人群，我们继续在所有这些人群中招募新客人……我们将继续招募和获取客人，这意味着真正跨越年龄和规模", "news_prompt6": "洞察市场，不断调整，扩展产品矩阵……想重造增长神话，企业要做的还很多", "news_prompt7": "在上个月，该集团就已报告称，由于亚洲和美洲的两位数增长，其上半年收入按固定汇率计算增长了14.7％", "news_prompt8": "点评：作为全球奢侈品市场的重要一部分，中国早已成为各大品牌竞相争夺的战场", "news_prompt9": "本次“金色大秀”也意在通过品牌文化和艺术的高规格展示，进一步巩固迪奥在中国市场的影响力，同时表达对中国消费者的高度重视"}</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>{"21世纪经济报道记者高江虹实习生张亿珍北京报道 　　8月结束，各企业财报陆续发出": {"topic": "“生产投资”", "similarity": 0.5277523994445801, "prompt": "新闻文本是“21世纪经济报道记者高江虹实习生张亿珍北京报道 　　8月结束，各企业财报陆续发出”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,企业/事业(enterprise):0.0"}, "市场风云变幻莫测": {"topic": "“金融”", "similarity": 0.5586405396461487, "prompt": "新闻文本是“市场风云变幻莫测”，包含的情绪词典是：变幻莫测/反复无常(vagary):-0.2,不稳定的/易变的(volatile):-0.8"}, "另外，上周凯悦酒店集团宣布了一起新收购，宝诗龙官宣TWICE组合成员Mina为品牌代言人，维密秀也将于10月回归": {"topic": "“消费”", "similarity": 0.4527854919433594, "prompt": "新闻文本是“另外，上周凯悦酒店集团宣布了一起新收购，宝诗龙官宣TWICE组合成员Mina为品牌代言人，维密秀也将于10月回归”，包含的情绪词典是：最近的/新近的(recent):0.0,要约人/发盘人(offeror):0.0"}, "1. 增长放缓": {"topic": "“宏观经济”", "similarity": 0.5556653141975403, "prompt": "新闻文本是“1. 增长放缓”，包含的情绪词典是：已放慢的/已减速的(slowed):-0.4,衰退的/不景气的(recessionary):-0.8"}, "Lululemon下调年度预测 　　8月29日，Lululemon公布了2024财年第二季度财报，全球净营收同比增长7%，相较上年同季度的18%，增长明显放缓": {"topic": "“金融”", "similarity": 0.42297443747520447}, "对于不同年龄段的人群，我们继续在所有这些人群中招募新客人……我们将继续招募和获取客人，这意味着真正跨越年龄和规模": {"topic": "“消费”", "similarity": 0.4524865746498108, "prompt": "新闻文本是“对于不同年龄段的人群，我们继续在所有这些人群中招募新客人……我们将继续招募和获取客人，这意味着真正跨越年龄和规模”，包含的情绪词典是：招聘/招募(recruitment):0.0,吸引/招引(attract):0.5"}, "洞察市场，不断调整，扩展产品矩阵……想重造增长神话，企业要做的还很多": {"topic": "“生产投资”", "similarity": 0.4818442463874817, "prompt": "新闻文本是“洞察市场，不断调整，扩展产品矩阵……想重造增长神话，企业要做的还很多”，包含的情绪词典是：增长/发展(growth):0.7,重组/调整结构(restructuring):0.3"}, "2. Brunello Cucinelli上半年营业利润大涨19% 　　8月28日，意大利奢侈品集团Brunello Cucinelli发布上半年财务报告，期内，其营业利润增长19.3%，达到 1.046 亿欧元": {"topic": "“消费”", "similarity": 0.49290889501571655}, "在上个月，该集团就已报告称，由于亚洲和美洲的两位数增长，其上半年收入按固定汇率计算增长了14.7％": {"topic": "“宏观经济”", "similarity": 0.4261942207813263, "prompt": "新闻文本是“在上个月，该集团就已报告称，由于亚洲和美洲的两位数增长，其上半年收入按固定汇率计算增长了14.7％”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "3. 第四届“钟表与奇迹”高级钟表展在上海开幕 　　8月28日，2024第四届“钟表与奇迹”高级钟表展正式于上海西岸艺术中心开幕，展出品牌包括朗格（A. LANGE &amp; SHNE）、名士表（BAUME &amp; MERCIER） 、 卡地亚（CARTIER）、IWC万国表（IWC SCHAFFHAUSEN）、 NOMOS GLASHTTE 、沛纳海（PANERAI）、伯爵（PIAGET）、罗杰杜彼（ROGER DUBUIS）、江诗丹顿（VACHERON CONSTANTIN）9家高级制表品牌在内": {"topic": "“消费”", "similarity": 0.5337781310081482}, "据官方统计数据，25%的公众日门票由25岁以下的人年轻人购买，整体购票人群的平均年龄为35岁": {"topic": "“消费”", "similarity": 0.4539784789085388}, "点评：刚刚过去的7月已经是瑞士钟表在华业绩持续下跌的第七个月，在钟表遇冷的当下，此类展会或可保持人们对制表业的热情，并提高大众对于制表师作品的认知": {"topic": "“消费”", "similarity": 0.4771512746810913}, "4. “迪奥倾世之金”展览亮相北京 　　9月2日至29日，迪奥将于北京嘉德艺术中心举办“迪奥倾世之金” (L'OR DE DIOR)展览": {"topic": "“消费”", "similarity": 0.44996386766433716}, "点评：作为全球奢侈品市场的重要一部分，中国早已成为各大品牌竞相争夺的战场": {"topic": "“消费”", "similarity": 0.5770507454872131, "prompt": "新闻文本是“点评：作为全球奢侈品市场的重要一部分，中国早已成为各大品牌竞相争夺的战场”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,竞争者/竞争对手(competitor):0.0"}, "本次“金色大秀”也意在通过品牌文化和艺术的高规格展示，进一步巩固迪奥在中国市场的影响力，同时表达对中国消费者的高度重视": {"topic": "“消费”", "similarity": 0.45999836921691895, "prompt": "新闻文本是“本次“金色大秀”也意在通过品牌文化和艺术的高规格展示，进一步巩固迪奥在中国市场的影响力，同时表达对中国消费者的高度重视”，包含的情绪词典是：卓越/优秀(excellence):0.7,有影响力的/有势力的(influential):0.4"}, "5. 巴黎时装周预热准备就绪 　　Who's Next 贸易展将于9月8日举办名为“Bouncy Thirties”的庆祝活动，庆祝其成立30周年，并在巴黎拉开行业贸易展季的序幕，比巴黎女装周开幕提前两周， 　　除此之外，同期将有Bijorhca、Impact、Curve Paris 和Interfilière Paris五场展会在在凡尔赛门展览中心 7 号展厅举办，展览包括珠宝、皮革制品、鞋类、织物、配饰和一系列精品专业供应商，以及专门面向创意产业的新展区Loud，该展区将举办由法国女性成衣联合会FFPAP": {"topic": "“消费”", "similarity": 0.45870113372802734}}</t>
+          <t>{"21世纪经济报道记者高江虹实习生张亿珍北京报道 　　8月结束，各企业财报陆续发出": {"topic": "“生产投资”", "similarity": 0.5277526378631592, "prompt": "新闻文本是“21世纪经济报道记者高江虹实习生张亿珍北京报道 　　8月结束，各企业财报陆续发出”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,企业/事业(enterprise):0.0"}, "市场风云变幻莫测": {"topic": "“金融”", "similarity": 0.5586405992507935, "prompt": "新闻文本是“市场风云变幻莫测”，包含的情绪词典是：变幻莫测/反复无常(vagary):-0.2,不稳定的/易变的(volatile):-0.8"}, "另外，上周凯悦酒店集团宣布了一起新收购，宝诗龙官宣TWICE组合成员Mina为品牌代言人，维密秀也将于10月回归": {"topic": "“消费”", "similarity": 0.45278555154800415, "prompt": "新闻文本是“另外，上周凯悦酒店集团宣布了一起新收购，宝诗龙官宣TWICE组合成员Mina为品牌代言人，维密秀也将于10月回归”，包含的情绪词典是：最近的/新近的(recent):0.0,要约人/发盘人(offeror):0.0"}, "1. 增长放缓": {"topic": "“宏观经济”", "similarity": 0.5556656122207642, "prompt": "新闻文本是“1. 增长放缓”，包含的情绪词典是：已放慢的/已减速的(slowed):-0.4,衰退的/不景气的(recessionary):-0.8"}, "对于不同年龄段的人群，我们继续在所有这些人群中招募新客人……我们将继续招募和获取客人，这意味着真正跨越年龄和规模": {"topic": "“消费”", "similarity": 0.4524867534637451, "prompt": "新闻文本是“对于不同年龄段的人群，我们继续在所有这些人群中招募新客人……我们将继续招募和获取客人，这意味着真正跨越年龄和规模”，包含的情绪词典是：招聘/招募(recruitment):0.0,吸引/招引(attract):0.5"}, "洞察市场，不断调整，扩展产品矩阵……想重造增长神话，企业要做的还很多": {"topic": "“生产投资”", "similarity": 0.48184454441070557, "prompt": "新闻文本是“洞察市场，不断调整，扩展产品矩阵……想重造增长神话，企业要做的还很多”，包含的情绪词典是：增长/发展(growth):0.7,重组/调整结构(restructuring):0.3"}, "在上个月，该集团就已报告称，由于亚洲和美洲的两位数增长，其上半年收入按固定汇率计算增长了14.7％": {"topic": "“宏观经济”", "similarity": 0.42619454860687256, "prompt": "新闻文本是“在上个月，该集团就已报告称，由于亚洲和美洲的两位数增长，其上半年收入按固定汇率计算增长了14.7％”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "点评：作为全球奢侈品市场的重要一部分，中国早已成为各大品牌竞相争夺的战场": {"topic": "“消费”", "similarity": 0.5770508646965027, "prompt": "新闻文本是“点评：作为全球奢侈品市场的重要一部分，中国早已成为各大品牌竞相争夺的战场”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,竞争者/竞争对手(competitor):0.0"}, "本次“金色大秀”也意在通过品牌文化和艺术的高规格展示，进一步巩固迪奥在中国市场的影响力，同时表达对中国消费者的高度重视": {"topic": "“消费”", "similarity": 0.4599987268447876, "prompt": "新闻文本是“本次“金色大秀”也意在通过品牌文化和艺术的高规格展示，进一步巩固迪奥在中国市场的影响力，同时表达对中国消费者的高度重视”，包含的情绪词典是：卓越/优秀(excellence):0.7,有影响力的/有势力的(influential):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -3520,16 +3496,8 @@
           <t>界面新闻</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>{"news_prompt1": "天眼查经营风险信息显示，近日，贵州足球俱乐部有限公司因通过登记的住所或者经营场所无法联系，被贵阳市市场监督管理局列入经营异常名录", "news_prompt2": "贵州足球俱乐部有限公司成立于2005年7月，法定代表人为施明亮，注册资本8000万人民币，经营范围含体育活动组织、策划，体育培训，体育项目人力资源开发等，由贵州恒丰伟业物业管理有限公司和贵州智诚企业集团投资有限公司共同持股", "news_prompt3": "（文章来源：界面新闻）"}</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>{"天眼查经营风险信息显示，近日，贵州足球俱乐部有限公司因通过登记的住所或者经营场所无法联系，被贵阳市市场监督管理局列入经营异常名录": {"topic": "“消费”", "similarity": 0.49809765815734863}, "贵州足球俱乐部有限公司成立于2005年7月，法定代表人为施明亮，注册资本8000万人民币，经营范围含体育活动组织、策划，体育培训，体育项目人力资源开发等，由贵州恒丰伟业物业管理有限公司和贵州智诚企业集团投资有限公司共同持股": {"topic": "“消费”", "similarity": 0.44956278800964355}}</t>
-        </is>
-      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3573,12 +3541,12 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月首个交易日，A股市场低开后低位调整，核心资产代表MSCI中国A50互联互通指数盘中跌逾1.5%，成分股涨跌分化，农业银行、中国石化等领涨，泸州老窖、山西汾酒等领跌", "news_prompt2": "热门ETF方面，A50ETF（159601）已连续5日净流入超2.16亿元，资金低位布局特征显著", "news_prompt3": "中信证券表示，内需提振政策在9月有望陆续推出：地产政策方面，理论上存量按揭利率仍有下调的必要和空间，进一步支持政策值得期待", "news_prompt4": "货币政策方面，央行未来会通过更多操作维持流动性充裕，可能继续降准降息，并继续加大结构性货币工具投放", "news_prompt5": "此外，半年报落地后A股暂时迎来业绩空窗期，且市场流动性压力缓解，将共同推动市场悲观情绪修复", "news_prompt6": "A50ETF（159601）紧密跟踪MSCI中国A50互联互通指数，一键打包50只龙头个股，均衡覆盖A股市场核心龙头资产表现", "news_prompt7": "相较市场其余“漂亮50”指数，MSCI中国A50互联互通指数在编制过程中更侧重于流动性与行业均衡，大市值特征显著", "news_prompt8": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "热门ETF方面，A50ETF（159601）已连续5日净流入超2.16亿元，资金低位布局特征显著", "news_prompt2": "中信证券表示，内需提振政策在9月有望陆续推出：地产政策方面，理论上存量按揭利率仍有下调的必要和空间，进一步支持政策值得期待", "news_prompt3": "货币政策方面，央行未来会通过更多操作维持流动性充裕，可能继续降准降息，并继续加大结构性货币工具投放", "news_prompt4": "此外，半年报落地后A股暂时迎来业绩空窗期，且市场流动性压力缓解，将共同推动市场悲观情绪修复", "news_prompt5": "A50ETF（159601）紧密跟踪MSCI中国A50互联互通指数，一键打包50只龙头个股，均衡覆盖A股市场核心龙头资产表现", "news_prompt6": "相较市场其余“漂亮50”指数，MSCI中国A50互联互通指数在编制过程中更侧重于流动性与行业均衡，大市值特征显著"}</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>{"9月首个交易日，A股市场低开后低位调整，核心资产代表MSCI中国A50互联互通指数盘中跌逾1.5%，成分股涨跌分化，农业银行、中国石化等领涨，泸州老窖、山西汾酒等领跌": {"topic": "“金融”", "similarity": 0.6215102672576904}, "热门ETF方面，A50ETF（159601）已连续5日净流入超2.16亿元，资金低位布局特征显著": {"topic": "“金融”", "similarity": 0.5559993386268616, "prompt": "新闻文本是“热门ETF方面，A50ETF（159601）已连续5日净流入超2.16亿元，资金低位布局特征显著”，包含的情绪词典是：清仓/抛售(closeouts):-0.2,清仓/抛售(closeout):-0.2"}, "中信证券表示，内需提振政策在9月有望陆续推出：地产政策方面，理论上存量按揭利率仍有下调的必要和空间，进一步支持政策值得期待": {"topic": "“房地产”", "similarity": 0.6987858414649963, "prompt": "新闻文本是“中信证券表示，内需提振政策在9月有望陆续推出：地产政策方面，理论上存量按揭利率仍有下调的必要和空间，进一步支持政策值得期待”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,衰退的/不景气的(recessionary):-0.8"}, "货币政策方面，央行未来会通过更多操作维持流动性充裕，可能继续降准降息，并继续加大结构性货币工具投放": {"topic": "“宏观经济”", "similarity": 0.613051176071167, "prompt": "新闻文本是“货币政策方面，央行未来会通过更多操作维持流动性充裕，可能继续降准降息，并继续加大结构性货币工具投放”，包含的情绪词典是：丰富/充裕(abundance):0.7,货币/通货(currency):0.0"}, "此外，半年报落地后A股暂时迎来业绩空窗期，且市场流动性压力缓解，将共同推动市场悲观情绪修复": {"topic": "“金融”", "similarity": 0.49307817220687866, "prompt": "新闻文本是“此外，半年报落地后A股暂时迎来业绩空窗期，且市场流动性压力缓解，将共同推动市场悲观情绪修复”，包含的情绪词典是：悲观主义/悲观情绪(pessimism):-0.7,表现不佳/业绩低于预期(underperforming):-0.4"}, "A50ETF（159601）紧密跟踪MSCI中国A50互联互通指数，一键打包50只龙头个股，均衡覆盖A股市场核心龙头资产表现": {"topic": "“金融”", "similarity": 0.6334907412528992, "prompt": "新闻文本是“A50ETF（159601）紧密跟踪MSCI中国A50互联互通指数，一键打包50只龙头个股，均衡覆盖A股市场核心龙头资产表现”，包含的情绪词典是：指数/指标(index):0.0,投资者/投资人(investor):0.4"}, "相较市场其余“漂亮50”指数，MSCI中国A50互联互通指数在编制过程中更侧重于流动性与行业均衡，大市值特征显著": {"topic": "“金融”", "similarity": 0.5923956632614136, "prompt": "新闻文本是“相较市场其余“漂亮50”指数，MSCI中国A50互联互通指数在编制过程中更侧重于流动性与行业均衡，大市值特征显著”，包含的情绪词典是：指数/指标(index):0.0,上升的/占优势的(ascendant):0.3"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"热门ETF方面，A50ETF（159601）已连续5日净流入超2.16亿元，资金低位布局特征显著": {"topic": "“金融”", "similarity": 0.5559995174407959, "prompt": "新闻文本是“热门ETF方面，A50ETF（159601）已连续5日净流入超2.16亿元，资金低位布局特征显著”，包含的情绪词典是：清仓/抛售(closeouts):-0.2,清仓/抛售(closeout):-0.2"}, "中信证券表示，内需提振政策在9月有望陆续推出：地产政策方面，理论上存量按揭利率仍有下调的必要和空间，进一步支持政策值得期待": {"topic": "“房地产”", "similarity": 0.6987857222557068, "prompt": "新闻文本是“中信证券表示，内需提振政策在9月有望陆续推出：地产政策方面，理论上存量按揭利率仍有下调的必要和空间，进一步支持政策值得期待”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,衰退的/不景气的(recessionary):-0.8"}, "货币政策方面，央行未来会通过更多操作维持流动性充裕，可能继续降准降息，并继续加大结构性货币工具投放": {"topic": "“宏观经济”", "similarity": 0.6130512952804565, "prompt": "新闻文本是“货币政策方面，央行未来会通过更多操作维持流动性充裕，可能继续降准降息，并继续加大结构性货币工具投放”，包含的情绪词典是：丰富/充裕(abundance):0.7,货币/通货(currency):0.0"}, "此外，半年报落地后A股暂时迎来业绩空窗期，且市场流动性压力缓解，将共同推动市场悲观情绪修复": {"topic": "“金融”", "similarity": 0.49307841062545776, "prompt": "新闻文本是“此外，半年报落地后A股暂时迎来业绩空窗期，且市场流动性压力缓解，将共同推动市场悲观情绪修复”，包含的情绪词典是：悲观主义/悲观情绪(pessimism):-0.7,表现不佳/业绩低于预期(underperforming):-0.4"}, "A50ETF（159601）紧密跟踪MSCI中国A50互联互通指数，一键打包50只龙头个股，均衡覆盖A股市场核心龙头资产表现": {"topic": "“金融”", "similarity": 0.633491039276123, "prompt": "新闻文本是“A50ETF（159601）紧密跟踪MSCI中国A50互联互通指数，一键打包50只龙头个股，均衡覆盖A股市场核心龙头资产表现”，包含的情绪词典是：指数/指标(index):0.0,投资者/投资人(investor):0.4"}, "相较市场其余“漂亮50”指数，MSCI中国A50互联互通指数在编制过程中更侧重于流动性与行业均衡，大市值特征显著": {"topic": "“金融”", "similarity": 0.5923957824707031, "prompt": "新闻文本是“相较市场其余“漂亮50”指数，MSCI中国A50互联互通指数在编制过程中更侧重于流动性与行业均衡，大市值特征显著”，包含的情绪词典是：指数/指标(index):0.0,上升的/占优势的(ascendant):0.3"}}</t>
         </is>
       </c>
     </row>
@@ -3628,12 +3596,12 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上证报中国证券网讯日前，海信家电发布2024半年报", "news_prompt2": "报告期内，公司坚守长期主义，不断提升家电智能化、数字化水平，持续推进全球化战略，深入践行ESG理念，实现业绩稳健增长", "news_prompt3": "上半年，公司实现营业收入486.42亿元，同比增长13.27%", "news_prompt4": "归属上市公司股东的净利润20.16亿元，同比增长34.61%", "news_prompt5": "公司始终坚持“技术立企”的核心理念，围绕智慧生活战略，持续开展以“智能、健康、节能”为核心的技术创新", "news_prompt6": "公司拥有国家级企业技术中心、博士后科研工作站、国家级工业设计中心等20多个省部级及以上的科技创新平台", "news_prompt7": "公司大力推进IPD流程变革和工程师文化建设，成立欧洲研发中心，进一步完善全球研发体系布局和资源协同，在低碳节能、舒适健康、智能保鲜、洗烘高能效、恒风量风道控制等多个方向取得重点突破，技术水平保持行业领先并实现产品应用", "news_prompt8": "报告期内，公司在国内外市场的品牌影响力持续提升", "news_prompt9": "公司产品涵盖“Hisense”“Ronshen”“KELON”“HITACHI”、“YORK”“gorenje”“ASKO”“SANDEN”八大品牌，品牌阵容丰富，拥有良好的品牌美誉度和市场基础", "news_prompt10": "公司借助不同品牌覆盖的产品范围及其产品特性，能满足不同用户需求", "news_prompt11": "随着海信国际化战略的不断推进，品牌海外知名度和影响力不断提升", "news_prompt12": "同时，海信持续加码体育营销，连续赞助2016年欧洲杯、2018年世界杯、2020年欧洲杯、2022年世界杯、2024年欧洲杯等世界顶级体育赛事，借助国际顶级体育赛事大幅提升海信在国际市场的品牌影响力", "news_prompt13": "2024年欧洲杯营销效果调研数据显示，欧洲杯后，海信品牌资产海外同比增长8%，法国市场同比增长12%，西班牙同比增长11%", "news_prompt14": "海信品牌认知度海外同比增长7%，德国同比增长7%，法国同比增长6%", "news_prompt15": "报告期内，公司积极打造海外五大区域引擎，深化本地化建设，发力体育营销，海外自有品牌影响力不断提升", "news_prompt16": "2024年上半年，海外白电业务实现收入147.8亿元，同比增长36.91%", "news_prompt17": "同日，公司发布“质量回报双提升”行动方案", "news_prompt18": "（张阳）（文章来源：上海证券报·中国证券网）"}</t>
+          <t>{"news_prompt1": "上证报中国证券网讯日前，海信家电发布2024半年报", "news_prompt2": "报告期内，公司坚守长期主义，不断提升家电智能化、数字化水平，持续推进全球化战略，深入践行ESG理念，实现业绩稳健增长", "news_prompt3": "上半年，公司实现营业收入486.42亿元，同比增长13.27%", "news_prompt4": "公司始终坚持“技术立企”的核心理念，围绕智慧生活战略，持续开展以“智能、健康、节能”为核心的技术创新", "news_prompt5": "公司拥有国家级企业技术中心、博士后科研工作站、国家级工业设计中心等20多个省部级及以上的科技创新平台", "news_prompt6": "公司大力推进IPD流程变革和工程师文化建设，成立欧洲研发中心，进一步完善全球研发体系布局和资源协同，在低碳节能、舒适健康、智能保鲜、洗烘高能效、恒风量风道控制等多个方向取得重点突破，技术水平保持行业领先并实现产品应用", "news_prompt7": "报告期内，公司在国内外市场的品牌影响力持续提升", "news_prompt8": "公司产品涵盖“Hisense”“Ronshen”“KELON”“HITACHI”、“YORK”“gorenje”“ASKO”“SANDEN”八大品牌，品牌阵容丰富，拥有良好的品牌美誉度和市场基础", "news_prompt9": "公司借助不同品牌覆盖的产品范围及其产品特性，能满足不同用户需求", "news_prompt10": "随着海信国际化战略的不断推进，品牌海外知名度和影响力不断提升", "news_prompt11": "同时，海信持续加码体育营销，连续赞助2016年欧洲杯、2018年世界杯、2020年欧洲杯、2022年世界杯、2024年欧洲杯等世界顶级体育赛事，借助国际顶级体育赛事大幅提升海信在国际市场的品牌影响力", "news_prompt12": "2024年欧洲杯营销效果调研数据显示，欧洲杯后，海信品牌资产海外同比增长8%，法国市场同比增长12%，西班牙同比增长11%", "news_prompt13": "海信品牌认知度海外同比增长7%，德国同比增长7%，法国同比增长6%", "news_prompt14": "报告期内，公司积极打造海外五大区域引擎，深化本地化建设，发力体育营销，海外自有品牌影响力不断提升", "news_prompt15": "2024年上半年，海外白电业务实现收入147.8亿元，同比增长36.91%", "news_prompt16": "同日，公司发布“质量回报双提升”行动方案"}</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>{"上证报中国证券网讯日前，海信家电发布2024半年报": {"topic": "“消费”", "similarity": 0.4612104296684265, "prompt": "新闻文本是“上证报中国证券网讯日前，海信家电发布2024半年报”，包含的情绪词典是：电的/电气的(electrical):0.0,盈利能力/获利能力(profitability):0.6"}, "报告期内，公司坚守长期主义，不断提升家电智能化、数字化水平，持续推进全球化战略，深入践行ESG理念，实现业绩稳健增长": {"topic": "“生产投资”", "similarity": 0.5408881902694702, "prompt": "新闻文本是“报告期内，公司坚守长期主义，不断提升家电智能化、数字化水平，持续推进全球化战略，深入践行ESG理念，实现业绩稳健增长”，包含的情绪词典是：公司的/企业的(corporate):0.0,增长/发展(growth):0.7"}, "上半年，公司实现营业收入486.42亿元，同比增长13.27%": {"topic": "“生产投资”", "similarity": 0.4337271451950073, "prompt": "新闻文本是“上半年，公司实现营业收入486.42亿元，同比增长13.27%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司始终坚持“技术立企”的核心理念，围绕智慧生活战略，持续开展以“智能、健康、节能”为核心的技术创新": {"topic": "“生产投资”", "similarity": 0.5913339257240295, "prompt": "新闻文本是“公司始终坚持“技术立企”的核心理念，围绕智慧生活战略，持续开展以“智能、健康、节能”为核心的技术创新”，包含的情绪词典是：技术(tech):0.0,公司的/企业的(corporate):0.0"}, "公司拥有国家级企业技术中心、博士后科研工作站、国家级工业设计中心等20多个省部级及以上的科技创新平台": {"topic": "“生产投资”", "similarity": 0.6105549335479736, "prompt": "新闻文本是“公司拥有国家级企业技术中心、博士后科研工作站、国家级工业设计中心等20多个省部级及以上的科技创新平台”，包含的情绪词典是：公司/企业(company):0.0,公司的/企业的(corporate):0.0"}, "公司大力推进IPD流程变革和工程师文化建设，成立欧洲研发中心，进一步完善全球研发体系布局和资源协同，在低碳节能、舒适健康、智能保鲜、洗烘高能效、恒风量风道控制等多个方向取得重点突破，技术水平保持行业领先并实现产品应用": {"topic": "“生产投资”", "similarity": 0.5700052976608276, "prompt": "新闻文本是“公司大力推进IPD流程变革和工程师文化建设，成立欧洲研发中心，进一步完善全球研发体系布局和资源协同，在低碳节能、舒适健康、智能保鲜、洗烘高能效、恒风量风道控制等多个方向取得重点突破，技术水平保持行业领先并实现产品应用”，包含的情绪词典是：公司的/企业的(corporate):0.0,创新的/革新的(innovative):0.7"}, "报告期内，公司在国内外市场的品牌影响力持续提升": {"topic": "“消费”", "similarity": 0.4299602508544922, "prompt": "新闻文本是“报告期内，公司在国内外市场的品牌影响力持续提升”，包含的情绪词典是：增强的/提高的(enhanced):0.6,增强/提高(enhancement):0.6"}, "公司产品涵盖“Hisense”“Ronshen”“KELON”“HITACHI”、“YORK”“gorenje”“ASKO”“SANDEN”八大品牌，品牌阵容丰富，拥有良好的品牌美誉度和市场基础": {"topic": "“消费”", "similarity": 0.4767770767211914, "prompt": "新闻文本是“公司产品涵盖“Hisense”“Ronshen”“KELON”“HITACHI”、“YORK”“gorenje”“ASKO”“SANDEN”八大品牌，品牌阵容丰富，拥有良好的品牌美誉度和市场基础”，包含的情绪词典是：公司/企业(company):0.0,公司的/企业的(corporate):0.0"}, "公司借助不同品牌覆盖的产品范围及其产品特性，能满足不同用户需求": {"topic": "“消费”", "similarity": 0.5128675699234009, "prompt": "新闻文本是“公司借助不同品牌覆盖的产品范围及其产品特性，能满足不同用户需求”，包含的情绪词典是：品牌/商标(brand):0.0,公司/企业(firm):0.0"}, "随着海信国际化战略的不断推进，品牌海外知名度和影响力不断提升": {"topic": "“消费”", "similarity": 0.4982672333717346, "prompt": "新闻文本是“随着海信国际化战略的不断推进，品牌海外知名度和影响力不断提升”，包含的情绪词典是：海外的/国外的(overseas):0.0,进步/提升(advancement):0.5"}, "同时，海信持续加码体育营销，连续赞助2016年欧洲杯、2018年世界杯、2020年欧洲杯、2022年世界杯、2024年欧洲杯等世界顶级体育赛事，借助国际顶级体育赛事大幅提升海信在国际市场的品牌影响力": {"topic": "“消费”", "similarity": 0.5730283260345459, "prompt": "新闻文本是“同时，海信持续加码体育营销，连续赞助2016年欧洲杯、2018年世界杯、2020年欧洲杯、2022年世界杯、2024年欧洲杯等世界顶级体育赛事，借助国际顶级体育赛事大幅提升海信在国际市场的品牌影响力”，包含的情绪词典是：有影响力的/有势力的(influential):0.4,跑赢/表现优于(outperform):0.65"}, "2024年欧洲杯营销效果调研数据显示，欧洲杯后，海信品牌资产海外同比增长8%，法国市场同比增长12%，西班牙同比增长11%": {"topic": "“消费”", "similarity": 0.5796729922294617, "prompt": "新闻文本是“2024年欧洲杯营销效果调研数据显示，欧洲杯后，海信品牌资产海外同比增长8%，法国市场同比增长12%，西班牙同比增长11%”，包含的情绪词典是：欧元(euro):0.0,海外的/国外的(overseas):0.0"}, "海信品牌认知度海外同比增长7%，德国同比增长7%，法国同比增长6%": {"topic": "“消费”", "similarity": 0.505298912525177, "prompt": "新闻文本是“海信品牌认知度海外同比增长7%，德国同比增长7%，法国同比增长6%”，包含的情绪词典是：增长/发展(growth):0.7,海外的/国外的(overseas):0.0"}, "报告期内，公司积极打造海外五大区域引擎，深化本地化建设，发力体育营销，海外自有品牌影响力不断提升": {"topic": "“消费”", "similarity": 0.5075114965438843, "prompt": "新闻文本是“报告期内，公司积极打造海外五大区域引擎，深化本地化建设，发力体育营销，海外自有品牌影响力不断提升”，包含的情绪词典是：海外的/国外的(overseas):0.0,有影响力的/有势力的(influential):0.4"}, "2024年上半年，海外白电业务实现收入147.8亿元，同比增长36.91%": {"topic": "“消费”", "similarity": 0.47967904806137085, "prompt": "新闻文本是“2024年上半年，海外白电业务实现收入147.8亿元，同比增长36.91%”，包含的情绪词典是：电的/电气的(electrical):0.0,海外的/国外的(overseas):0.0"}, "同日，公司发布“质量回报双提升”行动方案": {"topic": "“生产投资”", "similarity": 0.42054229974746704, "prompt": "新闻文本是“同日，公司发布“质量回报双提升”行动方案”，包含的情绪词典是：计划/方案(programme):0.0,公司的/企业的(corporate):0.0"}, "（张阳）（文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.4649379849433899, "prompt": "新闻文本是“（张阳）（文章来源：上海证券报·中国证券网）”，包含的情绪词典是：投资者/投资人(investor):0.4,资本/资金(capital):0.1"}}</t>
+          <t>{"上证报中国证券网讯日前，海信家电发布2024半年报": {"topic": "“消费”", "similarity": 0.46121060848236084, "prompt": "新闻文本是“上证报中国证券网讯日前，海信家电发布2024半年报”，包含的情绪词典是：电的/电气的(electrical):0.0,盈利能力/获利能力(profitability):0.6"}, "报告期内，公司坚守长期主义，不断提升家电智能化、数字化水平，持续推进全球化战略，深入践行ESG理念，实现业绩稳健增长": {"topic": "“生产投资”", "similarity": 0.5408881902694702, "prompt": "新闻文本是“报告期内，公司坚守长期主义，不断提升家电智能化、数字化水平，持续推进全球化战略，深入践行ESG理念，实现业绩稳健增长”，包含的情绪词典是：公司的/企业的(corporate):0.0,增长/发展(growth):0.7"}, "上半年，公司实现营业收入486.42亿元，同比增长13.27%": {"topic": "“生产投资”", "similarity": 0.4337272346019745, "prompt": "新闻文本是“上半年，公司实现营业收入486.42亿元，同比增长13.27%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司始终坚持“技术立企”的核心理念，围绕智慧生活战略，持续开展以“智能、健康、节能”为核心的技术创新": {"topic": "“生产投资”", "similarity": 0.5913339853286743, "prompt": "新闻文本是“公司始终坚持“技术立企”的核心理念，围绕智慧生活战略，持续开展以“智能、健康、节能”为核心的技术创新”，包含的情绪词典是：技术(tech):0.0,公司的/企业的(corporate):0.0"}, "公司拥有国家级企业技术中心、博士后科研工作站、国家级工业设计中心等20多个省部级及以上的科技创新平台": {"topic": "“生产投资”", "similarity": 0.6105550527572632, "prompt": "新闻文本是“公司拥有国家级企业技术中心、博士后科研工作站、国家级工业设计中心等20多个省部级及以上的科技创新平台”，包含的情绪词典是：公司/企业(company):0.0,公司的/企业的(corporate):0.0"}, "公司大力推进IPD流程变革和工程师文化建设，成立欧洲研发中心，进一步完善全球研发体系布局和资源协同，在低碳节能、舒适健康、智能保鲜、洗烘高能效、恒风量风道控制等多个方向取得重点突破，技术水平保持行业领先并实现产品应用": {"topic": "“生产投资”", "similarity": 0.5700052976608276, "prompt": "新闻文本是“公司大力推进IPD流程变革和工程师文化建设，成立欧洲研发中心，进一步完善全球研发体系布局和资源协同，在低碳节能、舒适健康、智能保鲜、洗烘高能效、恒风量风道控制等多个方向取得重点突破，技术水平保持行业领先并实现产品应用”，包含的情绪词典是：公司的/企业的(corporate):0.0,创新的/革新的(innovative):0.7"}, "报告期内，公司在国内外市场的品牌影响力持续提升": {"topic": "“消费”", "similarity": 0.42996034026145935, "prompt": "新闻文本是“报告期内，公司在国内外市场的品牌影响力持续提升”，包含的情绪词典是：增强的/提高的(enhanced):0.6,增强/提高(enhancement):0.6"}, "公司产品涵盖“Hisense”“Ronshen”“KELON”“HITACHI”、“YORK”“gorenje”“ASKO”“SANDEN”八大品牌，品牌阵容丰富，拥有良好的品牌美誉度和市场基础": {"topic": "“消费”", "similarity": 0.47677719593048096, "prompt": "新闻文本是“公司产品涵盖“Hisense”“Ronshen”“KELON”“HITACHI”、“YORK”“gorenje”“ASKO”“SANDEN”八大品牌，品牌阵容丰富，拥有良好的品牌美誉度和市场基础”，包含的情绪词典是：公司/企业(company):0.0,公司的/企业的(corporate):0.0"}, "公司借助不同品牌覆盖的产品范围及其产品特性，能满足不同用户需求": {"topic": "“消费”", "similarity": 0.5128676891326904, "prompt": "新闻文本是“公司借助不同品牌覆盖的产品范围及其产品特性，能满足不同用户需求”，包含的情绪词典是：品牌/商标(brand):0.0,公司/企业(firm):0.0"}, "随着海信国际化战略的不断推进，品牌海外知名度和影响力不断提升": {"topic": "“消费”", "similarity": 0.49826744198799133, "prompt": "新闻文本是“随着海信国际化战略的不断推进，品牌海外知名度和影响力不断提升”，包含的情绪词典是：海外的/国外的(overseas):0.0,进步/提升(advancement):0.5"}, "同时，海信持续加码体育营销，连续赞助2016年欧洲杯、2018年世界杯、2020年欧洲杯、2022年世界杯、2024年欧洲杯等世界顶级体育赛事，借助国际顶级体育赛事大幅提升海信在国际市场的品牌影响力": {"topic": "“消费”", "similarity": 0.573028564453125, "prompt": "新闻文本是“同时，海信持续加码体育营销，连续赞助2016年欧洲杯、2018年世界杯、2020年欧洲杯、2022年世界杯、2024年欧洲杯等世界顶级体育赛事，借助国际顶级体育赛事大幅提升海信在国际市场的品牌影响力”，包含的情绪词典是：有影响力的/有势力的(influential):0.4,跑赢/表现优于(outperform):0.65"}, "2024年欧洲杯营销效果调研数据显示，欧洲杯后，海信品牌资产海外同比增长8%，法国市场同比增长12%，西班牙同比增长11%": {"topic": "“消费”", "similarity": 0.5796730518341064, "prompt": "新闻文本是“2024年欧洲杯营销效果调研数据显示，欧洲杯后，海信品牌资产海外同比增长8%，法国市场同比增长12%，西班牙同比增长11%”，包含的情绪词典是：欧元(euro):0.0,海外的/国外的(overseas):0.0"}, "海信品牌认知度海外同比增长7%，德国同比增长7%，法国同比增长6%": {"topic": "“消费”", "similarity": 0.5052990317344666, "prompt": "新闻文本是“海信品牌认知度海外同比增长7%，德国同比增长7%，法国同比增长6%”，包含的情绪词典是：增长/发展(growth):0.7,海外的/国外的(overseas):0.0"}, "报告期内，公司积极打造海外五大区域引擎，深化本地化建设，发力体育营销，海外自有品牌影响力不断提升": {"topic": "“消费”", "similarity": 0.5075114965438843, "prompt": "新闻文本是“报告期内，公司积极打造海外五大区域引擎，深化本地化建设，发力体育营销，海外自有品牌影响力不断提升”，包含的情绪词典是：海外的/国外的(overseas):0.0,有影响力的/有势力的(influential):0.4"}, "2024年上半年，海外白电业务实现收入147.8亿元，同比增长36.91%": {"topic": "“消费”", "similarity": 0.4796792268753052, "prompt": "新闻文本是“2024年上半年，海外白电业务实现收入147.8亿元，同比增长36.91%”，包含的情绪词典是：电的/电气的(electrical):0.0,海外的/国外的(overseas):0.0"}, "同日，公司发布“质量回报双提升”行动方案": {"topic": "“生产投资”", "similarity": 0.42054247856140137, "prompt": "新闻文本是“同日，公司发布“质量回报双提升”行动方案”，包含的情绪词典是：计划/方案(programme):0.0,公司的/企业的(corporate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3679,12 +3647,12 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，大参林(603233.SH)发布2024年中报", "news_prompt2": "公司营业总收入为133.45亿元，在已披露的同业公司中排名第10，较去年同报告期营业总收入增加13.53亿元，实现5年连续上涨，同比较去年同期上涨11.29%", "news_prompt3": "归母净利润为6.58亿元，在已披露的同业公司中排名第6，较去年同报告期归母净利润减少2.60亿元，同比较去年同期下降28.32%", "news_prompt4": "经营活动现金净流入为17.67亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入增加2.90亿元，实现5年连续上涨，同比较去年同期上涨19.61%", "news_prompt5": "公司最新资产负债率为67.15%，在已披露的同业公司中排名第22，较上季度资产负债率增加0.50个百分点，较去年同季度资产负债率增加3.81个百分点", "news_prompt6": "公司最新毛利率为34.89%，在已披露的同业公司中排名第3，较上季度毛利率减少0.56个百分点，较去年同季度毛利率减少2.55个百分点", "news_prompt7": "最新ROE为9.25%，在已披露的同业公司中排名第3，较去年同季度ROE减少4.71个百分点", "news_prompt8": "公司摊薄每股收益为0.58元，在已披露的同业公司中排名第9，较去年同报告期摊薄每股收益减少0.23元，同比较去年同期下降28.32%", "news_prompt9": "公司最新总资产周转率为0.54次，在已披露的同业公司中排名第15，较去年同季度总资产周转率减少0.04次，同比较去年同期下降6.52%", "news_prompt10": "最新存货周转率为2.05次，在已披露的同业公司中排名第23，较去年同季度存货周转率增加0.18次，实现2年连续上涨，同比较去年同期上涨9.54%", "news_prompt11": "公司股东户数为4.09万户，前十大股东持股数量为7.99亿股，占总股本比例为70.20%", "news_prompt12": "前十大股东分别为柯云峰、柯金龙、柯康保、柯舟、香港中央结算有限公司、宋茗、刘景荣、梁嘉盈、中信证券股份有限公司、富达基金(香港)有限公司-客户资金，持股比例分别为21.30%、20.16%、15.65%、3.60%、2.80%、1.94%、1.79%、1.05%、0.97%、0.93%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为133.45亿元，在已披露的同业公司中排名第10，较去年同报告期营业总收入增加13.53亿元，实现5年连续上涨，同比较去年同期上涨11.29%", "news_prompt2": "归母净利润为6.58亿元，在已披露的同业公司中排名第6，较去年同报告期归母净利润减少2.60亿元，同比较去年同期下降28.32%", "news_prompt3": "经营活动现金净流入为17.67亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入增加2.90亿元，实现5年连续上涨，同比较去年同期上涨19.61%", "news_prompt4": "公司最新资产负债率为67.15%，在已披露的同业公司中排名第22，较上季度资产负债率增加0.50个百分点，较去年同季度资产负债率增加3.81个百分点", "news_prompt5": "公司最新毛利率为34.89%，在已披露的同业公司中排名第3，较上季度毛利率减少0.56个百分点，较去年同季度毛利率减少2.55个百分点", "news_prompt6": "公司摊薄每股收益为0.58元，在已披露的同业公司中排名第9，较去年同报告期摊薄每股收益减少0.23元，同比较去年同期下降28.32%", "news_prompt7": "公司最新总资产周转率为0.54次，在已披露的同业公司中排名第15，较去年同季度总资产周转率减少0.04次，同比较去年同期下降6.52%", "news_prompt8": "最新存货周转率为2.05次，在已披露的同业公司中排名第23，较去年同季度存货周转率增加0.18次，实现2年连续上涨，同比较去年同期上涨9.54%", "news_prompt9": "公司股东户数为4.09万户，前十大股东持股数量为7.99亿股，占总股本比例为70.20%"}</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，大参林(603233.SH)发布2024年中报": {"topic": "“金融”", "similarity": 0.5014618635177612, "prompt": "新闻文本是“2024年8月31日，大参林(603233.SH)发布2024年中报”，包含的情绪词典是：股票/库存(stock):0.0,储备/囤积(stockpile):0.1"}, "公司营业总收入为133.45亿元，在已披露的同业公司中排名第10，较去年同报告期营业总收入增加13.53亿元，实现5年连续上涨，同比较去年同期上涨11.29%": {"topic": "“消费”", "similarity": 0.5564631819725037, "prompt": "新闻文本是“公司营业总收入为133.45亿元，在已披露的同业公司中排名第10，较去年同报告期营业总收入增加13.53亿元，实现5年连续上涨，同比较去年同期上涨11.29%”，包含的情绪词典是：公司的/企业的(corporate):0.0,盈利能力/获利能力(profitability):0.6"}, "归母净利润为6.58亿元，在已披露的同业公司中排名第6，较去年同报告期归母净利润减少2.60亿元，同比较去年同期下降28.32%": {"topic": "“消费”", "similarity": 0.5165526866912842, "prompt": "新闻文本是“归母净利润为6.58亿元，在已披露的同业公司中排名第6，较去年同报告期归母净利润减少2.60亿元，同比较去年同期下降28.32%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为17.67亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入增加2.90亿元，实现5年连续上涨，同比较去年同期上涨19.61%": {"topic": "“金融”", "similarity": 0.572669506072998, "prompt": "新闻文本是“经营活动现金净流入为17.67亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入增加2.90亿元，实现5年连续上涨，同比较去年同期上涨19.61%”，包含的情绪词典是：营业额/周转(turnover):0.0,盈利能力/获利能力(profitability):0.6"}, "公司最新资产负债率为67.15%，在已披露的同业公司中排名第22，较上季度资产负债率增加0.50个百分点，较去年同季度资产负债率增加3.81个百分点": {"topic": "“消费”", "similarity": 0.47558143734931946, "prompt": "新闻文本是“公司最新资产负债率为67.15%，在已披露的同业公司中排名第22，较上季度资产负债率增加0.50个百分点，较去年同季度资产负债率增加3.81个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,负债的/欠债的(indebted):-0.5"}, "公司最新毛利率为34.89%，在已披露的同业公司中排名第3，较上季度毛利率减少0.56个百分点，较去年同季度毛利率减少2.55个百分点": {"topic": "“消费”", "similarity": 0.44268670678138733, "prompt": "新闻文本是“公司最新毛利率为34.89%，在已披露的同业公司中排名第3，较上季度毛利率减少0.56个百分点，较去年同季度毛利率减少2.55个百分点”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "公司摊薄每股收益为0.58元，在已披露的同业公司中排名第9，较去年同报告期摊薄每股收益减少0.23元，同比较去年同期下降28.32%": {"topic": "“金融”", "similarity": 0.4609742760658264, "prompt": "新闻文本是“公司摊薄每股收益为0.58元，在已披露的同业公司中排名第9，较去年同报告期摊薄每股收益减少0.23元，同比较去年同期下降28.32%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "公司最新总资产周转率为0.54次，在已披露的同业公司中排名第15，较去年同季度总资产周转率减少0.04次，同比较去年同期下降6.52%": {"topic": "“金融”", "similarity": 0.48299598693847656, "prompt": "新闻文本是“公司最新总资产周转率为0.54次，在已披露的同业公司中排名第15，较去年同季度总资产周转率减少0.04次，同比较去年同期下降6.52%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "最新存货周转率为2.05次，在已披露的同业公司中排名第23，较去年同季度存货周转率增加0.18次，实现2年连续上涨，同比较去年同期上涨9.54%": {"topic": "“消费”", "similarity": 0.4645923376083374, "prompt": "新闻文本是“最新存货周转率为2.05次，在已披露的同业公司中排名第23，较去年同季度存货周转率增加0.18次，实现2年连续上涨，同比较去年同期上涨9.54%”，包含的情绪词典是：股票/库存(stock):0.0,营业额/周转(turnover):0.0"}, "公司股东户数为4.09万户，前十大股东持股数量为7.99亿股，占总股本比例为70.20%": {"topic": "“金融”", "similarity": 0.48454082012176514, "prompt": "新闻文本是“公司股东户数为4.09万户，前十大股东持股数量为7.99亿股，占总股本比例为70.20%”，包含的情绪词典是：公司/企业(company):0.0,公司/企业(firm):0.0"}, "前十大股东分别为柯云峰、柯金龙、柯康保、柯舟、香港中央结算有限公司、宋茗、刘景荣、梁嘉盈、中信证券股份有限公司、富达基金(香港)有限公司-客户资金，持股比例分别为21.30%、20.16%、15.65%、3.60%、2.80%、1.94%、1.79%、1.05%、0.97%、0.93%": {"topic": "“金融”", "similarity": 0.5591738224029541}}</t>
+          <t>{"公司营业总收入为133.45亿元，在已披露的同业公司中排名第10，较去年同报告期营业总收入增加13.53亿元，实现5年连续上涨，同比较去年同期上涨11.29%": {"topic": "“消费”", "similarity": 0.5564631223678589, "prompt": "新闻文本是“公司营业总收入为133.45亿元，在已披露的同业公司中排名第10，较去年同报告期营业总收入增加13.53亿元，实现5年连续上涨，同比较去年同期上涨11.29%”，包含的情绪词典是：公司的/企业的(corporate):0.0,盈利能力/获利能力(profitability):0.6"}, "归母净利润为6.58亿元，在已披露的同业公司中排名第6，较去年同报告期归母净利润减少2.60亿元，同比较去年同期下降28.32%": {"topic": "“消费”", "similarity": 0.5165525674819946, "prompt": "新闻文本是“归母净利润为6.58亿元，在已披露的同业公司中排名第6，较去年同报告期归母净利润减少2.60亿元，同比较去年同期下降28.32%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "经营活动现金净流入为17.67亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入增加2.90亿元，实现5年连续上涨，同比较去年同期上涨19.61%": {"topic": "“金融”", "similarity": 0.5726696252822876, "prompt": "新闻文本是“经营活动现金净流入为17.67亿元，在已披露的同业公司中排名第2，较去年同报告期经营活动现金净流入增加2.90亿元，实现5年连续上涨，同比较去年同期上涨19.61%”，包含的情绪词典是：营业额/周转(turnover):0.0,盈利能力/获利能力(profitability):0.6"}, "公司最新资产负债率为67.15%，在已披露的同业公司中排名第22，较上季度资产负债率增加0.50个百分点，较去年同季度资产负债率增加3.81个百分点": {"topic": "“消费”", "similarity": 0.4755816161632538, "prompt": "新闻文本是“公司最新资产负债率为67.15%，在已披露的同业公司中排名第22，较上季度资产负债率增加0.50个百分点，较去年同季度资产负债率增加3.81个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,负债的/欠债的(indebted):-0.5"}, "公司最新毛利率为34.89%，在已披露的同业公司中排名第3，较上季度毛利率减少0.56个百分点，较去年同季度毛利率减少2.55个百分点": {"topic": "“消费”", "similarity": 0.4426867961883545, "prompt": "新闻文本是“公司最新毛利率为34.89%，在已披露的同业公司中排名第3，较上季度毛利率减少0.56个百分点，较去年同季度毛利率减少2.55个百分点”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "公司摊薄每股收益为0.58元，在已披露的同业公司中排名第9，较去年同报告期摊薄每股收益减少0.23元，同比较去年同期下降28.32%": {"topic": "“金融”", "similarity": 0.46097463369369507, "prompt": "新闻文本是“公司摊薄每股收益为0.58元，在已披露的同业公司中排名第9，较去年同报告期摊薄每股收益减少0.23元，同比较去年同期下降28.32%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "公司最新总资产周转率为0.54次，在已披露的同业公司中排名第15，较去年同季度总资产周转率减少0.04次，同比较去年同期下降6.52%": {"topic": "“金融”", "similarity": 0.4829961955547333, "prompt": "新闻文本是“公司最新总资产周转率为0.54次，在已披露的同业公司中排名第15，较去年同季度总资产周转率减少0.04次，同比较去年同期下降6.52%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "最新存货周转率为2.05次，在已披露的同业公司中排名第23，较去年同季度存货周转率增加0.18次，实现2年连续上涨，同比较去年同期上涨9.54%": {"topic": "“消费”", "similarity": 0.4645925462245941, "prompt": "新闻文本是“最新存货周转率为2.05次，在已披露的同业公司中排名第23，较去年同季度存货周转率增加0.18次，实现2年连续上涨，同比较去年同期上涨9.54%”，包含的情绪词典是：股票/库存(stock):0.0,营业额/周转(turnover):0.0"}, "公司股东户数为4.09万户，前十大股东持股数量为7.99亿股，占总股本比例为70.20%": {"topic": "“金融”", "similarity": 0.4845410883426666, "prompt": "新闻文本是“公司股东户数为4.09万户，前十大股东持股数量为7.99亿股，占总股本比例为70.20%”，包含的情绪词典是：公司/企业(company):0.0,公司/企业(firm):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3730,12 +3698,12 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "｜2024年9月2日星期一｜  　　NO.1 43家上市券商上半年取得净利639.61亿元，同比降逾两成 　　随着半年报披露落幕，上市券商今年上半年业绩集体出炉", "news_prompt2": "整体来看，今年上半年，43家上市券商合计取得净利639.61亿元，同比降逾两成", "news_prompt3": "净利排名前五的是中信证券、华泰证券、国泰君安、招商证券、中国银河", "news_prompt4": "约四分之一的券商净利同比实现正增长，1家券商亏损", "news_prompt5": "业务结构方面，自营业务收入成业绩压舱石，营收占比超三成", "news_prompt6": "经纪业务收入业务占比近20%", "news_prompt7": "资管业务、信用业务、投行业务营收占比均不到10%", "news_prompt8": "此外，其他业务营收占比约26%", "news_prompt9": "其中，投行业务及信用业务降幅最大，分别同比下降四成、三成", "news_prompt10": "点评：上市券商业绩下滑反映出中国证券市场在2024年上半年面临的挑战，净利润下降超过20%可能与市场波动、交易量减少、佣金率下降等因素有关", "news_prompt11": "尽管部分券商通过业务结构调整和成本控制实现了正增长，但整体行业仍需面对激烈的市场竞争和转型压力", "news_prompt12": "特别是投行业务和信用业务的大幅下降，可能意味着资本市场的融资活动减缓，以及市场对信用风险的担忧", "news_prompt13": "NO.2 二季度末中央汇金持有ETF规模约5700亿元 　　多家公募基金日前公布2024年中报", "news_prompt14": "记者统计发现，今年上半年，中央汇金投资有限责任公司投资的宽基交易型开放式指数基金（ETF）品种明显增加", "news_prompt15": "除沪深300ETF、上证50ETF、中证500ETF等传统宽基外，中央汇金还新进买入创业板ETF、上证科创板50ETF、中证1000ETF等其他宽基品种", "news_prompt16": "整体来看，中央汇金持有的ETF总规模从年初约1100亿元，增加至二季度末约5700亿元", "news_prompt17": "截至二季度末，股票型ETF的总规模约1.81万亿元，以此计算，中央汇金持有的ETF规模约占股票型ETF总规模约三成", "news_prompt18": "(央视新闻) 　　点评：中央汇金持有ETF规模的大幅增长，显示了其对市场的信心以及对ETF作为投资工具的重视", "news_prompt19": "ETF因其流动性好、成本低廉、透明度高等特点，成为机构投资者的重要配置工具，中央汇金的这一策略可能旨在通过多元化投资来分散风险", "news_prompt20": "其持有规模占股票型ETF总规模的三成，表明其在市场中的影响力，也可能对市场情绪和ETF流动性产生积极影响", "news_prompt21": "NO.3 银河基金新任胡泊为公司董事长 　　近日，银河基金发布董事长任职公告，新任胡泊为公司董事长", "news_prompt22": "履历显示，胡泊曾任中国银河金融控股有限责任公司战略发展部副总经理、银河基金董事，现任中国银河金融控股有限责任公司首席运营官兼战略发展部总经理、股权管理部总经理", "news_prompt23": "回看今年7月20日时，银河基金曾公告称，宋卫刚因工作安排不再担任银河基金董事长一职，由总经理史平武代任", "news_prompt24": "而随着新任董事长到任，史平武不再代为履行董事长职务", "news_prompt25": "点评：银河基金董事长的更迭可能预示着公司战略和管理层面的调整", "news_prompt26": "胡泊的背景显示其在金融控股公司有丰富的战略发展和运营管理经验，这可能有助于银河基金在竞争激烈的基金行业中寻找新的增长点", "news_prompt27": "同时，这一人事变动也可能带来公司治理结构和业务发展方向的变化，对公司的长期发展产生重要影响", "news_prompt28": "在当前基金行业竞争激烈的背景下，银河基金需要明确其核心竞争力，加强产品创新和风险管理，以实现可持续发展", "news_prompt29": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "｜2024年9月2日星期一｜  　　NO.1 43家上市券商上半年取得净利639.61亿元，同比降逾两成 　　随着半年报披露落幕，上市券商今年上半年业绩集体出炉", "news_prompt2": "整体来看，今年上半年，43家上市券商合计取得净利639.61亿元，同比降逾两成", "news_prompt3": "净利排名前五的是中信证券、华泰证券、国泰君安、招商证券、中国银河", "news_prompt4": "约四分之一的券商净利同比实现正增长，1家券商亏损", "news_prompt5": "业务结构方面，自营业务收入成业绩压舱石，营收占比超三成", "news_prompt6": "经纪业务收入业务占比近20%", "news_prompt7": "资管业务、信用业务、投行业务营收占比均不到10%", "news_prompt8": "其中，投行业务及信用业务降幅最大，分别同比下降四成、三成", "news_prompt9": "点评：上市券商业绩下滑反映出中国证券市场在2024年上半年面临的挑战，净利润下降超过20%可能与市场波动、交易量减少、佣金率下降等因素有关", "news_prompt10": "尽管部分券商通过业务结构调整和成本控制实现了正增长，但整体行业仍需面对激烈的市场竞争和转型压力", "news_prompt11": "特别是投行业务和信用业务的大幅下降，可能意味着资本市场的融资活动减缓，以及市场对信用风险的担忧", "news_prompt12": "记者统计发现，今年上半年，中央汇金投资有限责任公司投资的宽基交易型开放式指数基金（ETF）品种明显增加", "news_prompt13": "整体来看，中央汇金持有的ETF总规模从年初约1100亿元，增加至二季度末约5700亿元", "news_prompt14": "(央视新闻) 　　点评：中央汇金持有ETF规模的大幅增长，显示了其对市场的信心以及对ETF作为投资工具的重视", "news_prompt15": "ETF因其流动性好、成本低廉、透明度高等特点，成为机构投资者的重要配置工具，中央汇金的这一策略可能旨在通过多元化投资来分散风险", "news_prompt16": "其持有规模占股票型ETF总规模的三成，表明其在市场中的影响力，也可能对市场情绪和ETF流动性产生积极影响", "news_prompt17": "NO.3 银河基金新任胡泊为公司董事长 　　近日，银河基金发布董事长任职公告，新任胡泊为公司董事长", "news_prompt18": "回看今年7月20日时，银河基金曾公告称，宋卫刚因工作安排不再担任银河基金董事长一职，由总经理史平武代任", "news_prompt19": "点评：银河基金董事长的更迭可能预示着公司战略和管理层面的调整", "news_prompt20": "在当前基金行业竞争激烈的背景下，银河基金需要明确其核心竞争力，加强产品创新和风险管理，以实现可持续发展"}</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>{"｜2024年9月2日星期一｜  　　NO.1 43家上市券商上半年取得净利639.61亿元，同比降逾两成 　　随着半年报披露落幕，上市券商今年上半年业绩集体出炉": {"topic": "“金融”", "similarity": 0.6527515649795532, "prompt": "新闻文本是“｜2024年9月2日星期一｜  　　NO.1 43家上市券商上半年取得净利639.61亿元，同比降逾两成 　　随着半年报披露落幕，上市券商今年上半年业绩集体出炉”，包含的情绪词典是：表现不佳/业绩低于预期(underperforms):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "整体来看，今年上半年，43家上市券商合计取得净利639.61亿元，同比降逾两成": {"topic": "“金融”", "similarity": 0.526042103767395, "prompt": "新闻文本是“整体来看，今年上半年，43家上市券商合计取得净利639.61亿元，同比降逾两成”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "净利排名前五的是中信证券、华泰证券、国泰君安、招商证券、中国银河": {"topic": "“金融”", "similarity": 0.6007387638092041, "prompt": "新闻文本是“净利排名前五的是中信证券、华泰证券、国泰君安、招商证券、中国银河”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "约四分之一的券商净利同比实现正增长，1家券商亏损": {"topic": "“金融”", "similarity": 0.45162832736968994, "prompt": "新闻文本是“约四分之一的券商净利同比实现正增长，1家券商亏损”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "业务结构方面，自营业务收入成业绩压舱石，营收占比超三成": {"topic": "“金融”", "similarity": 0.48150402307510376, "prompt": "新闻文本是“业务结构方面，自营业务收入成业绩压舱石，营收占比超三成”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,框架/结构(framework):0.0"}, "经纪业务收入业务占比近20%": {"topic": "“金融”", "similarity": 0.4579852819442749, "prompt": "新闻文本是“经纪业务收入业务占比近20%”，包含的情绪词典是：服务/业务(service):0.0,管理/经营(manage):0.2"}, "资管业务、信用业务、投行业务营收占比均不到10%": {"topic": "“金融”", "similarity": 0.5243003368377686, "prompt": "新闻文本是“资管业务、信用业务、投行业务营收占比均不到10%”，包含的情绪词典是：金融的/财政的(financial):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "其中，投行业务及信用业务降幅最大，分别同比下降四成、三成": {"topic": "“金融”", "similarity": 0.5086998343467712, "prompt": "新闻文本是“其中，投行业务及信用业务降幅最大，分别同比下降四成、三成”，包含的情绪词典是：降级/降低评级(downgrade):-0.6,下跌/下降(fall):-0.6"}, "点评：上市券商业绩下滑反映出中国证券市场在2024年上半年面临的挑战，净利润下降超过20%可能与市场波动、交易量减少、佣金率下降等因素有关": {"topic": "“金融”", "similarity": 0.659977376461029, "prompt": "新闻文本是“点评：上市券商业绩下滑反映出中国证券市场在2024年上半年面临的挑战，净利润下降超过20%可能与市场波动、交易量减少、佣金率下降等因素有关”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "尽管部分券商通过业务结构调整和成本控制实现了正增长，但整体行业仍需面对激烈的市场竞争和转型压力": {"topic": "“金融”", "similarity": 0.48728519678115845, "prompt": "新闻文本是“尽管部分券商通过业务结构调整和成本控制实现了正增长，但整体行业仍需面对激烈的市场竞争和转型压力”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,监管/调控(regulate):0.0"}, "特别是投行业务和信用业务的大幅下降，可能意味着资本市场的融资活动减缓，以及市场对信用风险的担忧": {"topic": "“金融”", "similarity": 0.5020744800567627, "prompt": "新闻文本是“特别是投行业务和信用业务的大幅下降，可能意味着资本市场的融资活动减缓，以及市场对信用风险的担忧”，包含的情绪词典是：下降的/衰退的(declining):-0.6,下跌/下降(fall):-0.6"}, "NO.2 二季度末中央汇金持有ETF规模约5700亿元 　　多家公募基金日前公布2024年中报": {"topic": "“金融”", "similarity": 0.5685322880744934, "prompt": "新闻文本是“NO.2 二季度末中央汇金持有ETF规模约5700亿元 　　多家公募基金日前公布2024年中报”，包含的情绪词典是：基金/资金(fund):0.1,金融的/财政的(financial):0.0"}, "记者统计发现，今年上半年，中央汇金投资有限责任公司投资的宽基交易型开放式指数基金（ETF）品种明显增加": {"topic": "“金融”", "similarity": 0.5347812175750732, "prompt": "新闻文本是“记者统计发现，今年上半年，中央汇金投资有限责任公司投资的宽基交易型开放式指数基金（ETF）品种明显增加”，包含的情绪词典是：基金/资金(fund):0.1,投资/投入(invest):0.3"}, "除沪深300ETF、上证50ETF、中证500ETF等传统宽基外，中央汇金还新进买入创业板ETF、上证科创板50ETF、中证1000ETF等其他宽基品种": {"topic": "“金融”", "similarity": 0.6445674300193787}, "整体来看，中央汇金持有的ETF总规模从年初约1100亿元，增加至二季度末约5700亿元": {"topic": "“金融”", "similarity": 0.4941613972187042, "prompt": "新闻文本是“整体来看，中央汇金持有的ETF总规模从年初约1100亿元，增加至二季度末约5700亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "截至二季度末，股票型ETF的总规模约1.81万亿元，以此计算，中央汇金持有的ETF规模约占股票型ETF总规模约三成": {"topic": "“金融”", "similarity": 0.5861092805862427}, "(央视新闻) 　　点评：中央汇金持有ETF规模的大幅增长，显示了其对市场的信心以及对ETF作为投资工具的重视": {"topic": "“金融”", "similarity": 0.5745396018028259, "prompt": "新闻文本是“(央视新闻) 　　点评：中央汇金持有ETF规模的大幅增长，显示了其对市场的信心以及对ETF作为投资工具的重视”，包含的情绪词典是：自信的/有信心的(confident):0.5,持有/握住(hold):0.0"}, "ETF因其流动性好、成本低廉、透明度高等特点，成为机构投资者的重要配置工具，中央汇金的这一策略可能旨在通过多元化投资来分散风险": {"topic": "“金融”", "similarity": 0.5730206966400146, "prompt": "新闻文本是“ETF因其流动性好、成本低廉、透明度高等特点，成为机构投资者的重要配置工具，中央汇金的这一策略可能旨在通过多元化投资来分散风险”，包含的情绪词典是：基金/资金(fund):0.1,处于优势的/有利的(advantaged):0.7"}, "其持有规模占股票型ETF总规模的三成，表明其在市场中的影响力，也可能对市场情绪和ETF流动性产生积极影响": {"topic": "“金融”", "similarity": 0.4895419478416443, "prompt": "新闻文本是“其持有规模占股票型ETF总规模的三成，表明其在市场中的影响力，也可能对市场情绪和ETF流动性产生积极影响”，包含的情绪词典是：占有(权)(possessory):0.0,有影响力的/有势力的(influential):0.4"}, "NO.3 银河基金新任胡泊为公司董事长 　　近日，银河基金发布董事长任职公告，新任胡泊为公司董事长": {"topic": "“金融”", "similarity": 0.5773901343345642, "prompt": "新闻文本是“NO.3 银河基金新任胡泊为公司董事长 　　近日，银河基金发布董事长任职公告，新任胡泊为公司董事长”，包含的情绪词典是：基金/资金(fund):0.1,公司的/企业的(corporate):0.0"}, "履历显示，胡泊曾任中国银河金融控股有限责任公司战略发展部副总经理、银河基金董事，现任中国银河金融控股有限责任公司首席运营官兼战略发展部总经理、股权管理部总经理": {"topic": "“金融”", "similarity": 0.48557811975479126}, "回看今年7月20日时，银河基金曾公告称，宋卫刚因工作安排不再担任银河基金董事长一职，由总经理史平武代任": {"topic": "“金融”", "similarity": 0.5109206438064575, "prompt": "新闻文本是“回看今年7月20日时，银河基金曾公告称，宋卫刚因工作安排不再担任银河基金董事长一职，由总经理史平武代任”，包含的情绪词典是：基金/资金(fund):0.1,取代/接替(subrogated):-0.1"}, "点评：银河基金董事长的更迭可能预示着公司战略和管理层面的调整": {"topic": "“金融”", "similarity": 0.5040895938873291, "prompt": "新闻文本是“点评：银河基金董事长的更迭可能预示着公司战略和管理层面的调整”，包含的情绪词典是：基金/资金(fund):0.1,管理不善/管理失误(mismanagement):-0.5"}, "胡泊的背景显示其在金融控股公司有丰富的战略发展和运营管理经验，这可能有助于银河基金在竞争激烈的基金行业中寻找新的增长点": {"topic": "“金融”", "similarity": 0.4291466474533081}, "在当前基金行业竞争激烈的背景下，银河基金需要明确其核心竞争力，加强产品创新和风险管理，以实现可持续发展": {"topic": "“金融”", "similarity": 0.4787115752696991, "prompt": "新闻文本是“在当前基金行业竞争激烈的背景下，银河基金需要明确其核心竞争力，加强产品创新和风险管理，以实现可持续发展”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,竞赛/竞争(contest):-0.1"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"｜2024年9月2日星期一｜  　　NO.1 43家上市券商上半年取得净利639.61亿元，同比降逾两成 　　随着半年报披露落幕，上市券商今年上半年业绩集体出炉": {"topic": "“金融”", "similarity": 0.6527516841888428, "prompt": "新闻文本是“｜2024年9月2日星期一｜  　　NO.1 43家上市券商上半年取得净利639.61亿元，同比降逾两成 　　随着半年报披露落幕，上市券商今年上半年业绩集体出炉”，包含的情绪词典是：表现不佳/业绩低于预期(underperforms):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "整体来看，今年上半年，43家上市券商合计取得净利639.61亿元，同比降逾两成": {"topic": "“金融”", "similarity": 0.5260422825813293, "prompt": "新闻文本是“整体来看，今年上半年，43家上市券商合计取得净利639.61亿元，同比降逾两成”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "净利排名前五的是中信证券、华泰证券、国泰君安、招商证券、中国银河": {"topic": "“金融”", "similarity": 0.6007388234138489, "prompt": "新闻文本是“净利排名前五的是中信证券、华泰证券、国泰君安、招商证券、中国银河”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "约四分之一的券商净利同比实现正增长，1家券商亏损": {"topic": "“金融”", "similarity": 0.45162853598594666, "prompt": "新闻文本是“约四分之一的券商净利同比实现正增长，1家券商亏损”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "业务结构方面，自营业务收入成业绩压舱石，营收占比超三成": {"topic": "“金融”", "similarity": 0.4815042018890381, "prompt": "新闻文本是“业务结构方面，自营业务收入成业绩压舱石，营收占比超三成”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,框架/结构(framework):0.0"}, "经纪业务收入业务占比近20%": {"topic": "“金融”", "similarity": 0.45798537135124207, "prompt": "新闻文本是“经纪业务收入业务占比近20%”，包含的情绪词典是：服务/业务(service):0.0,管理/经营(manage):0.2"}, "资管业务、信用业务、投行业务营收占比均不到10%": {"topic": "“金融”", "similarity": 0.5243004560470581, "prompt": "新闻文本是“资管业务、信用业务、投行业务营收占比均不到10%”，包含的情绪词典是：金融的/财政的(financial):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "其中，投行业务及信用业务降幅最大，分别同比下降四成、三成": {"topic": "“金融”", "similarity": 0.5087001323699951, "prompt": "新闻文本是“其中，投行业务及信用业务降幅最大，分别同比下降四成、三成”，包含的情绪词典是：降级/降低评级(downgrade):-0.6,下跌/下降(fall):-0.6"}, "点评：上市券商业绩下滑反映出中国证券市场在2024年上半年面临的挑战，净利润下降超过20%可能与市场波动、交易量减少、佣金率下降等因素有关": {"topic": "“金融”", "similarity": 0.6599774956703186, "prompt": "新闻文本是“点评：上市券商业绩下滑反映出中国证券市场在2024年上半年面临的挑战，净利润下降超过20%可能与市场波动、交易量减少、佣金率下降等因素有关”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "尽管部分券商通过业务结构调整和成本控制实现了正增长，但整体行业仍需面对激烈的市场竞争和转型压力": {"topic": "“金融”", "similarity": 0.48728543519973755, "prompt": "新闻文本是“尽管部分券商通过业务结构调整和成本控制实现了正增长，但整体行业仍需面对激烈的市场竞争和转型压力”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,监管/调控(regulate):0.0"}, "特别是投行业务和信用业务的大幅下降，可能意味着资本市场的融资活动减缓，以及市场对信用风险的担忧": {"topic": "“金融”", "similarity": 0.502074658870697, "prompt": "新闻文本是“特别是投行业务和信用业务的大幅下降，可能意味着资本市场的融资活动减缓，以及市场对信用风险的担忧”，包含的情绪词典是：下降的/衰退的(declining):-0.6,下跌/下降(fall):-0.6"}, "记者统计发现，今年上半年，中央汇金投资有限责任公司投资的宽基交易型开放式指数基金（ETF）品种明显增加": {"topic": "“金融”", "similarity": 0.5347813367843628, "prompt": "新闻文本是“记者统计发现，今年上半年，中央汇金投资有限责任公司投资的宽基交易型开放式指数基金（ETF）品种明显增加”，包含的情绪词典是：基金/资金(fund):0.1,投资/投入(invest):0.3"}, "整体来看，中央汇金持有的ETF总规模从年初约1100亿元，增加至二季度末约5700亿元": {"topic": "“金融”", "similarity": 0.49416154623031616, "prompt": "新闻文本是“整体来看，中央汇金持有的ETF总规模从年初约1100亿元，增加至二季度末约5700亿元”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "(央视新闻) 　　点评：中央汇金持有ETF规模的大幅增长，显示了其对市场的信心以及对ETF作为投资工具的重视": {"topic": "“金融”", "similarity": 0.5745398998260498, "prompt": "新闻文本是“(央视新闻) 　　点评：中央汇金持有ETF规模的大幅增长，显示了其对市场的信心以及对ETF作为投资工具的重视”，包含的情绪词典是：自信的/有信心的(confident):0.5,持有/握住(hold):0.0"}, "ETF因其流动性好、成本低廉、透明度高等特点，成为机构投资者的重要配置工具，中央汇金的这一策略可能旨在通过多元化投资来分散风险": {"topic": "“金融”", "similarity": 0.5730207562446594, "prompt": "新闻文本是“ETF因其流动性好、成本低廉、透明度高等特点，成为机构投资者的重要配置工具，中央汇金的这一策略可能旨在通过多元化投资来分散风险”，包含的情绪词典是：基金/资金(fund):0.1,处于优势的/有利的(advantaged):0.7"}, "其持有规模占股票型ETF总规模的三成，表明其在市场中的影响力，也可能对市场情绪和ETF流动性产生积极影响": {"topic": "“金融”", "similarity": 0.4895420968532562, "prompt": "新闻文本是“其持有规模占股票型ETF总规模的三成，表明其在市场中的影响力，也可能对市场情绪和ETF流动性产生积极影响”，包含的情绪词典是：占有(权)(possessory):0.0,有影响力的/有势力的(influential):0.4"}, "NO.3 银河基金新任胡泊为公司董事长 　　近日，银河基金发布董事长任职公告，新任胡泊为公司董事长": {"topic": "“金融”", "similarity": 0.5773900747299194, "prompt": "新闻文本是“NO.3 银河基金新任胡泊为公司董事长 　　近日，银河基金发布董事长任职公告，新任胡泊为公司董事长”，包含的情绪词典是：基金/资金(fund):0.1,公司的/企业的(corporate):0.0"}, "回看今年7月20日时，银河基金曾公告称，宋卫刚因工作安排不再担任银河基金董事长一职，由总经理史平武代任": {"topic": "“金融”", "similarity": 0.5109208822250366, "prompt": "新闻文本是“回看今年7月20日时，银河基金曾公告称，宋卫刚因工作安排不再担任银河基金董事长一职，由总经理史平武代任”，包含的情绪词典是：基金/资金(fund):0.1,取代/接替(subrogated):-0.1"}, "点评：银河基金董事长的更迭可能预示着公司战略和管理层面的调整": {"topic": "“金融”", "similarity": 0.5040897130966187, "prompt": "新闻文本是“点评：银河基金董事长的更迭可能预示着公司战略和管理层面的调整”，包含的情绪词典是：基金/资金(fund):0.1,管理不善/管理失误(mismanagement):-0.5"}, "在当前基金行业竞争激烈的背景下，银河基金需要明确其核心竞争力，加强产品创新和风险管理，以实现可持续发展": {"topic": "“金融”", "similarity": 0.47871172428131104, "prompt": "新闻文本是“在当前基金行业竞争激烈的背景下，银河基金需要明确其核心竞争力，加强产品创新和风险管理，以实现可持续发展”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,竞赛/竞争(contest):-0.1"}}</t>
         </is>
       </c>
     </row>
@@ -3781,12 +3749,12 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "南方财经9月2日电，天眼查App显示，近日，中国金融期货交易所股份有限公司发生工商变更，霍瑞戎卸任法定代表人、董事兼总经理，由张晓刚接任法定代表人并担任董事、经理，同时该公司注册资本由150亿人民币增至180亿人民币", "news_prompt2": "中国金融期货交易所股份有限公司成立于2006年9月，由上海证券交易所、上海期货交易所、深圳证券交易所、大连商品交易所、郑州商品交易所共同持股", "news_prompt3": "（文章来源：南方财经网）"}</t>
+          <t>{"news_prompt1": "中国金融期货交易所股份有限公司成立于2006年9月，由上海证券交易所、上海期货交易所、深圳证券交易所、大连商品交易所、郑州商品交易所共同持股"}</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>{"南方财经9月2日电，天眼查App显示，近日，中国金融期货交易所股份有限公司发生工商变更，霍瑞戎卸任法定代表人、董事兼总经理，由张晓刚接任法定代表人并担任董事、经理，同时该公司注册资本由150亿人民币增至180亿人民币": {"topic": "“金融”", "similarity": 0.5468480587005615}, "中国金融期货交易所股份有限公司成立于2006年9月，由上海证券交易所、上海期货交易所、深圳证券交易所、大连商品交易所、郑州商品交易所共同持股": {"topic": "“金融”", "similarity": 0.6598047614097595, "prompt": "新闻文本是“中国金融期货交易所股份有限公司成立于2006年9月，由上海证券交易所、上海期货交易所、深圳证券交易所、大连商品交易所、郑州商品交易所共同持股”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "（文章来源：南方财经网）": {"topic": "“金融”", "similarity": 0.4414668679237366, "prompt": "新闻文本是“（文章来源：南方财经网）”，包含的情绪词典是：金融/财政(finance):0.0,金融的/财政的(financial):0.0"}}</t>
+          <t>{"中国金融期货交易所股份有限公司成立于2006年9月，由上海证券交易所、上海期货交易所、深圳证券交易所、大连商品交易所、郑州商品交易所共同持股": {"topic": "“金融”", "similarity": 0.6598047614097595, "prompt": "新闻文本是“中国金融期货交易所股份有限公司成立于2006年9月，由上海证券交易所、上海期货交易所、深圳证券交易所、大连商品交易所、郑州商品交易所共同持股”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3832,12 +3800,12 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日，A股三大股指集体低开，截至发稿，科创100指数跌0.98%，成分股涨跌互现，微导纳米涨超3%，中信博、华兴源创、杰华特、九号公司-WD等涨超2%，唯捷创芯跌超8%，光峰科技、中科飞测、奥普特等跟跌", "news_prompt2": "相关ETF方面，科创100ETF（588190）截至发稿跌1.03%，成交额超2100万元，换手率超1.1%，早盘交投活跃，溢折率0.15%，早盘频现溢价交易", "news_prompt3": "资金面上，Wind数据显示，该ETF上一交易日获资金净流入2880万元，近5个交易日则有4日获资金净流入", "news_prompt4": "科创100ETF（588190）紧密跟踪科创100指数，该指数是从上海证券交易所科创板中选取市值中等且流动性较好的100只证券作为样本", "news_prompt5": "消息面上，9月1日，中国上市公司协会发布中国上市公司2024年半年度经营业绩报告", "news_prompt6": "截至8月31日，677家上市公司公布一季度、半年度现金分红预案（含特别分红），较去年同期增加近500家，其中科创板80家公司中期分红，是去年的5倍", "news_prompt7": "合计现金分红达5312亿元，分红公司整体股利支付率31.74%，分红的稳定性增强", "news_prompt8": "国投证券称，面向9月，基于最新“央地财政支出增速差”出现企稳的观察，我们对大盘指数较7-8月谨慎的态度有所改观，市场有望摆脱“难有持续下跌，或有小幅反弹”的阴跌状态", "news_prompt9": "随着中报利空结束叠加外围降息提升国内降息预期，大盘指数在9月的阶段性温和回升是可以期待的", "news_prompt10": "（本文机构观点来自持牌证券机构，不构成任何投资建议，亦不代表平台观点，请投资人独立判断和决策", "news_prompt11": "）（文章来源：21世纪经济报道）"}</t>
+          <t>{"news_prompt1": "相关ETF方面，科创100ETF（588190）截至发稿跌1.03%，成交额超2100万元，换手率超1.1%，早盘交投活跃，溢折率0.15%，早盘频现溢价交易", "news_prompt2": "资金面上，Wind数据显示，该ETF上一交易日获资金净流入2880万元，近5个交易日则有4日获资金净流入", "news_prompt3": "科创100ETF（588190）紧密跟踪科创100指数，该指数是从上海证券交易所科创板中选取市值中等且流动性较好的100只证券作为样本", "news_prompt4": "消息面上，9月1日，中国上市公司协会发布中国上市公司2024年半年度经营业绩报告", "news_prompt5": "合计现金分红达5312亿元，分红公司整体股利支付率31.74%，分红的稳定性增强", "news_prompt6": "国投证券称，面向9月，基于最新“央地财政支出增速差”出现企稳的观察，我们对大盘指数较7-8月谨慎的态度有所改观，市场有望摆脱“难有持续下跌，或有小幅反弹”的阴跌状态"}</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>{"9月2日，A股三大股指集体低开，截至发稿，科创100指数跌0.98%，成分股涨跌互现，微导纳米涨超3%，中信博、华兴源创、杰华特、九号公司-WD等涨超2%，唯捷创芯跌超8%，光峰科技、中科飞测、奥普特等跟跌": {"topic": "“金融”", "similarity": 0.6128178834915161}, "相关ETF方面，科创100ETF（588190）截至发稿跌1.03%，成交额超2100万元，换手率超1.1%，早盘交投活跃，溢折率0.15%，早盘频现溢价交易": {"topic": "“金融”", "similarity": 0.6265231370925903, "prompt": "新闻文本是“相关ETF方面，科创100ETF（588190）截至发稿跌1.03%，成交额超2100万元，换手率超1.1%，早盘交投活跃，溢折率0.15%，早盘频现溢价交易”，包含的情绪词典是：贬值/减值(devaluation):-0.5,储备/囤积(stockpile):0.1"}, "资金面上，Wind数据显示，该ETF上一交易日获资金净流入2880万元，近5个交易日则有4日获资金净流入": {"topic": "“金融”", "similarity": 0.5326354503631592, "prompt": "新闻文本是“资金面上，Wind数据显示，该ETF上一交易日获资金净流入2880万元，近5个交易日则有4日获资金净流入”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "科创100ETF（588190）紧密跟踪科创100指数，该指数是从上海证券交易所科创板中选取市值中等且流动性较好的100只证券作为样本": {"topic": "“金融”", "similarity": 0.6453219056129456, "prompt": "新闻文本是“科创100ETF（588190）紧密跟踪科创100指数，该指数是从上海证券交易所科创板中选取市值中等且流动性较好的100只证券作为样本”，包含的情绪词典是：指数/指标(index):0.0,创新的/革新的(innovative):0.7"}, "消息面上，9月1日，中国上市公司协会发布中国上市公司2024年半年度经营业绩报告": {"topic": "“金融”", "similarity": 0.6508122086524963, "prompt": "新闻文本是“消息面上，9月1日，中国上市公司协会发布中国上市公司2024年半年度经营业绩报告”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,表现不佳/业绩低于预期(underperforming):-0.4"}, "截至8月31日，677家上市公司公布一季度、半年度现金分红预案（含特别分红），较去年同期增加近500家，其中科创板80家公司中期分红，是去年的5倍": {"topic": "“金融”", "similarity": 0.6001834869384766}, "合计现金分红达5312亿元，分红公司整体股利支付率31.74%，分红的稳定性增强": {"topic": "“金融”", "similarity": 0.5089856386184692, "prompt": "新闻文本是“合计现金分红达5312亿元，分红公司整体股利支付率31.74%，分红的稳定性增强”，包含的情绪词典是：稳定/稳定性(stability):0.6,使稳定/稳定(stabilize):0.5"}, "国投证券称，面向9月，基于最新“央地财政支出增速差”出现企稳的观察，我们对大盘指数较7-8月谨慎的态度有所改观，市场有望摆脱“难有持续下跌，或有小幅反弹”的阴跌状态": {"topic": "“金融”", "similarity": 0.6658658981323242, "prompt": "新闻文本是“国投证券称，面向9月，基于最新“央地财政支出增速差”出现企稳的观察，我们对大盘指数较7-8月谨慎的态度有所改观，市场有望摆脱“难有持续下跌，或有小幅反弹”的阴跌状态”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "随着中报利空结束叠加外围降息提升国内降息预期，大盘指数在9月的阶段性温和回升是可以期待的": {"topic": "“金融”", "similarity": 0.6552560925483704, "prompt": "新闻文本是“随着中报利空结束叠加外围降息提升国内降息预期，大盘指数在9月的阶段性温和回升是可以期待的”，包含的情绪词典是：反弹/回升(rebounding):0.3,反弹/回升(rebound):0.1"}, "（本文机构观点来自持牌证券机构，不构成任何投资建议，亦不代表平台观点，请投资人独立判断和决策": {"topic": "“金融”", "similarity": 0.571772038936615, "prompt": "新闻文本是“（本文机构观点来自持牌证券机构，不构成任何投资建议，亦不代表平台观点，请投资人独立判断和决策”，包含的情绪词典是：投机性的/推测性的(speculative):-0.2,投资者/投资人(investor):0.4"}, "）（文章来源：21世纪经济报道）": {"topic": "“宏观经济”", "similarity": 0.43245604634284973, "prompt": "新闻文本是“）（文章来源：21世纪经济报道）”，包含的情绪词典是：经济/经济体(economy):0.0,金融的/财政的(financial):0.0"}}</t>
+          <t>{"相关ETF方面，科创100ETF（588190）截至发稿跌1.03%，成交额超2100万元，换手率超1.1%，早盘交投活跃，溢折率0.15%，早盘频现溢价交易": {"topic": "“金融”", "similarity": 0.6265233159065247, "prompt": "新闻文本是“相关ETF方面，科创100ETF（588190）截至发稿跌1.03%，成交额超2100万元，换手率超1.1%，早盘交投活跃，溢折率0.15%，早盘频现溢价交易”，包含的情绪词典是：贬值/减值(devaluation):-0.5,储备/囤积(stockpile):0.1"}, "资金面上，Wind数据显示，该ETF上一交易日获资金净流入2880万元，近5个交易日则有4日获资金净流入": {"topic": "“金融”", "similarity": 0.5326355695724487, "prompt": "新闻文本是“资金面上，Wind数据显示，该ETF上一交易日获资金净流入2880万元，近5个交易日则有4日获资金净流入”，包含的情绪词典是：基金/资金(fund):0.1,投资/投资额(investment):0.4"}, "科创100ETF（588190）紧密跟踪科创100指数，该指数是从上海证券交易所科创板中选取市值中等且流动性较好的100只证券作为样本": {"topic": "“金融”", "similarity": 0.6453219652175903, "prompt": "新闻文本是“科创100ETF（588190）紧密跟踪科创100指数，该指数是从上海证券交易所科创板中选取市值中等且流动性较好的100只证券作为样本”，包含的情绪词典是：指数/指标(index):0.0,创新的/革新的(innovative):0.7"}, "消息面上，9月1日，中国上市公司协会发布中国上市公司2024年半年度经营业绩报告": {"topic": "“金融”", "similarity": 0.6508123278617859, "prompt": "新闻文本是“消息面上，9月1日，中国上市公司协会发布中国上市公司2024年半年度经营业绩报告”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,表现不佳/业绩低于预期(underperforming):-0.4"}, "合计现金分红达5312亿元，分红公司整体股利支付率31.74%，分红的稳定性增强": {"topic": "“金融”", "similarity": 0.5089858174324036, "prompt": "新闻文本是“合计现金分红达5312亿元，分红公司整体股利支付率31.74%，分红的稳定性增强”，包含的情绪词典是：稳定/稳定性(stability):0.6,使稳定/稳定(stabilize):0.5"}, "国投证券称，面向9月，基于最新“央地财政支出增速差”出现企稳的观察，我们对大盘指数较7-8月谨慎的态度有所改观，市场有望摆脱“难有持续下跌，或有小幅反弹”的阴跌状态": {"topic": "“金融”", "similarity": 0.665865957736969, "prompt": "新闻文本是“国投证券称，面向9月，基于最新“央地财政支出增速差”出现企稳的观察，我们对大盘指数较7-8月谨慎的态度有所改观，市场有望摆脱“难有持续下跌，或有小幅反弹”的阴跌状态”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -3883,12 +3851,12 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "【大河财立方记者陈薇】9月1日，科林电气发布股东大会决议及董事会完成换届选举公告，新一届董事会7名董事席位中，青岛海信网络能源股份有限公司（简称“海信网能”）提名的2名非独立董事、2名独立董事当选，石家庄国有资本投资运营集团有限责任公司（简称“石家庄国投”）提名的2名非独立董事、1名独立董事当选", "news_prompt2": "新一届监事会3名监事席位中，除职工代表监事外，海信网能和石家庄国投各提名并当选一位非职工代表监事", "news_prompt3": "海信网能、石家庄国投等各方都严格遵守法治精神、契约精神和资本市场规则", "news_prompt4": "海信网能与石家庄国投以4：3比例组建新的董事会", "news_prompt5": "新一届董事会组建后将尽快召开会议，完成董事长选举、管理层选聘等工作，实现公司平稳过渡，并坚持股东利益至上原则，最大程度保护广大投资者利益", "news_prompt6": "海信网能方面表示，将与石家庄国投、公司原有团队等各方团结合作、共谋上市公司发展，共同努力，一起把科林电气做大做强", "news_prompt7": "科林电气新一届董事会及后续的经营层，将持续提升上市公司价值，与投资者共享发展成果，不断增强投资者获得感", "news_prompt8": "同时，海信网能将在合法合规基础上积极调动海信集团内部的优质资源，例如海信集团在芯片、功率半导体、电子、电力电子、软件、温控等方面的技术优势及研发平台、供应链平台、人才机制、全国乃至全球的营销渠道资源等，特别是国际营销渠道资源，不断支持上市公司拓展国内、国际业务，充分发挥业务、资本、管理等方面的优势支持上市公司发展", "news_prompt9": "与此同时，还将强化激励机制，保持上市公司经营管理团队、员工队伍稳定", "news_prompt10": "此次新当选的科林电气董事史文伯此前在接受记者采访时曾代表海信承诺，控股科林电气后，科林电气的注册地、生产地、纳税地、生产场所、管理机构等不会搬离石家庄", "news_prompt11": "这一表态，不仅展现了其对科林电气未来发展的信心，也体现了海信愿意与各方股东共享发展成果的信心，尤其体现了海信愿意对石家庄当地经济做贡献的诚心与信心", "news_prompt12": "科林电气此次换届选举，为公司管理团队注入新鲜血液，公司治理结构进一步完善，各方股东强强联合，共谋公司发展，对公司未来发展迈向新能级具有关键意义", "news_prompt13": "在新一届董事会和新的管理团队带领下，科林电气有望实现从区域性企业向全球性企业的跨越", "news_prompt14": "（文章来源：大河财立方）"}</t>
+          <t>{"news_prompt1": "新一届监事会3名监事席位中，除职工代表监事外，海信网能和石家庄国投各提名并当选一位非职工代表监事", "news_prompt2": "海信网能、石家庄国投等各方都严格遵守法治精神、契约精神和资本市场规则", "news_prompt3": "海信网能与石家庄国投以4：3比例组建新的董事会", "news_prompt4": "新一届董事会组建后将尽快召开会议，完成董事长选举、管理层选聘等工作，实现公司平稳过渡，并坚持股东利益至上原则，最大程度保护广大投资者利益", "news_prompt5": "海信网能方面表示，将与石家庄国投、公司原有团队等各方团结合作、共谋上市公司发展，共同努力，一起把科林电气做大做强", "news_prompt6": "科林电气新一届董事会及后续的经营层，将持续提升上市公司价值，与投资者共享发展成果，不断增强投资者获得感", "news_prompt7": "同时，海信网能将在合法合规基础上积极调动海信集团内部的优质资源，例如海信集团在芯片、功率半导体、电子、电力电子、软件、温控等方面的技术优势及研发平台、供应链平台、人才机制、全国乃至全球的营销渠道资源等，特别是国际营销渠道资源，不断支持上市公司拓展国内、国际业务，充分发挥业务、资本、管理等方面的优势支持上市公司发展", "news_prompt8": "与此同时，还将强化激励机制，保持上市公司经营管理团队、员工队伍稳定", "news_prompt9": "此次新当选的科林电气董事史文伯此前在接受记者采访时曾代表海信承诺，控股科林电气后，科林电气的注册地、生产地、纳税地、生产场所、管理机构等不会搬离石家庄", "news_prompt10": "这一表态，不仅展现了其对科林电气未来发展的信心，也体现了海信愿意与各方股东共享发展成果的信心，尤其体现了海信愿意对石家庄当地经济做贡献的诚心与信心", "news_prompt11": "科林电气此次换届选举，为公司管理团队注入新鲜血液，公司治理结构进一步完善，各方股东强强联合，共谋公司发展，对公司未来发展迈向新能级具有关键意义"}</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>{"【大河财立方记者陈薇】9月1日，科林电气发布股东大会决议及董事会完成换届选举公告，新一届董事会7名董事席位中，青岛海信网络能源股份有限公司（简称“海信网能”）提名的2名非独立董事、2名独立董事当选，石家庄国有资本投资运营集团有限责任公司（简称“石家庄国投”）提名的2名非独立董事、1名独立董事当选": {"topic": "“生产投资”", "similarity": 0.5270013809204102}, "新一届监事会3名监事席位中，除职工代表监事外，海信网能和石家庄国投各提名并当选一位非职工代表监事": {"topic": "“生产投资”", "similarity": 0.48071596026420593, "prompt": "新闻文本是“新一届监事会3名监事席位中，除职工代表监事外，海信网能和石家庄国投各提名并当选一位非职工代表监事”，包含的情绪词典是：监管的/调控的(regulatory):0.0,选举/推选(election):0.0"}, "海信网能、石家庄国投等各方都严格遵守法治精神、契约精神和资本市场规则": {"topic": "“生产投资”", "similarity": 0.5304059982299805, "prompt": "新闻文本是“海信网能、石家庄国投等各方都严格遵守法治精神、契约精神和资本市场规则”，包含的情绪词典是：契约/盟约(covenant):0.0,合同/契约(contract):0.0"}, "海信网能与石家庄国投以4：3比例组建新的董事会": {"topic": "“生产投资”", "similarity": 0.4877719283103943, "prompt": "新闻文本是“海信网能与石家庄国投以4：3比例组建新的董事会”，包含的情绪词典是：董事会/木板(board):0.0,转让/割让(cession):0.0"}, "新一届董事会组建后将尽快召开会议，完成董事长选举、管理层选聘等工作，实现公司平稳过渡，并坚持股东利益至上原则，最大程度保护广大投资者利益": {"topic": "“金融”", "similarity": 0.578275203704834, "prompt": "新闻文本是“新一届董事会组建后将尽快召开会议，完成董事长选举、管理层选聘等工作，实现公司平稳过渡，并坚持股东利益至上原则，最大程度保护广大投资者利益”，包含的情绪词典是：董事会/木板(board):0.0,公司的/企业的(corporate):0.0"}, "海信网能方面表示，将与石家庄国投、公司原有团队等各方团结合作、共谋上市公司发展，共同努力，一起把科林电气做大做强": {"topic": "“生产投资”", "similarity": 0.5563782453536987, "prompt": "新闻文本是“海信网能方面表示，将与石家庄国投、公司原有团队等各方团结合作、共谋上市公司发展，共同努力，一起把科林电气做大做强”，包含的情绪词典是：电的/电气的(electrical):0.0,公司的/企业的(corporate):0.0"}, "科林电气新一届董事会及后续的经营层，将持续提升上市公司价值，与投资者共享发展成果，不断增强投资者获得感": {"topic": "“金融”", "similarity": 0.5590029358863831, "prompt": "新闻文本是“科林电气新一届董事会及后续的经营层，将持续提升上市公司价值，与投资者共享发展成果，不断增强投资者获得感”，包含的情绪词典是：电的/电气的(electrical):0.0,增强/提高(enhancement):0.6"}, "同时，海信网能将在合法合规基础上积极调动海信集团内部的优质资源，例如海信集团在芯片、功率半导体、电子、电力电子、软件、温控等方面的技术优势及研发平台、供应链平台、人才机制、全国乃至全球的营销渠道资源等，特别是国际营销渠道资源，不断支持上市公司拓展国内、国际业务，充分发挥业务、资本、管理等方面的优势支持上市公司发展": {"topic": "“生产投资”", "similarity": 0.5798695683479309, "prompt": "新闻文本是“同时，海信网能将在合法合规基础上积极调动海信集团内部的优质资源，例如海信集团在芯片、功率半导体、电子、电力电子、软件、温控等方面的技术优势及研发平台、供应链平台、人才机制、全国乃至全球的营销渠道资源等，特别是国际营销渠道资源，不断支持上市公司拓展国内、国际业务，充分发挥业务、资本、管理等方面的优势支持上市公司发展”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,优势/有利条件(advantage):0.7"}, "与此同时，还将强化激励机制，保持上市公司经营管理团队、员工队伍稳定": {"topic": "“金融”", "similarity": 0.4528171420097351, "prompt": "新闻文本是“与此同时，还将强化激励机制，保持上市公司经营管理团队、员工队伍稳定”，包含的情绪词典是：使稳定/稳定(stabilize):0.5,鼓励/激励(encouragement):0.6"}, "此次新当选的科林电气董事史文伯此前在接受记者采访时曾代表海信承诺，控股科林电气后，科林电气的注册地、生产地、纳税地、生产场所、管理机构等不会搬离石家庄": {"topic": "“生产投资”", "similarity": 0.5259331464767456, "prompt": "新闻文本是“此次新当选的科林电气董事史文伯此前在接受记者采访时曾代表海信承诺，控股科林电气后，科林电气的注册地、生产地、纳税地、生产场所、管理机构等不会搬离石家庄”，包含的情绪词典是：电的/电气的(electrical):0.0"}, "这一表态，不仅展现了其对科林电气未来发展的信心，也体现了海信愿意与各方股东共享发展成果的信心，尤其体现了海信愿意对石家庄当地经济做贡献的诚心与信心": {"topic": "“生产投资”", "similarity": 0.582343578338623, "prompt": "新闻文本是“这一表态，不仅展现了其对科林电气未来发展的信心，也体现了海信愿意与各方股东共享发展成果的信心，尤其体现了海信愿意对石家庄当地经济做贡献的诚心与信心”，包含的情绪词典是：自信的/有信心的(confident):0.5,有利的/赞成的(favorable):0.6"}, "科林电气此次换届选举，为公司管理团队注入新鲜血液，公司治理结构进一步完善，各方股东强强联合，共谋公司发展，对公司未来发展迈向新能级具有关键意义": {"topic": "“生产投资”", "similarity": 0.5770071744918823, "prompt": "新闻文本是“科林电气此次换届选举，为公司管理团队注入新鲜血液，公司治理结构进一步完善，各方股东强强联合，共谋公司发展，对公司未来发展迈向新能级具有关键意义”，包含的情绪词典是：电的/电气的(electrical):0.0,公司的/企业的(corporate):0.0"}, "（文章来源：大河财立方）": {"topic": "“金融”", "similarity": 0.47285929322242737, "prompt": "新闻文本是“（文章来源：大河财立方）”，包含的情绪词典是：金钱/货币(money):0.2,资本/资金(capital):0.1"}}</t>
+          <t>{"新一届监事会3名监事席位中，除职工代表监事外，海信网能和石家庄国投各提名并当选一位非职工代表监事": {"topic": "“生产投资”", "similarity": 0.48071593046188354, "prompt": "新闻文本是“新一届监事会3名监事席位中，除职工代表监事外，海信网能和石家庄国投各提名并当选一位非职工代表监事”，包含的情绪词典是：监管的/调控的(regulatory):0.0,选举/推选(election):0.0"}, "海信网能、石家庄国投等各方都严格遵守法治精神、契约精神和资本市场规则": {"topic": "“生产投资”", "similarity": 0.5304060578346252, "prompt": "新闻文本是“海信网能、石家庄国投等各方都严格遵守法治精神、契约精神和资本市场规则”，包含的情绪词典是：契约/盟约(covenant):0.0,合同/契约(contract):0.0"}, "海信网能与石家庄国投以4：3比例组建新的董事会": {"topic": "“生产投资”", "similarity": 0.4877719283103943, "prompt": "新闻文本是“海信网能与石家庄国投以4：3比例组建新的董事会”，包含的情绪词典是：董事会/木板(board):0.0,转让/割让(cession):0.0"}, "新一届董事会组建后将尽快召开会议，完成董事长选举、管理层选聘等工作，实现公司平稳过渡，并坚持股东利益至上原则，最大程度保护广大投资者利益": {"topic": "“金融”", "similarity": 0.5782753825187683, "prompt": "新闻文本是“新一届董事会组建后将尽快召开会议，完成董事长选举、管理层选聘等工作，实现公司平稳过渡，并坚持股东利益至上原则，最大程度保护广大投资者利益”，包含的情绪词典是：董事会/木板(board):0.0,公司的/企业的(corporate):0.0"}, "海信网能方面表示，将与石家庄国投、公司原有团队等各方团结合作、共谋上市公司发展，共同努力，一起把科林电气做大做强": {"topic": "“生产投资”", "similarity": 0.5563783049583435, "prompt": "新闻文本是“海信网能方面表示，将与石家庄国投、公司原有团队等各方团结合作、共谋上市公司发展，共同努力，一起把科林电气做大做强”，包含的情绪词典是：电的/电气的(electrical):0.0,公司的/企业的(corporate):0.0"}, "科林电气新一届董事会及后续的经营层，将持续提升上市公司价值，与投资者共享发展成果，不断增强投资者获得感": {"topic": "“金融”", "similarity": 0.5590028762817383, "prompt": "新闻文本是“科林电气新一届董事会及后续的经营层，将持续提升上市公司价值，与投资者共享发展成果，不断增强投资者获得感”，包含的情绪词典是：电的/电气的(electrical):0.0,增强/提高(enhancement):0.6"}, "同时，海信网能将在合法合规基础上积极调动海信集团内部的优质资源，例如海信集团在芯片、功率半导体、电子、电力电子、软件、温控等方面的技术优势及研发平台、供应链平台、人才机制、全国乃至全球的营销渠道资源等，特别是国际营销渠道资源，不断支持上市公司拓展国内、国际业务，充分发挥业务、资本、管理等方面的优势支持上市公司发展": {"topic": "“生产投资”", "similarity": 0.57986980676651, "prompt": "新闻文本是“同时，海信网能将在合法合规基础上积极调动海信集团内部的优质资源，例如海信集团在芯片、功率半导体、电子、电力电子、软件、温控等方面的技术优势及研发平台、供应链平台、人才机制、全国乃至全球的营销渠道资源等，特别是国际营销渠道资源，不断支持上市公司拓展国内、国际业务，充分发挥业务、资本、管理等方面的优势支持上市公司发展”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,优势/有利条件(advantage):0.7"}, "与此同时，还将强化激励机制，保持上市公司经营管理团队、员工队伍稳定": {"topic": "“金融”", "similarity": 0.45281723141670227, "prompt": "新闻文本是“与此同时，还将强化激励机制，保持上市公司经营管理团队、员工队伍稳定”，包含的情绪词典是：使稳定/稳定(stabilize):0.5,鼓励/激励(encouragement):0.6"}, "此次新当选的科林电气董事史文伯此前在接受记者采访时曾代表海信承诺，控股科林电气后，科林电气的注册地、生产地、纳税地、生产场所、管理机构等不会搬离石家庄": {"topic": "“生产投资”", "similarity": 0.5259331464767456, "prompt": "新闻文本是“此次新当选的科林电气董事史文伯此前在接受记者采访时曾代表海信承诺，控股科林电气后，科林电气的注册地、生产地、纳税地、生产场所、管理机构等不会搬离石家庄”，包含的情绪词典是：电的/电气的(electrical):0.0"}, "这一表态，不仅展现了其对科林电气未来发展的信心，也体现了海信愿意与各方股东共享发展成果的信心，尤其体现了海信愿意对石家庄当地经济做贡献的诚心与信心": {"topic": "“生产投资”", "similarity": 0.5823436379432678, "prompt": "新闻文本是“这一表态，不仅展现了其对科林电气未来发展的信心，也体现了海信愿意与各方股东共享发展成果的信心，尤其体现了海信愿意对石家庄当地经济做贡献的诚心与信心”，包含的情绪词典是：自信的/有信心的(confident):0.5,有利的/赞成的(favorable):0.6"}, "科林电气此次换届选举，为公司管理团队注入新鲜血液，公司治理结构进一步完善，各方股东强强联合，共谋公司发展，对公司未来发展迈向新能级具有关键意义": {"topic": "“生产投资”", "similarity": 0.5770072340965271, "prompt": "新闻文本是“科林电气此次换届选举，为公司管理团队注入新鲜血液，公司治理结构进一步完善，各方股东强强联合，共谋公司发展，对公司未来发展迈向新能级具有关键意义”，包含的情绪词典是：电的/电气的(electrical):0.0,公司的/企业的(corporate):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3934,12 +3902,12 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，春立医疗(688236.SH)发布2024年中报", "news_prompt2": "公司营业总收入为3.80亿元，在已披露的同业公司中排名第69，较去年同报告期营业总收入减少1.61亿元，同比较去年同期下降29.70%", "news_prompt3": "归母净利润为7902.61万元，在已披露的同业公司中排名第53，较去年同报告期归母净利润减少4705.10万元，同比较去年同期下降37.32%", "news_prompt4": "经营活动现金净流入为-6905.79万元，在已披露的同业公司中排名第111，较去年同报告期经营活动现金净流入减少3008.60万元", "news_prompt5": "公司最新资产负债率为22.39%，在已披露的同业公司中排名第74，较上季度资产负债率增加5.22个百分点，较去年同季度资产负债率增加0.94个百分点", "news_prompt6": "公司最新毛利率为71.52%，在已披露的同业公司中排名第23，较上季度毛利率减少2.31个百分点，较去年同季度毛利率减少0.86个百分点", "news_prompt7": "最新ROE为2.80%，在已披露的同业公司中排名第68，较去年同季度ROE减少1.82个百分点", "news_prompt8": "公司摊薄每股收益为0.21元，在已披露的同业公司中排名第73，较去年同报告期摊薄每股收益减少0.12元，同比较去年同期下降37.33%", "news_prompt9": "公司最新总资产周转率为0.10次，在已披露的同业公司中排名第100，较去年同季度总资产周转率减少0.05次，同比较去年同期下降33.55%", "news_prompt10": "最新存货周转率为0.23次，在已披露的同业公司中排名第125，较去年同季度存货周转率减少0.23次，同比较去年同期下降50.87%", "news_prompt11": "公司股东户数为7510户，前十大股东持股数量为2.42亿股，占总股本比例为63.12%", "news_prompt12": "前十大股东分别为史春宝、岳术俊、北京磐茂投资管理有限公司-磐茂(上海)投资中心(有限合伙)、黄东、北京磐茂投资管理有限公司-磐信(上海)投资中心(有限合伙)、中国人寿保险股份有限公司-传统-普通保险产品-005L-CT001沪、香港中央结算有限公司、招商银行股份有限公司-朱雀恒心一年持有期混合型证券投资基金、龙赢富泽资产管理(北京)有限公司-龙赢医疗健康优选1期私募证券投资基金、金杰，持股比例分别为29.64%、24.88%、4.50%、0.66%、0.65%、0.65%、0.60%、0.54%、0.53%、0.48%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为3.80亿元，在已披露的同业公司中排名第69，较去年同报告期营业总收入减少1.61亿元，同比较去年同期下降29.70%", "news_prompt2": "归母净利润为7902.61万元，在已披露的同业公司中排名第53，较去年同报告期归母净利润减少4705.10万元，同比较去年同期下降37.32%", "news_prompt3": "经营活动现金净流入为-6905.79万元，在已披露的同业公司中排名第111，较去年同报告期经营活动现金净流入减少3008.60万元", "news_prompt4": "公司最新资产负债率为22.39%，在已披露的同业公司中排名第74，较上季度资产负债率增加5.22个百分点，较去年同季度资产负债率增加0.94个百分点", "news_prompt5": "公司最新毛利率为71.52%，在已披露的同业公司中排名第23，较上季度毛利率减少2.31个百分点，较去年同季度毛利率减少0.86个百分点", "news_prompt6": "公司摊薄每股收益为0.21元，在已披露的同业公司中排名第73，较去年同报告期摊薄每股收益减少0.12元，同比较去年同期下降37.33%", "news_prompt7": "公司最新总资产周转率为0.10次，在已披露的同业公司中排名第100，较去年同季度总资产周转率减少0.05次，同比较去年同期下降33.55%", "news_prompt8": "最新存货周转率为0.23次，在已披露的同业公司中排名第125，较去年同季度存货周转率减少0.23次，同比较去年同期下降50.87%", "news_prompt9": "公司股东户数为7510户，前十大股东持股数量为2.42亿股，占总股本比例为63.12%"}</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，春立医疗(688236.SH)发布2024年中报": {"topic": "“金融”", "similarity": 0.45271867513656616, "prompt": "新闻文本是“2024年8月31日，春立医疗(688236.SH)发布2024年中报”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "公司营业总收入为3.80亿元，在已披露的同业公司中排名第69，较去年同报告期营业总收入减少1.61亿元，同比较去年同期下降29.70%": {"topic": "“消费”", "similarity": 0.5267640948295593, "prompt": "新闻文本是“公司营业总收入为3.80亿元，在已披露的同业公司中排名第69，较去年同报告期营业总收入减少1.61亿元，同比较去年同期下降29.70%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "归母净利润为7902.61万元，在已披露的同业公司中排名第53，较去年同报告期归母净利润减少4705.10万元，同比较去年同期下降37.32%": {"topic": "“消费”", "similarity": 0.505182147026062, "prompt": "新闻文本是“归母净利润为7902.61万元，在已披露的同业公司中排名第53，较去年同报告期归母净利润减少4705.10万元，同比较去年同期下降37.32%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "经营活动现金净流入为-6905.79万元，在已披露的同业公司中排名第111，较去年同报告期经营活动现金净流入减少3008.60万元": {"topic": "“金融”", "similarity": 0.5118440389633179, "prompt": "新闻文本是“经营活动现金净流入为-6905.79万元，在已披露的同业公司中排名第111，较去年同报告期经营活动现金净流入减少3008.60万元”，包含的情绪词典是：营业额/周转(turnover):0.0,非流动性/缺乏流动性(illiquidity):-0.5"}, "公司最新资产负债率为22.39%，在已披露的同业公司中排名第74，较上季度资产负债率增加5.22个百分点，较去年同季度资产负债率增加0.94个百分点": {"topic": "“消费”", "similarity": 0.4721578359603882, "prompt": "新闻文本是“公司最新资产负债率为22.39%，在已披露的同业公司中排名第74，较上季度资产负债率增加5.22个百分点，较去年同季度资产负债率增加0.94个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,赤字/亏损(deficit):-0.6"}, "公司最新毛利率为71.52%，在已披露的同业公司中排名第23，较上季度毛利率减少2.31个百分点，较去年同季度毛利率减少0.86个百分点": {"topic": "“消费”", "similarity": 0.4357486367225647, "prompt": "新闻文本是“公司最新毛利率为71.52%，在已披露的同业公司中排名第23，较上季度毛利率减少2.31个百分点，较去年同季度毛利率减少0.86个百分点”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司摊薄每股收益为0.21元，在已披露的同业公司中排名第73，较去年同报告期摊薄每股收益减少0.12元，同比较去年同期下降37.33%": {"topic": "“金融”", "similarity": 0.4614843726158142, "prompt": "新闻文本是“公司摊薄每股收益为0.21元，在已披露的同业公司中排名第73，较去年同报告期摊薄每股收益减少0.12元，同比较去年同期下降37.33%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新总资产周转率为0.10次，在已披露的同业公司中排名第100，较去年同季度总资产周转率减少0.05次，同比较去年同期下降33.55%": {"topic": "“消费”", "similarity": 0.508526086807251, "prompt": "新闻文本是“公司最新总资产周转率为0.10次，在已披露的同业公司中排名第100，较去年同季度总资产周转率减少0.05次，同比较去年同期下降33.55%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "最新存货周转率为0.23次，在已披露的同业公司中排名第125，较去年同季度存货周转率减少0.23次，同比较去年同期下降50.87%": {"topic": "“消费”", "similarity": 0.4467793107032776, "prompt": "新闻文本是“最新存货周转率为0.23次，在已披露的同业公司中排名第125，较去年同季度存货周转率减少0.23次，同比较去年同期下降50.87%”，包含的情绪词典是：营业额/周转(turnover):0.0,减少/降低(reduction):-0.4"}, "公司股东户数为7510户，前十大股东持股数量为2.42亿股，占总股本比例为63.12%": {"topic": "“金融”", "similarity": 0.47583699226379395, "prompt": "新闻文本是“公司股东户数为7510户，前十大股东持股数量为2.42亿股，占总股本比例为63.12%”，包含的情绪词典是：公司的/企业的(corporate):0.0,百分比(percentage):0.0"}, "前十大股东分别为史春宝、岳术俊、北京磐茂投资管理有限公司-磐茂(上海)投资中心(有限合伙)、黄东、北京磐茂投资管理有限公司-磐信(上海)投资中心(有限合伙)、中国人寿保险股份有限公司-传统-普通保险产品-005L-CT001沪、香港中央结算有限公司、招商银行股份有限公司-朱雀恒心一年持有期混合型证券投资基金、龙赢富泽资产管理(北京)有限公司-龙赢医疗健康优选1期私募证券投资基金、金杰，持股比例分别为29.64%、24.88%、4.50%、0.66%、0.65%、0.65%、0.60%、0.54%、0.53%、0.48%": {"topic": "“生产投资”", "similarity": 0.5805981159210205}}</t>
+          <t>{"公司营业总收入为3.80亿元，在已披露的同业公司中排名第69，较去年同报告期营业总收入减少1.61亿元，同比较去年同期下降29.70%": {"topic": "“消费”", "similarity": 0.5267641544342041, "prompt": "新闻文本是“公司营业总收入为3.80亿元，在已披露的同业公司中排名第69，较去年同报告期营业总收入减少1.61亿元，同比较去年同期下降29.70%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "归母净利润为7902.61万元，在已披露的同业公司中排名第53，较去年同报告期归母净利润减少4705.10万元，同比较去年同期下降37.32%": {"topic": "“消费”", "similarity": 0.505182147026062, "prompt": "新闻文本是“归母净利润为7902.61万元，在已披露的同业公司中排名第53，较去年同报告期归母净利润减少4705.10万元，同比较去年同期下降37.32%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "经营活动现金净流入为-6905.79万元，在已披露的同业公司中排名第111，较去年同报告期经营活动现金净流入减少3008.60万元": {"topic": "“金融”", "similarity": 0.5118441581726074, "prompt": "新闻文本是“经营活动现金净流入为-6905.79万元，在已披露的同业公司中排名第111，较去年同报告期经营活动现金净流入减少3008.60万元”，包含的情绪词典是：营业额/周转(turnover):0.0,非流动性/缺乏流动性(illiquidity):-0.5"}, "公司最新资产负债率为22.39%，在已披露的同业公司中排名第74，较上季度资产负债率增加5.22个百分点，较去年同季度资产负债率增加0.94个百分点": {"topic": "“消费”", "similarity": 0.4721578359603882, "prompt": "新闻文本是“公司最新资产负债率为22.39%，在已披露的同业公司中排名第74，较上季度资产负债率增加5.22个百分点，较去年同季度资产负债率增加0.94个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,赤字/亏损(deficit):-0.6"}, "公司最新毛利率为71.52%，在已披露的同业公司中排名第23，较上季度毛利率减少2.31个百分点，较去年同季度毛利率减少0.86个百分点": {"topic": "“消费”", "similarity": 0.4357486367225647, "prompt": "新闻文本是“公司最新毛利率为71.52%，在已披露的同业公司中排名第23，较上季度毛利率减少2.31个百分点，较去年同季度毛利率减少0.86个百分点”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "公司摊薄每股收益为0.21元，在已披露的同业公司中排名第73，较去年同报告期摊薄每股收益减少0.12元，同比较去年同期下降37.33%": {"topic": "“金融”", "similarity": 0.46148452162742615, "prompt": "新闻文本是“公司摊薄每股收益为0.21元，在已披露的同业公司中排名第73，较去年同报告期摊薄每股收益减少0.12元，同比较去年同期下降37.33%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新总资产周转率为0.10次，在已披露的同业公司中排名第100，较去年同季度总资产周转率减少0.05次，同比较去年同期下降33.55%": {"topic": "“消费”", "similarity": 0.5085263252258301, "prompt": "新闻文本是“公司最新总资产周转率为0.10次，在已披露的同业公司中排名第100，较去年同季度总资产周转率减少0.05次，同比较去年同期下降33.55%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "最新存货周转率为0.23次，在已披露的同业公司中排名第125，较去年同季度存货周转率减少0.23次，同比较去年同期下降50.87%": {"topic": "“消费”", "similarity": 0.44677942991256714, "prompt": "新闻文本是“最新存货周转率为0.23次，在已披露的同业公司中排名第125，较去年同季度存货周转率减少0.23次，同比较去年同期下降50.87%”，包含的情绪词典是：营业额/周转(turnover):0.0,减少/降低(reduction):-0.4"}, "公司股东户数为7510户，前十大股东持股数量为2.42亿股，占总股本比例为63.12%": {"topic": "“金融”", "similarity": 0.47583717107772827, "prompt": "新闻文本是“公司股东户数为7510户，前十大股东持股数量为2.42亿股，占总股本比例为63.12%”，包含的情绪词典是：公司的/企业的(corporate):0.0,百分比(percentage):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -3985,12 +3953,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "【1】重庆取消限售、按区认定首套房 　　近日，重庆市住房城乡建委发布《关于调整优化房地产交易政策的通知》显示，自2024年9月1日起，凡在重庆市中心城区新购新建商品住房和二手住房的（以网签备案时间为准），取得《不动产权证书》后即可上市交易", "news_prompt2": "此次，重庆还优化住房套数认定标准，居民家庭（包括借款人、配偶及未成年子女）在重庆市申请商业性个人住房贷款购买商品住房时，仅核查家庭成员在拟购住房所在区县（自治县，以下简称区县）的住房情况，家庭成员在拟购住房所在区县无住房的，认定为首套房", "news_prompt3": "【2】万科:“一揽子方案”不是简单做“减法” 　　近日，万科举行中期业绩会", "news_prompt4": "万科董事会秘书朱旭在介绍当前阶段整体工作思路时表示，上半年制定并落地的“一揽子方案”是万科集团全面化解潜在风险，积极适应行业向新发展模式转变的五年计划", "news_prompt5": "朱旭称，“一揽子方案”不是简单的做“减法”，还包括发展方案，具体包括：积极推进综合住区产品模块研发创新，提升开发业务竞争力", "news_prompt6": "确保投资兑现水平", "news_prompt7": "实现长租公寓、物业服务等经营服务业务资产管理规模有质量增长，竞争力行业领先等", "news_prompt8": "随着“一揽子方案”的推进，万科渡过近两年的阶段性困难之后，业务将更加聚焦，投资将更加聚焦，能力将更加聚焦，步入高质量发展轨道", "news_prompt9": "【3】碧桂园延迟刊发2024年中期业绩 　　近日，碧桂园发布公告称，将延迟刊发2024年中期业绩及寄发2024年中期报告，进一步延迟刊发2023年度业绩及寄发2023年度报告", "news_prompt10": "碧桂园称，由于行业持续波动以及集团正在进行债务重组工作，集团需要更多时间去收集资料以作出适当的会计估计及判断，以及收集相关财务资料以谨慎评估其现时及未来的财务资源及财务义务，以便落实2023年度业绩及2023年度报告", "news_prompt11": "目前，上述工作仍在进行中", "news_prompt12": "因此，预期将会进一步延迟刊发2023年度业绩", "news_prompt13": "【4】中交地产上半年归母净利润同比下降72.86% 　　近日，中交地产发布2024年半年报显示，2024年1—6月，中交地产营业收入为89.8亿元，同比增长2.48%", "news_prompt14": "归母净利润为-9.83亿元，同比下降72.86%", "news_prompt15": "扣非归母净利润为-10.01亿元，同比下降70.54%", "news_prompt16": "基本每股收益-1.41元", "news_prompt17": "【5】格力地产上半年归母净亏损同比扩大266.46% 　　近日，格力地产发布2024年半年度报告显示，2024年1—6月，格力地产营业收入18.93亿元，同比增加2.01%", "news_prompt18": "净亏损7.77亿元，同比扩大264.79%", "news_prompt19": "归母净亏损7.769亿元，同比扩大266.46%", "news_prompt20": "（文章来源：北京商报）"}</t>
+          <t>{"news_prompt1": "【2】万科:“一揽子方案”不是简单做“减法” 　　近日，万科举行中期业绩会", "news_prompt2": "确保投资兑现水平", "news_prompt3": "实现长租公寓、物业服务等经营服务业务资产管理规模有质量增长，竞争力行业领先等", "news_prompt4": "随着“一揽子方案”的推进，万科渡过近两年的阶段性困难之后，业务将更加聚焦，投资将更加聚焦，能力将更加聚焦，步入高质量发展轨道", "news_prompt5": "【3】碧桂园延迟刊发2024年中期业绩 　　近日，碧桂园发布公告称，将延迟刊发2024年中期业绩及寄发2024年中期报告，进一步延迟刊发2023年度业绩及寄发2023年度报告", "news_prompt6": "碧桂园称，由于行业持续波动以及集团正在进行债务重组工作，集团需要更多时间去收集资料以作出适当的会计估计及判断，以及收集相关财务资料以谨慎评估其现时及未来的财务资源及财务义务，以便落实2023年度业绩及2023年度报告", "news_prompt7": "【4】中交地产上半年归母净利润同比下降72.86% 　　近日，中交地产发布2024年半年报显示，2024年1—6月，中交地产营业收入为89.8亿元，同比增长2.48%", "news_prompt8": "基本每股收益-1.41元", "news_prompt9": "【5】格力地产上半年归母净亏损同比扩大266.46% 　　近日，格力地产发布2024年半年度报告显示，2024年1—6月，格力地产营业收入18.93亿元，同比增加2.01%"}</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>{"【1】重庆取消限售、按区认定首套房 　　近日，重庆市住房城乡建委发布《关于调整优化房地产交易政策的通知》显示，自2024年9月1日起，凡在重庆市中心城区新购新建商品住房和二手住房的（以网签备案时间为准），取得《不动产权证书》后即可上市交易": {"topic": "“房地产”", "similarity": 0.7005307078361511}, "此次，重庆还优化住房套数认定标准，居民家庭（包括借款人、配偶及未成年子女）在重庆市申请商业性个人住房贷款购买商品住房时，仅核查家庭成员在拟购住房所在区县（自治县，以下简称区县）的住房情况，家庭成员在拟购住房所在区县无住房的，认定为首套房": {"topic": "“房地产”", "similarity": 0.6375501155853271}, "【2】万科:“一揽子方案”不是简单做“减法” 　　近日，万科举行中期业绩会": {"topic": "“房地产”", "similarity": 0.5632310509681702, "prompt": "新闻文本是“【2】万科:“一揽子方案”不是简单做“减法” 　　近日，万科举行中期业绩会”，包含的情绪词典是：削减/缩减(curtailment):-0.2,削减/减少(cutbacks):-0.4"}, "万科董事会秘书朱旭在介绍当前阶段整体工作思路时表示，上半年制定并落地的“一揽子方案”是万科集团全面化解潜在风险，积极适应行业向新发展模式转变的五年计划": {"topic": "“宏观经济”", "similarity": 0.5557401180267334}, "朱旭称，“一揽子方案”不是简单的做“减法”，还包括发展方案，具体包括：积极推进综合住区产品模块研发创新，提升开发业务竞争力": {"topic": "“房地产”", "similarity": 0.5554367303848267}, "确保投资兑现水平": {"topic": "“生产投资”", "similarity": 0.44131430983543396, "prompt": "新闻文本是“确保投资兑现水平”，包含的情绪词典是：确保/保证(ensure):0.2,保证/确保(assure):0.3"}, "实现长租公寓、物业服务等经营服务业务资产管理规模有质量增长，竞争力行业领先等": {"topic": "“生产投资”", "similarity": 0.5836606025695801, "prompt": "新闻文本是“实现长租公寓、物业服务等经营服务业务资产管理规模有质量增长，竞争力行业领先等”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,服务/业务(service):0.0"}, "随着“一揽子方案”的推进，万科渡过近两年的阶段性困难之后，业务将更加聚焦，投资将更加聚焦，能力将更加聚焦，步入高质量发展轨道": {"topic": "“生产投资”", "similarity": 0.5854915976524353, "prompt": "新闻文本是“随着“一揽子方案”的推进，万科渡过近两年的阶段性困难之后，业务将更加聚焦，投资将更加聚焦，能力将更加聚焦，步入高质量发展轨道”，包含的情绪词典是：进步/进展(progressing):0.6,进步/进展(progresses):0.6"}, "【3】碧桂园延迟刊发2024年中期业绩 　　近日，碧桂园发布公告称，将延迟刊发2024年中期业绩及寄发2024年中期报告，进一步延迟刊发2023年度业绩及寄发2023年度报告": {"topic": "“房地产”", "similarity": 0.5892837643623352, "prompt": "新闻文本是“【3】碧桂园延迟刊发2024年中期业绩 　　近日，碧桂园发布公告称，将延迟刊发2024年中期业绩及寄发2024年中期报告，进一步延迟刊发2023年度业绩及寄发2023年度报告”，包含的情绪词典是：推迟/延期(postponement):-0.3,推迟/延期(postponed):-0.2"}, "碧桂园称，由于行业持续波动以及集团正在进行债务重组工作，集团需要更多时间去收集资料以作出适当的会计估计及判断，以及收集相关财务资料以谨慎评估其现时及未来的财务资源及财务义务，以便落实2023年度业绩及2023年度报告": {"topic": "“房地产”", "similarity": 0.5425916910171509, "prompt": "新闻文本是“碧桂园称，由于行业持续波动以及集团正在进行债务重组工作，集团需要更多时间去收集资料以作出适当的会计估计及判断，以及收集相关财务资料以谨慎评估其现时及未来的财务资源及财务义务，以便落实2023年度业绩及2023年度报告”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "【4】中交地产上半年归母净利润同比下降72.86% 　　近日，中交地产发布2024年半年报显示，2024年1—6月，中交地产营业收入为89.8亿元，同比增长2.48%": {"topic": "“房地产”", "similarity": 0.6387419104576111, "prompt": "新闻文本是“【4】中交地产上半年归母净利润同比下降72.86% 　　近日，中交地产发布2024年半年报显示，2024年1—6月，中交地产营业收入为89.8亿元，同比增长2.48%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "基本每股收益-1.41元": {"topic": "“金融”", "similarity": 0.4390885829925537, "prompt": "新闻文本是“基本每股收益-1.41元”，包含的情绪词典是：基本的/基础的(basic):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "【5】格力地产上半年归母净亏损同比扩大266.46% 　　近日，格力地产发布2024年半年度报告显示，2024年1—6月，格力地产营业收入18.93亿元，同比增加2.01%": {"topic": "“房地产”", "similarity": 0.6076622009277344, "prompt": "新闻文本是“【5】格力地产上半年归母净亏损同比扩大266.46% 　　近日，格力地产发布2024年半年度报告显示，2024年1—6月，格力地产营业收入18.93亿元，同比增加2.01%”，包含的情绪词典是：损失/亏损(loss):-0.7,消耗/亏损(burn):-0.2"}}</t>
+          <t>{"【2】万科:“一揽子方案”不是简单做“减法” 　　近日，万科举行中期业绩会": {"topic": "“房地产”", "similarity": 0.5632312297821045, "prompt": "新闻文本是“【2】万科:“一揽子方案”不是简单做“减法” 　　近日，万科举行中期业绩会”，包含的情绪词典是：削减/缩减(curtailment):-0.2,削减/减少(cutbacks):-0.4"}, "确保投资兑现水平": {"topic": "“生产投资”", "similarity": 0.44131433963775635, "prompt": "新闻文本是“确保投资兑现水平”，包含的情绪词典是：确保/保证(ensure):0.2,保证/确保(assure):0.3"}, "实现长租公寓、物业服务等经营服务业务资产管理规模有质量增长，竞争力行业领先等": {"topic": "“生产投资”", "similarity": 0.5836604833602905, "prompt": "新闻文本是“实现长租公寓、物业服务等经营服务业务资产管理规模有质量增长，竞争力行业领先等”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,服务/业务(service):0.0"}, "随着“一揽子方案”的推进，万科渡过近两年的阶段性困难之后，业务将更加聚焦，投资将更加聚焦，能力将更加聚焦，步入高质量发展轨道": {"topic": "“生产投资”", "similarity": 0.5854917764663696, "prompt": "新闻文本是“随着“一揽子方案”的推进，万科渡过近两年的阶段性困难之后，业务将更加聚焦，投资将更加聚焦，能力将更加聚焦，步入高质量发展轨道”，包含的情绪词典是：进步/进展(progressing):0.6,进步/进展(progresses):0.6"}, "【3】碧桂园延迟刊发2024年中期业绩 　　近日，碧桂园发布公告称，将延迟刊发2024年中期业绩及寄发2024年中期报告，进一步延迟刊发2023年度业绩及寄发2023年度报告": {"topic": "“房地产”", "similarity": 0.5892837643623352, "prompt": "新闻文本是“【3】碧桂园延迟刊发2024年中期业绩 　　近日，碧桂园发布公告称，将延迟刊发2024年中期业绩及寄发2024年中期报告，进一步延迟刊发2023年度业绩及寄发2023年度报告”，包含的情绪词典是：推迟/延期(postponement):-0.3,推迟/延期(postponed):-0.2"}, "碧桂园称，由于行业持续波动以及集团正在进行债务重组工作，集团需要更多时间去收集资料以作出适当的会计估计及判断，以及收集相关财务资料以谨慎评估其现时及未来的财务资源及财务义务，以便落实2023年度业绩及2023年度报告": {"topic": "“房地产”", "similarity": 0.5425920486450195, "prompt": "新闻文本是“碧桂园称，由于行业持续波动以及集团正在进行债务重组工作，集团需要更多时间去收集资料以作出适当的会计估计及判断，以及收集相关财务资料以谨慎评估其现时及未来的财务资源及财务义务，以便落实2023年度业绩及2023年度报告”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforms):-0.4"}, "【4】中交地产上半年归母净利润同比下降72.86% 　　近日，中交地产发布2024年半年报显示，2024年1—6月，中交地产营业收入为89.8亿元，同比增长2.48%": {"topic": "“房地产”", "similarity": 0.6387419700622559, "prompt": "新闻文本是“【4】中交地产上半年归母净利润同比下降72.86% 　　近日，中交地产发布2024年半年报显示，2024年1—6月，中交地产营业收入为89.8亿元，同比增长2.48%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "基本每股收益-1.41元": {"topic": "“金融”", "similarity": 0.4390886425971985, "prompt": "新闻文本是“基本每股收益-1.41元”，包含的情绪词典是：基本的/基础的(basic):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "【5】格力地产上半年归母净亏损同比扩大266.46% 　　近日，格力地产发布2024年半年度报告显示，2024年1—6月，格力地产营业收入18.93亿元，同比增加2.01%": {"topic": "“房地产”", "similarity": 0.6076623201370239, "prompt": "新闻文本是“【5】格力地产上半年归母净亏损同比扩大266.46% 　　近日，格力地产发布2024年半年度报告显示，2024年1—6月，格力地产营业收入18.93亿元，同比增加2.01%”，包含的情绪词典是：损失/亏损(loss):-0.7,消耗/亏损(burn):-0.2"}}</t>
         </is>
       </c>
     </row>
@@ -4036,12 +4004,12 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "界面新闻记者 | 黄华 　　曾经的明星疫苗企业斯微生物如今与其创始人对簿公堂", "news_prompt2": "8月21日，在上海浦东自由贸易区法庭，李航文起诉斯微（上海）生物科技股份有限公司的案子如期开庭", "news_prompt3": "庭上，原告方李航文本人没有出现，被告方斯微生物也缺席了审判现场", "news_prompt4": "不过，沈海法及其律师团队作为第三方出现在了庭上", "news_prompt5": "但在庭上，不仅原告方李航文本人没有出现，李航文的律师也表示不知李航文身在何处", "news_prompt6": "斯微生物曾是国内知名的独角兽公司，成立于2016年，李航文和沈海法都是斯微生物的联合创始人", "news_prompt7": "在今年5月7日召开的斯微生物董事会上，李航文被罢免了公司董事长兼首席执行官一职", "news_prompt8": "同一时间，原首席技术官（CTO）沈海法接替他成为了这家公司的新任董事长兼首席执行官", "news_prompt9": "这样的变动也是这起案件的导火索", "news_prompt10": "庭上，李航文一方提出，其仍有履职能力和意愿，希望法院判决斯微生物董事会在今年5月7日做出的罢免任命等决议不成立", "news_prompt11": "李航文一方认为，依据公司章程，该公司的董事会设有7个席位，董事会之际，应有7名董事的过半人数出席，也就是4人及以上，而若是一项决议想要获得通过，也应有7名董事的过半人数通过", "news_prompt12": "不过，在今年5月7日的那场董事会上，在职的董事人数已仅有5名，当天会议有4人出席，并有3票支持决议通过，由此，这场董事会的出席人数虽然达到了4人及以上的标准，但通过人数没有达到", "news_prompt13": "基于该理由，李航文一方希望法院能支持其请求，判决其被罢免等事项不成立", "news_prompt14": "庭上，沈海法一方表示，被告方斯微生物知悉此诉讼案，但公司没有诉讼代表人，所以缺席", "news_prompt15": "另外，沈海法一方希望法院支持董事会决议成立", "news_prompt16": "诉讼当日，法院未有宣判", "news_prompt17": "目前，围绕3票通过的董事会决议是否成立这一问题，诉讼仍在进行中", "news_prompt18": "8月21日，沈海法方面向界面新闻记者表示，由于诉讼还在进行中，关于案件其不便多言", "news_prompt19": "目前，斯微生物由他主持工作，公司境况也确实不佳，但他认为公司还有价值，值得拯救", "news_prompt20": "同日，李航文方面没有回复记者的采访短信", "news_prompt21": "公开资料显示，李航文最初是微量元素营养硕士，之后到美国德州大学安德森癌症中心读博，2010年获得肿瘤生物学博士学位", "news_prompt22": "2016年，他在导师唐定国的建议下，回国创业", "news_prompt23": "据企业官网，唐定国也是斯微生物的联合创始人", "news_prompt24": "2020年初，新冠疫情危机骤起，mRNA领域的投资热情随之爆发，李航文的创业公司便开启了疾速发展的三年", "news_prompt25": "另一位创始人沈海法原是康奈尔大学医学院休斯顿卫理会医院纳米医学系教授、医院肿瘤中心转化医学部门负责人，在2021年11月全职加入斯微生物担任首席技术官，他也是LPP（自主知识产权的脂质多聚物纳米载体技术平台）技术发明人", "news_prompt26": "斯微生物的风光也仅存续了三年", "news_prompt27": "在去年9月15日，据行业媒体医药魔方Invest等多家媒体报道，斯微生物及公司法定代表人李航文被限制高消费", "news_prompt28": "去年9月18日，据《每日经济新闻》实地探查，斯微生物位于上海浦东川桥路附近的办公楼内已无人办公", "news_prompt29": "由此，该公司在新冠疫苗红利散去后的经营窘况也开始暴露在公众面前", "news_prompt30": "另外，据行业媒体深蓝观今年5月20日报道，斯微生物宣布的债务就有3.5亿元，截至今年3月，该公司已出现现金流断裂数月、员工纷纷离职、供应商诉讼追讨欠款等问题，在2月里，公司还讨论过重组方案", "news_prompt31": "高光时刻 　　在新冠疫情早期，这一史无前例的全球性公共卫生危机、却也是产业的风口下，海内外知名药企和科研团队的研发攻关战也在2020年初就拉开了序幕", "news_prompt32": "比起药物，拥有预防功能的疫苗更加引发关注", "news_prompt33": "疫苗领域内，一则最初引发全球关注的重磅消息是，在新冠病毒的基因序列于2020年1月11日被公布后，美国公司莫德纳（Moderna）于1月13日就完成了mRNA疫苗序列研究工作", "news_prompt34": "仅仅两日之内就实现了序列突破，让处于危机之中的全球喜出望外", "news_prompt35": "这一进度也提示了，mRNA疫苗合成工艺简单、生产速度快，从基因测序至生产只需数周时间，有望在对时间要求比较紧急的疫情中有望发挥重要作用", "news_prompt36": "同时，在以全球人口基数作为潜在需求对象的巨大市场想象中，商业价值不容小觑", "news_prompt37": "李航文也看到了美国莫德纳（Moderna）的那则 “于2020年1月13日完成mRNA疫苗序列研究工作”的消息", "news_prompt38": "于是，他赶忙发布了一篇新闻稿，介绍斯微生物也是一家可以在新冠疫苗中引入mRNA技术的公司", "news_prompt39": "此后，稿件引发关注", "news_prompt40": "作为斯微生物创始人，李航文意识到了机遇降临", "news_prompt41": "在2020年之前，mRNA技术在国内的知晓度并不高，斯微生物的融资也并不顺利", "news_prompt42": "其中，北京华瑞健生科技有限公司（简称“华瑞健生”）是天使轮融资者，投资时间是2017年4月，后在2018年6月退出", "news_prompt43": "这笔钱让李航文买下了沈海法在美国研发出的新型脂质体纳米材料（lipopolyplex，LPP）递送系统的专利归属权，余下的钱花在了团队搭建和购买设备上", "news_prompt44": "2018年6月，华瑞健生退出"}</t>
+          <t>{"news_prompt1": "这样的变动也是这起案件的导火索", "news_prompt2": "李航文一方认为，依据公司章程，该公司的董事会设有7个席位，董事会之际，应有7名董事的过半人数出席，也就是4人及以上，而若是一项决议想要获得通过，也应有7名董事的过半人数通过", "news_prompt3": "不过，在今年5月7日的那场董事会上，在职的董事人数已仅有5名，当天会议有4人出席，并有3票支持决议通过，由此，这场董事会的出席人数虽然达到了4人及以上的标准，但通过人数没有达到", "news_prompt4": "据企业官网，唐定国也是斯微生物的联合创始人", "news_prompt5": "在去年9月15日，据行业媒体医药魔方Invest等多家媒体报道，斯微生物及公司法定代表人李航文被限制高消费", "news_prompt6": "另外，据行业媒体深蓝观今年5月20日报道，斯微生物宣布的债务就有3.5亿元，截至今年3月，该公司已出现现金流断裂数月、员工纷纷离职、供应商诉讼追讨欠款等问题，在2月里，公司还讨论过重组方案", "news_prompt7": "高光时刻 　　在新冠疫情早期，这一史无前例的全球性公共卫生危机、却也是产业的风口下，海内外知名药企和科研团队的研发攻关战也在2020年初就拉开了序幕", "news_prompt8": "这一进度也提示了，mRNA疫苗合成工艺简单、生产速度快，从基因测序至生产只需数周时间，有望在对时间要求比较紧急的疫情中有望发挥重要作用", "news_prompt9": "同时，在以全球人口基数作为潜在需求对象的巨大市场想象中，商业价值不容小觑", "news_prompt10": "此后，稿件引发关注"}</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>{"斯微生物曾是国内知名的独角兽公司，成立于2016年，李航文和沈海法都是斯微生物的联合创始人": {"topic": "“生产投资”", "similarity": 0.4712781310081482}, "这样的变动也是这起案件的导火索": {"topic": "“金融”", "similarity": 0.4253292679786682, "prompt": "新闻文本是“这样的变动也是这起案件的导火索”，包含的情绪词典是：改变/变化(vary):0.0,改变/变更(alteration):0.0"}, "李航文一方认为，依据公司章程，该公司的董事会设有7个席位，董事会之际，应有7名董事的过半人数出席，也就是4人及以上，而若是一项决议想要获得通过，也应有7名董事的过半人数通过": {"topic": "“金融”", "similarity": 0.48431211709976196, "prompt": "新闻文本是“李航文一方认为，依据公司章程，该公司的董事会设有7个席位，董事会之际，应有7名董事的过半人数出席，也就是4人及以上，而若是一项决议想要获得通过，也应有7名董事的过半人数通过”，包含的情绪词典是：公司的/企业的(corporate):0.0,几个/数个(several):0.0"}, "不过，在今年5月7日的那场董事会上，在职的董事人数已仅有5名，当天会议有4人出席，并有3票支持决议通过，由此，这场董事会的出席人数虽然达到了4人及以上的标准，但通过人数没有达到": {"topic": "“金融”", "similarity": 0.4443470239639282, "prompt": "新闻文本是“不过，在今年5月7日的那场董事会上，在职的董事人数已仅有5名，当天会议有4人出席，并有3票支持决议通过，由此，这场董事会的出席人数虽然达到了4人及以上的标准，但通过人数没有达到”，包含的情绪词典是：出席人数/产量(turnout):0.0,失败/未通过(fails):-0.8"}, "据企业官网，唐定国也是斯微生物的联合创始人": {"topic": "“生产投资”", "similarity": 0.4727717936038971, "prompt": "新闻文本是“据企业官网，唐定国也是斯微生物的联合创始人”，包含的情绪词典是：公司/企业(firm):0.0,公司的/企业的(corporate):0.0"}, "另一位创始人沈海法原是康奈尔大学医学院休斯顿卫理会医院纳米医学系教授、医院肿瘤中心转化医学部门负责人，在2021年11月全职加入斯微生物担任首席技术官，他也是LPP（自主知识产权的脂质多聚物纳米载体技术平台）技术发明人": {"topic": "“生产投资”", "similarity": 0.4891204237937927}, "在去年9月15日，据行业媒体医药魔方Invest等多家媒体报道，斯微生物及公司法定代表人李航文被限制高消费": {"topic": "“消费”", "similarity": 0.4784824252128601, "prompt": "新闻文本是“在去年9月15日，据行业媒体医药魔方Invest等多家媒体报道，斯微生物及公司法定代表人李航文被限制高消费”，包含的情绪词典是：限制/限定(limit):-0.1,限制/局限(confine):-0.3"}, "另外，据行业媒体深蓝观今年5月20日报道，斯微生物宣布的债务就有3.5亿元，截至今年3月，该公司已出现现金流断裂数月、员工纷纷离职、供应商诉讼追讨欠款等问题，在2月里，公司还讨论过重组方案": {"topic": "“生产投资”", "similarity": 0.49985599517822266, "prompt": "新闻文本是“另外，据行业媒体深蓝观今年5月20日报道，斯微生物宣布的债务就有3.5亿元，截至今年3月，该公司已出现现金流断裂数月、员工纷纷离职、供应商诉讼追讨欠款等问题，在2月里，公司还讨论过重组方案”，包含的情绪词典是：负债的/欠债的(indebted):-0.5,表现不佳/业绩低于预期(underperformed):-0.4"}, "高光时刻 　　在新冠疫情早期，这一史无前例的全球性公共卫生危机、却也是产业的风口下，海内外知名药企和科研团队的研发攻关战也在2020年初就拉开了序幕": {"topic": "“生产投资”", "similarity": 0.5955730676651001, "prompt": "新闻文本是“高光时刻 　　在新冠疫情早期，这一史无前例的全球性公共卫生危机、却也是产业的风口下，海内外知名药企和科研团队的研发攻关战也在2020年初就拉开了序幕”，包含的情绪词典是：高的/高等的(high):0.7,最高的/最高级的(highest):0.7"}, "这一进度也提示了，mRNA疫苗合成工艺简单、生产速度快，从基因测序至生产只需数周时间，有望在对时间要求比较紧急的疫情中有望发挥重要作用": {"topic": "“生产投资”", "similarity": 0.5202807784080505, "prompt": "新闻文本是“这一进度也提示了，mRNA疫苗合成工艺简单、生产速度快，从基因测序至生产只需数周时间，有望在对时间要求比较紧急的疫情中有望发挥重要作用”，包含的情绪词典是：技术的/工艺的(technical):0.0,过程/进程(process):0.0"}, "同时，在以全球人口基数作为潜在需求对象的巨大市场想象中，商业价值不容小觑": {"topic": "“宏观经济”", "similarity": 0.4260770082473755, "prompt": "新闻文本是“同时，在以全球人口基数作为潜在需求对象的巨大市场想象中，商业价值不容小觑”，包含的情绪词典是：潜在的/潜力(potential):0.3,可想象的/可设想的(conceivable):0.0"}, "此后，稿件引发关注": {"topic": "“金融”", "similarity": 0.4458432197570801, "prompt": "新闻文本是“此后，稿件引发关注”，包含的情绪词典是：此后/以后(thereafter):0.0,此后/今后(hereafter):0.0"}, "其中，北京华瑞健生科技有限公司（简称“华瑞健生”）是天使轮融资者，投资时间是2017年4月，后在2018年6月退出": {"topic": "“生产投资”", "similarity": 0.4479614198207855}, "这笔钱让李航文买下了沈海法在美国研发出的新型脂质体纳米材料（lipopolyplex，LPP）递送系统的专利归属权，余下的钱花在了团队搭建和购买设备上": {"topic": "“生产投资”", "similarity": 0.44149839878082275}}</t>
+          <t>{"这样的变动也是这起案件的导火索": {"topic": "“金融”", "similarity": 0.425329327583313, "prompt": "新闻文本是“这样的变动也是这起案件的导火索”，包含的情绪词典是：改变/变化(vary):0.0,改变/变更(alteration):0.0"}, "李航文一方认为，依据公司章程，该公司的董事会设有7个席位，董事会之际，应有7名董事的过半人数出席，也就是4人及以上，而若是一项决议想要获得通过，也应有7名董事的过半人数通过": {"topic": "“金融”", "similarity": 0.4843122363090515, "prompt": "新闻文本是“李航文一方认为，依据公司章程，该公司的董事会设有7个席位，董事会之际，应有7名董事的过半人数出席，也就是4人及以上，而若是一项决议想要获得通过，也应有7名董事的过半人数通过”，包含的情绪词典是：公司的/企业的(corporate):0.0,几个/数个(several):0.0"}, "不过，在今年5月7日的那场董事会上，在职的董事人数已仅有5名，当天会议有4人出席，并有3票支持决议通过，由此，这场董事会的出席人数虽然达到了4人及以上的标准，但通过人数没有达到": {"topic": "“金融”", "similarity": 0.444347083568573, "prompt": "新闻文本是“不过，在今年5月7日的那场董事会上，在职的董事人数已仅有5名，当天会议有4人出席，并有3票支持决议通过，由此，这场董事会的出席人数虽然达到了4人及以上的标准，但通过人数没有达到”，包含的情绪词典是：出席人数/产量(turnout):0.0,失败/未通过(fails):-0.8"}, "据企业官网，唐定国也是斯微生物的联合创始人": {"topic": "“生产投资”", "similarity": 0.47277188301086426, "prompt": "新闻文本是“据企业官网，唐定国也是斯微生物的联合创始人”，包含的情绪词典是：公司/企业(firm):0.0,公司的/企业的(corporate):0.0"}, "在去年9月15日，据行业媒体医药魔方Invest等多家媒体报道，斯微生物及公司法定代表人李航文被限制高消费": {"topic": "“消费”", "similarity": 0.4784824252128601, "prompt": "新闻文本是“在去年9月15日，据行业媒体医药魔方Invest等多家媒体报道，斯微生物及公司法定代表人李航文被限制高消费”，包含的情绪词典是：限制/限定(limit):-0.1,限制/局限(confine):-0.3"}, "另外，据行业媒体深蓝观今年5月20日报道，斯微生物宣布的债务就有3.5亿元，截至今年3月，该公司已出现现金流断裂数月、员工纷纷离职、供应商诉讼追讨欠款等问题，在2月里，公司还讨论过重组方案": {"topic": "“生产投资”", "similarity": 0.49985626339912415, "prompt": "新闻文本是“另外，据行业媒体深蓝观今年5月20日报道，斯微生物宣布的债务就有3.5亿元，截至今年3月，该公司已出现现金流断裂数月、员工纷纷离职、供应商诉讼追讨欠款等问题，在2月里，公司还讨论过重组方案”，包含的情绪词典是：负债的/欠债的(indebted):-0.5,表现不佳/业绩低于预期(underperformed):-0.4"}, "高光时刻 　　在新冠疫情早期，这一史无前例的全球性公共卫生危机、却也是产业的风口下，海内外知名药企和科研团队的研发攻关战也在2020年初就拉开了序幕": {"topic": "“生产投资”", "similarity": 0.5955730676651001, "prompt": "新闻文本是“高光时刻 　　在新冠疫情早期，这一史无前例的全球性公共卫生危机、却也是产业的风口下，海内外知名药企和科研团队的研发攻关战也在2020年初就拉开了序幕”，包含的情绪词典是：高的/高等的(high):0.7,最高的/最高级的(highest):0.7"}, "这一进度也提示了，mRNA疫苗合成工艺简单、生产速度快，从基因测序至生产只需数周时间，有望在对时间要求比较紧急的疫情中有望发挥重要作用": {"topic": "“生产投资”", "similarity": 0.5202807188034058, "prompt": "新闻文本是“这一进度也提示了，mRNA疫苗合成工艺简单、生产速度快，从基因测序至生产只需数周时间，有望在对时间要求比较紧急的疫情中有望发挥重要作用”，包含的情绪词典是：技术的/工艺的(technical):0.0,过程/进程(process):0.0"}, "同时，在以全球人口基数作为潜在需求对象的巨大市场想象中，商业价值不容小觑": {"topic": "“宏观经济”", "similarity": 0.42607736587524414, "prompt": "新闻文本是“同时，在以全球人口基数作为潜在需求对象的巨大市场想象中，商业价值不容小觑”，包含的情绪词典是：潜在的/潜力(potential):0.3,可想象的/可设想的(conceivable):0.0"}, "此后，稿件引发关注": {"topic": "“金融”", "similarity": 0.44584327936172485, "prompt": "新闻文本是“此后，稿件引发关注”，包含的情绪词典是：此后/以后(thereafter):0.0,此后/今后(hereafter):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -4087,12 +4055,12 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "据央视新闻2日报道，当地时间9月1日，在德国中部的图林根州和东部的萨克森州举行的州议会选举中，德国选择党和基民盟分别成为两州议会第一大党", "news_prompt2": "目前，在联邦政府中联合执政的社民党、绿党和自民党得票大幅减少，得票率均不足10%", "news_prompt3": "初步结果显示，德国选择党以32.8%的得票率成为图林根州议会第一大党，这是德国选择党成立11年来首次在州议会选举中获胜，也是德国二战以后首次有极右翼党派在州议会选举中获胜", "news_prompt4": "在萨克森州，基民盟以31.9%的得票率超过得票率为30.6%的选择党，维持该州议会第一大党地位", "news_prompt5": "图片来源：视频截图  　　德国各党派将于9月2日对两州的议会选举结果进行讨论", "news_prompt6": "尽管选择党已获得了较高的支持率，但由于目前其他党派都已明确表示不会与德国选择党合作组建联合政府，最终选择党在这两个州上台执政仍然面临比较大的困难", "news_prompt7": "两德统一以来，东部各州社会发展、基础设施建设和就业率等方面都和西部州有很大的差距，东部州的选民立场因此趋于保守和民粹化", "news_prompt8": "俄乌冲突爆发后，德国面临通胀高企和能源价格攀升等问题，经济发展迟缓，而联邦政府不断加大对乌克兰的支持力度，也令民众失去耐心，执政联盟的支持率不断下降", "news_prompt9": "选择党对外主张严格限制外来移民，停止对乌克兰支持，减少承担欧盟的义务，因此在东部州更受欢迎", "news_prompt10": "此外，在两州议会选举过程中，从左翼党分裂出的“莎拉·瓦根克内希特联盟”以限制移民、中止对乌军事支持和谈判解决俄乌冲突的态度，均获得了超过10%的支持率，成为两州州议会的第三大党", "news_prompt11": "据证券时报报道，此次选举结果必然会给朔尔茨带来更大压力，迫使他采取更加强硬的移民政策，并加剧有关支持乌克兰问题的辩论，因为这些问题已成为竞选活动中的主导问题", "news_prompt12": "图片来源：视频截图  　　许多人认为，图林根州和萨克森州的地方选举结果是明年大选前对朔尔茨及其联盟伙伴的试金石", "news_prompt13": "尽管德国选择党将移民问题放在了议程的首位，但朔尔茨组建的联盟摇摇欲坠，内斗不断，政策分歧不断，民选官员被指责不再代表他们当选时的价值观", "news_prompt14": "德国选择党联合主席艾丽丝·韦塞尔称图林根州的选举结果是“历史性的胜利”，反映出民众对朔尔茨联合政府的拒绝", "news_prompt15": "那么，德国地区选举的结果如何影响格局", "news_prompt16": "分析人士认为，首先，在欧盟另一个大国法国于六月和七月提前选举后仍在努力组建政府的情况下，德国政府权威的动摇可能使欧洲政策复杂化", "news_prompt17": "其次，选举结果反映出，随着各国政府努力应对乌克兰战争和通货膨胀等危机，欧洲政治格局日益分裂，反建制政党不断崛起", "news_prompt18": "第三，反北约、反移民和亲俄政党（比如左翼政党）的崛起，将使得在州和联邦层面形成意识形态一致的联盟变得更加困难", "news_prompt19": "事实上，自2021年执政以来，联盟伙伴在选举前就已存在分歧，去年年底围绕今年和明年的预算爆发了紧张局势", "news_prompt20": "研究机构Teneo的Carsten Nickel在一份研究报告中表示：“由于2025年预算法案仍存在约120亿欧元（132.5亿美元）的缺口，联盟紧张局势可能再次出现", "news_prompt21": "”然而，杜塞尔多夫大学政治学家斯蒂芬·马沙尔表示，朔尔茨的执政联盟不太可能完全解散，因为这不符合三个政党的利益", "news_prompt22": "但由于支持率的下降，可能会导致主流政党在移民问题上采取强硬立场，并可能削弱对乌克兰的支持", "news_prompt23": "伦敦国王学院的亚历山大·克拉克森表示，问题将变得更加棘手，德国可能陷入更加无力的境地，这意味着波兰、法国和意大利等国家将需要带头", "news_prompt24": "另一方面，德国的执政联盟建设也将变得极为复杂", "news_prompt25": "德国选择党的分支机构被德国情报机构列为疑似极右翼分子，该党在图林根州的头号候选人比约恩·霍克(Bjrn Hcke)曾因使用纳粹口号被罚款两次", "news_prompt26": "鉴于此，作为胜利者的他们可能也很难组建地区政府，更难以在议会形成多数席位，因为他们很难在其他政党中寻找盟友", "news_prompt27": "因此将由排在第二位的保守党来争夺多数席位", "news_prompt28": "但在图林根州，尽管存在重大意识形态差异，但如果没有德国社会党的支持，保守党也将无法形成多数席位", "news_prompt29": "由于上述预期，选民可能会在随后的选举中投票给更多反建制政党，以此惩罚主流政党不连贯的联盟", "news_prompt30": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "两德统一以来，东部各州社会发展、基础设施建设和就业率等方面都和西部州有很大的差距，东部州的选民立场因此趋于保守和民粹化", "news_prompt2": "俄乌冲突爆发后，德国面临通胀高企和能源价格攀升等问题，经济发展迟缓，而联邦政府不断加大对乌克兰的支持力度，也令民众失去耐心，执政联盟的支持率不断下降", "news_prompt3": "其次，选举结果反映出，随着各国政府努力应对乌克兰战争和通货膨胀等危机，欧洲政治格局日益分裂，反建制政党不断崛起", "news_prompt4": "研究机构Teneo的Carsten Nickel在一份研究报告中表示：“由于2025年预算法案仍存在约120亿欧元（132.5亿美元）的缺口，联盟紧张局势可能再次出现"}</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>{"两德统一以来，东部各州社会发展、基础设施建设和就业率等方面都和西部州有很大的差距，东部州的选民立场因此趋于保守和民粹化": {"topic": "“宏观经济”", "similarity": 0.4562174081802368, "prompt": "新闻文本是“两德统一以来，东部各州社会发展、基础设施建设和就业率等方面都和西部州有很大的差距，东部州的选民立场因此趋于保守和民粹化”，包含的情绪词典是：不同/相异(differing):0.0,东方/东部(east):0.0"}, "俄乌冲突爆发后，德国面临通胀高企和能源价格攀升等问题，经济发展迟缓，而联邦政府不断加大对乌克兰的支持力度，也令民众失去耐心，执政联盟的支持率不断下降": {"topic": "“宏观经济”", "similarity": 0.49890822172164917, "prompt": "新闻文本是“俄乌冲突爆发后，德国面临通胀高企和能源价格攀升等问题，经济发展迟缓，而联邦政府不断加大对乌克兰的支持力度，也令民众失去耐心，执政联盟的支持率不断下降”，包含的情绪词典是：通货紧缩(deflation):-0.6,欧盟/欧洲联盟(eu):0.0"}, "其次，选举结果反映出，随着各国政府努力应对乌克兰战争和通货膨胀等危机，欧洲政治格局日益分裂，反建制政党不断崛起": {"topic": "“宏观经济”", "similarity": 0.4336211383342743, "prompt": "新闻文本是“其次，选举结果反映出，随着各国政府努力应对乌克兰战争和通货膨胀等危机，欧洲政治格局日益分裂，反建制政党不断崛起”，包含的情绪词典是：选举/推选(election):0.0,反对/对立(opposition):-0.2"}, "研究机构Teneo的Carsten Nickel在一份研究报告中表示：“由于2025年预算法案仍存在约120亿欧元（132.5亿美元）的缺口，联盟紧张局势可能再次出现": {"topic": "“宏观经济”", "similarity": 0.4635116755962372, "prompt": "新闻文本是“研究机构Teneo的Carsten Nickel在一份研究报告中表示：“由于2025年预算法案仍存在约120亿欧元（132.5亿美元）的缺口，联盟紧张局势可能再次出现”，包含的情绪词典是：资金不足的(underfunded):-0.3,资本不足的(undercapitalized):-0.4"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"两德统一以来，东部各州社会发展、基础设施建设和就业率等方面都和西部州有很大的差距，东部州的选民立场因此趋于保守和民粹化": {"topic": "“宏观经济”", "similarity": 0.4562177062034607, "prompt": "新闻文本是“两德统一以来，东部各州社会发展、基础设施建设和就业率等方面都和西部州有很大的差距，东部州的选民立场因此趋于保守和民粹化”，包含的情绪词典是：不同/相异(differing):0.0,东方/东部(east):0.0"}, "俄乌冲突爆发后，德国面临通胀高企和能源价格攀升等问题，经济发展迟缓，而联邦政府不断加大对乌克兰的支持力度，也令民众失去耐心，执政联盟的支持率不断下降": {"topic": "“宏观经济”", "similarity": 0.4989085793495178, "prompt": "新闻文本是“俄乌冲突爆发后，德国面临通胀高企和能源价格攀升等问题，经济发展迟缓，而联邦政府不断加大对乌克兰的支持力度，也令民众失去耐心，执政联盟的支持率不断下降”，包含的情绪词典是：通货紧缩(deflation):-0.6,欧盟/欧洲联盟(eu):0.0"}, "其次，选举结果反映出，随着各国政府努力应对乌克兰战争和通货膨胀等危机，欧洲政治格局日益分裂，反建制政党不断崛起": {"topic": "“宏观经济”", "similarity": 0.4336214065551758, "prompt": "新闻文本是“其次，选举结果反映出，随着各国政府努力应对乌克兰战争和通货膨胀等危机，欧洲政治格局日益分裂，反建制政党不断崛起”，包含的情绪词典是：选举/推选(election):0.0,反对/对立(opposition):-0.2"}, "研究机构Teneo的Carsten Nickel在一份研究报告中表示：“由于2025年预算法案仍存在约120亿欧元（132.5亿美元）的缺口，联盟紧张局势可能再次出现": {"topic": "“宏观经济”", "similarity": 0.46351200342178345, "prompt": "新闻文本是“研究机构Teneo的Carsten Nickel在一份研究报告中表示：“由于2025年预算法案仍存在约120亿欧元（132.5亿美元）的缺口，联盟紧张局势可能再次出现”，包含的情绪词典是：资金不足的(underfunded):-0.3,资本不足的(undercapitalized):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -4138,12 +4106,12 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "中银证券09月02日发布研报称，给予天目湖（603136.SH，最新价：9.94元）买入评级", "news_prompt2": "评级理由主要包括：1）Q2业绩略有下滑", "news_prompt3": "2）费用率略有上升，Q2毛利率、净利率同比基本持平", "news_prompt4": "3）各业务表现分化，酒店业务相对承压", "news_prompt5": "4）项目建设稳步推进，中长期增长空间可期", "news_prompt6": "5）社会服务：旅游及景区", "news_prompt7": "风险提示：安全性风险、项目推进不及预期风险、行业竞争风险", "news_prompt8": "AI点评：天目湖近一个月获得3份券商研报关注，买入1家，增持1家", "news_prompt9": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "评级理由主要包括：1）Q2业绩略有下滑", "news_prompt2": "2）费用率略有上升，Q2毛利率、净利率同比基本持平", "news_prompt3": "3）各业务表现分化，酒店业务相对承压", "news_prompt4": "4）项目建设稳步推进，中长期增长空间可期", "news_prompt5": "5）社会服务：旅游及景区", "news_prompt6": "AI点评：天目湖近一个月获得3份券商研报关注，买入1家，增持1家"}</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>{"中银证券09月02日发布研报称，给予天目湖（603136.SH，最新价：9.94元）买入评级": {"topic": "“金融”", "similarity": 0.49020931124687195}, "评级理由主要包括：1）Q2业绩略有下滑": {"topic": "“金融”", "similarity": 0.4228411912918091, "prompt": "新闻文本是“评级理由主要包括：1）Q2业绩略有下滑”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "2）费用率略有上升，Q2毛利率、净利率同比基本持平": {"topic": "“消费”", "similarity": 0.45761412382125854, "prompt": "新闻文本是“2）费用率略有上升，Q2毛利率、净利率同比基本持平”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "3）各业务表现分化，酒店业务相对承压": {"topic": "“消费”", "similarity": 0.5115610957145691, "prompt": "新闻文本是“3）各业务表现分化，酒店业务相对承压”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,服务/业务(service):0.0"}, "4）项目建设稳步推进，中长期增长空间可期": {"topic": "“生产投资”", "similarity": 0.5731460452079773, "prompt": "新闻文本是“4）项目建设稳步推进，中长期增长空间可期”，包含的情绪词典是：增长/发展(growth):0.7,进步/进展(progresses):0.6"}, "5）社会服务：旅游及景区": {"topic": "“消费”", "similarity": 0.5000007152557373, "prompt": "新闻文本是“5）社会服务：旅游及景区”，包含的情绪词典是：服务/服役(serve):0.0,享受/喜爱(enjoyment):0.5"}, "风险提示：安全性风险、项目推进不及预期风险、行业竞争风险": {"topic": "“金融”", "similarity": 0.5303966999053955, "prompt": "新闻文本是“风险提示：安全性风险、项目推进不及预期风险、行业竞争风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "AI点评：天目湖近一个月获得3份券商研报关注，买入1家，增持1家": {"topic": "“金融”", "similarity": 0.5321847796440125, "prompt": "新闻文本是“AI点评：天目湖近一个月获得3份券商研报关注，买入1家，增持1家”，包含的情绪词典是：投机性的/推测性的(speculative):-0.2,投资者/投资人(investor):0.4"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"评级理由主要包括：1）Q2业绩略有下滑": {"topic": "“金融”", "similarity": 0.42284131050109863, "prompt": "新闻文本是“评级理由主要包括：1）Q2业绩略有下滑”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "2）费用率略有上升，Q2毛利率、净利率同比基本持平": {"topic": "“消费”", "similarity": 0.4576142728328705, "prompt": "新闻文本是“2）费用率略有上升，Q2毛利率、净利率同比基本持平”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "3）各业务表现分化，酒店业务相对承压": {"topic": "“消费”", "similarity": 0.5115610957145691, "prompt": "新闻文本是“3）各业务表现分化，酒店业务相对承压”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,服务/业务(service):0.0"}, "4）项目建设稳步推进，中长期增长空间可期": {"topic": "“生产投资”", "similarity": 0.5731459856033325, "prompt": "新闻文本是“4）项目建设稳步推进，中长期增长空间可期”，包含的情绪词典是：增长/发展(growth):0.7,进步/进展(progresses):0.6"}, "5）社会服务：旅游及景区": {"topic": "“消费”", "similarity": 0.5000008344650269, "prompt": "新闻文本是“5）社会服务：旅游及景区”，包含的情绪词典是：服务/服役(serve):0.0,享受/喜爱(enjoyment):0.5"}, "AI点评：天目湖近一个月获得3份券商研报关注，买入1家，增持1家": {"topic": "“金融”", "similarity": 0.532184898853302, "prompt": "新闻文本是“AI点评：天目湖近一个月获得3份券商研报关注，买入1家，增持1家”，包含的情绪词典是：投机性的/推测性的(speculative):-0.2,投资者/投资人(investor):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -4189,12 +4157,12 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "国产首艘大型邮轮“爱达·魔都号”已成功运营50余个航次，服务超过22万国内外游客", "news_prompt2": "自主研发的30.8万吨超大型油船打破国外技术垄断", "news_prompt3": "全球最大功率双燃料低速发动机助力船舶动力绿色革命……　　日前，中国船舶集团2024年国企开放日活动举办，记者走进中国船舶集团旗下多家科研院所、企业，近距离感受中国造船工业的发展脉动", "news_prompt4": "登上“爱达·魔都号”，船上空间宽敞明亮，住宿、餐饮、休闲设施一应俱全，可容纳乘客5246人，宛如一座“海上城市”", "news_prompt5": "大型邮轮设计建造难度极大，曾长期被少数几家欧洲船厂垄断", "news_prompt6": "“爱达·魔都号”的成功建造，使我国集齐了造船工业“皇冠上的三颗明珠”，也是我国造船工业持续向高端迈进的一个缩影", "news_prompt7": "中国船舶工业行业协会数据显示，2023年，我国船企交付了20艘24000箱超大集装箱船，4艘17.4万立方米大型LNG运输船等高端船型，一批新型深远海大型风电安装船、深远海养殖装备等高端海洋工程装备顺利交付", "news_prompt8": "在中国船舶集团第七〇八研究所，记者了解到，该所正加快开展关键核心技术攻关，自主研发设计了一批高端化、智能化船型：两个月前交付的新一代破冰调查船“极地”号，搭载无人机、无人船、水下机器人等一系列最新装备，可开展大量无人化作业", "news_prompt9": "建造中的3万方级巨型耙吸挖泥船，建成后将是亚洲最大耙吸挖泥船，有力提升我国疏浚装备研发设计和建造水平……　　绿色低碳是船舶工业发展的必然趋势", "news_prompt10": "记者在走访过程中切身感受到，我国船舶工业正积极“拥抱”绿色化，从船用发动机到减排设备，一系列绿色技术被攻克，助力船舶工业加速绿色转型", "news_prompt11": "发动机是船舶的“心脏”，动力系统的绿色化是船舶工业绿色转型的关键", "news_prompt12": "在中船动力集团下属中船三井的生产车间里，我国研制的全球首台最大功率带智能控制废气再循环系统双燃料发动机12X92DF-2.0正在试车，这个庞然大物占地面积相当于一个标准篮球场，可产生相当于700辆小轿车同时输出的动力", "news_prompt13": "12X92DF系列发动机采用液化天然气和燃油为燃料，相对于常规重油模式发动机，燃气模式下可实现硫化物减排99%以上，二氧化碳减排20%以上，氮氧化物减排80%以上", "news_prompt14": "“公司持续推进液化天然气、甲醇、氨等零碳低碳燃料发动机关键技术研究及产业化，低碳零碳发动机在公司产品中的占比持续提升", "news_prompt15": "”中船动力集团董事长李琤说", "news_prompt16": "船上捕集、液化存储、卸岸转运、再利用，中国船舶集团第七一一研究所自主研制的全流程船舶碳捕集系统，对船舶排放二氧化碳的捕集率可达80%以上，并能高效转化为液态二氧化碳带回岸上进行再利用，液态二氧化碳纯度可达99.5%以上", "news_prompt17": "记者获悉，今年4月，配备该系统的14000箱大型集装箱船在上海洋山港靠岸，成功完成液态二氧化碳卸岸工作，并正式交付给使用方，标志着该系统成功实现实船装配应用", "news_prompt18": "“不断加强自主研发和技术创新，是造船工业高质量发展的必然要求", "news_prompt19": "”中国船舶集团第七一一研究所所长董建福说，未来将面向国家重大需求，持续加强自主研发，力争攻克更多关键核心技术，为推动我国向造船强国迈进贡献力量", "news_prompt20": "新华社北京8月31日电（文章来源：新华社）"}</t>
+          <t>{"news_prompt1": "国产首艘大型邮轮“爱达·魔都号”已成功运营50余个航次，服务超过22万国内外游客", "news_prompt2": "自主研发的30.8万吨超大型油船打破国外技术垄断", "news_prompt3": "全球最大功率双燃料低速发动机助力船舶动力绿色革命……　　日前，中国船舶集团2024年国企开放日活动举办，记者走进中国船舶集团旗下多家科研院所、企业，近距离感受中国造船工业的发展脉动", "news_prompt4": "登上“爱达·魔都号”，船上空间宽敞明亮，住宿、餐饮、休闲设施一应俱全，可容纳乘客5246人，宛如一座“海上城市”", "news_prompt5": "“爱达·魔都号”的成功建造，使我国集齐了造船工业“皇冠上的三颗明珠”，也是我国造船工业持续向高端迈进的一个缩影", "news_prompt6": "中国船舶工业行业协会数据显示，2023年，我国船企交付了20艘24000箱超大集装箱船，4艘17.4万立方米大型LNG运输船等高端船型，一批新型深远海大型风电安装船、深远海养殖装备等高端海洋工程装备顺利交付", "news_prompt7": "在中国船舶集团第七〇八研究所，记者了解到，该所正加快开展关键核心技术攻关，自主研发设计了一批高端化、智能化船型：两个月前交付的新一代破冰调查船“极地”号，搭载无人机、无人船、水下机器人等一系列最新装备，可开展大量无人化作业", "news_prompt8": "建造中的3万方级巨型耙吸挖泥船，建成后将是亚洲最大耙吸挖泥船，有力提升我国疏浚装备研发设计和建造水平……　　绿色低碳是船舶工业发展的必然趋势", "news_prompt9": "记者在走访过程中切身感受到，我国船舶工业正积极“拥抱”绿色化，从船用发动机到减排设备，一系列绿色技术被攻克，助力船舶工业加速绿色转型", "news_prompt10": "发动机是船舶的“心脏”，动力系统的绿色化是船舶工业绿色转型的关键", "news_prompt11": "在中船动力集团下属中船三井的生产车间里，我国研制的全球首台最大功率带智能控制废气再循环系统双燃料发动机12X92DF-2.0正在试车，这个庞然大物占地面积相当于一个标准篮球场，可产生相当于700辆小轿车同时输出的动力", "news_prompt12": "12X92DF系列发动机采用液化天然气和燃油为燃料，相对于常规重油模式发动机，燃气模式下可实现硫化物减排99%以上，二氧化碳减排20%以上，氮氧化物减排80%以上", "news_prompt13": "“公司持续推进液化天然气、甲醇、氨等零碳低碳燃料发动机关键技术研究及产业化，低碳零碳发动机在公司产品中的占比持续提升", "news_prompt14": "”中船动力集团董事长李琤说", "news_prompt15": "“不断加强自主研发和技术创新，是造船工业高质量发展的必然要求", "news_prompt16": "”中国船舶集团第七一一研究所所长董建福说，未来将面向国家重大需求，持续加强自主研发，力争攻克更多关键核心技术，为推动我国向造船强国迈进贡献力量"}</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>{"国产首艘大型邮轮“爱达·魔都号”已成功运营50余个航次，服务超过22万国内外游客": {"topic": "“生产投资”", "similarity": 0.46597421169281006, "prompt": "新闻文本是“国产首艘大型邮轮“爱达·魔都号”已成功运营50余个航次，服务超过22万国内外游客”，包含的情绪词典是：达到/实现(achieve):0.6,海外的/国外的(overseas):0.0"}, "自主研发的30.8万吨超大型油船打破国外技术垄断": {"topic": "“生产投资”", "similarity": 0.4321322441101074, "prompt": "新闻文本是“自主研发的30.8万吨超大型油船打破国外技术垄断”，包含的情绪词典是：公吨(tonne):0.0,石油/油类(oil):0.0"}, "全球最大功率双燃料低速发动机助力船舶动力绿色革命……　　日前，中国船舶集团2024年国企开放日活动举办，记者走进中国船舶集团旗下多家科研院所、企业，近距离感受中国造船工业的发展脉动": {"topic": "“生产投资”", "similarity": 0.5690320134162903, "prompt": "新闻文本是“全球最大功率双燃料低速发动机助力船舶动力绿色革命……　　日前，中国船舶集团2024年国企开放日活动举办，记者走进中国船舶集团旗下多家科研院所、企业，近距离感受中国造船工业的发展脉动”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "登上“爱达·魔都号”，船上空间宽敞明亮，住宿、餐饮、休闲设施一应俱全，可容纳乘客5246人，宛如一座“海上城市”": {"topic": "“消费”", "similarity": 0.4691193401813507, "prompt": "新闻文本是“登上“爱达·魔都号”，船上空间宽敞明亮，住宿、餐饮、休闲设施一应俱全，可容纳乘客5246人，宛如一座“海上城市””，包含的情绪词典是：相当大的/可观的(sizeable):0.0,相当大的/可观的(considerable):0.3"}, "“爱达·魔都号”的成功建造，使我国集齐了造船工业“皇冠上的三颗明珠”，也是我国造船工业持续向高端迈进的一个缩影": {"topic": "“生产投资”", "similarity": 0.5277248024940491, "prompt": "新闻文本是““爱达·魔都号”的成功建造，使我国集齐了造船工业“皇冠上的三颗明珠”，也是我国造船工业持续向高端迈进的一个缩影”，包含的情绪词典是：成功的/圆满的(successful):0.9,工业的/产业的(industrial):0.0"}, "中国船舶工业行业协会数据显示，2023年，我国船企交付了20艘24000箱超大集装箱船，4艘17.4万立方米大型LNG运输船等高端船型，一批新型深远海大型风电安装船、深远海养殖装备等高端海洋工程装备顺利交付": {"topic": "“生产投资”", "similarity": 0.6020731925964355, "prompt": "新闻文本是“中国船舶工业行业协会数据显示，2023年，我国船企交付了20艘24000箱超大集装箱船，4艘17.4万立方米大型LNG运输船等高端船型，一批新型深远海大型风电安装船、深远海养殖装备等高端海洋工程装备顺利交付”，包含的情绪词典是：相当大的/可观的(sizeable):0.0,相当大的/可观的(considerable):0.3"}, "在中国船舶集团第七〇八研究所，记者了解到，该所正加快开展关键核心技术攻关，自主研发设计了一批高端化、智能化船型：两个月前交付的新一代破冰调查船“极地”号，搭载无人机、无人船、水下机器人等一系列最新装备，可开展大量无人化作业": {"topic": "“生产投资”", "similarity": 0.5796487331390381, "prompt": "新闻文本是“在中国船舶集团第七〇八研究所，记者了解到，该所正加快开展关键核心技术攻关，自主研发设计了一批高端化、智能化船型：两个月前交付的新一代破冰调查船“极地”号，搭载无人机、无人船、水下机器人等一系列最新装备，可开展大量无人化作业”，包含的情绪词典是：有发明才能的/有创造力的(inventive):0.5"}, "建造中的3万方级巨型耙吸挖泥船，建成后将是亚洲最大耙吸挖泥船，有力提升我国疏浚装备研发设计和建造水平……　　绿色低碳是船舶工业发展的必然趋势": {"topic": "“生产投资”", "similarity": 0.5503918528556824, "prompt": "新闻文本是“建造中的3万方级巨型耙吸挖泥船，建成后将是亚洲最大耙吸挖泥船，有力提升我国疏浚装备研发设计和建造水平……　　绿色低碳是船舶工业发展的必然趋势”，包含的情绪词典是：巨大的/惊人的(tremendous):0.7,相当大的/可观的(sizeable):0.0"}, "记者在走访过程中切身感受到，我国船舶工业正积极“拥抱”绿色化，从船用发动机到减排设备，一系列绿色技术被攻克，助力船舶工业加速绿色转型": {"topic": "“生产投资”", "similarity": 0.5293253660202026, "prompt": "新闻文本是“记者在走访过程中切身感受到，我国船舶工业正积极“拥抱”绿色化，从船用发动机到减排设备，一系列绿色技术被攻克，助力船舶工业加速绿色转型”，包含的情绪词典是：技术(tech):0.0,发动机/引擎(engine):0.0"}, "发动机是船舶的“心脏”，动力系统的绿色化是船舶工业绿色转型的关键": {"topic": "“生产投资”", "similarity": 0.4936908185482025, "prompt": "新闻文本是“发动机是船舶的“心脏”，动力系统的绿色化是船舶工业绿色转型的关键”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "在中船动力集团下属中船三井的生产车间里，我国研制的全球首台最大功率带智能控制废气再循环系统双燃料发动机12X92DF-2.0正在试车，这个庞然大物占地面积相当于一个标准篮球场，可产生相当于700辆小轿车同时输出的动力": {"topic": "“生产投资”", "similarity": 0.5461865067481995, "prompt": "新闻文本是“在中船动力集团下属中船三井的生产车间里，我国研制的全球首台最大功率带智能控制废气再循环系统双燃料发动机12X92DF-2.0正在试车，这个庞然大物占地面积相当于一个标准篮球场，可产生相当于700辆小轿车同时输出的动力”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "12X92DF系列发动机采用液化天然气和燃油为燃料，相对于常规重油模式发动机，燃气模式下可实现硫化物减排99%以上，二氧化碳减排20%以上，氮氧化物减排80%以上": {"topic": "“生产投资”", "similarity": 0.5213874578475952, "prompt": "新闻文本是“12X92DF系列发动机采用液化天然气和燃油为燃料，相对于常规重油模式发动机，燃气模式下可实现硫化物减排99%以上，二氧化碳减排20%以上，氮氧化物减排80%以上”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "“公司持续推进液化天然气、甲醇、氨等零碳低碳燃料发动机关键技术研究及产业化，低碳零碳发动机在公司产品中的占比持续提升": {"topic": "“生产投资”", "similarity": 0.5888060927391052, "prompt": "新闻文本是““公司持续推进液化天然气、甲醇、氨等零碳低碳燃料发动机关键技术研究及产业化，低碳零碳发动机在公司产品中的占比持续提升”，包含的情绪词典是：进步/提升(advancement):0.5,发动机/引擎(engine):0.0"}, "”中船动力集团董事长李琤说": {"topic": "“生产投资”", "similarity": 0.501444935798645, "prompt": "新闻文本是“”中船动力集团董事长李琤说”，包含的情绪词典是：企业/事业(enterprise):0.0,领导能力/领导力(leadership):0.7"}, "船上捕集、液化存储、卸岸转运、再利用，中国船舶集团第七一一研究所自主研制的全流程船舶碳捕集系统，对船舶排放二氧化碳的捕集率可达80%以上，并能高效转化为液态二氧化碳带回岸上进行再利用，液态二氧化碳纯度可达99.5%以上": {"topic": "“生产投资”", "similarity": 0.5595358610153198}, "记者获悉，今年4月，配备该系统的14000箱大型集装箱船在上海洋山港靠岸，成功完成液态二氧化碳卸岸工作，并正式交付给使用方，标志着该系统成功实现实船装配应用": {"topic": "“生产投资”", "similarity": 0.4994979500770569}, "“不断加强自主研发和技术创新，是造船工业高质量发展的必然要求": {"topic": "“生产投资”", "similarity": 0.47222965955734253, "prompt": "新闻文本是““不断加强自主研发和技术创新，是造船工业高质量发展的必然要求”，包含的情绪词典是：技术的/工艺的(technical):0.0,创新/革新(innovation):0.7"}, "”中国船舶集团第七一一研究所所长董建福说，未来将面向国家重大需求，持续加强自主研发，力争攻克更多关键核心技术，为推动我国向造船强国迈进贡献力量": {"topic": "“生产投资”", "similarity": 0.5710628032684326, "prompt": "新闻文本是“”中国船舶集团第七一一研究所所长董建福说，未来将面向国家重大需求，持续加强自主研发，力争攻克更多关键核心技术，为推动我国向造船强国迈进贡献力量”，包含的情绪词典是：突破/重大进展(breakthrough):0.5,正在改善的/正在改进的(improving):0.5"}}</t>
+          <t>{"国产首艘大型邮轮“爱达·魔都号”已成功运营50余个航次，服务超过22万国内外游客": {"topic": "“生产投资”", "similarity": 0.46597424149513245, "prompt": "新闻文本是“国产首艘大型邮轮“爱达·魔都号”已成功运营50余个航次，服务超过22万国内外游客”，包含的情绪词典是：达到/实现(achieve):0.6,海外的/国外的(overseas):0.0"}, "自主研发的30.8万吨超大型油船打破国外技术垄断": {"topic": "“生产投资”", "similarity": 0.43213218450546265, "prompt": "新闻文本是“自主研发的30.8万吨超大型油船打破国外技术垄断”，包含的情绪词典是：公吨(tonne):0.0,石油/油类(oil):0.0"}, "全球最大功率双燃料低速发动机助力船舶动力绿色革命……　　日前，中国船舶集团2024年国企开放日活动举办，记者走进中国船舶集团旗下多家科研院所、企业，近距离感受中国造船工业的发展脉动": {"topic": "“生产投资”", "similarity": 0.5690320134162903, "prompt": "新闻文本是“全球最大功率双燃料低速发动机助力船舶动力绿色革命……　　日前，中国船舶集团2024年国企开放日活动举办，记者走进中国船舶集团旗下多家科研院所、企业，近距离感受中国造船工业的发展脉动”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "登上“爱达·魔都号”，船上空间宽敞明亮，住宿、餐饮、休闲设施一应俱全，可容纳乘客5246人，宛如一座“海上城市”": {"topic": "“消费”", "similarity": 0.4691193103790283, "prompt": "新闻文本是“登上“爱达·魔都号”，船上空间宽敞明亮，住宿、餐饮、休闲设施一应俱全，可容纳乘客5246人，宛如一座“海上城市””，包含的情绪词典是：相当大的/可观的(sizeable):0.0,相当大的/可观的(considerable):0.3"}, "“爱达·魔都号”的成功建造，使我国集齐了造船工业“皇冠上的三颗明珠”，也是我国造船工业持续向高端迈进的一个缩影": {"topic": "“生产投资”", "similarity": 0.5277249217033386, "prompt": "新闻文本是““爱达·魔都号”的成功建造，使我国集齐了造船工业“皇冠上的三颗明珠”，也是我国造船工业持续向高端迈进的一个缩影”，包含的情绪词典是：成功的/圆满的(successful):0.9,工业的/产业的(industrial):0.0"}, "中国船舶工业行业协会数据显示，2023年，我国船企交付了20艘24000箱超大集装箱船，4艘17.4万立方米大型LNG运输船等高端船型，一批新型深远海大型风电安装船、深远海养殖装备等高端海洋工程装备顺利交付": {"topic": "“生产投资”", "similarity": 0.6020731925964355, "prompt": "新闻文本是“中国船舶工业行业协会数据显示，2023年，我国船企交付了20艘24000箱超大集装箱船，4艘17.4万立方米大型LNG运输船等高端船型，一批新型深远海大型风电安装船、深远海养殖装备等高端海洋工程装备顺利交付”，包含的情绪词典是：相当大的/可观的(sizeable):0.0,相当大的/可观的(considerable):0.3"}, "在中国船舶集团第七〇八研究所，记者了解到，该所正加快开展关键核心技术攻关，自主研发设计了一批高端化、智能化船型：两个月前交付的新一代破冰调查船“极地”号，搭载无人机、无人船、水下机器人等一系列最新装备，可开展大量无人化作业": {"topic": "“生产投资”", "similarity": 0.5796487331390381, "prompt": "新闻文本是“在中国船舶集团第七〇八研究所，记者了解到，该所正加快开展关键核心技术攻关，自主研发设计了一批高端化、智能化船型：两个月前交付的新一代破冰调查船“极地”号，搭载无人机、无人船、水下机器人等一系列最新装备，可开展大量无人化作业”，包含的情绪词典是：有发明才能的/有创造力的(inventive):0.5"}, "建造中的3万方级巨型耙吸挖泥船，建成后将是亚洲最大耙吸挖泥船，有力提升我国疏浚装备研发设计和建造水平……　　绿色低碳是船舶工业发展的必然趋势": {"topic": "“生产投资”", "similarity": 0.5503917932510376, "prompt": "新闻文本是“建造中的3万方级巨型耙吸挖泥船，建成后将是亚洲最大耙吸挖泥船，有力提升我国疏浚装备研发设计和建造水平……　　绿色低碳是船舶工业发展的必然趋势”，包含的情绪词典是：巨大的/惊人的(tremendous):0.7,相当大的/可观的(sizeable):0.0"}, "记者在走访过程中切身感受到，我国船舶工业正积极“拥抱”绿色化，从船用发动机到减排设备，一系列绿色技术被攻克，助力船舶工业加速绿色转型": {"topic": "“生产投资”", "similarity": 0.5293253064155579, "prompt": "新闻文本是“记者在走访过程中切身感受到，我国船舶工业正积极“拥抱”绿色化，从船用发动机到减排设备，一系列绿色技术被攻克，助力船舶工业加速绿色转型”，包含的情绪词典是：技术(tech):0.0,发动机/引擎(engine):0.0"}, "发动机是船舶的“心脏”，动力系统的绿色化是船舶工业绿色转型的关键": {"topic": "“生产投资”", "similarity": 0.4936909079551697, "prompt": "新闻文本是“发动机是船舶的“心脏”，动力系统的绿色化是船舶工业绿色转型的关键”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "在中船动力集团下属中船三井的生产车间里，我国研制的全球首台最大功率带智能控制废气再循环系统双燃料发动机12X92DF-2.0正在试车，这个庞然大物占地面积相当于一个标准篮球场，可产生相当于700辆小轿车同时输出的动力": {"topic": "“生产投资”", "similarity": 0.5461865663528442, "prompt": "新闻文本是“在中船动力集团下属中船三井的生产车间里，我国研制的全球首台最大功率带智能控制废气再循环系统双燃料发动机12X92DF-2.0正在试车，这个庞然大物占地面积相当于一个标准篮球场，可产生相当于700辆小轿车同时输出的动力”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "12X92DF系列发动机采用液化天然气和燃油为燃料，相对于常规重油模式发动机，燃气模式下可实现硫化物减排99%以上，二氧化碳减排20%以上，氮氧化物减排80%以上": {"topic": "“生产投资”", "similarity": 0.5213874578475952, "prompt": "新闻文本是“12X92DF系列发动机采用液化天然气和燃油为燃料，相对于常规重油模式发动机，燃气模式下可实现硫化物减排99%以上，二氧化碳减排20%以上，氮氧化物减排80%以上”，包含的情绪词典是：发动机/引擎(engine):0.0,发动机/马达(motor):0.0"}, "“公司持续推进液化天然气、甲醇、氨等零碳低碳燃料发动机关键技术研究及产业化，低碳零碳发动机在公司产品中的占比持续提升": {"topic": "“生产投资”", "similarity": 0.58880615234375, "prompt": "新闻文本是““公司持续推进液化天然气、甲醇、氨等零碳低碳燃料发动机关键技术研究及产业化，低碳零碳发动机在公司产品中的占比持续提升”，包含的情绪词典是：进步/提升(advancement):0.5,发动机/引擎(engine):0.0"}, "”中船动力集团董事长李琤说": {"topic": "“生产投资”", "similarity": 0.5014448761940002, "prompt": "新闻文本是“”中船动力集团董事长李琤说”，包含的情绪词典是：企业/事业(enterprise):0.0,领导能力/领导力(leadership):0.7"}, "“不断加强自主研发和技术创新，是造船工业高质量发展的必然要求": {"topic": "“生产投资”", "similarity": 0.47222980856895447, "prompt": "新闻文本是““不断加强自主研发和技术创新，是造船工业高质量发展的必然要求”，包含的情绪词典是：技术的/工艺的(technical):0.0,创新/革新(innovation):0.7"}, "”中国船舶集团第七一一研究所所长董建福说，未来将面向国家重大需求，持续加强自主研发，力争攻克更多关键核心技术，为推动我国向造船强国迈进贡献力量": {"topic": "“生产投资”", "similarity": 0.5710629224777222, "prompt": "新闻文本是“”中国船舶集团第七一一研究所所长董建福说，未来将面向国家重大需求，持续加强自主研发，力争攻克更多关键核心技术，为推动我国向造船强国迈进贡献力量”，包含的情绪词典是：突破/重大进展(breakthrough):0.5,正在改善的/正在改进的(improving):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -4240,12 +4208,12 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "据俄媒周日报道，俄罗斯副外长谢尔盖·里亚布科夫警告称，俄罗斯将修改其核武器使用原则，以回应西方国家在俄乌冲突中的升级行为", "news_prompt2": "俄罗斯总统普京在2020年颁布的一项法令中规定，俄罗斯在遭遇敌人的核攻击或威胁到国家存在的常规攻击时，可以动用核武器", "news_prompt3": "俄罗斯军事分析人士中的一些鹰派人士敦促普京降低动用核武器的门槛，以“震慑”俄罗斯的西方敌人", "news_prompt4": "普京今年6月表示，核原则是一种“活的工具”，可能会根据世界局势的变化而变化", "news_prompt5": "里亚布科夫周日的言论是迄今为止最明确的声明，表明核武器使用原则确实会发生改变", "news_prompt6": "“这项工作已进入后期阶段，有明确的修改意图", "news_prompt7": "”里亚布科夫称", "news_prompt8": "他还表示，这一决定“与我们的西方对手在乌克兰冲突中的升级行动有关”", "news_prompt9": "里亚布科夫没有透露更新后的核原则何时会准备就绪", "news_prompt10": "俄罗斯拥有的核武器比其他任何国家都多", "news_prompt11": "普京今年3月份表示，莫斯科“从军事技术的角度”已经为可能发生的核战争做好了准备，但他也指出核战争“并不着急”，没有必要在乌克兰使用核武器", "news_prompt12": "践踏俄罗斯红线 　　普京在2022年2月俄乌冲突爆发的第一天就警告称，任何试图阻碍或威胁俄罗斯的人，都将遭受“你们历史上从未面临过的后果”", "news_prompt13": "此后，俄罗斯又发表了一系列被西方视为核威胁的声明，并宣布在白俄罗斯部署俄罗斯战术核武器", "news_prompt14": "但这并没能阻止美国及其盟友加大对乌克兰的军事援助，包括提供坦克、远程导弹和F-16战斗机", "news_prompt15": "这在战争开始时是不可想象的", "news_prompt16": "俄罗斯指责西方利用乌克兰作为代理人对其发动战争，目的是对俄罗斯造成“战略挫败”并使其分裂", "news_prompt17": "但美国及其西方盟友对此予以否认，称他们是在帮助乌克兰抵御俄罗斯攻击", "news_prompt18": "上个月，乌克兰派遣数千名士兵越过边境进入俄罗斯西部库尔斯克地区，此举震惊了莫斯科", "news_prompt19": "乌克兰总统泽连斯基表示，此次行动表明普京所谓的“红线”是虚张声势", "news_prompt20": "他还在极力劝说美国允许其使用先进的西方武器打击俄罗斯境内目标", "news_prompt21": "克里姆林宫发言人德米特里·佩斯科夫周日发表的采访中表示，西方“做得太过了”，俄罗斯将尽一切努力保护自己的利益", "news_prompt22": "（文章来源：财联社）"}</t>
+          <t>{"news_prompt1": "“这项工作已进入后期阶段，有明确的修改意图"}</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>{"“这项工作已进入后期阶段，有明确的修改意图": {"topic": "“生产投资”", "similarity": 0.4303567707538605, "prompt": "新闻文本是““这项工作已进入后期阶段，有明确的修改意图”，包含的情绪词典是：修正/修订(amendment):0.1,正在改善的/正在改进的(improving):0.5"}, "（文章来源：财联社）": {"topic": "“金融”", "similarity": 0.4321631193161011, "prompt": "新闻文本是“（文章来源：财联社）”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}}</t>
+          <t>{"“这项工作已进入后期阶段，有明确的修改意图": {"topic": "“生产投资”", "similarity": 0.43035683035850525, "prompt": "新闻文本是““这项工作已进入后期阶段，有明确的修改意图”，包含的情绪词典是：修正/修订(amendment):0.1,正在改善的/正在改进的(improving):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -4291,12 +4259,12 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "A股8月30日共有1784只个股获融资资金买入，有59股买入金额超亿元", "news_prompt2": "其中，农业银行、工商银行、赛力斯融资买入金额排名前三，分别获买入5.37亿元、4.49亿元、4.28亿元", "news_prompt3": "从融资买入额占当日总成交金额比重来看，有7只个股融资买入额占比超30%", "news_prompt4": "其中海利尔、爱科赛博、钜泉科技融资买入额占成交额比重排名前三，分别为37.33%、32.93%、32.43%", "news_prompt5": "从融资净买入金额来看，有5只个股获融资净买入超亿元", "news_prompt6": "其中，交通银行、中金黄金、招商银行融资净买入金额排名前三，分别获净买入1.32亿元、1.32亿元、1.17亿元", "news_prompt7": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "A股8月30日共有1784只个股获融资资金买入，有59股买入金额超亿元", "news_prompt2": "其中，农业银行、工商银行、赛力斯融资买入金额排名前三，分别获买入5.37亿元、4.49亿元、4.28亿元", "news_prompt3": "从融资买入额占当日总成交金额比重来看，有7只个股融资买入额占比超30%", "news_prompt4": "其中海利尔、爱科赛博、钜泉科技融资买入额占成交额比重排名前三，分别为37.33%、32.93%、32.43%", "news_prompt5": "从融资净买入金额来看，有5只个股获融资净买入超亿元", "news_prompt6": "其中，交通银行、中金黄金、招商银行融资净买入金额排名前三，分别获净买入1.32亿元、1.32亿元、1.17亿元"}</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>{"A股8月30日共有1784只个股获融资资金买入，有59股买入金额超亿元": {"topic": "“金融”", "similarity": 0.6299508810043335, "prompt": "新闻文本是“A股8月30日共有1784只个股获融资资金买入，有59股买入金额超亿元”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "其中，农业银行、工商银行、赛力斯融资买入金额排名前三，分别获买入5.37亿元、4.49亿元、4.28亿元": {"topic": "“金融”", "similarity": 0.6075814366340637, "prompt": "新闻文本是“其中，农业银行、工商银行、赛力斯融资买入金额排名前三，分别获买入5.37亿元、4.49亿元、4.28亿元”，包含的情绪词典是：投资/投资额(investment):0.4,金融的/财政的(financial):0.0"}, "从融资买入额占当日总成交金额比重来看，有7只个股融资买入额占比超30%": {"topic": "“金融”", "similarity": 0.592864990234375, "prompt": "新闻文本是“从融资买入额占当日总成交金额比重来看，有7只个股融资买入额占比超30%”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "其中海利尔、爱科赛博、钜泉科技融资买入额占成交额比重排名前三，分别为37.33%、32.93%、32.43%": {"topic": "“金融”", "similarity": 0.5536131262779236, "prompt": "新闻文本是“其中海利尔、爱科赛博、钜泉科技融资买入额占成交额比重排名前三，分别为37.33%、32.93%、32.43%”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "从融资净买入金额来看，有5只个股获融资净买入超亿元": {"topic": "“金融”", "similarity": 0.5476346015930176, "prompt": "新闻文本是“从融资净买入金额来看，有5只个股获融资净买入超亿元”，包含的情绪词典是：投资/投资额(investment):0.4,资本/资金(capital):0.1"}, "其中，交通银行、中金黄金、招商银行融资净买入金额排名前三，分别获净买入1.32亿元、1.32亿元、1.17亿元": {"topic": "“金融”", "similarity": 0.6381269693374634, "prompt": "新闻文本是“其中，交通银行、中金黄金、招商银行融资净买入金额排名前三，分别获净买入1.32亿元、1.32亿元、1.17亿元”，包含的情绪词典是：投资/投资额(investment):0.4,资本/资金(capital):0.1"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"A股8月30日共有1784只个股获融资资金买入，有59股买入金额超亿元": {"topic": "“金融”", "similarity": 0.629951000213623, "prompt": "新闻文本是“A股8月30日共有1784只个股获融资资金买入，有59股买入金额超亿元”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "其中，农业银行、工商银行、赛力斯融资买入金额排名前三，分别获买入5.37亿元、4.49亿元、4.28亿元": {"topic": "“金融”", "similarity": 0.607581615447998, "prompt": "新闻文本是“其中，农业银行、工商银行、赛力斯融资买入金额排名前三，分别获买入5.37亿元、4.49亿元、4.28亿元”，包含的情绪词典是：投资/投资额(investment):0.4,金融的/财政的(financial):0.0"}, "从融资买入额占当日总成交金额比重来看，有7只个股融资买入额占比超30%": {"topic": "“金融”", "similarity": 0.5928651690483093, "prompt": "新闻文本是“从融资买入额占当日总成交金额比重来看，有7只个股融资买入额占比超30%”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "其中海利尔、爱科赛博、钜泉科技融资买入额占成交额比重排名前三，分别为37.33%、32.93%、32.43%": {"topic": "“金融”", "similarity": 0.5536131858825684, "prompt": "新闻文本是“其中海利尔、爱科赛博、钜泉科技融资买入额占成交额比重排名前三，分别为37.33%、32.93%、32.43%”，包含的情绪词典是：投资/投资额(investment):0.4,投资/投入(invest):0.3"}, "从融资净买入金额来看，有5只个股获融资净买入超亿元": {"topic": "“金融”", "similarity": 0.5476348400115967, "prompt": "新闻文本是“从融资净买入金额来看，有5只个股获融资净买入超亿元”，包含的情绪词典是：投资/投资额(investment):0.4,资本/资金(capital):0.1"}, "其中，交通银行、中金黄金、招商银行融资净买入金额排名前三，分别获净买入1.32亿元、1.32亿元、1.17亿元": {"topic": "“金融”", "similarity": 0.6381270885467529, "prompt": "新闻文本是“其中，交通银行、中金黄金、招商银行融资净买入金额排名前三，分别获净买入1.32亿元、1.32亿元、1.17亿元”，包含的情绪词典是：投资/投资额(investment):0.4,资本/资金(capital):0.1"}}</t>
         </is>
       </c>
     </row>
@@ -4340,16 +4308,8 @@
           <t>每日经济新闻</t>
         </is>
       </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>{"news_prompt1": "每经AI快讯，港股次新股嘀嗒出行持续拉升，现涨超45%", "news_prompt2": "（文章来源：每日经济新闻）"}</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>{"每经AI快讯，港股次新股嘀嗒出行持续拉升，现涨超45%": {"topic": "“金融”", "similarity": 0.4414985179901123}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
-        </is>
-      </c>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4397,12 +4357,12 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "近日，一起因教师节礼物引发的劳动争议案尘埃落定", "news_prompt2": "重庆市九龙坡区三峡幼儿园前园长王某仙（化名）因在2023年教师节前夕“收受”学生一盒价值6.16元的巧克力，被幼儿园开除", "news_prompt3": "王某仙对此不服，将幼儿园告上法庭", "news_prompt4": "法院认为，王某仙收受的巧克力价值较低，是小朋友出于喜爱和尊敬而赠送，不宜定性为收受学生及家长礼品礼金", "news_prompt5": "同时，在双方未能就调岗达成一致的情况下，幼儿园未给予改正机会便径行解除劳动合同，明显不够审慎，属于违法解除，应支付赔偿金", "news_prompt6": "就事论事，确实存在相关规定禁止教师收礼", "news_prompt7": "2014年，教育部公开发布《严禁教师违规收受学生及家长礼金等行为的规定》，其中指出：严禁以任何方式索要或接受学生及家长赠送的礼品礼金、有价证券和支付凭证等财物", "news_prompt8": "对照来看，巧克力充其量能与其中的礼品扯上关系", "news_prompt9": "不过稍加琢磨不难发现，这6.16元的巧克力分明是小朋友出于敬爱送给园长的零食", "news_prompt10": "擅自给其扣上礼品的帽子，无疑玷污了小朋友纯粹的喜爱之情，也破坏了师生正常交流的边界，而边界的收缩，无疑会让教师束手束脚、无所适从", "news_prompt11": "评论区里，网友纷纷在为王某仙抱不平，某网友调侃“难道这个巧克力是LV的", "news_prompt12": "”还有同样身为教育工作者的网友在线求助：“那天值班，一名学生给我买了一瓶冰镇饮料，我接过来就喝了，咋办", "news_prompt13": "”网友的种种态度，无疑说明幼儿园的做法突破了公众朴素的认知", "news_prompt14": "一般而言，礼品具有如下的一个或几个特征：一是得有一定的价值", "news_prompt15": "二是得满足送礼对象的个性需求，对旁人或许没有价值，但对当事人则另说", "news_prompt16": "三是具备较强的流通性，容易变现", "news_prompt17": "而案例中的巧克力显然不在此列", "news_prompt18": "另外，鉴于“园长随后就把巧克力给小朋友分了”，可以说王某仙没有将巧克力作私人用途", "news_prompt19": "退一万步说，即便将其定义为礼品，把园长开除的处理也不合适", "news_prompt20": "除了开除外，还有警告、记过等可用的手段，如果过罚不一致，就有失公平公正", "news_prompt21": "事实上，这也是此事为公众诟病之处", "news_prompt22": "可为佐证的是：不少网友纷纷喊话，按照这一标准，全国的所有园长怕是都要下岗了", "news_prompt23": "从小处维护师德师风，对一些违规行为坚决说“不”并严格处理，这并没有什么问题，但处理不能不分青红皂白，脱离现实语境", "news_prompt24": "园长作为幼教团队的一员，需要与学生相处，进行正常的情感互动，而这种动辄得咎的处理方式于教书育人无疑大大不利", "news_prompt25": "此外，也需要关心一下那位送出巧克力的孩子及其家长是否会被自责、愧疚的情绪笼罩", "news_prompt26": "一言以蔽之，教师收礼行为当然需要治理，但不宜盲目扩大范围并且一味地“高高举起，重重落下”", "news_prompt27": "案例中，幼儿园将学生送来的价值6块多的零食视为礼品，并且将园长开除的做法显然就用力过猛了", "news_prompt28": "幸而法律进行了纠偏，亮出了鲜明的态度，将事情拉回正轨", "news_prompt29": "文l胡一刀（文章来源：南方都市报）"}</t>
+          <t>{"news_prompt1": "同时，在双方未能就调岗达成一致的情况下，幼儿园未给予改正机会便径行解除劳动合同，明显不够审慎，属于违法解除，应支付赔偿金", "news_prompt2": "就事论事，确实存在相关规定禁止教师收礼", "news_prompt3": "擅自给其扣上礼品的帽子，无疑玷污了小朋友纯粹的喜爱之情，也破坏了师生正常交流的边界，而边界的收缩，无疑会让教师束手束脚、无所适从", "news_prompt4": "”还有同样身为教育工作者的网友在线求助：“那天值班，一名学生给我买了一瓶冰镇饮料，我接过来就喝了，咋办", "news_prompt5": "一般而言，礼品具有如下的一个或几个特征：一是得有一定的价值", "news_prompt6": "二是得满足送礼对象的个性需求，对旁人或许没有价值，但对当事人则另说", "news_prompt7": "三是具备较强的流通性，容易变现", "news_prompt8": "从小处维护师德师风，对一些违规行为坚决说“不”并严格处理，这并没有什么问题，但处理不能不分青红皂白，脱离现实语境", "news_prompt9": "园长作为幼教团队的一员，需要与学生相处，进行正常的情感互动，而这种动辄得咎的处理方式于教书育人无疑大大不利", "news_prompt10": "一言以蔽之，教师收礼行为当然需要治理，但不宜盲目扩大范围并且一味地“高高举起，重重落下”", "news_prompt11": "案例中，幼儿园将学生送来的价值6块多的零食视为礼品，并且将园长开除的做法显然就用力过猛了"}</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>{"法院认为，王某仙收受的巧克力价值较低，是小朋友出于喜爱和尊敬而赠送，不宜定性为收受学生及家长礼品礼金": {"topic": "“消费”", "similarity": 0.42972826957702637}, "同时，在双方未能就调岗达成一致的情况下，幼儿园未给予改正机会便径行解除劳动合同，明显不够审慎，属于违法解除，应支付赔偿金": {"topic": "“房地产”", "similarity": 0.44037187099456787, "prompt": "新闻文本是“同时，在双方未能就调岗达成一致的情况下，幼儿园未给予改正机会便径行解除劳动合同，明显不够审慎，属于违法解除，应支付赔偿金”，包含的情绪词典是：未和解的/未协调的(unreconciled):-0.3,不同意/不一致(disagreement):-0.5"}, "就事论事，确实存在相关规定禁止教师收礼": {"topic": "“房地产”", "similarity": 0.4206409752368927, "prompt": "新闻文本是“就事论事，确实存在相关规定禁止教师收礼”，包含的情绪词典是：规定/约定(stipulate):0.0,禁止/禁令(prohibition):-0.3"}, "2014年，教育部公开发布《严禁教师违规收受学生及家长礼金等行为的规定》，其中指出：严禁以任何方式索要或接受学生及家长赠送的礼品礼金、有价证券和支付凭证等财物": {"topic": "“消费”", "similarity": 0.5091487169265747}, "擅自给其扣上礼品的帽子，无疑玷污了小朋友纯粹的喜爱之情，也破坏了师生正常交流的边界，而边界的收缩，无疑会让教师束手束脚、无所适从": {"topic": "“消费”", "similarity": 0.43430060148239136, "prompt": "新闻文本是“擅自给其扣上礼品的帽子，无疑玷污了小朋友纯粹的喜爱之情，也破坏了师生正常交流的边界，而边界的收缩，无疑会让教师束手束脚、无所适从”，包含的情绪词典是：不适当的/猥亵的(indecent):-0.5,不适当/猥亵(indecency):-0.4"}, "”还有同样身为教育工作者的网友在线求助：“那天值班，一名学生给我买了一瓶冰镇饮料，我接过来就喝了，咋办": {"topic": "“消费”", "similarity": 0.46241313219070435, "prompt": "新闻文本是“”还有同样身为教育工作者的网友在线求助：“那天值班，一名学生给我买了一瓶冰镇饮料，我接过来就喝了，咋办”，包含的情绪词典是：喝/饮用(drink):0.0"}, "一般而言，礼品具有如下的一个或几个特征：一是得有一定的价值": {"topic": "“消费”", "similarity": 0.47054606676101685, "prompt": "新闻文本是“一般而言，礼品具有如下的一个或几个特征：一是得有一定的价值”，包含的情绪词典是：有价值的/宝贵的(valuable):0.6,值得的/有价值的(worthy):0.4"}, "二是得满足送礼对象的个性需求，对旁人或许没有价值，但对当事人则另说": {"topic": "“消费”", "similarity": 0.4678238034248352, "prompt": "新闻文本是“二是得满足送礼对象的个性需求，对旁人或许没有价值，但对当事人则另说”，包含的情绪词典是：被要求的/必需的(required):0.0,有条件的/附条件的(conditional):0.0"}, "三是具备较强的流通性，容易变现": {"topic": "“金融”", "similarity": 0.5438585877418518, "prompt": "新闻文本是“三是具备较强的流通性，容易变现”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,有利可图的/赚钱的(lucrative):0.7"}, "可为佐证的是：不少网友纷纷喊话，按照这一标准，全国的所有园长怕是都要下岗了": {"topic": "“房地产”", "similarity": 0.42188066244125366}, "从小处维护师德师风，对一些违规行为坚决说“不”并严格处理，这并没有什么问题，但处理不能不分青红皂白，脱离现实语境": {"topic": "“金融”", "similarity": 0.42018038034439087, "prompt": "新闻文本是“从小处维护师德师风，对一些违规行为坚决说“不”并严格处理，这并没有什么问题，但处理不能不分青红皂白，脱离现实语境”，包含的情绪词典是：不遵守的/违反的(noncompliant):-0.5,不可取的/不宜的(inadvisable):-0.5"}, "园长作为幼教团队的一员，需要与学生相处，进行正常的情感互动，而这种动辄得咎的处理方式于教书育人无疑大大不利": {"topic": "“房地产”", "similarity": 0.4216141700744629, "prompt": "新闻文本是“园长作为幼教团队的一员，需要与学生相处，进行正常的情感互动，而这种动辄得咎的处理方式于教书育人无疑大大不利”，包含的情绪词典是：不合意的/难相处的(disagreeable):-0.4,处理不当/误操作(mishandle):-0.5"}, "一言以蔽之，教师收礼行为当然需要治理，但不宜盲目扩大范围并且一味地“高高举起，重重落下”": {"topic": "“消费”", "similarity": 0.47619450092315674, "prompt": "新闻文本是“一言以蔽之，教师收礼行为当然需要治理，但不宜盲目扩大范围并且一味地“高高举起，重重落下””，包含的情绪词典是：应受惩罚的/可惩处的(punishable):-0.4,使负有义务的/有义务的(obligated):-0.1"}, "案例中，幼儿园将学生送来的价值6块多的零食视为礼品，并且将园长开除的做法显然就用力过猛了": {"topic": "“消费”", "similarity": 0.4437327980995178, "prompt": "新闻文本是“案例中，幼儿园将学生送来的价值6块多的零食视为礼品，并且将园长开除的做法显然就用力过猛了”，包含的情绪词典是：不合理的/不正当的(unjustifiable):-0.5,不合理的/不正当的(unjustified):-0.3"}}</t>
+          <t>{"同时，在双方未能就调岗达成一致的情况下，幼儿园未给予改正机会便径行解除劳动合同，明显不够审慎，属于违法解除，应支付赔偿金": {"topic": "“房地产”", "similarity": 0.4403718411922455, "prompt": "新闻文本是“同时，在双方未能就调岗达成一致的情况下，幼儿园未给予改正机会便径行解除劳动合同，明显不够审慎，属于违法解除，应支付赔偿金”，包含的情绪词典是：未和解的/未协调的(unreconciled):-0.3,不同意/不一致(disagreement):-0.5"}, "就事论事，确实存在相关规定禁止教师收礼": {"topic": "“房地产”", "similarity": 0.4206410050392151, "prompt": "新闻文本是“就事论事，确实存在相关规定禁止教师收礼”，包含的情绪词典是：规定/约定(stipulate):0.0,禁止/禁令(prohibition):-0.3"}, "擅自给其扣上礼品的帽子，无疑玷污了小朋友纯粹的喜爱之情，也破坏了师生正常交流的边界，而边界的收缩，无疑会让教师束手束脚、无所适从": {"topic": "“消费”", "similarity": 0.4343007802963257, "prompt": "新闻文本是“擅自给其扣上礼品的帽子，无疑玷污了小朋友纯粹的喜爱之情，也破坏了师生正常交流的边界，而边界的收缩，无疑会让教师束手束脚、无所适从”，包含的情绪词典是：不适当的/猥亵的(indecent):-0.5,不适当/猥亵(indecency):-0.4"}, "”还有同样身为教育工作者的网友在线求助：“那天值班，一名学生给我买了一瓶冰镇饮料，我接过来就喝了，咋办": {"topic": "“消费”", "similarity": 0.4624131917953491, "prompt": "新闻文本是“”还有同样身为教育工作者的网友在线求助：“那天值班，一名学生给我买了一瓶冰镇饮料，我接过来就喝了，咋办”，包含的情绪词典是：喝/饮用(drink):0.0"}, "一般而言，礼品具有如下的一个或几个特征：一是得有一定的价值": {"topic": "“消费”", "similarity": 0.4705463647842407, "prompt": "新闻文本是“一般而言，礼品具有如下的一个或几个特征：一是得有一定的价值”，包含的情绪词典是：有价值的/宝贵的(valuable):0.6,值得的/有价值的(worthy):0.4"}, "二是得满足送礼对象的个性需求，对旁人或许没有价值，但对当事人则另说": {"topic": "“消费”", "similarity": 0.46782398223876953, "prompt": "新闻文本是“二是得满足送礼对象的个性需求，对旁人或许没有价值，但对当事人则另说”，包含的情绪词典是：被要求的/必需的(required):0.0,有条件的/附条件的(conditional):0.0"}, "三是具备较强的流通性，容易变现": {"topic": "“金融”", "similarity": 0.5438586473464966, "prompt": "新闻文本是“三是具备较强的流通性，容易变现”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,有利可图的/赚钱的(lucrative):0.7"}, "从小处维护师德师风，对一些违规行为坚决说“不”并严格处理，这并没有什么问题，但处理不能不分青红皂白，脱离现实语境": {"topic": "“金融”", "similarity": 0.42018046975135803, "prompt": "新闻文本是“从小处维护师德师风，对一些违规行为坚决说“不”并严格处理，这并没有什么问题，但处理不能不分青红皂白，脱离现实语境”，包含的情绪词典是：不遵守的/违反的(noncompliant):-0.5,不可取的/不宜的(inadvisable):-0.5"}, "园长作为幼教团队的一员，需要与学生相处，进行正常的情感互动，而这种动辄得咎的处理方式于教书育人无疑大大不利": {"topic": "“房地产”", "similarity": 0.4216141998767853, "prompt": "新闻文本是“园长作为幼教团队的一员，需要与学生相处，进行正常的情感互动，而这种动辄得咎的处理方式于教书育人无疑大大不利”，包含的情绪词典是：不合意的/难相处的(disagreeable):-0.4,处理不当/误操作(mishandle):-0.5"}, "一言以蔽之，教师收礼行为当然需要治理，但不宜盲目扩大范围并且一味地“高高举起，重重落下”": {"topic": "“消费”", "similarity": 0.4761945605278015, "prompt": "新闻文本是“一言以蔽之，教师收礼行为当然需要治理，但不宜盲目扩大范围并且一味地“高高举起，重重落下””，包含的情绪词典是：应受惩罚的/可惩处的(punishable):-0.4,使负有义务的/有义务的(obligated):-0.1"}, "案例中，幼儿园将学生送来的价值6块多的零食视为礼品，并且将园长开除的做法显然就用力过猛了": {"topic": "“消费”", "similarity": 0.4437329173088074, "prompt": "新闻文本是“案例中，幼儿园将学生送来的价值6块多的零食视为礼品，并且将园长开除的做法显然就用力过猛了”，包含的情绪词典是：不合理的/不正当的(unjustifiable):-0.5,不合理的/不正当的(unjustified):-0.3"}}</t>
         </is>
       </c>
     </row>
@@ -4448,12 +4408,12 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "南方日报讯 （记者/李霭莹通讯员/江关宣）为进一步优化口岸营商环境，促进跨境贸易便利化，海关总署发布2024年第106号公告，自2024年9月1日起，增加《区域全面经济伙伴关系协定》（RCEP）项下输越南原产地证书以及《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚、越南的原产地证书为可自助打印证书", "news_prompt2": "9月1日，维达纸业（中国）有限公司通过国际贸易“单一窗口”自助打印系统，成功为其出口马来西亚的一批卷装纸自助打印原产地证书", "news_prompt3": "这是我国签发的首份《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚原产地自助打印证书", "news_prompt4": "该公司关务负责人李玉钿表示：“以前申报原产地证书每月要跑几趟海关", "news_prompt5": "输马来西亚原产地证书自助打印开通后，企业实现了足不出户就可以打印证书，非常方便，同时也大大节省了企业的人力物力成本", "news_prompt6": "”今年前8个月，该公司出口马来西亚卫生卷纸4076.1吨，货值4301.8万元，同比分别增长28%、10.9%", "news_prompt7": "“目前可以自助打印的原产地证书有20多种，其中出口马来西亚和越南的原产地证书已全部实现自助打印", "news_prompt8": "”江门海关所属新会海关企业管理科科长丘锦堂介绍，原产地证书申请人或代理人可通过国际贸易“单一窗口”或“互联网+海关”一体化网上办事平台，自行打印海关审核通过的原产地证书，无须再到海关领取，实现了企业“零跑腿”、签证“零见面”", "news_prompt9": "“在海关推动下，江门关区原产地证书自助打印率在逐年提升，1—7月自助打印率达到98.88%，较去年同期增长了0.61个百分点", "news_prompt10": "”该关关税处罗衡副处长表示“本次原产地证书自助打印再次扩围，证书申领电子化程度进一步深化，我关将持续推动该项改革，让广大企业切实感受到智慧海关带来的通关便利", "news_prompt11": "” 　　据海关统计，今年1—7月，该关已为企业签发各类原产地证书4.36万份，签证货值138.70亿元，同比分别增长14.7%和8.4%", "news_prompt12": "（文章来源：南方日报）"}</t>
+          <t>{"news_prompt1": "这是我国签发的首份《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚原产地自助打印证书", "news_prompt2": "输马来西亚原产地证书自助打印开通后，企业实现了足不出户就可以打印证书，非常方便，同时也大大节省了企业的人力物力成本", "news_prompt3": "”今年前8个月，该公司出口马来西亚卫生卷纸4076.1吨，货值4301.8万元，同比分别增长28%、10.9%", "news_prompt4": "”江门海关所属新会海关企业管理科科长丘锦堂介绍，原产地证书申请人或代理人可通过国际贸易“单一窗口”或“互联网+海关”一体化网上办事平台，自行打印海关审核通过的原产地证书，无须再到海关领取，实现了企业“零跑腿”、签证“零见面”", "news_prompt5": "“在海关推动下，江门关区原产地证书自助打印率在逐年提升，1—7月自助打印率达到98.88%，较去年同期增长了0.61个百分点", "news_prompt6": "”该关关税处罗衡副处长表示“本次原产地证书自助打印再次扩围，证书申领电子化程度进一步深化，我关将持续推动该项改革，让广大企业切实感受到智慧海关带来的通关便利", "news_prompt7": "” 　　据海关统计，今年1—7月，该关已为企业签发各类原产地证书4.36万份，签证货值138.70亿元，同比分别增长14.7%和8.4%"}</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>{"南方日报讯 （记者/李霭莹通讯员/江关宣）为进一步优化口岸营商环境，促进跨境贸易便利化，海关总署发布2024年第106号公告，自2024年9月1日起，增加《区域全面经济伙伴关系协定》（RCEP）项下输越南原产地证书以及《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚、越南的原产地证书为可自助打印证书": {"topic": "“消费”", "similarity": 0.46611398458480835}, "这是我国签发的首份《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚原产地自助打印证书": {"topic": "“生产投资”", "similarity": 0.4789712429046631, "prompt": "新闻文本是“这是我国签发的首份《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚原产地自助打印证书”，包含的情绪词典是：协议/协定(agreement):0.4,联盟/同盟(alliance):0.3"}, "输马来西亚原产地证书自助打印开通后，企业实现了足不出户就可以打印证书，非常方便，同时也大大节省了企业的人力物力成本": {"topic": "“消费”", "similarity": 0.4485621750354767, "prompt": "新闻文本是“输马来西亚原产地证书自助打印开通后，企业实现了足不出户就可以打印证书，非常方便，同时也大大节省了企业的人力物力成本”，包含的情绪词典是：本土的/本地的(indigenous):0.0,可得到的/可用的(available):0.1"}, "”今年前8个月，该公司出口马来西亚卫生卷纸4076.1吨，货值4301.8万元，同比分别增长28%、10.9%": {"topic": "“宏观经济”", "similarity": 0.4510953426361084, "prompt": "新闻文本是“”今年前8个月，该公司出口马来西亚卫生卷纸4076.1吨，货值4301.8万元，同比分别增长28%、10.9%”，包含的情绪词典是：出口/输出(export):0.0,出口商/输出者(exporter):0.0"}, "”江门海关所属新会海关企业管理科科长丘锦堂介绍，原产地证书申请人或代理人可通过国际贸易“单一窗口”或“互联网+海关”一体化网上办事平台，自行打印海关审核通过的原产地证书，无须再到海关领取，实现了企业“零跑腿”、签证“零见面”": {"topic": "“生产投资”", "similarity": 0.48611146211624146, "prompt": "新闻文本是“”江门海关所属新会海关企业管理科科长丘锦堂介绍，原产地证书申请人或代理人可通过国际贸易“单一窗口”或“互联网+海关”一体化网上办事平台，自行打印海关审核通过的原产地证书，无须再到海关领取，实现了企业“零跑腿”、签证“零见面””，包含的情绪词典是：已公证的/已证实的(notarized):0.0,出口商/输出者(exporter):0.0"}, "“在海关推动下，江门关区原产地证书自助打印率在逐年提升，1—7月自助打印率达到98.88%，较去年同期增长了0.61个百分点": {"topic": "“消费”", "similarity": 0.47190260887145996, "prompt": "新闻文本是““在海关推动下，江门关区原产地证书自助打印率在逐年提升，1—7月自助打印率达到98.88%，较去年同期增长了0.61个百分点”，包含的情绪词典是：已公证的/已证实的(notarized):0.0"}, "”该关关税处罗衡副处长表示“本次原产地证书自助打印再次扩围，证书申领电子化程度进一步深化，我关将持续推动该项改革，让广大企业切实感受到智慧海关带来的通关便利": {"topic": "“生产投资”", "similarity": 0.519092321395874, "prompt": "新闻文本是“”该关关税处罗衡副处长表示“本次原产地证书自助打印再次扩围，证书申领电子化程度进一步深化，我关将持续推动该项改革，让广大企业切实感受到智慧海关带来的通关便利”，包含的情绪词典是：本土的/本地的(indigenous):0.0,正在改善的/正在改进的(improving):0.5"}, "” 　　据海关统计，今年1—7月，该关已为企业签发各类原产地证书4.36万份，签证货值138.70亿元，同比分别增长14.7%和8.4%": {"topic": "“生产投资”", "similarity": 0.5645448565483093, "prompt": "新闻文本是“” 　　据海关统计，今年1—7月，该关已为企业签发各类原产地证书4.36万份，签证货值138.70亿元，同比分别增长14.7%和8.4%”，包含的情绪词典是：企业/事业(enterprise):0.0,本土的/本地的(indigenous):0.0"}}</t>
+          <t>{"这是我国签发的首份《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚原产地自助打印证书": {"topic": "“生产投资”", "similarity": 0.4789712429046631, "prompt": "新闻文本是“这是我国签发的首份《中华人民共和国与东南亚国家联盟全面经济合作框架协议》项下输马来西亚原产地自助打印证书”，包含的情绪词典是：协议/协定(agreement):0.4,联盟/同盟(alliance):0.3"}, "输马来西亚原产地证书自助打印开通后，企业实现了足不出户就可以打印证书，非常方便，同时也大大节省了企业的人力物力成本": {"topic": "“消费”", "similarity": 0.4485622048377991, "prompt": "新闻文本是“输马来西亚原产地证书自助打印开通后，企业实现了足不出户就可以打印证书，非常方便，同时也大大节省了企业的人力物力成本”，包含的情绪词典是：本土的/本地的(indigenous):0.0,可得到的/可用的(available):0.1"}, "”今年前8个月，该公司出口马来西亚卫生卷纸4076.1吨，货值4301.8万元，同比分别增长28%、10.9%": {"topic": "“宏观经济”", "similarity": 0.45109543204307556, "prompt": "新闻文本是“”今年前8个月，该公司出口马来西亚卫生卷纸4076.1吨，货值4301.8万元，同比分别增长28%、10.9%”，包含的情绪词典是：出口/输出(export):0.0,出口商/输出者(exporter):0.0"}, "”江门海关所属新会海关企业管理科科长丘锦堂介绍，原产地证书申请人或代理人可通过国际贸易“单一窗口”或“互联网+海关”一体化网上办事平台，自行打印海关审核通过的原产地证书，无须再到海关领取，实现了企业“零跑腿”、签证“零见面”": {"topic": "“生产投资”", "similarity": 0.48611152172088623, "prompt": "新闻文本是“”江门海关所属新会海关企业管理科科长丘锦堂介绍，原产地证书申请人或代理人可通过国际贸易“单一窗口”或“互联网+海关”一体化网上办事平台，自行打印海关审核通过的原产地证书，无须再到海关领取，实现了企业“零跑腿”、签证“零见面””，包含的情绪词典是：已公证的/已证实的(notarized):0.0,出口商/输出者(exporter):0.0"}, "“在海关推动下，江门关区原产地证书自助打印率在逐年提升，1—7月自助打印率达到98.88%，较去年同期增长了0.61个百分点": {"topic": "“消费”", "similarity": 0.4719028174877167, "prompt": "新闻文本是““在海关推动下，江门关区原产地证书自助打印率在逐年提升，1—7月自助打印率达到98.88%，较去年同期增长了0.61个百分点”，包含的情绪词典是：已公证的/已证实的(notarized):0.0"}, "”该关关税处罗衡副处长表示“本次原产地证书自助打印再次扩围，证书申领电子化程度进一步深化，我关将持续推动该项改革，让广大企业切实感受到智慧海关带来的通关便利": {"topic": "“生产投资”", "similarity": 0.5190923810005188, "prompt": "新闻文本是“”该关关税处罗衡副处长表示“本次原产地证书自助打印再次扩围，证书申领电子化程度进一步深化，我关将持续推动该项改革，让广大企业切实感受到智慧海关带来的通关便利”，包含的情绪词典是：本土的/本地的(indigenous):0.0,正在改善的/正在改进的(improving):0.5"}, "” 　　据海关统计，今年1—7月，该关已为企业签发各类原产地证书4.36万份，签证货值138.70亿元，同比分别增长14.7%和8.4%": {"topic": "“生产投资”", "similarity": 0.5645449161529541, "prompt": "新闻文本是“” 　　据海关统计，今年1—7月，该关已为企业签发各类原产地证书4.36万份，签证货值138.70亿元，同比分别增长14.7%和8.4%”，包含的情绪词典是：企业/事业(enterprise):0.0,本土的/本地的(indigenous):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -4503,12 +4463,12 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "“伟大出自平凡，平凡造就伟大", "news_prompt2": "能够成就伟大者，无不是由点点滴滴的平凡积累而成", "news_prompt3": "” 　　今天，在“农情同筑梦行远向未来”农行萧山分行2024年度“员工礼”表彰会上，“平凡”二字有了生动的注解", "news_prompt4": "表彰会的主角，是来自各个岗位的员工，他们日复一日坚守在平凡岗位上，脚踏实地、默默耕耘，与农行同奋进、共成长", "news_prompt5": "在职5年、10年、20年、30年、35年/40年的员工分别获得“成长礼”、“担当礼”、“敬业礼”、“忠诚礼”和“荣耀礼”五个“员工礼”", "news_prompt6": "活动通过“视频+图片”直播的方式，全行近700名员工和家属代表共赴一场精神传承的盛会", "news_prompt7": "从平凡到不凡他们见证一路发展 　　干一行，专一行，精一行", "news_prompt8": "在农行萧山分行，员工按照入职年份获得“员工礼”，年份最长的员工，已经进入农行工作40余年，从激情到稳重，从稚嫩到成熟，从一头黑发到两鬓斑白，从一名青年蜕变成农行栋梁", "news_prompt9": "5年，他们在最美好的青春，拥有无穷的未来，无限的可能", "news_prompt10": "10年，用“勤勉”谱写悦耳的青春乐章，用“担当”叩开职业理想的大门", "news_prompt11": "20年，他们用最美好的年华，与农行相伴成长", "news_prompt12": "30年，“农业银行”已经融入他们的骨血，他们是农行的忠诚卫士", "news_prompt13": "40年，他们见证历史，用汗水、智慧和忠诚谱写了农行萧山分行波澜壮阔的发展篇章", "news_prompt14": "“我见证了金融业脱胎换骨的变化：从珠算到计算机到AI人工智能的应用", "news_prompt15": "见证了祖国日新月异的变化", "news_prompt16": "同时也见证了农行的蓬勃发展", "news_prompt17": "”入职30余年的 “忠诚礼”获得者沈伟中激动地表示，忠诚不仅是对过去的传承，更是对未来的期许", "news_prompt18": "从网点走到部门，来自风险管理部的陈羿花了十年", "news_prompt19": "这十年，她对农行、对银行、对金融有了属于自己的认识", "news_prompt20": "“有陪伴、有教导、有收获、有成长，最终这3650天的点点滴滴都化为我成长路上的珍贵回忆，支撑着我克服惰性、松懈和缺点，努力成为这大家庭里更好的一份子", "news_prompt21": "”陈羿说", "news_prompt22": "当晚，像沈伟中和陈羿这样获得“员工礼”的人有104人", "news_prompt23": "自2017年起，农行萧山分行已连续八年对不同行龄的员工进行表彰，感谢员工们辛勤付出的同时，更表达关怀与肯定，截至目前，共表彰1081人次", "news_prompt24": "家园文化让爱与成长薪火相传 　　活动现场，各单位通过舞蹈、情景剧、配音秀、说唱、小组唱、诗歌朗诵等多种演绎形式，集中展示了农行萧山分行家园文化建设的最新成果，充分展现全行员工爱党爱行、积极向上的良好精神风貌", "news_prompt25": "歌曲《飘向北方》献给所有异地员工，为每一个来自五湖四海的员工鼓掌", "news_prompt26": "情景剧《跨越时空的电台》让大家在欢笑中看到平时工作中的自己，展现着农行人的责任与担当", "news_prompt27": "情景剧《反诈风云》聚焦了一次特殊的业务办理，以来自银行的温暖力量，守护每一份来之不易的安宁与信任", "news_prompt28": "配音秀《甄嬛传之合规经营篇》以独特的创意诠释“安全”这一银行经营的基础…… 　　在现场，“家园文化”成为高频词汇", "news_prompt29": "正如农行萧山分行相关负责人所说，作为改革开放后萧山辖区内第一家从人民银行分设的国有银行，农行萧山分行成立40多年来，成果颇丰", "news_prompt30": "这背后离不开每一位员工的奋勇拼搏", "news_prompt31": "农行萧山分行也为员工打造了温暖的“家”", "news_prompt32": "通过以业务技能、拜师“传帮带”、专业培训为主要内容的培养机制，以及各种具有知识性、趣味性的特色活动，农行充分调动员工参与“家园”建设活动的积极性，激发了员工爱岗敬业、奋发向上的工作热情，增进凝聚力和感召力", "news_prompt33": "当前，农行萧山分行所辖29家营业网点“职工之家”覆盖率达100%", "news_prompt34": "小小的空间连接起了员工的工作与业余文化生活，也打造了一个看得见、摸得到的温暖家园", "news_prompt35": "“员工礼”的出现，是员工职业生涯价值的体现，也是农业银行萧山分行“家园文化”建设的重要载体，激荡着人心", "news_prompt36": "人人期盼着，自己的奉献能为农行发展历史增添一抹亮丽色彩，并通过“员工礼”留下最美好的见证", "news_prompt37": "（文章来源：潮新闻）"}</t>
+          <t>{"news_prompt1": "能够成就伟大者，无不是由点点滴滴的平凡积累而成", "news_prompt2": "表彰会的主角，是来自各个岗位的员工，他们日复一日坚守在平凡岗位上，脚踏实地、默默耕耘，与农行同奋进、共成长", "news_prompt3": "在职5年、10年、20年、30年、35年/40年的员工分别获得“成长礼”、“担当礼”、“敬业礼”、“忠诚礼”和“荣耀礼”五个“员工礼”", "news_prompt4": "活动通过“视频+图片”直播的方式，全行近700名员工和家属代表共赴一场精神传承的盛会", "news_prompt5": "从平凡到不凡他们见证一路发展 　　干一行，专一行，精一行", "news_prompt6": "40年，他们见证历史，用汗水、智慧和忠诚谱写了农行萧山分行波澜壮阔的发展篇章", "news_prompt7": "“我见证了金融业脱胎换骨的变化：从珠算到计算机到AI人工智能的应用", "news_prompt8": "见证了祖国日新月异的变化", "news_prompt9": "同时也见证了农行的蓬勃发展", "news_prompt10": "这十年，她对农行、对银行、对金融有了属于自己的认识", "news_prompt11": "“有陪伴、有教导、有收获、有成长，最终这3650天的点点滴滴都化为我成长路上的珍贵回忆，支撑着我克服惰性、松懈和缺点，努力成为这大家庭里更好的一份子", "news_prompt12": "家园文化让爱与成长薪火相传 　　活动现场，各单位通过舞蹈、情景剧、配音秀、说唱、小组唱、诗歌朗诵等多种演绎形式，集中展示了农行萧山分行家园文化建设的最新成果，充分展现全行员工爱党爱行、积极向上的良好精神风貌", "news_prompt13": "歌曲《飘向北方》献给所有异地员工，为每一个来自五湖四海的员工鼓掌", "news_prompt14": "情景剧《跨越时空的电台》让大家在欢笑中看到平时工作中的自己，展现着农行人的责任与担当", "news_prompt15": "情景剧《反诈风云》聚焦了一次特殊的业务办理，以来自银行的温暖力量，守护每一份来之不易的安宁与信任", "news_prompt16": "配音秀《甄嬛传之合规经营篇》以独特的创意诠释“安全”这一银行经营的基础…… 　　在现场，“家园文化”成为高频词汇", "news_prompt17": "这背后离不开每一位员工的奋勇拼搏", "news_prompt18": "通过以业务技能、拜师“传帮带”、专业培训为主要内容的培养机制，以及各种具有知识性、趣味性的特色活动，农行充分调动员工参与“家园”建设活动的积极性，激发了员工爱岗敬业、奋发向上的工作热情，增进凝聚力和感召力", "news_prompt19": "当前，农行萧山分行所辖29家营业网点“职工之家”覆盖率达100%", "news_prompt20": "“员工礼”的出现，是员工职业生涯价值的体现，也是农业银行萧山分行“家园文化”建设的重要载体，激荡着人心"}</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>{"能够成就伟大者，无不是由点点滴滴的平凡积累而成": {"topic": "“消费”", "similarity": 0.42019450664520264, "prompt": "新闻文本是“能够成就伟大者，无不是由点点滴滴的平凡积累而成”，包含的情绪词典是：成就/成绩(accomplishment):0.5,成就/成绩(achievement):0.5"}, "” 　　今天，在“农情同筑梦行远向未来”农行萧山分行2024年度“员工礼”表彰会上，“平凡”二字有了生动的注解": {"topic": "“消费”", "similarity": 0.4714670181274414}, "表彰会的主角，是来自各个岗位的员工，他们日复一日坚守在平凡岗位上，脚踏实地、默默耕耘，与农行同奋进、共成长": {"topic": "“消费”", "similarity": 0.5014982223510742, "prompt": "新闻文本是“表彰会的主角，是来自各个岗位的员工，他们日复一日坚守在平凡岗位上，脚踏实地、默默耕耘，与农行同奋进、共成长”，包含的情绪词典是：勤奋地/勤勉地(diligently):0.4,成就/成绩(achievement):0.5"}, "在职5年、10年、20年、30年、35年/40年的员工分别获得“成长礼”、“担当礼”、“敬业礼”、“忠诚礼”和“荣耀礼”五个“员工礼”": {"topic": "“生产投资”", "similarity": 0.5444313883781433, "prompt": "新闻文本是“在职5年、10年、20年、30年、35年/40年的员工分别获得“成长礼”、“担当礼”、“敬业礼”、“忠诚礼”和“荣耀礼”五个“员工礼””，包含的情绪词典是：荣誉/光荣(honors):0.4,荣誉/名誉(honor):0.4"}, "活动通过“视频+图片”直播的方式，全行近700名员工和家属代表共赴一场精神传承的盛会": {"topic": "“消费”", "similarity": 0.44132936000823975, "prompt": "新闻文本是“活动通过“视频+图片”直播的方式，全行近700名员工和家属代表共赴一场精神传承的盛会”，包含的情绪词典是：活动/行动(activity):0.2,银行/河岸(bank):0.0"}, "从平凡到不凡他们见证一路发展 　　干一行，专一行，精一行": {"topic": "“生产投资”", "similarity": 0.5106342434883118, "prompt": "新闻文本是“从平凡到不凡他们见证一路发展 　　干一行，专一行，精一行”，包含的情绪词典是：熟练/精通(proficiency):0.5,熟练的/精通的(proficient):0.6"}, "在农行萧山分行，员工按照入职年份获得“员工礼”，年份最长的员工，已经进入农行工作40余年，从激情到稳重，从稚嫩到成熟，从一头黑发到两鬓斑白，从一名青年蜕变成农行栋梁": {"topic": "“消费”", "similarity": 0.5225637555122375}, "40年，他们见证历史，用汗水、智慧和忠诚谱写了农行萧山分行波澜壮阔的发展篇章": {"topic": "“金融”", "similarity": 0.4678669571876526, "prompt": "新闻文本是“40年，他们见证历史，用汗水、智慧和忠诚谱写了农行萧山分行波澜壮阔的发展篇章”，包含的情绪词典是：历史的/历史性的(historical):0.0,农业的/农学的(agricultural):0.0"}, "“我见证了金融业脱胎换骨的变化：从珠算到计算机到AI人工智能的应用": {"topic": "“金融”", "similarity": 0.42567476630210876, "prompt": "新闻文本是““我见证了金融业脱胎换骨的变化：从珠算到计算机到AI人工智能的应用”，包含的情绪词典是：金融的/财政的(financial):0.0,计算/核算(calculate):0.0"}, "见证了祖国日新月异的变化": {"topic": "“生产投资”", "similarity": 0.4913620948791504, "prompt": "新闻文本是“见证了祖国日新月异的变化”，包含的情绪词典是：改变/变化(vary):0.0,变化/变异(variation):0.0"}, "同时也见证了农行的蓬勃发展": {"topic": "“金融”", "similarity": 0.49572378396987915, "prompt": "新闻文本是“同时也见证了农行的蓬勃发展”，包含的情绪词典是：繁荣/兴旺(prospering):0.7,繁荣/兴旺(exuberance):0.6"}, "这十年，她对农行、对银行、对金融有了属于自己的认识": {"topic": "“金融”", "similarity": 0.4607347249984741, "prompt": "新闻文本是“这十年，她对农行、对银行、对金融有了属于自己的认识”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "“有陪伴、有教导、有收获、有成长，最终这3650天的点点滴滴都化为我成长路上的珍贵回忆，支撑着我克服惰性、松懈和缺点，努力成为这大家庭里更好的一份子": {"topic": "“消费”", "similarity": 0.4689076542854309, "prompt": "新闻文本是““有陪伴、有教导、有收获、有成长，最终这3650天的点点滴滴都化为我成长路上的珍贵回忆，支撑着我克服惰性、松懈和缺点，努力成为这大家庭里更好的一份子”，包含的情绪词典是：生长/成长(grow):0.6,成就/成绩(accomplishment):0.5"}, "自2017年起，农行萧山分行已连续八年对不同行龄的员工进行表彰，感谢员工们辛勤付出的同时，更表达关怀与肯定，截至目前，共表彰1081人次": {"topic": "“消费”", "similarity": 0.4877377152442932}, "家园文化让爱与成长薪火相传 　　活动现场，各单位通过舞蹈、情景剧、配音秀、说唱、小组唱、诗歌朗诵等多种演绎形式，集中展示了农行萧山分行家园文化建设的最新成果，充分展现全行员工爱党爱行、积极向上的良好精神风貌": {"topic": "“消费”", "similarity": 0.4835894703865051, "prompt": "新闻文本是“家园文化让爱与成长薪火相传 　　活动现场，各单位通过舞蹈、情景剧、配音秀、说唱、小组唱、诗歌朗诵等多种演绎形式，集中展示了农行萧山分行家园文化建设的最新成果，充分展现全行员工爱党爱行、积极向上的良好精神风貌”，包含的情绪词典是：家/家庭(home):0.0,家庭/户(household):0.0"}, "歌曲《飘向北方》献给所有异地员工，为每一个来自五湖四海的员工鼓掌": {"topic": "“生产投资”", "similarity": 0.45543962717056274, "prompt": "新闻文本是“歌曲《飘向北方》献给所有异地员工，为每一个来自五湖四海的员工鼓掌”，包含的情绪词典是：北方/北部(north):0.0,公司的/企业的(corporate):0.0"}, "情景剧《跨越时空的电台》让大家在欢笑中看到平时工作中的自己，展现着农行人的责任与担当": {"topic": "“金融”", "similarity": 0.46177518367767334, "prompt": "新闻文本是“情景剧《跨越时空的电台》让大家在欢笑中看到平时工作中的自己，展现着农行人的责任与担当”，包含的情绪词典是：阶段/舞台(stage):0.0,在某时(sometime):0.0"}, "情景剧《反诈风云》聚焦了一次特殊的业务办理，以来自银行的温暖力量，守护每一份来之不易的安宁与信任": {"topic": "“金融”", "similarity": 0.48433977365493774, "prompt": "新闻文本是“情景剧《反诈风云》聚焦了一次特殊的业务办理，以来自银行的温暖力量，守护每一份来之不易的安宁与信任”，包含的情绪词典是：欺诈/诈骗(fraud):-0.8,欺诈的/诈骗的(fraudulent):-0.8"}, "配音秀《甄嬛传之合规经营篇》以独特的创意诠释“安全”这一银行经营的基础…… 　　在现场，“家园文化”成为高频词汇": {"topic": "“金融”", "similarity": 0.4974193572998047, "prompt": "新闻文本是“配音秀《甄嬛传之合规经营篇》以独特的创意诠释“安全”这一银行经营的基础…… 　　在现场，“家园文化”成为高频词汇”，包含的情绪词典是：有礼貌的/谦恭的(courteous):0.3,银行/河岸(bank):0.0"}, "正如农行萧山分行相关负责人所说，作为改革开放后萧山辖区内第一家从人民银行分设的国有银行，农行萧山分行成立40多年来，成果颇丰": {"topic": "“金融”", "similarity": 0.5217552781105042}, "这背后离不开每一位员工的奋勇拼搏": {"topic": "“生产投资”", "similarity": 0.4553191661834717, "prompt": "新闻文本是“这背后离不开每一位员工的奋勇拼搏”，包含的情绪词典是：勤奋的/勤勉的(diligent):0.4,勤奋地/勤勉地(diligently):0.4"}, "通过以业务技能、拜师“传帮带”、专业培训为主要内容的培养机制，以及各种具有知识性、趣味性的特色活动，农行充分调动员工参与“家园”建设活动的积极性，激发了员工爱岗敬业、奋发向上的工作热情，增进凝聚力和感召力": {"topic": "“消费”", "similarity": 0.5568172931671143, "prompt": "新闻文本是“通过以业务技能、拜师“传帮带”、专业培训为主要内容的培养机制，以及各种具有知识性、趣味性的特色活动，农行充分调动员工参与“家园”建设活动的积极性，激发了员工爱岗敬业、奋发向上的工作热情，增进凝聚力和感召力”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,家/家庭(home):0.0"}, "当前，农行萧山分行所辖29家营业网点“职工之家”覆盖率达100%": {"topic": "“消费”", "similarity": 0.4323253929615021, "prompt": "新闻文本是“当前，农行萧山分行所辖29家营业网点“职工之家”覆盖率达100%”，包含的情绪词典是：百分比(percentage):0.0,劳动力/职工总数(workforce):0.01"}, "“员工礼”的出现，是员工职业生涯价值的体现，也是农业银行萧山分行“家园文化”建设的重要载体，激荡着人心": {"topic": "“消费”", "similarity": 0.4825224280357361, "prompt": "新闻文本是““员工礼”的出现，是员工职业生涯价值的体现，也是农业银行萧山分行“家园文化”建设的重要载体，激荡着人心”，包含的情绪词典是：有礼貌的/谦恭的(courteous):0.3,有功的/值得赞扬的(meritorious):0.6"}}</t>
+          <t>{"能够成就伟大者，无不是由点点滴滴的平凡积累而成": {"topic": "“消费”", "similarity": 0.4201946258544922, "prompt": "新闻文本是“能够成就伟大者，无不是由点点滴滴的平凡积累而成”，包含的情绪词典是：成就/成绩(accomplishment):0.5,成就/成绩(achievement):0.5"}, "表彰会的主角，是来自各个岗位的员工，他们日复一日坚守在平凡岗位上，脚踏实地、默默耕耘，与农行同奋进、共成长": {"topic": "“消费”", "similarity": 0.5014984607696533, "prompt": "新闻文本是“表彰会的主角，是来自各个岗位的员工，他们日复一日坚守在平凡岗位上，脚踏实地、默默耕耘，与农行同奋进、共成长”，包含的情绪词典是：勤奋地/勤勉地(diligently):0.4,成就/成绩(achievement):0.5"}, "在职5年、10年、20年、30年、35年/40年的员工分别获得“成长礼”、“担当礼”、“敬业礼”、“忠诚礼”和“荣耀礼”五个“员工礼”": {"topic": "“生产投资”", "similarity": 0.5444313883781433, "prompt": "新闻文本是“在职5年、10年、20年、30年、35年/40年的员工分别获得“成长礼”、“担当礼”、“敬业礼”、“忠诚礼”和“荣耀礼”五个“员工礼””，包含的情绪词典是：荣誉/光荣(honors):0.4,荣誉/名誉(honor):0.4"}, "活动通过“视频+图片”直播的方式，全行近700名员工和家属代表共赴一场精神传承的盛会": {"topic": "“消费”", "similarity": 0.44132959842681885, "prompt": "新闻文本是“活动通过“视频+图片”直播的方式，全行近700名员工和家属代表共赴一场精神传承的盛会”，包含的情绪词典是：活动/行动(activity):0.2,银行/河岸(bank):0.0"}, "从平凡到不凡他们见证一路发展 　　干一行，专一行，精一行": {"topic": "“生产投资”", "similarity": 0.5106343030929565, "prompt": "新闻文本是“从平凡到不凡他们见证一路发展 　　干一行，专一行，精一行”，包含的情绪词典是：熟练/精通(proficiency):0.5,熟练的/精通的(proficient):0.6"}, "40年，他们见证历史，用汗水、智慧和忠诚谱写了农行萧山分行波澜壮阔的发展篇章": {"topic": "“金融”", "similarity": 0.4678671956062317, "prompt": "新闻文本是“40年，他们见证历史，用汗水、智慧和忠诚谱写了农行萧山分行波澜壮阔的发展篇章”，包含的情绪词典是：历史的/历史性的(historical):0.0,农业的/农学的(agricultural):0.0"}, "“我见证了金融业脱胎换骨的变化：从珠算到计算机到AI人工智能的应用": {"topic": "“金融”", "similarity": 0.4256749153137207, "prompt": "新闻文本是““我见证了金融业脱胎换骨的变化：从珠算到计算机到AI人工智能的应用”，包含的情绪词典是：金融的/财政的(financial):0.0,计算/核算(calculate):0.0"}, "见证了祖国日新月异的变化": {"topic": "“生产投资”", "similarity": 0.49136215448379517, "prompt": "新闻文本是“见证了祖国日新月异的变化”，包含的情绪词典是：改变/变化(vary):0.0,变化/变异(variation):0.0"}, "同时也见证了农行的蓬勃发展": {"topic": "“金融”", "similarity": 0.4957239031791687, "prompt": "新闻文本是“同时也见证了农行的蓬勃发展”，包含的情绪词典是：繁荣/兴旺(prospering):0.7,繁荣/兴旺(exuberance):0.6"}, "这十年，她对农行、对银行、对金融有了属于自己的认识": {"topic": "“金融”", "similarity": 0.46073490381240845, "prompt": "新闻文本是“这十年，她对农行、对银行、对金融有了属于自己的认识”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "“有陪伴、有教导、有收获、有成长，最终这3650天的点点滴滴都化为我成长路上的珍贵回忆，支撑着我克服惰性、松懈和缺点，努力成为这大家庭里更好的一份子": {"topic": "“消费”", "similarity": 0.46890780329704285, "prompt": "新闻文本是““有陪伴、有教导、有收获、有成长，最终这3650天的点点滴滴都化为我成长路上的珍贵回忆，支撑着我克服惰性、松懈和缺点，努力成为这大家庭里更好的一份子”，包含的情绪词典是：生长/成长(grow):0.6,成就/成绩(accomplishment):0.5"}, "家园文化让爱与成长薪火相传 　　活动现场，各单位通过舞蹈、情景剧、配音秀、说唱、小组唱、诗歌朗诵等多种演绎形式，集中展示了农行萧山分行家园文化建设的最新成果，充分展现全行员工爱党爱行、积极向上的良好精神风貌": {"topic": "“消费”", "similarity": 0.48358967900276184, "prompt": "新闻文本是“家园文化让爱与成长薪火相传 　　活动现场，各单位通过舞蹈、情景剧、配音秀、说唱、小组唱、诗歌朗诵等多种演绎形式，集中展示了农行萧山分行家园文化建设的最新成果，充分展现全行员工爱党爱行、积极向上的良好精神风貌”，包含的情绪词典是：家/家庭(home):0.0,家庭/户(household):0.0"}, "歌曲《飘向北方》献给所有异地员工，为每一个来自五湖四海的员工鼓掌": {"topic": "“生产投资”", "similarity": 0.4554397165775299, "prompt": "新闻文本是“歌曲《飘向北方》献给所有异地员工，为每一个来自五湖四海的员工鼓掌”，包含的情绪词典是：北方/北部(north):0.0,公司的/企业的(corporate):0.0"}, "情景剧《跨越时空的电台》让大家在欢笑中看到平时工作中的自己，展现着农行人的责任与担当": {"topic": "“金融”", "similarity": 0.46177512407302856, "prompt": "新闻文本是“情景剧《跨越时空的电台》让大家在欢笑中看到平时工作中的自己，展现着农行人的责任与担当”，包含的情绪词典是：阶段/舞台(stage):0.0,在某时(sometime):0.0"}, "情景剧《反诈风云》聚焦了一次特殊的业务办理，以来自银行的温暖力量，守护每一份来之不易的安宁与信任": {"topic": "“金融”", "similarity": 0.4843398928642273, "prompt": "新闻文本是“情景剧《反诈风云》聚焦了一次特殊的业务办理，以来自银行的温暖力量，守护每一份来之不易的安宁与信任”，包含的情绪词典是：欺诈/诈骗(fraud):-0.8,欺诈的/诈骗的(fraudulent):-0.8"}, "配音秀《甄嬛传之合规经营篇》以独特的创意诠释“安全”这一银行经营的基础…… 　　在现场，“家园文化”成为高频词汇": {"topic": "“金融”", "similarity": 0.4974193572998047, "prompt": "新闻文本是“配音秀《甄嬛传之合规经营篇》以独特的创意诠释“安全”这一银行经营的基础…… 　　在现场，“家园文化”成为高频词汇”，包含的情绪词典是：有礼貌的/谦恭的(courteous):0.3,银行/河岸(bank):0.0"}, "这背后离不开每一位员工的奋勇拼搏": {"topic": "“生产投资”", "similarity": 0.4553191363811493, "prompt": "新闻文本是“这背后离不开每一位员工的奋勇拼搏”，包含的情绪词典是：勤奋的/勤勉的(diligent):0.4,勤奋地/勤勉地(diligently):0.4"}, "通过以业务技能、拜师“传帮带”、专业培训为主要内容的培养机制，以及各种具有知识性、趣味性的特色活动，农行充分调动员工参与“家园”建设活动的积极性，激发了员工爱岗敬业、奋发向上的工作热情，增进凝聚力和感召力": {"topic": "“消费”", "similarity": 0.5568172931671143, "prompt": "新闻文本是“通过以业务技能、拜师“传帮带”、专业培训为主要内容的培养机制，以及各种具有知识性、趣味性的特色活动，农行充分调动员工参与“家园”建设活动的积极性，激发了员工爱岗敬业、奋发向上的工作热情，增进凝聚力和感召力”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,家/家庭(home):0.0"}, "当前，农行萧山分行所辖29家营业网点“职工之家”覆盖率达100%": {"topic": "“消费”", "similarity": 0.432325541973114, "prompt": "新闻文本是“当前，农行萧山分行所辖29家营业网点“职工之家”覆盖率达100%”，包含的情绪词典是：百分比(percentage):0.0,劳动力/职工总数(workforce):0.01"}, "“员工礼”的出现，是员工职业生涯价值的体现，也是农业银行萧山分行“家园文化”建设的重要载体，激荡着人心": {"topic": "“消费”", "similarity": 0.48252248764038086, "prompt": "新闻文本是““员工礼”的出现，是员工职业生涯价值的体现，也是农业银行萧山分行“家园文化”建设的重要载体，激荡着人心”，包含的情绪词典是：有礼貌的/谦恭的(courteous):0.3,有功的/值得赞扬的(meritorious):0.6"}}</t>
         </is>
       </c>
     </row>
@@ -4558,12 +4518,12 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "8月30日，恒辉安防（300952.SZ）发布2024年半年报", "news_prompt2": "报告显示，2024年上半年，公司实现营业收入5.14亿元，同比增长16.51%", "news_prompt3": "归属于上市公司股东的净利润为4916.40万元，同比增加17.09%", "news_prompt4": "报告期内，公司不断深化全产业布局，以高质量发展为导向、以科技创新为引领，加快产业链资源整合，在传统功能性安全防护手套基础板块之外，积极向战略新材料板块拓展，一方面满足公司对高端核心原材料的需求保障，同时开辟第二、第三成长曲线，助推公司高质量可持续发展", "news_prompt5": "聚焦主业，深耕功能性安全防护手套领域 　　资料显示，恒辉安防成立于2004年，主要从事手部安全防护用品、超高分子量聚乙烯纤维及其复合纤维的研发、生产及销售，同时，也是江苏省科技厅、财政厅、税务局联合认定的高新技术企业", "news_prompt6": "从行业发展趋势来看，目前，功能性安全防护手套替代普通安全防护手套已成为各国安全生产及劳动保护的发展趋势", "news_prompt7": "恒辉安防是国内较早从事功能性安全防护手套业务的企业之一", "news_prompt8": "经过多年持续的研发投入和工艺改进，公司掌握了数十种高性能涂层配方和浸渍工艺，以及高性能纤维新材料制备技术、包覆及针织技术、专用设备适应性改造技术等一系列核心技术和工艺", "news_prompt9": "公司产品规格型号多达百余种，能够为客户提供功能性安全防护手套产品一站式服务", "news_prompt10": "产品销售区域覆盖全球50多个国家和地区，多项产品通过了欧盟CE认证、美国ANSI认证、日本JIS认证或OEKO-TEX Standard 100认证等严格的国际级认证", "news_prompt11": "凭借持续的技术开发、严格的质量控制和稳定的产品性能，公司功能性安全防护手套的销售及出口规模逐年增长，市场影响力不断扩大，已跻身于我国功能性安全防护手套领域的第一梯队", "news_prompt12": "布局超高分子量聚乙烯产业链 　　近年来，超高分子量聚乙烯纤维在产品性能逐渐提升、应用领域稳步拓展，产能规模不断加码三重因素带动的背景下，其需求在全球范围内稳定增长", "news_prompt13": "根据中商研究院发布的数据，2022年全球超高分子量聚乙烯纤维的需求量约为12.68万吨，2020年至2022年复合增长率达13.75%，到2026年需求量将达到22.72万吨", "news_prompt14": "我国超高分子量聚乙烯纤维的产业化时间晚于国际市场，但市场需求量逐年攀升，由2015年的约2万吨攀升至2022年的6.76万吨，其间增速约19%", "news_prompt15": "另外，我国于2019年在《重点新材料首批次应用示范指导目录》中将超高分子量聚乙烯纤维定义为关键战略材料", "news_prompt16": "同年，国内超高分子量聚乙烯纤维的理论需求量4.25万吨首次超越了国内产能4.10万吨，并在2020年显现出差距扩大的趋势，未来国内整体行业的供需关系将更加显现出供不应求的趋势", "news_prompt17": "2022年中国超高分子量聚乙烯纤维需求量为6.76万吨，产能为4.78万吨", "news_prompt18": "恒辉安防半年报显示，报告期内，公司加速推进子公司恒尚材料“超纤维新材料及功能性安全防护用品开发应用项目”建设及产线磨合、 工艺制备技术突破、产线提质增效，公司超高分子量聚乙烯纤维满负荷产能已经达到3000吨", "news_prompt19": "同时，公司还在规划建设的产能4800吨，系公司拟发行可转债募集资金投资项目，该项目为公司安防产业园“年产12000吨超高分子量聚乙烯纤维”一期建设项目", "news_prompt20": "恒辉安防表示，通过这一项目的建设，一方面可以保障公司主营业务上游原材料的稳定供应、控制原材料价格波动风险", "news_prompt21": "另一方面，也是响应国家提升高性能纤维生产应用水平的发展目标，让公司把握高性能纤维产业的发展机遇，更快发展新质生产力", "news_prompt22": "随着超高分子量聚乙烯纤维及其复合材料产能的释放，公司将成为国内少数几家实现超高分子量聚乙烯纤维及其复合材料规模化生产的企业之一，拥有超高分子量聚乙烯纤维行业生产及应用端全产业链布局，预计未来几年整体行业订单将保持充足", "news_prompt23": "值得一提的是，在全球化布局方面，恒辉安防在越南工厂项目目前进展顺利，综合办公楼已结构封顶，预计明年下半年将贡献产能", "news_prompt24": "同时，公司还积极与国内知名企业建立战略合作关系，构建多地域、多渠道的运营架构，以应对市场不确定性风险", "news_prompt25": "（齐和宁）（文章来源：证券时报网）"}</t>
+          <t>{"news_prompt1": "8月30日，恒辉安防（300952.SZ）发布2024年半年报", "news_prompt2": "报告显示，2024年上半年，公司实现营业收入5.14亿元，同比增长16.51%", "news_prompt3": "聚焦主业，深耕功能性安全防护手套领域 　　资料显示，恒辉安防成立于2004年，主要从事手部安全防护用品、超高分子量聚乙烯纤维及其复合纤维的研发、生产及销售，同时，也是江苏省科技厅、财政厅、税务局联合认定的高新技术企业", "news_prompt4": "从行业发展趋势来看，目前，功能性安全防护手套替代普通安全防护手套已成为各国安全生产及劳动保护的发展趋势", "news_prompt5": "经过多年持续的研发投入和工艺改进，公司掌握了数十种高性能涂层配方和浸渍工艺，以及高性能纤维新材料制备技术、包覆及针织技术、专用设备适应性改造技术等一系列核心技术和工艺", "news_prompt6": "产品销售区域覆盖全球50多个国家和地区，多项产品通过了欧盟CE认证、美国ANSI认证、日本JIS认证或OEKO-TEX Standard 100认证等严格的国际级认证", "news_prompt7": "凭借持续的技术开发、严格的质量控制和稳定的产品性能，公司功能性安全防护手套的销售及出口规模逐年增长，市场影响力不断扩大，已跻身于我国功能性安全防护手套领域的第一梯队", "news_prompt8": "布局超高分子量聚乙烯产业链 　　近年来，超高分子量聚乙烯纤维在产品性能逐渐提升、应用领域稳步拓展，产能规模不断加码三重因素带动的背景下，其需求在全球范围内稳定增长", "news_prompt9": "另外，我国于2019年在《重点新材料首批次应用示范指导目录》中将超高分子量聚乙烯纤维定义为关键战略材料", "news_prompt10": "同年，国内超高分子量聚乙烯纤维的理论需求量4.25万吨首次超越了国内产能4.10万吨，并在2020年显现出差距扩大的趋势，未来国内整体行业的供需关系将更加显现出供不应求的趋势", "news_prompt11": "2022年中国超高分子量聚乙烯纤维需求量为6.76万吨，产能为4.78万吨", "news_prompt12": "恒辉安防半年报显示，报告期内，公司加速推进子公司恒尚材料“超纤维新材料及功能性安全防护用品开发应用项目”建设及产线磨合、 工艺制备技术突破、产线提质增效，公司超高分子量聚乙烯纤维满负荷产能已经达到3000吨", "news_prompt13": "同时，公司还在规划建设的产能4800吨，系公司拟发行可转债募集资金投资项目，该项目为公司安防产业园“年产12000吨超高分子量聚乙烯纤维”一期建设项目", "news_prompt14": "恒辉安防表示，通过这一项目的建设，一方面可以保障公司主营业务上游原材料的稳定供应、控制原材料价格波动风险", "news_prompt15": "另一方面，也是响应国家提升高性能纤维生产应用水平的发展目标，让公司把握高性能纤维产业的发展机遇，更快发展新质生产力", "news_prompt16": "值得一提的是，在全球化布局方面，恒辉安防在越南工厂项目目前进展顺利，综合办公楼已结构封顶，预计明年下半年将贡献产能", "news_prompt17": "同时，公司还积极与国内知名企业建立战略合作关系，构建多地域、多渠道的运营架构，以应对市场不确定性风险"}</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>{"8月30日，恒辉安防（300952.SZ）发布2024年半年报": {"topic": "“金融”", "similarity": 0.4802634119987488, "prompt": "新闻文本是“8月30日，恒辉安防（300952.SZ）发布2024年半年报”，包含的情绪词典是：表现不佳/业绩低于预期(underperforms):-0.4,表现不佳/业绩低于预期(underperformance):-0.4"}, "报告显示，2024年上半年，公司实现营业收入5.14亿元，同比增长16.51%": {"topic": "“生产投资”", "similarity": 0.4688622057437897, "prompt": "新闻文本是“报告显示，2024年上半年，公司实现营业收入5.14亿元，同比增长16.51%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,增长/发展(growth):0.7"}, "报告期内，公司不断深化全产业布局，以高质量发展为导向、以科技创新为引领，加快产业链资源整合，在传统功能性安全防护手套基础板块之外，积极向战略新材料板块拓展，一方面满足公司对高端核心原材料的需求保障，同时开辟第二、第三成长曲线，助推公司高质量可持续发展": {"topic": "“生产投资”", "similarity": 0.5347171425819397}, "聚焦主业，深耕功能性安全防护手套领域 　　资料显示，恒辉安防成立于2004年，主要从事手部安全防护用品、超高分子量聚乙烯纤维及其复合纤维的研发、生产及销售，同时，也是江苏省科技厅、财政厅、税务局联合认定的高新技术企业": {"topic": "“生产投资”", "similarity": 0.5294289588928223, "prompt": "新闻文本是“聚焦主业，深耕功能性安全防护手套领域 　　资料显示，恒辉安防成立于2004年，主要从事手部安全防护用品、超高分子量聚乙烯纤维及其复合纤维的研发、生产及销售，同时，也是江苏省科技厅、财政厅、税务局联合认定的高新技术企业”，包含的情绪词典是：手/人手(hand):0.0"}, "从行业发展趋势来看，目前，功能性安全防护手套替代普通安全防护手套已成为各国安全生产及劳动保护的发展趋势": {"topic": "“生产投资”", "similarity": 0.4988335967063904, "prompt": "新闻文本是“从行业发展趋势来看，目前，功能性安全防护手套替代普通安全防护手套已成为各国安全生产及劳动保护的发展趋势”，包含的情绪词典是：预防措施/防范(precaution):0.0,多才多艺/多功能性(versatility):0.5"}, "经过多年持续的研发投入和工艺改进，公司掌握了数十种高性能涂层配方和浸渍工艺，以及高性能纤维新材料制备技术、包覆及针织技术、专用设备适应性改造技术等一系列核心技术和工艺": {"topic": "“生产投资”", "similarity": 0.5537825226783752, "prompt": "新闻文本是“经过多年持续的研发投入和工艺改进，公司掌握了数十种高性能涂层配方和浸渍工艺，以及高性能纤维新材料制备技术、包覆及针织技术、专用设备适应性改造技术等一系列核心技术和工艺”，包含的情绪词典是：技术的/工艺的(technical):0.0,公司的/企业的(corporate):0.0"}, "产品销售区域覆盖全球50多个国家和地区，多项产品通过了欧盟CE认证、美国ANSI认证、日本JIS认证或OEKO-TEX Standard 100认证等严格的国际级认证": {"topic": "“消费”", "similarity": 0.5332226753234863, "prompt": "新闻文本是“产品销售区域覆盖全球50多个国家和地区，多项产品通过了欧盟CE认证、美国ANSI认证、日本JIS认证或OEKO-TEX Standard 100认证等严格的国际级认证”，包含的情绪词典是：全世界的/在世界范围内(worldwide):0.0,全球的/全世界的(global):0.0"}, "凭借持续的技术开发、严格的质量控制和稳定的产品性能，公司功能性安全防护手套的销售及出口规模逐年增长，市场影响力不断扩大，已跻身于我国功能性安全防护手套领域的第一梯队": {"topic": "“生产投资”", "similarity": 0.47092968225479126, "prompt": "新闻文本是“凭借持续的技术开发、严格的质量控制和稳定的产品性能，公司功能性安全防护手套的销售及出口规模逐年增长，市场影响力不断扩大，已跻身于我国功能性安全防护手套领域的第一梯队”，包含的情绪词典是：多才多艺/多功能性(versatility):0.5,公司的/企业的(corporate):0.0"}, "布局超高分子量聚乙烯产业链 　　近年来，超高分子量聚乙烯纤维在产品性能逐渐提升、应用领域稳步拓展，产能规模不断加码三重因素带动的背景下，其需求在全球范围内稳定增长": {"topic": "“生产投资”", "similarity": 0.6315768957138062, "prompt": "新闻文本是“布局超高分子量聚乙烯产业链 　　近年来，超高分子量聚乙烯纤维在产品性能逐渐提升、应用领域稳步拓展，产能规模不断加码三重因素带动的背景下，其需求在全球范围内稳定增长”，包含的情绪词典是：广泛的/大规模的(extensive):0.2,高的/高等的(high):0.7"}, "根据中商研究院发布的数据，2022年全球超高分子量聚乙烯纤维的需求量约为12.68万吨，2020年至2022年复合增长率达13.75%，到2026年需求量将达到22.72万吨": {"topic": "“生产投资”", "similarity": 0.4972380995750427}, "我国超高分子量聚乙烯纤维的产业化时间晚于国际市场，但市场需求量逐年攀升，由2015年的约2万吨攀升至2022年的6.76万吨，其间增速约19%": {"topic": "“生产投资”", "similarity": 0.5051158666610718}, "另外，我国于2019年在《重点新材料首批次应用示范指导目录》中将超高分子量聚乙烯纤维定义为关键战略材料": {"topic": "“生产投资”", "similarity": 0.5936303734779358, "prompt": "新闻文本是“另外，我国于2019年在《重点新材料首批次应用示范指导目录》中将超高分子量聚乙烯纤维定义为关键战略材料”，包含的情绪词典是：高的/高等的(high):0.7,最高的/最高级的(highest):0.7"}, "同年，国内超高分子量聚乙烯纤维的理论需求量4.25万吨首次超越了国内产能4.10万吨，并在2020年显现出差距扩大的趋势，未来国内整体行业的供需关系将更加显现出供不应求的趋势": {"topic": "“生产投资”", "similarity": 0.5938977003097534, "prompt": "新闻文本是“同年，国内超高分子量聚乙烯纤维的理论需求量4.25万吨首次超越了国内产能4.10万吨，并在2020年显现出差距扩大的趋势，未来国内整体行业的供需关系将更加显现出供不应求的趋势”，包含的情绪词典是：产能过剩(overcapacity):-0.5,超过量/超越量(exceedances):0.2"}, "2022年中国超高分子量聚乙烯纤维需求量为6.76万吨，产能为4.78万吨": {"topic": "“生产投资”", "similarity": 0.5091560482978821, "prompt": "新闻文本是“2022年中国超高分子量聚乙烯纤维需求量为6.76万吨，产能为4.78万吨”，包含的情绪词典是：生产不足的/产量低于预期的(underproduced):-0.5,生产不足/产量低于预期(underproduction):-0.5"}, "恒辉安防半年报显示，报告期内，公司加速推进子公司恒尚材料“超纤维新材料及功能性安全防护用品开发应用项目”建设及产线磨合、 工艺制备技术突破、产线提质增效，公司超高分子量聚乙烯纤维满负荷产能已经达到3000吨": {"topic": "“生产投资”", "similarity": 0.5414124727249146, "prompt": "新闻文本是“恒辉安防半年报显示，报告期内，公司加速推进子公司恒尚材料“超纤维新材料及功能性安全防护用品开发应用项目”建设及产线磨合、 工艺制备技术突破、产线提质增效，公司超高分子量聚乙烯纤维满负荷产能已经达到3000吨”，包含的情绪词典是：可防御的/可保卫的(defendable):0.3"}, "同时，公司还在规划建设的产能4800吨，系公司拟发行可转债募集资金投资项目，该项目为公司安防产业园“年产12000吨超高分子量聚乙烯纤维”一期建设项目": {"topic": "“生产投资”", "similarity": 0.6194550395011902, "prompt": "新闻文本是“同时，公司还在规划建设的产能4800吨，系公司拟发行可转债募集资金投资项目，该项目为公司安防产业园“年产12000吨超高分子量聚乙烯纤维”一期建设项目”，包含的情绪词典是：产能过剩(overcapacity):-0.5,生产过剩的/过度生产的(overproduced):-0.3"}, "恒辉安防表示，通过这一项目的建设，一方面可以保障公司主营业务上游原材料的稳定供应、控制原材料价格波动风险": {"topic": "“生产投资”", "similarity": 0.519359290599823, "prompt": "新闻文本是“恒辉安防表示，通过这一项目的建设，一方面可以保障公司主营业务上游原材料的稳定供应、控制原材料价格波动风险”，包含的情绪词典是：稳定的/稳固的(stable):0.5,保证/确保(assures):0.3"}, "另一方面，也是响应国家提升高性能纤维生产应用水平的发展目标，让公司把握高性能纤维产业的发展机遇，更快发展新质生产力": {"topic": "“生产投资”", "similarity": 0.6215603947639465, "prompt": "新闻文本是“另一方面，也是响应国家提升高性能纤维生产应用水平的发展目标，让公司把握高性能纤维产业的发展机遇，更快发展新质生产力”，包含的情绪词典是：增强的/提高的(enhanced):0.6,多产的/富有成效的(productive):0.7"}, "随着超高分子量聚乙烯纤维及其复合材料产能的释放，公司将成为国内少数几家实现超高分子量聚乙烯纤维及其复合材料规模化生产的企业之一，拥有超高分子量聚乙烯纤维行业生产及应用端全产业链布局，预计未来几年整体行业订单将保持充足": {"topic": "“生产投资”", "similarity": 0.5801183581352234}, "值得一提的是，在全球化布局方面，恒辉安防在越南工厂项目目前进展顺利，综合办公楼已结构封顶，预计明年下半年将贡献产能": {"topic": "“生产投资”", "similarity": 0.5430521368980408, "prompt": "新闻文本是“值得一提的是，在全球化布局方面，恒辉安防在越南工厂项目目前进展顺利，综合办公楼已结构封顶，预计明年下半年将贡献产能”，包含的情绪词典是：工厂/制造厂(factory):0.0,工业/产业(industry):0.0"}, "同时，公司还积极与国内知名企业建立战略合作关系，构建多地域、多渠道的运营架构，以应对市场不确定性风险": {"topic": "“金融”", "similarity": 0.5258092880249023, "prompt": "新闻文本是“同时，公司还积极与国内知名企业建立战略合作关系，构建多地域、多渠道的运营架构，以应对市场不确定性风险”，包含的情绪词典是：合作性的/协作性的(collaborative):0.3,公司/企业(company):0.0"}}</t>
+          <t>{"8月30日，恒辉安防（300952.SZ）发布2024年半年报": {"topic": "“金融”", "similarity": 0.4802634119987488, "prompt": "新闻文本是“8月30日，恒辉安防（300952.SZ）发布2024年半年报”，包含的情绪词典是：表现不佳/业绩低于预期(underperforms):-0.4,表现不佳/业绩低于预期(underperformance):-0.4"}, "报告显示，2024年上半年，公司实现营业收入5.14亿元，同比增长16.51%": {"topic": "“生产投资”", "similarity": 0.4688624441623688, "prompt": "新闻文本是“报告显示，2024年上半年，公司实现营业收入5.14亿元，同比增长16.51%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,增长/发展(growth):0.7"}, "聚焦主业，深耕功能性安全防护手套领域 　　资料显示，恒辉安防成立于2004年，主要从事手部安全防护用品、超高分子量聚乙烯纤维及其复合纤维的研发、生产及销售，同时，也是江苏省科技厅、财政厅、税务局联合认定的高新技术企业": {"topic": "“生产投资”", "similarity": 0.5294290781021118, "prompt": "新闻文本是“聚焦主业，深耕功能性安全防护手套领域 　　资料显示，恒辉安防成立于2004年，主要从事手部安全防护用品、超高分子量聚乙烯纤维及其复合纤维的研发、生产及销售，同时，也是江苏省科技厅、财政厅、税务局联合认定的高新技术企业”，包含的情绪词典是：手/人手(hand):0.0"}, "从行业发展趋势来看，目前，功能性安全防护手套替代普通安全防护手套已成为各国安全生产及劳动保护的发展趋势": {"topic": "“生产投资”", "similarity": 0.4988335967063904, "prompt": "新闻文本是“从行业发展趋势来看，目前，功能性安全防护手套替代普通安全防护手套已成为各国安全生产及劳动保护的发展趋势”，包含的情绪词典是：预防措施/防范(precaution):0.0,多才多艺/多功能性(versatility):0.5"}, "经过多年持续的研发投入和工艺改进，公司掌握了数十种高性能涂层配方和浸渍工艺，以及高性能纤维新材料制备技术、包覆及针织技术、专用设备适应性改造技术等一系列核心技术和工艺": {"topic": "“生产投资”", "similarity": 0.5537825226783752, "prompt": "新闻文本是“经过多年持续的研发投入和工艺改进，公司掌握了数十种高性能涂层配方和浸渍工艺，以及高性能纤维新材料制备技术、包覆及针织技术、专用设备适应性改造技术等一系列核心技术和工艺”，包含的情绪词典是：技术的/工艺的(technical):0.0,公司的/企业的(corporate):0.0"}, "产品销售区域覆盖全球50多个国家和地区，多项产品通过了欧盟CE认证、美国ANSI认证、日本JIS认证或OEKO-TEX Standard 100认证等严格的国际级认证": {"topic": "“消费”", "similarity": 0.5332226753234863, "prompt": "新闻文本是“产品销售区域覆盖全球50多个国家和地区，多项产品通过了欧盟CE认证、美国ANSI认证、日本JIS认证或OEKO-TEX Standard 100认证等严格的国际级认证”，包含的情绪词典是：全世界的/在世界范围内(worldwide):0.0,全球的/全世界的(global):0.0"}, "凭借持续的技术开发、严格的质量控制和稳定的产品性能，公司功能性安全防护手套的销售及出口规模逐年增长，市场影响力不断扩大，已跻身于我国功能性安全防护手套领域的第一梯队": {"topic": "“生产投资”", "similarity": 0.47092968225479126, "prompt": "新闻文本是“凭借持续的技术开发、严格的质量控制和稳定的产品性能，公司功能性安全防护手套的销售及出口规模逐年增长，市场影响力不断扩大，已跻身于我国功能性安全防护手套领域的第一梯队”，包含的情绪词典是：多才多艺/多功能性(versatility):0.5,公司的/企业的(corporate):0.0"}, "布局超高分子量聚乙烯产业链 　　近年来，超高分子量聚乙烯纤维在产品性能逐渐提升、应用领域稳步拓展，产能规模不断加码三重因素带动的背景下，其需求在全球范围内稳定增长": {"topic": "“生产投资”", "similarity": 0.6315768957138062, "prompt": "新闻文本是“布局超高分子量聚乙烯产业链 　　近年来，超高分子量聚乙烯纤维在产品性能逐渐提升、应用领域稳步拓展，产能规模不断加码三重因素带动的背景下，其需求在全球范围内稳定增长”，包含的情绪词典是：广泛的/大规模的(extensive):0.2,高的/高等的(high):0.7"}, "另外，我国于2019年在《重点新材料首批次应用示范指导目录》中将超高分子量聚乙烯纤维定义为关键战略材料": {"topic": "“生产投资”", "similarity": 0.5936305522918701, "prompt": "新闻文本是“另外，我国于2019年在《重点新材料首批次应用示范指导目录》中将超高分子量聚乙烯纤维定义为关键战略材料”，包含的情绪词典是：高的/高等的(high):0.7,最高的/最高级的(highest):0.7"}, "同年，国内超高分子量聚乙烯纤维的理论需求量4.25万吨首次超越了国内产能4.10万吨，并在2020年显现出差距扩大的趋势，未来国内整体行业的供需关系将更加显现出供不应求的趋势": {"topic": "“生产投资”", "similarity": 0.5938977003097534, "prompt": "新闻文本是“同年，国内超高分子量聚乙烯纤维的理论需求量4.25万吨首次超越了国内产能4.10万吨，并在2020年显现出差距扩大的趋势，未来国内整体行业的供需关系将更加显现出供不应求的趋势”，包含的情绪词典是：产能过剩(overcapacity):-0.5,超过量/超越量(exceedances):0.2"}, "2022年中国超高分子量聚乙烯纤维需求量为6.76万吨，产能为4.78万吨": {"topic": "“生产投资”", "similarity": 0.5091561079025269, "prompt": "新闻文本是“2022年中国超高分子量聚乙烯纤维需求量为6.76万吨，产能为4.78万吨”，包含的情绪词典是：生产不足的/产量低于预期的(underproduced):-0.5,生产不足/产量低于预期(underproduction):-0.5"}, "恒辉安防半年报显示，报告期内，公司加速推进子公司恒尚材料“超纤维新材料及功能性安全防护用品开发应用项目”建设及产线磨合、 工艺制备技术突破、产线提质增效，公司超高分子量聚乙烯纤维满负荷产能已经达到3000吨": {"topic": "“生产投资”", "similarity": 0.5414125323295593, "prompt": "新闻文本是“恒辉安防半年报显示，报告期内，公司加速推进子公司恒尚材料“超纤维新材料及功能性安全防护用品开发应用项目”建设及产线磨合、 工艺制备技术突破、产线提质增效，公司超高分子量聚乙烯纤维满负荷产能已经达到3000吨”，包含的情绪词典是：可防御的/可保卫的(defendable):0.3"}, "同时，公司还在规划建设的产能4800吨，系公司拟发行可转债募集资金投资项目，该项目为公司安防产业园“年产12000吨超高分子量聚乙烯纤维”一期建设项目": {"topic": "“生产投资”", "similarity": 0.6194549798965454, "prompt": "新闻文本是“同时，公司还在规划建设的产能4800吨，系公司拟发行可转债募集资金投资项目，该项目为公司安防产业园“年产12000吨超高分子量聚乙烯纤维”一期建设项目”，包含的情绪词典是：产能过剩(overcapacity):-0.5,生产过剩的/过度生产的(overproduced):-0.3"}, "恒辉安防表示，通过这一项目的建设，一方面可以保障公司主营业务上游原材料的稳定供应、控制原材料价格波动风险": {"topic": "“生产投资”", "similarity": 0.5193594694137573, "prompt": "新闻文本是“恒辉安防表示，通过这一项目的建设，一方面可以保障公司主营业务上游原材料的稳定供应、控制原材料价格波动风险”，包含的情绪词典是：稳定的/稳固的(stable):0.5,保证/确保(assures):0.3"}, "另一方面，也是响应国家提升高性能纤维生产应用水平的发展目标，让公司把握高性能纤维产业的发展机遇，更快发展新质生产力": {"topic": "“生产投资”", "similarity": 0.6215605735778809, "prompt": "新闻文本是“另一方面，也是响应国家提升高性能纤维生产应用水平的发展目标，让公司把握高性能纤维产业的发展机遇，更快发展新质生产力”，包含的情绪词典是：增强的/提高的(enhanced):0.6,多产的/富有成效的(productive):0.7"}, "值得一提的是，在全球化布局方面，恒辉安防在越南工厂项目目前进展顺利，综合办公楼已结构封顶，预计明年下半年将贡献产能": {"topic": "“生产投资”", "similarity": 0.543052077293396, "prompt": "新闻文本是“值得一提的是，在全球化布局方面，恒辉安防在越南工厂项目目前进展顺利，综合办公楼已结构封顶，预计明年下半年将贡献产能”，包含的情绪词典是：工厂/制造厂(factory):0.0,工业/产业(industry):0.0"}, "同时，公司还积极与国内知名企业建立战略合作关系，构建多地域、多渠道的运营架构，以应对市场不确定性风险": {"topic": "“金融”", "similarity": 0.5258094072341919, "prompt": "新闻文本是“同时，公司还积极与国内知名企业建立战略合作关系，构建多地域、多渠道的运营架构，以应对市场不确定性风险”，包含的情绪词典是：合作性的/协作性的(collaborative):0.3,公司/企业(company):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -4609,12 +4569,12 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "医药板块近期回暖迹象明显，聚焦创新药产业链的恒生医药ETF（159892）上周连续5个交易日（8月26日~30日）收涨，医疗器械ETF（562600）连续2日大涨，医药板块活跃度提升", "news_prompt2": "兴业证券表示，尽管受到基数、行业大环境及细分领域景气度等多重因素影响，但医药板块整体业绩保持稳健增长，多数公司业绩符合预期，部分公司业绩或订单实现超预期", "news_prompt3": "展望2024Q3，预计板块基本面将进一步呈现边际向好趋势", "news_prompt4": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "兴业证券表示，尽管受到基数、行业大环境及细分领域景气度等多重因素影响，但医药板块整体业绩保持稳健增长，多数公司业绩符合预期，部分公司业绩或订单实现超预期", "news_prompt2": "展望2024Q3，预计板块基本面将进一步呈现边际向好趋势"}</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>{"医药板块近期回暖迹象明显，聚焦创新药产业链的恒生医药ETF（159892）上周连续5个交易日（8月26日~30日）收涨，医疗器械ETF（562600）连续2日大涨，医药板块活跃度提升": {"topic": "“金融”", "similarity": 0.5710659027099609}, "兴业证券表示，尽管受到基数、行业大环境及细分领域景气度等多重因素影响，但医药板块整体业绩保持稳健增长，多数公司业绩符合预期，部分公司业绩或订单实现超预期": {"topic": "“金融”", "similarity": 0.593159019947052, "prompt": "新闻文本是“兴业证券表示，尽管受到基数、行业大环境及细分领域景气度等多重因素影响，但医药板块整体业绩保持稳健增长，多数公司业绩符合预期，部分公司业绩或订单实现超预期”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "展望2024Q3，预计板块基本面将进一步呈现边际向好趋势": {"topic": "“金融”", "similarity": 0.5356159210205078, "prompt": "新闻文本是“展望2024Q3，预计板块基本面将进一步呈现边际向好趋势”，包含的情绪词典是：好转/向上趋势(upturn):0.4,乐观的/看好的(optimistic):0.7"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"兴业证券表示，尽管受到基数、行业大环境及细分领域景气度等多重因素影响，但医药板块整体业绩保持稳健增长，多数公司业绩符合预期，部分公司业绩或订单实现超预期": {"topic": "“金融”", "similarity": 0.5931590795516968, "prompt": "新闻文本是“兴业证券表示，尽管受到基数、行业大环境及细分领域景气度等多重因素影响，但医药板块整体业绩保持稳健增长，多数公司业绩符合预期，部分公司业绩或订单实现超预期”，包含的情绪词典是：稳定的/稳固的(stable):0.5,已稳定的/稳定的(stabilized):0.5"}, "展望2024Q3，预计板块基本面将进一步呈现边际向好趋势": {"topic": "“金融”", "similarity": 0.5356161594390869, "prompt": "新闻文本是“展望2024Q3，预计板块基本面将进一步呈现边际向好趋势”，包含的情绪词典是：好转/向上趋势(upturn):0.4,乐观的/看好的(optimistic):0.7"}}</t>
         </is>
       </c>
     </row>
@@ -4660,12 +4620,12 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "白云山9月1日公告，公司董事会于8月30日收到公司董事张春波递交的书面辞职报告", "news_prompt2": "张春波因个人原因，辞去公司第九届董事会执行董事、董事会预算委员会委员及子公司的任何职务", "news_prompt3": "辞职后，张春波不再担任公司及子公司的任何职务", "news_prompt4": "中国证券报·中证金牛座9月2日从业内人士处了解到，张春波或已被有关部门带走调查", "news_prompt5": "公开资料显示，张春波于2000年7月在中国药科大学毕业，同年参加工作", "news_prompt6": "自2015年1月至2021年8月任白云山副总经理，自2019年6月28日起任白云山董事，任广药集团党委委员、副总经理、公司党委委员，中一药业与奇星药业党委书记、董事长，天心药业董事，广州白云山医药销售有限公司董事，广州医药海马品牌整合传播有限公司董事和医药公司董事", "news_prompt7": "广东省纪委监委官网8月30日发布消息显示，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查", "news_prompt8": "7月22日晚，白云山公告，公司董事会当日收到公司董事长李楚源递交的书面辞职报告", "news_prompt9": "李楚源因个人原因，辞去公司第九届董事会董事长、执行董事及董事会战略发展与投资委员会主任的职务", "news_prompt10": "辞职后，李楚源不再担任公司任何职务", "news_prompt11": "（文章来源：中国证券报·中证金牛座）"}</t>
+          <t>{"news_prompt1": "广东省纪委监委官网8月30日发布消息显示，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查"}</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>{"中国证券报·中证金牛座9月2日从业内人士处了解到，张春波或已被有关部门带走调查": {"topic": "“金融”", "similarity": 0.43361392617225647}, "自2015年1月至2021年8月任白云山副总经理，自2019年6月28日起任白云山董事，任广药集团党委委员、副总经理、公司党委委员，中一药业与奇星药业党委书记、董事长，天心药业董事，广州白云山医药销售有限公司董事，广州医药海马品牌整合传播有限公司董事和医药公司董事": {"topic": "“生产投资”", "similarity": 0.4517068862915039}, "广东省纪委监委官网8月30日发布消息显示，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查": {"topic": "“生产投资”", "similarity": 0.4650470018386841, "prompt": "新闻文本是“广东省纪委监委官网8月30日发布消息显示，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查”，包含的情绪词典是：管理不善/管理失误(mismanagement):-0.5"}, "（文章来源：中国证券报·中证金牛座）": {"topic": "“金融”", "similarity": 0.4767891764640808, "prompt": "新闻文本是“（文章来源：中国证券报·中证金牛座）”，包含的情绪词典是：投资者/投资人(investor):0.4,金钱上的(pecuniarily):0.0"}}</t>
+          <t>{"广东省纪委监委官网8月30日发布消息显示，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查": {"topic": "“生产投资”", "similarity": 0.46504703164100647, "prompt": "新闻文本是“广东省纪委监委官网8月30日发布消息显示，广州医药集团有限公司原党委书记、董事长李楚源涉嫌严重违纪违法，目前正接受广东省纪委监委纪律审查和监察调查”，包含的情绪词典是：管理不善/管理失误(mismanagement):-0.5"}}</t>
         </is>
       </c>
     </row>
@@ -4711,12 +4671,12 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "中央气象台9月2日消息，昨日，西北地区中东部、西南地区东部和南部、江南东部、华南及内蒙古中部、山西北部、河北东北部等地出现分散性大雨或暴雨，局地有大暴雨", "news_prompt2": "预计今天，降雨将主要出现在山西南部、河南西部、山东西部、辽宁西部等地，降雨量以中到大雨为主，局地有暴雨 ，公众需警惕短时强降水、冰雹、雷暴大风等强对流天气", "news_prompt3": "另外，北方地区公众还需关注9月2日至4日的降水和降温过程", "news_prompt4": "预计，新疆、西北地区、内蒙古中西部、华北、黄淮、东北地区等地将自西向东出现小到中雨，局地有大雨或暴雨", "news_prompt5": "北方大部地区气温将有所下滑，并伴有4～6级风，新疆山口风力可达10～12级", "news_prompt6": "最后关注一下南方的高温天气，预计今天，南方高温范围仍较大，37℃以上的高温天气将范围覆盖四川东部、重庆及江南北部、江淮、江汉等地", "news_prompt7": "明后两天，南方高温范围将逐步收缩，黄淮、江淮、江南东部等地暑气有所消退，但四川东部、重庆等地高温愈演愈烈，40℃以上高温范围将进一步扩大", "news_prompt8": "今天白天，陕西南部、河南中南部、安徽大部、湖北、湖南大部、江西大部、浙江中西部、四川东部、重庆、贵州东北部等地部分地区最高气温37～39℃，重庆东北部和西部、湖北西部局地可达40℃以上", "news_prompt9": "中央气象台今晨继续发布高温黄色预警", "news_prompt10": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "中央气象台9月2日消息，昨日，西北地区中东部、西南地区东部和南部、江南东部、华南及内蒙古中部、山西北部、河北东北部等地出现分散性大雨或暴雨，局地有大暴雨", "news_prompt2": "预计今天，降雨将主要出现在山西南部、河南西部、山东西部、辽宁西部等地，降雨量以中到大雨为主，局地有暴雨 ，公众需警惕短时强降水、冰雹、雷暴大风等强对流天气", "news_prompt3": "预计，新疆、西北地区、内蒙古中西部、华北、黄淮、东北地区等地将自西向东出现小到中雨，局地有大雨或暴雨", "news_prompt4": "北方大部地区气温将有所下滑，并伴有4～6级风，新疆山口风力可达10～12级", "news_prompt5": "最后关注一下南方的高温天气，预计今天，南方高温范围仍较大，37℃以上的高温天气将范围覆盖四川东部、重庆及江南北部、江淮、江汉等地", "news_prompt6": "今天白天，陕西南部、河南中南部、安徽大部、湖北、湖南大部、江西大部、浙江中西部、四川东部、重庆、贵州东北部等地部分地区最高气温37～39℃，重庆东北部和西部、湖北西部局地可达40℃以上"}</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>{"中央气象台9月2日消息，昨日，西北地区中东部、西南地区东部和南部、江南东部、华南及内蒙古中部、山西北部、河北东北部等地出现分散性大雨或暴雨，局地有大暴雨": {"topic": "“宏观经济”", "similarity": 0.5268524289131165, "prompt": "新闻文本是“中央气象台9月2日消息，昨日，西北地区中东部、西南地区东部和南部、江南东部、华南及内蒙古中部、山西北部、河北东北部等地出现分散性大雨或暴雨，局地有大暴雨”，包含的情绪词典是：大灾难/浩劫(catastrophe):-1.0,灾难性的/灾祸性的(disastrous):-0.8"}, "预计今天，降雨将主要出现在山西南部、河南西部、山东西部、辽宁西部等地，降雨量以中到大雨为主，局地有暴雨 ，公众需警惕短时强降水、冰雹、雷暴大风等强对流天气": {"topic": "“消费”", "similarity": 0.539929986000061, "prompt": "新闻文本是“预计今天，降雨将主要出现在山西南部、河南西部、山东西部、辽宁西部等地，降雨量以中到大雨为主，局地有暴雨 ，公众需警惕短时强降水、冰雹、雷暴大风等强对流天气”，包含的情绪词典是：预防措施/防范(precaution):0.0,预防的/防备的(precautionary):0.1"}, "预计，新疆、西北地区、内蒙古中西部、华北、黄淮、东北地区等地将自西向东出现小到中雨，局地有大雨或暴雨": {"topic": "“房地产”", "similarity": 0.4784244894981384, "prompt": "新闻文本是“预计，新疆、西北地区、内蒙古中西部、华北、黄淮、东北地区等地将自西向东出现小到中雨，局地有大雨或暴雨”，包含的情绪词典是：预期的/预料的(anticipated):0.2,预测性的/预兆的(predictive):0.2"}, "北方大部地区气温将有所下滑，并伴有4～6级风，新疆山口风力可达10～12级": {"topic": "“宏观经济”", "similarity": 0.5027201175689697, "prompt": "新闻文本是“北方大部地区气温将有所下滑，并伴有4～6级风，新疆山口风力可达10～12级”，包含的情绪词典是：下跌/下降(fall):-0.6,北方/北部(north):0.0"}, "最后关注一下南方的高温天气，预计今天，南方高温范围仍较大，37℃以上的高温天气将范围覆盖四川东部、重庆及江南北部、江淮、江汉等地": {"topic": "“消费”", "similarity": 0.603934645652771, "prompt": "新闻文本是“最后关注一下南方的高温天气，预计今天，南方高温范围仍较大，37℃以上的高温天气将范围覆盖四川东部、重庆及江南北部、江淮、江汉等地”，包含的情绪词典是：炎热的/酷热的(torrid):-0.3,北方/北部(north):0.0"}, "明后两天，南方高温范围将逐步收缩，黄淮、江淮、江南东部等地暑气有所消退，但四川东部、重庆等地高温愈演愈烈，40℃以上高温范围将进一步扩大": {"topic": "“宏观经济”", "similarity": 0.5069157481193542}, "今天白天，陕西南部、河南中南部、安徽大部、湖北、湖南大部、江西大部、浙江中西部、四川东部、重庆、贵州东北部等地部分地区最高气温37～39℃，重庆东北部和西部、湖北西部局地可达40℃以上": {"topic": "“消费”", "similarity": 0.5402765274047852, "prompt": "新闻文本是“今天白天，陕西南部、河南中南部、安徽大部、湖北、湖南大部、江西大部、浙江中西部、四川东部、重庆、贵州东北部等地部分地区最高气温37～39℃，重庆东北部和西部、湖北西部局地可达40℃以上”，包含的情绪词典是：炎热的/酷热的(torrid):-0.3,天气/气象(weather):0.0"}}</t>
+          <t>{"中央气象台9月2日消息，昨日，西北地区中东部、西南地区东部和南部、江南东部、华南及内蒙古中部、山西北部、河北东北部等地出现分散性大雨或暴雨，局地有大暴雨": {"topic": "“宏观经济”", "similarity": 0.5268526077270508, "prompt": "新闻文本是“中央气象台9月2日消息，昨日，西北地区中东部、西南地区东部和南部、江南东部、华南及内蒙古中部、山西北部、河北东北部等地出现分散性大雨或暴雨，局地有大暴雨”，包含的情绪词典是：大灾难/浩劫(catastrophe):-1.0,灾难性的/灾祸性的(disastrous):-0.8"}, "预计今天，降雨将主要出现在山西南部、河南西部、山东西部、辽宁西部等地，降雨量以中到大雨为主，局地有暴雨 ，公众需警惕短时强降水、冰雹、雷暴大风等强对流天气": {"topic": "“消费”", "similarity": 0.539929986000061, "prompt": "新闻文本是“预计今天，降雨将主要出现在山西南部、河南西部、山东西部、辽宁西部等地，降雨量以中到大雨为主，局地有暴雨 ，公众需警惕短时强降水、冰雹、雷暴大风等强对流天气”，包含的情绪词典是：预防措施/防范(precaution):0.0,预防的/防备的(precautionary):0.1"}, "预计，新疆、西北地区、内蒙古中西部、华北、黄淮、东北地区等地将自西向东出现小到中雨，局地有大雨或暴雨": {"topic": "“房地产”", "similarity": 0.4784245193004608, "prompt": "新闻文本是“预计，新疆、西北地区、内蒙古中西部、华北、黄淮、东北地区等地将自西向东出现小到中雨，局地有大雨或暴雨”，包含的情绪词典是：预期的/预料的(anticipated):0.2,预测性的/预兆的(predictive):0.2"}, "北方大部地区气温将有所下滑，并伴有4～6级风，新疆山口风力可达10～12级": {"topic": "“宏观经济”", "similarity": 0.502720296382904, "prompt": "新闻文本是“北方大部地区气温将有所下滑，并伴有4～6级风，新疆山口风力可达10～12级”，包含的情绪词典是：下跌/下降(fall):-0.6,北方/北部(north):0.0"}, "最后关注一下南方的高温天气，预计今天，南方高温范围仍较大，37℃以上的高温天气将范围覆盖四川东部、重庆及江南北部、江淮、江汉等地": {"topic": "“消费”", "similarity": 0.6039345264434814, "prompt": "新闻文本是“最后关注一下南方的高温天气，预计今天，南方高温范围仍较大，37℃以上的高温天气将范围覆盖四川东部、重庆及江南北部、江淮、江汉等地”，包含的情绪词典是：炎热的/酷热的(torrid):-0.3,北方/北部(north):0.0"}, "今天白天，陕西南部、河南中南部、安徽大部、湖北、湖南大部、江西大部、浙江中西部、四川东部、重庆、贵州东北部等地部分地区最高气温37～39℃，重庆东北部和西部、湖北西部局地可达40℃以上": {"topic": "“消费”", "similarity": 0.5402765274047852, "prompt": "新闻文本是“今天白天，陕西南部、河南中南部、安徽大部、湖北、湖南大部、江西大部、浙江中西部、四川东部、重庆、贵州东北部等地部分地区最高气温37～39℃，重庆东北部和西部、湖北西部局地可达40℃以上”，包含的情绪词典是：炎热的/酷热的(torrid):-0.3,天气/气象(weather):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -4762,12 +4722,12 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，金帝股份(603270.SH)发布2024年中报", "news_prompt2": "公司营业总收入为5.94亿元，在已披露的同业公司中排名第95，较去年同报告期营业总收入增加1987.86万元，实现2年连续上涨，同比较去年同期上涨3.46%", "news_prompt3": "归母净利润为5715.40万元，在已披露的同业公司中排名第76，较去年同报告期归母净利润减少3302.23万元，同比较去年同期下降36.62%", "news_prompt4": "经营活动现金净流入为-8759.57万元，在已披露的同业公司中排名第206，较去年同报告期经营活动现金净流入减少1.75亿元，同比较去年同期下降200.52%", "news_prompt5": "公司最新资产负债率为28.25%，在已披露的同业公司中排名第102，较上季度资产负债率增加3.06个百分点，较去年同季度资产负债率减少20.14个百分点", "news_prompt6": "公司最新毛利率为30.58%，在已披露的同业公司中排名第106，较上季度毛利率减少3.10个百分点，较去年同季度毛利率减少4.26个百分点", "news_prompt7": "最新ROE为2.67%，在已披露的同业公司中排名第130，较去年同季度ROE减少6.36个百分点", "news_prompt8": "公司摊薄每股收益为0.26元，在已披露的同业公司中排名第84，较去年同报告期摊薄每股收益减少0.29元，同比较去年同期下降52.46%", "news_prompt9": "公司最新总资产周转率为0.20次，在已披露的同业公司中排名第141，较去年同季度总资产周转率减少0.10次，同比较去年同期下降33.23%", "news_prompt10": "最新存货周转率为1.12次，在已披露的同业公司中排名第110，较去年同季度存货周转率减少0.23次，同比较去年同期下降17.33%", "news_prompt11": "公司股东户数为2.56万户，前十大股东持股数量为1.69亿股，占总股本比例为76.99%", "news_prompt12": "前十大股东分别为聊城市金帝企业管理咨询有限公司、聊城市金源新旧动能转换股权投资基金合伙企业(有限合伙)、郑广会、聊城市鑫智源创业投资中心合伙企业(有限合伙)、洛阳新强联回转支承股份有限公司、国信证券-兴业银行-国信证券金帝股份员工参与战略配售1号集合资产管理计划、宁波澜溪创新股权投资合伙企业(有限合伙)、宁波澳源股权投资有限公司、聊城市鑫慧源创业投资中心合伙企业(有限合伙)、聊城市鑫创源创业投资合伙企业(有限合伙)，持股比例分别为36.51%、15.06%、9.13%、5.79%、3.38%、1.99%、1.69%、1.69%、1.23%、0.52%", "news_prompt13": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "公司营业总收入为5.94亿元，在已披露的同业公司中排名第95，较去年同报告期营业总收入增加1987.86万元，实现2年连续上涨，同比较去年同期上涨3.46%", "news_prompt2": "归母净利润为5715.40万元，在已披露的同业公司中排名第76，较去年同报告期归母净利润减少3302.23万元，同比较去年同期下降36.62%", "news_prompt3": "经营活动现金净流入为-8759.57万元，在已披露的同业公司中排名第206，较去年同报告期经营活动现金净流入减少1.75亿元，同比较去年同期下降200.52%", "news_prompt4": "公司最新资产负债率为28.25%，在已披露的同业公司中排名第102，较上季度资产负债率增加3.06个百分点，较去年同季度资产负债率减少20.14个百分点", "news_prompt5": "公司最新毛利率为30.58%，在已披露的同业公司中排名第106，较上季度毛利率减少3.10个百分点，较去年同季度毛利率减少4.26个百分点", "news_prompt6": "公司摊薄每股收益为0.26元，在已披露的同业公司中排名第84，较去年同报告期摊薄每股收益减少0.29元，同比较去年同期下降52.46%", "news_prompt7": "公司最新总资产周转率为0.20次，在已披露的同业公司中排名第141，较去年同季度总资产周转率减少0.10次，同比较去年同期下降33.23%", "news_prompt8": "最新存货周转率为1.12次，在已披露的同业公司中排名第110，较去年同季度存货周转率减少0.23次，同比较去年同期下降17.33%", "news_prompt9": "公司股东户数为2.56万户，前十大股东持股数量为1.69亿股，占总股本比例为76.99%"}</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，金帝股份(603270.SH)发布2024年中报": {"topic": "“金融”", "similarity": 0.54323410987854, "prompt": "新闻文本是“2024年8月31日，金帝股份(603270.SH)发布2024年中报”，包含的情绪词典是：金融/财政(finance):0.0,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司营业总收入为5.94亿元，在已披露的同业公司中排名第95，较去年同报告期营业总收入增加1987.86万元，实现2年连续上涨，同比较去年同期上涨3.46%": {"topic": "“消费”", "similarity": 0.5442439317703247, "prompt": "新闻文本是“公司营业总收入为5.94亿元，在已披露的同业公司中排名第95，较去年同报告期营业总收入增加1987.86万元，实现2年连续上涨，同比较去年同期上涨3.46%”，包含的情绪词典是：公司的/企业的(corporate):0.0,上升/上涨(rise):0.5"}, "归母净利润为5715.40万元，在已披露的同业公司中排名第76，较去年同报告期归母净利润减少3302.23万元，同比较去年同期下降36.62%": {"topic": "“消费”", "similarity": 0.5063539743423462, "prompt": "新闻文本是“归母净利润为5715.40万元，在已披露的同业公司中排名第76，较去年同报告期归母净利润减少3302.23万元，同比较去年同期下降36.62%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "经营活动现金净流入为-8759.57万元，在已披露的同业公司中排名第206，较去年同报告期经营活动现金净流入减少1.75亿元，同比较去年同期下降200.52%": {"topic": "“金融”", "similarity": 0.5495230555534363, "prompt": "新闻文本是“经营活动现金净流入为-8759.57万元，在已披露的同业公司中排名第206，较去年同报告期经营活动现金净流入减少1.75亿元，同比较去年同期下降200.52%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新资产负债率为28.25%，在已披露的同业公司中排名第102，较上季度资产负债率增加3.06个百分点，较去年同季度资产负债率减少20.14个百分点": {"topic": "“消费”", "similarity": 0.48585575819015503, "prompt": "新闻文本是“公司最新资产负债率为28.25%，在已披露的同业公司中排名第102，较上季度资产负债率增加3.06个百分点，较去年同季度资产负债率减少20.14个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新毛利率为30.58%，在已披露的同业公司中排名第106，较上季度毛利率减少3.10个百分点，较去年同季度毛利率减少4.26个百分点": {"topic": "“消费”", "similarity": 0.4468623995780945, "prompt": "新闻文本是“公司最新毛利率为30.58%，在已披露的同业公司中排名第106，较上季度毛利率减少3.10个百分点，较去年同季度毛利率减少4.26个百分点”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,百分比(percentage):0.0"}, "公司摊薄每股收益为0.26元，在已披露的同业公司中排名第84，较去年同报告期摊薄每股收益减少0.29元，同比较去年同期下降52.46%": {"topic": "“金融”", "similarity": 0.4707624912261963, "prompt": "新闻文本是“公司摊薄每股收益为0.26元，在已披露的同业公司中排名第84，较去年同报告期摊薄每股收益减少0.29元，同比较去年同期下降52.46%”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新总资产周转率为0.20次，在已披露的同业公司中排名第141，较去年同季度总资产周转率减少0.10次，同比较去年同期下降33.23%": {"topic": "“消费”", "similarity": 0.49974948167800903, "prompt": "新闻文本是“公司最新总资产周转率为0.20次，在已披露的同业公司中排名第141，较去年同季度总资产周转率减少0.10次，同比较去年同期下降33.23%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "最新存货周转率为1.12次，在已披露的同业公司中排名第110，较去年同季度存货周转率减少0.23次，同比较去年同期下降17.33%": {"topic": "“消费”", "similarity": 0.4586881995201111, "prompt": "新闻文本是“最新存货周转率为1.12次，在已披露的同业公司中排名第110，较去年同季度存货周转率减少0.23次，同比较去年同期下降17.33%”，包含的情绪词典是：营业额/周转(turnover):0.0,周期/循环(cycle):0.0"}, "公司股东户数为2.56万户，前十大股东持股数量为1.69亿股，占总股本比例为76.99%": {"topic": "“金融”", "similarity": 0.46469688415527344, "prompt": "新闻文本是“公司股东户数为2.56万户，前十大股东持股数量为1.69亿股，占总股本比例为76.99%”，包含的情绪词典是：公司/企业(company):0.0,公司/企业(firm):0.0"}, "前十大股东分别为聊城市金帝企业管理咨询有限公司、聊城市金源新旧动能转换股权投资基金合伙企业(有限合伙)、郑广会、聊城市鑫智源创业投资中心合伙企业(有限合伙)、洛阳新强联回转支承股份有限公司、国信证券-兴业银行-国信证券金帝股份员工参与战略配售1号集合资产管理计划、宁波澜溪创新股权投资合伙企业(有限合伙)、宁波澳源股权投资有限公司、聊城市鑫慧源创业投资中心合伙企业(有限合伙)、聊城市鑫创源创业投资合伙企业(有限合伙)，持股比例分别为36.51%、15.06%、9.13%、5.79%、3.38%、1.99%、1.69%、1.69%、1.23%、0.52%": {"topic": "“生产投资”", "similarity": 0.6218016743659973}}</t>
+          <t>{"公司营业总收入为5.94亿元，在已披露的同业公司中排名第95，较去年同报告期营业总收入增加1987.86万元，实现2年连续上涨，同比较去年同期上涨3.46%": {"topic": "“消费”", "similarity": 0.5442439317703247, "prompt": "新闻文本是“公司营业总收入为5.94亿元，在已披露的同业公司中排名第95，较去年同报告期营业总收入增加1987.86万元，实现2年连续上涨，同比较去年同期上涨3.46%”，包含的情绪词典是：公司的/企业的(corporate):0.0,上升/上涨(rise):0.5"}, "归母净利润为5715.40万元，在已披露的同业公司中排名第76，较去年同报告期归母净利润减少3302.23万元，同比较去年同期下降36.62%": {"topic": "“消费”", "similarity": 0.5063540935516357, "prompt": "新闻文本是“归母净利润为5715.40万元，在已披露的同业公司中排名第76，较去年同报告期归母净利润减少3302.23万元，同比较去年同期下降36.62%”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperforming):-0.4"}, "经营活动现金净流入为-8759.57万元，在已披露的同业公司中排名第206，较去年同报告期经营活动现金净流入减少1.75亿元，同比较去年同期下降200.52%": {"topic": "“金融”", "similarity": 0.5495231747627258, "prompt": "新闻文本是“经营活动现金净流入为-8759.57万元，在已披露的同业公司中排名第206，较去年同报告期经营活动现金净流入减少1.75亿元，同比较去年同期下降200.52%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新资产负债率为28.25%，在已披露的同业公司中排名第102，较上季度资产负债率增加3.06个百分点，较去年同季度资产负债率减少20.14个百分点": {"topic": "“消费”", "similarity": 0.4858558475971222, "prompt": "新闻文本是“公司最新资产负债率为28.25%，在已披露的同业公司中排名第102，较上季度资产负债率增加3.06个百分点，较去年同季度资产负债率减少20.14个百分点”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,表现不佳/业绩低于预期(underperforming):-0.4"}, "公司最新毛利率为30.58%，在已披露的同业公司中排名第106，较上季度毛利率减少3.10个百分点，较去年同季度毛利率减少4.26个百分点": {"topic": "“消费”", "similarity": 0.44686242938041687, "prompt": "新闻文本是“公司最新毛利率为30.58%，在已披露的同业公司中排名第106，较上季度毛利率减少3.10个百分点，较去年同季度毛利率减少4.26个百分点”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,百分比(percentage):0.0"}, "公司摊薄每股收益为0.26元，在已披露的同业公司中排名第84，较去年同报告期摊薄每股收益减少0.29元，同比较去年同期下降52.46%": {"topic": "“金融”", "similarity": 0.4707626700401306, "prompt": "新闻文本是“公司摊薄每股收益为0.26元，在已披露的同业公司中排名第84，较去年同报告期摊薄每股收益减少0.29元，同比较去年同期下降52.46%”，包含的情绪词典是：表现不佳/业绩低于预期(underperform):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "公司最新总资产周转率为0.20次，在已披露的同业公司中排名第141，较去年同季度总资产周转率减少0.10次，同比较去年同期下降33.23%": {"topic": "“消费”", "similarity": 0.49974948167800903, "prompt": "新闻文本是“公司最新总资产周转率为0.20次，在已披露的同业公司中排名第141，较去年同季度总资产周转率减少0.10次，同比较去年同期下降33.23%”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}, "最新存货周转率为1.12次，在已披露的同业公司中排名第110，较去年同季度存货周转率减少0.23次，同比较去年同期下降17.33%": {"topic": "“消费”", "similarity": 0.45868825912475586, "prompt": "新闻文本是“最新存货周转率为1.12次，在已披露的同业公司中排名第110，较去年同季度存货周转率减少0.23次，同比较去年同期下降17.33%”，包含的情绪词典是：营业额/周转(turnover):0.0,周期/循环(cycle):0.0"}, "公司股东户数为2.56万户，前十大股东持股数量为1.69亿股，占总股本比例为76.99%": {"topic": "“金融”", "similarity": 0.46469709277153015, "prompt": "新闻文本是“公司股东户数为2.56万户，前十大股东持股数量为1.69亿股，占总股本比例为76.99%”，包含的情绪词典是：公司/企业(company):0.0,公司/企业(firm):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -4813,12 +4773,12 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "近日，一向对美股科技股“金句频出”的华尔街知名分析师——Wedbush分析师丹·艾夫斯又说出了“金句”，形容英伟达的潜力巨大，并将其比作有史以来最伟大的篮球运动员巨星之一——勒布朗·詹姆斯", "news_prompt2": "艾夫斯在接受采访时表示：“如果你看看英伟达，就这个故事的最终走向而言，它就像是高中时期的勒布朗", "news_prompt3": "”　　在随后的采访中，他又再次提到了这个比喻，并表示，英伟达之所以像年轻的勒布朗·詹姆斯，是因为它远远领先于其他竞争对手，是AI半导体领域“唯一的玩家”", "news_prompt4": "英伟达前景仍然强劲　　美东时间上周三，英伟达发布了重磅的第二季度财报", "news_prompt5": "尽管这份财报超出了分析师的平均预期，但由于其距离市场最高预期仍有距离，投资者仍然推低了其股价", "news_prompt6": "截至上周五收盘，英伟达股价收于119.37美元，周跌幅约为8%", "news_prompt7": "事实上，相比于今年上半年的顺风顺水，今年下半年英伟达股价似乎陷入了震荡", "news_prompt8": "自今年6月20日达到纪录新高之后，英伟达股价就开始了大幅震荡，显示出投资者开始对其高估值和增长前景产生了犹豫", "news_prompt9": "不过，艾夫斯认为，英伟达CEO黄仁勋给出的营收预期仍然强劲，尽管低于分析师最乐观的预期，但足以打消市场的担忧", "news_prompt10": "“他们来了，他们做到了", "news_prompt11": "”他在谈到英伟达的盈利时补充道，“我认为，对科技股来说，这将为反弹提供动力", "news_prompt12": "”　　艾夫斯估计，英伟达的新一代芯片Balckwell的收入前景可能将达到数百亿美元", "news_prompt13": "他认为，公司对Blackwell的预期指引之所以相对模糊，是因为黄仁勋不愿透露他的剧本", "news_prompt14": "他还吹捧了英伟达在更广泛科技领域的乘数效应，称英伟达在其芯片上花费的每一美元，都会在整个行业产生8-10倍的涟漪效应", "news_prompt15": "AI前景仍然不可估量　　艾夫斯预计，未来三年人工智能领域的资本支出将达到1万亿美元——这一数字是他六个月前预测的两倍", "news_prompt16": "他补充说，市场对英伟达芯片的需求也在加速扩大", "news_prompt17": "不仅是微软、OpenAI、亚马逊和谷歌等所谓的超大规模客户，随着更多人工智能用例的出现，其他中小型企业也在加快步伐", "news_prompt18": "“罗马不是一天建成的，人工智能革命也不是一天建成的，”他预测道，“现在（AI革命）已经开始成型了", "news_prompt19": "”　　华尔街仍然坚定看好　　尽管在财报发布后，英伟达股价暂时走低，但华尔街上的大多数人仍将其股票归为“买入”类别", "news_prompt20": "事实上，艾夫斯并不是华尔街上唯一一个不受股价短期走低影响、仍然坚持看好英伟达股价前景的分析师", "news_prompt21": "美国银行全球研究部重申了买入评级，并将其股票目标价从150美元上调至165美元，称英伟达仍是“关键的基因周期受益者”，并恳请投资者“忽略季度噪音”", "news_prompt22": "凯投宏观亚太区市场主管托马斯·马修斯也在报告中表示:“我们认为，尽管投资者对英伟达的快速利润增长前景明显感到失望，但人工智能的涨势仍将持续下去", "news_prompt23": "”（文章来源：财联社）"}</t>
+          <t>{"news_prompt1": "近日，一向对美股科技股“金句频出”的华尔街知名分析师——Wedbush分析师丹·艾夫斯又说出了“金句”，形容英伟达的潜力巨大，并将其比作有史以来最伟大的篮球运动员巨星之一——勒布朗·詹姆斯", "news_prompt2": "自今年6月20日达到纪录新高之后，英伟达股价就开始了大幅震荡，显示出投资者开始对其高估值和增长前景产生了犹豫", "news_prompt3": "AI前景仍然不可估量　　艾夫斯预计，未来三年人工智能领域的资本支出将达到1万亿美元——这一数字是他六个月前预测的两倍", "news_prompt4": "不仅是微软、OpenAI、亚马逊和谷歌等所谓的超大规模客户，随着更多人工智能用例的出现，其他中小型企业也在加快步伐", "news_prompt5": "“罗马不是一天建成的，人工智能革命也不是一天建成的，”他预测道，“现在（AI革命）已经开始成型了", "news_prompt6": "”　　华尔街仍然坚定看好　　尽管在财报发布后，英伟达股价暂时走低，但华尔街上的大多数人仍将其股票归为“买入”类别"}</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>{"近日，一向对美股科技股“金句频出”的华尔街知名分析师——Wedbush分析师丹·艾夫斯又说出了“金句”，形容英伟达的潜力巨大，并将其比作有史以来最伟大的篮球运动员巨星之一——勒布朗·詹姆斯": {"topic": "“生产投资”", "similarity": 0.4489184617996216, "prompt": "新闻文本是“近日，一向对美股科技股“金句频出”的华尔街知名分析师——Wedbush分析师丹·艾夫斯又说出了“金句”，形容英伟达的潜力巨大，并将其比作有史以来最伟大的篮球运动员巨星之一——勒布朗·詹姆斯”，包含的情绪词典是：潜在的/潜力(potential):0.3,杰出的/非凡的(exceptional):1.0"}, "自今年6月20日达到纪录新高之后，英伟达股价就开始了大幅震荡，显示出投资者开始对其高估值和增长前景产生了犹豫": {"topic": "“金融”", "similarity": 0.45626527070999146, "prompt": "新闻文本是“自今年6月20日达到纪录新高之后，英伟达股价就开始了大幅震荡，显示出投资者开始对其高估值和增长前景产生了犹豫”，包含的情绪词典是：高估的/估价过高的(overvalued):-0.3,高估/对…估价过高(overvalue):-0.3"}, "AI前景仍然不可估量　　艾夫斯预计，未来三年人工智能领域的资本支出将达到1万亿美元——这一数字是他六个月前预测的两倍": {"topic": "“生产投资”", "similarity": 0.4585675001144409, "prompt": "新闻文本是“AI前景仍然不可估量　　艾夫斯预计，未来三年人工智能领域的资本支出将达到1万亿美元——这一数字是他六个月前预测的两倍”，包含的情绪词典是：潜在的/潜力(potential):0.3,相当大的/可观的(considerable):0.3"}, "不仅是微软、OpenAI、亚马逊和谷歌等所谓的超大规模客户，随着更多人工智能用例的出现，其他中小型企业也在加快步伐": {"topic": "“生产投资”", "similarity": 0.4222356975078583, "prompt": "新闻文本是“不仅是微软、OpenAI、亚马逊和谷歌等所谓的超大规模客户，随着更多人工智能用例的出现，其他中小型企业也在加快步伐”，包含的情绪词典是：相当大的/可观的(sizeable):0.0"}, "“罗马不是一天建成的，人工智能革命也不是一天建成的，”他预测道，“现在（AI革命）已经开始成型了": {"topic": "“生产投资”", "similarity": 0.4277763068675995, "prompt": "新闻文本是““罗马不是一天建成的，人工智能革命也不是一天建成的，”他预测道，“现在（AI革命）已经开始成型了”，包含的情绪词典是：预测性的/预兆的(predictive):0.2,注定的/命定的(destined):0.0"}, "”　　华尔街仍然坚定看好　　尽管在财报发布后，英伟达股价暂时走低，但华尔街上的大多数人仍将其股票归为“买入”类别": {"topic": "“金融”", "similarity": 0.4328293800354004, "prompt": "新闻文本是“”　　华尔街仍然坚定看好　　尽管在财报发布后，英伟达股价暂时走低，但华尔街上的大多数人仍将其股票归为“买入”类别”，包含的情绪词典是：乐观的/看好的(optimistic):0.7,跑赢/表现优于(outperform):0.65"}, "美国银行全球研究部重申了买入评级，并将其股票目标价从150美元上调至165美元，称英伟达仍是“关键的基因周期受益者”，并恳请投资者“忽略季度噪音”": {"topic": "“金融”", "similarity": 0.4288443922996521}, "凯投宏观亚太区市场主管托马斯·马修斯也在报告中表示:“我们认为，尽管投资者对英伟达的快速利润增长前景明显感到失望，但人工智能的涨势仍将持续下去": {"topic": "“宏观经济”", "similarity": 0.4772312641143799}, "”（文章来源：财联社）": {"topic": "“金融”", "similarity": 0.4526078701019287, "prompt": "新闻文本是“”（文章来源：财联社）”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}}</t>
+          <t>{"近日，一向对美股科技股“金句频出”的华尔街知名分析师——Wedbush分析师丹·艾夫斯又说出了“金句”，形容英伟达的潜力巨大，并将其比作有史以来最伟大的篮球运动员巨星之一——勒布朗·詹姆斯": {"topic": "“生产投资”", "similarity": 0.4489186406135559, "prompt": "新闻文本是“近日，一向对美股科技股“金句频出”的华尔街知名分析师——Wedbush分析师丹·艾夫斯又说出了“金句”，形容英伟达的潜力巨大，并将其比作有史以来最伟大的篮球运动员巨星之一——勒布朗·詹姆斯”，包含的情绪词典是：潜在的/潜力(potential):0.3,杰出的/非凡的(exceptional):1.0"}, "自今年6月20日达到纪录新高之后，英伟达股价就开始了大幅震荡，显示出投资者开始对其高估值和增长前景产生了犹豫": {"topic": "“金融”", "similarity": 0.45626550912857056, "prompt": "新闻文本是“自今年6月20日达到纪录新高之后，英伟达股价就开始了大幅震荡，显示出投资者开始对其高估值和增长前景产生了犹豫”，包含的情绪词典是：高估的/估价过高的(overvalued):-0.3,高估/对…估价过高(overvalue):-0.3"}, "AI前景仍然不可估量　　艾夫斯预计，未来三年人工智能领域的资本支出将达到1万亿美元——这一数字是他六个月前预测的两倍": {"topic": "“生产投资”", "similarity": 0.4585675001144409, "prompt": "新闻文本是“AI前景仍然不可估量　　艾夫斯预计，未来三年人工智能领域的资本支出将达到1万亿美元——这一数字是他六个月前预测的两倍”，包含的情绪词典是：潜在的/潜力(potential):0.3,相当大的/可观的(considerable):0.3"}, "不仅是微软、OpenAI、亚马逊和谷歌等所谓的超大规模客户，随着更多人工智能用例的出现，其他中小型企业也在加快步伐": {"topic": "“生产投资”", "similarity": 0.42223572731018066, "prompt": "新闻文本是“不仅是微软、OpenAI、亚马逊和谷歌等所谓的超大规模客户，随着更多人工智能用例的出现，其他中小型企业也在加快步伐”，包含的情绪词典是：相当大的/可观的(sizeable):0.0"}, "“罗马不是一天建成的，人工智能革命也不是一天建成的，”他预测道，“现在（AI革命）已经开始成型了": {"topic": "“生产投资”", "similarity": 0.4277764558792114, "prompt": "新闻文本是““罗马不是一天建成的，人工智能革命也不是一天建成的，”他预测道，“现在（AI革命）已经开始成型了”，包含的情绪词典是：预测性的/预兆的(predictive):0.2,注定的/命定的(destined):0.0"}, "”　　华尔街仍然坚定看好　　尽管在财报发布后，英伟达股价暂时走低，但华尔街上的大多数人仍将其股票归为“买入”类别": {"topic": "“金融”", "similarity": 0.43282949924468994, "prompt": "新闻文本是“”　　华尔街仍然坚定看好　　尽管在财报发布后，英伟达股价暂时走低，但华尔街上的大多数人仍将其股票归为“买入”类别”，包含的情绪词典是：乐观的/看好的(optimistic):0.7,跑赢/表现优于(outperform):0.65"}}</t>
         </is>
       </c>
     </row>
@@ -4864,12 +4824,12 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日，A股三大指数集体低开，中证A50指数截至发稿跌超0.5%", "news_prompt2": "成分股多数下跌，北方华创、福耀玻璃、美的集团、三一重工、盐湖股份、珀莱雅、京东方A、长江电力等股飘红", "news_prompt3": "相关ETF方面，A50ETF基金（159592）截至发稿下跌0.83%，溢折率0.01%，盘中溢价", "news_prompt4": "Wind数据显示，该ETF上一交易日净流入超1300万元，基金最新份额与流通规模分别为44.42亿份与42.50亿份，均创历史新高", "news_prompt5": "A50ETF基金（159592）紧密跟踪中证A50指数，该指数布局A股核心资产，从各行业龙头上市公司证券中，选取市值最大的50只证券作为指数样本，以反映各行业最具代表性的龙头上市公司证券的整体表现", "news_prompt6": "消息面上，8月30日国务院常务会议召开，研究推动保险业高质量发展的若干意见", "news_prompt7": "会议指出，要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资", "news_prompt8": "中原证券表示，中央提出要“壮大耐心资本”，未来市场资金有望更稳定，投资方向更集中", "news_prompt9": "虽然海内外经济政策和形势的变动较快，市场的波动性增高，但无论其市场价格怎么波动，假如资产能长期为投资者带来正向现金流，就具备长期投资潜力", "news_prompt10": "中金公司指出，9月市场有望边际回稳，关注稳增长政策落地进度", "news_prompt11": "伴随中报披露完毕，9月进入业绩真空期，部分领域基本面压力阶段性释缓", "news_prompt12": "近期7月工业企业利润、8月PMI数据陆续公布，均反映国内需求阶段性不强现状，需要稳增长政策发力支持", "news_prompt13": "此外，9月美国降息预期抬升，全球资金有望迎来再配置，或利好中国资产", "news_prompt14": "（本文机构观点来自持牌证券机构，不构成任何投资建议，亦不代表平台观点，请投资人独立判断和决策", "news_prompt15": "）（文章来源：21世纪经济报道）"}</t>
+          <t>{"news_prompt1": "9月2日，A股三大指数集体低开，中证A50指数截至发稿跌超0.5%", "news_prompt2": "成分股多数下跌，北方华创、福耀玻璃、美的集团、三一重工、盐湖股份、珀莱雅、京东方A、长江电力等股飘红", "news_prompt3": "相关ETF方面，A50ETF基金（159592）截至发稿下跌0.83%，溢折率0.01%，盘中溢价", "news_prompt4": "Wind数据显示，该ETF上一交易日净流入超1300万元，基金最新份额与流通规模分别为44.42亿份与42.50亿份，均创历史新高", "news_prompt5": "消息面上，8月30日国务院常务会议召开，研究推动保险业高质量发展的若干意见", "news_prompt6": "会议指出，要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资", "news_prompt7": "中原证券表示，中央提出要“壮大耐心资本”，未来市场资金有望更稳定，投资方向更集中", "news_prompt8": "虽然海内外经济政策和形势的变动较快，市场的波动性增高，但无论其市场价格怎么波动，假如资产能长期为投资者带来正向现金流，就具备长期投资潜力", "news_prompt9": "中金公司指出，9月市场有望边际回稳，关注稳增长政策落地进度", "news_prompt10": "近期7月工业企业利润、8月PMI数据陆续公布，均反映国内需求阶段性不强现状，需要稳增长政策发力支持", "news_prompt11": "此外，9月美国降息预期抬升，全球资金有望迎来再配置，或利好中国资产"}</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>{"9月2日，A股三大指数集体低开，中证A50指数截至发稿跌超0.5%": {"topic": "“金融”", "similarity": 0.5640262961387634, "prompt": "新闻文本是“9月2日，A股三大指数集体低开，中证A50指数截至发稿跌超0.5%”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退/低迷(downturn):-0.6"}, "成分股多数下跌，北方华创、福耀玻璃、美的集团、三一重工、盐湖股份、珀莱雅、京东方A、长江电力等股飘红": {"topic": "“金融”", "similarity": 0.6186585426330566, "prompt": "新闻文本是“成分股多数下跌，北方华创、福耀玻璃、美的集团、三一重工、盐湖股份、珀莱雅、京东方A、长江电力等股飘红”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "相关ETF方面，A50ETF基金（159592）截至发稿下跌0.83%，溢折率0.01%，盘中溢价": {"topic": "“金融”", "similarity": 0.48490646481513977, "prompt": "新闻文本是“相关ETF方面，A50ETF基金（159592）截至发稿下跌0.83%，溢折率0.01%，盘中溢价”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "Wind数据显示，该ETF上一交易日净流入超1300万元，基金最新份额与流通规模分别为44.42亿份与42.50亿份，均创历史新高": {"topic": "“金融”", "similarity": 0.5575500726699829, "prompt": "新闻文本是“Wind数据显示，该ETF上一交易日净流入超1300万元，基金最新份额与流通规模分别为44.42亿份与42.50亿份，均创历史新高”，包含的情绪词典是：高估的/估价过高的(overvalued):-0.3,储备/囤积(stockpile):0.1"}, "A50ETF基金（159592）紧密跟踪中证A50指数，该指数布局A股核心资产，从各行业龙头上市公司证券中，选取市值最大的50只证券作为指数样本，以反映各行业最具代表性的龙头上市公司证券的整体表现": {"topic": "“金融”", "similarity": 0.6173725724220276}, "消息面上，8月30日国务院常务会议召开，研究推动保险业高质量发展的若干意见": {"topic": "“金融”", "similarity": 0.6731833219528198, "prompt": "新闻文本是“消息面上，8月30日国务院常务会议召开，研究推动保险业高质量发展的若干意见”，包含的情绪词典是：保险不足的(underinsured):-0.3,风险(risk):-0.4"}, "会议指出，要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资": {"topic": "“金融”", "similarity": 0.6313339471817017, "prompt": "新闻文本是“会议指出，要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资”，包含的情绪词典是：资本/资金(capital):0.1,稳定/稳定性(stability):0.6"}, "中原证券表示，中央提出要“壮大耐心资本”，未来市场资金有望更稳定，投资方向更集中": {"topic": "“金融”", "similarity": 0.5223621726036072, "prompt": "新闻文本是“中原证券表示，中央提出要“壮大耐心资本”，未来市场资金有望更稳定，投资方向更集中”，包含的情绪词典是：稳定的/稳固的(stable):0.5,资本/资金(capital):0.1"}, "虽然海内外经济政策和形势的变动较快，市场的波动性增高，但无论其市场价格怎么波动，假如资产能长期为投资者带来正向现金流，就具备长期投资潜力": {"topic": "“宏观经济”", "similarity": 0.6219462752342224, "prompt": "新闻文本是“虽然海内外经济政策和形势的变动较快，市场的波动性增高，但无论其市场价格怎么波动，假如资产能长期为投资者带来正向现金流，就具备长期投资潜力”，包含的情绪词典是：波动/起伏(fluctuate):-0.2,波动/起伏(fluctuates):-0.2"}, "中金公司指出，9月市场有望边际回稳，关注稳增长政策落地进度": {"topic": "“金融”", "similarity": 0.4982292354106903, "prompt": "新闻文本是“中金公司指出，9月市场有望边际回稳，关注稳增长政策落地进度”，包含的情绪词典是：稳定的/稳固的(stable):0.5,稳定/稳定性(stability):0.6"}, "伴随中报披露完毕，9月进入业绩真空期，部分领域基本面压力阶段性释缓": {"topic": "“金融”", "similarity": 0.5522174835205078, "prompt": "新闻文本是“伴随中报披露完毕，9月进入业绩真空期，部分领域基本面压力阶段性释缓”，包含的情绪词典是：缓和/放松(easing):0.3,表现不佳/业绩低于预期(underperform):-0.4"}, "近期7月工业企业利润、8月PMI数据陆续公布，均反映国内需求阶段性不强现状，需要稳增长政策发力支持": {"topic": "“宏观经济”", "similarity": 0.6633315682411194, "prompt": "新闻文本是“近期7月工业企业利润、8月PMI数据陆续公布，均反映国内需求阶段性不强现状，需要稳增长政策发力支持”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,衰退的/不景气的(recessionary):-0.8"}, "此外，9月美国降息预期抬升，全球资金有望迎来再配置，或利好中国资产": {"topic": "“金融”", "similarity": 0.5194090604782104, "prompt": "新闻文本是“此外，9月美国降息预期抬升，全球资金有望迎来再配置，或利好中国资产”，包含的情绪词典是：乐观的/看好的(optimistic):0.7,清仓/抛售(closeout):-0.2"}, "（本文机构观点来自持牌证券机构，不构成任何投资建议，亦不代表平台观点，请投资人独立判断和决策": {"topic": "“金融”", "similarity": 0.571772038936615, "prompt": "新闻文本是“（本文机构观点来自持牌证券机构，不构成任何投资建议，亦不代表平台观点，请投资人独立判断和决策”，包含的情绪词典是：投机性的/推测性的(speculative):-0.2,投资者/投资人(investor):0.4"}, "）（文章来源：21世纪经济报道）": {"topic": "“宏观经济”", "similarity": 0.43245604634284973, "prompt": "新闻文本是“）（文章来源：21世纪经济报道）”，包含的情绪词典是：经济/经济体(economy):0.0,金融的/财政的(financial):0.0"}}</t>
+          <t>{"9月2日，A股三大指数集体低开，中证A50指数截至发稿跌超0.5%": {"topic": "“金融”", "similarity": 0.5640265941619873, "prompt": "新闻文本是“9月2日，A股三大指数集体低开，中证A50指数截至发稿跌超0.5%”，包含的情绪词典是：下跌/下降(fall):-0.6,衰退/低迷(downturn):-0.6"}, "成分股多数下跌，北方华创、福耀玻璃、美的集团、三一重工、盐湖股份、珀莱雅、京东方A、长江电力等股飘红": {"topic": "“金融”", "similarity": 0.6186586618423462, "prompt": "新闻文本是“成分股多数下跌，北方华创、福耀玻璃、美的集团、三一重工、盐湖股份、珀莱雅、京东方A、长江电力等股飘红”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "相关ETF方面，A50ETF基金（159592）截至发稿下跌0.83%，溢折率0.01%，盘中溢价": {"topic": "“金融”", "similarity": 0.48490673303604126, "prompt": "新闻文本是“相关ETF方面，A50ETF基金（159592）截至发稿下跌0.83%，溢折率0.01%，盘中溢价”，包含的情绪词典是：下跌/下降(fall):-0.6,向下/下跌(down):-0.4"}, "Wind数据显示，该ETF上一交易日净流入超1300万元，基金最新份额与流通规模分别为44.42亿份与42.50亿份，均创历史新高": {"topic": "“金融”", "similarity": 0.5575502514839172, "prompt": "新闻文本是“Wind数据显示，该ETF上一交易日净流入超1300万元，基金最新份额与流通规模分别为44.42亿份与42.50亿份，均创历史新高”，包含的情绪词典是：高估的/估价过高的(overvalued):-0.3,储备/囤积(stockpile):0.1"}, "消息面上，8月30日国务院常务会议召开，研究推动保险业高质量发展的若干意见": {"topic": "“金融”", "similarity": 0.6731834411621094, "prompt": "新闻文本是“消息面上，8月30日国务院常务会议召开，研究推动保险业高质量发展的若干意见”，包含的情绪词典是：保险不足的(underinsured):-0.3,风险(risk):-0.4"}, "会议指出，要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资": {"topic": "“金融”", "similarity": 0.6313339471817017, "prompt": "新闻文本是“会议指出，要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资”，包含的情绪词典是：资本/资金(capital):0.1,稳定/稳定性(stability):0.6"}, "中原证券表示，中央提出要“壮大耐心资本”，未来市场资金有望更稳定，投资方向更集中": {"topic": "“金融”", "similarity": 0.522362470626831, "prompt": "新闻文本是“中原证券表示，中央提出要“壮大耐心资本”，未来市场资金有望更稳定，投资方向更集中”，包含的情绪词典是：稳定的/稳固的(stable):0.5,资本/资金(capital):0.1"}, "虽然海内外经济政策和形势的变动较快，市场的波动性增高，但无论其市场价格怎么波动，假如资产能长期为投资者带来正向现金流，就具备长期投资潜力": {"topic": "“宏观经济”", "similarity": 0.6219465732574463, "prompt": "新闻文本是“虽然海内外经济政策和形势的变动较快，市场的波动性增高，但无论其市场价格怎么波动，假如资产能长期为投资者带来正向现金流，就具备长期投资潜力”，包含的情绪词典是：波动/起伏(fluctuate):-0.2,波动/起伏(fluctuates):-0.2"}, "中金公司指出，9月市场有望边际回稳，关注稳增长政策落地进度": {"topic": "“金融”", "similarity": 0.49822935461997986, "prompt": "新闻文本是“中金公司指出，9月市场有望边际回稳，关注稳增长政策落地进度”，包含的情绪词典是：稳定的/稳固的(stable):0.5,稳定/稳定性(stability):0.6"}, "近期7月工业企业利润、8月PMI数据陆续公布，均反映国内需求阶段性不强现状，需要稳增长政策发力支持": {"topic": "“宏观经济”", "similarity": 0.6633318066596985, "prompt": "新闻文本是“近期7月工业企业利润、8月PMI数据陆续公布，均反映国内需求阶段性不强现状，需要稳增长政策发力支持”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,衰退的/不景气的(recessionary):-0.8"}, "此外，9月美国降息预期抬升，全球资金有望迎来再配置，或利好中国资产": {"topic": "“金融”", "similarity": 0.5194092392921448, "prompt": "新闻文本是“此外，9月美国降息预期抬升，全球资金有望迎来再配置，或利好中国资产”，包含的情绪词典是：乐观的/看好的(optimistic):0.7,清仓/抛售(closeout):-0.2"}}</t>
         </is>
       </c>
     </row>
@@ -4915,12 +4875,12 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081，以下简称“金螳螂”）发布公告，计划新增为其合并报表范围内的子公司提供总额不超过6亿元人民币的担保", "news_prompt2": "此举旨在支持子公司金螳螂建筑装饰（马来西亚）有限公司、柬埔寨金瑞建筑装饰有限公司、金螳螂装饰中东有限责任公司的业务发展和融资需求", "news_prompt3": "公告同时披露：马来西亚金螳螂、柬埔寨金瑞装饰均为新设公司，尚未开展业务", "news_prompt4": "中东金螳螂 2023 年度实现营业收入 0 万元，净利润-8.56 万元，截止 2023 年 12 月 31 日，资产总额 20.86 万元，负债总额 857.21 万元，净资产-836.35 万元", "news_prompt5": "（以上数据已经审计）2024 年上半年实现营业收入 0 万元，净利润 0 万元，截止 2024 年 6月 30 日，资产总额 21.01 万元，负债总额 863.30 万元，净资产-842.29 万元", "news_prompt6": "（以上数据未经审计） 　　已审批通过的原有担保额度，加上本次拟提交公司股东大会审议的新增担保额度的担保事项全部生效后，公司累计对外担保总额不超过人民币 1,486,000 万元，占公司 2023 年末经审计总资产的 40.07%", "news_prompt7": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081，以下简称“金螳螂”）发布公告，计划新增为其合并报表范围内的子公司提供总额不超过6亿元人民币的担保", "news_prompt2": "此举旨在支持子公司金螳螂建筑装饰（马来西亚）有限公司、柬埔寨金瑞建筑装饰有限公司、金螳螂装饰中东有限责任公司的业务发展和融资需求", "news_prompt3": "公告同时披露：马来西亚金螳螂、柬埔寨金瑞装饰均为新设公司，尚未开展业务", "news_prompt4": "中东金螳螂 2023 年度实现营业收入 0 万元，净利润-8.56 万元，截止 2023 年 12 月 31 日，资产总额 20.86 万元，负债总额 857.21 万元，净资产-836.35 万元", "news_prompt5": "（以上数据已经审计）2024 年上半年实现营业收入 0 万元，净利润 0 万元，截止 2024 年 6月 30 日，资产总额 21.01 万元，负债总额 863.30 万元，净资产-842.29 万元", "news_prompt6": "（以上数据未经审计） 　　已审批通过的原有担保额度，加上本次拟提交公司股东大会审议的新增担保额度的担保事项全部生效后，公司累计对外担保总额不超过人民币 1,486,000 万元，占公司 2023 年末经审计总资产的 40.07%"}</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>{"2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081，以下简称“金螳螂”）发布公告，计划新增为其合并报表范围内的子公司提供总额不超过6亿元人民币的担保": {"topic": "“金融”", "similarity": 0.5495724081993103, "prompt": "新闻文本是“2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081，以下简称“金螳螂”）发布公告，计划新增为其合并报表范围内的子公司提供总额不超过6亿元人民币的担保”，包含的情绪词典是：保证/担保(surety):0.2"}, "此举旨在支持子公司金螳螂建筑装饰（马来西亚）有限公司、柬埔寨金瑞建筑装饰有限公司、金螳螂装饰中东有限责任公司的业务发展和融资需求": {"topic": "“金融”", "similarity": 0.4512825608253479, "prompt": "新闻文本是“此举旨在支持子公司金螳螂建筑装饰（马来西亚）有限公司、柬埔寨金瑞建筑装饰有限公司、金螳螂装饰中东有限责任公司的业务发展和融资需求”，包含的情绪词典是：附属的/子公司(subsidiary):0.0,投资/投资额(investment):0.4"}, "公告同时披露：马来西亚金螳螂、柬埔寨金瑞装饰均为新设公司，尚未开展业务": {"topic": "“金融”", "similarity": 0.4610634446144104, "prompt": "新闻文本是“公告同时披露：马来西亚金螳螂、柬埔寨金瑞装饰均为新设公司，尚未开展业务”，包含的情绪词典是：未报告的/未汇报的(unreported):-0.3,未实现的/未完成的(unfulfilled):-0.4"}, "中东金螳螂 2023 年度实现营业收入 0 万元，净利润-8.56 万元，截止 2023 年 12 月 31 日，资产总额 20.86 万元，负债总额 857.21 万元，净资产-836.35 万元": {"topic": "“生产投资”", "similarity": 0.505338728427887, "prompt": "新闻文本是“中东金螳螂 2023 年度实现营业收入 0 万元，净利润-8.56 万元，截止 2023 年 12 月 31 日，资产总额 20.86 万元，负债总额 857.21 万元，净资产-836.35 万元”，包含的情绪词典是：破产/无力偿还(insolvency):-0.7,破产的/无力偿还的(insolvent):-0.6"}, "（以上数据已经审计）2024 年上半年实现营业收入 0 万元，净利润 0 万元，截止 2024 年 6月 30 日，资产总额 21.01 万元，负债总额 863.30 万元，净资产-842.29 万元": {"topic": "“生产投资”", "similarity": 0.541817307472229, "prompt": "新闻文本是“（以上数据已经审计）2024 年上半年实现营业收入 0 万元，净利润 0 万元，截止 2024 年 6月 30 日，资产总额 21.01 万元，负债总额 863.30 万元，净资产-842.29 万元”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,负债的/欠债的(indebted):-0.5"}, "（以上数据未经审计） 　　已审批通过的原有担保额度，加上本次拟提交公司股东大会审议的新增担保额度的担保事项全部生效后，公司累计对外担保总额不超过人民币 1,486,000 万元，占公司 2023 年末经审计总资产的 40.07%": {"topic": "“金融”", "similarity": 0.5322660803794861, "prompt": "新闻文本是“（以上数据未经审计） 　　已审批通过的原有担保额度，加上本次拟提交公司股东大会审议的新增担保额度的担保事项全部生效后，公司累计对外担保总额不超过人民币 1,486,000 万元，占公司 2023 年末经审计总资产的 40.07%”，包含的情绪词典是：保证/担保(surety):0.2,偿债能力/偿付能力(solvency):0.3"}}</t>
+          <t>{"2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081，以下简称“金螳螂”）发布公告，计划新增为其合并报表范围内的子公司提供总额不超过6亿元人民币的担保": {"topic": "“金融”", "similarity": 0.5495724081993103, "prompt": "新闻文本是“2024年8月31日，苏州金螳螂建筑装饰股份有限公司（证券代码：002081，以下简称“金螳螂”）发布公告，计划新增为其合并报表范围内的子公司提供总额不超过6亿元人民币的担保”，包含的情绪词典是：保证/担保(surety):0.2"}, "此举旨在支持子公司金螳螂建筑装饰（马来西亚）有限公司、柬埔寨金瑞建筑装饰有限公司、金螳螂装饰中东有限责任公司的业务发展和融资需求": {"topic": "“金融”", "similarity": 0.4512826204299927, "prompt": "新闻文本是“此举旨在支持子公司金螳螂建筑装饰（马来西亚）有限公司、柬埔寨金瑞建筑装饰有限公司、金螳螂装饰中东有限责任公司的业务发展和融资需求”，包含的情绪词典是：附属的/子公司(subsidiary):0.0,投资/投资额(investment):0.4"}, "公告同时披露：马来西亚金螳螂、柬埔寨金瑞装饰均为新设公司，尚未开展业务": {"topic": "“金融”", "similarity": 0.46106356382369995, "prompt": "新闻文本是“公告同时披露：马来西亚金螳螂、柬埔寨金瑞装饰均为新设公司，尚未开展业务”，包含的情绪词典是：未报告的/未汇报的(unreported):-0.3,未实现的/未完成的(unfulfilled):-0.4"}, "中东金螳螂 2023 年度实现营业收入 0 万元，净利润-8.56 万元，截止 2023 年 12 月 31 日，资产总额 20.86 万元，负债总额 857.21 万元，净资产-836.35 万元": {"topic": "“生产投资”", "similarity": 0.505338728427887, "prompt": "新闻文本是“中东金螳螂 2023 年度实现营业收入 0 万元，净利润-8.56 万元，截止 2023 年 12 月 31 日，资产总额 20.86 万元，负债总额 857.21 万元，净资产-836.35 万元”，包含的情绪词典是：破产/无力偿还(insolvency):-0.7,破产的/无力偿还的(insolvent):-0.6"}, "（以上数据已经审计）2024 年上半年实现营业收入 0 万元，净利润 0 万元，截止 2024 年 6月 30 日，资产总额 21.01 万元，负债总额 863.30 万元，净资产-842.29 万元": {"topic": "“生产投资”", "similarity": 0.5418174266815186, "prompt": "新闻文本是“（以上数据已经审计）2024 年上半年实现营业收入 0 万元，净利润 0 万元，截止 2024 年 6月 30 日，资产总额 21.01 万元，负债总额 863.30 万元，净资产-842.29 万元”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,负债的/欠债的(indebted):-0.5"}, "（以上数据未经审计） 　　已审批通过的原有担保额度，加上本次拟提交公司股东大会审议的新增担保额度的担保事项全部生效后，公司累计对外担保总额不超过人民币 1,486,000 万元，占公司 2023 年末经审计总资产的 40.07%": {"topic": "“金融”", "similarity": 0.5322661399841309, "prompt": "新闻文本是“（以上数据未经审计） 　　已审批通过的原有担保额度，加上本次拟提交公司股东大会审议的新增担保额度的担保事项全部生效后，公司累计对外担保总额不超过人民币 1,486,000 万元，占公司 2023 年末经审计总资产的 40.07%”，包含的情绪词典是：保证/担保(surety):0.2,偿债能力/偿付能力(solvency):0.3"}}</t>
         </is>
       </c>
     </row>
@@ -4964,16 +4924,8 @@
           <t>21世纪经济报道</t>
         </is>
       </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>{"news_prompt1": "据央视新闻，马上就要迎来中秋节小长假了，9月1日旅客就可以购买中秋假期首日（9月15日）的火车票，目前售票情况如何，哪些地方是热门目的地", "news_prompt2": "记者在购票平台搜索发现，中秋节首日火车票开售仅30分钟，北京出发到武汉、郑州、长沙、成都到黄龙九寨等热门线路的多个车次车票已经售罄", "news_prompt3": "数据显示，中秋假期出游以短途游为主，江浙沪、广深、成渝2小时高铁圈旅客流动更频繁，热门短途线路有重庆-成都、北京-天津、广州-深圳、上海-苏州、上海-杭州、昆明-大理、济南-淄博、成都-乐山等，9月14日15时-22时，9月15日7时-11时是热门出行时段", "news_prompt4": "近期《黑神话：悟空》游戏走红带火了山西旅游，旅游平台数据显示，9月15日出发北京-太原的部分热门车次迅速售罄，近一周内，山西大同、朔州等游戏取景地的搜索热度和酒店预订热度增长迅猛", "news_prompt5": "（文章来源：21世纪经济报道）"}</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>{"据央视新闻，马上就要迎来中秋节小长假了，9月1日旅客就可以购买中秋假期首日（9月15日）的火车票，目前售票情况如何，哪些地方是热门目的地": {"topic": "“消费”", "similarity": 0.5437152981758118}, "记者在购票平台搜索发现，中秋节首日火车票开售仅30分钟，北京出发到武汉、郑州、长沙、成都到黄龙九寨等热门线路的多个车次车票已经售罄": {"topic": "“消费”", "similarity": 0.45615994930267334}, "数据显示，中秋假期出游以短途游为主，江浙沪、广深、成渝2小时高铁圈旅客流动更频繁，热门短途线路有重庆-成都、北京-天津、广州-深圳、上海-苏州、上海-杭州、昆明-大理、济南-淄博、成都-乐山等，9月14日15时-22时，9月15日7时-11时是热门出行时段": {"topic": "“消费”", "similarity": 0.5629373788833618}, "近期《黑神话：悟空》游戏走红带火了山西旅游，旅游平台数据显示，9月15日出发北京-太原的部分热门车次迅速售罄，近一周内，山西大同、朔州等游戏取景地的搜索热度和酒店预订热度增长迅猛": {"topic": "“消费”", "similarity": 0.5276815295219421}}</t>
-        </is>
-      </c>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -5017,12 +4969,12 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "中银证券09月02日发布研报称，给予世运电路（603920.SH，最新价：20.14元）增持评级", "news_prompt2": "评级理由主要包括：1）公司发布2024年半年报，2024H1公司订单旺盛，产量提升，同时产品结构进一步优化，收入利润双增", "news_prompt3": "2）订单旺盛+产品结构优化，公司上半年营收利润双增", "news_prompt4": "3）巩固业务发展基本盘，汽车业务量价齐升", "news_prompt5": "4）提前布局，助力AI业务发展", "news_prompt6": "风险提示：宏观经济波动导致供需关系变化的风险、行业产能大幅扩张、竞争激烈导致产品价格下降的风险、股权交割不确定的风险", "news_prompt7": "AI点评：世运电路近一个月获得3份券商研报关注，买入2家，平均目标价为21.84元，与最新价20.14元相比，高1.7元，目标均价涨幅8.44%", "news_prompt8": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "评级理由主要包括：1）公司发布2024年半年报，2024H1公司订单旺盛，产量提升，同时产品结构进一步优化，收入利润双增", "news_prompt2": "2）订单旺盛+产品结构优化，公司上半年营收利润双增", "news_prompt3": "3）巩固业务发展基本盘，汽车业务量价齐升"}</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>{"中银证券09月02日发布研报称，给予世运电路（603920.SH，最新价：20.14元）增持评级": {"topic": "“金融”", "similarity": 0.47109678387641907}, "评级理由主要包括：1）公司发布2024年半年报，2024H1公司订单旺盛，产量提升，同时产品结构进一步优化，收入利润双增": {"topic": "“生产投资”", "similarity": 0.5469223260879517, "prompt": "新闻文本是“评级理由主要包括：1）公司发布2024年半年报，2024H1公司订单旺盛，产量提升，同时产品结构进一步优化，收入利润双增”，包含的情绪词典是：多产的/富有成效的(productive):0.7,有利可图的/盈利的(profitable):0.8"}, "2）订单旺盛+产品结构优化，公司上半年营收利润双增": {"topic": "“生产投资”", "similarity": 0.44534751772880554, "prompt": "新闻文本是“2）订单旺盛+产品结构优化，公司上半年营收利润双增”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,利润/利益(profit):0.8"}, "3）巩固业务发展基本盘，汽车业务量价齐升": {"topic": "“消费”", "similarity": 0.46102556586265564, "prompt": "新闻文本是“3）巩固业务发展基本盘，汽车业务量价齐升”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}, "风险提示：宏观经济波动导致供需关系变化的风险、行业产能大幅扩张、竞争激烈导致产品价格下降的风险、股权交割不确定的风险": {"topic": "“金融”", "similarity": 0.626556396484375, "prompt": "新闻文本是“风险提示：宏观经济波动导致供需关系变化的风险、行业产能大幅扩张、竞争激烈导致产品价格下降的风险、股权交割不确定的风险”，包含的情绪词典是：风险(risk):-0.4,风险/危险(risks):-0.4"}, "AI点评：世运电路近一个月获得3份券商研报关注，买入2家，平均目标价为21.84元，与最新价20.14元相比，高1.7元，目标均价涨幅8.44%": {"topic": "“金融”", "similarity": 0.5412701368331909}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"评级理由主要包括：1）公司发布2024年半年报，2024H1公司订单旺盛，产量提升，同时产品结构进一步优化，收入利润双增": {"topic": "“生产投资”", "similarity": 0.5469224452972412, "prompt": "新闻文本是“评级理由主要包括：1）公司发布2024年半年报，2024H1公司订单旺盛，产量提升，同时产品结构进一步优化，收入利润双增”，包含的情绪词典是：多产的/富有成效的(productive):0.7,有利可图的/盈利的(profitable):0.8"}, "2）订单旺盛+产品结构优化，公司上半年营收利润双增": {"topic": "“生产投资”", "similarity": 0.44534748792648315, "prompt": "新闻文本是“2）订单旺盛+产品结构优化，公司上半年营收利润双增”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,利润/利益(profit):0.8"}, "3）巩固业务发展基本盘，汽车业务量价齐升": {"topic": "“消费”", "similarity": 0.4610257148742676, "prompt": "新闻文本是“3）巩固业务发展基本盘，汽车业务量价齐升”，包含的情绪词典是：汽车/轿车(car):0.0,汽车/机动车(automobile):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -5068,12 +5020,12 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "中银证券09月02日发布研报称，给予承德露露（000848.SZ，最新价：7.12元）买入评级", "news_prompt2": "评级理由主要包括：1）淡季营收增速亮眼，吨价增速快于销量", "news_prompt3": "2）成本压力下毛利率回落，销售费用投放力度加大", "news_prompt4": "3）公司成本红利有望逐季释放，全年来看营收目标有望达成", "news_prompt5": "风险提示：新周期原材料采购价格不及预期、新品拓展不及预期", "news_prompt6": "AI点评：承德露露近一个月获得4份券商研报关注，买入3家，增持1家", "news_prompt7": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "2）成本压力下毛利率回落，销售费用投放力度加大", "news_prompt2": "3）公司成本红利有望逐季释放，全年来看营收目标有望达成", "news_prompt3": "AI点评：承德露露近一个月获得4份券商研报关注，买入3家，增持1家"}</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>{"中银证券09月02日发布研报称，给予承德露露（000848.SZ，最新价：7.12元）买入评级": {"topic": "“金融”", "similarity": 0.43046504259109497, "prompt": "新闻文本是“中银证券09月02日发布研报称，给予承德露露（000848.SZ，最新价：7.12元）买入评级”，包含的情绪词典是：高估的/估价过高的(overvalued):-0.3,削价/低价出售(undercuts):-0.3"}, "2）成本压力下毛利率回落，销售费用投放力度加大": {"topic": "“消费”", "similarity": 0.5165209174156189, "prompt": "新闻文本是“2）成本压力下毛利率回落，销售费用投放力度加大”，包含的情绪词典是：使贬值/使减值(devalue):-0.4,削价/低价出售(undercuts):-0.3"}, "3）公司成本红利有望逐季释放，全年来看营收目标有望达成": {"topic": "“宏观经济”", "similarity": 0.4801623821258545, "prompt": "新闻文本是“3）公司成本红利有望逐季释放，全年来看营收目标有望达成”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,达到/实现(achieve):0.6"}, "风险提示：新周期原材料采购价格不及预期、新品拓展不及预期": {"topic": "“金融”", "similarity": 0.5261019468307495, "prompt": "新闻文本是“风险提示：新周期原材料采购价格不及预期、新品拓展不及预期”，包含的情绪词典是：风险(risk):-0.4,生产不足的/产量低于预期的(underproduced):-0.5"}, "AI点评：承德露露近一个月获得4份券商研报关注，买入3家，增持1家": {"topic": "“金融”", "similarity": 0.4909101724624634, "prompt": "新闻文本是“AI点评：承德露露近一个月获得4份券商研报关注，买入3家，增持1家”，包含的情绪词典是：股票/库存(stock):0.0,清仓/抛售(closeout):-0.2"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"2）成本压力下毛利率回落，销售费用投放力度加大": {"topic": "“消费”", "similarity": 0.5165210366249084, "prompt": "新闻文本是“2）成本压力下毛利率回落，销售费用投放力度加大”，包含的情绪词典是：使贬值/使减值(devalue):-0.4,削价/低价出售(undercuts):-0.3"}, "3）公司成本红利有望逐季释放，全年来看营收目标有望达成": {"topic": "“宏观经济”", "similarity": 0.4801625609397888, "prompt": "新闻文本是“3）公司成本红利有望逐季释放，全年来看营收目标有望达成”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,达到/实现(achieve):0.6"}, "AI点评：承德露露近一个月获得4份券商研报关注，买入3家，增持1家": {"topic": "“金融”", "similarity": 0.49091026186943054, "prompt": "新闻文本是“AI点评：承德露露近一个月获得4份券商研报关注，买入3家，增持1家”，包含的情绪词典是：股票/库存(stock):0.0,清仓/抛售(closeout):-0.2"}}</t>
         </is>
       </c>
     </row>
@@ -5119,12 +5071,12 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "每经AI快讯，电池板块快速拉升，南都电源20%涨停，科恒股份涨超9%，骆驼股份、天能股份、鹏辉能源、华宝新能等跟涨", "news_prompt2": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "每经AI快讯，电池板块快速拉升，南都电源20%涨停，科恒股份涨超9%，骆驼股份、天能股份、鹏辉能源、华宝新能等跟涨"}</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>{"每经AI快讯，电池板块快速拉升，南都电源20%涨停，科恒股份涨超9%，骆驼股份、天能股份、鹏辉能源、华宝新能等跟涨": {"topic": "“生产投资”", "similarity": 0.49714842438697815, "prompt": "新闻文本是“每经AI快讯，电池板块快速拉升，南都电源20%涨停，科恒股份涨超9%，骆驼股份、天能股份、鹏辉能源、华宝新能等跟涨”，包含的情绪词典是：电的/电气的(electrical):0.0,能源/精力(energy):0.3"}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"每经AI快讯，电池板块快速拉升，南都电源20%涨停，科恒股份涨超9%，骆驼股份、天能股份、鹏辉能源、华宝新能等跟涨": {"topic": "“生产投资”", "similarity": 0.49714845418930054, "prompt": "新闻文本是“每经AI快讯，电池板块快速拉升，南都电源20%涨停，科恒股份涨超9%，骆驼股份、天能股份、鹏辉能源、华宝新能等跟涨”，包含的情绪词典是：电的/电气的(electrical):0.0,能源/精力(energy):0.3"}}</t>
         </is>
       </c>
     </row>
@@ -5170,12 +5122,12 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "深交所9月2日公告，因京基金融国际实施股份合并，根据《深圳证券交易所深港通业务实施办法》的有关规定，港股通标的证券名单发生调整并自2024年9月2日起生效", "news_prompt2": "具体调整信息为：代码2977的京基金融国际被调入，代码1468的京基金融国际被调出", "news_prompt3": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "具体调整信息为：代码2977的京基金融国际被调入，代码1468的京基金融国际被调出"}</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>{"深交所9月2日公告，因京基金融国际实施股份合并，根据《深圳证券交易所深港通业务实施办法》的有关规定，港股通标的证券名单发生调整并自2024年9月2日起生效": {"topic": "“金融”", "similarity": 0.6380067467689514}, "具体调整信息为：代码2977的京基金融国际被调入，代码1468的京基金融国际被调出": {"topic": "“金融”", "similarity": 0.5629421472549438, "prompt": "新闻文本是“具体调整信息为：代码2977的京基金融国际被调入，代码1468的京基金融国际被调出”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,被取代的/被置换的(displaced):-0.4"}}</t>
+          <t>{"具体调整信息为：代码2977的京基金融国际被调入，代码1468的京基金融国际被调出": {"topic": "“金融”", "similarity": 0.5629421472549438, "prompt": "新闻文本是“具体调整信息为：代码2977的京基金融国际被调入，代码1468的京基金融国际被调出”，包含的情绪词典是：调控性的/监管性的(regulative):0.0,被取代的/被置换的(displaced):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -5221,12 +5173,12 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "2024年巴黎奥运会期间，韶关乐昌的黄金柰李爆火出圈，从韶关田间一跃成为奥运赛场上的明星美食", "news_prompt2": "印有“乐昌心意黄金柰李”精美包装的韶关乐昌黄金柰李横跨太平洋直达法国巴黎，在超市上以24.39欧元（约190.39元人民币）/2.5斤的价格销售，这是过去乐昌果农想都不敢想的事情", "news_prompt3": "在韶关银行业保险业的支持下，乐昌黄金柰李如今借由奥运热以英文名“gold plum”勇闯国际市场", "news_prompt4": "韶关金融监管分局坚持以“四新”工程为引领，坚持把服务实体经济作为根本宗旨，锚定“百千万工程”目标任务，引导韶关银行业保险业以金融活水促进农业高质高效、农民富裕富足，为韶关“三农”工作持续注入金融动能", "news_prompt5": "施足“金融底肥”，乡村产业搭上金融快车 　　推进“百千万工程”，农村是“主战场”“主阵地”", "news_prompt6": "韶关金融监管分局积极指导辖区金融机构加大涉农领域信贷投入，政银保企合力深耕“三农”工作，为特色农业产业发展施足“金融底肥”", "news_prompt7": "今年出口法国等欧盟国家的乐昌黄金柰李，产自乐昌市梅花镇百臻生态农业科技发展有限公司", "news_prompt8": "目前该公司拥有2000亩优质柰李种植基地，今年已先后出口两批黄金柰李到法国和荷兰", "news_prompt9": "为满足企业扩大种养规模、升级基础设施、购买生产资料等资金需求，助力乐昌柰李产业升级，银行采用信用追加企业名下知识产权专利权质押担保方式，向该企业授信并发放中期流动资金贷款500万元，帮助企业推广产品、扩大销售渠道，并为农户提供就业岗位及发展机会，实现带动本地农户共同致富", "news_prompt10": "目前正值柰李成熟季节，乐昌黄金柰李种植面积约4.4万亩，产量约6.6万吨，是广东最大的黄金柰李生产基地，同时也是中国黄金柰李原产地和核心区", "news_prompt11": "“年初企业订购了一批肥料，但是回款还要再等一段时间", "news_prompt12": "多亏乐昌农商行提供信贷资金及时帮助我们补齐资金缺口，没有耽误种植的好时机，才有这满满当当的黄金柰李”，韶关泰永鑫旅游开发有限公司负责人看着丰收的果实感慨道", "news_prompt13": "早在今年2月，该企业为抢抓春耕农时，需储备大量农资", "news_prompt14": "乐昌农商行“金融特派员”走访对接过程中，了解到企业的资金难题，主动对接、靠前服务，及时将信贷资金发放到位", "news_prompt15": "在该企业辐射带动下，当地村民年均收入增加到4.2万元，大大带动农民经济收益和再就业，有力推动韶关特色农业产业规模化、产业化、品牌化发展", "news_prompt16": "截至今年7月末，韶关辖区银行机构聚焦现代农业产业建设，重点服务好农、林、牧、渔业及产业链，已累计发放“菜篮子”“米袋子”“果盘子”“茶罐子”“水缸子”五大工程贷款4.9万笔、贷款余额48.34亿元", "news_prompt17": "韶关金融监管分局同时推动政银保企合力深耕“三农”工作，今年以来指导各支局主动联合当地相关部门召开9场金融支持“百千万工程”工作推进会暨融资对接会，积极推动金融资源进一步向县镇村倾斜、金融服务进一步向县镇村下沉", "news_prompt18": "截至今年7月末，韶关辖区普惠型涉农贷款余额209.03亿元、较年初增长9.04%，贷款余额户数36791户、较年初增长6.14%，银行机构当年累计发放的普惠型涉农贷款平均利率4.20%，较2023年平均水平下降0.26个百分点", "news_prompt19": "县域贷款余额1033.42亿元，同比增速10.67%，增速比全辖高2.57个百分点", "news_prompt20": "韶关辖区保险机构探索建立“以防为先”的农业保险服务体系，加大防灾减损资源投入，充分发挥保险风险管理和农险科技优势，助力“三农”风险减量", "news_prompt21": "截至今年7月末，辖区农业保险为农企农户提供60.45亿元风险保障，已决赔款2.06亿元，防预费支出51.65万元，最大限度降低极端天气和自然灾害对农业生产的影响", "news_prompt22": "金融赋能冷链物流，助力农产品领“鲜”出海 　　受高温环境和虫害等因素影响，黄金柰李曾一度面临无法大规模种植的困境，同时其生长周期相当短暂，且贮存期只有半个月到一个月，导致黄金柰李难以出口至海外市场", "news_prompt23": "长期以来，黄金柰李的发展受制于“酒香也怕巷子深”的困境中", "news_prompt24": "如今，黄金柰李从枝头采摘下来迅速打包装箱，到运送至广州白云国际机场，随即空运至法国，再上架至巴黎的超市供巴黎市民选购品尝，全程仅需不到两天时间，整个过程离不开冷链物流的保驾护航", "news_prompt25": "韶关金融监管分局指导辖区银行机构聚焦岭南水果销售难题，引导辖区金融机构主动对接农产品生产加工和冷链物流行业发展金融需求，不断优化金融产品和服务", "news_prompt26": "截至2024年7月末，韶关辖区银行机构累计向冷链物流企业提供贷款134笔，授信11.65亿元，贷款余额5.89亿元，为打通韶关农业产业发展“最后一公里”提供有力金融支持", "news_prompt27": "据悉，邮储银行韶关市分行以利率优惠大力支持广东兴顺佳集团有限公司转型升级，助力蔬菜冷链仓储及物流配送中心项目建设", "news_prompt28": "工商银行韶关分行为农户及农企等涉农经营实体创新开发信用贷款，推出“粤农e贷”和以应收账款质押的“政采贷”等专属贷款产品，最高额度可达500万元，目前已通过“粤农e贷”为韶关市顶猪食品有限"}</t>
+          <t>{"news_prompt1": "在韶关银行业保险业的支持下，乐昌黄金柰李如今借由奥运热以英文名“gold plum”勇闯国际市场", "news_prompt2": "韶关金融监管分局坚持以“四新”工程为引领，坚持把服务实体经济作为根本宗旨，锚定“百千万工程”目标任务，引导韶关银行业保险业以金融活水促进农业高质高效、农民富裕富足，为韶关“三农”工作持续注入金融动能", "news_prompt3": "施足“金融底肥”，乡村产业搭上金融快车 　　推进“百千万工程”，农村是“主战场”“主阵地”", "news_prompt4": "韶关金融监管分局积极指导辖区金融机构加大涉农领域信贷投入，政银保企合力深耕“三农”工作，为特色农业产业发展施足“金融底肥”", "news_prompt5": "目前该公司拥有2000亩优质柰李种植基地，今年已先后出口两批黄金柰李到法国和荷兰", "news_prompt6": "目前正值柰李成熟季节，乐昌黄金柰李种植面积约4.4万亩，产量约6.6万吨，是广东最大的黄金柰李生产基地，同时也是中国黄金柰李原产地和核心区", "news_prompt7": "“年初企业订购了一批肥料，但是回款还要再等一段时间", "news_prompt8": "多亏乐昌农商行提供信贷资金及时帮助我们补齐资金缺口，没有耽误种植的好时机，才有这满满当当的黄金柰李”，韶关泰永鑫旅游开发有限公司负责人看着丰收的果实感慨道", "news_prompt9": "乐昌农商行“金融特派员”走访对接过程中，了解到企业的资金难题，主动对接、靠前服务，及时将信贷资金发放到位", "news_prompt10": "在该企业辐射带动下，当地村民年均收入增加到4.2万元，大大带动农民经济收益和再就业，有力推动韶关特色农业产业规模化、产业化、品牌化发展", "news_prompt11": "截至今年7月末，韶关辖区银行机构聚焦现代农业产业建设，重点服务好农、林、牧、渔业及产业链，已累计发放“菜篮子”“米袋子”“果盘子”“茶罐子”“水缸子”五大工程贷款4.9万笔、贷款余额48.34亿元", "news_prompt12": "韶关金融监管分局同时推动政银保企合力深耕“三农”工作，今年以来指导各支局主动联合当地相关部门召开9场金融支持“百千万工程”工作推进会暨融资对接会，积极推动金融资源进一步向县镇村倾斜、金融服务进一步向县镇村下沉", "news_prompt13": "县域贷款余额1033.42亿元，同比增速10.67%，增速比全辖高2.57个百分点", "news_prompt14": "韶关辖区保险机构探索建立“以防为先”的农业保险服务体系，加大防灾减损资源投入，充分发挥保险风险管理和农险科技优势，助力“三农”风险减量", "news_prompt15": "截至今年7月末，辖区农业保险为农企农户提供60.45亿元风险保障，已决赔款2.06亿元，防预费支出51.65万元，最大限度降低极端天气和自然灾害对农业生产的影响", "news_prompt16": "韶关金融监管分局指导辖区银行机构聚焦岭南水果销售难题，引导辖区金融机构主动对接农产品生产加工和冷链物流行业发展金融需求，不断优化金融产品和服务", "news_prompt17": "截至2024年7月末，韶关辖区银行机构累计向冷链物流企业提供贷款134笔，授信11.65亿元，贷款余额5.89亿元，为打通韶关农业产业发展“最后一公里”提供有力金融支持", "news_prompt18": "据悉，邮储银行韶关市分行以利率优惠大力支持广东兴顺佳集团有限公司转型升级，助力蔬菜冷链仓储及物流配送中心项目建设", "news_prompt19": "工商银行韶关分行为农户及农企等涉农经营实体创新开发信用贷款，推出“粤农e贷”和以应收账款质押的“政采贷”等专属贷款产品，最高额度可达500万元，目前已通过“粤农e贷”为韶关市顶猪食品有限"}</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>{"2024年巴黎奥运会期间，韶关乐昌的黄金柰李爆火出圈，从韶关田间一跃成为奥运赛场上的明星美食": {"topic": "“消费”", "similarity": 0.42233139276504517}, "印有“乐昌心意黄金柰李”精美包装的韶关乐昌黄金柰李横跨太平洋直达法国巴黎，在超市上以24.39欧元（约190.39元人民币）/2.5斤的价格销售，这是过去乐昌果农想都不敢想的事情": {"topic": "“消费”", "similarity": 0.4455205798149109}, "在韶关银行业保险业的支持下，乐昌黄金柰李如今借由奥运热以英文名“gold plum”勇闯国际市场": {"topic": "“金融”", "similarity": 0.4330877959728241, "prompt": "新闻文本是“在韶关银行业保险业的支持下，乐昌黄金柰李如今借由奥运热以英文名“gold plum”勇闯国际市场”，包含的情绪词典是：有影响力的/有势力的(influential):0.4,金融的/财政的(financial):0.0"}, "韶关金融监管分局坚持以“四新”工程为引领，坚持把服务实体经济作为根本宗旨，锚定“百千万工程”目标任务，引导韶关银行业保险业以金融活水促进农业高质高效、农民富裕富足，为韶关“三农”工作持续注入金融动能": {"topic": "“宏观经济”", "similarity": 0.5929836630821228, "prompt": "新闻文本是“韶关金融监管分局坚持以“四新”工程为引领，坚持把服务实体经济作为根本宗旨，锚定“百千万工程”目标任务，引导韶关银行业保险业以金融活水促进农业高质高效、农民富裕富足，为韶关“三农”工作持续注入金融动能”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "施足“金融底肥”，乡村产业搭上金融快车 　　推进“百千万工程”，农村是“主战场”“主阵地”": {"topic": "“金融”", "similarity": 0.540086030960083, "prompt": "新闻文本是“施足“金融底肥”，乡村产业搭上金融快车 　　推进“百千万工程”，农村是“主战场”“主阵地””，包含的情绪词典是：领域/田地(field):0.0,金融的/财政的(financial):0.0"}, "韶关金融监管分局积极指导辖区金融机构加大涉农领域信贷投入，政银保企合力深耕“三农”工作，为特色农业产业发展施足“金融底肥”": {"topic": "“金融”", "similarity": 0.5090588927268982, "prompt": "新闻文本是“韶关金融监管分局积极指导辖区金融机构加大涉农领域信贷投入，政银保企合力深耕“三农”工作，为特色农业产业发展施足“金融底肥””，包含的情绪词典是：农业的/农学的(agricultural):0.0,金融的/财政的(financial):0.0"}, "目前该公司拥有2000亩优质柰李种植基地，今年已先后出口两批黄金柰李到法国和荷兰": {"topic": "“生产投资”", "similarity": 0.43010738492012024, "prompt": "新闻文本是“目前该公司拥有2000亩优质柰李种植基地，今年已先后出口两批黄金柰李到法国和荷兰”，包含的情绪词典是：出口/输出(export):0.0,植物/工厂(plant):0.0"}, "为满足企业扩大种养规模、升级基础设施、购买生产资料等资金需求，助力乐昌柰李产业升级，银行采用信用追加企业名下知识产权专利权质押担保方式，向该企业授信并发放中期流动资金贷款500万元，帮助企业推广产品、扩大销售渠道，并为农户提供就业岗位及发展机会，实现带动本地农户共同致富": {"topic": "“生产投资”", "similarity": 0.5894415378570557}, "目前正值柰李成熟季节，乐昌黄金柰李种植面积约4.4万亩，产量约6.6万吨，是广东最大的黄金柰李生产基地，同时也是中国黄金柰李原产地和核心区": {"topic": "“生产投资”", "similarity": 0.48752278089523315, "prompt": "新闻文本是“目前正值柰李成熟季节，乐昌黄金柰李种植面积约4.4万亩，产量约6.6万吨，是广东最大的黄金柰李生产基地，同时也是中国黄金柰李原产地和核心区”，包含的情绪词典是：植物/工厂(plant):0.0,作物/庄稼(crop):0.0"}, "“年初企业订购了一批肥料，但是回款还要再等一段时间": {"topic": "“生产投资”", "similarity": 0.45366376638412476, "prompt": "新闻文本是““年初企业订购了一批肥料，但是回款还要再等一段时间”，包含的情绪词典是：被延迟的/被耽搁的(delayed):-0.3,拖延的/延长的(protracted):0.0"}, "多亏乐昌农商行提供信贷资金及时帮助我们补齐资金缺口，没有耽误种植的好时机，才有这满满当当的黄金柰李”，韶关泰永鑫旅游开发有限公司负责人看着丰收的果实感慨道": {"topic": "“生产投资”", "similarity": 0.5134124159812927, "prompt": "新闻文本是“多亏乐昌农商行提供信贷资金及时帮助我们补齐资金缺口，没有耽误种植的好时机，才有这满满当当的黄金柰李”，韶关泰永鑫旅游开发有限公司负责人看着丰收的果实感慨道”，包含的情绪词典是：资金不足的(underfunded):-0.3,农业的/农学的(agricultural):0.0"}, "乐昌农商行“金融特派员”走访对接过程中，了解到企业的资金难题，主动对接、靠前服务，及时将信贷资金发放到位": {"topic": "“金融”", "similarity": 0.4933561086654663, "prompt": "新闻文本是“乐昌农商行“金融特派员”走访对接过程中，了解到企业的资金难题，主动对接、靠前服务，及时将信贷资金发放到位”，包含的情绪词典是：资金不足的(underfunded):-0.3,金钱上的(pecuniarily):0.0"}, "在该企业辐射带动下，当地村民年均收入增加到4.2万元，大大带动农民经济收益和再就业，有力推动韶关特色农业产业规模化、产业化、品牌化发展": {"topic": "“生产投资”", "similarity": 0.5752741098403931, "prompt": "新闻文本是“在该企业辐射带动下，当地村民年均收入增加到4.2万元，大大带动农民经济收益和再就业，有力推动韶关特色农业产业规模化、产业化、品牌化发展”，包含的情绪词典是：多产的/富有成效的(productive):0.7,农业的/农学的(agricultural):0.0"}, "截至今年7月末，韶关辖区银行机构聚焦现代农业产业建设，重点服务好农、林、牧、渔业及产业链，已累计发放“菜篮子”“米袋子”“果盘子”“茶罐子”“水缸子”五大工程贷款4.9万笔、贷款余额48.34亿元": {"topic": "“生产投资”", "similarity": 0.5570964813232422, "prompt": "新闻文本是“截至今年7月末，韶关辖区银行机构聚焦现代农业产业建设，重点服务好农、林、牧、渔业及产业链，已累计发放“菜篮子”“米袋子”“果盘子”“茶罐子”“水缸子”五大工程贷款4.9万笔、贷款余额48.34亿元”，包含的情绪词典是：农业的/农学的(agricultural):0.0,专款/专用款项(earmarks):0.0"}, "韶关金融监管分局同时推动政银保企合力深耕“三农”工作，今年以来指导各支局主动联合当地相关部门召开9场金融支持“百千万工程”工作推进会暨融资对接会，积极推动金融资源进一步向县镇村倾斜、金融服务进一步向县镇村下沉": {"topic": "“金融”", "similarity": 0.5701631307601929, "prompt": "新闻文本是“韶关金融监管分局同时推动政银保企合力深耕“三农”工作，今年以来指导各支局主动联合当地相关部门召开9场金融支持“百千万工程”工作推进会暨融资对接会，积极推动金融资源进一步向县镇村倾斜、金融服务进一步向县镇村下沉”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "截至今年7月末，韶关辖区普惠型涉农贷款余额209.03亿元、较年初增长9.04%，贷款余额户数36791户、较年初增长6.14%，银行机构当年累计发放的普惠型涉农贷款平均利率4.20%，较2023年平均水平下降0.26个百分点": {"topic": "“宏观经济”", "similarity": 0.5996640920639038}, "县域贷款余额1033.42亿元，同比增速10.67%，增速比全辖高2.57个百分点": {"topic": "“宏观经济”", "similarity": 0.49597036838531494, "prompt": "新闻文本是“县域贷款余额1033.42亿元，同比增速10.67%，增速比全辖高2.57个百分点”，包含的情绪词典是：百分比(percentage):0.0,投资/投资额(investment):0.4"}, "韶关辖区保险机构探索建立“以防为先”的农业保险服务体系，加大防灾减损资源投入，充分发挥保险风险管理和农险科技优势，助力“三农”风险减量": {"topic": "“金融”", "similarity": 0.49248766899108887, "prompt": "新闻文本是“韶关辖区保险机构探索建立“以防为先”的农业保险服务体系，加大防灾减损资源投入，充分发挥保险风险管理和农险科技优势，助力“三农”风险减量”，包含的情绪词典是：防止/预防(prevention):0.05,预防措施/防范(precaution):0.0"}, "截至今年7月末，辖区农业保险为农企农户提供60.45亿元风险保障，已决赔款2.06亿元，防预费支出51.65万元，最大限度降低极端天气和自然灾害对农业生产的影响": {"topic": "“消费”", "similarity": 0.5091893672943115, "prompt": "新闻文本是“截至今年7月末，辖区农业保险为农企农户提供60.45亿元风险保障，已决赔款2.06亿元，防预费支出51.65万元，最大限度降低极端天气和自然灾害对农业生产的影响”，包含的情绪词典是：农业的/农学的(agricultural):0.0,风险(risk):-0.4"}, "金融赋能冷链物流，助力农产品领“鲜”出海 　　受高温环境和虫害等因素影响，黄金柰李曾一度面临无法大规模种植的困境，同时其生长周期相当短暂，且贮存期只有半个月到一个月，导致黄金柰李难以出口至海外市场": {"topic": "“生产投资”", "similarity": 0.5306985974311829}, "如今，黄金柰李从枝头采摘下来迅速打包装箱，到运送至广州白云国际机场，随即空运至法国，再上架至巴黎的超市供巴黎市民选购品尝，全程仅需不到两天时间，整个过程离不开冷链物流的保驾护航": {"topic": "“消费”", "similarity": 0.4795956313610077}, "韶关金融监管分局指导辖区银行机构聚焦岭南水果销售难题，引导辖区金融机构主动对接农产品生产加工和冷链物流行业发展金融需求，不断优化金融产品和服务": {"topic": "“金融”", "similarity": 0.5386999845504761, "prompt": "新闻文本是“韶关金融监管分局指导辖区银行机构聚焦岭南水果销售难题，引导辖区金融机构主动对接农产品生产加工和冷链物流行业发展金融需求，不断优化金融产品和服务”，包含的情绪词典是：金融的/财政的(financial):0.0,农业的/农学的(agricultural):0.0"}, "截至2024年7月末，韶关辖区银行机构累计向冷链物流企业提供贷款134笔，授信11.65亿元，贷款余额5.89亿元，为打通韶关农业产业发展“最后一公里”提供有力金融支持": {"topic": "“宏观经济”", "similarity": 0.5349775552749634, "prompt": "新闻文本是“截至2024年7月末，韶关辖区银行机构累计向冷链物流企业提供贷款134笔，授信11.65亿元，贷款余额5.89亿元，为打通韶关农业产业发展“最后一公里”提供有力金融支持”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,专款/专用款项(earmarks):0.0"}, "据悉，邮储银行韶关市分行以利率优惠大力支持广东兴顺佳集团有限公司转型升级，助力蔬菜冷链仓储及物流配送中心项目建设": {"topic": "“金融”", "similarity": 0.5180540084838867, "prompt": "新闻文本是“据悉，邮储银行韶关市分行以利率优惠大力支持广东兴顺佳集团有限公司转型升级，助力蔬菜冷链仓储及物流配送中心项目建设”，包含的情绪词典是：优势/有利条件(advantage):0.7,有益的/有回报的(rewarding):0.5"}, "工商银行韶关分行为农户及农企等涉农经营实体创新开发信用贷款，推出“粤农e贷”和以应收账款质押的“政采贷”等专属贷款产品，最高额度可达500万元，目前已通过“粤农e贷”为韶关市顶猪食品有限": {"topic": "“生产投资”", "similarity": 0.5750964283943176, "prompt": "新闻文本是“工商银行韶关分行为农户及农企等涉农经营实体创新开发信用贷款，推出“粤农e贷”和以应收账款质押的“政采贷”等专属贷款产品，最高额度可达500万元，目前已通过“粤农e贷”为韶关市顶猪食品有限”，包含的情绪词典是：专款/专用款项(earmarks):0.0"}}</t>
+          <t>{"在韶关银行业保险业的支持下，乐昌黄金柰李如今借由奥运热以英文名“gold plum”勇闯国际市场": {"topic": "“金融”", "similarity": 0.43308788537979126, "prompt": "新闻文本是“在韶关银行业保险业的支持下，乐昌黄金柰李如今借由奥运热以英文名“gold plum”勇闯国际市场”，包含的情绪词典是：有影响力的/有势力的(influential):0.4,金融的/财政的(financial):0.0"}, "韶关金融监管分局坚持以“四新”工程为引领，坚持把服务实体经济作为根本宗旨，锚定“百千万工程”目标任务，引导韶关银行业保险业以金融活水促进农业高质高效、农民富裕富足，为韶关“三农”工作持续注入金融动能": {"topic": "“宏观经济”", "similarity": 0.5929837226867676, "prompt": "新闻文本是“韶关金融监管分局坚持以“四新”工程为引领，坚持把服务实体经济作为根本宗旨，锚定“百千万工程”目标任务，引导韶关银行业保险业以金融活水促进农业高质高效、农民富裕富足，为韶关“三农”工作持续注入金融动能”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "施足“金融底肥”，乡村产业搭上金融快车 　　推进“百千万工程”，农村是“主战场”“主阵地”": {"topic": "“金融”", "similarity": 0.5400862693786621, "prompt": "新闻文本是“施足“金融底肥”，乡村产业搭上金融快车 　　推进“百千万工程”，农村是“主战场”“主阵地””，包含的情绪词典是：领域/田地(field):0.0,金融的/财政的(financial):0.0"}, "韶关金融监管分局积极指导辖区金融机构加大涉农领域信贷投入，政银保企合力深耕“三农”工作，为特色农业产业发展施足“金融底肥”": {"topic": "“金融”", "similarity": 0.5090588927268982, "prompt": "新闻文本是“韶关金融监管分局积极指导辖区金融机构加大涉农领域信贷投入，政银保企合力深耕“三农”工作，为特色农业产业发展施足“金融底肥””，包含的情绪词典是：农业的/农学的(agricultural):0.0,金融的/财政的(financial):0.0"}, "目前该公司拥有2000亩优质柰李种植基地，今年已先后出口两批黄金柰李到法国和荷兰": {"topic": "“生产投资”", "similarity": 0.430107444524765, "prompt": "新闻文本是“目前该公司拥有2000亩优质柰李种植基地，今年已先后出口两批黄金柰李到法国和荷兰”，包含的情绪词典是：出口/输出(export):0.0,植物/工厂(plant):0.0"}, "目前正值柰李成熟季节，乐昌黄金柰李种植面积约4.4万亩，产量约6.6万吨，是广东最大的黄金柰李生产基地，同时也是中国黄金柰李原产地和核心区": {"topic": "“生产投资”", "similarity": 0.48752281069755554, "prompt": "新闻文本是“目前正值柰李成熟季节，乐昌黄金柰李种植面积约4.4万亩，产量约6.6万吨，是广东最大的黄金柰李生产基地，同时也是中国黄金柰李原产地和核心区”，包含的情绪词典是：植物/工厂(plant):0.0,作物/庄稼(crop):0.0"}, "“年初企业订购了一批肥料，但是回款还要再等一段时间": {"topic": "“生产投资”", "similarity": 0.4536638855934143, "prompt": "新闻文本是““年初企业订购了一批肥料，但是回款还要再等一段时间”，包含的情绪词典是：被延迟的/被耽搁的(delayed):-0.3,拖延的/延长的(protracted):0.0"}, "多亏乐昌农商行提供信贷资金及时帮助我们补齐资金缺口，没有耽误种植的好时机，才有这满满当当的黄金柰李”，韶关泰永鑫旅游开发有限公司负责人看着丰收的果实感慨道": {"topic": "“生产投资”", "similarity": 0.5134124159812927, "prompt": "新闻文本是“多亏乐昌农商行提供信贷资金及时帮助我们补齐资金缺口，没有耽误种植的好时机，才有这满满当当的黄金柰李”，韶关泰永鑫旅游开发有限公司负责人看着丰收的果实感慨道”，包含的情绪词典是：资金不足的(underfunded):-0.3,农业的/农学的(agricultural):0.0"}, "乐昌农商行“金融特派员”走访对接过程中，了解到企业的资金难题，主动对接、靠前服务，及时将信贷资金发放到位": {"topic": "“金融”", "similarity": 0.49335622787475586, "prompt": "新闻文本是“乐昌农商行“金融特派员”走访对接过程中，了解到企业的资金难题，主动对接、靠前服务，及时将信贷资金发放到位”，包含的情绪词典是：资金不足的(underfunded):-0.3,金钱上的(pecuniarily):0.0"}, "在该企业辐射带动下，当地村民年均收入增加到4.2万元，大大带动农民经济收益和再就业，有力推动韶关特色农业产业规模化、产业化、品牌化发展": {"topic": "“生产投资”", "similarity": 0.5752741098403931, "prompt": "新闻文本是“在该企业辐射带动下，当地村民年均收入增加到4.2万元，大大带动农民经济收益和再就业，有力推动韶关特色农业产业规模化、产业化、品牌化发展”，包含的情绪词典是：多产的/富有成效的(productive):0.7,农业的/农学的(agricultural):0.0"}, "截至今年7月末，韶关辖区银行机构聚焦现代农业产业建设，重点服务好农、林、牧、渔业及产业链，已累计发放“菜篮子”“米袋子”“果盘子”“茶罐子”“水缸子”五大工程贷款4.9万笔、贷款余额48.34亿元": {"topic": "“生产投资”", "similarity": 0.5570967197418213, "prompt": "新闻文本是“截至今年7月末，韶关辖区银行机构聚焦现代农业产业建设，重点服务好农、林、牧、渔业及产业链，已累计发放“菜篮子”“米袋子”“果盘子”“茶罐子”“水缸子”五大工程贷款4.9万笔、贷款余额48.34亿元”，包含的情绪词典是：农业的/农学的(agricultural):0.0,专款/专用款项(earmarks):0.0"}, "韶关金融监管分局同时推动政银保企合力深耕“三农”工作，今年以来指导各支局主动联合当地相关部门召开9场金融支持“百千万工程”工作推进会暨融资对接会，积极推动金融资源进一步向县镇村倾斜、金融服务进一步向县镇村下沉": {"topic": "“金融”", "similarity": 0.570163369178772, "prompt": "新闻文本是“韶关金融监管分局同时推动政银保企合力深耕“三农”工作，今年以来指导各支局主动联合当地相关部门召开9场金融支持“百千万工程”工作推进会暨融资对接会，积极推动金融资源进一步向县镇村倾斜、金融服务进一步向县镇村下沉”，包含的情绪词典是：金融的/财政的(financial):0.0,金融/财政(finance):0.0"}, "县域贷款余额1033.42亿元，同比增速10.67%，增速比全辖高2.57个百分点": {"topic": "“宏观经济”", "similarity": 0.4959705173969269, "prompt": "新闻文本是“县域贷款余额1033.42亿元，同比增速10.67%，增速比全辖高2.57个百分点”，包含的情绪词典是：百分比(percentage):0.0,投资/投资额(investment):0.4"}, "韶关辖区保险机构探索建立“以防为先”的农业保险服务体系，加大防灾减损资源投入，充分发挥保险风险管理和农险科技优势，助力“三农”风险减量": {"topic": "“金融”", "similarity": 0.49248769879341125, "prompt": "新闻文本是“韶关辖区保险机构探索建立“以防为先”的农业保险服务体系，加大防灾减损资源投入，充分发挥保险风险管理和农险科技优势，助力“三农”风险减量”，包含的情绪词典是：防止/预防(prevention):0.05,预防措施/防范(precaution):0.0"}, "截至今年7月末，辖区农业保险为农企农户提供60.45亿元风险保障，已决赔款2.06亿元，防预费支出51.65万元，最大限度降低极端天气和自然灾害对农业生产的影响": {"topic": "“消费”", "similarity": 0.5091893672943115, "prompt": "新闻文本是“截至今年7月末，辖区农业保险为农企农户提供60.45亿元风险保障，已决赔款2.06亿元，防预费支出51.65万元，最大限度降低极端天气和自然灾害对农业生产的影响”，包含的情绪词典是：农业的/农学的(agricultural):0.0,风险(risk):-0.4"}, "韶关金融监管分局指导辖区银行机构聚焦岭南水果销售难题，引导辖区金融机构主动对接农产品生产加工和冷链物流行业发展金融需求，不断优化金融产品和服务": {"topic": "“金融”", "similarity": 0.5387001633644104, "prompt": "新闻文本是“韶关金融监管分局指导辖区银行机构聚焦岭南水果销售难题，引导辖区金融机构主动对接农产品生产加工和冷链物流行业发展金融需求，不断优化金融产品和服务”，包含的情绪词典是：金融的/财政的(financial):0.0,农业的/农学的(agricultural):0.0"}, "截至2024年7月末，韶关辖区银行机构累计向冷链物流企业提供贷款134笔，授信11.65亿元，贷款余额5.89亿元，为打通韶关农业产业发展“最后一公里”提供有力金融支持": {"topic": "“宏观经济”", "similarity": 0.5349777936935425, "prompt": "新闻文本是“截至2024年7月末，韶关辖区银行机构累计向冷链物流企业提供贷款134笔，授信11.65亿元，贷款余额5.89亿元，为打通韶关农业产业发展“最后一公里”提供有力金融支持”，包含的情绪词典是：偿债能力/偿付能力(solvency):0.3,专款/专用款项(earmarks):0.0"}, "据悉，邮储银行韶关市分行以利率优惠大力支持广东兴顺佳集团有限公司转型升级，助力蔬菜冷链仓储及物流配送中心项目建设": {"topic": "“金融”", "similarity": 0.5180539488792419, "prompt": "新闻文本是“据悉，邮储银行韶关市分行以利率优惠大力支持广东兴顺佳集团有限公司转型升级，助力蔬菜冷链仓储及物流配送中心项目建设”，包含的情绪词典是：优势/有利条件(advantage):0.7,有益的/有回报的(rewarding):0.5"}, "工商银行韶关分行为农户及农企等涉农经营实体创新开发信用贷款，推出“粤农e贷”和以应收账款质押的“政采贷”等专属贷款产品，最高额度可达500万元，目前已通过“粤农e贷”为韶关市顶猪食品有限": {"topic": "“生产投资”", "similarity": 0.5750964283943176, "prompt": "新闻文本是“工商银行韶关分行为农户及农企等涉农经营实体创新开发信用贷款，推出“粤农e贷”和以应收账款质押的“政采贷”等专属贷款产品，最高额度可达500万元，目前已通过“粤农e贷”为韶关市顶猪食品有限”，包含的情绪词典是：专款/专用款项(earmarks):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -5272,12 +5224,12 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "【大河财立方消息】9月2日消息，工业和信息化部近日印发《工业中小企业管理提升指南（试行）》", "news_prompt2": "《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门", "news_prompt3": "《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引", "news_prompt4": "实施中坚持企业主体、需求导向，政府引导、协同联动，分类指导、分步实施等三项原则", "news_prompt5": "其中提到，引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力", "news_prompt6": "明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果", "news_prompt7": "建立清晰、详细的战略执行计划和监控评估机制，定期检查战略执行进度和效果，及时调整优化", "news_prompt8": "引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值", "news_prompt9": "基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距", "news_prompt10": "引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现", "news_prompt11": "积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围", "news_prompt12": "引导中小企业建立清晰公平的薪酬制度，明确薪酬政策依据、构成、差异的原因及调整机制，激发员工积极性和创造力", "news_prompt13": "为管理层、部门和员工设定明确工作目标、任务、责任和预期成果，并建立绩效评价机制，为高贡献、高技能人才制定个性化激励机制", "news_prompt14": "引导中小企业依法为员工提供“五险一金”", "news_prompt15": "统筹考虑企业实际情况和员工福利需求，逐步提供补充性保险和健康体检、节日福利、重大事件补助等员工福利，以及适度的文体设施，增强员工的归属感和认同感", "news_prompt16": "附全文： 工业中小企业管理提升指南（试行）　　习近平总书记多次强调“促进中小企业专精特新发展”“练好企业内功，特别是要提高经营能力、管理水平”", "news_prompt17": "党的二十届三中全会提出“支持和引导各类企业提高资源要素利用效率和经营管理水平”", "news_prompt18": "提高企业管理能力和水平，是推动中小企业内部挖潜、降本增效、防范风险的重要手段，是促进中小企业专精特新发展的内在需要，也是推进新型工业化建设的必然要求", "news_prompt19": "为贯彻落实党中央、国务院关于促进中小企业专精特新发展、推进新型工业化的决策部署，推动工业中小企业提升管理能力和水平，特制定《工业中小企业管理提升指南（试行）》（以下简称《指南》）", "news_prompt20": "一、总体要求 　　《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门", "news_prompt21": "《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引", "news_prompt22": "实施中坚持以下原则： 　　坚持企业主体、需求导向", "news_prompt23": "尊重市场经济规律和企业主体地位，以中小企业实际需求为导向，以企业管理存在问题为牵引，因企制宜推进中小企业管理提升工作", "news_prompt24": "坚持政府引导、协同联动", "news_prompt25": "充分发挥有为政府作用，加强政策支持、资源统筹和服务协同，推动形成多方参与、专业高效的工作格局，营造良好服务生态", "news_prompt26": "坚持分类指导、分步实施", "news_prompt27": "工业中小企业管理提升工作遵循由点及面、由易到难的思路，针对不同类型企业特点，分层分类分步实施，突出重点企业、重点领域，注重实效", "news_prompt28": "二、提升企业战略管理能力 　　（一）明确战略定位", "news_prompt29": "引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力", "news_prompt30": "明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果", "news_prompt31": "建立清晰、详细的战略执行计划和监控评估机制，定期检查战略执行进度和效果，及时调整优化", "news_prompt32": "（二）明晰市场定位", "news_prompt33": "引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值", "news_prompt34": "基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距", "news_prompt35": "（三）塑造企业文化", "news_prompt36": "引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现", "news_prompt37": "积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围", "news_prompt38": "三、提升企业人力资源管理能力 　　（一）保障关键岗位人员配备", "news_prompt39": "引导中小企业评估部门和岗位设置与企业发展匹配情况，建立招工、人才引进机制，招聘人员数量、结构、质量基本满足需求", "news_prompt40": "员工的技能、经验和资质与岗位要求基"}</t>
+          <t>{"news_prompt1": "【大河财立方消息】9月2日消息，工业和信息化部近日印发《工业中小企业管理提升指南（试行）》", "news_prompt2": "《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门", "news_prompt3": "《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引", "news_prompt4": "实施中坚持企业主体、需求导向，政府引导、协同联动，分类指导、分步实施等三项原则", "news_prompt5": "其中提到，引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力", "news_prompt6": "明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果", "news_prompt7": "引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值", "news_prompt8": "基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距", "news_prompt9": "引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现", "news_prompt10": "积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围", "news_prompt11": "引导中小企业建立清晰公平的薪酬制度，明确薪酬政策依据、构成、差异的原因及调整机制，激发员工积极性和创造力", "news_prompt12": "引导中小企业依法为员工提供“五险一金”", "news_prompt13": "统筹考虑企业实际情况和员工福利需求，逐步提供补充性保险和健康体检、节日福利、重大事件补助等员工福利，以及适度的文体设施，增强员工的归属感和认同感", "news_prompt14": "附全文： 工业中小企业管理提升指南（试行）　　习近平总书记多次强调“促进中小企业专精特新发展”“练好企业内功，特别是要提高经营能力、管理水平”", "news_prompt15": "党的二十届三中全会提出“支持和引导各类企业提高资源要素利用效率和经营管理水平”", "news_prompt16": "提高企业管理能力和水平，是推动中小企业内部挖潜、降本增效、防范风险的重要手段，是促进中小企业专精特新发展的内在需要，也是推进新型工业化建设的必然要求", "news_prompt17": "为贯彻落实党中央、国务院关于促进中小企业专精特新发展、推进新型工业化的决策部署，推动工业中小企业提升管理能力和水平，特制定《工业中小企业管理提升指南（试行）》（以下简称《指南》）", "news_prompt18": "一、总体要求 　　《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门", "news_prompt19": "《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引", "news_prompt20": "实施中坚持以下原则： 　　坚持企业主体、需求导向", "news_prompt21": "尊重市场经济规律和企业主体地位，以中小企业实际需求为导向，以企业管理存在问题为牵引，因企制宜推进中小企业管理提升工作", "news_prompt22": "坚持政府引导、协同联动", "news_prompt23": "充分发挥有为政府作用，加强政策支持、资源统筹和服务协同，推动形成多方参与、专业高效的工作格局，营造良好服务生态", "news_prompt24": "坚持分类指导、分步实施", "news_prompt25": "工业中小企业管理提升工作遵循由点及面、由易到难的思路，针对不同类型企业特点，分层分类分步实施，突出重点企业、重点领域，注重实效", "news_prompt26": "二、提升企业战略管理能力 　　（一）明确战略定位", "news_prompt27": "引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力", "news_prompt28": "明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果", "news_prompt29": "（二）明晰市场定位", "news_prompt30": "引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值", "news_prompt31": "基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距", "news_prompt32": "引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现", "news_prompt33": "积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围", "news_prompt34": "三、提升企业人力资源管理能力 　　（一）保障关键岗位人员配备", "news_prompt35": "引导中小企业评估部门和岗位设置与企业发展匹配情况，建立招工、人才引进机制，招聘人员数量、结构、质量基本满足需求", "news_prompt36": "员工的技能、经验和资质与岗位要求基"}</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>{"【大河财立方消息】9月2日消息，工业和信息化部近日印发《工业中小企业管理提升指南（试行）》": {"topic": "“生产投资”", "similarity": 0.5633765459060669, "prompt": "新闻文本是“【大河财立方消息】9月2日消息，工业和信息化部近日印发《工业中小企业管理提升指南（试行）》”，包含的情绪词典是：工业的/产业的(industrial):0.0,工业/产业(industry):0.0"}, "《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门": {"topic": "“生产投资”", "similarity": 0.647686779499054, "prompt": "新闻文本是“《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引": {"topic": "“生产投资”", "similarity": 0.4915046691894531, "prompt": "新闻文本是“《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引”，包含的情绪词典是：工业的/产业的(industrial):0.0,提供信息的/增长见闻的(informative):0.5"}, "实施中坚持企业主体、需求导向，政府引导、协同联动，分类指导、分步实施等三项原则": {"topic": "“生产投资”", "similarity": 0.5185019969940186, "prompt": "新闻文本是“实施中坚持企业主体、需求导向，政府引导、协同联动，分类指导、分步实施等三项原则”，包含的情绪词典是：公司/企业(firm):0.0,公司的/企业的(corporate):0.0"}, "其中提到，引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力": {"topic": "“生产投资”", "similarity": 0.5516548156738281, "prompt": "新闻文本是“其中提到，引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力”，包含的情绪词典是：公司/企业(company):0.0,企业/事业(enterprise):0.0"}, "明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果": {"topic": "“生产投资”", "similarity": 0.5429637432098389, "prompt": "新闻文本是“明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果”，包含的情绪词典是：公司/企业(firm):0.0,公司/企业(company):0.0"}, "引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值": {"topic": "“生产投资”", "similarity": 0.6074585914611816, "prompt": "新闻文本是“引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,盈利能力/获利能力(profitability):0.6"}, "基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距": {"topic": "“消费”", "similarity": 0.6108177900314331, "prompt": "新闻文本是“基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,优势/有利条件(advantage):0.7"}, "引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现": {"topic": "“生产投资”", "similarity": 0.4837614595890045, "prompt": "新闻文本是“引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现”，包含的情绪词典是：企业/事业(enterprise):0.0,公司/企业(firm):0.0"}, "积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围": {"topic": "“消费”", "similarity": 0.5041860938072205, "prompt": "新闻文本是“积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围”，包含的情绪词典是：活动/行动(activity):0.2,提供信息的/增长见闻的(informative):0.5"}, "引导中小企业建立清晰公平的薪酬制度，明确薪酬政策依据、构成、差异的原因及调整机制，激发员工积极性和创造力": {"topic": "“生产投资”", "similarity": 0.5918818116188049, "prompt": "新闻文本是“引导中小企业建立清晰公平的薪酬制度，明确薪酬政策依据、构成、差异的原因及调整机制，激发员工积极性和创造力”，包含的情绪词典是：工资/报酬(wage):0.0,报酬过低的/工资过低的(underpaid):-0.4"}, "引导中小企业依法为员工提供“五险一金”": {"topic": "“生产投资”", "similarity": 0.48518815636634827, "prompt": "新闻文本是“引导中小企业依法为员工提供“五险一金””，包含的情绪词典是：企业/事业(enterprise):0.0,合法的/法定的(lawful):0.3"}, "统筹考虑企业实际情况和员工福利需求，逐步提供补充性保险和健康体检、节日福利、重大事件补助等员工福利，以及适度的文体设施，增强员工的归属感和认同感": {"topic": "“生产投资”", "similarity": 0.5718382596969604, "prompt": "新闻文本是“统筹考虑企业实际情况和员工福利需求，逐步提供补充性保险和健康体检、节日福利、重大事件补助等员工福利，以及适度的文体设施，增强员工的归属感和认同感”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(company):0.0"}, "附全文： 工业中小企业管理提升指南（试行）　　习近平总书记多次强调“促进中小企业专精特新发展”“练好企业内功，特别是要提高经营能力、管理水平”": {"topic": "“生产投资”", "similarity": 0.6257044076919556, "prompt": "新闻文本是“附全文： 工业中小企业管理提升指南（试行）　　习近平总书记多次强调“促进中小企业专精特新发展”“练好企业内功，特别是要提高经营能力、管理水平””，包含的情绪词典是：工业的/产业的(industrial):0.0,工业/产业(industry):0.0"}, "党的二十届三中全会提出“支持和引导各类企业提高资源要素利用效率和经营管理水平”": {"topic": "“生产投资”", "similarity": 0.5777791142463684, "prompt": "新闻文本是“党的二十届三中全会提出“支持和引导各类企业提高资源要素利用效率和经营管理水平””，包含的情绪词典是：管理/经营(manage):0.2,效率/效能(efficiency):0.6"}, "提高企业管理能力和水平，是推动中小企业内部挖潜、降本增效、防范风险的重要手段，是促进中小企业专精特新发展的内在需要，也是推进新型工业化建设的必然要求": {"topic": "“生产投资”", "similarity": 0.6533380746841431, "prompt": "新闻文本是“提高企业管理能力和水平，是推动中小企业内部挖潜、降本增效、防范风险的重要手段，是促进中小企业专精特新发展的内在需要，也是推进新型工业化建设的必然要求”，包含的情绪词典是：增强/提高(enhancement):0.6,增强的/提高的(enhanced):0.6"}, "为贯彻落实党中央、国务院关于促进中小企业专精特新发展、推进新型工业化的决策部署，推动工业中小企业提升管理能力和水平，特制定《工业中小企业管理提升指南（试行）》（以下简称《指南》）": {"topic": "“生产投资”", "similarity": 0.6182966232299805, "prompt": "新闻文本是“为贯彻落实党中央、国务院关于促进中小企业专精特新发展、推进新型工业化的决策部署，推动工业中小企业提升管理能力和水平，特制定《工业中小企业管理提升指南（试行）》（以下简称《指南》）”，包含的情绪词典是：进步/提升(advancement):0.5,工业的/产业的(industrial):0.0"}, "一、总体要求 　　《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门": {"topic": "“生产投资”", "similarity": 0.6379719972610474, "prompt": "新闻文本是“一、总体要求 　　《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "实施中坚持以下原则： 　　坚持企业主体、需求导向": {"topic": "“生产投资”", "similarity": 0.521693229675293, "prompt": "新闻文本是“实施中坚持以下原则： 　　坚持企业主体、需求导向”，包含的情绪词典是：需求/要求(demand):0.0,坚持/坚决要求(insistence):0.0"}, "尊重市场经济规律和企业主体地位，以中小企业实际需求为导向，以企业管理存在问题为牵引，因企制宜推进中小企业管理提升工作": {"topic": "“生产投资”", "similarity": 0.5376196503639221, "prompt": "新闻文本是“尊重市场经济规律和企业主体地位，以中小企业实际需求为导向，以企业管理存在问题为牵引，因企制宜推进中小企业管理提升工作”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}, "坚持政府引导、协同联动": {"topic": "“生产投资”", "similarity": 0.49388033151626587, "prompt": "新闻文本是“坚持政府引导、协同联动”，包含的情绪词典是：政府/政体(government):0.0,联合的/共同的(joint):0.0"}, "充分发挥有为政府作用，加强政策支持、资源统筹和服务协同，推动形成多方参与、专业高效的工作格局，营造良好服务生态": {"topic": "“生产投资”", "similarity": 0.4855487048625946, "prompt": "新闻文本是“充分发挥有为政府作用，加强政策支持、资源统筹和服务协同，推动形成多方参与、专业高效的工作格局，营造良好服务生态”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,政府/政体(government):0.0"}, "坚持分类指导、分步实施": {"topic": "“宏观经济”", "similarity": 0.4398585557937622, "prompt": "新闻文本是“坚持分类指导、分步实施”，包含的情绪词典是：实施/执行(inforce):0.0,执行的/实施的(executory):0.0"}, "工业中小企业管理提升工作遵循由点及面、由易到难的思路，针对不同类型企业特点，分层分类分步实施，突出重点企业、重点领域，注重实效": {"topic": "“生产投资”", "similarity": 0.6121667623519897, "prompt": "新闻文本是“工业中小企业管理提升工作遵循由点及面、由易到难的思路，针对不同类型企业特点，分层分类分步实施，突出重点企业、重点领域，注重实效”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "二、提升企业战略管理能力 　　（一）明确战略定位": {"topic": "“生产投资”", "similarity": 0.48383551836013794, "prompt": "新闻文本是“二、提升企业战略管理能力 　　（一）明确战略定位”，包含的情绪词典是：公司/企业(firm):0.0,企业/事业(enterprise):0.0"}, "引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力": {"topic": "“生产投资”", "similarity": 0.5121883153915405, "prompt": "新闻文本是“引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力”，包含的情绪词典是：公司/企业(firm):0.0,公司/企业(company):0.0"}, "（二）明晰市场定位": {"topic": "“消费”", "similarity": 0.4814695715904236, "prompt": "新闻文本是“（二）明晰市场定位”，包含的情绪词典是：清晰地/明确地(clearly):0.0,清晰的/明确的(clear):0.1"}, "三、提升企业人力资源管理能力 　　（一）保障关键岗位人员配备": {"topic": "“生产投资”", "similarity": 0.46500444412231445, "prompt": "新闻文本是“三、提升企业人力资源管理能力 　　（一）保障关键岗位人员配备”，包含的情绪词典是：企业/事业(enterprise):0.0,增强/提高(enhancement):0.6"}, "引导中小企业评估部门和岗位设置与企业发展匹配情况，建立招工、人才引进机制，招聘人员数量、结构、质量基本满足需求": {"topic": "“生产投资”", "similarity": 0.5713885426521301, "prompt": "新闻文本是“引导中小企业评估部门和岗位设置与企业发展匹配情况，建立招工、人才引进机制，招聘人员数量、结构、质量基本满足需求”，包含的情绪词典是：招聘/招募(recruitment):0.0,劳动力/职工总数(workforce):0.01"}, "员工的技能、经验和资质与岗位要求基": {"topic": "“生产投资”", "similarity": 0.4616782069206238, "prompt": "新闻文本是“员工的技能、经验和资质与岗位要求基”，包含的情绪词典是：经验/经历(experience):0.2,基本的/基础的(basic):0.0"}}</t>
+          <t>{"【大河财立方消息】9月2日消息，工业和信息化部近日印发《工业中小企业管理提升指南（试行）》": {"topic": "“生产投资”", "similarity": 0.563376784324646, "prompt": "新闻文本是“【大河财立方消息】9月2日消息，工业和信息化部近日印发《工业中小企业管理提升指南（试行）》”，包含的情绪词典是：工业的/产业的(industrial):0.0,工业/产业(industry):0.0"}, "《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门": {"topic": "“生产投资”", "similarity": 0.6476868391036987, "prompt": "新闻文本是“《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引": {"topic": "“生产投资”", "similarity": 0.4915047585964203, "prompt": "新闻文本是“《指南》旨在帮助工业中小企业提高科学化规范化管理意识和水平，提升服务机构提供标准化规范化管理诊断咨询服务的能力，为各地推进中小企业管理诊断工作提供指引”，包含的情绪词典是：工业的/产业的(industrial):0.0,提供信息的/增长见闻的(informative):0.5"}, "实施中坚持企业主体、需求导向，政府引导、协同联动，分类指导、分步实施等三项原则": {"topic": "“生产投资”", "similarity": 0.5185021162033081, "prompt": "新闻文本是“实施中坚持企业主体、需求导向，政府引导、协同联动，分类指导、分步实施等三项原则”，包含的情绪词典是：公司/企业(firm):0.0,公司的/企业的(corporate):0.0"}, "其中提到，引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力": {"topic": "“生产投资”", "similarity": 0.5516549944877625, "prompt": "新闻文本是“其中提到，引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力”，包含的情绪词典是：公司/企业(company):0.0,企业/事业(enterprise):0.0"}, "明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果": {"topic": "“生产投资”", "similarity": 0.5429638624191284, "prompt": "新闻文本是“明确企业主业和发展方向，以及中长期战略目标和中短期工作目标、关键任务、责任分配、预期成果”，包含的情绪词典是：公司/企业(firm):0.0,公司/企业(company):0.0"}, "引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值": {"topic": "“生产投资”", "similarity": 0.607458770275116, "prompt": "新闻文本是“引导中小企业明确企业的核心竞争力，即产品能为客户解决什么痛点难点问题或者能为客户带来什么独特价值”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,盈利能力/获利能力(profitability):0.6"}, "基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距": {"topic": "“消费”", "similarity": 0.6108177900314331, "prompt": "新闻文本是“基于行业和地理位置、自身优势等因素，精准定位细分市场和潜在客户群体，明确主要竞争对手、对标标杆以及自身的优势差距”，包含的情绪词典是：竞争力/竞争能力(competitiveness):0.3,优势/有利条件(advantage):0.7"}, "引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现": {"topic": "“生产投资”", "similarity": 0.4837616980075836, "prompt": "新闻文本是“引导中小企业建立与企业使命、愿景、价值观相适应的企业文化，强化创新导向，并加强内部宣贯和外部展现”，包含的情绪词典是：企业/事业(enterprise):0.0,公司/企业(firm):0.0"}, "积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围": {"topic": "“消费”", "similarity": 0.5041862726211548, "prompt": "新闻文本是“积极组织知识分享、社会服务、文艺体育、团队拓展等方面的活动，营造尊重信任、积极向上、奋发进取的良好文化氛围”，包含的情绪词典是：活动/行动(activity):0.2,提供信息的/增长见闻的(informative):0.5"}, "引导中小企业建立清晰公平的薪酬制度，明确薪酬政策依据、构成、差异的原因及调整机制，激发员工积极性和创造力": {"topic": "“生产投资”", "similarity": 0.5918818116188049, "prompt": "新闻文本是“引导中小企业建立清晰公平的薪酬制度，明确薪酬政策依据、构成、差异的原因及调整机制，激发员工积极性和创造力”，包含的情绪词典是：工资/报酬(wage):0.0,报酬过低的/工资过低的(underpaid):-0.4"}, "引导中小企业依法为员工提供“五险一金”": {"topic": "“生产投资”", "similarity": 0.4851882755756378, "prompt": "新闻文本是“引导中小企业依法为员工提供“五险一金””，包含的情绪词典是：企业/事业(enterprise):0.0,合法的/法定的(lawful):0.3"}, "统筹考虑企业实际情况和员工福利需求，逐步提供补充性保险和健康体检、节日福利、重大事件补助等员工福利，以及适度的文体设施，增强员工的归属感和认同感": {"topic": "“生产投资”", "similarity": 0.5718383193016052, "prompt": "新闻文本是“统筹考虑企业实际情况和员工福利需求，逐步提供补充性保险和健康体检、节日福利、重大事件补助等员工福利，以及适度的文体设施，增强员工的归属感和认同感”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(company):0.0"}, "附全文： 工业中小企业管理提升指南（试行）　　习近平总书记多次强调“促进中小企业专精特新发展”“练好企业内功，特别是要提高经营能力、管理水平”": {"topic": "“生产投资”", "similarity": 0.6257044672966003, "prompt": "新闻文本是“附全文： 工业中小企业管理提升指南（试行）　　习近平总书记多次强调“促进中小企业专精特新发展”“练好企业内功，特别是要提高经营能力、管理水平””，包含的情绪词典是：工业的/产业的(industrial):0.0,工业/产业(industry):0.0"}, "党的二十届三中全会提出“支持和引导各类企业提高资源要素利用效率和经营管理水平”": {"topic": "“生产投资”", "similarity": 0.5777792930603027, "prompt": "新闻文本是“党的二十届三中全会提出“支持和引导各类企业提高资源要素利用效率和经营管理水平””，包含的情绪词典是：管理/经营(manage):0.2,效率/效能(efficiency):0.6"}, "提高企业管理能力和水平，是推动中小企业内部挖潜、降本增效、防范风险的重要手段，是促进中小企业专精特新发展的内在需要，也是推进新型工业化建设的必然要求": {"topic": "“生产投资”", "similarity": 0.6533380746841431, "prompt": "新闻文本是“提高企业管理能力和水平，是推动中小企业内部挖潜、降本增效、防范风险的重要手段，是促进中小企业专精特新发展的内在需要，也是推进新型工业化建设的必然要求”，包含的情绪词典是：增强/提高(enhancement):0.6,增强的/提高的(enhanced):0.6"}, "为贯彻落实党中央、国务院关于促进中小企业专精特新发展、推进新型工业化的决策部署，推动工业中小企业提升管理能力和水平，特制定《工业中小企业管理提升指南（试行）》（以下简称《指南》）": {"topic": "“生产投资”", "similarity": 0.61829674243927, "prompt": "新闻文本是“为贯彻落实党中央、国务院关于促进中小企业专精特新发展、推进新型工业化的决策部署，推动工业中小企业提升管理能力和水平，特制定《工业中小企业管理提升指南（试行）》（以下简称《指南》）”，包含的情绪词典是：进步/提升(advancement):0.5,工业的/产业的(industrial):0.0"}, "一、总体要求 　　《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门": {"topic": "“生产投资”", "similarity": 0.6379719972610474, "prompt": "新闻文本是“一、总体要求 　　《指南》主要面向工业中小企业特别是专精特新“小巨人”企业、专精特新中小企业、科技型和创新型中小企业，管理咨询服务机构和中小企业公共服务机构，地方各级中小企业主管部门”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "实施中坚持以下原则： 　　坚持企业主体、需求导向": {"topic": "“生产投资”", "similarity": 0.5216932892799377, "prompt": "新闻文本是“实施中坚持以下原则： 　　坚持企业主体、需求导向”，包含的情绪词典是：需求/要求(demand):0.0,坚持/坚决要求(insistence):0.0"}, "尊重市场经济规律和企业主体地位，以中小企业实际需求为导向，以企业管理存在问题为牵引，因企制宜推进中小企业管理提升工作": {"topic": "“生产投资”", "similarity": 0.5376197099685669, "prompt": "新闻文本是“尊重市场经济规律和企业主体地位，以中小企业实际需求为导向，以企业管理存在问题为牵引，因企制宜推进中小企业管理提升工作”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}, "坚持政府引导、协同联动": {"topic": "“生产投资”", "similarity": 0.4938802719116211, "prompt": "新闻文本是“坚持政府引导、协同联动”，包含的情绪词典是：政府/政体(government):0.0,联合的/共同的(joint):0.0"}, "充分发挥有为政府作用，加强政策支持、资源统筹和服务协同，推动形成多方参与、专业高效的工作格局，营造良好服务生态": {"topic": "“生产投资”", "similarity": 0.4855487644672394, "prompt": "新闻文本是“充分发挥有为政府作用，加强政策支持、资源统筹和服务协同，推动形成多方参与、专业高效的工作格局，营造良好服务生态”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,政府/政体(government):0.0"}, "坚持分类指导、分步实施": {"topic": "“宏观经济”", "similarity": 0.43985867500305176, "prompt": "新闻文本是“坚持分类指导、分步实施”，包含的情绪词典是：实施/执行(inforce):0.0,执行的/实施的(executory):0.0"}, "工业中小企业管理提升工作遵循由点及面、由易到难的思路，针对不同类型企业特点，分层分类分步实施，突出重点企业、重点领域，注重实效": {"topic": "“生产投资”", "similarity": 0.6121667623519897, "prompt": "新闻文本是“工业中小企业管理提升工作遵循由点及面、由易到难的思路，针对不同类型企业特点，分层分类分步实施，突出重点企业、重点领域，注重实效”，包含的情绪词典是：工业/产业(industry):0.0,工业的/产业的(industrial):0.0"}, "二、提升企业战略管理能力 　　（一）明确战略定位": {"topic": "“生产投资”", "similarity": 0.4838356077671051, "prompt": "新闻文本是“二、提升企业战略管理能力 　　（一）明确战略定位”，包含的情绪词典是：公司/企业(firm):0.0,企业/事业(enterprise):0.0"}, "引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力": {"topic": "“生产投资”", "similarity": 0.5121884346008301, "prompt": "新闻文本是“引导中小企业以长期可持续发展为导向，明确企业的使命、愿景、价值观，凝聚全体员工向心力”，包含的情绪词典是：公司/企业(firm):0.0,公司/企业(company):0.0"}, "（二）明晰市场定位": {"topic": "“消费”", "similarity": 0.48146969079971313, "prompt": "新闻文本是“（二）明晰市场定位”，包含的情绪词典是：清晰地/明确地(clearly):0.0,清晰的/明确的(clear):0.1"}, "三、提升企业人力资源管理能力 　　（一）保障关键岗位人员配备": {"topic": "“生产投资”", "similarity": 0.465004563331604, "prompt": "新闻文本是“三、提升企业人力资源管理能力 　　（一）保障关键岗位人员配备”，包含的情绪词典是：企业/事业(enterprise):0.0,增强/提高(enhancement):0.6"}, "引导中小企业评估部门和岗位设置与企业发展匹配情况，建立招工、人才引进机制，招聘人员数量、结构、质量基本满足需求": {"topic": "“生产投资”", "similarity": 0.5713886618614197, "prompt": "新闻文本是“引导中小企业评估部门和岗位设置与企业发展匹配情况，建立招工、人才引进机制，招聘人员数量、结构、质量基本满足需求”，包含的情绪词典是：招聘/招募(recruitment):0.0,劳动力/职工总数(workforce):0.01"}, "员工的技能、经验和资质与岗位要求基": {"topic": "“生产投资”", "similarity": 0.46167826652526855, "prompt": "新闻文本是“员工的技能、经验和资质与岗位要求基”，包含的情绪词典是：经验/经历(experience):0.2,基本的/基础的(basic):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -5323,12 +5275,12 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "9月2日上午，港股次新股嘀嗒出行持续拉升，现涨超31%", "news_prompt2": "公司上半年总收入4.04亿元", "news_prompt3": "经调整利润净额1.3亿元，同比增长51.3%", "news_prompt4": "（文章来源：界面新闻）"}</t>
+          <t>{"news_prompt1": "9月2日上午，港股次新股嘀嗒出行持续拉升，现涨超31%", "news_prompt2": "公司上半年总收入4.04亿元"}</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>{"9月2日上午，港股次新股嘀嗒出行持续拉升，现涨超31%": {"topic": "“金融”", "similarity": 0.4726751446723938, "prompt": "新闻文本是“9月2日上午，港股次新股嘀嗒出行持续拉升，现涨超31%”，包含的情绪词典是：上升/上涨(rise):0.5,上升的/占优势的(ascendant):0.3"}, "公司上半年总收入4.04亿元": {"topic": "“生产投资”", "similarity": 0.44129878282546997, "prompt": "新闻文本是“公司上半年总收入4.04亿元”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(firm):0.0"}}</t>
+          <t>{"9月2日上午，港股次新股嘀嗒出行持续拉升，现涨超31%": {"topic": "“金融”", "similarity": 0.4726753234863281, "prompt": "新闻文本是“9月2日上午，港股次新股嘀嗒出行持续拉升，现涨超31%”，包含的情绪词典是：上升/上涨(rise):0.5,上升的/占优势的(ascendant):0.3"}, "公司上半年总收入4.04亿元": {"topic": "“生产投资”", "similarity": 0.4412987530231476, "prompt": "新闻文本是“公司上半年总收入4.04亿元”，包含的情绪词典是：公司的/企业的(corporate):0.0,公司/企业(firm):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -5374,12 +5326,12 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "东莞证券09月02日发布研报称，给予中际旭创（300308.SZ，最新价：104.36元）买入评级", "news_prompt2": "评级理由主要包括：1）上半年业绩高速增长", "news_prompt3": "2）降本增效彰显公司优秀管理能力", "news_prompt4": "3）以太网用光模块更替需求在即", "news_prompt5": "4）T比特级/相干产品有望导入上量", "news_prompt6": "风险提示：需求不及预期", "news_prompt7": "行业竞争加剧", "news_prompt8": "高端产品利润率下降风险等", "news_prompt9": "AI点评：中际旭创近一个月获得9份券商研报关注，买入7家，平均目标价为150.76元，与最新价104.36元相比，高46.4元，目标均价涨幅44.46%", "news_prompt10": "（文章来源：每日经济新闻）"}</t>
+          <t>{"news_prompt1": "2）降本增效彰显公司优秀管理能力", "news_prompt2": "3）以太网用光模块更替需求在即", "news_prompt3": "4）T比特级/相干产品有望导入上量", "news_prompt4": "行业竞争加剧", "news_prompt5": "高端产品利润率下降风险等"}</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>{"东莞证券09月02日发布研报称，给予中际旭创（300308.SZ，最新价：104.36元）买入评级": {"topic": "“金融”", "similarity": 0.4941168427467346}, "2）降本增效彰显公司优秀管理能力": {"topic": "“生产投资”", "similarity": 0.4796581268310547, "prompt": "新闻文本是“2）降本增效彰显公司优秀管理能力”，包含的情绪词典是：公司/企业(company):0.0,管理/经营(manage):0.2"}, "3）以太网用光模块更替需求在即": {"topic": "“生产投资”", "similarity": 0.5098541378974915, "prompt": "新闻文本是“3）以太网用光模块更替需求在即”，包含的情绪词典是：需求/要求(demand):0.0,需要/需求(need):0.0"}, "4）T比特级/相干产品有望导入上量": {"topic": "“生产投资”", "similarity": 0.509259045124054, "prompt": "新闻文本是“4）T比特级/相干产品有望导入上量”，包含的情绪词典是：产品/产物(product):0.15,产量/输出(output):0.0"}, "风险提示：需求不及预期": {"topic": "“房地产”", "similarity": 0.5171370506286621, "prompt": "新闻文本是“风险提示：需求不及预期”，包含的情绪词典是：生产不足/产量低于预期(underproduction):-0.5,生产不足的/产量低于预期的(underproduced):-0.5"}, "行业竞争加剧": {"topic": "“生产投资”", "similarity": 0.5042920708656311, "prompt": "新闻文本是“行业竞争加剧”，包含的情绪词典是：竞赛/竞争(contestation):-0.1,竞争对手/敌手(rival):-0.3"}, "高端产品利润率下降风险等": {"topic": "“宏观经济”", "similarity": 0.5248177647590637, "prompt": "新闻文本是“高端产品利润率下降风险等”，包含的情绪词典是：风险(risk):-0.4,风险程度(riskines):-0.7"}, "AI点评：中际旭创近一个月获得9份券商研报关注，买入7家，平均目标价为150.76元，与最新价104.36元相比，高46.4元，目标均价涨幅44.46%": {"topic": "“金融”", "similarity": 0.5528229475021362}, "（文章来源：每日经济新闻）": {"topic": "“宏观经济”", "similarity": 0.4272976517677307, "prompt": "新闻文本是“（文章来源：每日经济新闻）”，包含的情绪词典是：经济/经济体(economy):0.0,通货膨胀(inflation):-0.5"}}</t>
+          <t>{"2）降本增效彰显公司优秀管理能力": {"topic": "“生产投资”", "similarity": 0.4796581268310547, "prompt": "新闻文本是“2）降本增效彰显公司优秀管理能力”，包含的情绪词典是：公司/企业(company):0.0,管理/经营(manage):0.2"}, "3）以太网用光模块更替需求在即": {"topic": "“生产投资”", "similarity": 0.5098540782928467, "prompt": "新闻文本是“3）以太网用光模块更替需求在即”，包含的情绪词典是：需求/要求(demand):0.0,需要/需求(need):0.0"}, "4）T比特级/相干产品有望导入上量": {"topic": "“生产投资”", "similarity": 0.5092591047286987, "prompt": "新闻文本是“4）T比特级/相干产品有望导入上量”，包含的情绪词典是：产品/产物(product):0.15,产量/输出(output):0.0"}, "行业竞争加剧": {"topic": "“生产投资”", "similarity": 0.5042921304702759, "prompt": "新闻文本是“行业竞争加剧”，包含的情绪词典是：竞赛/竞争(contestation):-0.1,竞争对手/敌手(rival):-0.3"}, "高端产品利润率下降风险等": {"topic": "“宏观经济”", "similarity": 0.5248178839683533, "prompt": "新闻文本是“高端产品利润率下降风险等”，包含的情绪词典是：风险(risk):-0.4,风险程度(riskines):-0.7"}}</t>
         </is>
       </c>
     </row>
@@ -5425,12 +5377,12 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "小雨淅沥，并没有影响广东三顺矿山机械制造有限公司（下称“三顺制造”）的生产进度", "news_prompt2": "将生产工厂从广州搬回五华，三顺制造负责人张育林直言不后悔", "news_prompt3": "“在五华发展产业，特别实在", "news_prompt4": "”今年前7月，三顺制造克服市场不利因素，营业额达千万元", "news_prompt5": "“下半年也在赶进度，力争今年营业额实现更大的增长", "news_prompt6": "” 　　作为广东五华经济开发区智能机械产业基地的一员，三顺制造的发展历程和五华县建设智能矿山机械产业基地建设息息相关", "news_prompt7": "结合产业发展基础和从事矿山机械制造行业的众多乡贤资源，五华县谋划建设五华智能矿山机械产业基地，不仅引进2家企业实现当年建设、当年投产、当年上规，还同步对接了数家矿山机械意向企业落户，积极培育新的经济增长点，深挖五华机械制造业“富矿”", "news_prompt8": "“希望有更多的上下游企业集聚在这里，一起做大做强五华机械制造业", "news_prompt9": "”张育林的话带着期盼，也带着公司奋斗的方向", "news_prompt10": "●南方日报记者黄培强通讯员曾文敏 　　从湾区到苏区 　　实现“三个当年” 　　三顺制造是华兴矿机旗下的制造基地", "news_prompt11": "品牌始创于1998年，是专业从事研发及制造大型破碎筛分成套设备、专业矿山设备及提供相关技术咨询的现代化高新技术企业", "news_prompt12": "说起三顺制造的发展历程，张育林随口便可以详细讲述", "news_prompt13": "作为见证人，他说：“从广州回到五华，是五华成就了三顺制造，而三顺制造也为五华发展作出了贡献", "news_prompt14": "” 　　2021年，从广州转移到五华的三顺制造，实现“当年拿地、当年建设、当年投产”的目标", "news_prompt15": "在张育林看来，这“三个当年”不简单", "news_prompt16": "“五华县委、县政府积极搭建平台，为企业提供政策支持、优质服务和良好的发展空间，全方位地支持让企业能够安心发展，专注于生产和创新", "news_prompt17": "” 　　毋庸置疑，三顺制造的快速发展，得益于五华县良好的营商环境和对乡贤回归的高度重视", "news_prompt18": "“项目总投资额约6000万元，待两期全面投产后，年产值可达1个亿", "news_prompt19": "”张育林说，该项目既有喜人的“财务报表”，更有亮眼的“社会报表”", "news_prompt20": "“解决当地的剩余劳动力，50多名员工大部分都是本地的", "news_prompt21": "” 　　任何一种产业的发展都有着历史和现实的原因", "news_prompt22": "制造业的发展，也要根据各自的资源禀赋和产业基础，因地制宜，打好特色牌、优势仗", "news_prompt23": "围绕做大做强机械制造业，根据产业发展趋势，五华依托传统制造行业的沉淀，优化产业结构，向机械制造业吹响“冲锋号角”", "news_prompt24": "位于广州番禺（五华）产业转移工业园西南侧，广东五华经济开发区智能机械产业基地便是生动实践之一", "news_prompt25": "按照规划，基地将打造成华南地区规模最大、专业聚集度最高、品种最齐全、竞争力强的智能机械产业基地", "news_prompt26": "广州番禺（五华）产业转移工业园相关负责人表示，政府主导先行实施“五通一平”建设工作，为后续企业拍地入驻提供必要的基础条件，建设标准厂房引进智能机械、装备制造等上下游产业链中小企业落户，培育智能机械产业集群，配套员工公寓和公共停车场，满足入驻企业必要的生活需求", "news_prompt27": "扩量提质增效 　　加快智能化生产 　　机器运转隆隆作响，工人们忙碌有序，广州番禺（五华）产业转移工业园里奏响“制造业当家”的五华声音", "news_prompt28": "三顺制造车间里，各类先进的生产设备有序运转，精准地完成每一道工序", "news_prompt29": "“主要生产颚式破碎机、反击式破碎机、多缸液压圆锥机、双轴高频振动筛、脱水筛、给料机、细沙提取机、螺旋洗砂机、轮式洗砂机、输送设备等，广泛适用于大型石矿场、码头和建筑垃圾破碎及筛分等", "news_prompt30": "”张育林说，生产设备更需要先进设备的支撑", "news_prompt31": "“这些设备代表着三顺制造的技术实力和创新精神", "news_prompt32": "” 　　近年来，为了满足市场需求，三顺制造不断加大研发投入，致力于提升产品的质量和性能，引入先进的技术和理念，对现有产品进行优化升级", "news_prompt33": "“同时，企业注重人才培养，吸引了一批高素质的技术人才和管理人才，为企业发展提供了坚实的人才保障", "news_prompt34": "”谈及公司发展思路，张育林用了六个字概括：扩量、提质、增效", "news_prompt35": "在扩量方面，三顺制造积极拓展市场，加大营销力度，加强与客户的沟通与合作，根据客户的需求提供个性化的解决方案，提高企业的知名度和产品的市场占有率", "news_prompt36": "提质是三顺制造始终坚持的发展理念", "news_prompt37": "企业严格把控产品质量，从原材料的采购到生产过程的每一个环节，都建立了严格的质量检测体系，确保每一台出厂的设备都符合国家标准和客户的要求", "news_prompt38": "同时，企业还积极推行质量管理体系认证，不断提升企业的质量管理水平", "news_prompt39": "增效是企业发展的重要目标", "news_prompt40": "对于引进先进的生产设备和管理经验，提高生产效率，降低生产成本，张育林深有感触", "news_prompt41": "来到一台机器旁，他饶有兴致介绍着：“这台折弯机器的引进，使得工作效率可以提高60%", "news_prompt42": "” 　　随着科技的不断进步，智能化生产已经成为制造业的发展趋势", "news_prompt43": "目前，三顺制造已经成为集研发设计、设备制造、生产运营、安装调试、售后无忧为一体的专业矿山机械制造商", "news_prompt44": "加快智能化生产，是三顺制造未来的发展方向", "news_prompt45": "“一步步来，设备要提高生产效率，产品要提高质量", "news_prompt46": "”张"}</t>
+          <t>{"news_prompt1": "“在五华发展产业，特别实在", "news_prompt2": "“下半年也在赶进度，力争今年营业额实现更大的增长", "news_prompt3": "” 　　作为广东五华经济开发区智能机械产业基地的一员，三顺制造的发展历程和五华县建设智能矿山机械产业基地建设息息相关", "news_prompt4": "“希望有更多的上下游企业集聚在这里，一起做大做强五华机械制造业", "news_prompt5": "”张育林的话带着期盼，也带着公司奋斗的方向", "news_prompt6": "品牌始创于1998年，是专业从事研发及制造大型破碎筛分成套设备、专业矿山设备及提供相关技术咨询的现代化高新技术企业", "news_prompt7": "“五华县委、县政府积极搭建平台，为企业提供政策支持、优质服务和良好的发展空间，全方位地支持让企业能够安心发展，专注于生产和创新", "news_prompt8": "“项目总投资额约6000万元，待两期全面投产后，年产值可达1个亿", "news_prompt9": "” 　　任何一种产业的发展都有着历史和现实的原因", "news_prompt10": "制造业的发展，也要根据各自的资源禀赋和产业基础，因地制宜，打好特色牌、优势仗", "news_prompt11": "围绕做大做强机械制造业，根据产业发展趋势，五华依托传统制造行业的沉淀，优化产业结构，向机械制造业吹响“冲锋号角”", "news_prompt12": "位于广州番禺（五华）产业转移工业园西南侧，广东五华经济开发区智能机械产业基地便是生动实践之一", "news_prompt13": "按照规划，基地将打造成华南地区规模最大、专业聚集度最高、品种最齐全、竞争力强的智能机械产业基地", "news_prompt14": "扩量提质增效 　　加快智能化生产 　　机器运转隆隆作响，工人们忙碌有序，广州番禺（五华）产业转移工业园里奏响“制造业当家”的五华声音", "news_prompt15": "”张育林说，生产设备更需要先进设备的支撑", "news_prompt16": "“这些设备代表着三顺制造的技术实力和创新精神", "news_prompt17": "” 　　近年来，为了满足市场需求，三顺制造不断加大研发投入，致力于提升产品的质量和性能，引入先进的技术和理念，对现有产品进行优化升级", "news_prompt18": "“同时，企业注重人才培养，吸引了一批高素质的技术人才和管理人才，为企业发展提供了坚实的人才保障", "news_prompt19": "”谈及公司发展思路，张育林用了六个字概括：扩量、提质、增效", "news_prompt20": "在扩量方面，三顺制造积极拓展市场，加大营销力度，加强与客户的沟通与合作，根据客户的需求提供个性化的解决方案，提高企业的知名度和产品的市场占有率", "news_prompt21": "提质是三顺制造始终坚持的发展理念", "news_prompt22": "企业严格把控产品质量，从原材料的采购到生产过程的每一个环节，都建立了严格的质量检测体系，确保每一台出厂的设备都符合国家标准和客户的要求", "news_prompt23": "增效是企业发展的重要目标", "news_prompt24": "” 　　随着科技的不断进步，智能化生产已经成为制造业的发展趋势", "news_prompt25": "目前，三顺制造已经成为集研发设计、设备制造、生产运营、安装调试、售后无忧为一体的专业矿山机械制造商", "news_prompt26": "加快智能化生产，是三顺制造未来的发展方向", "news_prompt27": "“一步步来，设备要提高生产效率，产品要提高质量"}</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>{"“在五华发展产业，特别实在": {"topic": "“生产投资”", "similarity": 0.48535701632499695, "prompt": "新闻文本是““在五华发展产业，特别实在”，包含的情绪词典是：实际的/真实的(actual):0.01,事实上/实际上(facto):0.0"}, "“下半年也在赶进度，力争今年营业额实现更大的增长": {"topic": "“生产投资”", "similarity": 0.47635141015052795, "prompt": "新闻文本是““下半年也在赶进度，力争今年营业额实现更大的增长”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "” 　　作为广东五华经济开发区智能机械产业基地的一员，三顺制造的发展历程和五华县建设智能矿山机械产业基地建设息息相关": {"topic": "“生产投资”", "similarity": 0.5410346388816833, "prompt": "新闻文本是“” 　　作为广东五华经济开发区智能机械产业基地的一员，三顺制造的发展历程和五华县建设智能矿山机械产业基地建设息息相关”，包含的情绪词典是：工业的/产业的(industrial):0.0,工业/产业(industry):0.0"}, "结合产业发展基础和从事矿山机械制造行业的众多乡贤资源，五华县谋划建设五华智能矿山机械产业基地，不仅引进2家企业实现当年建设、当年投产、当年上规，还同步对接了数家矿山机械意向企业落户，积极培育新的经济增长点，深挖五华机械制造业“富矿”": {"topic": "“生产投资”", "similarity": 0.5856994390487671}, "“希望有更多的上下游企业集聚在这里，一起做大做强五华机械制造业": {"topic": "“生产投资”", "similarity": 0.4812912940979004, "prompt": "新闻文本是““希望有更多的上下游企业集聚在这里，一起做大做强五华机械制造业”，包含的情绪词典是：机械/机器(machinery):0.0,工业/产业(industry):0.0"}, "”张育林的话带着期盼，也带着公司奋斗的方向": {"topic": "“生产投资”", "similarity": 0.47057491540908813, "prompt": "新闻文本是“”张育林的话带着期盼，也带着公司奋斗的方向”，包含的情绪词典是：期望的/想要的(desired):0.3,希望/期望(hope):0.5"}, "品牌始创于1998年，是专业从事研发及制造大型破碎筛分成套设备、专业矿山设备及提供相关技术咨询的现代化高新技术企业": {"topic": "“生产投资”", "similarity": 0.5227445960044861, "prompt": "新闻文本是“品牌始创于1998年，是专业从事研发及制造大型破碎筛分成套设备、专业矿山设备及提供相关技术咨询的现代化高新技术企业”，包含的情绪词典是：选矿/精选(beneficiation):0.4,技术的/工艺的(technical):0.0"}, "” 　　2021年，从广州转移到五华的三顺制造，实现“当年拿地、当年建设、当年投产”的目标": {"topic": "“生产投资”", "similarity": 0.5003372430801392}, "“五华县委、县政府积极搭建平台，为企业提供政策支持、优质服务和良好的发展空间，全方位地支持让企业能够安心发展，专注于生产和创新": {"topic": "“生产投资”", "similarity": 0.6330556273460388, "prompt": "新闻文本是““五华县委、县政府积极搭建平台，为企业提供政策支持、优质服务和良好的发展空间，全方位地支持让企业能够安心发展，专注于生产和创新”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}, "“项目总投资额约6000万元，待两期全面投产后，年产值可达1个亿": {"topic": "“生产投资”", "similarity": 0.5612166523933411, "prompt": "新闻文本是““项目总投资额约6000万元，待两期全面投产后，年产值可达1个亿”，包含的情绪词典是：投资/投资额(investment):0.4,多产的/富有成效的(productive):0.7"}, "” 　　任何一种产业的发展都有着历史和现实的原因": {"topic": "“生产投资”", "similarity": 0.5395311713218689, "prompt": "新闻文本是“” 　　任何一种产业的发展都有着历史和现实的原因”，包含的情绪词典是：原因/理由(reason):0.0,原因/理由(wherefore):0.0"}, "制造业的发展，也要根据各自的资源禀赋和产业基础，因地制宜，打好特色牌、优势仗": {"topic": "“生产投资”", "similarity": 0.6140984296798706, "prompt": "新闻文本是“制造业的发展，也要根据各自的资源禀赋和产业基础，因地制宜，打好特色牌、优势仗”，包含的情绪词典是：工业的/产业的(industrial):0.0,制造/生产(manufacture):0.0"}, "围绕做大做强机械制造业，根据产业发展趋势，五华依托传统制造行业的沉淀，优化产业结构，向机械制造业吹响“冲锋号角”": {"topic": "“生产投资”", "similarity": 0.5633334517478943, "prompt": "新闻文本是“围绕做大做强机械制造业，根据产业发展趋势，五华依托传统制造行业的沉淀，优化产业结构，向机械制造业吹响“冲锋号角””，包含的情绪词典是：机械/机器(machinery):0.0,工业的/产业的(industrial):0.0"}, "位于广州番禺（五华）产业转移工业园西南侧，广东五华经济开发区智能机械产业基地便是生动实践之一": {"topic": "“生产投资”", "similarity": 0.473733514547348, "prompt": "新闻文本是“位于广州番禺（五华）产业转移工业园西南侧，广东五华经济开发区智能机械产业基地便是生动实践之一”，包含的情绪词典是：机械/机器(machinery):0.0,工业的/产业的(industrial):0.0"}, "按照规划，基地将打造成华南地区规模最大、专业聚集度最高、品种最齐全、竞争力强的智能机械产业基地": {"topic": "“生产投资”", "similarity": 0.553911566734314, "prompt": "新闻文本是“按照规划，基地将打造成华南地区规模最大、专业聚集度最高、品种最齐全、竞争力强的智能机械产业基地”，包含的情绪词典是：机械/机器(machinery):0.0,工业/产业(industry):0.0"}, "广州番禺（五华）产业转移工业园相关负责人表示，政府主导先行实施“五通一平”建设工作，为后续企业拍地入驻提供必要的基础条件，建设标准厂房引进智能机械、装备制造等上下游产业链中小企业落户，培育智能机械产业集群，配套员工公寓和公共停车场，满足入驻企业必要的生活需求": {"topic": "“生产投资”", "similarity": 0.6221321225166321}, "扩量提质增效 　　加快智能化生产 　　机器运转隆隆作响，工人们忙碌有序，广州番禺（五华）产业转移工业园里奏响“制造业当家”的五华声音": {"topic": "“生产投资”", "similarity": 0.5916871428489685, "prompt": "新闻文本是“扩量提质增效 　　加快智能化生产 　　机器运转隆隆作响，工人们忙碌有序，广州番禺（五华）产业转移工业园里奏响“制造业当家”的五华声音”，包含的情绪词典是：工业的/产业的(industrial):0.0,多产的/富有成效的(productive):0.7"}, "“主要生产颚式破碎机、反击式破碎机、多缸液压圆锥机、双轴高频振动筛、脱水筛、给料机、细沙提取机、螺旋洗砂机、轮式洗砂机、输送设备等，广泛适用于大型石矿场、码头和建筑垃圾破碎及筛分等": {"topic": "“生产投资”", "similarity": 0.5517550110816956}, "”张育林说，生产设备更需要先进设备的支撑": {"topic": "“生产投资”", "similarity": 0.4629253149032593, "prompt": "新闻文本是“”张育林说，生产设备更需要先进设备的支撑”，包含的情绪词典是：生产/制造(produce):0.3,生产率/生产力(productivity):0.5"}, "“这些设备代表着三顺制造的技术实力和创新精神": {"topic": "“生产投资”", "similarity": 0.4328167140483856, "prompt": "新闻文本是““这些设备代表着三顺制造的技术实力和创新精神”，包含的情绪词典是：技术的/工艺的(technical):0.0,发明创造能力/创造力(inventiveness):0.4"}, "” 　　近年来，为了满足市场需求，三顺制造不断加大研发投入，致力于提升产品的质量和性能，引入先进的技术和理念，对现有产品进行优化升级": {"topic": "“生产投资”", "similarity": 0.5725831985473633, "prompt": "新闻文本是“” 　　近年来，为了满足市场需求，三顺制造不断加大研发投入，致力于提升产品的质量和性能，引入先进的技术和理念，对现有产品进行优化升级”，包含的情绪词典是：多产的/富有成效的(productive):0.7,前进/进步(advance):0.6"}, "“同时，企业注重人才培养，吸引了一批高素质的技术人才和管理人才，为企业发展提供了坚实的人才保障": {"topic": "“生产投资”", "similarity": 0.47853443026542664, "prompt": "新闻文本是““同时，企业注重人才培养，吸引了一批高素质的技术人才和管理人才，为企业发展提供了坚实的人才保障”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}, "”谈及公司发展思路，张育林用了六个字概括：扩量、提质、增效": {"topic": "“生产投资”", "similarity": 0.45797622203826904, "prompt": "新闻文本是“”谈及公司发展思路，张育林用了六个字概括：扩量、提质、增效”，包含的情绪词典是：增长/发展(growth):0.7,公司的/企业的(corporate):0.0"}, "在扩量方面，三顺制造积极拓展市场，加大营销力度，加强与客户的沟通与合作，根据客户的需求提供个性化的解决方案，提高企业的知名度和产品的市场占有率": {"topic": "“生产投资”", "similarity": 0.5667634010314941, "prompt": "新闻文本是“在扩量方面，三顺制造积极拓展市场，加大营销力度，加强与客户的沟通与合作，根据客户的需求提供个性化的解决方案，提高企业的知名度和产品的市场占有率”，包含的情绪词典是：生产/制造(produce):0.3,制造/生产(manufacture):0.0"}, "提质是三顺制造始终坚持的发展理念": {"topic": "“生产投资”", "similarity": 0.42267492413520813, "prompt": "新闻文本是“提质是三顺制造始终坚持的发展理念”，包含的情绪词典是：增强的/提高的(enhanced):0.6,生产/制造(produce):0.3"}, "企业严格把控产品质量，从原材料的采购到生产过程的每一个环节，都建立了严格的质量检测体系，确保每一台出厂的设备都符合国家标准和客户的要求": {"topic": "“生产投资”", "similarity": 0.5599492192268372, "prompt": "新闻文本是“企业严格把控产品质量，从原材料的采购到生产过程的每一个环节，都建立了严格的质量检测体系，确保每一台出厂的设备都符合国家标准和客户的要求”，包含的情绪词典是：严格的/严厉的(strict):-0.2,公司的/企业的(corporate):0.0"}, "增效是企业发展的重要目标": {"topic": "“生产投资”", "similarity": 0.5227967500686646, "prompt": "新闻文本是“增效是企业发展的重要目标”，包含的情绪词典是：增长/发展(growth):0.7,效率/效能(efficiency):0.6"}, "” 　　随着科技的不断进步，智能化生产已经成为制造业的发展趋势": {"topic": "“生产投资”", "similarity": 0.49410396814346313, "prompt": "新闻文本是“” 　　随着科技的不断进步，智能化生产已经成为制造业的发展趋势”，包含的情绪词典是：生产/产量(production):0.4,生产/制造(produce):0.3"}, "目前，三顺制造已经成为集研发设计、设备制造、生产运营、安装调试、售后无忧为一体的专业矿山机械制造商": {"topic": "“生产投资”", "similarity": 0.5137159824371338, "prompt": "新闻文本是“目前，三顺制造已经成为集研发设计、设备制造、生产运营、安装调试、售后无忧为一体的专业矿山机械制造商”，包含的情绪词典是：机械/机器(machinery):0.0,制造/生产(manufacture):0.0"}, "加快智能化生产，是三顺制造未来的发展方向": {"topic": "“生产投资”", "similarity": 0.48246142268180847, "prompt": "新闻文本是“加快智能化生产，是三顺制造未来的发展方向”，包含的情绪词典是：制造/生产(manufacture):0.0,生产/制造(produce):0.3"}, "“一步步来，设备要提高生产效率，产品要提高质量": {"topic": "“生产投资”", "similarity": 0.45981448888778687, "prompt": "新闻文本是““一步步来，设备要提高生产效率，产品要提高质量”，包含的情绪词典是：逐渐的/渐进的(gradual):0.1,正在改善的/正在改进的(improving):0.5"}}</t>
+          <t>{"“在五华发展产业，特别实在": {"topic": "“生产投资”", "similarity": 0.48535698652267456, "prompt": "新闻文本是““在五华发展产业，特别实在”，包含的情绪词典是：实际的/真实的(actual):0.01,事实上/实际上(facto):0.0"}, "“下半年也在赶进度，力争今年营业额实现更大的增长": {"topic": "“生产投资”", "similarity": 0.47635143995285034, "prompt": "新闻文本是““下半年也在赶进度，力争今年营业额实现更大的增长”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "” 　　作为广东五华经济开发区智能机械产业基地的一员，三顺制造的发展历程和五华县建设智能矿山机械产业基地建设息息相关": {"topic": "“生产投资”", "similarity": 0.5410346388816833, "prompt": "新闻文本是“” 　　作为广东五华经济开发区智能机械产业基地的一员，三顺制造的发展历程和五华县建设智能矿山机械产业基地建设息息相关”，包含的情绪词典是：工业的/产业的(industrial):0.0,工业/产业(industry):0.0"}, "“希望有更多的上下游企业集聚在这里，一起做大做强五华机械制造业": {"topic": "“生产投资”", "similarity": 0.48129141330718994, "prompt": "新闻文本是““希望有更多的上下游企业集聚在这里，一起做大做强五华机械制造业”，包含的情绪词典是：机械/机器(machinery):0.0,工业/产业(industry):0.0"}, "”张育林的话带着期盼，也带着公司奋斗的方向": {"topic": "“生产投资”", "similarity": 0.4705749750137329, "prompt": "新闻文本是“”张育林的话带着期盼，也带着公司奋斗的方向”，包含的情绪词典是：期望的/想要的(desired):0.3,希望/期望(hope):0.5"}, "品牌始创于1998年，是专业从事研发及制造大型破碎筛分成套设备、专业矿山设备及提供相关技术咨询的现代化高新技术企业": {"topic": "“生产投资”", "similarity": 0.5227445960044861, "prompt": "新闻文本是“品牌始创于1998年，是专业从事研发及制造大型破碎筛分成套设备、专业矿山设备及提供相关技术咨询的现代化高新技术企业”，包含的情绪词典是：选矿/精选(beneficiation):0.4,技术的/工艺的(technical):0.0"}, "“五华县委、县政府积极搭建平台，为企业提供政策支持、优质服务和良好的发展空间，全方位地支持让企业能够安心发展，专注于生产和创新": {"topic": "“生产投资”", "similarity": 0.6330555081367493, "prompt": "新闻文本是““五华县委、县政府积极搭建平台，为企业提供政策支持、优质服务和良好的发展空间，全方位地支持让企业能够安心发展，专注于生产和创新”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}, "“项目总投资额约6000万元，待两期全面投产后，年产值可达1个亿": {"topic": "“生产投资”", "similarity": 0.5612167716026306, "prompt": "新闻文本是““项目总投资额约6000万元，待两期全面投产后，年产值可达1个亿”，包含的情绪词典是：投资/投资额(investment):0.4,多产的/富有成效的(productive):0.7"}, "” 　　任何一种产业的发展都有着历史和现实的原因": {"topic": "“生产投资”", "similarity": 0.5395312309265137, "prompt": "新闻文本是“” 　　任何一种产业的发展都有着历史和现实的原因”，包含的情绪词典是：原因/理由(reason):0.0,原因/理由(wherefore):0.0"}, "制造业的发展，也要根据各自的资源禀赋和产业基础，因地制宜，打好特色牌、优势仗": {"topic": "“生产投资”", "similarity": 0.6140984296798706, "prompt": "新闻文本是“制造业的发展，也要根据各自的资源禀赋和产业基础，因地制宜，打好特色牌、优势仗”，包含的情绪词典是：工业的/产业的(industrial):0.0,制造/生产(manufacture):0.0"}, "围绕做大做强机械制造业，根据产业发展趋势，五华依托传统制造行业的沉淀，优化产业结构，向机械制造业吹响“冲锋号角”": {"topic": "“生产投资”", "similarity": 0.5633334517478943, "prompt": "新闻文本是“围绕做大做强机械制造业，根据产业发展趋势，五华依托传统制造行业的沉淀，优化产业结构，向机械制造业吹响“冲锋号角””，包含的情绪词典是：机械/机器(machinery):0.0,工业的/产业的(industrial):0.0"}, "位于广州番禺（五华）产业转移工业园西南侧，广东五华经济开发区智能机械产业基地便是生动实践之一": {"topic": "“生产投资”", "similarity": 0.4737336039543152, "prompt": "新闻文本是“位于广州番禺（五华）产业转移工业园西南侧，广东五华经济开发区智能机械产业基地便是生动实践之一”，包含的情绪词典是：机械/机器(machinery):0.0,工业的/产业的(industrial):0.0"}, "按照规划，基地将打造成华南地区规模最大、专业聚集度最高、品种最齐全、竞争力强的智能机械产业基地": {"topic": "“生产投资”", "similarity": 0.5539114475250244, "prompt": "新闻文本是“按照规划，基地将打造成华南地区规模最大、专业聚集度最高、品种最齐全、竞争力强的智能机械产业基地”，包含的情绪词典是：机械/机器(machinery):0.0,工业/产业(industry):0.0"}, "扩量提质增效 　　加快智能化生产 　　机器运转隆隆作响，工人们忙碌有序，广州番禺（五华）产业转移工业园里奏响“制造业当家”的五华声音": {"topic": "“生产投资”", "similarity": 0.5916870832443237, "prompt": "新闻文本是“扩量提质增效 　　加快智能化生产 　　机器运转隆隆作响，工人们忙碌有序，广州番禺（五华）产业转移工业园里奏响“制造业当家”的五华声音”，包含的情绪词典是：工业的/产业的(industrial):0.0,多产的/富有成效的(productive):0.7"}, "”张育林说，生产设备更需要先进设备的支撑": {"topic": "“生产投资”", "similarity": 0.46292534470558167, "prompt": "新闻文本是“”张育林说，生产设备更需要先进设备的支撑”，包含的情绪词典是：生产/制造(produce):0.3,生产率/生产力(productivity):0.5"}, "“这些设备代表着三顺制造的技术实力和创新精神": {"topic": "“生产投资”", "similarity": 0.4328168034553528, "prompt": "新闻文本是““这些设备代表着三顺制造的技术实力和创新精神”，包含的情绪词典是：技术的/工艺的(technical):0.0,发明创造能力/创造力(inventiveness):0.4"}, "” 　　近年来，为了满足市场需求，三顺制造不断加大研发投入，致力于提升产品的质量和性能，引入先进的技术和理念，对现有产品进行优化升级": {"topic": "“生产投资”", "similarity": 0.5725831985473633, "prompt": "新闻文本是“” 　　近年来，为了满足市场需求，三顺制造不断加大研发投入，致力于提升产品的质量和性能，引入先进的技术和理念，对现有产品进行优化升级”，包含的情绪词典是：多产的/富有成效的(productive):0.7,前进/进步(advance):0.6"}, "“同时，企业注重人才培养，吸引了一批高素质的技术人才和管理人才，为企业发展提供了坚实的人才保障": {"topic": "“生产投资”", "similarity": 0.47853466868400574, "prompt": "新闻文本是““同时，企业注重人才培养，吸引了一批高素质的技术人才和管理人才，为企业发展提供了坚实的人才保障”，包含的情绪词典是：企业/事业(enterprise):0.0,公司的/企业的(corporate):0.0"}, "”谈及公司发展思路，张育林用了六个字概括：扩量、提质、增效": {"topic": "“生产投资”", "similarity": 0.4579762816429138, "prompt": "新闻文本是“”谈及公司发展思路，张育林用了六个字概括：扩量、提质、增效”，包含的情绪词典是：增长/发展(growth):0.7,公司的/企业的(corporate):0.0"}, "在扩量方面，三顺制造积极拓展市场，加大营销力度，加强与客户的沟通与合作，根据客户的需求提供个性化的解决方案，提高企业的知名度和产品的市场占有率": {"topic": "“生产投资”", "similarity": 0.5667634606361389, "prompt": "新闻文本是“在扩量方面，三顺制造积极拓展市场，加大营销力度，加强与客户的沟通与合作，根据客户的需求提供个性化的解决方案，提高企业的知名度和产品的市场占有率”，包含的情绪词典是：生产/制造(produce):0.3,制造/生产(manufacture):0.0"}, "提质是三顺制造始终坚持的发展理念": {"topic": "“生产投资”", "similarity": 0.42267483472824097, "prompt": "新闻文本是“提质是三顺制造始终坚持的发展理念”，包含的情绪词典是：增强的/提高的(enhanced):0.6,生产/制造(produce):0.3"}, "企业严格把控产品质量，从原材料的采购到生产过程的每一个环节，都建立了严格的质量检测体系，确保每一台出厂的设备都符合国家标准和客户的要求": {"topic": "“生产投资”", "similarity": 0.5599493980407715, "prompt": "新闻文本是“企业严格把控产品质量，从原材料的采购到生产过程的每一个环节，都建立了严格的质量检测体系，确保每一台出厂的设备都符合国家标准和客户的要求”，包含的情绪词典是：严格的/严厉的(strict):-0.2,公司的/企业的(corporate):0.0"}, "增效是企业发展的重要目标": {"topic": "“生产投资”", "similarity": 0.5227968692779541, "prompt": "新闻文本是“增效是企业发展的重要目标”，包含的情绪词典是：增长/发展(growth):0.7,效率/效能(efficiency):0.6"}, "” 　　随着科技的不断进步，智能化生产已经成为制造业的发展趋势": {"topic": "“生产投资”", "similarity": 0.4941040873527527, "prompt": "新闻文本是“” 　　随着科技的不断进步，智能化生产已经成为制造业的发展趋势”，包含的情绪词典是：生产/产量(production):0.4,生产/制造(produce):0.3"}, "目前，三顺制造已经成为集研发设计、设备制造、生产运营、安装调试、售后无忧为一体的专业矿山机械制造商": {"topic": "“生产投资”", "similarity": 0.5137161016464233, "prompt": "新闻文本是“目前，三顺制造已经成为集研发设计、设备制造、生产运营、安装调试、售后无忧为一体的专业矿山机械制造商”，包含的情绪词典是：机械/机器(machinery):0.0,制造/生产(manufacture):0.0"}, "加快智能化生产，是三顺制造未来的发展方向": {"topic": "“生产投资”", "similarity": 0.4824616312980652, "prompt": "新闻文本是“加快智能化生产，是三顺制造未来的发展方向”，包含的情绪词典是：制造/生产(manufacture):0.0,生产/制造(produce):0.3"}, "“一步步来，设备要提高生产效率，产品要提高质量": {"topic": "“生产投资”", "similarity": 0.45981454849243164, "prompt": "新闻文本是““一步步来，设备要提高生产效率，产品要提高质量”，包含的情绪词典是：逐渐的/渐进的(gradual):0.1,正在改善的/正在改进的(improving):0.5"}}</t>
         </is>
       </c>
     </row>
@@ -5480,12 +5432,12 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "上证报中国证券网讯中国船舶日前披露的2024年半年度报告显示，报告期内，公司实现营业收入360.17亿元，同比增长17.99%，其中船舶造修及海洋工程业务营业收入344.46亿元，同比增长22.39%", "news_prompt2": "归属于上市公司股东的净利润14.12亿元，同比增长155.31%", "news_prompt3": "归属于上市公司股东的扣非净利润11.98亿元，同比扭亏为盈", "news_prompt4": "报告期内，公司手持订单结构改善，交付的民品船舶数量和单船平均价格同比提升，营业毛利同比增加", "news_prompt5": "公司参股联营企业盈利情况改善，权益法核算的长期股权投资收益同比增加2.63亿元", "news_prompt6": "研发方面，报告期内，中国船舶完成专利申请937项，其中发明专利843项", "news_prompt7": "授权专利236项，获得科技进步奖41项", "news_prompt8": "（鲁仪诗）（文章来源：上海证券报·中国证券网）"}</t>
+          <t>{"news_prompt1": "归属于上市公司股东的净利润14.12亿元，同比增长155.31%", "news_prompt2": "公司参股联营企业盈利情况改善，权益法核算的长期股权投资收益同比增加2.63亿元", "news_prompt3": "研发方面，报告期内，中国船舶完成专利申请937项，其中发明专利843项", "news_prompt4": "授权专利236项，获得科技进步奖41项"}</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>{"上证报中国证券网讯中国船舶日前披露的2024年半年度报告显示，报告期内，公司实现营业收入360.17亿元，同比增长17.99%，其中船舶造修及海洋工程业务营业收入344.46亿元，同比增长22.39%": {"topic": "“生产投资”", "similarity": 0.46500176191329956}, "归属于上市公司股东的净利润14.12亿元，同比增长155.31%": {"topic": "“金融”", "similarity": 0.42860162258148193, "prompt": "新闻文本是“归属于上市公司股东的净利润14.12亿元，同比增长155.31%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "公司参股联营企业盈利情况改善，权益法核算的长期股权投资收益同比增加2.63亿元": {"topic": "“金融”", "similarity": 0.4597300887107849, "prompt": "新闻文本是“公司参股联营企业盈利情况改善，权益法核算的长期股权投资收益同比增加2.63亿元”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,盈利能力/获利能力(profitability):0.6"}, "研发方面，报告期内，中国船舶完成专利申请937项，其中发明专利843项": {"topic": "“生产投资”", "similarity": 0.5014914274215698, "prompt": "新闻文本是“研发方面，报告期内，中国船舶完成专利申请937项，其中发明专利843项”，包含的情绪词典是：发明/创造(invention):0.4,发明/创造(invent):0.3"}, "授权专利236项，获得科技进步奖41项": {"topic": "“生产投资”", "similarity": 0.4848751127719879, "prompt": "新闻文本是“授权专利236项，获得科技进步奖41项”，包含的情绪词典是：技术(tech):0.0,专利权人(patentee):0.0"}, "（鲁仪诗）（文章来源：上海证券报·中国证券网）": {"topic": "“金融”", "similarity": 0.4445471167564392, "prompt": "新闻文本是“（鲁仪诗）（文章来源：上海证券报·中国证券网）”，包含的情绪词典是：投资者/投资人(investor):0.4,占有(权)(possessory):0.0"}}</t>
+          <t>{"归属于上市公司股东的净利润14.12亿元，同比增长155.31%": {"topic": "“金融”", "similarity": 0.4286017417907715, "prompt": "新闻文本是“归属于上市公司股东的净利润14.12亿元，同比增长155.31%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "公司参股联营企业盈利情况改善，权益法核算的长期股权投资收益同比增加2.63亿元": {"topic": "“金融”", "similarity": 0.4597301781177521, "prompt": "新闻文本是“公司参股联营企业盈利情况改善，权益法核算的长期股权投资收益同比增加2.63亿元”，包含的情绪词典是：有利可图的/盈利的(profitable):0.8,盈利能力/获利能力(profitability):0.6"}, "研发方面，报告期内，中国船舶完成专利申请937项，其中发明专利843项": {"topic": "“生产投资”", "similarity": 0.5014914274215698, "prompt": "新闻文本是“研发方面，报告期内，中国船舶完成专利申请937项，其中发明专利843项”，包含的情绪词典是：发明/创造(invention):0.4,发明/创造(invent):0.3"}, "授权专利236项，获得科技进步奖41项": {"topic": "“生产投资”", "similarity": 0.4848750829696655, "prompt": "新闻文本是“授权专利236项，获得科技进步奖41项”，包含的情绪词典是：技术(tech):0.0,专利权人(patentee):0.0"}}</t>
         </is>
       </c>
     </row>
@@ -5531,12 +5483,12 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "界面新闻记者｜马悦然 　　相较于去年上半年普遍两位数的净利降幅，今年上半年A股风电企业业绩有所好转", "news_prompt2": "在界面新闻不完全统计的六家主要风电整机商业绩中，两家龙头金风科技(002202.SZ)、明阳智能(601615.SH)上半年净利润实现同比增长，运达股份净利润微降0.54%", "news_prompt3": "去年上半年，金风科技净利降幅达34.82%、运达股份降幅49.75%、明阳智能降幅超73%", "news_prompt4": "作为中国第五大风电整机商，三一重能(688349.SH)上半年业绩增速则由增转降", "news_prompt5": "其今年上半年净利为4.34亿元，同比下降46.92%，在统计企业中同比下滑幅度最大", "news_prompt6": "其去年同期净利同比增2.38%", "news_prompt7": "主营业务较多的东方电气(600875.SH)，上半年净利额在统计企业中最高，但出现15.52%的同比下滑", "news_prompt8": "电气风电(688660.SH)则仍为亏损", "news_prompt9": "根据彭博新能源财经发布的2023年中国风电整机制造商排名，排名前七的企业分别为金风科技、远景能源、运达股份、明阳智能、三一重能、东方电气和电气风电", "news_prompt10": "数据来源：公司财报制图：马悦然  　　全球风电老大金风科技凭借海外及海上业务的开拓，净利润增速在上述企业中最高", "news_prompt11": "其上半年盈利13.87亿元，同比增长10.83%", "news_prompt12": "其中，二季度净利达10.54亿元，同比暴增6249%，去年同期净利仅为0.166亿元", "news_prompt13": "明阳智能上半年净利为6.61亿元，同比微增0.94%", "news_prompt14": "其中，一季度业绩同比增长两倍以上，但二季度同比下滑近六成", "news_prompt15": "上半年，明阳智能实现风机对外销售4.01 GW，对应实现风机及相关配件销售79.22亿元", "news_prompt16": "风机新增订单9.73 GW", "news_prompt17": "明阳智能陆上风机机型单机功率正在以3-4MW主力机型向5-8 MW机型推进", "news_prompt18": "海上风机机型单机功率从5.5 MW到6.45MW已经迭代到8 MW、11 MW、12 MW和更高的18 MW、22 MW机型", "news_prompt19": "同期，电站销售为明阳智能贡献了9.75亿元收入", "news_prompt20": "该公司目前在运营的新能源电站装机容量2.71 GW，在运营的新能源电站共实现发电量27.35亿千瓦时", "news_prompt21": "三一重能今年一、二季度净利润均同比下滑超四成", "news_prompt22": "一季度，该公司净利润2.66亿元，二季度环比下降近37%至1.68亿元", "news_prompt23": "上半年，三一重能93.97%的收入来自于风机及配件收入，去年同期这部分业务占比为75.78%", "news_prompt24": "相较之下，该公司风电建设服务收入占比大幅下滑，从去年上半年的近两成，降至不足3%，目前这部分营收为1.45亿元", "news_prompt25": "图片来源：三一重能财报  　　但环比看，三一重能的风机盈利能力有所提升", "news_prompt26": "上半年，其总体毛利率16.01%，较去年下半年增加4.82个百分点", "news_prompt27": "其中，风机业务毛利率15.13%，较去年下半年增加6.14个百分点，已连续两个季度改善", "news_prompt28": "今年上半年，三一重能陆上风机对外销售容量3.3 GW，同比增长121%，创造历史同期最好交付业绩", "news_prompt29": "海上风机方面，该公司称将力争下半年尽快实现突破", "news_prompt30": "另一陆上风机龙头运达股份业绩与去年上半年基本持平", "news_prompt31": "去年，在彭博新能源财经的中国风电整机制造商新增吊装容量排名中，运达股份再次重返前三，仅次于金风科技和远景能源", "news_prompt32": "上半年，运达股份实现对外销售容量约4.05 GW，同比上升19.25%", "news_prompt33": "报告期内，其新增订单14.29 GW，累计在手订单34.2 GW", "news_prompt34": "运达股份披露的各产品毛利率均有所下滑，其中风电机组毛利率10.34%，同比下滑5.52个百分点", "news_prompt35": "即使发电收入毛利率下滑11.08个百分点，但依然高达56.11%，在所有产品中最高", "news_prompt36": "在风机价格内卷、利润率持续低迷的情况下，风电场开发、电站销售成了风电整机商新的业绩增长点", "news_prompt37": "海上风电龙头电气风电(688660.SH)业绩仍维持亏损状态，上半年亏损3.87亿元，在被统计企业中垫底，亏损额同比减少1.78%", "news_prompt38": "去年，该公司的海上霸主地位被明阳智能取代，跌至第二", "news_prompt39": "上半年，电气风电新增订单为3.2 GW，较上年同期增长113.71%，其中已中标尚未签订合同的订单为1.42 GW", "news_prompt40": "截至6月底，电气风电累计在手订单为11.51 GW，较上年同期增加了21.99%，其中已中标尚未签订合同的订单为2.14 GW", "news_prompt41": "此外，电气风电在印尼等地实现零突破，取得部分订单", "news_prompt42": "在风资源开发方面，电气风电自持风场产生的发电收入为0.48亿元，较去年同期增长36.92%", "news_prompt43": "电气风电称，已经采取切换陆上产品技术路线、海上产品大型化升级、管理优化等多项措施应对市场挑战，但若后续风机市场招标价格仍持续大幅快速下降，而公司无法保证产品成本随销售价格同步下降，或因部分产品未来可能受较为恶劣工作环境等因素影响产生质量问题，对经营业绩产生不利影响，公司业绩仍可能存在亏损的风险", "news_prompt44": "该公司表示，将重点在陆上大基"}</t>
+          <t>{"news_prompt1": "去年上半年，金风科技净利降幅达34.82%、运达股份降幅49.75%、明阳智能降幅超73%", "news_prompt2": "作为中国第五大风电整机商，三一重能(688349.SH)上半年业绩增速则由增转降", "news_prompt3": "其今年上半年净利为4.34亿元，同比下降46.92%，在统计企业中同比下滑幅度最大", "news_prompt4": "数据来源：公司财报制图：马悦然  　　全球风电老大金风科技凭借海外及海上业务的开拓，净利润增速在上述企业中最高", "news_prompt5": "其中，二季度净利达10.54亿元，同比暴增6249%，去年同期净利仅为0.166亿元", "news_prompt6": "明阳智能上半年净利为6.61亿元，同比微增0.94%", "news_prompt7": "上半年，明阳智能实现风机对外销售4.01 GW，对应实现风机及相关配件销售79.22亿元", "news_prompt8": "三一重能今年一、二季度净利润均同比下滑超四成", "news_prompt9": "上半年，三一重能93.97%的收入来自于风机及配件收入，去年同期这部分业务占比为75.78%", "news_prompt10": "相较之下，该公司风电建设服务收入占比大幅下滑，从去年上半年的近两成，降至不足3%，目前这部分营收为1.45亿元", "news_prompt11": "今年上半年，三一重能陆上风机对外销售容量3.3 GW，同比增长121%，创造历史同期最好交付业绩", "news_prompt12": "另一陆上风机龙头运达股份业绩与去年上半年基本持平", "news_prompt13": "上半年，运达股份实现对外销售容量约4.05 GW，同比上升19.25%", "news_prompt14": "运达股份披露的各产品毛利率均有所下滑，其中风电机组毛利率10.34%，同比下滑5.52个百分点", "news_prompt15": "在风机价格内卷、利润率持续低迷的情况下，风电场开发、电站销售成了风电整机商新的业绩增长点", "news_prompt16": "海上风电龙头电气风电(688660.SH)业绩仍维持亏损状态，上半年亏损3.87亿元，在被统计企业中垫底，亏损额同比减少1.78%", "news_prompt17": "上半年，电气风电新增订单为3.2 GW，较上年同期增长113.71%，其中已中标尚未签订合同的订单为1.42 GW", "news_prompt18": "截至6月底，电气风电累计在手订单为11.51 GW，较上年同期增加了21.99%，其中已中标尚未签订合同的订单为2.14 GW", "news_prompt19": "在风资源开发方面，电气风电自持风场产生的发电收入为0.48亿元，较去年同期增长36.92%", "news_prompt20": "电气风电称，已经采取切换陆上产品技术路线、海上产品大型化升级、管理优化等多项措施应对市场挑战，但若后续风机市场招标价格仍持续大幅快速下降，而公司无法保证产品成本随销售价格同步下降，或因部分产品未来可能受较为恶劣工作环境等因素影响产生质量问题，对经营业绩产生不利影响，公司业绩仍可能存在亏损的风险"}</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>{"在界面新闻不完全统计的六家主要风电整机商业绩中，两家龙头金风科技(002202.SZ)、明阳智能(601615.SH)上半年净利润实现同比增长，运达股份净利润微降0.54%": {"topic": "“生产投资”", "similarity": 0.521571159362793}, "去年上半年，金风科技净利降幅达34.82%、运达股份降幅49.75%、明阳智能降幅超73%": {"topic": "“金融”", "similarity": 0.49998292326927185, "prompt": "新闻文本是“去年上半年，金风科技净利降幅达34.82%、运达股份降幅49.75%、明阳智能降幅超73%”，包含的情绪词典是：下跌/下降(fall):-0.6,下降的/衰退的(declining):-0.6"}, "作为中国第五大风电整机商，三一重能(688349.SH)上半年业绩增速则由增转降": {"topic": "“生产投资”", "similarity": 0.4602355659008026, "prompt": "新闻文本是“作为中国第五大风电整机商，三一重能(688349.SH)上半年业绩增速则由增转降”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "其今年上半年净利为4.34亿元，同比下降46.92%，在统计企业中同比下滑幅度最大": {"topic": "“金融”", "similarity": 0.45976197719573975, "prompt": "新闻文本是“其今年上半年净利为4.34亿元，同比下降46.92%，在统计企业中同比下滑幅度最大”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "根据彭博新能源财经发布的2023年中国风电整机制造商排名，排名前七的企业分别为金风科技、远景能源、运达股份、明阳智能、三一重能、东方电气和电气风电": {"topic": "“生产投资”", "similarity": 0.5315525531768799}, "数据来源：公司财报制图：马悦然  　　全球风电老大金风科技凭借海外及海上业务的开拓，净利润增速在上述企业中最高": {"topic": "“生产投资”", "similarity": 0.5722098350524902, "prompt": "新闻文本是“数据来源：公司财报制图：马悦然  　　全球风电老大金风科技凭借海外及海上业务的开拓，净利润增速在上述企业中最高”，包含的情绪词典是：公司的/企业的(corporate):0.0,有利可图的/盈利的(profitable):0.8"}, "其中，二季度净利达10.54亿元，同比暴增6249%，去年同期净利仅为0.166亿元": {"topic": "“生产投资”", "similarity": 0.4565325975418091, "prompt": "新闻文本是“其中，二季度净利达10.54亿元，同比暴增6249%，去年同期净利仅为0.166亿元”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "明阳智能上半年净利为6.61亿元，同比微增0.94%": {"topic": "“生产投资”", "similarity": 0.4241518974304199, "prompt": "新闻文本是“明阳智能上半年净利为6.61亿元，同比微增0.94%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "上半年，明阳智能实现风机对外销售4.01 GW，对应实现风机及相关配件销售79.22亿元": {"topic": "“生产投资”", "similarity": 0.5019135475158691, "prompt": "新闻文本是“上半年，明阳智能实现风机对外销售4.01 GW，对应实现风机及相关配件销售79.22亿元”，包含的情绪词典是：风/气流(wind):0.0,机械/机器(machinery):0.0"}, "三一重能今年一、二季度净利润均同比下滑超四成": {"topic": "“生产投资”", "similarity": 0.4416607618331909, "prompt": "新闻文本是“三一重能今年一、二季度净利润均同比下滑超四成”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "上半年，三一重能93.97%的收入来自于风机及配件收入，去年同期这部分业务占比为75.78%": {"topic": "“生产投资”", "similarity": 0.5115621089935303, "prompt": "新闻文本是“上半年，三一重能93.97%的收入来自于风机及配件收入，去年同期这部分业务占比为75.78%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,三倍的/三重的(triple):0.0"}, "相较之下，该公司风电建设服务收入占比大幅下滑，从去年上半年的近两成，降至不足3%，目前这部分营收为1.45亿元": {"topic": "“生产投资”", "similarity": 0.5253503322601318, "prompt": "新闻文本是“相较之下，该公司风电建设服务收入占比大幅下滑，从去年上半年的近两成，降至不足3%，目前这部分营收为1.45亿元”，包含的情绪词典是：衰退的/不景气的(recessionary):-0.8,表现不佳/业绩低于预期(underperforming):-0.4"}, "图片来源：三一重能财报  　　但环比看，三一重能的风机盈利能力有所提升": {"topic": "“生产投资”", "similarity": 0.5175154209136963, "prompt": "新闻文本是“图片来源：三一重能财报  　　但环比看，三一重能的风机盈利能力有所提升”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,三倍的/三重的(triple):0.0"}, "今年上半年，三一重能陆上风机对外销售容量3.3 GW，同比增长121%，创造历史同期最好交付业绩": {"topic": "“生产投资”", "similarity": 0.4833005666732788, "prompt": "新闻文本是“今年上半年，三一重能陆上风机对外销售容量3.3 GW，同比增长121%，创造历史同期最好交付业绩”，包含的情绪词典是：风/气流(wind):0.0,三倍的/三重的(triple):0.0"}, "另一陆上风机龙头运达股份业绩与去年上半年基本持平": {"topic": "“金融”", "similarity": 0.4345538914203644, "prompt": "新闻文本是“另一陆上风机龙头运达股份业绩与去年上半年基本持平”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "去年，在彭博新能源财经的中国风电整机制造商新增吊装容量排名中，运达股份再次重返前三，仅次于金风科技和远景能源": {"topic": "“生产投资”", "similarity": 0.4633735120296478}, "上半年，运达股份实现对外销售容量约4.05 GW，同比上升19.25%": {"topic": "“生产投资”", "similarity": 0.47731995582580566, "prompt": "新闻文本是“上半年，运达股份实现对外销售容量约4.05 GW，同比上升19.25%”，包含的情绪词典是：能力/容量(capacity):0.0,上升的/占优势的(ascendant):0.3"}, "运达股份披露的各产品毛利率均有所下滑，其中风电机组毛利率10.34%，同比下滑5.52个百分点": {"topic": "“生产投资”", "similarity": 0.4684721827507019, "prompt": "新闻文本是“运达股份披露的各产品毛利率均有所下滑，其中风电机组毛利率10.34%，同比下滑5.52个百分点”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "在风机价格内卷、利润率持续低迷的情况下，风电场开发、电站销售成了风电整机商新的业绩增长点": {"topic": "“生产投资”", "similarity": 0.4610344171524048, "prompt": "新闻文本是“在风机价格内卷、利润率持续低迷的情况下，风电场开发、电站销售成了风电整机商新的业绩增长点”，包含的情绪词典是：风/气流(wind):0.0,有利可图的/盈利的(profitable):0.8"}, "海上风电龙头电气风电(688660.SH)业绩仍维持亏损状态，上半年亏损3.87亿元，在被统计企业中垫底，亏损额同比减少1.78%": {"topic": "“金融”", "similarity": 0.49704670906066895, "prompt": "新闻文本是“海上风电龙头电气风电(688660.SH)业绩仍维持亏损状态，上半年亏损3.87亿元，在被统计企业中垫底，亏损额同比减少1.78%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "上半年，电气风电新增订单为3.2 GW，较上年同期增长113.71%，其中已中标尚未签订合同的订单为1.42 GW": {"topic": "“生产投资”", "similarity": 0.4996989071369171, "prompt": "新闻文本是“上半年，电气风电新增订单为3.2 GW，较上年同期增长113.71%，其中已中标尚未签订合同的订单为1.42 GW”，包含的情绪词典是：电的/电气的(electrical):0.0,风/气流(wind):0.0"}, "截至6月底，电气风电累计在手订单为11.51 GW，较上年同期增加了21.99%，其中已中标尚未签订合同的订单为2.14 GW": {"topic": "“生产投资”", "similarity": 0.440963476896286, "prompt": "新闻文本是“截至6月底，电气风电累计在手订单为11.51 GW，较上年同期增加了21.99%，其中已中标尚未签订合同的订单为2.14 GW”，包含的情绪词典是：电的/电气的(electrical):0.0,风/气流(wind):0.0"}, "在风资源开发方面，电气风电自持风场产生的发电收入为0.48亿元，较去年同期增长36.92%": {"topic": "“生产投资”", "similarity": 0.4511945843696594, "prompt": "新闻文本是“在风资源开发方面，电气风电自持风场产生的发电收入为0.48亿元，较去年同期增长36.92%”，包含的情绪词典是：风/气流(wind):0.0,开发/利用(exploitation):-0.5"}, "电气风电称，已经采取切换陆上产品技术路线、海上产品大型化升级、管理优化等多项措施应对市场挑战，但若后续风机市场招标价格仍持续大幅快速下降，而公司无法保证产品成本随销售价格同步下降，或因部分产品未来可能受较为恶劣工作环境等因素影响产生质量问题，对经营业绩产生不利影响，公司业绩仍可能存在亏损的风险": {"topic": "“生产投资”", "similarity": 0.5851413607597351, "prompt": "新闻文本是“电气风电称，已经采取切换陆上产品技术路线、海上产品大型化升级、管理优化等多项措施应对市场挑战，但若后续风机市场招标价格仍持续大幅快速下降，而公司无法保证产品成本随销售价格同步下降，或因部分产品未来可能受较为恶劣工作环境等因素影响产生质量问题，对经营业绩产生不利影响，公司业绩仍可能存在亏损的风险”，包含的情绪词典是：电的/电气的(electrical):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}}</t>
+          <t>{"去年上半年，金风科技净利降幅达34.82%、运达股份降幅49.75%、明阳智能降幅超73%": {"topic": "“金融”", "similarity": 0.49998313188552856, "prompt": "新闻文本是“去年上半年，金风科技净利降幅达34.82%、运达股份降幅49.75%、明阳智能降幅超73%”，包含的情绪词典是：下跌/下降(fall):-0.6,下降的/衰退的(declining):-0.6"}, "作为中国第五大风电整机商，三一重能(688349.SH)上半年业绩增速则由增转降": {"topic": "“生产投资”", "similarity": 0.46023574471473694, "prompt": "新闻文本是“作为中国第五大风电整机商，三一重能(688349.SH)上半年业绩增速则由增转降”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "其今年上半年净利为4.34亿元，同比下降46.92%，在统计企业中同比下滑幅度最大": {"topic": "“金融”", "similarity": 0.4597620666027069, "prompt": "新闻文本是“其今年上半年净利为4.34亿元，同比下降46.92%，在统计企业中同比下滑幅度最大”，包含的情绪词典是：表现不佳/业绩低于预期(underperformed):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "数据来源：公司财报制图：马悦然  　　全球风电老大金风科技凭借海外及海上业务的开拓，净利润增速在上述企业中最高": {"topic": "“生产投资”", "similarity": 0.5722099542617798, "prompt": "新闻文本是“数据来源：公司财报制图：马悦然  　　全球风电老大金风科技凭借海外及海上业务的开拓，净利润增速在上述企业中最高”，包含的情绪词典是：公司的/企业的(corporate):0.0,有利可图的/盈利的(profitable):0.8"}, "其中，二季度净利达10.54亿元，同比暴增6249%，去年同期净利仅为0.166亿元": {"topic": "“生产投资”", "similarity": 0.45653271675109863, "prompt": "新闻文本是“其中，二季度净利达10.54亿元，同比暴增6249%，去年同期净利仅为0.166亿元”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,利润/利益(profit):0.8"}, "明阳智能上半年净利为6.61亿元，同比微增0.94%": {"topic": "“生产投资”", "similarity": 0.4241520166397095, "prompt": "新闻文本是“明阳智能上半年净利为6.61亿元，同比微增0.94%”，包含的情绪词典是：利润/利益(profit):0.8,盈利能力/获利能力(profitability):0.6"}, "上半年，明阳智能实现风机对外销售4.01 GW，对应实现风机及相关配件销售79.22亿元": {"topic": "“生产投资”", "similarity": 0.5019135475158691, "prompt": "新闻文本是“上半年，明阳智能实现风机对外销售4.01 GW，对应实现风机及相关配件销售79.22亿元”，包含的情绪词典是：风/气流(wind):0.0,机械/机器(machinery):0.0"}, "三一重能今年一、二季度净利润均同比下滑超四成": {"topic": "“生产投资”", "similarity": 0.4416608512401581, "prompt": "新闻文本是“三一重能今年一、二季度净利润均同比下滑超四成”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperform):-0.4"}, "上半年，三一重能93.97%的收入来自于风机及配件收入，去年同期这部分业务占比为75.78%": {"topic": "“生产投资”", "similarity": 0.5115621089935303, "prompt": "新闻文本是“上半年，三一重能93.97%的收入来自于风机及配件收入，去年同期这部分业务占比为75.78%”，包含的情绪词典是：盈利能力/获利能力(profitability):0.6,三倍的/三重的(triple):0.0"}, "相较之下，该公司风电建设服务收入占比大幅下滑，从去年上半年的近两成，降至不足3%，目前这部分营收为1.45亿元": {"topic": "“生产投资”", "similarity": 0.5253504514694214, "prompt": "新闻文本是“相较之下，该公司风电建设服务收入占比大幅下滑，从去年上半年的近两成，降至不足3%，目前这部分营收为1.45亿元”，包含的情绪词典是：衰退的/不景气的(recessionary):-0.8,表现不佳/业绩低于预期(underperforming):-0.4"}, "今年上半年，三一重能陆上风机对外销售容量3.3 GW，同比增长121%，创造历史同期最好交付业绩": {"topic": "“生产投资”", "similarity": 0.48330074548721313, "prompt": "新闻文本是“今年上半年，三一重能陆上风机对外销售容量3.3 GW，同比增长121%，创造历史同期最好交付业绩”，包含的情绪词典是：风/气流(wind):0.0,三倍的/三重的(triple):0.0"}, "另一陆上风机龙头运达股份业绩与去年上半年基本持平": {"topic": "“金融”", "similarity": 0.4345541000366211, "prompt": "新闻文本是“另一陆上风机龙头运达股份业绩与去年上半年基本持平”，包含的情绪词典是：营业额/周转(turnover):0.0,表现不佳/业绩低于预期(underperform):-0.4"}, "上半年，运达股份实现对外销售容量约4.05 GW，同比上升19.25%": {"topic": "“生产投资”", "similarity": 0.4773200750350952, "prompt": "新闻文本是“上半年，运达股份实现对外销售容量约4.05 GW，同比上升19.25%”，包含的情绪词典是：能力/容量(capacity):0.0,上升的/占优势的(ascendant):0.3"}, "运达股份披露的各产品毛利率均有所下滑，其中风电机组毛利率10.34%，同比下滑5.52个百分点": {"topic": "“生产投资”", "similarity": 0.4684722423553467, "prompt": "新闻文本是“运达股份披露的各产品毛利率均有所下滑，其中风电机组毛利率10.34%，同比下滑5.52个百分点”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "在风机价格内卷、利润率持续低迷的情况下，风电场开发、电站销售成了风电整机商新的业绩增长点": {"topic": "“生产投资”", "similarity": 0.4610346555709839, "prompt": "新闻文本是“在风机价格内卷、利润率持续低迷的情况下，风电场开发、电站销售成了风电整机商新的业绩增长点”，包含的情绪词典是：风/气流(wind):0.0,有利可图的/盈利的(profitable):0.8"}, "海上风电龙头电气风电(688660.SH)业绩仍维持亏损状态，上半年亏损3.87亿元，在被统计企业中垫底，亏损额同比减少1.78%": {"topic": "“金融”", "similarity": 0.4970467686653137, "prompt": "新闻文本是“海上风电龙头电气风电(688660.SH)业绩仍维持亏损状态，上半年亏损3.87亿元，在被统计企业中垫底，亏损额同比减少1.78%”，包含的情绪词典是：表现不佳/业绩低于预期(underperforming):-0.4,表现不佳/业绩低于预期(underperformed):-0.4"}, "上半年，电气风电新增订单为3.2 GW，较上年同期增长113.71%，其中已中标尚未签订合同的订单为1.42 GW": {"topic": "“生产投资”", "similarity": 0.4996989965438843, "prompt": "新闻文本是“上半年，电气风电新增订单为3.2 GW，较上年同期增长113.71%，其中已中标尚未签订合同的订单为1.42 GW”，包含的情绪词典是：电的/电气的(electrical):0.0,风/气流(wind):0.0"}, "截至6月底，电气风电累计在手订单为11.51 GW，较上年同期增加了21.99%，其中已中标尚未签订合同的订单为2.14 GW": {"topic": "“生产投资”", "similarity": 0.4409636855125427, "prompt": "新闻文本是“截至6月底，电气风电累计在手订单为11.51 GW，较上年同期增加了21.99%，其中已中标尚未签订合同的订单为2.14 GW”，包含的情绪词典是：电的/电气的(electrical):0.0,风/气流(wind):0.0"}, "在风资源开发方面，电气风电自持风场产生的发电收入为0.48亿元，较去年同期增长36.92%": {"topic": "“生产投资”", "similarity": 0.4511946737766266, "prompt": "新闻文本是“在风资源开发方面，电气风电自持风场产生的发电收入为0.48亿元，较去年同期增长36.92%”，包含的情绪词典是：风/气流(wind):0.0,开发/利用(exploitation):-0.5"}, "电气风电称，已经采取切换陆上产品技术路线、海上产品大型化升级、管理优化等多项措施应对市场挑战，但若后续风机市场招标价格仍持续大幅快速下降，而公司无法保证产品成本随销售价格同步下降，或因部分产品未来可能受较为恶劣工作环境等因素影响产生质量问题，对经营业绩产生不利影响，公司业绩仍可能存在亏损的风险": {"topic": "“生产投资”", "similarity": 0.5851414203643799, "prompt": "新闻文本是“电气风电称，已经采取切换陆上产品技术路线、海上产品大型化升级、管理优化等多项措施应对市场挑战，但若后续风机市场招标价格仍持续大幅快速下降，而公司无法保证产品成本随销售价格同步下降，或因部分产品未来可能受较为恶劣工作环境等因素影响产生质量问题，对经营业绩产生不利影响，公司业绩仍可能存在亏损的风险”，包含的情绪词典是：电的/电气的(electrical):0.0,表现不佳/业绩低于预期(underperformed):-0.4"}}</t>
         </is>
       </c>
     </row>
@@ -5582,12 +5534,12 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "文旅市场不断上新，各种各样的文旅活动备受欢迎，避暑胜地旅游热度攀升……在刚刚过去的暑期，“清凉”旅游“出圈”又“出彩”，激发出文旅市场新活力", "news_prompt2": "日前，《关于促进服务消费高质量发展的意见》发布，明确提出激发改善型消费活力，并围绕旅游消费作出了重要部署", "news_prompt3": "文化和旅游部最新数据显示，今年上半年，国内出游人次27.25亿，同比增长14.3%", "news_prompt4": "国内游客出游总花费2.73万亿元，同比增长19.0%", "news_prompt5": "这个夏天，“清凉”旅游释放经济新动能，各地文旅纷纷上新，推出避暑旅游新产品，让“轻装上阵”的旅行更清爽", "news_prompt6": "在贵州黔东南，以水为主题的各项体验活动陆续上演，玩水、观瀑，游客可以在青山绿水间享受夏日的清凉与速度的激情", "news_prompt7": "在黑龙江哈尔滨，宜人的气候为远道而来的游客“降温”，室内冰雪馆通过冰块的反季储存、利用，让“冰雪奇遇”不再是“季节限定”", "news_prompt8": "在云南，火爆的“采菌游”开启美食之旅，游客在品尝美食的同时，也能深入了解当地的菌文化，“清凉”不仅是一种体感，更是一场味蕾的盛宴", "news_prompt9": "业内专家表示，人们对“清凉消费”的需求增加，不仅有助于激发旅游、餐饮、娱乐等传统行业的活力，还将为数字经济、共享经济、平台经济等新业态、新模式提供更加丰富的内容，催生更多新业态", "news_prompt10": "清凉消费市场火热，让诸多相关产业也迎来了新的机遇和发展空间", "news_prompt11": "一些出行目的地抢抓“凉”机，不断丰富旅游业态", "news_prompt12": "贵州六盘水与海南、重庆、武汉等城市建立“候鸟式”养老联盟，开辟农业观光游、林果游、花卉游等不同特色的游玩场景，吸引游客旅居", "news_prompt13": "吉林延边凭借生态、气候、文化等优势，打造“民俗+旅游+体验”新风尚，将民俗风情展示、文化演艺体验、特色餐饮民宿、古朴传统建筑等相互融合，让游客感受朝鲜族民俗文化特色，把“冷资源”变成了“热产业”", "news_prompt14": "在今年暑期，避暑旅游目的地的热度持续增长", "news_prompt15": "相关旅游平台数据，7月以来，避暑相关搜索量大幅增长，其中，张北坝上草原、承德避暑山庄的搜索量大大增加，以伊春、哈尔滨、大兴安岭等为目的地的酒店预订数量增幅均超50%", "news_prompt16": "平台上还出现了周边小镇避暑出游的新趋势、新玩法，进一步丰富了游客的旅行体验", "news_prompt17": "“清凉消费”为消费市场带来更多人气，对于激发经济活力具有重要意义", "news_prompt18": "业内专家表示，在进一步挖掘和整合资源，打造更多创新性消费场景和模式的同时，也要加大对市场的监管力度，维护好市场秩序和消费者权益，为夏日经济的健康发展提供有力保障", "news_prompt19": "“目前，我国旅游业已经从观光为主进一步向观光、休闲、研学等多元化格局转变，旅游者的价值追求更加多样", "news_prompt20": "”中国旅游研究院政策与科教研究所所长宋子千表示，未来，除了持续推进旅游与各领域融合、积极发展文旅新业态，还应瞄准文化强国和旅游强国建设，推进文旅标准化进程，积极培育优质文旅产品", "news_prompt21": "（文章来源：人民网）"}</t>
+          <t>{"news_prompt1": "文旅市场不断上新，各种各样的文旅活动备受欢迎，避暑胜地旅游热度攀升……在刚刚过去的暑期，“清凉”旅游“出圈”又“出彩”，激发出文旅市场新活力", "news_prompt2": "日前，《关于促进服务消费高质量发展的意见》发布，明确提出激发改善型消费活力，并围绕旅游消费作出了重要部署", "news_prompt3": "文化和旅游部最新数据显示，今年上半年，国内出游人次27.25亿，同比增长14.3%", "news_prompt4": "国内游客出游总花费2.73万亿元，同比增长19.0%", "news_prompt5": "这个夏天，“清凉”旅游释放经济新动能，各地文旅纷纷上新，推出避暑旅游新产品，让“轻装上阵”的旅行更清爽", "news_prompt6": "在贵州黔东南，以水为主题的各项体验活动陆续上演，玩水、观瀑，游客可以在青山绿水间享受夏日的清凉与速度的激情", "news_prompt7": "在黑龙江哈尔滨，宜人的气候为远道而来的游客“降温”，室内冰雪馆通过冰块的反季储存、利用，让“冰雪奇遇”不再是“季节限定”", "news_prompt8": "在云南，火爆的“采菌游”开启美食之旅，游客在品尝美食的同时，也能深入了解当地的菌文化，“清凉”不仅是一种体感，更是一场味蕾的盛宴", "news_prompt9": "业内专家表示，人们对“清凉消费”的需求增加，不仅有助于激发旅游、餐饮、娱乐等传统行业的活力，还将为数字经济、共享经济、平台经济等新业态、新模式提供更加丰富的内容，催生更多新业态", "news_prompt10": "清凉消费市场火热，让诸多相关产业也迎来了新的机遇和发展空间", "news_prompt11": "一些出行目的地抢抓“凉”机，不断丰富旅游业态", "news_prompt12": "贵州六盘水与海南、重庆、武汉等城市建立“候鸟式”养老联盟，开辟农业观光游、林果游、花卉游等不同特色的游玩场景，吸引游客旅居", "news_prompt13": "吉林延边凭借生态、气候、文化等优势，打造“民俗+旅游+体验”新风尚，将民俗风情展示、文化演艺体验、特色餐饮民宿、古朴传统建筑等相互融合，让游客感受朝鲜族民俗文化特色，把“冷资源”变成了“热产业”", "news_prompt14": "相关旅游平台数据，7月以来，避暑相关搜索量大幅增长，其中，张北坝上草原、承德避暑山庄的搜索量大大增加，以伊春、哈尔滨、大兴安岭等为目的地的酒店预订数量增幅均超50%", "news_prompt15": "平台上还出现了周边小镇避暑出游的新趋势、新玩法，进一步丰富了游客的旅行体验", "news_prompt16": "“清凉消费”为消费市场带来更多人气，对于激发经济活力具有重要意义", "news_prompt17": "业内专家表示，在进一步挖掘和整合资源，打造更多创新性消费场景和模式的同时，也要加大对市场的监管力度，维护好市场秩序和消费者权益，为夏日经济的健康发展提供有力保障", "news_prompt18": "“目前，我国旅游业已经从观光为主进一步向观光、休闲、研学等多元化格局转变，旅游者的价值追求更加多样", "news_prompt19": "”中国旅游研究院政策与科教研究所所长宋子千表示，未来，除了持续推进旅游与各领域融合、积极发展文旅新业态，还应瞄准文化强国和旅游强国建设，推进文旅标准化进程，积极培育优质文旅产品"}</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>{"文旅市场不断上新，各种各样的文旅活动备受欢迎，避暑胜地旅游热度攀升……在刚刚过去的暑期，“清凉”旅游“出圈”又“出彩”，激发出文旅市场新活力": {"topic": "“消费”", "similarity": 0.5154359936714172, "prompt": "新闻文本是“文旅市场不断上新，各种各样的文旅活动备受欢迎，避暑胜地旅游热度攀升……在刚刚过去的暑期，“清凉”旅游“出圈”又“出彩”，激发出文旅市场新活力”，包含的情绪词典是：流行的/受欢迎的(popular):0.3,繁荣的/兴旺的(prosperous):0.9"}, "日前，《关于促进服务消费高质量发展的意见》发布，明确提出激发改善型消费活力，并围绕旅游消费作出了重要部署": {"topic": "“消费”", "similarity": 0.6730010509490967, "prompt": "新闻文本是“日前，《关于促进服务消费高质量发展的意见》发布，明确提出激发改善型消费活力，并围绕旅游消费作出了重要部署”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,已改善的/已改进的(improved):0.5"}, "文化和旅游部最新数据显示，今年上半年，国内出游人次27.25亿，同比增长14.3%": {"topic": "“消费”", "similarity": 0.5418322086334229, "prompt": "新闻文本是“文化和旅游部最新数据显示，今年上半年，国内出游人次27.25亿，同比增长14.3%”，包含的情绪词典是：增加/增长(increase):0.6,费用/票价(fare):0.4"}, "国内游客出游总花费2.73万亿元，同比增长19.0%": {"topic": "“消费”", "similarity": 0.43158936500549316, "prompt": "新闻文本是“国内游客出游总花费2.73万亿元，同比增长19.0%”，包含的情绪词典是：花费/消费(spend):0.0,费用/票价(fare):0.4"}, "这个夏天，“清凉”旅游释放经济新动能，各地文旅纷纷上新，推出避暑旅游新产品，让“轻装上阵”的旅行更清爽": {"topic": "“消费”", "similarity": 0.5176712274551392, "prompt": "新闻文本是“这个夏天，“清凉”旅游释放经济新动能，各地文旅纷纷上新，推出避暑旅游新产品，让“轻装上阵”的旅行更清爽”，包含的情绪词典是：夏季(summer):0.0,冷静的/凉爽的(cool):0.3"}, "在贵州黔东南，以水为主题的各项体验活动陆续上演，玩水、观瀑，游客可以在青山绿水间享受夏日的清凉与速度的激情": {"topic": "“消费”", "similarity": 0.44273054599761963, "prompt": "新闻文本是“在贵州黔东南，以水为主题的各项体验活动陆续上演，玩水、观瀑，游客可以在青山绿水间享受夏日的清凉与速度的激情”，包含的情绪词典是：水/水资源(water):0.0,夏季(summer):0.0"}, "在黑龙江哈尔滨，宜人的气候为远道而来的游客“降温”，室内冰雪馆通过冰块的反季储存、利用，让“冰雪奇遇”不再是“季节限定”": {"topic": "“消费”", "similarity": 0.46864157915115356, "prompt": "新闻文本是“在黑龙江哈尔滨，宜人的气候为远道而来的游客“降温”，室内冰雪馆通过冰块的反季储存、利用，让“冰雪奇遇”不再是“季节限定””，包含的情绪词典是：季节/时期(season):0.0,季度/四分之一(quarter):0.0"}, "在云南，火爆的“采菌游”开启美食之旅，游客在品尝美食的同时，也能深入了解当地的菌文化，“清凉”不仅是一种体感，更是一场味蕾的盛宴": {"topic": "“消费”", "similarity": 0.4952791929244995, "prompt": "新闻文本是“在云南，火爆的“采菌游”开启美食之旅，游客在品尝美食的同时，也能深入了解当地的菌文化，“清凉”不仅是一种体感，更是一场味蕾的盛宴”，包含的情绪词典是：食物/食品(food):0.0,农业的/农学的(agricultural):0.0"}, "业内专家表示，人们对“清凉消费”的需求增加，不仅有助于激发旅游、餐饮、娱乐等传统行业的活力，还将为数字经济、共享经济、平台经济等新业态、新模式提供更加丰富的内容，催生更多新业态": {"topic": "“消费”", "similarity": 0.6588506698608398, "prompt": "新闻文本是“业内专家表示，人们对“清凉消费”的需求增加，不仅有助于激发旅游、餐饮、娱乐等传统行业的活力，还将为数字经济、共享经济、平台经济等新业态、新模式提供更加丰富的内容，催生更多新业态”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,消费者/用户(consumer):0.0"}, "清凉消费市场火热，让诸多相关产业也迎来了新的机遇和发展空间": {"topic": "“消费”", "similarity": 0.5701321363449097, "prompt": "新闻文本是“清凉消费市场火热，让诸多相关产业也迎来了新的机遇和发展空间”，包含的情绪词典是：冷静的/凉爽的(cool):0.3,机会/时机(opportunity):0.5"}, "一些出行目的地抢抓“凉”机，不断丰富旅游业态": {"topic": "“消费”", "similarity": 0.42341387271881104, "prompt": "新闻文本是“一些出行目的地抢抓“凉”机，不断丰富旅游业态”，包含的情绪词典是：冷静的/凉爽的(cool):0.3,夏季(summer):0.0"}, "贵州六盘水与海南、重庆、武汉等城市建立“候鸟式”养老联盟，开辟农业观光游、林果游、花卉游等不同特色的游玩场景，吸引游客旅居": {"topic": "“消费”", "similarity": 0.5551329851150513, "prompt": "新闻文本是“贵州六盘水与海南、重庆、武汉等城市建立“候鸟式”养老联盟，开辟农业观光游、林果游、花卉游等不同特色的游玩场景，吸引游客旅居”，包含的情绪词典是：受抚养者/受赡养者(dependant):0.0,国内的/本国的(domestic):0.0"}, "吉林延边凭借生态、气候、文化等优势，打造“民俗+旅游+体验”新风尚，将民俗风情展示、文化演艺体验、特色餐饮民宿、古朴传统建筑等相互融合，让游客感受朝鲜族民俗文化特色，把“冷资源”变成了“热产业”": {"topic": "“消费”", "similarity": 0.5208747386932373, "prompt": "新闻文本是“吉林延边凭借生态、气候、文化等优势，打造“民俗+旅游+体验”新风尚，将民俗风情展示、文化演艺体验、特色餐饮民宿、古朴传统建筑等相互融合，让游客感受朝鲜族民俗文化特色，把“冷资源”变成了“热产业””，包含的情绪词典是：优势/有利条件(advantage):0.7,独特地/有特色地(distinctively):0.0"}, "相关旅游平台数据，7月以来，避暑相关搜索量大幅增长，其中，张北坝上草原、承德避暑山庄的搜索量大大增加，以伊春、哈尔滨、大兴安岭等为目的地的酒店预订数量增幅均超50%": {"topic": "“消费”", "similarity": 0.5376425981521606, "prompt": "新闻文本是“相关旅游平台数据，7月以来，避暑相关搜索量大幅增长，其中，张北坝上草原、承德避暑山庄的搜索量大大增加，以伊春、哈尔滨、大兴安岭等为目的地的酒店预订数量增幅均超50%”，包含的情绪词典是：夏季(summer):0.0,流行的/受欢迎的(popular):0.3"}, "平台上还出现了周边小镇避暑出游的新趋势、新玩法，进一步丰富了游客的旅行体验": {"topic": "“消费”", "similarity": 0.45989885926246643, "prompt": "新闻文本是“平台上还出现了周边小镇避暑出游的新趋势、新玩法，进一步丰富了游客的旅行体验”，包含的情绪词典是：夏季(summer):0.0,玩耍/发挥(play):0.0"}, "“清凉消费”为消费市场带来更多人气，对于激发经济活力具有重要意义": {"topic": "“消费”", "similarity": 0.5370025634765625, "prompt": "新闻文本是““清凉消费”为消费市场带来更多人气，对于激发经济活力具有重要意义”，包含的情绪词典是：消费者/用户(consumer):0.0,冷静的/凉爽的(cool):0.3"}, "业内专家表示，在进一步挖掘和整合资源，打造更多创新性消费场景和模式的同时，也要加大对市场的监管力度，维护好市场秩序和消费者权益，为夏日经济的健康发展提供有力保障": {"topic": "“消费”", "similarity": 0.5924826264381409, "prompt": "新闻文本是“业内专家表示，在进一步挖掘和整合资源，打造更多创新性消费场景和模式的同时，也要加大对市场的监管力度，维护好市场秩序和消费者权益，为夏日经济的健康发展提供有力保障”，包含的情绪词典是：监管的/调控的(regulatory):0.0,调控性的/监管性的(regulative):0.0"}, "“目前，我国旅游业已经从观光为主进一步向观光、休闲、研学等多元化格局转变，旅游者的价值追求更加多样": {"topic": "“消费”", "similarity": 0.6023675203323364, "prompt": "新闻文本是““目前，我国旅游业已经从观光为主进一步向观光、休闲、研学等多元化格局转变，旅游者的价值追求更加多样”，包含的情绪词典是：多样的/不同的(diverse):0.0,价值/价值观(value):0.2"}, "”中国旅游研究院政策与科教研究所所长宋子千表示，未来，除了持续推进旅游与各领域融合、积极发展文旅新业态，还应瞄准文化强国和旅游强国建设，推进文旅标准化进程，积极培育优质文旅产品": {"topic": "“消费”", "similarity": 0.6076182126998901, "prompt": "新闻文本是“”中国旅游研究院政策与科教研究所所长宋子千表示，未来，除了持续推进旅游与各领域融合、积极发展文旅新业态，还应瞄准文化强国和旅游强国建设，推进文旅标准化进程，积极培育优质文旅产品”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,有影响力的/有势力的(influential):0.4"}, "（文章来源：人民网）": {"topic": "“宏观经济”", "similarity": 0.4227719306945801, "prompt": "新闻文本是“（文章来源：人民网）”，包含的情绪词典是：人民/人们(people):0.0,中国的/中国人的(chinese):0.0"}}</t>
+          <t>{"文旅市场不断上新，各种各样的文旅活动备受欢迎，避暑胜地旅游热度攀升……在刚刚过去的暑期，“清凉”旅游“出圈”又“出彩”，激发出文旅市场新活力": {"topic": "“消费”", "similarity": 0.515436053276062, "prompt": "新闻文本是“文旅市场不断上新，各种各样的文旅活动备受欢迎，避暑胜地旅游热度攀升……在刚刚过去的暑期，“清凉”旅游“出圈”又“出彩”，激发出文旅市场新活力”，包含的情绪词典是：流行的/受欢迎的(popular):0.3,繁荣的/兴旺的(prosperous):0.9"}, "日前，《关于促进服务消费高质量发展的意见》发布，明确提出激发改善型消费活力，并围绕旅游消费作出了重要部署": {"topic": "“消费”", "similarity": 0.6730011701583862, "prompt": "新闻文本是“日前，《关于促进服务消费高质量发展的意见》发布，明确提出激发改善型消费活力，并围绕旅游消费作出了重要部署”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,已改善的/已改进的(improved):0.5"}, "文化和旅游部最新数据显示，今年上半年，国内出游人次27.25亿，同比增长14.3%": {"topic": "“消费”", "similarity": 0.5418325066566467, "prompt": "新闻文本是“文化和旅游部最新数据显示，今年上半年，国内出游人次27.25亿，同比增长14.3%”，包含的情绪词典是：增加/增长(increase):0.6,费用/票价(fare):0.4"}, "国内游客出游总花费2.73万亿元，同比增长19.0%": {"topic": "“消费”", "similarity": 0.4315895438194275, "prompt": "新闻文本是“国内游客出游总花费2.73万亿元，同比增长19.0%”，包含的情绪词典是：花费/消费(spend):0.0,费用/票价(fare):0.4"}, "这个夏天，“清凉”旅游释放经济新动能，各地文旅纷纷上新，推出避暑旅游新产品，让“轻装上阵”的旅行更清爽": {"topic": "“消费”", "similarity": 0.5176713466644287, "prompt": "新闻文本是“这个夏天，“清凉”旅游释放经济新动能，各地文旅纷纷上新，推出避暑旅游新产品，让“轻装上阵”的旅行更清爽”，包含的情绪词典是：夏季(summer):0.0,冷静的/凉爽的(cool):0.3"}, "在贵州黔东南，以水为主题的各项体验活动陆续上演，玩水、观瀑，游客可以在青山绿水间享受夏日的清凉与速度的激情": {"topic": "“消费”", "similarity": 0.4427306056022644, "prompt": "新闻文本是“在贵州黔东南，以水为主题的各项体验活动陆续上演，玩水、观瀑，游客可以在青山绿水间享受夏日的清凉与速度的激情”，包含的情绪词典是：水/水资源(water):0.0,夏季(summer):0.0"}, "在黑龙江哈尔滨，宜人的气候为远道而来的游客“降温”，室内冰雪馆通过冰块的反季储存、利用，让“冰雪奇遇”不再是“季节限定”": {"topic": "“消费”", "similarity": 0.4686417579650879, "prompt": "新闻文本是“在黑龙江哈尔滨，宜人的气候为远道而来的游客“降温”，室内冰雪馆通过冰块的反季储存、利用，让“冰雪奇遇”不再是“季节限定””，包含的情绪词典是：季节/时期(season):0.0,季度/四分之一(quarter):0.0"}, "在云南，火爆的“采菌游”开启美食之旅，游客在品尝美食的同时，也能深入了解当地的菌文化，“清凉”不仅是一种体感，更是一场味蕾的盛宴": {"topic": "“消费”", "similarity": 0.49527931213378906, "prompt": "新闻文本是“在云南，火爆的“采菌游”开启美食之旅，游客在品尝美食的同时，也能深入了解当地的菌文化，“清凉”不仅是一种体感，更是一场味蕾的盛宴”，包含的情绪词典是：食物/食品(food):0.0,农业的/农学的(agricultural):0.0"}, "业内专家表示，人们对“清凉消费”的需求增加，不仅有助于激发旅游、餐饮、娱乐等传统行业的活力，还将为数字经济、共享经济、平台经济等新业态、新模式提供更加丰富的内容，催生更多新业态": {"topic": "“消费”", "similarity": 0.6588507294654846, "prompt": "新闻文本是“业内专家表示，人们对“清凉消费”的需求增加，不仅有助于激发旅游、餐饮、娱乐等传统行业的活力，还将为数字经济、共享经济、平台经济等新业态、新模式提供更加丰富的内容，催生更多新业态”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,消费者/用户(consumer):0.0"}, "清凉消费市场火热，让诸多相关产业也迎来了新的机遇和发展空间": {"topic": "“消费”", "similarity": 0.5701322555541992, "prompt": "新闻文本是“清凉消费市场火热，让诸多相关产业也迎来了新的机遇和发展空间”，包含的情绪词典是：冷静的/凉爽的(cool):0.3,机会/时机(opportunity):0.5"}, "一些出行目的地抢抓“凉”机，不断丰富旅游业态": {"topic": "“消费”", "similarity": 0.42341411113739014, "prompt": "新闻文本是“一些出行目的地抢抓“凉”机，不断丰富旅游业态”，包含的情绪词典是：冷静的/凉爽的(cool):0.3,夏季(summer):0.0"}, "贵州六盘水与海南、重庆、武汉等城市建立“候鸟式”养老联盟，开辟农业观光游、林果游、花卉游等不同特色的游玩场景，吸引游客旅居": {"topic": "“消费”", "similarity": 0.555133044719696, "prompt": "新闻文本是“贵州六盘水与海南、重庆、武汉等城市建立“候鸟式”养老联盟，开辟农业观光游、林果游、花卉游等不同特色的游玩场景，吸引游客旅居”，包含的情绪词典是：受抚养者/受赡养者(dependant):0.0,国内的/本国的(domestic):0.0"}, "吉林延边凭借生态、气候、文化等优势，打造“民俗+旅游+体验”新风尚，将民俗风情展示、文化演艺体验、特色餐饮民宿、古朴传统建筑等相互融合，让游客感受朝鲜族民俗文化特色，把“冷资源”变成了“热产业”": {"topic": "“消费”", "similarity": 0.5208749771118164, "prompt": "新闻文本是“吉林延边凭借生态、气候、文化等优势，打造“民俗+旅游+体验”新风尚，将民俗风情展示、文化演艺体验、特色餐饮民宿、古朴传统建筑等相互融合，让游客感受朝鲜族民俗文化特色，把“冷资源”变成了“热产业””，包含的情绪词典是：优势/有利条件(advantage):0.7,独特地/有特色地(distinctively):0.0"}, "相关旅游平台数据，7月以来，避暑相关搜索量大幅增长，其中，张北坝上草原、承德避暑山庄的搜索量大大增加，以伊春、哈尔滨、大兴安岭等为目的地的酒店预订数量增幅均超50%": {"topic": "“消费”", "similarity": 0.5376427173614502, "prompt": "新闻文本是“相关旅游平台数据，7月以来，避暑相关搜索量大幅增长，其中，张北坝上草原、承德避暑山庄的搜索量大大增加，以伊春、哈尔滨、大兴安岭等为目的地的酒店预订数量增幅均超50%”，包含的情绪词典是：夏季(summer):0.0,流行的/受欢迎的(popular):0.3"}, "平台上还出现了周边小镇避暑出游的新趋势、新玩法，进一步丰富了游客的旅行体验": {"topic": "“消费”", "similarity": 0.4598991274833679, "prompt": "新闻文本是“平台上还出现了周边小镇避暑出游的新趋势、新玩法，进一步丰富了游客的旅行体验”，包含的情绪词典是：夏季(summer):0.0,玩耍/发挥(play):0.0"}, "“清凉消费”为消费市场带来更多人气，对于激发经济活力具有重要意义": {"topic": "“消费”", "similarity": 0.5370028018951416, "prompt": "新闻文本是““清凉消费”为消费市场带来更多人气，对于激发经济活力具有重要意义”，包含的情绪词典是：消费者/用户(consumer):0.0,冷静的/凉爽的(cool):0.3"}, "业内专家表示，在进一步挖掘和整合资源，打造更多创新性消费场景和模式的同时，也要加大对市场的监管力度，维护好市场秩序和消费者权益，为夏日经济的健康发展提供有力保障": {"topic": "“消费”", "similarity": 0.5924827456474304, "prompt": "新闻文本是“业内专家表示，在进一步挖掘和整合资源，打造更多创新性消费场景和模式的同时，也要加大对市场的监管力度，维护好市场秩序和消费者权益，为夏日经济的健康发展提供有力保障”，包含的情绪词典是：监管的/调控的(regulatory):0.0,调控性的/监管性的(regulative):0.0"}, "“目前，我国旅游业已经从观光为主进一步向观光、休闲、研学等多元化格局转变，旅游者的价值追求更加多样": {"topic": "“消费”", "similarity": 0.6023676991462708, "prompt": "新闻文本是““目前，我国旅游业已经从观光为主进一步向观光、休闲、研学等多元化格局转变，旅游者的价值追求更加多样”，包含的情绪词典是：多样的/不同的(diverse):0.0,价值/价值观(value):0.2"}, "”中国旅游研究院政策与科教研究所所长宋子千表示，未来，除了持续推进旅游与各领域融合、积极发展文旅新业态，还应瞄准文化强国和旅游强国建设，推进文旅标准化进程，积极培育优质文旅产品": {"topic": "“消费”", "similarity": 0.6076183319091797, "prompt": "新闻文本是“”中国旅游研究院政策与科教研究所所长宋子千表示，未来，除了持续推进旅游与各领域融合、积极发展文旅新业态，还应瞄准文化强国和旅游强国建设，推进文旅标准化进程，积极培育优质文旅产品”，包含的情绪词典是：提供信息的/增长见闻的(informative):0.5,有影响力的/有势力的(influential):0.4"}}</t>
         </is>
       </c>
     </row>
@@ -5633,12 +5585,12 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>{"news_prompt1": "人民网北京9月2日电 （记者王震）据财政部网站消息，近日，财政部公布2024年7月份全国彩票销售情况", "news_prompt2": "数据显示，7月份，全国共销售彩票546.55亿元，同比增加57.50亿元，增长11.8%", "news_prompt3": "其中，福利彩票机构销售176.35亿元，同比减少2.31亿元，下降1.3%，主要原因是去年同期基数相对较高，以及即开型彩票销量下降", "news_prompt4": "体育彩票机构销售370.20亿元，同比增加59.81亿元，增长19.3%，主要原因是欧洲杯赛事拉动竞猜型彩票销量短期快速增长", "news_prompt5": "1至7月累计，全国共销售彩票3631.33亿元，同比增加403.29亿元，增长12.5%", "news_prompt6": "其中，福利彩票机构销售1226.54亿元，同比增加149.72亿元，增长13.9%", "news_prompt7": "体育彩票机构销售2404.79亿元，同比增加253.57亿元，增长11.8%", "news_prompt8": "（文章来源：人民网）"}</t>
+          <t>{"news_prompt1": "数据显示，7月份，全国共销售彩票546.55亿元，同比增加57.50亿元，增长11.8%", "news_prompt2": "其中，福利彩票机构销售176.35亿元，同比减少2.31亿元，下降1.3%，主要原因是去年同期基数相对较高，以及即开型彩票销量下降", "news_prompt3": "体育彩票机构销售370.20亿元，同比增加59.81亿元，增长19.3%，主要原因是欧洲杯赛事拉动竞猜型彩票销量短期快速增长", "news_prompt4": "1至7月累计，全国共销售彩票3631.33亿元，同比增加403.29亿元，增长12.5%", "news_prompt5": "其中，福利彩票机构销售1226.54亿元，同比增加149.72亿元，增长13.9%", "news_prompt6": "体育彩票机构销售2404.79亿元，同比增加253.57亿元，增长11.8%"}</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>{"人民网北京9月2日电 （记者王震）据财政部网站消息，近日，财政部公布2024年7月份全国彩票销售情况": {"topic": "“消费”", "similarity": 0.5080578327178955}, "数据显示，7月份，全国共销售彩票546.55亿元，同比增加57.50亿元，增长11.8%": {"topic": "“消费”", "similarity": 0.5330165028572083, "prompt": "新闻文本是“数据显示，7月份，全国共销售彩票546.55亿元，同比增加57.50亿元，增长11.8%”，包含的情绪词典是：数字/数位(digit):0.0,获胜者/赢家(winner):0.8"}, "其中，福利彩票机构销售176.35亿元，同比减少2.31亿元，下降1.3%，主要原因是去年同期基数相对较高，以及即开型彩票销量下降": {"topic": "“消费”", "similarity": 0.589133083820343, "prompt": "新闻文本是“其中，福利彩票机构销售176.35亿元，同比减少2.31亿元，下降1.3%，主要原因是去年同期基数相对较高，以及即开型彩票销量下降”，包含的情绪词典是：下降/衰退(decline):-0.6,减少/降低(reduction):-0.4"}, "体育彩票机构销售370.20亿元，同比增加59.81亿元，增长19.3%，主要原因是欧洲杯赛事拉动竞猜型彩票销量短期快速增长": {"topic": "“消费”", "similarity": 0.5419489741325378, "prompt": "新闻文本是“体育彩票机构销售370.20亿元，同比增加59.81亿元，增长19.3%，主要原因是欧洲杯赛事拉动竞猜型彩票销量短期快速增长”，包含的情绪词典是：游戏/比赛(game):0.0,投机性的/推测性的(speculative):-0.2"}, "1至7月累计，全国共销售彩票3631.33亿元，同比增加403.29亿元，增长12.5%": {"topic": "“消费”", "similarity": 0.5292794704437256, "prompt": "新闻文本是“1至7月累计，全国共销售彩票3631.33亿元，同比增加403.29亿元，增长12.5%”，包含的情绪词典是：增加/增长(increase):0.6,销售/售卖(sell):0.0"}, "其中，福利彩票机构销售1226.54亿元，同比增加149.72亿元，增长13.9%": {"topic": "“消费”", "similarity": 0.472761869430542, "prompt": "新闻文本是“其中，福利彩票机构销售1226.54亿元，同比增加149.72亿元，增长13.9%”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "体育彩票机构销售2404.79亿元，同比增加253.57亿元，增长11.8%": {"topic": "“消费”", "similarity": 0.42016491293907166, "prompt": "新闻文本是“体育彩票机构销售2404.79亿元，同比增加253.57亿元，增长11.8%”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "（文章来源：人民网）": {"topic": "“宏观经济”", "similarity": 0.4227719306945801, "prompt": "新闻文本是“（文章来源：人民网）”，包含的情绪词典是：人民/人们(people):0.0,中国的/中国人的(chinese):0.0"}}</t>
+          <t>{"数据显示，7月份，全国共销售彩票546.55亿元，同比增加57.50亿元，增长11.8%": {"topic": "“消费”", "similarity": 0.5330166816711426, "prompt": "新闻文本是“数据显示，7月份，全国共销售彩票546.55亿元，同比增加57.50亿元，增长11.8%”，包含的情绪词典是：数字/数位(digit):0.0,获胜者/赢家(winner):0.8"}, "其中，福利彩票机构销售176.35亿元，同比减少2.31亿元，下降1.3%，主要原因是去年同期基数相对较高，以及即开型彩票销量下降": {"topic": "“消费”", "similarity": 0.5891332030296326, "prompt": "新闻文本是“其中，福利彩票机构销售176.35亿元，同比减少2.31亿元，下降1.3%，主要原因是去年同期基数相对较高，以及即开型彩票销量下降”，包含的情绪词典是：下降/衰退(decline):-0.6,减少/降低(reduction):-0.4"}, "体育彩票机构销售370.20亿元，同比增加59.81亿元，增长19.3%，主要原因是欧洲杯赛事拉动竞猜型彩票销量短期快速增长": {"topic": "“消费”", "similarity": 0.5419489741325378, "prompt": "新闻文本是“体育彩票机构销售370.20亿元，同比增加59.81亿元，增长19.3%，主要原因是欧洲杯赛事拉动竞猜型彩票销量短期快速增长”，包含的情绪词典是：游戏/比赛(game):0.0,投机性的/推测性的(speculative):-0.2"}, "1至7月累计，全国共销售彩票3631.33亿元，同比增加403.29亿元，增长12.5%": {"topic": "“消费”", "similarity": 0.5292794704437256, "prompt": "新闻文本是“1至7月累计，全国共销售彩票3631.33亿元，同比增加403.29亿元，增长12.5%”，包含的情绪词典是：增加/增长(increase):0.6,销售/售卖(sell):0.0"}, "其中，福利彩票机构销售1226.54亿元，同比增加149.72亿元，增长13.9%": {"topic": "“消费”", "similarity": 0.47276198863983154, "prompt": "新闻文本是“其中，福利彩票机构销售1226.54亿元，同比增加149.72亿元，增长13.9%”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}, "体育彩票机构销售2404.79亿元，同比增加253.57亿元，增长11.8%": {"topic": "“消费”", "similarity": 0.42016491293907166, "prompt": "新闻文本是“体育彩票机构销售2404.79亿元，同比增加253.57亿元，增长11.8%”，包含的情绪词典是：增长/发展(growth):0.7,增加/增长(increase):0.6"}}</t>
         </is>
       </c>
     </row>

</xml_diff>